<commit_message>
Add ranking data for 2025-06-23
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -1,57 +1,51 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\156608\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67933895-F636-475C-B57E-C7ED93520976}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9012" xr2:uid="{72F17BA6-9809-4D1E-A41D-F997EBE89B8B}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9012" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="2025-06-23" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
+      <name val="游ゴシック"/>
+      <charset val="128"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="游ゴシック"/>
-      <family val="2"/>
-      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="游ゴシック"/>
+      <charset val="128"/>
+      <family val="2"/>
       <sz val="6"/>
-      <name val="游ゴシック"/>
-      <family val="2"/>
-      <charset val="128"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -59,30 +53,98 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -382,14 +444,1060 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B270870B-31C1-4BA9-BAEA-E44EEBA42EF3}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <sheetData/>
-  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>姫様“拷問”の時間です</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>拷問143</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>塔の管理をしてみよう</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>第90話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>いとこのこ</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>いぬちく(著者)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>第35話</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>黒幕一家に転生したけど原作無視して独立する</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>空野進 赤村晃人 笠間三四郎 るろお</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>第４話　盗賊を撃破して独立する（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>モブ高生の俺でも冒険者になればリア充になれますか？</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>原作：百均 漫画：さぎやまれん キャラクター原案：hai</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>第29.5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>窓際編集とバカにされた俺が、双子ＪＫと同居することになった</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>うさおとめ(著者) 茨木野(原作) トモゼロ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>第3話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>宇崎ちゃんは遊びたい！</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>丈(著者)</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>第124話</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Fate/kaleid liner プリズマ☆イリヤ ドライ！！</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>ひろやまひろし(著者) ＴＹＰＥ－ＭＯＯＮ(原作)</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>第76話 前編　双つ星</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>不純な彼女達は懺悔しない</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>ポロロッカ(著者)</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>第27話</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ぽんドロイド！ はまさん</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>はれやまはれぞう(著者)</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>第1話</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>第70話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>地味子な三葉さんが僕を誘惑する</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>はぶらえる(著者)</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>第9話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ギャルゲーマーに褒められたい</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>げしゅまろ(著者)</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>30話</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>男子高校生だけどギャルにTSしました</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>太陽まりい(著者)</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>第17話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>「才能の器」で目指す迷宮最深部 スキル横伸ばしのはずが、万能チートだった!</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>漫画：かくばやしつよし 原作：とんび キャラクター原案： りりんら</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>第38話</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>理想の彼女</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>もりまりも(著者)</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>第21話</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>アラサーがVTuberになった話。</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>犬威赤彦(漫画) とくめい(原作) カラスBTK(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>第21話</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>きみの願いが叶うまで</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>浅月のりと(著者)</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>第2話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>彼女にしたい女子一位、の隣で見つけたあまりちゃん</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>寝巻ネルゾ(漫画) 裕時悠示(原作) たん旦(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>休載イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>規格外のダンジョン攻略者、実は異世界帰りの元勇者</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>作画：やまざき君 原作：榊与一</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>第3話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>アースウィズダンジョン ～固有スキル≪等価交換ストア≫を駆使して世界救済を目指します～</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>原作：バッド 漫画：高遠けい キャラクター原案：揚 茄子央</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>第8話</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>番外編四コマ！</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>ろぐあうと！</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>人参(著者)</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>読切</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>魔都精兵のスレイブ</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>原作:タカヒロ　漫画:竹村洋平</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>第155話　大極</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>ソードアート・オンライン Re:Aincrad</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>樹深(作画) 佐藤ミト(構成) 川原礫(原作) ａｂｅｃ(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>第39話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>半人前の恋人</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>川田大智</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>第46話</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>異世界のんびり農家</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>第300話</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>六志麻あさ 業務用餅 kisui</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>第６６話</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>転生してあらゆるモノに好かれながら異世界で好きな事をして生きて行く</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>都尾琉(漫画) 御峰。(原作)</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>第25話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>ダウナーお姉さんは遊びたい</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>山鷹景</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>第10話</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>第134話 よくわからないけれどトリップしちゃうみたいです（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>無敵商人の異世界成り上がり物語 ～現代の製品を自在に取り寄せるスキルがあるので異世界では楽勝です～</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>隆原ヒロタ(漫画) 青山有(原作) ぷきゅのすけ(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>第34話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>ギルドを追放された回復術士、実は魔力無限だったので規格外の回復魔法で伝説となる</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>漫画：坂下コウ 原作：霞杏檎</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>第2話(3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>俺堕ちスレイブヒーローコレクション</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>ゆっ栗栖(著者)</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>第10話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>くらいあの子としたいこと</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>碇マナツ(著者)</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>第78話</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>天獄で悪魔がボクを魅惑する</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>銀河味めてお(著者)</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>第33話</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>小林さんちのメイドラゴン</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>クール教信者</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>外伝 前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>お前妹じゃなくて許嫁だったのかよ!?</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>湯猫子(漫画) 未来人A(原作)</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>第27話</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>千年英雄</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>原作/福島航平 作画/中村ゆきひろ</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>8話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>理想のヒモ生活</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>第85話　その2</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>豚のレバーは加熱しろ</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>みなみ(漫画) 逆井卓馬(原作) 遠坂あさぎ(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>第41話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>愚かな天使は悪魔と踊る</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>アズマサワヨシ(著者)</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>第99話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>クマとウサギは友達ではいられない</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>犬好晶</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>第1話</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>修羅幼女の英雄譚～半端者と言われた傭兵、幼女に転生して成り上がる～</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>作画：むらたん 原作：沙城流</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>第6話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>異種族追放コンカフェ</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>佐々木マサヒト(著者)</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>第15話</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>北海道は今日も平和です</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>テンコ</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>第25話</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>ホームセンターごと呼び出された私の大迷宮リノベーション！</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>ばたっち(漫画) 星崎崑(原作) 志田(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>第4話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>最強勇者パーティーは愛が知りたい</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>山田肌襦袢</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>第25話「別れの挨拶はそれぞれでいい」</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>第71話 reinterpretaion</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>勇者パーティから追い出された不遇職【罠士】、ユニークスキル【矢印】で最強になる</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>作画：たつひこ 原作：白石 有希</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>第6話(1)</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add ranking data for 2025-06-24
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -8,6 +8,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="2025-06-23" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="2025-06-24" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -498,22 +499,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>姫様“拷問”の時間です</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>拷問143</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>塔の管理をしてみよう</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第90話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>いとこのこ</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>いぬちく(著者)</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第35話</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>黒幕一家に転生したけど原作無視して独立する</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>空野進 赤村晃人 笠間三四郎 るろお</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第４話　盗賊を撃破して独立する（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>モブ高生の俺でも冒険者になればリア充になれますか？</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>原作：百均 漫画：さぎやまれん キャラクター原案：hai</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第29.5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>窓際編集とバカにされた俺が、双子ＪＫと同居することになった</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>うさおとめ(著者) 茨木野(原作) トモゼロ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第3話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>宇崎ちゃんは遊びたい！</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>丈(著者)</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第124話</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>Fate/kaleid liner プリズマ☆イリヤ ドライ！！</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>ひろやまひろし(著者) ＴＹＰＥ－ＭＯＯＮ(原作)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第76話 前編　双つ星</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>不純な彼女達は懺悔しない</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>ポロロッカ(著者)</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第27話</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>ぽんドロイド！ はまさん</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>はれやまはれぞう(著者)</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第1話</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第70話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>地味子な三葉さんが僕を誘惑する</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>はぶらえる(著者)</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第9話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>ギャルゲーマーに褒められたい</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>げしゅまろ(著者)</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>30話</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>男子高校生だけどギャルにTSしました</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>太陽まりい(著者)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第17話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>「才能の器」で目指す迷宮最深部 スキル横伸ばしのはずが、万能チートだった!</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>漫画：かくばやしつよし 原作：とんび キャラクター原案： りりんら</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第38話</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>理想の彼女</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>もりまりも(著者)</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第21話</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>アラサーがVTuberになった話。</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>犬威赤彦(漫画) とくめい(原作) カラスBTK(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第21話</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>きみの願いが叶うまで</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>浅月のりと(著者)</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第2話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>彼女にしたい女子一位、の隣で見つけたあまりちゃん</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>寝巻ネルゾ(漫画) 裕時悠示(原作) たん旦(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>休載イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>規格外のダンジョン攻略者、実は異世界帰りの元勇者</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>作画：やまざき君 原作：榊与一</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第3話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>アースウィズダンジョン ～固有スキル≪等価交換ストア≫を駆使して世界救済を目指します～</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>原作：バッド 漫画：高遠けい キャラクター原案：揚 茄子央</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第8話</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>番外編四コマ！</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>ろぐあうと！</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>人参(著者)</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>読切</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>魔都精兵のスレイブ</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>原作:タカヒロ　漫画:竹村洋平</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第155話　大極</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>ソードアート・オンライン Re:Aincrad</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>樹深(作画) 佐藤ミト(構成) 川原礫(原作) ａｂｅｃ(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第39話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>半人前の恋人</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>川田大智</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第46話</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>異世界のんびり農家</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第300話</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>六志麻あさ 業務用餅 kisui</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第６６話</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>転生してあらゆるモノに好かれながら異世界で好きな事をして生きて行く</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>都尾琉(漫画) 御峰。(原作)</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第25話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>ダウナーお姉さんは遊びたい</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>山鷹景</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第10話</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第134話 よくわからないけれどトリップしちゃうみたいです（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>無敵商人の異世界成り上がり物語 ～現代の製品を自在に取り寄せるスキルがあるので異世界では楽勝です～</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>隆原ヒロタ(漫画) 青山有(原作) ぷきゅのすけ(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第34話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>ギルドを追放された回復術士、実は魔力無限だったので規格外の回復魔法で伝説となる</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>漫画：坂下コウ 原作：霞杏檎</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第2話(3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>俺堕ちスレイブヒーローコレクション</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>ゆっ栗栖(著者)</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第10話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>くらいあの子としたいこと</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>碇マナツ(著者)</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第78話</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>天獄で悪魔がボクを魅惑する</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>銀河味めてお(著者)</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第33話</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>小林さんちのメイドラゴン</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>クール教信者</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>外伝 前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>お前妹じゃなくて許嫁だったのかよ!?</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>湯猫子(漫画) 未来人A(原作)</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第27話</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>千年英雄</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>原作/福島航平 作画/中村ゆきひろ</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>8話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>理想のヒモ生活</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第85話　その2</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>豚のレバーは加熱しろ</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>みなみ(漫画) 逆井卓馬(原作) 遠坂あさぎ(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第41話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>愚かな天使は悪魔と踊る</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>アズマサワヨシ(著者)</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第99話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>クマとウサギは友達ではいられない</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>犬好晶</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第1話</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>修羅幼女の英雄譚～半端者と言われた傭兵、幼女に転生して成り上がる～</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>作画：むらたん 原作：沙城流</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第6話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>異種族追放コンカフェ</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>佐々木マサヒト(著者)</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第15話</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>北海道は今日も平和です</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>テンコ</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第25話</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>ホームセンターごと呼び出された私の大迷宮リノベーション！</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>ばたっち(漫画) 星崎崑(原作) 志田(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第4話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>最強勇者パーティーは愛が知りたい</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>山田肌襦袢</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第25話「別れの挨拶はそれぞれでいい」</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第71話 reinterpretaion</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティから追い出された不遇職【罠士】、ユニークスキル【矢印】で最強になる</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>作画：たつひこ 原作：白石 有希</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第6話(1)</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>姫様“拷問”の時間です</t>
+          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>拷問143</t>
+          <t>第68話</t>
         </is>
       </c>
     </row>
@@ -523,17 +1565,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>塔の管理をしてみよう</t>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第90話前編</t>
+          <t>第４９話　全脳力を駆使する器用貧乏（４）</t>
         </is>
       </c>
     </row>
@@ -543,17 +1585,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>いとこのこ</t>
+          <t>転生貴族の異世界冒険録 ～自重を知らない神々の使徒～</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>いぬちく(著者)</t>
+          <t>夜州 nini 藻</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第35話</t>
+          <t>第68話</t>
         </is>
       </c>
     </row>
@@ -563,17 +1605,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>黒幕一家に転生したけど原作無視して独立する</t>
+          <t>「おかえり、パパ」</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>空野進 赤村晃人 笠間三四郎 るろお</t>
+          <t>蝉丸</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第４話　盗賊を撃破して独立する（２）</t>
+          <t>単行本4巻限定描きおろし「羽化」試し読み</t>
         </is>
       </c>
     </row>
@@ -583,17 +1625,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>モブ高生の俺でも冒険者になればリア充になれますか？</t>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>原作：百均 漫画：さぎやまれん キャラクター原案：hai</t>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第29.5話</t>
+          <t>第47話 魔導具師とつながれたもの①</t>
         </is>
       </c>
     </row>
@@ -603,17 +1645,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>窓際編集とバカにされた俺が、双子ＪＫと同居することになった</t>
+          <t>氷結令嬢さまをフォローしたら、メチャメチャ溺愛されてしまった件@comic</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>うさおとめ(著者) 茨木野(原作) トモゼロ(キャラクター原案)</t>
+          <t>漫画：ハレノチアメ 原作：愛坂タカト キャラクター原案：Bcoca</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第3話②</t>
+          <t>1巻表紙イラスト案大公開！</t>
         </is>
       </c>
     </row>
@@ -623,17 +1665,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>宇崎ちゃんは遊びたい！</t>
+          <t>回復術士のやり直し</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>丈(著者)</t>
+          <t>月夜涙(原作) 羽賀ソウケン(漫画) しおこんぶ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第124話</t>
+          <t>第71話-2</t>
         </is>
       </c>
     </row>
@@ -643,17 +1685,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Fate/kaleid liner プリズマ☆イリヤ ドライ！！</t>
+          <t>賢者の孫</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ひろやまひろし(著者) ＴＹＰＥ－ＭＯＯＮ(原作)</t>
+          <t>緒方俊輔(漫画) 吉岡剛(原作) 菊池政治(キャラクター原案)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第76話 前編　双つ星</t>
+          <t>第94話-1</t>
         </is>
       </c>
     </row>
@@ -663,17 +1705,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>不純な彼女達は懺悔しない</t>
+          <t>大学入学時から噂されていた美少女三姉妹、生き別れていた義妹だった。</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>ポロロッカ(著者)</t>
+          <t>こすずめ(著者) 夏乃実(原作) ポメ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第27話</t>
+          <t>第8話②</t>
         </is>
       </c>
     </row>
@@ -683,17 +1725,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ぽんドロイド！ はまさん</t>
+          <t>異世界のすみっこで快適ものづくり生活 ～女神さまのくれた工房はちょっとやりすぎ性能だった～</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>はれやまはれぞう(著者)</t>
+          <t>西山アラタ(漫画) 長田信織(原作) 東上文(キャラクター原案)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第1話</t>
+          <t>EP.18②</t>
         </is>
       </c>
     </row>
@@ -703,17 +1745,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>リビルドワールド</t>
+          <t>レベル１だけどユニークスキルで最強です</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+          <t>漫画：真綿 原作：三木なずな キャラクター原案：すばち</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第70話②</t>
+          <t>第７１話 ダンジョンの精霊との遭遇！？（２）</t>
         </is>
       </c>
     </row>
@@ -723,17 +1765,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>地味子な三葉さんが僕を誘惑する</t>
+          <t>北海道の現役ハンターが異世界に放り込まれてみた 〜エルフ嫁と巡る異世界狩猟ライフ〜</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>はぶらえる(著者)</t>
+          <t>原作：ジュピタースタジオ「北海道の現役ハンターが異世界に放り込まれてみた」（小学館「ガガガブックス」刊） 漫画：カルトマ キャラクター原案：夕薙</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第9話後半</t>
+          <t>第25話②</t>
         </is>
       </c>
     </row>
@@ -743,17 +1785,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ギャルゲーマーに褒められたい</t>
+          <t>めっちゃ召喚された件 THE COMIC</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>げしゅまろ(著者)</t>
+          <t>漫画：六甲島カモメ 原作：さいとうさ キャラクター原案：ツグトク</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>30話</t>
+          <t>番外編10</t>
         </is>
       </c>
     </row>
@@ -763,17 +1805,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>男子高校生だけどギャルにTSしました</t>
+          <t>姫騎士は蛮族の嫁</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>太陽まりい(著者)</t>
+          <t>コトバノリアキ</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第17話後編</t>
+          <t>第51話②	昵懇は昔日の回顧</t>
         </is>
       </c>
     </row>
@@ -783,17 +1825,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>「才能の器」で目指す迷宮最深部 スキル横伸ばしのはずが、万能チートだった!</t>
+          <t>外れスキル『レベルアップ』のせいでパーティーを追放された少年は、レベルを上げて物理で殴る</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>漫画：かくばやしつよし 原作：とんび キャラクター原案： りりんら</t>
+          <t>しんこせい 大橋ウルオ てんまそ</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第38話</t>
+          <t>第17話　後（後編）</t>
         </is>
       </c>
     </row>
@@ -803,17 +1845,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>理想の彼女</t>
+          <t>無能と呼ばれた『精霊たらし』～実は異能で、精霊界では伝説的ヒーローでした～＠COMIC</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>もりまりも(著者)</t>
+          <t>原作：佐藤謙羊 漫画：タバタグランドキャニオン</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第21話</t>
+          <t>第26話③「雪の女王、俺を溺愛」</t>
         </is>
       </c>
     </row>
@@ -823,17 +1865,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>アラサーがVTuberになった話。</t>
+          <t>骨ドラゴンのマナ娘</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>犬威赤彦(漫画) とくめい(原作) カラスBTK(キャラクター原案)</t>
+          <t>雪白いち</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第21話</t>
+          <t>第38話①「祖先から継いだもの」</t>
         </is>
       </c>
     </row>
@@ -843,17 +1885,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>きみの願いが叶うまで</t>
+          <t>人外姫様、始めました　-Free Life Fantasy Online-</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>浅月のりと(著者)</t>
+          <t>園原アオ 割田コマ 子日あきすず Sherry</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第2話-2</t>
+          <t>第５９話　再チャレンジと思ったら、まさかの冥府へ！（１）</t>
         </is>
       </c>
     </row>
@@ -863,17 +1905,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>彼女にしたい女子一位、の隣で見つけたあまりちゃん</t>
+          <t>国王である兄から辺境に追放されたけど平穏に暮らしたい ～目指せスローライフ～</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>寝巻ネルゾ(漫画) 裕時悠示(原作) たん旦(キャラクター原案)</t>
+          <t>おとら(原作) 西沢秀二(漫画) 夜ノみつき(キャラクター原案)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>休載イラスト</t>
+          <t>第10話-2</t>
         </is>
       </c>
     </row>
@@ -883,17 +1925,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>規格外のダンジョン攻略者、実は異世界帰りの元勇者</t>
+          <t>創造錬金術師は自由を謳歌する 故郷を追放されたら、魔王のお膝元で超絶効果のマジックアイテム作り放題になりました</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>作画：やまざき君 原作：榊与一</t>
+          <t>姫乃タカ(漫画) 千月さかき(原作) かぼちゃ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第3話(1)</t>
+          <t>第19話-1</t>
         </is>
       </c>
     </row>
@@ -903,17 +1945,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>アースウィズダンジョン ～固有スキル≪等価交換ストア≫を駆使して世界救済を目指します～</t>
+          <t>迷宮メトロ ～目覚めたら最強職だったのでシマリスを連れて新世界を歩く～</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>原作：バッド 漫画：高遠けい キャラクター原案：揚 茄子央</t>
+          <t>漫画：高瀬若弥 原作：佐々木ラスト キャラクター原案：かわすみ</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第8話</t>
+          <t>第44話</t>
         </is>
       </c>
     </row>
@@ -923,17 +1965,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+          <t>器用貧乏、城を建てる～開拓学園の劣等生なのに、 上級職のスキルと魔法がすべて使えます～＠COMIC</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+          <t>原作：佐藤謙羊 漫画：スガン</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>番外編四コマ！</t>
+          <t>第21話①「ルールの代償」</t>
         </is>
       </c>
     </row>
@@ -943,17 +1985,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ろぐあうと！</t>
+          <t>暴食のベルセルク～俺だけレベルという概念を突破する～</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>人参(著者)</t>
+          <t>漫画：滝乃大祐 原作：一色一凛 キャラクター原案：fame</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>読切</t>
+          <t>第72話後半</t>
         </is>
       </c>
     </row>
@@ -963,17 +2005,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>魔都精兵のスレイブ</t>
+          <t>尾守つみきと奇日常。</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>原作:タカヒロ　漫画:竹村洋平</t>
+          <t>森下みゆ</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第155話　大極</t>
+          <t>第56話 雷漸会長とレンジ。</t>
         </is>
       </c>
     </row>
@@ -983,17 +2025,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ソードアート・オンライン Re:Aincrad</t>
+          <t>転生少女はまず一歩からはじめたい～魔物がいるとか聞いてない！～</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>樹深(作画) 佐藤ミト(構成) 川原礫(原作) ａｂｅｃ(キャラクターデザイン)</t>
+          <t>原作：カヤ 漫画：岡村アユム キャラクター原案：那流</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第39話②</t>
+          <t>第36話 ご領主登場②</t>
         </is>
       </c>
     </row>
@@ -1003,17 +2045,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>半人前の恋人</t>
+          <t>拝啓…殺し屋さんと結婚しました</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>川田大智</t>
+          <t>高坂曇天(著者)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第46話</t>
+          <t>第64話</t>
         </is>
       </c>
     </row>
@@ -1023,17 +2065,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>異世界のんびり農家</t>
+          <t>魔眼の悪役に転生したので推しキャラを見守るモブを目指します</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+          <t>在間りしん(漫画) 瀧岡くるじ(原作) 福きつね(キャラクター原案)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第300話</t>
+          <t>第10話①</t>
         </is>
       </c>
     </row>
@@ -1043,17 +2085,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
+          <t>クラス最安値で売られた俺は、実は最強パラメーター</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>六志麻あさ 業務用餅 kisui</t>
+          <t>カンブリア爆発太郎(漫画) RYOMA(原作) 黒井ススム(キャラクター原案)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第６６話</t>
+          <t>第35話-1</t>
         </is>
       </c>
     </row>
@@ -1063,17 +2105,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>転生してあらゆるモノに好かれながら異世界で好きな事をして生きて行く</t>
+          <t>宇崎ちゃんは遊びたい！</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>都尾琉(漫画) 御峰。(原作)</t>
+          <t>丈(著者)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第25話③</t>
+          <t>第124話</t>
         </is>
       </c>
     </row>
@@ -1083,17 +2125,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ダウナーお姉さんは遊びたい</t>
+          <t>いとこのこ</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>山鷹景</t>
+          <t>いぬちく(著者)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第10話</t>
+          <t>第35話</t>
         </is>
       </c>
     </row>
@@ -1103,17 +2145,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>よくわからないけれど異世界に転生していたようです</t>
+          <t>ネタキャラ転生とかあんまりだ！ THE COMIC</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>内々けやき あし カオミン</t>
+          <t>漫画：あまねかむらぎ 原作：音無奏 キャラクター原案：azuタロウ</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第134話 よくわからないけれどトリップしちゃうみたいです（２）</t>
+          <t>第30話①</t>
         </is>
       </c>
     </row>
@@ -1123,17 +2165,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>無敵商人の異世界成り上がり物語 ～現代の製品を自在に取り寄せるスキルがあるので異世界では楽勝です～</t>
+          <t>特殊性癖教室へようこそ</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>隆原ヒロタ(漫画) 青山有(原作) ぷきゅのすけ(キャラクターデザイン)</t>
+          <t>紫苑寺七瀬(原作) 能呂やすとき(漫画) 魔太郎(キャラクター原案)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第34話②</t>
+          <t>12限目-3</t>
         </is>
       </c>
     </row>
@@ -1143,17 +2185,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ギルドを追放された回復術士、実は魔力無限だったので規格外の回復魔法で伝説となる</t>
+          <t>姫様“拷問”の時間です</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>漫画：坂下コウ 原作：霞杏檎</t>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第2話(3)</t>
+          <t>拷問143</t>
         </is>
       </c>
     </row>
@@ -1163,17 +2205,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>俺堕ちスレイブヒーローコレクション</t>
+          <t>ぽんドロイド！ はまさん</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>ゆっ栗栖(著者)</t>
+          <t>はれやまはれぞう(著者)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第10話前半</t>
+          <t>第1話</t>
         </is>
       </c>
     </row>
@@ -1183,17 +2225,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>くらいあの子としたいこと</t>
+          <t>SSSランクダンジョンでナイフ一本手渡され追放された白魔導師 ユグドラシルの呪いにより弱点である魔力不足を克服し世界最強へと至る</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>碇マナツ(著者)</t>
+          <t>上下瑞樹(漫画) カミトイチ(原作) 眠介(キャラクター原案)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第78話</t>
+          <t>第22話-1</t>
         </is>
       </c>
     </row>
@@ -1203,17 +2245,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>天獄で悪魔がボクを魅惑する</t>
+          <t>女神から『孵化』のスキルを授かった俺が、なぜか幻獣や神獣を従える最強テイマーになるまで</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>銀河味めてお(著者)</t>
+          <t>漫画家：春夏冬 唯人 原作：まるせい</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第33話</t>
+          <t>第14話</t>
         </is>
       </c>
     </row>
@@ -1223,17 +2265,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>小林さんちのメイドラゴン</t>
+          <t>異世界のんびり開拓記  -平凡サラリーマン、万能自在のビルド&amp;クラフトスキルで、気ままなスローライフ 開拓始めます! -</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>クール教信者</t>
+          <t>漫画：しょうじひでまさ 原作：タライ和治 キャラクター原案：イシバシヨウスケ</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>外伝 前編</t>
+          <t>第22話 前編</t>
         </is>
       </c>
     </row>
@@ -1243,17 +2285,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>お前妹じゃなくて許嫁だったのかよ!?</t>
+          <t>黒幕一家に転生したけど原作無視して独立する</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>湯猫子(漫画) 未来人A(原作)</t>
+          <t>空野進 赤村晃人 笠間三四郎 るろお</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第27話</t>
+          <t>第４話　盗賊を撃破して独立する（２）</t>
         </is>
       </c>
     </row>
@@ -1263,17 +2305,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>千年英雄</t>
+          <t>忌み子と呼ばれた召喚士@COMIC</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>原作/福島航平 作画/中村ゆきひろ</t>
+          <t>漫画：コイシ 原作：緑黄色野菜 キャラクター原案：こよいみつき</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>8話②</t>
+          <t>第40話 ①</t>
         </is>
       </c>
     </row>
@@ -1283,17 +2325,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>理想のヒモ生活</t>
+          <t>アラフォーおっさんはスローライフの夢を見るか？</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+          <t>漫画：大関詠詞 原作：サイトウアユム キャラクター原案： ジョンディー</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第85話　その2</t>
+          <t>第13話</t>
         </is>
       </c>
     </row>
@@ -1303,17 +2345,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>豚のレバーは加熱しろ</t>
+          <t>塔の管理をしてみよう</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>みなみ(漫画) 逆井卓馬(原作) 遠坂あさぎ(キャラクターデザイン)</t>
+          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第41話①</t>
+          <t>第90話前編</t>
         </is>
       </c>
     </row>
@@ -1323,17 +2365,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>愚かな天使は悪魔と踊る</t>
+          <t>貰った三つの外れスキル、合わせたら最強でした</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>アズマサワヨシ(著者)</t>
+          <t>漫画：七谷八尋 原作：雪ノ狐 キャラクター原案：増田幹生</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第99話②</t>
+          <t>第10話</t>
         </is>
       </c>
     </row>
@@ -1343,17 +2385,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>クマとウサギは友達ではいられない</t>
+          <t>不純な彼女達は懺悔しない</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>犬好晶</t>
+          <t>ポロロッカ(著者)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第1話</t>
+          <t>第27話</t>
         </is>
       </c>
     </row>
@@ -1363,17 +2405,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>修羅幼女の英雄譚～半端者と言われた傭兵、幼女に転生して成り上がる～</t>
+          <t>アラサーがVTuberになった話。</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>作画：むらたん 原作：沙城流</t>
+          <t>犬威赤彦(漫画) とくめい(原作) カラスBTK(キャラクター原案)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第6話(1)</t>
+          <t>第21話</t>
         </is>
       </c>
     </row>
@@ -1383,17 +2425,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>異種族追放コンカフェ</t>
+          <t>人生逆転ダンジョン</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>佐々木マサヒト(著者)</t>
+          <t>尾張 ニコ どすこい花丸様</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第15話</t>
+          <t>第2-2話	魔力発散</t>
         </is>
       </c>
     </row>
@@ -1403,17 +2445,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>北海道は今日も平和です</t>
+          <t>異世界で最強のスキルを生み出せたので、ひたすら無双することにしました。　～俺だけがスキルの数値を勝手に操作～</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>テンコ</t>
+          <t>漫画：星トマジロウ 原作：ヒゲ抜き地蔵 キャラクター原案：山椒魚</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第25話</t>
+          <t>第9話 ①</t>
         </is>
       </c>
     </row>
@@ -1423,17 +2465,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>ホームセンターごと呼び出された私の大迷宮リノベーション！</t>
+          <t>クソ女に幸あれ</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>ばたっち(漫画) 星崎崑(原作) 志田(キャラクター原案)</t>
+          <t>岸川瑞樹</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第4話前編</t>
+          <t>第57話</t>
         </is>
       </c>
     </row>
@@ -1443,17 +2485,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>最強勇者パーティーは愛が知りたい</t>
+          <t>Fate/kaleid liner プリズマ☆イリヤ ドライ！！</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>山田肌襦袢</t>
+          <t>ひろやまひろし(著者) ＴＹＰＥ－ＭＯＯＮ(原作)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第25話「別れの挨拶はそれぞれでいい」</t>
+          <t>第76話 前編　双つ星</t>
         </is>
       </c>
     </row>
@@ -1463,17 +2505,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
+          <t>終焉の魔女と世界の旅</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
+          <t>片岡とんち</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第71話 reinterpretaion</t>
+          <t>第12話②	終焉の魔女エレナ</t>
         </is>
       </c>
     </row>
@@ -1483,17 +2525,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>勇者パーティから追い出された不遇職【罠士】、ユニークスキル【矢印】で最強になる</t>
+          <t>リビルドワールド</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>作画：たつひこ 原作：白石 有希</t>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第6話(1)</t>
+          <t>第70話②</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-06-25
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -9,6 +9,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="2025-06-23" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="2025-06-24" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="2025-06-25" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -1540,22 +1541,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第68話</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第４９話　全脳力を駆使する器用貧乏（４）</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>転生貴族の異世界冒険録 ～自重を知らない神々の使徒～</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>夜州 nini 藻</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第68話</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>「おかえり、パパ」</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>蝉丸</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>単行本4巻限定描きおろし「羽化」試し読み</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第47話 魔導具師とつながれたもの①</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>氷結令嬢さまをフォローしたら、メチャメチャ溺愛されてしまった件@comic</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>漫画：ハレノチアメ 原作：愛坂タカト キャラクター原案：Bcoca</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>1巻表紙イラスト案大公開！</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>回復術士のやり直し</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>月夜涙(原作) 羽賀ソウケン(漫画) しおこんぶ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第71話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>賢者の孫</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>緒方俊輔(漫画) 吉岡剛(原作) 菊池政治(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第94話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>大学入学時から噂されていた美少女三姉妹、生き別れていた義妹だった。</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>こすずめ(著者) 夏乃実(原作) ポメ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第8話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>異世界のすみっこで快適ものづくり生活 ～女神さまのくれた工房はちょっとやりすぎ性能だった～</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>西山アラタ(漫画) 長田信織(原作) 東上文(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>EP.18②</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>レベル１だけどユニークスキルで最強です</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>漫画：真綿 原作：三木なずな キャラクター原案：すばち</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第７１話 ダンジョンの精霊との遭遇！？（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>北海道の現役ハンターが異世界に放り込まれてみた 〜エルフ嫁と巡る異世界狩猟ライフ〜</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>原作：ジュピタースタジオ「北海道の現役ハンターが異世界に放り込まれてみた」（小学館「ガガガブックス」刊） 漫画：カルトマ キャラクター原案：夕薙</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第25話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>めっちゃ召喚された件 THE COMIC</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>漫画：六甲島カモメ 原作：さいとうさ キャラクター原案：ツグトク</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>番外編10</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>姫騎士は蛮族の嫁</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>コトバノリアキ</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第51話②	昵懇は昔日の回顧</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>外れスキル『レベルアップ』のせいでパーティーを追放された少年は、レベルを上げて物理で殴る</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>しんこせい 大橋ウルオ てんまそ</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第17話　後（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>無能と呼ばれた『精霊たらし』～実は異能で、精霊界では伝説的ヒーローでした～＠COMIC</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>原作：佐藤謙羊 漫画：タバタグランドキャニオン</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第26話③「雪の女王、俺を溺愛」</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>骨ドラゴンのマナ娘</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>雪白いち</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第38話①「祖先から継いだもの」</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>人外姫様、始めました　-Free Life Fantasy Online-</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>園原アオ 割田コマ 子日あきすず Sherry</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第５９話　再チャレンジと思ったら、まさかの冥府へ！（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>国王である兄から辺境に追放されたけど平穏に暮らしたい ～目指せスローライフ～</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>おとら(原作) 西沢秀二(漫画) 夜ノみつき(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第10話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>創造錬金術師は自由を謳歌する 故郷を追放されたら、魔王のお膝元で超絶効果のマジックアイテム作り放題になりました</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>姫乃タカ(漫画) 千月さかき(原作) かぼちゃ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第19話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>迷宮メトロ ～目覚めたら最強職だったのでシマリスを連れて新世界を歩く～</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>漫画：高瀬若弥 原作：佐々木ラスト キャラクター原案：かわすみ</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第44話</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>器用貧乏、城を建てる～開拓学園の劣等生なのに、 上級職のスキルと魔法がすべて使えます～＠COMIC</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>原作：佐藤謙羊 漫画：スガン</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第21話①「ルールの代償」</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>暴食のベルセルク～俺だけレベルという概念を突破する～</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>漫画：滝乃大祐 原作：一色一凛 キャラクター原案：fame</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第72話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>尾守つみきと奇日常。</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>森下みゆ</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第56話 雷漸会長とレンジ。</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>転生少女はまず一歩からはじめたい～魔物がいるとか聞いてない！～</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>原作：カヤ 漫画：岡村アユム キャラクター原案：那流</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第36話 ご領主登場②</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>拝啓…殺し屋さんと結婚しました</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>高坂曇天(著者)</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第64話</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>魔眼の悪役に転生したので推しキャラを見守るモブを目指します</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>在間りしん(漫画) 瀧岡くるじ(原作) 福きつね(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第10話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>クラス最安値で売られた俺は、実は最強パラメーター</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>カンブリア爆発太郎(漫画) RYOMA(原作) 黒井ススム(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第35話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>宇崎ちゃんは遊びたい！</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>丈(著者)</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第124話</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>いとこのこ</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>いぬちく(著者)</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第35話</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>ネタキャラ転生とかあんまりだ！ THE COMIC</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>漫画：あまねかむらぎ 原作：音無奏 キャラクター原案：azuタロウ</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第30話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>特殊性癖教室へようこそ</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>紫苑寺七瀬(原作) 能呂やすとき(漫画) 魔太郎(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>12限目-3</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>姫様“拷問”の時間です</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>拷問143</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>ぽんドロイド！ はまさん</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>はれやまはれぞう(著者)</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第1話</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>SSSランクダンジョンでナイフ一本手渡され追放された白魔導師 ユグドラシルの呪いにより弱点である魔力不足を克服し世界最強へと至る</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>上下瑞樹(漫画) カミトイチ(原作) 眠介(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第22話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>女神から『孵化』のスキルを授かった俺が、なぜか幻獣や神獣を従える最強テイマーになるまで</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>漫画家：春夏冬 唯人 原作：まるせい</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第14話</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>異世界のんびり開拓記  -平凡サラリーマン、万能自在のビルド&amp;クラフトスキルで、気ままなスローライフ 開拓始めます! -</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>漫画：しょうじひでまさ 原作：タライ和治 キャラクター原案：イシバシヨウスケ</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第22話 前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>黒幕一家に転生したけど原作無視して独立する</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>空野進 赤村晃人 笠間三四郎 るろお</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第４話　盗賊を撃破して独立する（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>忌み子と呼ばれた召喚士@COMIC</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>漫画：コイシ 原作：緑黄色野菜 キャラクター原案：こよいみつき</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第40話 ①</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>アラフォーおっさんはスローライフの夢を見るか？</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>漫画：大関詠詞 原作：サイトウアユム キャラクター原案： ジョンディー</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第13話</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>塔の管理をしてみよう</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第90話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>貰った三つの外れスキル、合わせたら最強でした</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>漫画：七谷八尋 原作：雪ノ狐 キャラクター原案：増田幹生</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第10話</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>不純な彼女達は懺悔しない</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>ポロロッカ(著者)</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第27話</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>アラサーがVTuberになった話。</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>犬威赤彦(漫画) とくめい(原作) カラスBTK(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第21話</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>人生逆転ダンジョン</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>尾張 ニコ どすこい花丸様</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第2-2話	魔力発散</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>異世界で最強のスキルを生み出せたので、ひたすら無双することにしました。　～俺だけがスキルの数値を勝手に操作～</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>漫画：星トマジロウ 原作：ヒゲ抜き地蔵 キャラクター原案：山椒魚</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第9話 ①</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>クソ女に幸あれ</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>岸川瑞樹</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第57話</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>Fate/kaleid liner プリズマ☆イリヤ ドライ！！</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>ひろやまひろし(著者) ＴＹＰＥ－ＭＯＯＮ(原作)</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第76話 前編　双つ星</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>終焉の魔女と世界の旅</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>片岡とんち</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第12話②	終焉の魔女エレナ</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第70話②</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
+          <t>光永康則</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第68話</t>
+          <t>第６６話『重機停止』④</t>
         </is>
       </c>
     </row>
@@ -1565,17 +2607,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+          <t>マツモトケンゴ</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第４９話　全脳力を駆使する器用貧乏（４）</t>
+          <t>第５９話　筋トレの戦いが始まった（１）</t>
         </is>
       </c>
     </row>
@@ -1585,17 +2627,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>転生貴族の異世界冒険録 ～自重を知らない神々の使徒～</t>
+          <t>いとこのこ</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>夜州 nini 藻</t>
+          <t>いぬちく(著者)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第68話</t>
+          <t>「次にくるマンガ大賞 2025」応援よろしくお願いします！</t>
         </is>
       </c>
     </row>
@@ -1605,17 +2647,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>「おかえり、パパ」</t>
+          <t>剥かせて！竜ケ崎さん</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>蝉丸</t>
+          <t>一智和智</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>単行本4巻限定描きおろし「羽化」試し読み</t>
+          <t>大学生編 第12話</t>
         </is>
       </c>
     </row>
@@ -1625,17 +2667,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
+          <t>戸賀 環 坂木持丸 riritto</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第47話 魔導具師とつながれたもの①</t>
+          <t>第48話①　お祭りを楽しんでみた</t>
         </is>
       </c>
     </row>
@@ -1645,17 +2687,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>氷結令嬢さまをフォローしたら、メチャメチャ溺愛されてしまった件@comic</t>
+          <t>骸骨騎士様、只今異世界へお出掛け中</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>漫画：ハレノチアメ 原作：愛坂タカト キャラクター原案：Bcoca</t>
+          <t>サワノアキラ（漫画） 秤猿鬼（原作） KeG（キャラクター原案）</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1巻表紙イラスト案大公開！</t>
+          <t>第64話　エルフ族の決断Ⅲ（後編）</t>
         </is>
       </c>
     </row>
@@ -1665,17 +2707,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>回復術士のやり直し</t>
+          <t>ありふれた職業で世界最強</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>月夜涙(原作) 羽賀ソウケン(漫画) しおこんぶ(キャラクター原案)</t>
+          <t>RoGa（漫画） 白米 良（原作） たかやKi（キャラクター原案）</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第71話-2</t>
+          <t>第83話　新しい私の身体</t>
         </is>
       </c>
     </row>
@@ -1685,17 +2727,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>賢者の孫</t>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>緒方俊輔(漫画) 吉岡剛(原作) 菊池政治(キャラクター原案)</t>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第94話-1</t>
+          <t>祝！ 連載10周年『異世界魔王』人気ヒロイン総選挙</t>
         </is>
       </c>
     </row>
@@ -1705,17 +2747,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>大学入学時から噂されていた美少女三姉妹、生き別れていた義妹だった。</t>
+          <t>絶対死なないステラ姫</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>こすずめ(著者) 夏乃実(原作) ポメ(キャラクター原案)</t>
+          <t>光永康則 大高稲</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第8話②</t>
+          <t>第１３話　絶対巣穴に入らない・解（３）</t>
         </is>
       </c>
     </row>
@@ -1725,17 +2767,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>異世界のすみっこで快適ものづくり生活 ～女神さまのくれた工房はちょっとやりすぎ性能だった～</t>
+          <t>ラスボス討伐後に始める二周目冒険者ライフ はじまりの街でワケあり美少女たちがめちゃくちゃ懐いてきます</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>西山アラタ(漫画) 長田信織(原作) 東上文(キャラクター原案)</t>
+          <t>鬼麻正明(漫画) 朱月十話(原作) ファルまろ(キャラ原案)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>EP.18②</t>
+          <t>第3話-2</t>
         </is>
       </c>
     </row>
@@ -1745,17 +2787,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>レベル１だけどユニークスキルで最強です</t>
+          <t>ひとりぼっちの異世界攻略</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>漫画：真綿 原作：三木なずな キャラクター原案：すばち</t>
+          <t>びび（漫画） 五示正司（原作）</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第７１話 ダンジョンの精霊との遭遇！？（２）</t>
+          <t>第224話　あくまで情報交換なんだよ？</t>
         </is>
       </c>
     </row>
@@ -1765,17 +2807,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>北海道の現役ハンターが異世界に放り込まれてみた 〜エルフ嫁と巡る異世界狩猟ライフ〜</t>
+          <t>煽り系ゲーム配信者（20歳）、配信の切り忘れによりいい人バレする。</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>原作：ジュピタースタジオ「北海道の現役ハンターが異世界に放り込まれてみた」（小学館「ガガガブックス」刊） 漫画：カルトマ キャラクター原案：夕薙</t>
+          <t>流嘉（漫画） 夏乃実（原作） 麦うさぎ（キャラクター原案）</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第25話②</t>
+          <t>第3話　切り抜き動画（後編）</t>
         </is>
       </c>
     </row>
@@ -1785,17 +2827,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>めっちゃ召喚された件 THE COMIC</t>
+          <t>ダウナー系お姉さんに毎日カスの嘘を流し込まれる話</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>漫画：六甲島カモメ 原作：さいとうさ キャラクター原案：ツグトク</t>
+          <t>生倉のゑる(著者) はるばーど屋(原作者)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>番外編10</t>
+          <t>第10話</t>
         </is>
       </c>
     </row>
@@ -1805,17 +2847,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>姫騎士は蛮族の嫁</t>
+          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>コトバノリアキ</t>
+          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第51話②	昵懇は昔日の回顧</t>
+          <t>第68話</t>
         </is>
       </c>
     </row>
@@ -1825,17 +2867,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>外れスキル『レベルアップ』のせいでパーティーを追放された少年は、レベルを上げて物理で殴る</t>
+          <t>元最強探索者のおじさん。美少女配信者を助けて大バズりしてしまった。</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>しんこせい 大橋ウルオ てんまそ</t>
+          <t>かなたろー(原作) 草壁レイ(漫画)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第17話　後（後編）</t>
+          <t>第3話　美少女、おじさんにハメられる。①</t>
         </is>
       </c>
     </row>
@@ -1845,17 +2887,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>無能と呼ばれた『精霊たらし』～実は異能で、精霊界では伝説的ヒーローでした～＠COMIC</t>
+          <t>ある日、惰眠を貪っていたら一族から追放されて森に捨てられました そのまま寝てたら周りが勝手に魔物の国を作ってたけど、私は気にせず今日も眠ります　コミック版</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>原作：佐藤謙羊 漫画：タバタグランドキャニオン</t>
+          <t>漫画/伊草さゆ 原作/白波ハクア キャラクター原案/まさよ</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第26話③「雪の女王、俺を溺愛」</t>
+          <t>chapter50【26話②】</t>
         </is>
       </c>
     </row>
@@ -1865,17 +2907,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>骨ドラゴンのマナ娘</t>
+          <t>無慈悲な悪役貴族に転生した僕は掌握魔法を駆使して魔法世界の頂点に立つ 〜ヒロインなんていないと諦めていたら向こうから勝手に寄ってきました〜</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>雪白いち</t>
+          <t>坂井オイ(漫画) びゃくし(原作) ファルまろ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第38話①「祖先から継いだもの」</t>
+          <t>第5話-2</t>
         </is>
       </c>
     </row>
@@ -1885,17 +2927,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>人外姫様、始めました　-Free Life Fantasy Online-</t>
+          <t>江戸前エルフ</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>園原アオ 割田コマ 子日あきすず Sherry</t>
+          <t>樋口彰彦</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第５９話　再チャレンジと思ったら、まさかの冥府へ！（１）</t>
+          <t>#111</t>
         </is>
       </c>
     </row>
@@ -1905,17 +2947,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>国王である兄から辺境に追放されたけど平穏に暮らしたい ～目指せスローライフ～</t>
+          <t>聖女に嘘は通じない</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>おとら(原作) 西沢秀二(漫画) 夜ノみつき(キャラクター原案)</t>
+          <t>日向 夏 浅見よう しんいし智歩</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第10話-2</t>
+          <t>第24話②　もったいない</t>
         </is>
       </c>
     </row>
@@ -1925,17 +2967,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>創造錬金術師は自由を謳歌する 故郷を追放されたら、魔王のお膝元で超絶効果のマジックアイテム作り放題になりました</t>
+          <t>序盤で死ぬ最強のサブキャラに転生したので、ゲーム知識で無双する</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>姫乃タカ(漫画) 千月さかき(原作) かぼちゃ(キャラクター原案)</t>
+          <t>作画：マエD 原作：新人</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第19話-1</t>
+          <t>第4話(1)</t>
         </is>
       </c>
     </row>
@@ -1945,17 +2987,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>迷宮メトロ ～目覚めたら最強職だったのでシマリスを連れて新世界を歩く～</t>
+          <t>一生働きたくない俺が、クラスメイトの大人気アイドルに懐かれたら</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>漫画：高瀬若弥 原作：佐々木ラスト キャラクター原案：かわすみ</t>
+          <t>三崎弓（漫画） 岸本和葉（原作） みわべさくら（キャラクター原案）</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第44話</t>
+          <t>第19話　水族館デート②</t>
         </is>
       </c>
     </row>
@@ -1965,17 +3007,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>器用貧乏、城を建てる～開拓学園の劣等生なのに、 上級職のスキルと魔法がすべて使えます～＠COMIC</t>
+          <t>勇者パーティを追放された【スキルサポーター】、仲間のスキルを解放して最強に成り上がる</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>原作：佐藤謙羊 漫画：スガン</t>
+          <t>作画：なかお 原作：前田氏</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第21話①「ルールの代償」</t>
+          <t>第4話(3)</t>
         </is>
       </c>
     </row>
@@ -1985,17 +3027,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>暴食のベルセルク～俺だけレベルという概念を突破する～</t>
+          <t>みだりに憑かせてはなりません</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>漫画：滝乃大祐 原作：一色一凛 キャラクター原案：fame</t>
+          <t>栗田あぐり(著者)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第72話後半</t>
+          <t>第7話②</t>
         </is>
       </c>
     </row>
@@ -2005,17 +3047,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>尾守つみきと奇日常。</t>
+          <t>最強の少年聖騎士、転生者を狩る</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>森下みゆ</t>
+          <t>作画：御塩 原作：宇奈木ユラ</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第56話 雷漸会長とレンジ。</t>
+          <t>第4話(3)</t>
         </is>
       </c>
     </row>
@@ -2025,17 +3067,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>転生少女はまず一歩からはじめたい～魔物がいるとか聞いてない！～</t>
+          <t>傭兵団の料理番</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>原作：カヤ 漫画：岡村アユム キャラクター原案：那流</t>
+          <t>梅木泰祐(漫画) 川井昂(原作) 四季童子(キャラクター原案)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第36話 ご領主登場②</t>
+          <t>第9話-1</t>
         </is>
       </c>
     </row>
@@ -2045,17 +3087,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>拝啓…殺し屋さんと結婚しました</t>
+          <t>「おかえり、パパ」</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>高坂曇天(著者)</t>
+          <t>蝉丸</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第64話</t>
+          <t>単行本4巻限定描きおろし「羽化」試し読み</t>
         </is>
       </c>
     </row>
@@ -2065,17 +3107,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>魔眼の悪役に転生したので推しキャラを見守るモブを目指します</t>
+          <t>悪役一家の奥方、死に戻りして心を入れ替える。</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>在間りしん(漫画) 瀧岡くるじ(原作) 福きつね(キャラクター原案)</t>
+          <t>鏡(漫画) 丘野優(原作) TEDDY(キャラクター原案)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第10話①</t>
+          <t>第31話①</t>
         </is>
       </c>
     </row>
@@ -2085,17 +3127,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>クラス最安値で売られた俺は、実は最強パラメーター</t>
+          <t>初歩魔法しか使わない謎の老魔法使いが旅をする</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>カンブリア爆発太郎(漫画) RYOMA(原作) 黒井ススム(キャラクター原案)</t>
+          <t>山代カゲツ(漫画) やまだのぼる(原作) にじまあるく(キャラクター原案)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第35話-1</t>
+          <t>第4話②</t>
         </is>
       </c>
     </row>
@@ -2105,17 +3147,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>宇崎ちゃんは遊びたい！</t>
+          <t>ラーメン大好き小泉さん</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>丈(著者)</t>
+          <t>鳴見なる</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第124話</t>
+          <t>13杯目 ようしょくてん</t>
         </is>
       </c>
     </row>
@@ -2125,17 +3167,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>いとこのこ</t>
+          <t>ゲーム　オブ　ファミリア-家族戦記-</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>いぬちく(著者)</t>
+          <t>Ｄ．Ｐ(作画) 山口ミコト(原作)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第35話</t>
+          <t>第72話④</t>
         </is>
       </c>
     </row>
@@ -2145,17 +3187,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ネタキャラ転生とかあんまりだ！ THE COMIC</t>
+          <t>亡びの国の征服者～魔王は世界を征服するようです～</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>漫画：あまねかむらぎ 原作：音無奏 キャラクター原案：azuタロウ</t>
+          <t>錆狗村昌（漫画） 不手折家（原作） toi8（キャラクター原案）</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第30話①</t>
+          <t>第30話　希望への出航（後編）</t>
         </is>
       </c>
     </row>
@@ -2165,17 +3207,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>特殊性癖教室へようこそ</t>
+          <t>二周目チートの転生魔導士～最強が1000年後に転生したら、人生余裕すぎました～</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>紫苑寺七瀬(原作) 能呂やすとき(漫画) 魔太郎(キャラクター原案)</t>
+          <t>石後千鳥 鬱沢色素 りいちゅ</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>12限目-3</t>
+          <t>第31話　合同授業（中編）</t>
         </is>
       </c>
     </row>
@@ -2185,17 +3227,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>姫様“拷問”の時間です</t>
+          <t>ギャルゲーマーに褒められたい</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+          <t>げしゅまろ(著者)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>拷問143</t>
+          <t>31話</t>
         </is>
       </c>
     </row>
@@ -2205,17 +3247,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ぽんドロイド！ はまさん</t>
+          <t>追放されたダンジョン配信者、《マッピング》スキルで最強パーティーを目指します</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>はれやまはれぞう(著者)</t>
+          <t>作画：入逢夕 原作：瀬戸夏樹</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第1話</t>
+          <t>第4話(3)</t>
         </is>
       </c>
     </row>
@@ -2225,17 +3267,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>SSSランクダンジョンでナイフ一本手渡され追放された白魔導師 ユグドラシルの呪いにより弱点である魔力不足を克服し世界最強へと至る</t>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>上下瑞樹(漫画) カミトイチ(原作) 眠介(キャラクター原案)</t>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第22話-1</t>
+          <t>第４９話　全脳力を駆使する器用貧乏（４）</t>
         </is>
       </c>
     </row>
@@ -2245,17 +3287,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>女神から『孵化』のスキルを授かった俺が、なぜか幻獣や神獣を従える最強テイマーになるまで</t>
+          <t>転生したら没落貴族だったので、【呪言】を極めて家族を救います</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>漫画家：春夏冬 唯人 原作：まるせい</t>
+          <t>作画：アマセケイ 原作：メソポ・たみあ</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第14話</t>
+          <t>第4話(3)</t>
         </is>
       </c>
     </row>
@@ -2265,17 +3307,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>異世界のんびり開拓記  -平凡サラリーマン、万能自在のビルド&amp;クラフトスキルで、気ままなスローライフ 開拓始めます! -</t>
+          <t>ちゃんと吸えない吸血鬼ちゃん</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>漫画：しょうじひでまさ 原作：タライ和治 キャラクター原案：イシバシヨウスケ</t>
+          <t>二式恭介(著者)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第22話 前編</t>
+          <t>第99話：吸血鬼ちゃんのおまもり③</t>
         </is>
       </c>
     </row>
@@ -2285,17 +3327,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>黒幕一家に転生したけど原作無視して独立する</t>
+          <t>豚貴族は未来を切り開くようです</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>空野進 赤村晃人 笠間三四郎 るろお</t>
+          <t>大出リコ（漫画） しんこせい（原作） riritto（原作イラスト）</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第４話　盗賊を撃破して独立する（２）</t>
+          <t>第10話　旅立ち（後編）</t>
         </is>
       </c>
     </row>
@@ -2305,17 +3347,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>忌み子と呼ばれた召喚士@COMIC</t>
+          <t>転生貴族の異世界冒険録 ～自重を知らない神々の使徒～</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>漫画：コイシ 原作：緑黄色野菜 キャラクター原案：こよいみつき</t>
+          <t>夜州 nini 藻</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第40話 ①</t>
+          <t>第68話</t>
         </is>
       </c>
     </row>
@@ -2325,17 +3367,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>アラフォーおっさんはスローライフの夢を見るか？</t>
+          <t>アラサーがVTuberになった話。</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>漫画：大関詠詞 原作：サイトウアユム キャラクター原案： ジョンディー</t>
+          <t>犬威赤彦(漫画) とくめい(原作) カラスBTK(キャラクター原案)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第13話</t>
+          <t>第21話</t>
         </is>
       </c>
     </row>
@@ -2345,17 +3387,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>塔の管理をしてみよう</t>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第90話前編</t>
+          <t>第47話 魔導具師とつながれたもの①</t>
         </is>
       </c>
     </row>
@@ -2365,17 +3407,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>貰った三つの外れスキル、合わせたら最強でした</t>
+          <t>二度追放された冒険者、激レアスキル駆使して美少女軍団を育成中！　コミック版</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>漫画：七谷八尋 原作：雪ノ狐 キャラクター原案：増田幹生</t>
+          <t>漫画/青木千尋 原作/南野雪花</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第10話</t>
+          <t>chapter65【33話②】</t>
         </is>
       </c>
     </row>
@@ -2385,17 +3427,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>不純な彼女達は懺悔しない</t>
+          <t>とある魔術の禁書目録外伝　とある科学の心理掌握</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>ポロロッカ(著者)</t>
+          <t>乃木康仁(漫画) 鎌池和馬(原作) はいむらきよたか(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第27話</t>
+          <t>第32.5話</t>
         </is>
       </c>
     </row>
@@ -2405,17 +3447,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>アラサーがVTuberになった話。</t>
+          <t>傷口と包帯</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>犬威赤彦(漫画) とくめい(原作) カラスBTK(キャラクター原案)</t>
+          <t>七井海星</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第21話</t>
+          <t>第12話　ドキドキ手当て①</t>
         </is>
       </c>
     </row>
@@ -2425,17 +3467,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>人生逆転ダンジョン</t>
+          <t>神猫ミーちゃんと猫用品召喚師の異世界奮闘記 ～目指すは、もふもふスローライフ！～</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>尾張 ニコ どすこい花丸様</t>
+          <t>にゃんたろう(原作) ねこのゆーま(作画) 岩崎美奈子(キャラクター原案)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第2-2話	魔力発散</t>
+          <t>第3話②</t>
         </is>
       </c>
     </row>
@@ -2445,17 +3487,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>異世界で最強のスキルを生み出せたので、ひたすら無双することにしました。　～俺だけがスキルの数値を勝手に操作～</t>
+          <t>回復術士のやり直し</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>漫画：星トマジロウ 原作：ヒゲ抜き地蔵 キャラクター原案：山椒魚</t>
+          <t>月夜涙(原作) 羽賀ソウケン(漫画) しおこんぶ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第9話 ①</t>
+          <t>第71話-2</t>
         </is>
       </c>
     </row>
@@ -2465,17 +3507,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>クソ女に幸あれ</t>
+          <t>宮廷をクビになった植物魔導師はスローライフを謳歌する～のんびり世界樹を育てたら、最強領地ができました～</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>岸川瑞樹</t>
+          <t>蛙田アメコ 十三木考 又市マタロー</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第57話</t>
+          <t>第22話①フニクリ村</t>
         </is>
       </c>
     </row>
@@ -2485,17 +3527,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Fate/kaleid liner プリズマ☆イリヤ ドライ！！</t>
+          <t>最凶貴族は死亡フラグを覆す</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>ひろやまひろし(著者) ＴＹＰＥ－ＭＯＯＮ(原作)</t>
+          <t>作画：sudekuma 原作：塚上</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第76話 前編　双つ星</t>
+          <t>第4話(3)</t>
         </is>
       </c>
     </row>
@@ -2505,17 +3547,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>終焉の魔女と世界の旅</t>
+          <t>氷結令嬢さまをフォローしたら、メチャメチャ溺愛されてしまった件@comic</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>片岡とんち</t>
+          <t>漫画：ハレノチアメ 原作：愛坂タカト キャラクター原案：Bcoca</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第12話②	終焉の魔女エレナ</t>
+          <t>1巻表紙イラスト案大公開！</t>
         </is>
       </c>
     </row>
@@ -2525,17 +3567,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>リビルドワールド</t>
+          <t>宇崎ちゃんは遊びたい！</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+          <t>丈(著者)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第70話②</t>
+          <t>第124話</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-06-26
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -10,6 +10,7 @@
     <sheet name="2025-06-23" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="2025-06-24" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="2025-06-25" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="2025-06-26" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -2582,22 +2583,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第６６話『重機停止』④</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>マツモトケンゴ</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第５９話　筋トレの戦いが始まった（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>いとこのこ</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>いぬちく(著者)</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>「次にくるマンガ大賞 2025」応援よろしくお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>剥かせて！竜ケ崎さん</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>一智和智</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>大学生編 第12話</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>戸賀 環 坂木持丸 riritto</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第48話①　お祭りを楽しんでみた</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>骸骨騎士様、只今異世界へお出掛け中</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>サワノアキラ（漫画） 秤猿鬼（原作） KeG（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第64話　エルフ族の決断Ⅲ（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>ありふれた職業で世界最強</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>RoGa（漫画） 白米 良（原作） たかやKi（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第83話　新しい私の身体</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>祝！ 連載10周年『異世界魔王』人気ヒロイン総選挙</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>絶対死なないステラ姫</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>光永康則 大高稲</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第１３話　絶対巣穴に入らない・解（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>ラスボス討伐後に始める二周目冒険者ライフ はじまりの街でワケあり美少女たちがめちゃくちゃ懐いてきます</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>鬼麻正明(漫画) 朱月十話(原作) ファルまろ(キャラ原案)</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第3話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>ひとりぼっちの異世界攻略</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>びび（漫画） 五示正司（原作）</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第224話　あくまで情報交換なんだよ？</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>煽り系ゲーム配信者（20歳）、配信の切り忘れによりいい人バレする。</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>流嘉（漫画） 夏乃実（原作） 麦うさぎ（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第3話　切り抜き動画（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>ダウナー系お姉さんに毎日カスの嘘を流し込まれる話</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>生倉のゑる(著者) はるばーど屋(原作者)</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第10話</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第68話</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>元最強探索者のおじさん。美少女配信者を助けて大バズりしてしまった。</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>かなたろー(原作) 草壁レイ(漫画)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第3話　美少女、おじさんにハメられる。①</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>ある日、惰眠を貪っていたら一族から追放されて森に捨てられました そのまま寝てたら周りが勝手に魔物の国を作ってたけど、私は気にせず今日も眠ります　コミック版</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>漫画/伊草さゆ 原作/白波ハクア キャラクター原案/まさよ</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>chapter50【26話②】</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>無慈悲な悪役貴族に転生した僕は掌握魔法を駆使して魔法世界の頂点に立つ 〜ヒロインなんていないと諦めていたら向こうから勝手に寄ってきました〜</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>坂井オイ(漫画) びゃくし(原作) ファルまろ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第5話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>江戸前エルフ</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>樋口彰彦</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>#111</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>聖女に嘘は通じない</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>日向 夏 浅見よう しんいし智歩</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第24話②　もったいない</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>序盤で死ぬ最強のサブキャラに転生したので、ゲーム知識で無双する</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>作画：マエD 原作：新人</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第4話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>一生働きたくない俺が、クラスメイトの大人気アイドルに懐かれたら</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>三崎弓（漫画） 岸本和葉（原作） みわべさくら（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第19話　水族館デート②</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追放された【スキルサポーター】、仲間のスキルを解放して最強に成り上がる</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>作画：なかお 原作：前田氏</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第4話(3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>みだりに憑かせてはなりません</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>栗田あぐり(著者)</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第7話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>最強の少年聖騎士、転生者を狩る</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>作画：御塩 原作：宇奈木ユラ</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第4話(3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>傭兵団の料理番</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>梅木泰祐(漫画) 川井昂(原作) 四季童子(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第9話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>「おかえり、パパ」</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>蝉丸</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>単行本4巻限定描きおろし「羽化」試し読み</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>悪役一家の奥方、死に戻りして心を入れ替える。</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>鏡(漫画) 丘野優(原作) TEDDY(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第31話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>初歩魔法しか使わない謎の老魔法使いが旅をする</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>山代カゲツ(漫画) やまだのぼる(原作) にじまあるく(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第4話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>ラーメン大好き小泉さん</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>鳴見なる</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>13杯目 ようしょくてん</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>ゲーム　オブ　ファミリア-家族戦記-</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>Ｄ．Ｐ(作画) 山口ミコト(原作)</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第72話④</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>亡びの国の征服者～魔王は世界を征服するようです～</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>錆狗村昌（漫画） 不手折家（原作） toi8（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第30話　希望への出航（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>二周目チートの転生魔導士～最強が1000年後に転生したら、人生余裕すぎました～</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>石後千鳥 鬱沢色素 りいちゅ</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第31話　合同授業（中編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>ギャルゲーマーに褒められたい</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>げしゅまろ(著者)</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>31話</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>追放されたダンジョン配信者、《マッピング》スキルで最強パーティーを目指します</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>作画：入逢夕 原作：瀬戸夏樹</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第4話(3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第４９話　全脳力を駆使する器用貧乏（４）</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>転生したら没落貴族だったので、【呪言】を極めて家族を救います</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>作画：アマセケイ 原作：メソポ・たみあ</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第4話(3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>ちゃんと吸えない吸血鬼ちゃん</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>二式恭介(著者)</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第99話：吸血鬼ちゃんのおまもり③</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>豚貴族は未来を切り開くようです</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>大出リコ（漫画） しんこせい（原作） riritto（原作イラスト）</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第10話　旅立ち（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>転生貴族の異世界冒険録 ～自重を知らない神々の使徒～</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>夜州 nini 藻</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第68話</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>アラサーがVTuberになった話。</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>犬威赤彦(漫画) とくめい(原作) カラスBTK(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第21話</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第47話 魔導具師とつながれたもの①</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>二度追放された冒険者、激レアスキル駆使して美少女軍団を育成中！　コミック版</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>漫画/青木千尋 原作/南野雪花</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>chapter65【33話②】</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>とある魔術の禁書目録外伝　とある科学の心理掌握</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>乃木康仁(漫画) 鎌池和馬(原作) はいむらきよたか(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第32.5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>傷口と包帯</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>七井海星</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第12話　ドキドキ手当て①</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>神猫ミーちゃんと猫用品召喚師の異世界奮闘記 ～目指すは、もふもふスローライフ！～</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>にゃんたろう(原作) ねこのゆーま(作画) 岩崎美奈子(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第3話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>回復術士のやり直し</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>月夜涙(原作) 羽賀ソウケン(漫画) しおこんぶ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第71話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>宮廷をクビになった植物魔導師はスローライフを謳歌する～のんびり世界樹を育てたら、最強領地ができました～</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>蛙田アメコ 十三木考 又市マタロー</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第22話①フニクリ村</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>最凶貴族は死亡フラグを覆す</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>作画：sudekuma 原作：塚上</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第4話(3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>氷結令嬢さまをフォローしたら、メチャメチャ溺愛されてしまった件@comic</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>漫画：ハレノチアメ 原作：愛坂タカト キャラクター原案：Bcoca</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>1巻表紙イラスト案大公開！</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>宇崎ちゃんは遊びたい！</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>丈(著者)</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第124話</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>光永康則</t>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第６６話『重機停止』④</t>
+          <t>第33話①</t>
         </is>
       </c>
     </row>
@@ -2607,17 +3649,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+          <t>実は俺、最強でした？</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>マツモトケンゴ</t>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第５９話　筋トレの戦いが始まった（１）</t>
+          <t>おまけ62</t>
         </is>
       </c>
     </row>
@@ -2627,17 +3669,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>いとこのこ</t>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>いぬちく(著者)</t>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>「次にくるマンガ大賞 2025」応援よろしくお願いします！</t>
+          <t>第8話-2</t>
         </is>
       </c>
     </row>
@@ -2647,17 +3689,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>剥かせて！竜ケ崎さん</t>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>一智和智</t>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>大学生編 第12話</t>
+          <t>第31話 独身貴族はヒラメが大事（2）</t>
         </is>
       </c>
     </row>
@@ -2667,17 +3709,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+          <t>アザミヤコを好きになる</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>戸賀 環 坂木持丸 riritto</t>
+          <t>ユニティコング(原作) ツノニガウ(作画)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第48話①　お祭りを楽しんでみた</t>
+          <t>休載イラスト</t>
         </is>
       </c>
     </row>
@@ -2687,17 +3729,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>骸骨騎士様、只今異世界へお出掛け中</t>
+          <t>世界最強の後衛 ～迷宮国の新人探索者～</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>サワノアキラ（漫画） 秤猿鬼（原作） KeG（キャラクター原案）</t>
+          <t>力蔵(著者) とーわ(原作) 風花風花(キャラクター原案)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第64話　エルフ族の決断Ⅲ（後編）</t>
+          <t>第39話-3</t>
         </is>
       </c>
     </row>
@@ -2707,17 +3749,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ありふれた職業で世界最強</t>
+          <t>隣の席のヤンキー清水さんが髪を黒く染めてきた</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>RoGa（漫画） 白米 良（原作） たかやKi（キャラクター原案）</t>
+          <t>底花(原作) 真田若楓(漫画) ハム(キャラクター原案)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第83話　新しい私の身体</t>
+          <t>第9話-2</t>
         </is>
       </c>
     </row>
@@ -2727,17 +3769,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>異世界魔王と召喚少女の奴隷魔術</t>
+          <t>北斗の拳 世紀末ドラマ撮影伝</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+          <t>原案/武論尊・原哲夫 漫画/倉尾宏</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>祝！ 連載10周年『異世界魔王』人気ヒロイン総選挙</t>
+          <t>第73話 決死の天空撮影回!!</t>
         </is>
       </c>
     </row>
@@ -2747,17 +3789,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>絶対死なないステラ姫</t>
+          <t>ダンジョン・シェルパ　迷宮道先案内人</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>光永康則 大高稲</t>
+          <t>原作/加茂セイ 漫画/刀坂アキラ</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第１３話　絶対巣穴に入らない・解（３）</t>
+          <t>潜行：59(前編)</t>
         </is>
       </c>
     </row>
@@ -2767,17 +3809,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ラスボス討伐後に始める二周目冒険者ライフ はじまりの街でワケあり美少女たちがめちゃくちゃ懐いてきます</t>
+          <t>オタクに優しいギャルはいない!?</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>鬼麻正明(漫画) 朱月十話(原作) ファルまろ(キャラ原案)</t>
+          <t>のりしろちゃん魚住さかな</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第3話-2</t>
+          <t>【#145】女子部屋にて…</t>
         </is>
       </c>
     </row>
@@ -2787,17 +3829,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ひとりぼっちの異世界攻略</t>
+          <t>他校の氷姫を助けたら、お友達から始める事になりました</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>びび（漫画） 五示正司（原作）</t>
+          <t>椀田くろ(作画) 皐月 陽龍(原作) みすみ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第224話　あくまで情報交換なんだよ？</t>
+          <t>第10話-2</t>
         </is>
       </c>
     </row>
@@ -2807,17 +3849,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>煽り系ゲーム配信者（20歳）、配信の切り忘れによりいい人バレする。</t>
+          <t>すだちの魔王城</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>流嘉（漫画） 夏乃実（原作） 麦うさぎ（キャラクター原案）</t>
+          <t>森下真</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第3話　切り抜き動画（後編）</t>
+          <t>第43話　【交流会】（後編）</t>
         </is>
       </c>
     </row>
@@ -2827,17 +3869,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ダウナー系お姉さんに毎日カスの嘘を流し込まれる話</t>
+          <t>生徒会役員共</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>生倉のゑる(著者) はるばーど屋(原作者)</t>
+          <t>氏家ト全</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第10話</t>
+          <t>#402</t>
         </is>
       </c>
     </row>
@@ -2847,17 +3889,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
+          <t>カナン様はあくまでチョロい</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
+          <t>nonco</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第68話</t>
+          <t>第139話	カナンと供犠の伝える恋</t>
         </is>
       </c>
     </row>
@@ -2867,17 +3909,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>元最強探索者のおじさん。美少女配信者を助けて大バズりしてしまった。</t>
+          <t>スキル【万物支配】に目覚めたおっさんは、ダンジョンで生計を立てることにしました～無職から始める支配者無双～</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>かなたろー(原作) 草壁レイ(漫画)</t>
+          <t>岸本和葉 原田 臙 シミズヒロノリ 吉武</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第3話　美少女、おじさんにハメられる。①</t>
+          <t>第3話　パーティ結成‼</t>
         </is>
       </c>
     </row>
@@ -2887,17 +3929,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ある日、惰眠を貪っていたら一族から追放されて森に捨てられました そのまま寝てたら周りが勝手に魔物の国を作ってたけど、私は気にせず今日も眠ります　コミック版</t>
+          <t>妹の迷宮配信を手伝っていた俺が、うっかりＳランクモンスター相手に無双した結果がこちらです</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>漫画/伊草さゆ 原作/白波ハクア キャラクター原案/まさよ</t>
+          <t>おおのいも(著者) 木嶋隆太(原作) motto(キャラクター原案)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>chapter50【26話②】</t>
+          <t>最終話②</t>
         </is>
       </c>
     </row>
@@ -2907,17 +3949,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>無慈悲な悪役貴族に転生した僕は掌握魔法を駆使して魔法世界の頂点に立つ 〜ヒロインなんていないと諦めていたら向こうから勝手に寄ってきました〜</t>
+          <t>田舎のホームセンター男の自由な異世界生活</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>坂井オイ(漫画) びゃくし(原作) ファルまろ(キャラクター原案)</t>
+          <t>うさぴょん(原作) 古来歩(漫画) 市丸きすけ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第5話-2</t>
+          <t>第75話その1</t>
         </is>
       </c>
     </row>
@@ -2927,17 +3969,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>江戸前エルフ</t>
+          <t>ポンコツ風紀委員とスカート丈が不適切なＪＫの話</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>樋口彰彦</t>
+          <t>横田卓馬</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>#111</t>
+          <t>描き下ろし休載イラスト</t>
         </is>
       </c>
     </row>
@@ -2947,17 +3989,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>聖女に嘘は通じない</t>
+          <t>すべての人類を破壊する。それらは再生できない。</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>日向 夏 浅見よう しんいし智歩</t>
+          <t>横田卓馬(漫画) 伊瀬勝良(原作)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第24話②　もったいない</t>
+          <t>第65話その4</t>
         </is>
       </c>
     </row>
@@ -2967,17 +4009,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>序盤で死ぬ最強のサブキャラに転生したので、ゲーム知識で無双する</t>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>作画：マエD 原作：新人</t>
+          <t>光永康則</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第4話(1)</t>
+          <t>第６６話『重機停止』④</t>
         </is>
       </c>
     </row>
@@ -2987,17 +4029,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>一生働きたくない俺が、クラスメイトの大人気アイドルに懐かれたら</t>
+          <t>よわよわ先生</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>三崎弓（漫画） 岸本和葉（原作） みわべさくら（キャラクター原案）</t>
+          <t>福地カミオ</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第19話　水族館デート②</t>
+          <t>第104話	よわよわの母①</t>
         </is>
       </c>
     </row>
@@ -3007,17 +4049,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>勇者パーティを追放された【スキルサポーター】、仲間のスキルを解放して最強に成り上がる</t>
+          <t>転生錬金少女のスローライフ</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>作画：なかお 原作：前田氏</t>
+          <t>里町(漫画) 夜想庭園(原作) potg(キャラクター原案)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第4話(3)</t>
+          <t>第16話-1</t>
         </is>
       </c>
     </row>
@@ -3027,17 +4069,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>みだりに憑かせてはなりません</t>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>栗田あぐり(著者)</t>
+          <t>マツモトケンゴ</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第7話②</t>
+          <t>第５９話　筋トレの戦いが始まった（１）</t>
         </is>
       </c>
     </row>
@@ -3047,17 +4089,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>最強の少年聖騎士、転生者を狩る</t>
+          <t>チート薬師のスローライフ ～異世界に作ろうドラッグストア～</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>作画：御塩 原作：宇奈木ユラ</t>
+          <t>ケンノジ 春乃えり</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第4話(3)</t>
+          <t>66本目　チョコの日[後半]</t>
         </is>
       </c>
     </row>
@@ -3067,17 +4109,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>傭兵団の料理番</t>
+          <t>いとこのこ</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>梅木泰祐(漫画) 川井昂(原作) 四季童子(キャラクター原案)</t>
+          <t>いぬちく(著者)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第9話-1</t>
+          <t>「次にくるマンガ大賞 2025」応援よろしくお願いします！</t>
         </is>
       </c>
     </row>
@@ -3087,17 +4129,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>「おかえり、パパ」</t>
+          <t>善人おっさん、生まれ変わったらSSSランク人生が確定した</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>蝉丸</t>
+          <t>原作／三木なずな 漫画／ゆづましろ キャラクター原案／伍長</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>単行本4巻限定描きおろし「羽化」試し読み</t>
+          <t>特別イラスト</t>
         </is>
       </c>
     </row>
@@ -3107,17 +4149,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>悪役一家の奥方、死に戻りして心を入れ替える。</t>
+          <t>百瀬アキラの初恋破綻中。</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>鏡(漫画) 丘野優(原作) TEDDY(キャラクター原案)</t>
+          <t>晴川シンタ</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第31話①</t>
+          <t>第28話 物騒な母と対面中。</t>
         </is>
       </c>
     </row>
@@ -3127,17 +4169,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>初歩魔法しか使わない謎の老魔法使いが旅をする</t>
+          <t>勇者パーティーの荷物持ち</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>山代カゲツ(漫画) やまだのぼる(原作) にじまあるく(キャラクター原案)</t>
+          <t>原作：河本ほむら／作画：八嶋諒</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第4話②</t>
+          <t>第23話 荷物持ちと勇者パーティーの僧侶②</t>
         </is>
       </c>
     </row>
@@ -3147,17 +4189,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ラーメン大好き小泉さん</t>
+          <t>異世界チート魔術師</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>鳴見なる</t>
+          <t>内田健（ヒーロー文庫／イマジカインフォス）(原作) 鈴羅木かりん(漫画) Ｎａｒｄａｃｋ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>13杯目 ようしょくてん</t>
+          <t>第91話-2</t>
         </is>
       </c>
     </row>
@@ -3167,17 +4209,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ゲーム　オブ　ファミリア-家族戦記-</t>
+          <t>剥かせて！竜ケ崎さん</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Ｄ．Ｐ(作画) 山口ミコト(原作)</t>
+          <t>一智和智</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第72話④</t>
+          <t>大学生編 第12話</t>
         </is>
       </c>
     </row>
@@ -3187,17 +4229,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>亡びの国の征服者～魔王は世界を征服するようです～</t>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>錆狗村昌（漫画） 不手折家（原作） toi8（キャラクター原案）</t>
+          <t>戸賀 環 坂木持丸 riritto</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第30話　希望への出航（後編）</t>
+          <t>第48話①　お祭りを楽しんでみた</t>
         </is>
       </c>
     </row>
@@ -3207,17 +4249,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>二周目チートの転生魔導士～最強が1000年後に転生したら、人生余裕すぎました～</t>
+          <t>303号室の神さま</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>石後千鳥 鬱沢色素 りいちゅ</t>
+          <t>ふに・無9(著者)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第31話　合同授業（中編）</t>
+          <t>Episode. 16</t>
         </is>
       </c>
     </row>
@@ -3227,17 +4269,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ギャルゲーマーに褒められたい</t>
+          <t>後宮メイドの災難～人使いの荒い宮廷書記官と推理する～</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>げしゅまろ(著者)</t>
+          <t>大野ちた 永井青</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>31話</t>
+          <t>8話③</t>
         </is>
       </c>
     </row>
@@ -3247,17 +4289,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>追放されたダンジョン配信者、《マッピング》スキルで最強パーティーを目指します</t>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>作画：入逢夕 原作：瀬戸夏樹</t>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第4話(3)</t>
+          <t>祝！ 連載10周年『異世界魔王』人気ヒロイン総選挙</t>
         </is>
       </c>
     </row>
@@ -3267,17 +4309,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+          <t>ありふれた職業で世界最強</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+          <t>RoGa（漫画） 白米 良（原作） たかやKi（キャラクター原案）</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第４９話　全脳力を駆使する器用貧乏（４）</t>
+          <t>第83話　新しい私の身体</t>
         </is>
       </c>
     </row>
@@ -3287,17 +4329,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>転生したら没落貴族だったので、【呪言】を極めて家族を救います</t>
+          <t>ジェノヴァの弟子～10秒しか戦えない魔術師、のちの『魔王』を育てる～</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>作画：アマセケイ 原作：メソポ・たみあ</t>
+          <t>原作：妹尾尻尾 漫画：魚塚じゃこ キャラクター原案：赤嶺直樹</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第4話(3)</t>
+          <t>第20話</t>
         </is>
       </c>
     </row>
@@ -3307,17 +4349,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ちゃんと吸えない吸血鬼ちゃん</t>
+          <t>骸骨騎士様、只今異世界へお出掛け中</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>二式恭介(著者)</t>
+          <t>サワノアキラ（漫画） 秤猿鬼（原作） KeG（キャラクター原案）</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第99話：吸血鬼ちゃんのおまもり③</t>
+          <t>第64話　エルフ族の決断Ⅲ（後編）</t>
         </is>
       </c>
     </row>
@@ -3327,17 +4369,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>豚貴族は未来を切り開くようです</t>
+          <t>シャドウ・アサシンズ・ワールド ～影は薄いけど、最強忍者やってます～</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>大出リコ（漫画） しんこせい（原作） riritto（原作イラスト）</t>
+          <t>空山トキ 五色安未 泉乃せん 伍長</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第10話　旅立ち（後編）</t>
+          <t>第10話　少女と本当の自分１（1）</t>
         </is>
       </c>
     </row>
@@ -3347,12 +4389,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>転生貴族の異世界冒険録 ～自重を知らない神々の使徒～</t>
+          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>夜州 nini 藻</t>
+          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -3367,17 +4409,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>アラサーがVTuberになった話。</t>
+          <t>追放されたダンジョン配信者、《マッピング》スキルで最強パーティーを目指します</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>犬威赤彦(漫画) とくめい(原作) カラスBTK(キャラクター原案)</t>
+          <t>作画：入逢夕 原作：瀬戸夏樹</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第21話</t>
+          <t>第4話(3)</t>
         </is>
       </c>
     </row>
@@ -3387,17 +4429,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
+          <t>葉木莉さんは君だけの死神になりたい</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
+          <t>３５まち</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第47話 魔導具師とつながれたもの①</t>
+          <t>第4話 でも俺 スタッフロールは最後まで観る派だから</t>
         </is>
       </c>
     </row>
@@ -3407,17 +4449,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>二度追放された冒険者、激レアスキル駆使して美少女軍団を育成中！　コミック版</t>
+          <t>ラスボス討伐後に始める二周目冒険者ライフ はじまりの街でワケあり美少女たちがめちゃくちゃ懐いてきます</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>漫画/青木千尋 原作/南野雪花</t>
+          <t>鬼麻正明(漫画) 朱月十話(原作) ファルまろ(キャラ原案)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>chapter65【33話②】</t>
+          <t>第3話-2</t>
         </is>
       </c>
     </row>
@@ -3427,17 +4469,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>とある魔術の禁書目録外伝　とある科学の心理掌握</t>
+          <t>ダウナー系お姉さんに毎日カスの嘘を流し込まれる話</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>乃木康仁(漫画) 鎌池和馬(原作) はいむらきよたか(キャラクターデザイン)</t>
+          <t>生倉のゑる(著者) はるばーど屋(原作者)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第32.5話</t>
+          <t>第10話</t>
         </is>
       </c>
     </row>
@@ -3447,17 +4489,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>傷口と包帯</t>
+          <t>絶対死なないステラ姫</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>七井海星</t>
+          <t>光永康則 大高稲</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第12話　ドキドキ手当て①</t>
+          <t>第１３話　絶対巣穴に入らない・解（３）</t>
         </is>
       </c>
     </row>
@@ -3467,17 +4509,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>神猫ミーちゃんと猫用品召喚師の異世界奮闘記 ～目指すは、もふもふスローライフ！～</t>
+          <t>煽り系ゲーム配信者（20歳）、配信の切り忘れによりいい人バレする。</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>にゃんたろう(原作) ねこのゆーま(作画) 岩崎美奈子(キャラクター原案)</t>
+          <t>流嘉（漫画） 夏乃実（原作） 麦うさぎ（キャラクター原案）</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第3話②</t>
+          <t>第3話　切り抜き動画（後編）</t>
         </is>
       </c>
     </row>
@@ -3487,17 +4529,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>回復術士のやり直し</t>
+          <t>ひとりぼっちの異世界攻略</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>月夜涙(原作) 羽賀ソウケン(漫画) しおこんぶ(キャラクター原案)</t>
+          <t>びび（漫画） 五示正司（原作）</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第71話-2</t>
+          <t>第224話　あくまで情報交換なんだよ？</t>
         </is>
       </c>
     </row>
@@ -3507,17 +4549,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>宮廷をクビになった植物魔導師はスローライフを謳歌する～のんびり世界樹を育てたら、最強領地ができました～</t>
+          <t>宇崎ちゃんは遊びたい！</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>蛙田アメコ 十三木考 又市マタロー</t>
+          <t>丈(著者)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第22話①フニクリ村</t>
+          <t>第124話</t>
         </is>
       </c>
     </row>
@@ -3527,17 +4569,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>最凶貴族は死亡フラグを覆す</t>
+          <t>千年英雄</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>作画：sudekuma 原作：塚上</t>
+          <t>原作/福島航平 作画/中村ゆきひろ</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第4話(3)</t>
+          <t>10話①</t>
         </is>
       </c>
     </row>
@@ -3547,17 +4589,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>氷結令嬢さまをフォローしたら、メチャメチャ溺愛されてしまった件@comic</t>
+          <t>アンゴルモア 元寇合戦記　【博多編】</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>漫画：ハレノチアメ 原作：愛坂タカト キャラクター原案：Bcoca</t>
+          <t>たかぎ七彦(著者)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>1巻表紙イラスト案大公開！</t>
+          <t>第四十四話その二</t>
         </is>
       </c>
     </row>
@@ -3567,17 +4609,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>宇崎ちゃんは遊びたい！</t>
+          <t>恋人以上友人未満</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>丈(著者)</t>
+          <t>yatoyato</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第124話</t>
+          <t>第91話</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-06-27
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -11,6 +11,7 @@
     <sheet name="2025-06-24" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="2025-06-25" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="2025-06-26" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="2025-06-27" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -3624,22 +3625,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第33話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>おまけ62</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第8話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第31話 独身貴族はヒラメが大事（2）</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>アザミヤコを好きになる</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>ユニティコング(原作) ツノニガウ(作画)</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>休載イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>世界最強の後衛 ～迷宮国の新人探索者～</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>力蔵(著者) とーわ(原作) 風花風花(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第39話-3</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>隣の席のヤンキー清水さんが髪を黒く染めてきた</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>底花(原作) 真田若楓(漫画) ハム(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第9話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>北斗の拳 世紀末ドラマ撮影伝</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>原案/武論尊・原哲夫 漫画/倉尾宏</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第73話 決死の天空撮影回!!</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>ダンジョン・シェルパ　迷宮道先案内人</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>原作/加茂セイ 漫画/刀坂アキラ</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>潜行：59(前編)</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>オタクに優しいギャルはいない!?</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>のりしろちゃん魚住さかな</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>【#145】女子部屋にて…</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>他校の氷姫を助けたら、お友達から始める事になりました</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>椀田くろ(作画) 皐月 陽龍(原作) みすみ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第10話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>すだちの魔王城</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>森下真</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第43話　【交流会】（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>生徒会役員共</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>氏家ト全</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>#402</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>カナン様はあくまでチョロい</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>nonco</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第139話	カナンと供犠の伝える恋</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>スキル【万物支配】に目覚めたおっさんは、ダンジョンで生計を立てることにしました～無職から始める支配者無双～</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>岸本和葉 原田 臙 シミズヒロノリ 吉武</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第3話　パーティ結成‼</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>妹の迷宮配信を手伝っていた俺が、うっかりＳランクモンスター相手に無双した結果がこちらです</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>おおのいも(著者) 木嶋隆太(原作) motto(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>最終話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>田舎のホームセンター男の自由な異世界生活</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>うさぴょん(原作) 古来歩(漫画) 市丸きすけ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第75話その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>ポンコツ風紀委員とスカート丈が不適切なＪＫの話</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>横田卓馬</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>描き下ろし休載イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>すべての人類を破壊する。それらは再生できない。</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>横田卓馬(漫画) 伊瀬勝良(原作)</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第65話その4</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第６６話『重機停止』④</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>よわよわ先生</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>福地カミオ</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第104話	よわよわの母①</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>転生錬金少女のスローライフ</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>里町(漫画) 夜想庭園(原作) potg(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第16話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>マツモトケンゴ</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第５９話　筋トレの戦いが始まった（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>チート薬師のスローライフ ～異世界に作ろうドラッグストア～</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>ケンノジ 春乃えり</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>66本目　チョコの日[後半]</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>いとこのこ</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>いぬちく(著者)</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>「次にくるマンガ大賞 2025」応援よろしくお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>善人おっさん、生まれ変わったらSSSランク人生が確定した</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>原作／三木なずな 漫画／ゆづましろ キャラクター原案／伍長</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>特別イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>百瀬アキラの初恋破綻中。</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>晴川シンタ</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第28話 物騒な母と対面中。</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティーの荷物持ち</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>原作：河本ほむら／作画：八嶋諒</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第23話 荷物持ちと勇者パーティーの僧侶②</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>異世界チート魔術師</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>内田健（ヒーロー文庫／イマジカインフォス）(原作) 鈴羅木かりん(漫画) Ｎａｒｄａｃｋ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第91話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>剥かせて！竜ケ崎さん</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>一智和智</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>大学生編 第12話</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>戸賀 環 坂木持丸 riritto</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第48話①　お祭りを楽しんでみた</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>303号室の神さま</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>ふに・無9(著者)</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>Episode. 16</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>後宮メイドの災難～人使いの荒い宮廷書記官と推理する～</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>大野ちた 永井青</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>8話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>祝！ 連載10周年『異世界魔王』人気ヒロイン総選挙</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>ありふれた職業で世界最強</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>RoGa（漫画） 白米 良（原作） たかやKi（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第83話　新しい私の身体</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>ジェノヴァの弟子～10秒しか戦えない魔術師、のちの『魔王』を育てる～</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>原作：妹尾尻尾 漫画：魚塚じゃこ キャラクター原案：赤嶺直樹</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第20話</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>骸骨騎士様、只今異世界へお出掛け中</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>サワノアキラ（漫画） 秤猿鬼（原作） KeG（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第64話　エルフ族の決断Ⅲ（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>シャドウ・アサシンズ・ワールド ～影は薄いけど、最強忍者やってます～</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>空山トキ 五色安未 泉乃せん 伍長</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第10話　少女と本当の自分１（1）</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第68話</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>追放されたダンジョン配信者、《マッピング》スキルで最強パーティーを目指します</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>作画：入逢夕 原作：瀬戸夏樹</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第4話(3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>葉木莉さんは君だけの死神になりたい</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>３５まち</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第4話 でも俺 スタッフロールは最後まで観る派だから</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>ラスボス討伐後に始める二周目冒険者ライフ はじまりの街でワケあり美少女たちがめちゃくちゃ懐いてきます</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>鬼麻正明(漫画) 朱月十話(原作) ファルまろ(キャラ原案)</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第3話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>ダウナー系お姉さんに毎日カスの嘘を流し込まれる話</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>生倉のゑる(著者) はるばーど屋(原作者)</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第10話</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>絶対死なないステラ姫</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>光永康則 大高稲</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第１３話　絶対巣穴に入らない・解（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>煽り系ゲーム配信者（20歳）、配信の切り忘れによりいい人バレする。</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>流嘉（漫画） 夏乃実（原作） 麦うさぎ（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第3話　切り抜き動画（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>ひとりぼっちの異世界攻略</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>びび（漫画） 五示正司（原作）</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第224話　あくまで情報交換なんだよ？</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>宇崎ちゃんは遊びたい！</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>丈(著者)</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第124話</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>千年英雄</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>原作/福島航平 作画/中村ゆきひろ</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>10話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>アンゴルモア 元寇合戦記　【博多編】</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>たかぎ七彦(著者)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第四十四話その二</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>恋人以上友人未満</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>yatoyato</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第91話</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+          <t>ワンパンマン</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第33話①</t>
+          <t>201撃目</t>
         </is>
       </c>
     </row>
@@ -3649,17 +4691,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>実は俺、最強でした？</t>
+          <t>ぽんドロイド！ はまさん</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>原作：澄守 彩 漫画：高橋 愛</t>
+          <t>はれやまはれぞう(著者)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>おまけ62</t>
+          <t>第1話</t>
         </is>
       </c>
     </row>
@@ -3669,17 +4711,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+          <t>物語の黒幕に転生して</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第8話-2</t>
+          <t>第31話</t>
         </is>
       </c>
     </row>
@@ -3689,17 +4731,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+          <t>村上よしゆき 茨木野 あるてら</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第31話 独身貴族はヒラメが大事（2）</t>
+          <t>第４０話　勇者、聖女と元聖騎士と再会し、魚人を追っ払う（２）</t>
         </is>
       </c>
     </row>
@@ -3709,17 +4751,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>アザミヤコを好きになる</t>
+          <t>ゲーム悪役貴族に転生した俺は、チート筋肉で無双する</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ユニティコング(原作) ツノニガウ(作画)</t>
+          <t>昼行燈（原作） しいたけ元帥（漫画）</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>休載イラスト</t>
+          <t>第24話</t>
         </is>
       </c>
     </row>
@@ -3729,17 +4771,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>世界最強の後衛 ～迷宮国の新人探索者～</t>
+          <t>俺以外誰も採取できない素材なのに「素材採取率が低い」とパワハラする幼馴染錬金術師と絶縁した専属魔導士、辺境の町でスローライフを送りたい。</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>力蔵(著者) とーわ(原作) 風花風花(キャラクター原案)</t>
+          <t>狐御前(原作) 西岡知三(作画) ＮＯＣＯ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第39話-3</t>
+          <t>第23話-1</t>
         </is>
       </c>
     </row>
@@ -3749,17 +4791,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>隣の席のヤンキー清水さんが髪を黒く染めてきた</t>
+          <t>バーサス</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>底花(原作) 真田若楓(漫画) ハム(キャラクター原案)</t>
+          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第9話-2</t>
+          <t>第25話 超越（2）</t>
         </is>
       </c>
     </row>
@@ -3769,17 +4811,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>北斗の拳 世紀末ドラマ撮影伝</t>
+          <t>幼女戦記</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>原案/武論尊・原哲夫 漫画/倉尾宏</t>
+          <t>東條チカ(漫画) カルロ・ゼン(原作) 篠月しのぶ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第73話 決死の天空撮影回!!</t>
+          <t>第百五章：再編Ⅷ</t>
         </is>
       </c>
     </row>
@@ -3789,17 +4831,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ダンジョン・シェルパ　迷宮道先案内人</t>
+          <t>デスゲームに巻き込まれた山本さん、気ままにゲームバランスを崩壊させる</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>原作/加茂セイ 漫画/刀坂アキラ</t>
+          <t>ぽち(原作) カモトタツヤ(作画) 久賀フーナ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>潜行：59(前編)</t>
+          <t>第5話</t>
         </is>
       </c>
     </row>
@@ -3809,17 +4851,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>オタクに優しいギャルはいない!?</t>
+          <t>魔石グルメ　魔物の力を食べたオレは最強！</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>のりしろちゃん魚住さかな</t>
+          <t>菅原健二(作画) 結城涼(原作) 成瀬ちさと(キャラクター原案)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>【#145】女子部屋にて…</t>
+          <t>第66話後半</t>
         </is>
       </c>
     </row>
@@ -3829,17 +4871,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>他校の氷姫を助けたら、お友達から始める事になりました</t>
+          <t>魔王になったので、ダンジョン造って人外娘とほのぼのする</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>椀田くろ(作画) 皐月 陽龍(原作) みすみ(キャラクター原案)</t>
+          <t>遠野ノオト(作画) 流優(原作) だぶ竜(キャラクター原案)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第10話-2</t>
+          <t>第81話後半</t>
         </is>
       </c>
     </row>
@@ -3849,17 +4891,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>すだちの魔王城</t>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>森下真</t>
+          <t>空野進 sorani ファルまろ</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第43話　【交流会】（後編）</t>
+          <t>第9話　最弱貴族、暗躍する（４）</t>
         </is>
       </c>
     </row>
@@ -3869,17 +4911,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>生徒会役員共</t>
+          <t>転生したらスライムだった件 異聞 ～魔国暮らしのトリニティ～</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>氏家ト全</t>
+          <t>伏瀬 戸野タエ みっつばー</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>#402</t>
+          <t>第105話　帰国！［後編］</t>
         </is>
       </c>
     </row>
@@ -3889,17 +4931,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>カナン様はあくまでチョロい</t>
+          <t>双子まとめて『カノジョ』にしない？</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>nonco</t>
+          <t>飴色みそ(漫画) 白井ムク(原作) 千種みのり(キャラクター原案)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第139話	カナンと供犠の伝える恋</t>
+          <t>第12話③</t>
         </is>
       </c>
     </row>
@@ -3909,17 +4951,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>スキル【万物支配】に目覚めたおっさんは、ダンジョンで生計を立てることにしました～無職から始める支配者無双～</t>
+          <t>デスマーチからはじまる異世界狂想曲</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>岸本和葉 原田 臙 シミズヒロノリ 吉武</t>
+          <t>あやめぐむ(作画) 愛七ひろ(原作) ｓｈｒｉ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第3話　パーティ結成‼</t>
+          <t>第126話</t>
         </is>
       </c>
     </row>
@@ -3929,17 +4971,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>妹の迷宮配信を手伝っていた俺が、うっかりＳランクモンスター相手に無双した結果がこちらです</t>
+          <t>極振り拒否して手探りスタート！　特化しないヒーラー、仲間と別れて旅に出る</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>おおのいも(著者) 木嶋隆太(原作) motto(キャラクター原案)</t>
+          <t>蒼井一秀(作画) 刻一(原作) MIYA*KI(キャラクター原案)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>最終話②</t>
+          <t>第63話</t>
         </is>
       </c>
     </row>
@@ -3949,17 +4991,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>田舎のホームセンター男の自由な異世界生活</t>
+          <t>貧乏騎士に嫁入りしたはずが!? ~野人令嬢は皇太子妃になっても竜を狩りたい~</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>うさぴょん(原作) 古来歩(漫画) 市丸きすけ(キャラクター原案)</t>
+          <t>漫画：夏川そぞろ 原作：宮前葵 キャラクター原案：ののまろ</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第75話その1</t>
+          <t>第10話①皇太子妃（仮）</t>
         </is>
       </c>
     </row>
@@ -3969,17 +5011,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ポンコツ風紀委員とスカート丈が不適切なＪＫの話</t>
+          <t>となりの席のヤツがそういう目で見てくる</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>横田卓馬</t>
+          <t>mmk</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>描き下ろし休載イラスト</t>
+          <t>第38話 読解力</t>
         </is>
       </c>
     </row>
@@ -3989,17 +5031,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>すべての人類を破壊する。それらは再生できない。</t>
+          <t>ヘルモード ～やり込み好きのゲーマーは廃設定の異世界で無双する～ はじまりの召喚士</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>横田卓馬(漫画) 伊瀬勝良(原作)</t>
+          <t>原作：ハム男・藻 漫画：鉄田猿児</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第65話その4</t>
+          <t>GAME 080　協力</t>
         </is>
       </c>
     </row>
@@ -4009,17 +5051,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+          <t>放課後はケンカ最強のギャルに連れこまれる生活 彼女たちに好かれて、僕も最強に!?</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>光永康則</t>
+          <t>亜逸(原作) あおやぎ孝夫(作画) ｋａｋａｏ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第６６話『重機停止』④</t>
+          <t>第15話</t>
         </is>
       </c>
     </row>
@@ -4029,17 +5071,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>よわよわ先生</t>
+          <t>【悲報】清楚系で売っていた底辺配信者、うっかり配信を切り忘れたままSS級モンスターを拳で殴り飛ばしてしまう</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>福地カミオ</t>
+          <t>アトハ NEO草野 pupps</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第104話	よわよわの母①</t>
+          <t>第４話　【悲報】ご乱行⁉ ダンジョンシーカー・アカデミー！（１）</t>
         </is>
       </c>
     </row>
@@ -4049,17 +5091,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>転生錬金少女のスローライフ</t>
+          <t>ガルルガール</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>里町(漫画) 夜想庭園(原作) potg(キャラクター原案)</t>
+          <t>原聡志(著者)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第16話-1</t>
+          <t>第14話</t>
         </is>
       </c>
     </row>
@@ -4069,17 +5111,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+          <t>どうやら私の身体は完全無敵のようですね</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>マツモトケンゴ</t>
+          <t>さばねこ(作画) ちゃつふさ(原作) ふーみ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第５９話　筋トレの戦いが始まった（１）</t>
+          <t>第78話</t>
         </is>
       </c>
     </row>
@@ -4089,17 +5131,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>チート薬師のスローライフ ～異世界に作ろうドラッグストア～</t>
+          <t>規格外のダンジョン攻略者、実は異世界帰りの元勇者</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ケンノジ 春乃えり</t>
+          <t>作画：やまざき君 原作：榊与一</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>66本目　チョコの日[後半]</t>
+          <t>第3話(2)</t>
         </is>
       </c>
     </row>
@@ -4109,17 +5151,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>いとこのこ</t>
+          <t>異世界ゆるっとサバイバル生活～学校の皆と異世界の無人島に転移したけど俺だけ楽勝です～</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>いぬちく(著者)</t>
+          <t>西尾洋一(作画) 絢乃(原作) 乾和音(キャラクター原案) 株式会社一二三書房(監修)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>「次にくるマンガ大賞 2025」応援よろしくお願いします！</t>
+          <t>第48話-2</t>
         </is>
       </c>
     </row>
@@ -4129,17 +5171,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>善人おっさん、生まれ変わったらSSSランク人生が確定した</t>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>原作／三木なずな 漫画／ゆづましろ キャラクター原案／伍長</t>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>特別イラスト</t>
+          <t>第33話①</t>
         </is>
       </c>
     </row>
@@ -4149,17 +5191,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>百瀬アキラの初恋破綻中。</t>
+          <t>放課後、ファミレスで、クラスのあの子と。</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>晴川シンタ</t>
+          <t>麦子(漫画) 左リュウ(原作) magako(キャラクター原案)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第28話 物騒な母と対面中。</t>
+          <t>第10話②</t>
         </is>
       </c>
     </row>
@@ -4169,17 +5211,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>勇者パーティーの荷物持ち</t>
+          <t>俺のクラスに若返った元嫁がいる</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>原作：河本ほむら／作画：八嶋諒</t>
+          <t>原作：猫又　ぬこ 漫画：akn坊 キャラクター原案：緑川　葉</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第23話 荷物持ちと勇者パーティーの僧侶②</t>
+          <t>最終話（後編）</t>
         </is>
       </c>
     </row>
@@ -4189,17 +5231,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>異世界チート魔術師</t>
+          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>内田健（ヒーロー文庫／イマジカインフォス）(原作) 鈴羅木かりん(漫画) Ｎａｒｄａｃｋ(キャラクター原案)</t>
+          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第91話-2</t>
+          <t>第1話②</t>
         </is>
       </c>
     </row>
@@ -4209,17 +5251,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>剥かせて！竜ケ崎さん</t>
+          <t>町人Aは悪役令嬢をどうしても救いたい　～どぶと空と氷の姫君～</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>一智和智</t>
+          <t>原作：一色孝太郎・Parum 漫画：目黒三吉</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>大学生編 第12話</t>
+          <t>第37話 軍議</t>
         </is>
       </c>
     </row>
@@ -4229,17 +5271,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>戸賀 環 坂木持丸 riritto</t>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第48話①　お祭りを楽しんでみた</t>
+          <t>第8話-2</t>
         </is>
       </c>
     </row>
@@ -4249,17 +5291,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>303号室の神さま</t>
+          <t>継母の連れ子が元カノだった</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>ふに・無9(著者)</t>
+          <t>草壁レイ(作画) 紙城境介(原作) たかやKi(キャラクター原案)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Episode. 16</t>
+          <t>第60話④</t>
         </is>
       </c>
     </row>
@@ -4269,17 +5311,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>後宮メイドの災難～人使いの荒い宮廷書記官と推理する～</t>
+          <t>村人ですが何か？</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>大野ちた 永井青</t>
+          <t>鯖夢(作画) 白石新(原案・監修) 白蘇ふぁみ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>8話③</t>
+          <t>第90話</t>
         </is>
       </c>
     </row>
@@ -4289,17 +5331,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>異世界魔王と召喚少女の奴隷魔術</t>
+          <t>実は俺、最強でした？</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>祝！ 連載10周年『異世界魔王』人気ヒロイン総選挙</t>
+          <t>おまけ62</t>
         </is>
       </c>
     </row>
@@ -4309,17 +5351,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>ありふれた職業で世界最強</t>
+          <t>とにかくウケたいぼっち女子(仮)</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>RoGa（漫画） 白米 良（原作） たかやKi（キャラクター原案）</t>
+          <t>佐藤ショーキ</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第83話　新しい私の身体</t>
+          <t>鋭意製作中です。</t>
         </is>
       </c>
     </row>
@@ -4329,17 +5371,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>ジェノヴァの弟子～10秒しか戦えない魔術師、のちの『魔王』を育てる～</t>
+          <t>戦姫サバイバルサガ-異世界の運命をかけた無人島フジュン異性交遊-</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>原作：妹尾尻尾 漫画：魚塚じゃこ キャラクター原案：赤嶺直樹</t>
+          <t>OTOSAMA(著者)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第20話</t>
+          <t>第16話</t>
         </is>
       </c>
     </row>
@@ -4349,17 +5391,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>骸骨騎士様、只今異世界へお出掛け中</t>
+          <t>斎藤義龍に生まれ変わったので、織田信長に国譲りして長生きするのを目指します！</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>サワノアキラ（漫画） 秤猿鬼（原作） KeG（キャラクター原案）</t>
+          <t>巽未頼 田村ゆうき マキムラシュンスケ</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第64話　エルフ族の決断Ⅲ（後編）</t>
+          <t>第70話「影」</t>
         </is>
       </c>
     </row>
@@ -4369,17 +5411,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>シャドウ・アサシンズ・ワールド ～影は薄いけど、最強忍者やってます～</t>
+          <t>異世界でスキルを解体したらチートな嫁が増殖しました 概念交差のストラクチャー</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>空山トキ 五色安未 泉乃せん 伍長</t>
+          <t>カタセミナミ(作画) 千月さかき(原作) 東西(キャラクター原案)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第10話　少女と本当の自分１（1）</t>
+          <t>第78話-2</t>
         </is>
       </c>
     </row>
@@ -4389,17 +5431,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
+          <t>ギャルゲーマーに褒められたい</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
+          <t>げしゅまろ(著者)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第68話</t>
+          <t>32話</t>
         </is>
       </c>
     </row>
@@ -4409,17 +5451,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>追放されたダンジョン配信者、《マッピング》スキルで最強パーティーを目指します</t>
+          <t>直径3cmの召喚陣&lt;リミットリング&gt;で「雑魚すら呼べない」と蔑まれた底辺召喚士が頂点に立つまで</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>作画：入逢夕 原作：瀬戸夏樹</t>
+          <t>作画：まっつー 原作：空松蓮司</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第4話(3)</t>
+          <t>第3話(2)</t>
         </is>
       </c>
     </row>
@@ -4429,17 +5471,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>葉木莉さんは君だけの死神になりたい</t>
+          <t>ルパン三世 異世界の姫君（ネイバーワールドプリンセス）</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>３５まち</t>
+          <t>モンキー・パンチ／エム・ピー・ワークス 内々けやき 佐伯庸介 白狼</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第4話 でも俺 スタッフロールは最後まで観る派だから</t>
+          <t>第98話：泥棒、心を盗めど縛りはせず❶</t>
         </is>
       </c>
     </row>
@@ -4449,17 +5491,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>ラスボス討伐後に始める二周目冒険者ライフ はじまりの街でワケあり美少女たちがめちゃくちゃ懐いてきます</t>
+          <t>ポンコツ勇者パーティー、竜をひろう</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>鬼麻正明(漫画) 朱月十話(原作) ファルまろ(キャラ原案)</t>
+          <t>優風(著者)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第3話-2</t>
+          <t>第2話</t>
         </is>
       </c>
     </row>
@@ -4469,17 +5511,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>ダウナー系お姉さんに毎日カスの嘘を流し込まれる話</t>
+          <t>転校先の清楚可憐な美少女が、昔男子と思って一緒に遊んだ幼馴染だった件</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>生倉のゑる(著者) はるばーど屋(原作者)</t>
+          <t>大山樹奈(作画) 雲雀湯(原作) シソ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第10話</t>
+          <t>最終話-2</t>
         </is>
       </c>
     </row>
@@ -4489,17 +5531,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>絶対死なないステラ姫</t>
+          <t>後宮メイドの災難～人使いの荒い宮廷書記官と推理する～</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>光永康則 大高稲</t>
+          <t>大野ちた 永井青</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第１３話　絶対巣穴に入らない・解（３）</t>
+          <t>8話③</t>
         </is>
       </c>
     </row>
@@ -4509,17 +5551,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>煽り系ゲーム配信者（20歳）、配信の切り忘れによりいい人バレする。</t>
+          <t>アザミヤコを好きになる</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>流嘉（漫画） 夏乃実（原作） 麦うさぎ（キャラクター原案）</t>
+          <t>ユニティコング(原作) ツノニガウ(作画)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第3話　切り抜き動画（後編）</t>
+          <t>休載イラスト</t>
         </is>
       </c>
     </row>
@@ -4529,17 +5571,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>ひとりぼっちの異世界攻略</t>
+          <t>おねえさんと猫を飼う</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>びび（漫画） 五示正司（原作）</t>
+          <t>上杉響士郎(著者)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第224話　あくまで情報交換なんだよ？</t>
+          <t>第1話：おねえさんと猫を拾う</t>
         </is>
       </c>
     </row>
@@ -4549,17 +5591,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>宇崎ちゃんは遊びたい！</t>
+          <t>辺境都市の育成者</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>丈(著者)</t>
+          <t>日高(著者) 七野りく(原作) 福きつね(キャラクター原案)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第124話</t>
+          <t>第30編②</t>
         </is>
       </c>
     </row>
@@ -4569,17 +5611,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>千年英雄</t>
+          <t>六姫は神護衛に恋をする　～最強の守護騎士、転生して魔法学園に行く～</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>原作/福島航平 作画/中村ゆきひろ</t>
+          <t>漫画:加古山 寿 原案:朱月 十話 キャラクター原案:てつぶた</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>10話①</t>
+          <t>第121話　解決策</t>
         </is>
       </c>
     </row>
@@ -4589,17 +5631,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>アンゴルモア 元寇合戦記　【博多編】</t>
+          <t>モブだけど最強を目指します！　～ゲーム世界に転生した俺は自由に強さを追い求める～</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>たかぎ七彦(著者)</t>
+          <t>反面教師(原作) 五條さやか(作画) 大熊猫介(キャラクター原案)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第四十四話その二</t>
+          <t>第11話</t>
         </is>
       </c>
     </row>
@@ -4609,17 +5651,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>恋人以上友人未満</t>
+          <t>没落予定なので、鍛冶職人を目指す</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>yatoyato</t>
+          <t>石田彩(作画) CK(原作) かわく(キャラクター原案)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第91話</t>
+          <t>第99話-2</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-06-28
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -12,6 +12,7 @@
     <sheet name="2025-06-25" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="2025-06-26" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="2025-06-27" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="2025-06-28" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -4666,22 +4667,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>ワンパンマン</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>201撃目</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>ぽんドロイド！ はまさん</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>はれやまはれぞう(著者)</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第1話</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>物語の黒幕に転生して</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第31話</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>村上よしゆき 茨木野 あるてら</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第４０話　勇者、聖女と元聖騎士と再会し、魚人を追っ払う（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>ゲーム悪役貴族に転生した俺は、チート筋肉で無双する</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>昼行燈（原作） しいたけ元帥（漫画）</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第24話</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>俺以外誰も採取できない素材なのに「素材採取率が低い」とパワハラする幼馴染錬金術師と絶縁した専属魔導士、辺境の町でスローライフを送りたい。</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>狐御前(原作) 西岡知三(作画) ＮＯＣＯ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第23話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>バーサス</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第25話 超越（2）</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>幼女戦記</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>東條チカ(漫画) カルロ・ゼン(原作) 篠月しのぶ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第百五章：再編Ⅷ</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>デスゲームに巻き込まれた山本さん、気ままにゲームバランスを崩壊させる</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>ぽち(原作) カモトタツヤ(作画) 久賀フーナ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>魔石グルメ　魔物の力を食べたオレは最強！</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>菅原健二(作画) 結城涼(原作) 成瀬ちさと(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第66話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>魔王になったので、ダンジョン造って人外娘とほのぼのする</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>遠野ノオト(作画) 流優(原作) だぶ竜(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第81話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>空野進 sorani ファルまろ</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第9話　最弱貴族、暗躍する（４）</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>転生したらスライムだった件 異聞 ～魔国暮らしのトリニティ～</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>伏瀬 戸野タエ みっつばー</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第105話　帰国！［後編］</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>双子まとめて『カノジョ』にしない？</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>飴色みそ(漫画) 白井ムク(原作) 千種みのり(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第12話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>デスマーチからはじまる異世界狂想曲</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>あやめぐむ(作画) 愛七ひろ(原作) ｓｈｒｉ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第126話</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>極振り拒否して手探りスタート！　特化しないヒーラー、仲間と別れて旅に出る</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>蒼井一秀(作画) 刻一(原作) MIYA*KI(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第63話</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>貧乏騎士に嫁入りしたはずが!? ~野人令嬢は皇太子妃になっても竜を狩りたい~</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>漫画：夏川そぞろ 原作：宮前葵 キャラクター原案：ののまろ</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第10話①皇太子妃（仮）</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>となりの席のヤツがそういう目で見てくる</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>mmk</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第38話 読解力</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>ヘルモード ～やり込み好きのゲーマーは廃設定の異世界で無双する～ はじまりの召喚士</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>原作：ハム男・藻 漫画：鉄田猿児</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>GAME 080　協力</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>放課後はケンカ最強のギャルに連れこまれる生活 彼女たちに好かれて、僕も最強に!?</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>亜逸(原作) あおやぎ孝夫(作画) ｋａｋａｏ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第15話</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>【悲報】清楚系で売っていた底辺配信者、うっかり配信を切り忘れたままSS級モンスターを拳で殴り飛ばしてしまう</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>アトハ NEO草野 pupps</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第４話　【悲報】ご乱行⁉ ダンジョンシーカー・アカデミー！（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>ガルルガール</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>原聡志(著者)</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第14話</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>どうやら私の身体は完全無敵のようですね</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>さばねこ(作画) ちゃつふさ(原作) ふーみ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第78話</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>規格外のダンジョン攻略者、実は異世界帰りの元勇者</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>作画：やまざき君 原作：榊与一</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第3話(2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>異世界ゆるっとサバイバル生活～学校の皆と異世界の無人島に転移したけど俺だけ楽勝です～</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>西尾洋一(作画) 絢乃(原作) 乾和音(キャラクター原案) 株式会社一二三書房(監修)</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第48話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第33話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>放課後、ファミレスで、クラスのあの子と。</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>麦子(漫画) 左リュウ(原作) magako(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第10話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>俺のクラスに若返った元嫁がいる</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>原作：猫又　ぬこ 漫画：akn坊 キャラクター原案：緑川　葉</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>最終話（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第1話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>町人Aは悪役令嬢をどうしても救いたい　～どぶと空と氷の姫君～</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>原作：一色孝太郎・Parum 漫画：目黒三吉</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第37話 軍議</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第8話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>継母の連れ子が元カノだった</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>草壁レイ(作画) 紙城境介(原作) たかやKi(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第60話④</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>村人ですが何か？</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>鯖夢(作画) 白石新(原案・監修) 白蘇ふぁみ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第90話</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>おまけ62</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>とにかくウケたいぼっち女子(仮)</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>佐藤ショーキ</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>鋭意製作中です。</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>戦姫サバイバルサガ-異世界の運命をかけた無人島フジュン異性交遊-</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>OTOSAMA(著者)</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第16話</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>斎藤義龍に生まれ変わったので、織田信長に国譲りして長生きするのを目指します！</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>巽未頼 田村ゆうき マキムラシュンスケ</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第70話「影」</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>異世界でスキルを解体したらチートな嫁が増殖しました 概念交差のストラクチャー</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>カタセミナミ(作画) 千月さかき(原作) 東西(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第78話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>ギャルゲーマーに褒められたい</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>げしゅまろ(著者)</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>32話</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>直径3cmの召喚陣&lt;リミットリング&gt;で「雑魚すら呼べない」と蔑まれた底辺召喚士が頂点に立つまで</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>作画：まっつー 原作：空松蓮司</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第3話(2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>ルパン三世 異世界の姫君（ネイバーワールドプリンセス）</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>モンキー・パンチ／エム・ピー・ワークス 内々けやき 佐伯庸介 白狼</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第98話：泥棒、心を盗めど縛りはせず❶</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>ポンコツ勇者パーティー、竜をひろう</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>優風(著者)</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第2話</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>転校先の清楚可憐な美少女が、昔男子と思って一緒に遊んだ幼馴染だった件</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>大山樹奈(作画) 雲雀湯(原作) シソ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>最終話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>後宮メイドの災難～人使いの荒い宮廷書記官と推理する～</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>大野ちた 永井青</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>8話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>アザミヤコを好きになる</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>ユニティコング(原作) ツノニガウ(作画)</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>休載イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>おねえさんと猫を飼う</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>上杉響士郎(著者)</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第1話：おねえさんと猫を拾う</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>辺境都市の育成者</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>日高(著者) 七野りく(原作) 福きつね(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第30編②</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>六姫は神護衛に恋をする　～最強の守護騎士、転生して魔法学園に行く～</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>漫画:加古山 寿 原案:朱月 十話 キャラクター原案:てつぶた</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第121話　解決策</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>モブだけど最強を目指します！　～ゲーム世界に転生した俺は自由に強さを追い求める～</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>反面教師(原作) 五條さやか(作画) 大熊猫介(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第11話</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>没落予定なので、鍛冶職人を目指す</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>石田彩(作画) CK(原作) かわく(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第99話-2</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ワンパンマン</t>
+          <t>異世界おじさん</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>原作/ＯＮＥ 作画/村田雄介</t>
+          <t>殆ど死んでいる(著者)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>201撃目</t>
+          <t>第69話</t>
         </is>
       </c>
     </row>
@@ -4691,17 +5733,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ぽんドロイド！ はまさん</t>
+          <t>魔術師クノンは見えている</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>はれやまはれぞう(著者)</t>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第1話</t>
+          <t>第38話①</t>
         </is>
       </c>
     </row>
@@ -4711,17 +5753,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>物語の黒幕に転生して</t>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第31話</t>
+          <t>第16話後半：「ストリア見聞録」</t>
         </is>
       </c>
     </row>
@@ -4731,17 +5773,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+          <t>ダンジョンの幼なじみ</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>村上よしゆき 茨木野 あるてら</t>
+          <t>久真やすひさ(著者)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第４０話　勇者、聖女と元聖騎士と再会し、魚人を追っ払う（２）</t>
+          <t>第54話</t>
         </is>
       </c>
     </row>
@@ -4751,17 +5793,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ゲーム悪役貴族に転生した俺は、チート筋肉で無双する</t>
+          <t>淫獄団地</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>昼行燈（原作） しいたけ元帥（漫画）</t>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第24話</t>
+          <t>第48話（前編）</t>
         </is>
       </c>
     </row>
@@ -4771,17 +5813,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>俺以外誰も採取できない素材なのに「素材採取率が低い」とパワハラする幼馴染錬金術師と絶縁した専属魔導士、辺境の町でスローライフを送りたい。</t>
+          <t>異世界のんびり農家</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>狐御前(原作) 西岡知三(作画) ＮＯＣＯ(キャラクター原案)</t>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第23話-1</t>
+          <t>第301話</t>
         </is>
       </c>
     </row>
@@ -4791,17 +5833,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>バーサス</t>
+          <t>ダークサモナーとデキている</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
+          <t>車王(著者)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第25話 超越（2）</t>
+          <t>第72話</t>
         </is>
       </c>
     </row>
@@ -4811,17 +5853,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>幼女戦記</t>
+          <t>まんきつしたい常連さん</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>東條チカ(漫画) カルロ・ゼン(原作) 篠月しのぶ(キャラクター原案)</t>
+          <t>しんみりん(著者)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第百五章：再編Ⅷ</t>
+          <t>第45話前編</t>
         </is>
       </c>
     </row>
@@ -4831,17 +5873,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>デスゲームに巻き込まれた山本さん、気ままにゲームバランスを崩壊させる</t>
+          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>ぽち(原作) カモトタツヤ(作画) 久賀フーナ(キャラクター原案)</t>
+          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第5話</t>
+          <t>第22話</t>
         </is>
       </c>
     </row>
@@ -4851,17 +5893,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>魔石グルメ　魔物の力を食べたオレは最強！</t>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>菅原健二(作画) 結城涼(原作) 成瀬ちさと(キャラクター原案)</t>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第66話後半</t>
+          <t>第80話その1</t>
         </is>
       </c>
     </row>
@@ -4871,17 +5913,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>魔王になったので、ダンジョン造って人外娘とほのぼのする</t>
+          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>遠野ノオト(作画) 流優(原作) だぶ竜(キャラクター原案)</t>
+          <t>FUNA 東西 モトエ恵介</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第81話後半</t>
+          <t>第118話　会談［その3］</t>
         </is>
       </c>
     </row>
@@ -4891,17 +5933,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>空野進 sorani ファルまろ</t>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第9話　最弱貴族、暗躍する（４）</t>
+          <t>第70話(前編) 特別報酬ミッション</t>
         </is>
       </c>
     </row>
@@ -4911,17 +5953,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>転生したらスライムだった件 異聞 ～魔国暮らしのトリニティ～</t>
+          <t>ワンパンマン</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>伏瀬 戸野タエ みっつばー</t>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第105話　帰国！［後編］</t>
+          <t>201撃目</t>
         </is>
       </c>
     </row>
@@ -4931,17 +5973,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>双子まとめて『カノジョ』にしない？</t>
+          <t>ぽんドロイド！ はまさん</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>飴色みそ(漫画) 白井ムク(原作) 千種みのり(キャラクター原案)</t>
+          <t>はれやまはれぞう(著者)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第12話③</t>
+          <t>第1話</t>
         </is>
       </c>
     </row>
@@ -4951,17 +5993,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>デスマーチからはじまる異世界狂想曲</t>
+          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>あやめぐむ(作画) 愛七ひろ(原作) ｓｈｒｉ(キャラクター原案)</t>
+          <t>神原絵理華(漫画) 一森一輝(原作)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第126話</t>
+          <t>第17話②</t>
         </is>
       </c>
     </row>
@@ -4971,17 +6013,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>極振り拒否して手探りスタート！　特化しないヒーラー、仲間と別れて旅に出る</t>
+          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>蒼井一秀(作画) 刻一(原作) MIYA*KI(キャラクター原案)</t>
+          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第63話</t>
+          <t>第72話 リレー</t>
         </is>
       </c>
     </row>
@@ -4991,17 +6033,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>貧乏騎士に嫁入りしたはずが!? ~野人令嬢は皇太子妃になっても竜を狩りたい~</t>
+          <t>冒険者絶対殺すダンジョン</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>漫画：夏川そぞろ 原作：宮前葵 キャラクター原案：ののまろ</t>
+          <t>道満晴明(著者)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第10話①皇太子妃（仮）</t>
+          <t>第33話</t>
         </is>
       </c>
     </row>
@@ -5011,17 +6053,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>となりの席のヤツがそういう目で見てくる</t>
+          <t>仕事帰り、独身の美人上司に頼まれて</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>mmk</t>
+          <t>望公太(原作) とんのすけ(作画) しの(キャラクター原案)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第38話 読解力</t>
+          <t>第19話-1</t>
         </is>
       </c>
     </row>
@@ -5031,17 +6073,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ヘルモード ～やり込み好きのゲーマーは廃設定の異世界で無双する～ はじまりの召喚士</t>
+          <t>未実装のラスボス達が仲間になりました。</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>原作：ハム男・藻 漫画：鉄田猿児</t>
+          <t>緋呂河とも(漫画) ながワサビ64(原作) かわく(キャラクター原案)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>GAME 080　協力</t>
+          <t>第31話</t>
         </is>
       </c>
     </row>
@@ -5051,17 +6093,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>放課後はケンカ最強のギャルに連れこまれる生活 彼女たちに好かれて、僕も最強に!?</t>
+          <t>センパイ、自宅警備員の雇用はいかがですか？</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>亜逸(原作) あおやぎ孝夫(作画) ｋａｋａｏ(キャラクター原案)</t>
+          <t>漫画：コブラサナギ 原作：二上圭 キャラ原案：日向あずり</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第15話</t>
+          <t>第4話後半</t>
         </is>
       </c>
     </row>
@@ -5071,17 +6113,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>【悲報】清楚系で売っていた底辺配信者、うっかり配信を切り忘れたままSS級モンスターを拳で殴り飛ばしてしまう</t>
+          <t>ヤンデレかと思ったらもっとヤベー女だった</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>アトハ NEO草野 pupps</t>
+          <t>八木戸マト</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第４話　【悲報】ご乱行⁉ ダンジョンシーカー・アカデミー！（１）</t>
+          <t>第64話　しっかり「見てた」ヤンデレ彼女②</t>
         </is>
       </c>
     </row>
@@ -5091,17 +6133,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ガルルガール</t>
+          <t>スキルがなければレベルを上げる～９９がカンストの世界でレベル800万からスタート～</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>原聡志(著者)</t>
+          <t>倉橋ユウス(漫画) 岡沢六十四(原作)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第14話</t>
+          <t>第50話④</t>
         </is>
       </c>
     </row>
@@ -5111,17 +6153,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>どうやら私の身体は完全無敵のようですね</t>
+          <t>断れない会長は友江くんにだけしてあげたい</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>さばねこ(作画) ちゃつふさ(原作) ふーみ(キャラクター原案)</t>
+          <t>沼地どろまる(著者)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第78話</t>
+          <t>特別編</t>
         </is>
       </c>
     </row>
@@ -5131,17 +6173,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>規格外のダンジョン攻略者、実は異世界帰りの元勇者</t>
+          <t>修羅幼女の英雄譚～半端者と言われた傭兵、幼女に転生して成り上がる～</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>作画：やまざき君 原作：榊与一</t>
+          <t>作画：むらたん 原作：沙城流</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第3話(2)</t>
+          <t>第6話(2)</t>
         </is>
       </c>
     </row>
@@ -5151,17 +6193,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>異世界ゆるっとサバイバル生活～学校の皆と異世界の無人島に転移したけど俺だけ楽勝です～</t>
+          <t>異世界はスマートフォンとともに。</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>西尾洋一(作画) 絢乃(原作) 乾和音(キャラクター原案) 株式会社一二三書房(監修)</t>
+          <t>そと(漫画) 冬原パトラ(原作) 兎塚エイジ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第48話-2</t>
+          <t>EPISODE:102‐①</t>
         </is>
       </c>
     </row>
@@ -5171,17 +6213,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+          <t>わたし、二番目の彼女でいいから。</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+          <t>にの子(漫画) 西条陽(原作) Re岳(キャラクター原案)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第33話①</t>
+          <t>第10話②：カーテンのなか</t>
         </is>
       </c>
     </row>
@@ -5191,17 +6233,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>放課後、ファミレスで、クラスのあの子と。</t>
+          <t>時森さんが無防備です!!</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>麦子(漫画) 左リュウ(原作) magako(キャラクター原案)</t>
+          <t>たざわ</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第10話②</t>
+          <t>第61話</t>
         </is>
       </c>
     </row>
@@ -5211,17 +6253,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>俺のクラスに若返った元嫁がいる</t>
+          <t>ダウナーお姉さんは遊びたい</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>原作：猫又　ぬこ 漫画：akn坊 キャラクター原案：緑川　葉</t>
+          <t>山鷹景</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>最終話（後編）</t>
+          <t>第11話</t>
         </is>
       </c>
     </row>
@@ -5231,17 +6273,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
+          <t>くじ引き特賞：無双ハーレム権</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
+          <t>原作／三木なずな（GA文庫／SBクリエイティブ刊） 漫画／長谷見亮 キャラクター原案／瑠奈璃亜</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第1話②</t>
+          <t>第57話-02　聖なる剣と呪われし炎、信念の決着!!</t>
         </is>
       </c>
     </row>
@@ -5251,17 +6293,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>町人Aは悪役令嬢をどうしても救いたい　～どぶと空と氷の姫君～</t>
+          <t>クラスの大嫌いな女子と結婚することになった。</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>原作：一色孝太郎・Parum 漫画：目黒三吉</t>
+          <t>天乃聖樹(原作) もすこんぶ(漫画)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第37話 軍議</t>
+          <t>第43話-2</t>
         </is>
       </c>
     </row>
@@ -5271,17 +6313,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+          <t>ボクの理想の異世界生活 ～転生したらケモ耳娘だらけの世界でハーレムに～</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+          <t>イチリ(原作) 空維深夜(作画)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第8話-2</t>
+          <t>第14話後半：存在分裂</t>
         </is>
       </c>
     </row>
@@ -5291,17 +6333,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>継母の連れ子が元カノだった</t>
+          <t>脱稿するまでオチません</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>草壁レイ(作画) 紙城境介(原作) たかやKi(キャラクター原案)</t>
+          <t>ヨシラギ(著者)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第60話④</t>
+          <t>第31話後半</t>
         </is>
       </c>
     </row>
@@ -5311,17 +6353,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>村人ですが何か？</t>
+          <t>俺の愛娘は悪役令嬢</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>鯖夢(作画) 白石新(原案・監修) 白蘇ふぁみ(キャラクター原案)</t>
+          <t>かわもり かぐら(原作) ほづみりや(漫画) 縞(キャラクター原案)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第90話</t>
+          <t>第3話-2</t>
         </is>
       </c>
     </row>
@@ -5331,17 +6373,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>実は俺、最強でした？</t>
+          <t>勇者パーティから追い出された不遇職【罠士】、ユニークスキル【矢印】で最強になる</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>原作：澄守 彩 漫画：高橋 愛</t>
+          <t>作画：たつひこ 原作：白石 有希</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>おまけ62</t>
+          <t>第6話(2)</t>
         </is>
       </c>
     </row>
@@ -5351,17 +6393,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>とにかくウケたいぼっち女子(仮)</t>
+          <t>クラスメイトは異世界で勇者になったけど、俺だけ現代日本に置き去りにされました</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>佐藤ショーキ</t>
+          <t>カボチャマスク(原作) 仲紙(漫画)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>鋭意製作中です。</t>
+          <t>第9話-2</t>
         </is>
       </c>
     </row>
@@ -5371,17 +6413,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>戦姫サバイバルサガ-異世界の運命をかけた無人島フジュン異性交遊-</t>
+          <t>その冒険者、取り扱い注意。 ～正体は無敵の下僕たちを統べる異世界最強の魔導王～</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>OTOSAMA(著者)</t>
+          <t>満月シオン(作画) Sin Guilty(ツギクル)(原作) M.B(キャラクター原案)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第16話</t>
+          <t>55章　はじまりの愚か者①　後編</t>
         </is>
       </c>
     </row>
@@ -5391,17 +6433,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>斎藤義龍に生まれ変わったので、織田信長に国譲りして長生きするのを目指します！</t>
+          <t>双子の姉が神子として引き取られて、私は捨てられたけど多分私が神子である。</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>巽未頼 田村ゆうき マキムラシュンスケ</t>
+          <t>雪(著者) 池中織奈(原作) カット(キャラクター原案)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第70話「影」</t>
+          <t>第31話後編</t>
         </is>
       </c>
     </row>
@@ -5411,17 +6453,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>異世界でスキルを解体したらチートな嫁が増殖しました 概念交差のストラクチャー</t>
+          <t>物語の黒幕に転生して</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>カタセミナミ(作画) 千月さかき(原作) 東西(キャラクター原案)</t>
+          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第78話-2</t>
+          <t>第31話</t>
         </is>
       </c>
     </row>
@@ -5431,17 +6473,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>ギャルゲーマーに褒められたい</t>
+          <t>ただの村人の僕が、三百年前の暴君皇子に転生してしまいました　～前世の知識で暗殺フラグを回避して、穏やかに生き残ります！～</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>げしゅまろ(著者)</t>
+          <t>た介(漫画) サンボン(原作) 夕子(キャラクター原案)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>32話</t>
+          <t>第2話</t>
         </is>
       </c>
     </row>
@@ -5451,17 +6493,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>直径3cmの召喚陣&lt;リミットリング&gt;で「雑魚すら呼べない」と蔑まれた底辺召喚士が頂点に立つまで</t>
+          <t>俺以外誰も採取できない素材なのに「素材採取率が低い」とパワハラする幼馴染錬金術師と絶縁した専属魔導士、辺境の町でスローライフを送りたい。</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>作画：まっつー 原作：空松蓮司</t>
+          <t>狐御前(原作) 西岡知三(作画) ＮＯＣＯ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第3話(2)</t>
+          <t>第23話-1</t>
         </is>
       </c>
     </row>
@@ -5471,17 +6513,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>ルパン三世 異世界の姫君（ネイバーワールドプリンセス）</t>
+          <t>ギルドを追放された回復術士、実は魔力無限だったので規格外の回復魔法で伝説となる</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>モンキー・パンチ／エム・ピー・ワークス 内々けやき 佐伯庸介 白狼</t>
+          <t>漫画：坂下コウ 原作：霞杏檎</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第98話：泥棒、心を盗めど縛りはせず❶</t>
+          <t>第3話(1)</t>
         </is>
       </c>
     </row>
@@ -5491,17 +6533,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>ポンコツ勇者パーティー、竜をひろう</t>
+          <t>転生して成長チートを手に入れたら、最凶スキルもついたのですが!?</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>優風(著者)</t>
+          <t>やま ゆずもと 我美蘭</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第2話</t>
+          <t>第9話</t>
         </is>
       </c>
     </row>
@@ -5511,17 +6553,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>転校先の清楚可憐な美少女が、昔男子と思って一緒に遊んだ幼馴染だった件</t>
+          <t>レベル１から始まる召喚無双</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>大山樹奈(作画) 雲雀湯(原作) シソ(キャラクター原案)</t>
+          <t>漫画：七桃りお 原作：白石新 キャラクター原案：夕薙</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>最終話-2</t>
+          <t>コミックス7巻特典情報</t>
         </is>
       </c>
     </row>
@@ -5531,17 +6573,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>後宮メイドの災難～人使いの荒い宮廷書記官と推理する～</t>
+          <t>デスゲームに巻き込まれた山本さん、気ままにゲームバランスを崩壊させる</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>大野ちた 永井青</t>
+          <t>ぽち(原作) カモトタツヤ(作画) 久賀フーナ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>8話③</t>
+          <t>第5話</t>
         </is>
       </c>
     </row>
@@ -5551,17 +6593,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>アザミヤコを好きになる</t>
+          <t>バーサス</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>ユニティコング(原作) ツノニガウ(作画)</t>
+          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>休載イラスト</t>
+          <t>第25話 超越（2）</t>
         </is>
       </c>
     </row>
@@ -5571,17 +6613,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>おねえさんと猫を飼う</t>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>上杉響士郎(著者)</t>
+          <t>村上よしゆき 茨木野 あるてら</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第1話：おねえさんと猫を拾う</t>
+          <t>第４０話　勇者、聖女と元聖騎士と再会し、魚人を追っ払う（２）</t>
         </is>
       </c>
     </row>
@@ -5591,17 +6633,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>辺境都市の育成者</t>
+          <t>錬金術師の辺境再生スローライフ～S級パーティーで孤立した少女をかばったら追放されたので、一緒に幸せに暮らします～</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>日高(著者) 七野りく(原作) 福きつね(キャラクター原案)</t>
+          <t>作画：弥永扇 原作：三月菫</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第30編②</t>
+          <t>第6話(2)</t>
         </is>
       </c>
     </row>
@@ -5611,17 +6653,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>六姫は神護衛に恋をする　～最強の守護騎士、転生して魔法学園に行く～</t>
+          <t>殺されたらゾンビになったので、進化しまくって無双しようと思います</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>漫画:加古山 寿 原案:朱月 十話 キャラクター原案:てつぶた</t>
+          <t>漫画：朝ケ夜 原作：幸運ピエロ キャラクター原案：東西</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第121話　解決策</t>
+          <t>第15話(前半)暴走ドラゴンと魔剣①</t>
         </is>
       </c>
     </row>
@@ -5631,17 +6673,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>モブだけど最強を目指します！　～ゲーム世界に転生した俺は自由に強さを追い求める～</t>
+          <t>幼女戦記</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>反面教師(原作) 五條さやか(作画) 大熊猫介(キャラクター原案)</t>
+          <t>東條チカ(漫画) カルロ・ゼン(原作) 篠月しのぶ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第11話</t>
+          <t>第百五章：再編Ⅷ</t>
         </is>
       </c>
     </row>
@@ -5651,17 +6693,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>没落予定なので、鍛冶職人を目指す</t>
+          <t>追放されたおっさんタンク、実は防御力最強だったのでダメージゼロで無双する</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>石田彩(作画) CK(原作) かわく(キャラクター原案)</t>
+          <t>漫画：化野九十九 原作：あけちともあき</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第99話-2</t>
+          <t>第3話(1)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-06-29
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -13,6 +13,7 @@
     <sheet name="2025-06-26" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="2025-06-27" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="2025-06-28" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="2025-06-29" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -5708,22 +5709,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>異世界おじさん</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>殆ど死んでいる(著者)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第69話</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>魔術師クノンは見えている</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第38話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第16話後半：「ストリア見聞録」</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>ダンジョンの幼なじみ</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>久真やすひさ(著者)</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第54話</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>淫獄団地</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第48話（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>異世界のんびり農家</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第301話</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>ダークサモナーとデキている</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>車王(著者)</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第72話</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>まんきつしたい常連さん</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>しんみりん(著者)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第45話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第22話</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第80話その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>FUNA 東西 モトエ恵介</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第118話　会談［その3］</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第70話(前編) 特別報酬ミッション</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>ワンパンマン</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>201撃目</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>ぽんドロイド！ はまさん</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>はれやまはれぞう(著者)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第1話</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>神原絵理華(漫画) 一森一輝(原作)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第17話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第72話 リレー</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>冒険者絶対殺すダンジョン</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>道満晴明(著者)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第33話</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>仕事帰り、独身の美人上司に頼まれて</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>望公太(原作) とんのすけ(作画) しの(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第19話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>未実装のラスボス達が仲間になりました。</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>緋呂河とも(漫画) ながワサビ64(原作) かわく(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第31話</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>センパイ、自宅警備員の雇用はいかがですか？</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>漫画：コブラサナギ 原作：二上圭 キャラ原案：日向あずり</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第4話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>ヤンデレかと思ったらもっとヤベー女だった</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>八木戸マト</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第64話　しっかり「見てた」ヤンデレ彼女②</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>スキルがなければレベルを上げる～９９がカンストの世界でレベル800万からスタート～</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>倉橋ユウス(漫画) 岡沢六十四(原作)</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第50話④</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>断れない会長は友江くんにだけしてあげたい</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>沼地どろまる(著者)</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>特別編</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>修羅幼女の英雄譚～半端者と言われた傭兵、幼女に転生して成り上がる～</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>作画：むらたん 原作：沙城流</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第6話(2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>異世界はスマートフォンとともに。</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>そと(漫画) 冬原パトラ(原作) 兎塚エイジ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>EPISODE:102‐①</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>わたし、二番目の彼女でいいから。</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>にの子(漫画) 西条陽(原作) Re岳(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第10話②：カーテンのなか</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>時森さんが無防備です!!</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>たざわ</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第61話</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>ダウナーお姉さんは遊びたい</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>山鷹景</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第11話</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>くじ引き特賞：無双ハーレム権</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>原作／三木なずな（GA文庫／SBクリエイティブ刊） 漫画／長谷見亮 キャラクター原案／瑠奈璃亜</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第57話-02　聖なる剣と呪われし炎、信念の決着!!</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>クラスの大嫌いな女子と結婚することになった。</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>天乃聖樹(原作) もすこんぶ(漫画)</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第43話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>ボクの理想の異世界生活 ～転生したらケモ耳娘だらけの世界でハーレムに～</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>イチリ(原作) 空維深夜(作画)</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第14話後半：存在分裂</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>脱稿するまでオチません</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>ヨシラギ(著者)</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第31話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>俺の愛娘は悪役令嬢</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>かわもり かぐら(原作) ほづみりや(漫画) 縞(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第3話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティから追い出された不遇職【罠士】、ユニークスキル【矢印】で最強になる</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>作画：たつひこ 原作：白石 有希</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第6話(2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>クラスメイトは異世界で勇者になったけど、俺だけ現代日本に置き去りにされました</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>カボチャマスク(原作) 仲紙(漫画)</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第9話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>その冒険者、取り扱い注意。 ～正体は無敵の下僕たちを統べる異世界最強の魔導王～</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>満月シオン(作画) Sin Guilty(ツギクル)(原作) M.B(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>55章　はじまりの愚か者①　後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>双子の姉が神子として引き取られて、私は捨てられたけど多分私が神子である。</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>雪(著者) 池中織奈(原作) カット(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第31話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>物語の黒幕に転生して</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第31話</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>ただの村人の僕が、三百年前の暴君皇子に転生してしまいました　～前世の知識で暗殺フラグを回避して、穏やかに生き残ります！～</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>た介(漫画) サンボン(原作) 夕子(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第2話</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>俺以外誰も採取できない素材なのに「素材採取率が低い」とパワハラする幼馴染錬金術師と絶縁した専属魔導士、辺境の町でスローライフを送りたい。</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>狐御前(原作) 西岡知三(作画) ＮＯＣＯ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第23話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>ギルドを追放された回復術士、実は魔力無限だったので規格外の回復魔法で伝説となる</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>漫画：坂下コウ 原作：霞杏檎</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第3話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>転生して成長チートを手に入れたら、最凶スキルもついたのですが!?</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>やま ゆずもと 我美蘭</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第9話</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>レベル１から始まる召喚無双</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>漫画：七桃りお 原作：白石新 キャラクター原案：夕薙</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>コミックス7巻特典情報</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>デスゲームに巻き込まれた山本さん、気ままにゲームバランスを崩壊させる</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>ぽち(原作) カモトタツヤ(作画) 久賀フーナ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>バーサス</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第25話 超越（2）</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>村上よしゆき 茨木野 あるてら</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第４０話　勇者、聖女と元聖騎士と再会し、魚人を追っ払う（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>錬金術師の辺境再生スローライフ～S級パーティーで孤立した少女をかばったら追放されたので、一緒に幸せに暮らします～</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>作画：弥永扇 原作：三月菫</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第6話(2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>殺されたらゾンビになったので、進化しまくって無双しようと思います</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>漫画：朝ケ夜 原作：幸運ピエロ キャラクター原案：東西</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第15話(前半)暴走ドラゴンと魔剣①</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>幼女戦記</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>東條チカ(漫画) カルロ・ゼン(原作) 篠月しのぶ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第百五章：再編Ⅷ</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>追放されたおっさんタンク、実は防御力最強だったのでダメージゼロで無双する</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>漫画：化野九十九 原作：あけちともあき</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第3話(1)</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>異世界おじさん</t>
+          <t>クセ強彼女は床にいざなう</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>殆ど死んでいる(著者)</t>
+          <t>須河篤志(著者)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第69話</t>
+          <t>第13話前半</t>
         </is>
       </c>
     </row>
@@ -5733,17 +6775,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>魔術師クノンは見えている</t>
+          <t>リビルドワールド</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第38話①</t>
+          <t>第70話③</t>
         </is>
       </c>
     </row>
@@ -5753,17 +6795,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+          <t>ぽんドロイド！ はまさん</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+          <t>はれやまはれぞう(著者)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第16話後半：「ストリア見聞録」</t>
+          <t>第2話</t>
         </is>
       </c>
     </row>
@@ -5773,17 +6815,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ダンジョンの幼なじみ</t>
+          <t>異世界おじさん</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>久真やすひさ(著者)</t>
+          <t>殆ど死んでいる(著者)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第54話</t>
+          <t>第69話</t>
         </is>
       </c>
     </row>
@@ -5793,17 +6835,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>淫獄団地</t>
+          <t>サーシャちゃんとクラスメイトオタクくん</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+          <t>はぐはぐ(著者)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第48話（前編）</t>
+          <t>第80話</t>
         </is>
       </c>
     </row>
@@ -5813,17 +6855,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>異世界のんびり農家</t>
+          <t>田舎の黒ギャルJKと結婚しました</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+          <t>カヅチ(著者)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第301話</t>
+          <t>第16話後半</t>
         </is>
       </c>
     </row>
@@ -5833,17 +6875,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ダークサモナーとデキている</t>
+          <t>オトナを知りたい女友達</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>車王(著者)</t>
+          <t>望公太(原作) ぷよちゃ(作画)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第72話</t>
+          <t>第7話 前半</t>
         </is>
       </c>
     </row>
@@ -5853,17 +6895,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>まんきつしたい常連さん</t>
+          <t>魔術師クノンは見えている</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>しんみりん(著者)</t>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第45話前編</t>
+          <t>第38話①</t>
         </is>
       </c>
     </row>
@@ -5873,17 +6915,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
+          <t>聖液鍛冶屋のエロランタ</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
+          <t>しげきっくす(著者)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第22話</t>
+          <t>第6話後半</t>
         </is>
       </c>
     </row>
@@ -5893,17 +6935,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第80話その1</t>
+          <t>第16話後半：「ストリア見聞録」</t>
         </is>
       </c>
     </row>
@@ -5913,17 +6955,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+          <t>ミルク搾りハンターの異世界搾乳記～農家の冴えない男があらゆる種族の地区Bを弄び虜にする～</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>FUNA 東西 モトエ恵介</t>
+          <t>空詠大智(著者)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第118話　会談［その3］</t>
+          <t>第15話前半</t>
         </is>
       </c>
     </row>
@@ -5933,17 +6975,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+          <t>転生してあらゆるモノに好かれながら異世界で好きな事をして生きて行く</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+          <t>都尾琉(漫画) 御峰。(原作)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第70話(前編) 特別報酬ミッション</t>
+          <t>第25話④</t>
         </is>
       </c>
     </row>
@@ -5953,17 +6995,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ワンパンマン</t>
+          <t>無敵商人の異世界成り上がり物語 ～現代の製品を自在に取り寄せるスキルがあるので異世界では楽勝です～</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>原作/ＯＮＥ 作画/村田雄介</t>
+          <t>隆原ヒロタ(漫画) 青山有(原作) ぷきゅのすけ(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>201撃目</t>
+          <t>第34話③</t>
         </is>
       </c>
     </row>
@@ -5973,17 +7015,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ぽんドロイド！ はまさん</t>
+          <t>ダンジョンの幼なじみ</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>はれやまはれぞう(著者)</t>
+          <t>久真やすひさ(著者)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第1話</t>
+          <t>第54話</t>
         </is>
       </c>
     </row>
@@ -5993,17 +7035,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
+          <t>淫獄団地</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>神原絵理華(漫画) 一森一輝(原作)</t>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第17話②</t>
+          <t>第48話（前編）</t>
         </is>
       </c>
     </row>
@@ -6013,17 +7055,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
+          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
+          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第72話 リレー</t>
+          <t>第22話</t>
         </is>
       </c>
     </row>
@@ -6033,17 +7075,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>冒険者絶対殺すダンジョン</t>
+          <t>ダークサモナーとデキている</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>道満晴明(著者)</t>
+          <t>車王(著者)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第33話</t>
+          <t>第72話</t>
         </is>
       </c>
     </row>
@@ -6053,17 +7095,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>仕事帰り、独身の美人上司に頼まれて</t>
+          <t>異世界のんびり農家</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>望公太(原作) とんのすけ(作画) しの(キャラクター原案)</t>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第19話-1</t>
+          <t>第301話</t>
         </is>
       </c>
     </row>
@@ -6073,17 +7115,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>未実装のラスボス達が仲間になりました。</t>
+          <t>まんきつしたい常連さん</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>緋呂河とも(漫画) ながワサビ64(原作) かわく(キャラクター原案)</t>
+          <t>しんみりん(著者)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第31話</t>
+          <t>第45話前編</t>
         </is>
       </c>
     </row>
@@ -6093,17 +7135,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>センパイ、自宅警備員の雇用はいかがですか？</t>
+          <t>ワンパンマン</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>漫画：コブラサナギ 原作：二上圭 キャラ原案：日向あずり</t>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第4話後半</t>
+          <t>201撃目</t>
         </is>
       </c>
     </row>
@@ -6113,17 +7155,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>ヤンデレかと思ったらもっとヤベー女だった</t>
+          <t>愚かな天使は悪魔と踊る</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>八木戸マト</t>
+          <t>アズマサワヨシ(著者)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第64話　しっかり「見てた」ヤンデレ彼女②</t>
+          <t>第99話③</t>
         </is>
       </c>
     </row>
@@ -6133,17 +7175,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>スキルがなければレベルを上げる～９９がカンストの世界でレベル800万からスタート～</t>
+          <t>ギャルゲーマーに褒められたい</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>倉橋ユウス(漫画) 岡沢六十四(原作)</t>
+          <t>げしゅまろ(著者)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第50話④</t>
+          <t>34話</t>
         </is>
       </c>
     </row>
@@ -6153,17 +7195,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>断れない会長は友江くんにだけしてあげたい</t>
+          <t>花子さん、食べないで</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>沼地どろまる(著者)</t>
+          <t>茸谷きの子(著者)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>特別編</t>
+          <t>第8話後半</t>
         </is>
       </c>
     </row>
@@ -6173,17 +7215,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>修羅幼女の英雄譚～半端者と言われた傭兵、幼女に転生して成り上がる～</t>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>作画：むらたん 原作：沙城流</t>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第6話(2)</t>
+          <t>第70話(前編) 特別報酬ミッション</t>
         </is>
       </c>
     </row>
@@ -6193,17 +7235,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>異世界はスマートフォンとともに。</t>
+          <t>辺境の魔法薬師 ～自由気ままな異世界ものづくり日記～</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>そと(漫画) 冬原パトラ(原作) 兎塚エイジ(キャラクター原案)</t>
+          <t>gum(漫画) えながゆうき(原作) パルプピロシ(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>EPISODE:102‐①</t>
+          <t>第16話</t>
         </is>
       </c>
     </row>
@@ -6213,17 +7255,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>わたし、二番目の彼女でいいから。</t>
+          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>にの子(漫画) 西条陽(原作) Re岳(キャラクター原案)</t>
+          <t>FUNA 東西 モトエ恵介</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第10話②：カーテンのなか</t>
+          <t>第118話　会談［その3］</t>
         </is>
       </c>
     </row>
@@ -6233,12 +7275,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>時森さんが無防備です!!</t>
+          <t>ステータス・オール∞（インフィニティ） ∞使いの最強能力者、異世界を自由気ままに暮らします！</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>たざわ</t>
+          <t>漫画：三津屋みやこ 原作：八又ナガト</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -6253,17 +7295,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ダウナーお姉さんは遊びたい</t>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>山鷹景</t>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第11話</t>
+          <t>第80話その1</t>
         </is>
       </c>
     </row>
@@ -6273,17 +7315,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>くじ引き特賞：無双ハーレム権</t>
+          <t>ラスボスたちの隠し仔　～魔王城に転生した元社畜プログラマーは自由気ままに『魔導言語《マジックコード》』を開発する～</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>原作／三木なずな（GA文庫／SBクリエイティブ刊） 漫画／長谷見亮 キャラクター原案／瑠奈璃亜</t>
+          <t>森清士郎(漫画) 熊乃げん骨(原作)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第57話-02　聖なる剣と呪われし炎、信念の決着!!</t>
+          <t>第13話②</t>
         </is>
       </c>
     </row>
@@ -6293,17 +7335,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>クラスの大嫌いな女子と結婚することになった。</t>
+          <t>ダンジョンバンド</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>天乃聖樹(原作) もすこんぶ(漫画)</t>
+          <t>新挑限(著者)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第43話-2</t>
+          <t>♯６Hello,Again ～昔からある場所～②</t>
         </is>
       </c>
     </row>
@@ -6313,17 +7355,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ボクの理想の異世界生活 ～転生したらケモ耳娘だらけの世界でハーレムに～</t>
+          <t>本物のカノジョにしたくなるまで、私で試していいよ。</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>イチリ(原作) 空維深夜(作画)</t>
+          <t>wano(漫画) 有丈ほえる(原作) 緋月ひぐれ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第14話後半：存在分裂</t>
+          <t>今週はスペシャルイラスト第2弾!!</t>
         </is>
       </c>
     </row>
@@ -6333,17 +7375,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>脱稿するまでオチません</t>
+          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>ヨシラギ(著者)</t>
+          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第31話後半</t>
+          <t>第72話 リレー</t>
         </is>
       </c>
     </row>
@@ -6353,17 +7395,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>俺の愛娘は悪役令嬢</t>
+          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>かわもり かぐら(原作) ほづみりや(漫画) 縞(キャラクター原案)</t>
+          <t>神原絵理華(漫画) 一森一輝(原作)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第3話-2</t>
+          <t>第17話②</t>
         </is>
       </c>
     </row>
@@ -6373,17 +7415,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>勇者パーティから追い出された不遇職【罠士】、ユニークスキル【矢印】で最強になる</t>
+          <t>八男って、それはないでしょう！　みそっかす</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>作画：たつひこ 原作：白石 有希</t>
+          <t>ながを(漫画) Ｙ．Ａ(原作) 藤ちょこ(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第6話(2)</t>
+          <t>episode.エリーゼ 第4話①</t>
         </is>
       </c>
     </row>
@@ -6393,17 +7435,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>クラスメイトは異世界で勇者になったけど、俺だけ現代日本に置き去りにされました</t>
+          <t>魔物喰らい ランキング最下位の冒険者は魔物の力で最強へ</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>カボチャマスク(原作) 仲紙(漫画)</t>
+          <t>赤井ハコ(漫画) 緒二葉(原作) とよた瑣織(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第9話-2</t>
+          <t>第8話-1</t>
         </is>
       </c>
     </row>
@@ -6413,17 +7455,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>その冒険者、取り扱い注意。 ～正体は無敵の下僕たちを統べる異世界最強の魔導王～</t>
+          <t>センパイ、自宅警備員の雇用はいかがですか？</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>満月シオン(作画) Sin Guilty(ツギクル)(原作) M.B(キャラクター原案)</t>
+          <t>漫画：コブラサナギ 原作：二上圭 キャラ原案：日向あずり</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>55章　はじまりの愚か者①　後編</t>
+          <t>第4話後半</t>
         </is>
       </c>
     </row>
@@ -6433,17 +7475,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>双子の姉が神子として引き取られて、私は捨てられたけど多分私が神子である。</t>
+          <t>冒険者絶対殺すダンジョン</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>雪(著者) 池中織奈(原作) カット(キャラクター原案)</t>
+          <t>道満晴明(著者)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第31話後編</t>
+          <t>第33話</t>
         </is>
       </c>
     </row>
@@ -6453,17 +7495,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>物語の黒幕に転生して</t>
+          <t>断れない会長は友江くんにだけしてあげたい</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
+          <t>沼地どろまる(著者)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第31話</t>
+          <t>特別編</t>
         </is>
       </c>
     </row>
@@ -6473,17 +7515,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>ただの村人の僕が、三百年前の暴君皇子に転生してしまいました　～前世の知識で暗殺フラグを回避して、穏やかに生き残ります！～</t>
+          <t>ダウナーお姉さんは遊びたい</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>た介(漫画) サンボン(原作) 夕子(キャラクター原案)</t>
+          <t>山鷹景</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第2話</t>
+          <t>第11話</t>
         </is>
       </c>
     </row>
@@ -6493,17 +7535,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>俺以外誰も採取できない素材なのに「素材採取率が低い」とパワハラする幼馴染錬金術師と絶縁した専属魔導士、辺境の町でスローライフを送りたい。</t>
+          <t>わたし、二番目の彼女でいいから。</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>狐御前(原作) 西岡知三(作画) ＮＯＣＯ(キャラクター原案)</t>
+          <t>にの子(漫画) 西条陽(原作) Re岳(キャラクター原案)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第23話-1</t>
+          <t>第10話②：カーテンのなか</t>
         </is>
       </c>
     </row>
@@ -6513,17 +7555,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>ギルドを追放された回復術士、実は魔力無限だったので規格外の回復魔法で伝説となる</t>
+          <t>仕事帰り、独身の美人上司に頼まれて</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>漫画：坂下コウ 原作：霞杏檎</t>
+          <t>望公太(原作) とんのすけ(作画) しの(キャラクター原案)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第3話(1)</t>
+          <t>第19話-1</t>
         </is>
       </c>
     </row>
@@ -6533,17 +7575,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>転生して成長チートを手に入れたら、最凶スキルもついたのですが!?</t>
+          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>やま ゆずもと 我美蘭</t>
+          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第9話</t>
+          <t>第1話②</t>
         </is>
       </c>
     </row>
@@ -6553,17 +7595,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>レベル１から始まる召喚無双</t>
+          <t>未実装のラスボス達が仲間になりました。</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>漫画：七桃りお 原作：白石新 キャラクター原案：夕薙</t>
+          <t>緋呂河とも(漫画) ながワサビ64(原作) かわく(キャラクター原案)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>コミックス7巻特典情報</t>
+          <t>第31話</t>
         </is>
       </c>
     </row>
@@ -6573,17 +7615,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>デスゲームに巻き込まれた山本さん、気ままにゲームバランスを崩壊させる</t>
+          <t>殺されたらゾンビになったので、進化しまくって無双しようと思います</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>ぽち(原作) カモトタツヤ(作画) 久賀フーナ(キャラクター原案)</t>
+          <t>漫画：朝ケ夜 原作：幸運ピエロ キャラクター原案：東西</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第5話</t>
+          <t>第15話(前半)暴走ドラゴンと魔剣①</t>
         </is>
       </c>
     </row>
@@ -6593,17 +7635,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>バーサス</t>
+          <t>時森さんが無防備です!!</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
+          <t>たざわ</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第25話 超越（2）</t>
+          <t>第61話</t>
         </is>
       </c>
     </row>
@@ -6613,17 +7655,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+          <t>修羅幼女の英雄譚～半端者と言われた傭兵、幼女に転生して成り上がる～</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>村上よしゆき 茨木野 あるてら</t>
+          <t>作画：むらたん 原作：沙城流</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第４０話　勇者、聖女と元聖騎士と再会し、魚人を追っ払う（２）</t>
+          <t>第6話(2)</t>
         </is>
       </c>
     </row>
@@ -6633,17 +7675,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>錬金術師の辺境再生スローライフ～S級パーティーで孤立した少女をかばったら追放されたので、一緒に幸せに暮らします～</t>
+          <t>ボクの理想の異世界生活 ～転生したらケモ耳娘だらけの世界でハーレムに～</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>作画：弥永扇 原作：三月菫</t>
+          <t>イチリ(原作) 空維深夜(作画)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第6話(2)</t>
+          <t>第14話後半：存在分裂</t>
         </is>
       </c>
     </row>
@@ -6653,17 +7695,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>殺されたらゾンビになったので、進化しまくって無双しようと思います</t>
+          <t>ヤンデレかと思ったらもっとヤベー女だった</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>漫画：朝ケ夜 原作：幸運ピエロ キャラクター原案：東西</t>
+          <t>八木戸マト</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第15話(前半)暴走ドラゴンと魔剣①</t>
+          <t>第64話　しっかり「見てた」ヤンデレ彼女②</t>
         </is>
       </c>
     </row>
@@ -6673,17 +7715,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>幼女戦記</t>
+          <t>物語の黒幕に転生して</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>東條チカ(漫画) カルロ・ゼン(原作) 篠月しのぶ(キャラクター原案)</t>
+          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第百五章：再編Ⅷ</t>
+          <t>第31話</t>
         </is>
       </c>
     </row>
@@ -6693,17 +7735,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>追放されたおっさんタンク、実は防御力最強だったのでダメージゼロで無双する</t>
+          <t>日々は過ぎれど飯うまし</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>漫画：化野九十九 原作：あけちともあき</t>
+          <t>Quro(漫画) あっと(原案)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第3話(1)</t>
+          <t>第7話①</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-06-30
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -14,6 +14,7 @@
     <sheet name="2025-06-27" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="2025-06-28" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="2025-06-29" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="2025-06-30" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -6750,22 +6751,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>クセ強彼女は床にいざなう</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>須河篤志(著者)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第13話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第70話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>ぽんドロイド！ はまさん</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>はれやまはれぞう(著者)</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第2話</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>異世界おじさん</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>殆ど死んでいる(著者)</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第69話</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>サーシャちゃんとクラスメイトオタクくん</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>はぐはぐ(著者)</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第80話</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>田舎の黒ギャルJKと結婚しました</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>カヅチ(著者)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第16話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>オトナを知りたい女友達</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>望公太(原作) ぷよちゃ(作画)</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第7話 前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>魔術師クノンは見えている</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第38話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>聖液鍛冶屋のエロランタ</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>しげきっくす(著者)</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第6話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第16話後半：「ストリア見聞録」</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>ミルク搾りハンターの異世界搾乳記～農家の冴えない男があらゆる種族の地区Bを弄び虜にする～</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>空詠大智(著者)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第15話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>転生してあらゆるモノに好かれながら異世界で好きな事をして生きて行く</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>都尾琉(漫画) 御峰。(原作)</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第25話④</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>無敵商人の異世界成り上がり物語 ～現代の製品を自在に取り寄せるスキルがあるので異世界では楽勝です～</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>隆原ヒロタ(漫画) 青山有(原作) ぷきゅのすけ(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第34話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>ダンジョンの幼なじみ</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>久真やすひさ(著者)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第54話</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>淫獄団地</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第48話（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第22話</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>ダークサモナーとデキている</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>車王(著者)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第72話</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>異世界のんびり農家</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第301話</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>まんきつしたい常連さん</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>しんみりん(著者)</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第45話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>ワンパンマン</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>201撃目</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>愚かな天使は悪魔と踊る</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>アズマサワヨシ(著者)</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第99話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>ギャルゲーマーに褒められたい</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>げしゅまろ(著者)</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>34話</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>花子さん、食べないで</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>茸谷きの子(著者)</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第8話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第70話(前編) 特別報酬ミッション</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>辺境の魔法薬師 ～自由気ままな異世界ものづくり日記～</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>gum(漫画) えながゆうき(原作) パルプピロシ(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第16話</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>FUNA 東西 モトエ恵介</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第118話　会談［その3］</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>ステータス・オール∞（インフィニティ） ∞使いの最強能力者、異世界を自由気ままに暮らします！</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>漫画：三津屋みやこ 原作：八又ナガト</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第61話</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第80話その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>ラスボスたちの隠し仔　～魔王城に転生した元社畜プログラマーは自由気ままに『魔導言語《マジックコード》』を開発する～</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>森清士郎(漫画) 熊乃げん骨(原作)</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第13話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>ダンジョンバンド</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>新挑限(著者)</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>♯６Hello,Again ～昔からある場所～②</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>本物のカノジョにしたくなるまで、私で試していいよ。</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>wano(漫画) 有丈ほえる(原作) 緋月ひぐれ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>今週はスペシャルイラスト第2弾!!</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第72話 リレー</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>神原絵理華(漫画) 一森一輝(原作)</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第17話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>八男って、それはないでしょう！　みそっかす</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>ながを(漫画) Ｙ．Ａ(原作) 藤ちょこ(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>episode.エリーゼ 第4話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>魔物喰らい ランキング最下位の冒険者は魔物の力で最強へ</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>赤井ハコ(漫画) 緒二葉(原作) とよた瑣織(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第8話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>センパイ、自宅警備員の雇用はいかがですか？</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>漫画：コブラサナギ 原作：二上圭 キャラ原案：日向あずり</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第4話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>冒険者絶対殺すダンジョン</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>道満晴明(著者)</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第33話</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>断れない会長は友江くんにだけしてあげたい</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>沼地どろまる(著者)</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>特別編</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>ダウナーお姉さんは遊びたい</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>山鷹景</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第11話</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>わたし、二番目の彼女でいいから。</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>にの子(漫画) 西条陽(原作) Re岳(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第10話②：カーテンのなか</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>仕事帰り、独身の美人上司に頼まれて</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>望公太(原作) とんのすけ(作画) しの(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第19話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第1話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>未実装のラスボス達が仲間になりました。</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>緋呂河とも(漫画) ながワサビ64(原作) かわく(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第31話</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>殺されたらゾンビになったので、進化しまくって無双しようと思います</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>漫画：朝ケ夜 原作：幸運ピエロ キャラクター原案：東西</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第15話(前半)暴走ドラゴンと魔剣①</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>時森さんが無防備です!!</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>たざわ</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第61話</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>修羅幼女の英雄譚～半端者と言われた傭兵、幼女に転生して成り上がる～</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>作画：むらたん 原作：沙城流</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第6話(2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>ボクの理想の異世界生活 ～転生したらケモ耳娘だらけの世界でハーレムに～</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>イチリ(原作) 空維深夜(作画)</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第14話後半：存在分裂</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>ヤンデレかと思ったらもっとヤベー女だった</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>八木戸マト</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第64話　しっかり「見てた」ヤンデレ彼女②</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>物語の黒幕に転生して</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第31話</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>日々は過ぎれど飯うまし</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>Quro(漫画) あっと(原案)</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第7話①</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>クセ強彼女は床にいざなう</t>
+          <t>異世界居酒屋「のぶ」</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>須河篤志(著者)</t>
+          <t>蝉川夏哉(原作) ヴァージニア二等兵(漫画) 転(キャラクター原案)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第13話前半</t>
+          <t>第122話</t>
         </is>
       </c>
     </row>
@@ -6775,17 +7817,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>リビルドワールド</t>
+          <t>ニチアサ好きのオタクが悪役生徒に転生した結果、破滅フラグが崩壊していく件について</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+          <t>烏丸英（原作） どんぐりす（漫画）</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第70話③</t>
+          <t>第14話（後編）急襲…事件の始まり</t>
         </is>
       </c>
     </row>
@@ -6795,17 +7837,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ぽんドロイド！ はまさん</t>
+          <t>異世界おじさん</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>はれやまはれぞう(著者)</t>
+          <t>殆ど死んでいる(著者)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第2話</t>
+          <t>第69話</t>
         </is>
       </c>
     </row>
@@ -6815,17 +7857,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>異世界おじさん</t>
+          <t>クセ強彼女は床にいざなう</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>殆ど死んでいる(著者)</t>
+          <t>須河篤志(著者)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第69話</t>
+          <t>第13話前半</t>
         </is>
       </c>
     </row>
@@ -6835,17 +7877,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>サーシャちゃんとクラスメイトオタクくん</t>
+          <t>ぽんドロイド！ はまさん</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>はぐはぐ(著者)</t>
+          <t>はれやまはれぞう(著者)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第80話</t>
+          <t>第2話</t>
         </is>
       </c>
     </row>
@@ -6855,17 +7897,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>田舎の黒ギャルJKと結婚しました</t>
+          <t>はずれスキル念動力（ただしレベルＭＡＸ）で無双する～手をかざすだけです。詠唱とか必殺技とかいりません。念じるだけで倒せます～</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>カヅチ(著者)</t>
+          <t>さとう うなぽっぽ トダフミト</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第16話後半</t>
+          <t>9話①</t>
         </is>
       </c>
     </row>
@@ -6875,17 +7917,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>オトナを知りたい女友達</t>
+          <t>外来魔法生物対策課</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>望公太(原作) ぷよちゃ(作画)</t>
+          <t>端(原作) 皐月木獏(作画)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第7話 前半</t>
+          <t>第1話</t>
         </is>
       </c>
     </row>
@@ -6895,17 +7937,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>魔術師クノンは見えている</t>
+          <t>異世界迷宮のオーパーツ</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+          <t>三狛ハル(著者)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第38話①</t>
+          <t>第1話：先端にお椀がついた棒</t>
         </is>
       </c>
     </row>
@@ -6915,17 +7957,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>聖液鍛冶屋のエロランタ</t>
+          <t>転生貴族の異世界冒険録 ～カインのやりすぎギルド日記～</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>しげきっくす(著者)</t>
+          <t>原作：夜州 漫画：佐々木あかね・香本セトラ キャラクター原案：藻</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第6話後半</t>
+          <t>第47話</t>
         </is>
       </c>
     </row>
@@ -6935,17 +7977,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+          <t>ギャルゲーマーに褒められたい</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+          <t>げしゅまろ(著者)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第16話後半：「ストリア見聞録」</t>
+          <t>34話</t>
         </is>
       </c>
     </row>
@@ -6955,17 +7997,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ミルク搾りハンターの異世界搾乳記～農家の冴えない男があらゆる種族の地区Bを弄び虜にする～</t>
+          <t>リビルドワールド</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>空詠大智(著者)</t>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第15話前半</t>
+          <t>第70話③</t>
         </is>
       </c>
     </row>
@@ -6975,17 +8017,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>転生してあらゆるモノに好かれながら異世界で好きな事をして生きて行く</t>
+          <t>サーシャちゃんとクラスメイトオタクくん</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>都尾琉(漫画) 御峰。(原作)</t>
+          <t>はぐはぐ(著者)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第25話④</t>
+          <t>第80話</t>
         </is>
       </c>
     </row>
@@ -6995,17 +8037,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>無敵商人の異世界成り上がり物語 ～現代の製品を自在に取り寄せるスキルがあるので異世界では楽勝です～</t>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>隆原ヒロタ(漫画) 青山有(原作) ぷきゅのすけ(キャラクターデザイン)</t>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第34話③</t>
+          <t>第8話-2</t>
         </is>
       </c>
     </row>
@@ -7015,17 +8057,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ダンジョンの幼なじみ</t>
+          <t>魔術師クノンは見えている</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>久真やすひさ(著者)</t>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第54話</t>
+          <t>第38話①</t>
         </is>
       </c>
     </row>
@@ -7035,17 +8077,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>淫獄団地</t>
+          <t>田舎の黒ギャルJKと結婚しました</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+          <t>カヅチ(著者)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第48話（前編）</t>
+          <t>第16話後半</t>
         </is>
       </c>
     </row>
@@ -7055,17 +8097,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第22話</t>
+          <t>第16話後半：「ストリア見聞録」</t>
         </is>
       </c>
     </row>
@@ -7075,17 +8117,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ダークサモナーとデキている</t>
+          <t>オトナを知りたい女友達</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>車王(著者)</t>
+          <t>望公太(原作) ぷよちゃ(作画)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第72話</t>
+          <t>第7話 前半</t>
         </is>
       </c>
     </row>
@@ -7095,17 +8137,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>異世界のんびり農家</t>
+          <t>淫獄団地</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第301話</t>
+          <t>第48話（前編）</t>
         </is>
       </c>
     </row>
@@ -7115,17 +8157,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>まんきつしたい常連さん</t>
+          <t>ワンパンマン</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>しんみりん(著者)</t>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第45話前編</t>
+          <t>201撃目</t>
         </is>
       </c>
     </row>
@@ -7135,17 +8177,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>ワンパンマン</t>
+          <t>聖液鍛冶屋のエロランタ</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>原作/ＯＮＥ 作画/村田雄介</t>
+          <t>しげきっくす(著者)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>201撃目</t>
+          <t>第6話後半</t>
         </is>
       </c>
     </row>
@@ -7155,17 +8197,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>愚かな天使は悪魔と踊る</t>
+          <t>ミルク搾りハンターの異世界搾乳記～農家の冴えない男があらゆる種族の地区Bを弄び虜にする～</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>アズマサワヨシ(著者)</t>
+          <t>空詠大智(著者)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第99話③</t>
+          <t>第15話前半</t>
         </is>
       </c>
     </row>
@@ -7175,17 +8217,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ギャルゲーマーに褒められたい</t>
+          <t>魔王令嬢の教育係 ～勇者学院を追放された平民教師は魔王の娘たちの家庭教師となる～</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>げしゅまろ(著者)</t>
+          <t>原作：新人 漫画：松原剛 キャラクター原案：巻羊</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>34話</t>
+          <t>第28話</t>
         </is>
       </c>
     </row>
@@ -7195,17 +8237,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>花子さん、食べないで</t>
+          <t>ダンジョンの幼なじみ</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>茸谷きの子(著者)</t>
+          <t>久真やすひさ(著者)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第8話後半</t>
+          <t>第54話</t>
         </is>
       </c>
     </row>
@@ -7215,17 +8257,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第70話(前編) 特別報酬ミッション</t>
+          <t>第22話</t>
         </is>
       </c>
     </row>
@@ -7235,17 +8277,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>辺境の魔法薬師 ～自由気ままな異世界ものづくり日記～</t>
+          <t>おねえさんと猫を飼う</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>gum(漫画) えながゆうき(原作) パルプピロシ(キャラクターデザイン)</t>
+          <t>上杉響士郎(著者)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第16話</t>
+          <t>第1話：おねえさんと猫を拾う</t>
         </is>
       </c>
     </row>
@@ -7255,17 +8297,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+          <t>ダークサモナーとデキている</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>FUNA 東西 モトエ恵介</t>
+          <t>車王(著者)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第118話　会談［その3］</t>
+          <t>第72話</t>
         </is>
       </c>
     </row>
@@ -7275,17 +8317,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ステータス・オール∞（インフィニティ） ∞使いの最強能力者、異世界を自由気ままに暮らします！</t>
+          <t>異世界のんびり農家</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>漫画：三津屋みやこ 原作：八又ナガト</t>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第61話</t>
+          <t>第301話</t>
         </is>
       </c>
     </row>
@@ -7295,17 +8337,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+          <t>無敵商人の異世界成り上がり物語 ～現代の製品を自在に取り寄せるスキルがあるので異世界では楽勝です～</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+          <t>隆原ヒロタ(漫画) 青山有(原作) ぷきゅのすけ(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第80話その1</t>
+          <t>第34話③</t>
         </is>
       </c>
     </row>
@@ -7315,17 +8357,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ラスボスたちの隠し仔　～魔王城に転生した元社畜プログラマーは自由気ままに『魔導言語《マジックコード》』を開発する～</t>
+          <t>まんきつしたい常連さん</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>森清士郎(漫画) 熊乃げん骨(原作)</t>
+          <t>しんみりん(著者)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第13話②</t>
+          <t>第45話前編</t>
         </is>
       </c>
     </row>
@@ -7335,17 +8377,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ダンジョンバンド</t>
+          <t>最強ギフトで領地経営スローライフ ～辺境の村を開拓していたら英雄級の人材がわんさかやってきた！～</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>新挑限(著者)</t>
+          <t>原作：音速炒飯 漫画：眠田瞼 キャラクター原案：riritto</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>♯６Hello,Again ～昔からある場所～②</t>
+          <t>第27話</t>
         </is>
       </c>
     </row>
@@ -7355,17 +8397,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>本物のカノジョにしたくなるまで、私で試していいよ。</t>
+          <t>転生してあらゆるモノに好かれながら異世界で好きな事をして生きて行く</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>wano(漫画) 有丈ほえる(原作) 緋月ひぐれ(キャラクター原案)</t>
+          <t>都尾琉(漫画) 御峰。(原作)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>今週はスペシャルイラスト第2弾!!</t>
+          <t>第25話④</t>
         </is>
       </c>
     </row>
@@ -7375,17 +8417,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第72話 リレー</t>
+          <t>第70話(前編) 特別報酬ミッション</t>
         </is>
       </c>
     </row>
@@ -7395,17 +8437,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
+          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>神原絵理華(漫画) 一森一輝(原作)</t>
+          <t>FUNA 東西 モトエ恵介</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第17話②</t>
+          <t>第118話　会談［その3］</t>
         </is>
       </c>
     </row>
@@ -7415,17 +8457,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>八男って、それはないでしょう！　みそっかす</t>
+          <t>千年英雄</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>ながを(漫画) Ｙ．Ａ(原作) 藤ちょこ(キャラクターデザイン)</t>
+          <t>原作/福島航平 作画/中村ゆきひろ</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>episode.エリーゼ 第4話①</t>
+          <t>12話①</t>
         </is>
       </c>
     </row>
@@ -7435,17 +8477,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>魔物喰らい ランキング最下位の冒険者は魔物の力で最強へ</t>
+          <t>オタクとギャル子</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>赤井ハコ(漫画) 緒二葉(原作) とよた瑣織(キャラクターデザイン)</t>
+          <t>皐月木 獏</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第8話-1</t>
+          <t>新連載のお知らせ</t>
         </is>
       </c>
     </row>
@@ -7455,17 +8497,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>センパイ、自宅警備員の雇用はいかがですか？</t>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>漫画：コブラサナギ 原作：二上圭 キャラ原案：日向あずり</t>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第4話後半</t>
+          <t>第80話その1</t>
         </is>
       </c>
     </row>
@@ -7475,17 +8517,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>冒険者絶対殺すダンジョン</t>
+          <t>愚かな天使は悪魔と踊る</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>道満晴明(著者)</t>
+          <t>アズマサワヨシ(著者)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第33話</t>
+          <t>第99話③</t>
         </is>
       </c>
     </row>
@@ -7495,17 +8537,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>断れない会長は友江くんにだけしてあげたい</t>
+          <t>殺されたらゾンビになったので、進化しまくって無双しようと思います</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>沼地どろまる(著者)</t>
+          <t>漫画：朝ケ夜 原作：幸運ピエロ キャラクター原案：東西</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>特別編</t>
+          <t>第15話(前半)暴走ドラゴンと魔剣①</t>
         </is>
       </c>
     </row>
@@ -7515,17 +8557,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>ダウナーお姉さんは遊びたい</t>
+          <t>実家に帰ったら甘やかされ生活が始まりました</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>山鷹景</t>
+          <t>漫画：幹藻ねずみ 原作：月夜乃古狸 キャラクター原案：うなさか</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第11話</t>
+          <t>第23話前半</t>
         </is>
       </c>
     </row>
@@ -7535,17 +8577,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>わたし、二番目の彼女でいいから。</t>
+          <t>花子さん、食べないで</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>にの子(漫画) 西条陽(原作) Re岳(キャラクター原案)</t>
+          <t>茸谷きの子(著者)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第10話②：カーテンのなか</t>
+          <t>第8話後半</t>
         </is>
       </c>
     </row>
@@ -7555,17 +8597,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>仕事帰り、独身の美人上司に頼まれて</t>
+          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>望公太(原作) とんのすけ(作画) しの(キャラクター原案)</t>
+          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第19話-1</t>
+          <t>第72話 リレー</t>
         </is>
       </c>
     </row>
@@ -7575,17 +8617,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
+          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
+          <t>神原絵理華(漫画) 一森一輝(原作)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第1話②</t>
+          <t>第17話②</t>
         </is>
       </c>
     </row>
@@ -7595,17 +8637,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>未実装のラスボス達が仲間になりました。</t>
+          <t>小さめの魔法師匠と大きめの魔法少女。report：3</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>緋呂河とも(漫画) ながワサビ64(原作) かわく(キャラクター原案)</t>
+          <t>とりから</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第31話</t>
+          <t>第36話の2</t>
         </is>
       </c>
     </row>
@@ -7615,17 +8657,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>殺されたらゾンビになったので、進化しまくって無双しようと思います</t>
+          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>漫画：朝ケ夜 原作：幸運ピエロ キャラクター原案：東西</t>
+          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第15話(前半)暴走ドラゴンと魔剣①</t>
+          <t>第1話②</t>
         </is>
       </c>
     </row>
@@ -7635,17 +8677,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>時森さんが無防備です!!</t>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>たざわ</t>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第61話</t>
+          <t>第33話①</t>
         </is>
       </c>
     </row>
@@ -7655,17 +8697,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>修羅幼女の英雄譚～半端者と言われた傭兵、幼女に転生して成り上がる～</t>
+          <t>物語の黒幕に転生して</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>作画：むらたん 原作：沙城流</t>
+          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第6話(2)</t>
+          <t>第31話</t>
         </is>
       </c>
     </row>
@@ -7675,17 +8717,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>ボクの理想の異世界生活 ～転生したらケモ耳娘だらけの世界でハーレムに～</t>
+          <t>わたし、二番目の彼女でいいから。</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>イチリ(原作) 空維深夜(作画)</t>
+          <t>にの子(漫画) 西条陽(原作) Re岳(キャラクター原案)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第14話後半：存在分裂</t>
+          <t>第10話②：カーテンのなか</t>
         </is>
       </c>
     </row>
@@ -7695,17 +8737,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ヤンデレかと思ったらもっとヤベー女だった</t>
+          <t>辺境の魔法薬師 ～自由気ままな異世界ものづくり日記～</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>八木戸マト</t>
+          <t>gum(漫画) えながゆうき(原作) パルプピロシ(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第64話　しっかり「見てた」ヤンデレ彼女②</t>
+          <t>第16話</t>
         </is>
       </c>
     </row>
@@ -7715,17 +8757,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>物語の黒幕に転生して</t>
+          <t>猫魔法が世界に革命を起こすそうですよ？～劣等種なんて言われるのならケモノ魔法でリベンジします！～</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
+          <t>原作：海野アロイ 漫画：かやこ キャラクター原案：ぷらこ</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第31話</t>
+          <t>第11話</t>
         </is>
       </c>
     </row>
@@ -7735,17 +8777,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>日々は過ぎれど飯うまし</t>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Quro(漫画) あっと(原案)</t>
+          <t>光永康則</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第7話①</t>
+          <t>第６６話『重機停止』④</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-07-01
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -15,6 +15,7 @@
     <sheet name="2025-06-28" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="2025-06-29" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="2025-06-30" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="2025-07-01" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -468,6 +469,1047 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>蜘蛛ですが、なにか？</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>かかし朝浩(著者) 馬場翁(原作) 輝竜司(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>第75話その2</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>帰ってください！ 阿久津さん</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>長岡太一(著者)</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>第191話</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>衛宮さんちの今日のごはん</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>TAa(漫画) 只野まこと(料理監修) ＴＹＰＥ－ＭＯＯＮ(原作)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>第74話</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>第１８話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>異世界居酒屋「のぶ」</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>蝉川夏哉(原作) ヴァージニア二等兵(漫画) 転(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>第122話</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>異世界建国記</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>ＫＯＩＺＵＭＩ(漫画) 桜木桜(原作) 屡那(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>第76話</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>一億年ボタンを連打した俺は、気付いたら最強になっていた ～落第剣士の学院無双～</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>士土幽太郎(漫画) 月島秀一(原作) もきゅ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>第40話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>尾守つみきと奇日常。</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>森下みゆ</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>第57話 つみきさん達とパーティー。</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>クラス最安値で売られた俺は、実は最強パラメーター</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>カンブリア爆発太郎(漫画) RYOMA(原作) 黒井ススム(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>第35話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>狂戦士なモブ、無自覚に本編を破壊する</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>漫画：佐藤良亮 原作：なるのるな キャラクター原案：霜月えいと</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>第11話 ①</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>レベル１から始まる召喚無双</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>漫画：七桃りお 原作：白石新 キャラクター原案：夕薙</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>第32話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>不遇皇子は天才錬金術師～皇帝なんて柄じゃないので弟妹を可愛がりたい～@COMIC</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>長先ザワ（漫画） うめー（原作） 瑛来イチ（構成） 雨銛（構成） かわく（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>第8話 ①</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>異世界おじさん</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>殆ど死んでいる(著者)</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>第69話</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ひきこもりの俺がかわいいギルドマスターに世話を焼かれまくったって別にいいだろう?</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>漫画：ミト 原作：東條功一 イラスト：にもし</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>第17話</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>S級パーティーから追放された狩人、実は世界最強 ～射程9999の男、帝国の狙撃手として無双する～</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>漫画：カズミヤアキラ 原作：茨木野 キャラクター原案：へいろー</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>第8話 ③</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>元最強の剣士は、異世界魔法に憧れる</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>漫画：天乃ちはる 原作：紅月シン キャラクター原案：necömi</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>第72話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>アラフォーになった最強の英雄たち、再び戦場で無双する!!</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>漫画：戸田泰成 原作：岸馬きらく 構成協力：森小太郎 キャラクター原案：peroshi</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>第23話 前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>スライムは最強たる可能性を秘めている～２回目の人生、ちゃんとスライムと向き合います～@COMIC</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>オサフネオウジ（漫画） 犬型大（原作） 風花風花（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>第6話</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>能あるオーガは角を隠す</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>漫画家： 蒼葉 結 原作： 津野瀬 文</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>第9話 前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>クセ強彼女は床にいざなう</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>須河篤志(著者)</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>第13話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>ニチアサ好きのオタクが悪役生徒に転生した結果、破滅フラグが崩壊していく件について</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>烏丸英（原作） どんぐりす（漫画）</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>第14話（後編）急襲…事件の始まり</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>第8話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>ちはるくんは女装をしたくない！</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>翁丸ジョン</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>【第19話】男装宗と交流したくない！その一</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>ぽんドロイド！ はまさん</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>はれやまはれぞう(著者)</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>第2話</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>大魔導士と呼ばれた侯爵令嬢〜世界が汚いので掃除していただけなんですけど……〜@COMIC</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>さいピン（漫画） K1you（原作） パルプピロシ（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>第6話</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>クソ女に幸あれ</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>岸川瑞樹</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>第58話</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>魔術師クノンは見えている</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>第38話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>第70話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>第16話後半：「ストリア見聞録」</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>ワンパンマン</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>201撃目</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>千年英雄</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>原作/福島航平 作画/中村ゆきひろ</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>12話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>サーシャちゃんとクラスメイトオタクくん</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>はぐはぐ(著者)</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>第80話</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>冒険者ギルドが十二歳からしか入れなかったので、サバよみました。</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>GUNP（漫画） KAME （原作） ox （キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>第12話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>《魔力無限》のマナポーター ～パーティの魔力を全て供給していたのに、勇者に追放されました。魔力不足で聖剣が使えないと焦っても、メンバー全員が勇者を見限ったのでもう遅い～</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>漫画：伊藤ひずみ 原作：アトハ キャラクター原案：夕薙</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>第10話 ②</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>淫獄団地</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>第48話（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>ダンジョンの幼なじみ</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>久真やすひさ(著者)</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>第54話</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>オトナを知りたい女友達</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>望公太(原作) ぷよちゃ(作画)</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>第7話 前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>田舎の黒ギャルJKと結婚しました</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>カヅチ(著者)</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>第16話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>異世界迷宮のオーパーツ</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>三狛ハル(著者)</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>第1話：先端にお椀がついた棒</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>ダークサモナーとデキている</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>車王(著者)</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>第72話</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>ギャルゲーマーに褒められたい</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>げしゅまろ(著者)</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>34話</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>転生貴族の異世界冒険録 ～カインのやりすぎギルド日記～</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>原作：夜州 漫画：佐々木あかね・香本セトラ キャラクター原案：藻</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>第47話</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>異世界のんびり農家</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>第301話</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>小さめの魔法師匠と大きめの魔法少女。report：3</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>とりから</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>第36話の3</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>第22話</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>聖液鍛冶屋のエロランタ</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>しげきっくす(著者)</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>第6話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>ロメリア戦記～伯爵令嬢、魔王を倒した後も人類やばそうだから軍隊組織する～</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>漫画：上戸 亮 原作：有山リョウ(小学館「ガガガブックス」刊) キャラクター原案：コダマ</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>第13話「助けてくれる人々」①</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>FUNA 東西 モトエ恵介</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>第118話　会談［その3］</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>まんきつしたい常連さん</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>しんみりん(著者)</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>第45話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>はずれスキル念動力（ただしレベルＭＡＸ）で無双する～手をかざすだけです。詠唱とか必殺技とかいりません。念じるだけで倒せます～</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>さとう うなぽっぽ トダフミト</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>9話①</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -7792,1000 +8834,1000 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="0" t="inlineStr">
         <is>
           <t>異世界居酒屋「のぶ」</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="0" t="inlineStr">
         <is>
           <t>蝉川夏哉(原作) ヴァージニア二等兵(漫画) 転(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="0" t="inlineStr">
         <is>
           <t>第122話</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="0" t="inlineStr">
         <is>
           <t>ニチアサ好きのオタクが悪役生徒に転生した結果、破滅フラグが崩壊していく件について</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="0" t="inlineStr">
         <is>
           <t>烏丸英（原作） どんぐりす（漫画）</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" s="0" t="inlineStr">
         <is>
           <t>第14話（後編）急襲…事件の始まり</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="0" t="inlineStr">
         <is>
           <t>異世界おじさん</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="0" t="inlineStr">
         <is>
           <t>殆ど死んでいる(著者)</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" s="0" t="inlineStr">
         <is>
           <t>第69話</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="0" t="inlineStr">
         <is>
           <t>クセ強彼女は床にいざなう</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="0" t="inlineStr">
         <is>
           <t>須河篤志(著者)</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D5" s="0" t="inlineStr">
         <is>
           <t>第13話前半</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="0" t="inlineStr">
         <is>
           <t>ぽんドロイド！ はまさん</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" s="0" t="inlineStr">
         <is>
           <t>はれやまはれぞう(著者)</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D6" s="0" t="inlineStr">
         <is>
           <t>第2話</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="0" t="inlineStr">
         <is>
           <t>はずれスキル念動力（ただしレベルＭＡＸ）で無双する～手をかざすだけです。詠唱とか必殺技とかいりません。念じるだけで倒せます～</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="0" t="inlineStr">
         <is>
           <t>さとう うなぽっぽ トダフミト</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D7" s="0" t="inlineStr">
         <is>
           <t>9話①</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" s="0" t="inlineStr">
         <is>
           <t>外来魔法生物対策課</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" s="0" t="inlineStr">
         <is>
           <t>端(原作) 皐月木獏(作画)</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D8" s="0" t="inlineStr">
         <is>
           <t>第1話</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="0" t="inlineStr">
         <is>
           <t>異世界迷宮のオーパーツ</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" s="0" t="inlineStr">
         <is>
           <t>三狛ハル(著者)</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D9" s="0" t="inlineStr">
         <is>
           <t>第1話：先端にお椀がついた棒</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" s="0" t="inlineStr">
         <is>
           <t>転生貴族の異世界冒険録 ～カインのやりすぎギルド日記～</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" s="0" t="inlineStr">
         <is>
           <t>原作：夜州 漫画：佐々木あかね・香本セトラ キャラクター原案：藻</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D10" s="0" t="inlineStr">
         <is>
           <t>第47話</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" s="0" t="inlineStr">
         <is>
           <t>ギャルゲーマーに褒められたい</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" s="0" t="inlineStr">
         <is>
           <t>げしゅまろ(著者)</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D11" s="0" t="inlineStr">
         <is>
           <t>34話</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
+      <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" s="0" t="inlineStr">
         <is>
           <t>リビルドワールド</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" s="0" t="inlineStr">
         <is>
           <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D12" s="0" t="inlineStr">
         <is>
           <t>第70話③</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
+      <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" s="0" t="inlineStr">
         <is>
           <t>サーシャちゃんとクラスメイトオタクくん</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" s="0" t="inlineStr">
         <is>
           <t>はぐはぐ(著者)</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D13" s="0" t="inlineStr">
         <is>
           <t>第80話</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
+      <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B14" s="0" t="inlineStr">
         <is>
           <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C14" s="0" t="inlineStr">
         <is>
           <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D14" s="0" t="inlineStr">
         <is>
           <t>第8話-2</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
+      <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B15" s="0" t="inlineStr">
         <is>
           <t>魔術師クノンは見えている</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C15" s="0" t="inlineStr">
         <is>
           <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D15" s="0" t="inlineStr">
         <is>
           <t>第38話①</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
+      <c r="A16" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B16" s="0" t="inlineStr">
         <is>
           <t>田舎の黒ギャルJKと結婚しました</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C16" s="0" t="inlineStr">
         <is>
           <t>カヅチ(著者)</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="D16" s="0" t="inlineStr">
         <is>
           <t>第16話後半</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
+      <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B17" s="0" t="inlineStr">
         <is>
           <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C17" s="0" t="inlineStr">
         <is>
           <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="D17" s="0" t="inlineStr">
         <is>
           <t>第16話後半：「ストリア見聞録」</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
+      <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B18" s="0" t="inlineStr">
         <is>
           <t>オトナを知りたい女友達</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C18" s="0" t="inlineStr">
         <is>
           <t>望公太(原作) ぷよちゃ(作画)</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="D18" s="0" t="inlineStr">
         <is>
           <t>第7話 前半</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
+      <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B19" s="0" t="inlineStr">
         <is>
           <t>淫獄団地</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C19" s="0" t="inlineStr">
         <is>
           <t>搾精研究所(原作) 丈山雄為(漫画)</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="D19" s="0" t="inlineStr">
         <is>
           <t>第48話（前編）</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
+      <c r="A20" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B20" s="0" t="inlineStr">
         <is>
           <t>ワンパンマン</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C20" s="0" t="inlineStr">
         <is>
           <t>原作/ＯＮＥ 作画/村田雄介</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="D20" s="0" t="inlineStr">
         <is>
           <t>201撃目</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
+      <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B21" s="0" t="inlineStr">
         <is>
           <t>聖液鍛冶屋のエロランタ</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C21" s="0" t="inlineStr">
         <is>
           <t>しげきっくす(著者)</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="D21" s="0" t="inlineStr">
         <is>
           <t>第6話後半</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
+      <c r="A22" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B22" s="0" t="inlineStr">
         <is>
           <t>ミルク搾りハンターの異世界搾乳記～農家の冴えない男があらゆる種族の地区Bを弄び虜にする～</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C22" s="0" t="inlineStr">
         <is>
           <t>空詠大智(著者)</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="D22" s="0" t="inlineStr">
         <is>
           <t>第15話前半</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="n">
+      <c r="A23" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B23" s="0" t="inlineStr">
         <is>
           <t>魔王令嬢の教育係 ～勇者学院を追放された平民教師は魔王の娘たちの家庭教師となる～</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C23" s="0" t="inlineStr">
         <is>
           <t>原作：新人 漫画：松原剛 キャラクター原案：巻羊</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="D23" s="0" t="inlineStr">
         <is>
           <t>第28話</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="n">
+      <c r="A24" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B24" s="0" t="inlineStr">
         <is>
           <t>ダンジョンの幼なじみ</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="C24" s="0" t="inlineStr">
         <is>
           <t>久真やすひさ(著者)</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="D24" s="0" t="inlineStr">
         <is>
           <t>第54話</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="n">
+      <c r="A25" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="B25" s="0" t="inlineStr">
         <is>
           <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C25" s="0" t="inlineStr">
         <is>
           <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="D25" s="0" t="inlineStr">
         <is>
           <t>第22話</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="n">
+      <c r="A26" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="B26" s="0" t="inlineStr">
         <is>
           <t>おねえさんと猫を飼う</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="C26" s="0" t="inlineStr">
         <is>
           <t>上杉響士郎(著者)</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="D26" s="0" t="inlineStr">
         <is>
           <t>第1話：おねえさんと猫を拾う</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="n">
+      <c r="A27" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="B27" s="0" t="inlineStr">
         <is>
           <t>ダークサモナーとデキている</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="C27" s="0" t="inlineStr">
         <is>
           <t>車王(著者)</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="D27" s="0" t="inlineStr">
         <is>
           <t>第72話</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="n">
+      <c r="A28" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B28" s="0" t="inlineStr">
         <is>
           <t>異世界のんびり農家</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C28" s="0" t="inlineStr">
         <is>
           <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="D28" s="0" t="inlineStr">
         <is>
           <t>第301話</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="n">
+      <c r="A29" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="B29" s="0" t="inlineStr">
         <is>
           <t>無敵商人の異世界成り上がり物語 ～現代の製品を自在に取り寄せるスキルがあるので異世界では楽勝です～</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="C29" s="0" t="inlineStr">
         <is>
           <t>隆原ヒロタ(漫画) 青山有(原作) ぷきゅのすけ(キャラクターデザイン)</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="D29" s="0" t="inlineStr">
         <is>
           <t>第34話③</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="n">
+      <c r="A30" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="B30" s="0" t="inlineStr">
         <is>
           <t>まんきつしたい常連さん</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="C30" s="0" t="inlineStr">
         <is>
           <t>しんみりん(著者)</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="D30" s="0" t="inlineStr">
         <is>
           <t>第45話前編</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="n">
+      <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="B31" s="0" t="inlineStr">
         <is>
           <t>最強ギフトで領地経営スローライフ ～辺境の村を開拓していたら英雄級の人材がわんさかやってきた！～</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="C31" s="0" t="inlineStr">
         <is>
           <t>原作：音速炒飯 漫画：眠田瞼 キャラクター原案：riritto</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="D31" s="0" t="inlineStr">
         <is>
           <t>第27話</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="n">
+      <c r="A32" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="B32" s="0" t="inlineStr">
         <is>
           <t>転生してあらゆるモノに好かれながら異世界で好きな事をして生きて行く</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="C32" s="0" t="inlineStr">
         <is>
           <t>都尾琉(漫画) 御峰。(原作)</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="D32" s="0" t="inlineStr">
         <is>
           <t>第25話④</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="n">
+      <c r="A33" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="B33" s="0" t="inlineStr">
         <is>
           <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="C33" s="0" t="inlineStr">
         <is>
           <t>岡沢六十四 るれくちぇ sage・ジョー</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="D33" s="0" t="inlineStr">
         <is>
           <t>第70話(前編) 特別報酬ミッション</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="n">
+      <c r="A34" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B34" s="0" t="inlineStr">
         <is>
           <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="C34" s="0" t="inlineStr">
         <is>
           <t>FUNA 東西 モトエ恵介</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="D34" s="0" t="inlineStr">
         <is>
           <t>第118話　会談［その3］</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="n">
+      <c r="A35" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="B35" s="0" t="inlineStr">
         <is>
           <t>千年英雄</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="C35" s="0" t="inlineStr">
         <is>
           <t>原作/福島航平 作画/中村ゆきひろ</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="D35" s="0" t="inlineStr">
         <is>
           <t>12話①</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="n">
+      <c r="A36" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="B36" s="0" t="inlineStr">
         <is>
           <t>オタクとギャル子</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="C36" s="0" t="inlineStr">
         <is>
           <t>皐月木 獏</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="D36" s="0" t="inlineStr">
         <is>
           <t>新連載のお知らせ</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="n">
+      <c r="A37" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="B37" s="0" t="inlineStr">
         <is>
           <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="C37" s="0" t="inlineStr">
         <is>
           <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
+      <c r="D37" s="0" t="inlineStr">
         <is>
           <t>第80話その1</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="n">
+      <c r="A38" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="B38" s="0" t="inlineStr">
         <is>
           <t>愚かな天使は悪魔と踊る</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
+      <c r="C38" s="0" t="inlineStr">
         <is>
           <t>アズマサワヨシ(著者)</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
+      <c r="D38" s="0" t="inlineStr">
         <is>
           <t>第99話③</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="n">
+      <c r="A39" s="0" t="n">
         <v>38</v>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="B39" s="0" t="inlineStr">
         <is>
           <t>殺されたらゾンビになったので、進化しまくって無双しようと思います</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="C39" s="0" t="inlineStr">
         <is>
           <t>漫画：朝ケ夜 原作：幸運ピエロ キャラクター原案：東西</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
+      <c r="D39" s="0" t="inlineStr">
         <is>
           <t>第15話(前半)暴走ドラゴンと魔剣①</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="n">
+      <c r="A40" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="B40" s="0" t="inlineStr">
         <is>
           <t>実家に帰ったら甘やかされ生活が始まりました</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="C40" s="0" t="inlineStr">
         <is>
           <t>漫画：幹藻ねずみ 原作：月夜乃古狸 キャラクター原案：うなさか</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="D40" s="0" t="inlineStr">
         <is>
           <t>第23話前半</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="n">
+      <c r="A41" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="B41" s="0" t="inlineStr">
         <is>
           <t>花子さん、食べないで</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="C41" s="0" t="inlineStr">
         <is>
           <t>茸谷きの子(著者)</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
+      <c r="D41" s="0" t="inlineStr">
         <is>
           <t>第8話後半</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="n">
+      <c r="A42" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="B42" s="0" t="inlineStr">
         <is>
           <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="C42" s="0" t="inlineStr">
         <is>
           <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
+      <c r="D42" s="0" t="inlineStr">
         <is>
           <t>第72話 リレー</t>
         </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="n">
+      <c r="A43" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B43" s="0" t="inlineStr">
         <is>
           <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="C43" s="0" t="inlineStr">
         <is>
           <t>神原絵理華(漫画) 一森一輝(原作)</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
+      <c r="D43" s="0" t="inlineStr">
         <is>
           <t>第17話②</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="n">
+      <c r="A44" s="0" t="n">
         <v>43</v>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="B44" s="0" t="inlineStr">
         <is>
           <t>小さめの魔法師匠と大きめの魔法少女。report：3</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="C44" s="0" t="inlineStr">
         <is>
           <t>とりから</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
+      <c r="D44" s="0" t="inlineStr">
         <is>
           <t>第36話の2</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="n">
+      <c r="A45" s="0" t="n">
         <v>44</v>
       </c>
-      <c r="B45" t="inlineStr">
+      <c r="B45" s="0" t="inlineStr">
         <is>
           <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="C45" s="0" t="inlineStr">
         <is>
           <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
+      <c r="D45" s="0" t="inlineStr">
         <is>
           <t>第1話②</t>
         </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="n">
+      <c r="A46" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="B46" t="inlineStr">
+      <c r="B46" s="0" t="inlineStr">
         <is>
           <t>クラスで２番目に可愛い女の子と友だちになった</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="C46" s="0" t="inlineStr">
         <is>
           <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
+      <c r="D46" s="0" t="inlineStr">
         <is>
           <t>第33話①</t>
         </is>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="n">
+      <c r="A47" s="0" t="n">
         <v>46</v>
       </c>
-      <c r="B47" t="inlineStr">
+      <c r="B47" s="0" t="inlineStr">
         <is>
           <t>物語の黒幕に転生して</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="C47" s="0" t="inlineStr">
         <is>
           <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
+      <c r="D47" s="0" t="inlineStr">
         <is>
           <t>第31話</t>
         </is>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="n">
+      <c r="A48" s="0" t="n">
         <v>47</v>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="B48" s="0" t="inlineStr">
         <is>
           <t>わたし、二番目の彼女でいいから。</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
+      <c r="C48" s="0" t="inlineStr">
         <is>
           <t>にの子(漫画) 西条陽(原作) Re岳(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
+      <c r="D48" s="0" t="inlineStr">
         <is>
           <t>第10話②：カーテンのなか</t>
         </is>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="n">
+      <c r="A49" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="B49" s="0" t="inlineStr">
         <is>
           <t>辺境の魔法薬師 ～自由気ままな異世界ものづくり日記～</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="C49" s="0" t="inlineStr">
         <is>
           <t>gum(漫画) えながゆうき(原作) パルプピロシ(キャラクターデザイン)</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
+      <c r="D49" s="0" t="inlineStr">
         <is>
           <t>第16話</t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="n">
+      <c r="A50" s="0" t="n">
         <v>49</v>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="B50" s="0" t="inlineStr">
         <is>
           <t>猫魔法が世界に革命を起こすそうですよ？～劣等種なんて言われるのならケモノ魔法でリベンジします！～</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="C50" s="0" t="inlineStr">
         <is>
           <t>原作：海野アロイ 漫画：かやこ キャラクター原案：ぷらこ</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
+      <c r="D50" s="0" t="inlineStr">
         <is>
           <t>第11話</t>
         </is>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="n">
+      <c r="A51" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="B51" s="0" t="inlineStr">
         <is>
           <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="C51" s="0" t="inlineStr">
         <is>
           <t>光永康則</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
+      <c r="D51" s="0" t="inlineStr">
         <is>
           <t>第６６話『重機停止』④</t>
         </is>

</xml_diff>

<commit_message>
Add ranking data for 2025-07-02
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -16,6 +16,7 @@
     <sheet name="2025-06-29" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="2025-06-30" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="2025-07-01" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="2025-07-02" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -506,22 +507,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>蜘蛛ですが、なにか？</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>かかし朝浩(著者) 馬場翁(原作) 輝竜司(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第75話その2</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>帰ってください！ 阿久津さん</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>長岡太一(著者)</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第191話</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>衛宮さんちの今日のごはん</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>TAa(漫画) 只野まこと(料理監修) ＴＹＰＥ－ＭＯＯＮ(原作)</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第74話</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第１８話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>異世界居酒屋「のぶ」</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>蝉川夏哉(原作) ヴァージニア二等兵(漫画) 転(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第122話</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>異世界建国記</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>ＫＯＩＺＵＭＩ(漫画) 桜木桜(原作) 屡那(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第76話</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>一億年ボタンを連打した俺は、気付いたら最強になっていた ～落第剣士の学院無双～</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>士土幽太郎(漫画) 月島秀一(原作) もきゅ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第40話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>尾守つみきと奇日常。</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>森下みゆ</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第57話 つみきさん達とパーティー。</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>クラス最安値で売られた俺は、実は最強パラメーター</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>カンブリア爆発太郎(漫画) RYOMA(原作) 黒井ススム(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第35話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>狂戦士なモブ、無自覚に本編を破壊する</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>漫画：佐藤良亮 原作：なるのるな キャラクター原案：霜月えいと</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第11話 ①</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>レベル１から始まる召喚無双</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>漫画：七桃りお 原作：白石新 キャラクター原案：夕薙</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第32話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>不遇皇子は天才錬金術師～皇帝なんて柄じゃないので弟妹を可愛がりたい～@COMIC</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>長先ザワ（漫画） うめー（原作） 瑛来イチ（構成） 雨銛（構成） かわく（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第8話 ①</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>異世界おじさん</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>殆ど死んでいる(著者)</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第69話</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>ひきこもりの俺がかわいいギルドマスターに世話を焼かれまくったって別にいいだろう?</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>漫画：ミト 原作：東條功一 イラスト：にもし</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第17話</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>S級パーティーから追放された狩人、実は世界最強 ～射程9999の男、帝国の狙撃手として無双する～</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>漫画：カズミヤアキラ 原作：茨木野 キャラクター原案：へいろー</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第8話 ③</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>元最強の剣士は、異世界魔法に憧れる</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>漫画：天乃ちはる 原作：紅月シン キャラクター原案：necömi</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第72話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>アラフォーになった最強の英雄たち、再び戦場で無双する!!</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>漫画：戸田泰成 原作：岸馬きらく 構成協力：森小太郎 キャラクター原案：peroshi</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第23話 前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>スライムは最強たる可能性を秘めている～２回目の人生、ちゃんとスライムと向き合います～@COMIC</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>オサフネオウジ（漫画） 犬型大（原作） 風花風花（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第6話</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>能あるオーガは角を隠す</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>漫画家： 蒼葉 結 原作： 津野瀬 文</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第9話 前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>クセ強彼女は床にいざなう</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>須河篤志(著者)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第13話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>ニチアサ好きのオタクが悪役生徒に転生した結果、破滅フラグが崩壊していく件について</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>烏丸英（原作） どんぐりす（漫画）</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第14話（後編）急襲…事件の始まり</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第8話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>ちはるくんは女装をしたくない！</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>翁丸ジョン</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>【第19話】男装宗と交流したくない！その一</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>ぽんドロイド！ はまさん</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>はれやまはれぞう(著者)</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第2話</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>大魔導士と呼ばれた侯爵令嬢〜世界が汚いので掃除していただけなんですけど……〜@COMIC</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>さいピン（漫画） K1you（原作） パルプピロシ（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第6話</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>クソ女に幸あれ</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>岸川瑞樹</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第58話</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>魔術師クノンは見えている</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第38話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第70話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第16話後半：「ストリア見聞録」</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>ワンパンマン</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>201撃目</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>千年英雄</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>原作/福島航平 作画/中村ゆきひろ</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>12話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>サーシャちゃんとクラスメイトオタクくん</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>はぐはぐ(著者)</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第80話</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>冒険者ギルドが十二歳からしか入れなかったので、サバよみました。</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>GUNP（漫画） KAME （原作） ox （キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第12話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>《魔力無限》のマナポーター ～パーティの魔力を全て供給していたのに、勇者に追放されました。魔力不足で聖剣が使えないと焦っても、メンバー全員が勇者を見限ったのでもう遅い～</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>漫画：伊藤ひずみ 原作：アトハ キャラクター原案：夕薙</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第10話 ②</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>淫獄団地</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第48話（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>ダンジョンの幼なじみ</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>久真やすひさ(著者)</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第54話</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>オトナを知りたい女友達</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>望公太(原作) ぷよちゃ(作画)</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第7話 前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>田舎の黒ギャルJKと結婚しました</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>カヅチ(著者)</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第16話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>異世界迷宮のオーパーツ</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>三狛ハル(著者)</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第1話：先端にお椀がついた棒</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>ダークサモナーとデキている</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>車王(著者)</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第72話</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>ギャルゲーマーに褒められたい</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>げしゅまろ(著者)</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>34話</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>転生貴族の異世界冒険録 ～カインのやりすぎギルド日記～</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>原作：夜州 漫画：佐々木あかね・香本セトラ キャラクター原案：藻</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第47話</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>異世界のんびり農家</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第301話</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>小さめの魔法師匠と大きめの魔法少女。report：3</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>とりから</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第36話の3</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第22話</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>聖液鍛冶屋のエロランタ</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>しげきっくす(著者)</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第6話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>ロメリア戦記～伯爵令嬢、魔王を倒した後も人類やばそうだから軍隊組織する～</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>漫画：上戸 亮 原作：有山リョウ(小学館「ガガガブックス」刊) キャラクター原案：コダマ</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第13話「助けてくれる人々」①</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>FUNA 東西 モトエ恵介</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第118話　会談［その3］</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>まんきつしたい常連さん</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>しんみりん(著者)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第45話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>はずれスキル念動力（ただしレベルＭＡＸ）で無双する～手をかざすだけです。詠唱とか必殺技とかいりません。念じるだけで倒せます～</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>さとう うなぽっぽ トダフミト</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>9話①</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>蜘蛛ですが、なにか？</t>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>かかし朝浩(著者) 馬場翁(原作) 輝竜司(キャラクター原案)</t>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第75話その2</t>
+          <t>第30話：一秒の奪い合い①</t>
         </is>
       </c>
     </row>
@@ -531,17 +1573,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>帰ってください！ 阿久津さん</t>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>長岡太一(著者)</t>
+          <t>光永康則</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第191話</t>
+          <t>第６７話『六花停止』①</t>
         </is>
       </c>
     </row>
@@ -551,17 +1593,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>衛宮さんちの今日のごはん</t>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>TAa(漫画) 只野まこと(料理監修) ＴＹＰＥ－ＭＯＯＮ(原作)</t>
+          <t>マツモトケンゴ</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第74話</t>
+          <t>第５９話　筋トレの戦いが始まった（２）</t>
         </is>
       </c>
     </row>
@@ -571,17 +1613,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第１８話①</t>
+          <t>第3話 前編</t>
         </is>
       </c>
     </row>
@@ -591,17 +1633,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>異世界居酒屋「のぶ」</t>
+          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>蝉川夏哉(原作) ヴァージニア二等兵(漫画) 転(キャラクター原案)</t>
+          <t>板垣恵介 猪原賽 陸井栄史</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第122話</t>
+          <t>第75話　大気の雷(いかづち)</t>
         </is>
       </c>
     </row>
@@ -611,17 +1653,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>異世界建国記</t>
+          <t>異世界食堂　洋食のねこや</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ＫＯＩＺＵＭＩ(漫画) 桜木桜(原作) 屡那(キャラクター原案)</t>
+          <t>犬塚惇平(ヒーロー文庫／イマジカインフォス)(原作) ヤミザワ(漫画) モロザワ(漫画) エナミカツミ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第76話</t>
+          <t>第39話②</t>
         </is>
       </c>
     </row>
@@ -631,17 +1673,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>一億年ボタンを連打した俺は、気付いたら最強になっていた ～落第剣士の学院無双～</t>
+          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>士土幽太郎(漫画) 月島秀一(原作) もきゅ(キャラクター原案)</t>
+          <t>板垣恵介 林たかあき</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第40話-1</t>
+          <t>第49話 日常</t>
         </is>
       </c>
     </row>
@@ -651,17 +1693,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>尾守つみきと奇日常。</t>
+          <t>10年ぶりに再会したクソガキは清純美少女JKに成長していた</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>森下みゆ</t>
+          <t>緑青黒羽（漫画） 館西夕木（原作） ひげ猫（キャラクター原案）</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第57話 つみきさん達とパーティー。</t>
+          <t>第5話　嫉妬、そして嫉妬（前編）</t>
         </is>
       </c>
     </row>
@@ -671,17 +1713,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>クラス最安値で売られた俺は、実は最強パラメーター</t>
+          <t>ハズレ枠の【状態異常スキル】で最強になった俺がすべてを蹂躙するまで</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>カンブリア爆発太郎(漫画) RYOMA(原作) 黒井ススム(キャラクター原案)</t>
+          <t>鵜吉しょう（作画） 内々けやき（構成） 篠崎 芳（原作） KWKM（キャラクター原案）</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第35話-2</t>
+          <t>第55話　壁外決戦</t>
         </is>
       </c>
     </row>
@@ -691,17 +1733,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>狂戦士なモブ、無自覚に本編を破壊する</t>
+          <t>絶対死なないステラ姫</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>漫画：佐藤良亮 原作：なるのるな キャラクター原案：霜月えいと</t>
+          <t>光永康則 大高稲</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第11話 ①</t>
+          <t>第１３話　絶対巣穴に入らない・解（４）</t>
         </is>
       </c>
     </row>
@@ -711,17 +1753,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>レベル１から始まる召喚無双</t>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>漫画：七桃りお 原作：白石新 キャラクター原案：夕薙</t>
+          <t>漫画/すたひろ 原作/Y.A</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第32話前半</t>
+          <t>chapter65【34話②】</t>
         </is>
       </c>
     </row>
@@ -731,17 +1773,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>不遇皇子は天才錬金術師～皇帝なんて柄じゃないので弟妹を可愛がりたい～@COMIC</t>
+          <t>ひとりぼっちの異世界攻略</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>長先ザワ（漫画） うめー（原作） 瑛来イチ（構成） 雨銛（構成） かわく（キャラクター原案）</t>
+          <t>びび（漫画） 五示正司（原作）</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第8話 ①</t>
+          <t>第225話　俺がもし使い物にならなくなったら…</t>
         </is>
       </c>
     </row>
@@ -751,17 +1793,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>異世界おじさん</t>
+          <t>暗殺者である俺のステータスが勇者よりも明らかに強いのだが</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>殆ど死んでいる(著者)</t>
+          <t>合鴨ひろゆき（漫画） 赤井まつり（原作） 東西（キャラクター原案）</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第69話</t>
+          <t>第33話　ブルート迷宮Ⅲ</t>
         </is>
       </c>
     </row>
@@ -771,17 +1813,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ひきこもりの俺がかわいいギルドマスターに世話を焼かれまくったって別にいいだろう?</t>
+          <t>クラス転移に巻き込まれたコンビニ店員のおっさん、勇者には必要なかった余り物スキルを駆使して最強となるようです。　コミック版</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>漫画：ミト 原作：東條功一 イラスト：にもし</t>
+          <t>漫画：結城焔 原作：Narrative Works　日浦あやせ キャラクター原案：鱈</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第17話</t>
+          <t>chapter49【23話②】</t>
         </is>
       </c>
     </row>
@@ -791,17 +1833,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>S級パーティーから追放された狩人、実は世界最強 ～射程9999の男、帝国の狙撃手として無双する～</t>
+          <t>彼女を奪ったイケメン美少女がなぜか俺まで狙ってくる</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>漫画：カズミヤアキラ 原作：茨木野 キャラクター原案：へいろー</t>
+          <t>鹿もみじ(漫画) 福田週人(原作) さなだケイスイ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第8話 ③</t>
+          <t>第9話</t>
         </is>
       </c>
     </row>
@@ -811,17 +1853,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>元最強の剣士は、異世界魔法に憧れる</t>
+          <t>ネットの『推し』とリアルの『推し』が隣に引っ越してきた</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>漫画：天乃ちはる 原作：紅月シン キャラクター原案：necömi</t>
+          <t>カタケイ（漫画） 遥 透子（原作） 秋乃える（キャラクター原案）</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第72話前半</t>
+          <t>第17話　誤解を紐解く回</t>
         </is>
       </c>
     </row>
@@ -831,17 +1873,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>アラフォーになった最強の英雄たち、再び戦場で無双する!!</t>
+          <t>蜘蛛ですが、なにか？</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>漫画：戸田泰成 原作：岸馬きらく 構成協力：森小太郎 キャラクター原案：peroshi</t>
+          <t>かかし朝浩(著者) 馬場翁(原作) 輝竜司(キャラクター原案)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第23話 前編</t>
+          <t>第75話その2</t>
         </is>
       </c>
     </row>
@@ -851,17 +1893,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>スライムは最強たる可能性を秘めている～２回目の人生、ちゃんとスライムと向き合います～@COMIC</t>
+          <t>元最強探索者のおじさん。美少女配信者を助けて大バズりしてしまった。</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>オサフネオウジ（漫画） 犬型大（原作） 風花風花（キャラクター原案）</t>
+          <t>かなたろー(原作) 草壁レイ(漫画)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第6話</t>
+          <t>第3話　美少女、おじさんにハメられる。②</t>
         </is>
       </c>
     </row>
@@ -871,17 +1913,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>能あるオーガは角を隠す</t>
+          <t>ダウナー系お姉さんに毎日カスの嘘を流し込まれる話</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>漫画家： 蒼葉 結 原作： 津野瀬 文</t>
+          <t>生倉のゑる(著者) はるばーど屋(原作者)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第9話 前編</t>
+          <t>10話 おまけ</t>
         </is>
       </c>
     </row>
@@ -891,17 +1933,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>クセ強彼女は床にいざなう</t>
+          <t>序盤で死ぬ最強のサブキャラに転生したので、ゲーム知識で無双する</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>須河篤志(著者)</t>
+          <t>作画：マエD 原作：新人</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第13話前半</t>
+          <t>第4話(2)</t>
         </is>
       </c>
     </row>
@@ -911,17 +1953,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>ニチアサ好きのオタクが悪役生徒に転生した結果、破滅フラグが崩壊していく件について</t>
+          <t>異世界魔法は遅れてる！</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>烏丸英（原作） どんぐりす（漫画）</t>
+          <t>COMTA（漫画） 樋辻臥命（原作）</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第14話（後編）急襲…事件の始まり</t>
+          <t>第61話　新月の夜にⅢ</t>
         </is>
       </c>
     </row>
@@ -931,17 +1973,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+          <t>肥満令嬢は細くなり、後は傾国の美女（物理）として生きるのみ@COMIC</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+          <t>宇斗リクツ（漫画） 八針来夏（原作） 輝竜司（キャラクター原案）</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第8話-2</t>
+          <t>【7/1コミックス第１巻発売!!】</t>
         </is>
       </c>
     </row>
@@ -951,17 +1993,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ちはるくんは女装をしたくない！</t>
+          <t>異世界マンチキン　―HP1のままで最強最速ダンジョン攻略―</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>翁丸ジョン</t>
+          <t>原作／志瑞 祐 漫画／青桐 良</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>【第19話】男装宗と交流したくない！その一</t>
+          <t>ページ127 多くの援軍</t>
         </is>
       </c>
     </row>
@@ -971,17 +2013,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ぽんドロイド！ はまさん</t>
+          <t>ハニートラップ・シェアハウス</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>はれやまはれぞう(著者)</t>
+          <t>久慈マサムネ(原作) 神月洸壱(作画)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第2話</t>
+          <t>第38話「芸能界にスパイは潜む」①</t>
         </is>
       </c>
     </row>
@@ -991,17 +2033,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>大魔導士と呼ばれた侯爵令嬢〜世界が汚いので掃除していただけなんですけど……〜@COMIC</t>
+          <t>竜と歩む成り上がり冒険者道～用済みとしてSランクパーティから追放された回復魔術師、捨てられた先で最強の神竜を復活させてしまう ～　コミック版</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>さいピン（漫画） K1you（原作） パルプピロシ（キャラクター原案）</t>
+          <t>漫画/＠カリカリうめ 原作/岸本和葉 キャラクター原案/シソ</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第6話</t>
+          <t>chapter49【25話①】</t>
         </is>
       </c>
     </row>
@@ -1011,17 +2053,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>クソ女に幸あれ</t>
+          <t>魔王様の街づくり！～最強のダンジョンは近代都市～</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>岸川瑞樹</t>
+          <t>吉川英朗（漫画） 月夜 涙（GAノベル/SBクリエイティブ刊）　（原作）</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第58話</t>
+          <t>第72話　【炎】の弔い</t>
         </is>
       </c>
     </row>
@@ -1031,17 +2073,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>魔術師クノンは見えている</t>
+          <t>帰ってください！ 阿久津さん</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+          <t>長岡太一(著者)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第38話①</t>
+          <t>第191話</t>
         </is>
       </c>
     </row>
@@ -1051,17 +2093,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>リビルドワールド</t>
+          <t>農学博士の異世界無双～禁忌の知識で築くモンスター娘ハーレム～</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+          <t>インド僧(原作) ヤスウミ(作画)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第70話③</t>
+          <t>コミックス告知</t>
         </is>
       </c>
     </row>
@@ -1071,17 +2113,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+          <t>世界最速のレベルアップ</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+          <t>鈴見敦(漫画) 八又ナガト(原作) fame(キャラクター原案)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第16話後半：「ストリア見聞録」</t>
+          <t>第47話②</t>
         </is>
       </c>
     </row>
@@ -1091,17 +2133,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ワンパンマン</t>
+          <t>黒の召喚士</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>原作/ＯＮＥ 作画/村田雄介</t>
+          <t>天羽 銀（漫画） 迷井豆腐（原作） 黒銀（DIGS）（キャラクター原案）</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>201撃目</t>
+          <t>第143話　聖槍イクリプスⅣ</t>
         </is>
       </c>
     </row>
@@ -1111,17 +2153,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>千年英雄</t>
+          <t>恋人のフリのフリ</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>原作/福島航平 作画/中村ゆきひろ</t>
+          <t>むねひろ(著者)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>12話②</t>
+          <t>第7話①</t>
         </is>
       </c>
     </row>
@@ -1131,17 +2173,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>サーシャちゃんとクラスメイトオタクくん</t>
+          <t>勇者パーティを追放された【スキルサポーター】、仲間のスキルを解放して最強に成り上がる</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>はぐはぐ(著者)</t>
+          <t>作画：なかお 原作：前田氏</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第80話</t>
+          <t>第5話(1)</t>
         </is>
       </c>
     </row>
@@ -1151,17 +2193,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>冒険者ギルドが十二歳からしか入れなかったので、サバよみました。</t>
+          <t>最強の少年聖騎士、転生者を狩る</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>GUNP（漫画） KAME （原作） ox （キャラクター原案）</t>
+          <t>作画：御塩 原作：宇奈木ユラ</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第12話前半</t>
+          <t>第5話(1)</t>
         </is>
       </c>
     </row>
@@ -1171,17 +2213,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>《魔力無限》のマナポーター ～パーティの魔力を全て供給していたのに、勇者に追放されました。魔力不足で聖剣が使えないと焦っても、メンバー全員が勇者を見限ったのでもう遅い～</t>
+          <t>行き着く先は勇者か魔王か　元・廃プレイヤーが征く異世界攻略記</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>漫画：伊藤ひずみ 原作：アトハ キャラクター原案：夕薙</t>
+          <t>輔艮（漫画） ニト（原作） ゆーにっと（原作イラスト）</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第10話 ②</t>
+          <t>第19話　地球</t>
         </is>
       </c>
     </row>
@@ -1191,17 +2233,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>淫獄団地</t>
+          <t>俺だけ使える古代魔法 ～基礎すら使えないと追放された俺の魔法は、実は1万年前に失われた伝説魔法でした～</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+          <t>原作／アトハ 漫画／川上ニナ キャラクター原案／片倉響</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第48話（前編）</t>
+          <t>第1話</t>
         </is>
       </c>
     </row>
@@ -1211,17 +2253,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>ダンジョンの幼なじみ</t>
+          <t>ギャルゲーマーに褒められたい</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>久真やすひさ(著者)</t>
+          <t>げしゅまろ(著者)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第54話</t>
+          <t>35話</t>
         </is>
       </c>
     </row>
@@ -1231,17 +2273,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>オトナを知りたい女友達</t>
+          <t>ラーメン大好き小泉さん</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>望公太(原作) ぷよちゃ(作画)</t>
+          <t>鳴見なる</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第7話 前半</t>
+          <t>14杯目 赤or白</t>
         </is>
       </c>
     </row>
@@ -1251,17 +2293,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>田舎の黒ギャルJKと結婚しました</t>
+          <t>ゲーム　オブ　ファミリア-家族戦記-</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>カヅチ(著者)</t>
+          <t>Ｄ．Ｐ(作画) 山口ミコト(原作)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第16話後半</t>
+          <t>第73話①</t>
         </is>
       </c>
     </row>
@@ -1271,17 +2313,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>異世界迷宮のオーパーツ</t>
+          <t>やり直し令嬢は竜帝陛下を攻略中</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>三狛ハル(著者)</t>
+          <t>柚アンコ(漫画) 永瀬さらさ（角川ビーンズ文庫）(原作) 藤未都也(キャラクター原案)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第1話：先端にお椀がついた棒</t>
+          <t>Episode40-3</t>
         </is>
       </c>
     </row>
@@ -1291,17 +2333,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>ダークサモナーとデキている</t>
+          <t>衛宮さんちの今日のごはん</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>車王(著者)</t>
+          <t>TAa(漫画) 只野まこと(料理監修) ＴＹＰＥ－ＭＯＯＮ(原作)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第72話</t>
+          <t>第74話</t>
         </is>
       </c>
     </row>
@@ -1311,17 +2353,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>ギャルゲーマーに褒められたい</t>
+          <t>無能の中の無能王子　スキル【無能】を授かりましたが、周りの女性は【傾国】【傾城】【奸婦】【毒婦】【悪婦】【妖婦】とかです</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>げしゅまろ(著者)</t>
+          <t>漫画/一夢 原作/福朗 キャラクター原案/菊池政治</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>34話</t>
+          <t>chapter8【5話①】</t>
         </is>
       </c>
     </row>
@@ -1331,17 +2373,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>転生貴族の異世界冒険録 ～カインのやりすぎギルド日記～</t>
+          <t>転生したら没落貴族だったので、【呪言】を極めて家族を救います</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>原作：夜州 漫画：佐々木あかね・香本セトラ キャラクター原案：藻</t>
+          <t>作画：アマセケイ 原作：メソポ・たみあ</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第47話</t>
+          <t>第5話(1)</t>
         </is>
       </c>
     </row>
@@ -1351,17 +2393,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>異世界のんびり農家</t>
+          <t>外れスキル《木の実マスター》 ～スキルの実(食べたら死ぬ)を無限に食べられるようになった件について～</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+          <t>漫画：松琴エア 原作：はにゅう キャラクター原案：イセ川ヤスタカ</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第301話</t>
+          <t>第29話　ライトと救いの子④</t>
         </is>
       </c>
     </row>
@@ -1371,17 +2413,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>小さめの魔法師匠と大きめの魔法少女。report：3</t>
+          <t>最凶貴族は死亡フラグを覆す</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>とりから</t>
+          <t>作画：sudekuma 原作：塚上</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第36話の3</t>
+          <t>第5話(1)</t>
         </is>
       </c>
     </row>
@@ -1391,17 +2433,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
+          <t>弱小国家の英雄王子　～最強の魔術師だけど、さっさと国出て自由に生きてぇぇ！～</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
+          <t>友山アキ（漫画） 楓原こうた（原作） トモゼロ（キャラクター原案）</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第22話</t>
+          <t>第3話　第一皇女護衛戦Ⅱ（前編）</t>
         </is>
       </c>
     </row>
@@ -1411,17 +2453,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>聖液鍛冶屋のエロランタ</t>
+          <t>この冒険者、人類史最強です～外れスキル『鑑定』が『継承』に覚醒したので、数多の英雄たちの力を受け継ぎ無双する～</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>しげきっくす(著者)</t>
+          <t>日之影ソラ みやけりく エシュアル</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第6話後半</t>
+          <t>第27話①双子の錬金術師</t>
         </is>
       </c>
     </row>
@@ -1431,17 +2473,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>ロメリア戦記～伯爵令嬢、魔王を倒した後も人類やばそうだから軍隊組織する～</t>
+          <t>元勇者、今はアイドルのドライバーやってます</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>漫画：上戸 亮 原作：有山リョウ(小学館「ガガガブックス」刊) キャラクター原案：コダマ</t>
+          <t>十本スイ(原作) 舞鶴山画太郎(漫画)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第13話「助けてくれる人々」①</t>
+          <t>第5話-2</t>
         </is>
       </c>
     </row>
@@ -1451,17 +2493,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+          <t>傷口と包帯</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>FUNA 東西 モトエ恵介</t>
+          <t>七井海星</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第118話　会談［その3］</t>
+          <t>第13話　ドキドキ手当て②</t>
         </is>
       </c>
     </row>
@@ -1471,17 +2513,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>まんきつしたい常連さん</t>
+          <t>ストラテジックラバーズ</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>しんみりん(著者)</t>
+          <t>三色網戸。(著者)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第45話前編</t>
+          <t>Move53 ダーク・スクエア②</t>
         </is>
       </c>
     </row>
@@ -1491,17 +2533,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>はずれスキル念動力（ただしレベルＭＡＸ）で無双する～手をかざすだけです。詠唱とか必殺技とかいりません。念じるだけで倒せます～</t>
+          <t>ジゼルの錬金飴</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>さとう うなぽっぽ トダフミト</t>
+          <t>漫画： katoson 原作：斯波 キャラクター原案：LINO</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>9話①</t>
+          <t>単行本 告知</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-07-03
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -17,6 +17,7 @@
     <sheet name="2025-06-30" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="2025-07-01" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="2025-07-02" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="2025-07-03" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -1548,22 +1549,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第30話：一秒の奪い合い①</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第６７話『六花停止』①</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>マツモトケンゴ</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第５９話　筋トレの戦いが始まった（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第3話 前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>板垣恵介 猪原賽 陸井栄史</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第75話　大気の雷(いかづち)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>異世界食堂　洋食のねこや</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>犬塚惇平(ヒーロー文庫／イマジカインフォス)(原作) ヤミザワ(漫画) モロザワ(漫画) エナミカツミ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第39話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>板垣恵介 林たかあき</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第49話 日常</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>10年ぶりに再会したクソガキは清純美少女JKに成長していた</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>緑青黒羽（漫画） 館西夕木（原作） ひげ猫（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第5話　嫉妬、そして嫉妬（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>ハズレ枠の【状態異常スキル】で最強になった俺がすべてを蹂躙するまで</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>鵜吉しょう（作画） 内々けやき（構成） 篠崎 芳（原作） KWKM（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第55話　壁外決戦</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>絶対死なないステラ姫</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>光永康則 大高稲</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第１３話　絶対巣穴に入らない・解（４）</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>漫画/すたひろ 原作/Y.A</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>chapter65【34話②】</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>ひとりぼっちの異世界攻略</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>びび（漫画） 五示正司（原作）</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第225話　俺がもし使い物にならなくなったら…</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>暗殺者である俺のステータスが勇者よりも明らかに強いのだが</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>合鴨ひろゆき（漫画） 赤井まつり（原作） 東西（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第33話　ブルート迷宮Ⅲ</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>クラス転移に巻き込まれたコンビニ店員のおっさん、勇者には必要なかった余り物スキルを駆使して最強となるようです。　コミック版</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>漫画：結城焔 原作：Narrative Works　日浦あやせ キャラクター原案：鱈</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>chapter49【23話②】</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>彼女を奪ったイケメン美少女がなぜか俺まで狙ってくる</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>鹿もみじ(漫画) 福田週人(原作) さなだケイスイ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第9話</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>ネットの『推し』とリアルの『推し』が隣に引っ越してきた</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>カタケイ（漫画） 遥 透子（原作） 秋乃える（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第17話　誤解を紐解く回</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>蜘蛛ですが、なにか？</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>かかし朝浩(著者) 馬場翁(原作) 輝竜司(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第75話その2</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>元最強探索者のおじさん。美少女配信者を助けて大バズりしてしまった。</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>かなたろー(原作) 草壁レイ(漫画)</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第3話　美少女、おじさんにハメられる。②</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>ダウナー系お姉さんに毎日カスの嘘を流し込まれる話</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>生倉のゑる(著者) はるばーど屋(原作者)</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>10話 おまけ</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>序盤で死ぬ最強のサブキャラに転生したので、ゲーム知識で無双する</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>作画：マエD 原作：新人</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第4話(2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>異世界魔法は遅れてる！</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>COMTA（漫画） 樋辻臥命（原作）</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第61話　新月の夜にⅢ</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>肥満令嬢は細くなり、後は傾国の美女（物理）として生きるのみ@COMIC</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>宇斗リクツ（漫画） 八針来夏（原作） 輝竜司（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>【7/1コミックス第１巻発売!!】</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>異世界マンチキン　―HP1のままで最強最速ダンジョン攻略―</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>原作／志瑞 祐 漫画／青桐 良</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>ページ127 多くの援軍</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>ハニートラップ・シェアハウス</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>久慈マサムネ(原作) 神月洸壱(作画)</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第38話「芸能界にスパイは潜む」①</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>竜と歩む成り上がり冒険者道～用済みとしてSランクパーティから追放された回復魔術師、捨てられた先で最強の神竜を復活させてしまう ～　コミック版</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>漫画/＠カリカリうめ 原作/岸本和葉 キャラクター原案/シソ</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>chapter49【25話①】</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>魔王様の街づくり！～最強のダンジョンは近代都市～</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>吉川英朗（漫画） 月夜 涙（GAノベル/SBクリエイティブ刊）　（原作）</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第72話　【炎】の弔い</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>帰ってください！ 阿久津さん</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>長岡太一(著者)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第191話</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>農学博士の異世界無双～禁忌の知識で築くモンスター娘ハーレム～</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>インド僧(原作) ヤスウミ(作画)</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>コミックス告知</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>世界最速のレベルアップ</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>鈴見敦(漫画) 八又ナガト(原作) fame(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第47話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>黒の召喚士</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>天羽 銀（漫画） 迷井豆腐（原作） 黒銀（DIGS）（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第143話　聖槍イクリプスⅣ</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>恋人のフリのフリ</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>むねひろ(著者)</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第7話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追放された【スキルサポーター】、仲間のスキルを解放して最強に成り上がる</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>作画：なかお 原作：前田氏</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第5話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>最強の少年聖騎士、転生者を狩る</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>作画：御塩 原作：宇奈木ユラ</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第5話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>行き着く先は勇者か魔王か　元・廃プレイヤーが征く異世界攻略記</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>輔艮（漫画） ニト（原作） ゆーにっと（原作イラスト）</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第19話　地球</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>俺だけ使える古代魔法 ～基礎すら使えないと追放された俺の魔法は、実は1万年前に失われた伝説魔法でした～</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>原作／アトハ 漫画／川上ニナ キャラクター原案／片倉響</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第1話</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>ギャルゲーマーに褒められたい</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>げしゅまろ(著者)</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>35話</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>ラーメン大好き小泉さん</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>鳴見なる</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>14杯目 赤or白</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>ゲーム　オブ　ファミリア-家族戦記-</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>Ｄ．Ｐ(作画) 山口ミコト(原作)</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第73話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>やり直し令嬢は竜帝陛下を攻略中</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>柚アンコ(漫画) 永瀬さらさ（角川ビーンズ文庫）(原作) 藤未都也(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>Episode40-3</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>衛宮さんちの今日のごはん</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>TAa(漫画) 只野まこと(料理監修) ＴＹＰＥ－ＭＯＯＮ(原作)</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第74話</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>無能の中の無能王子　スキル【無能】を授かりましたが、周りの女性は【傾国】【傾城】【奸婦】【毒婦】【悪婦】【妖婦】とかです</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>漫画/一夢 原作/福朗 キャラクター原案/菊池政治</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>chapter8【5話①】</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>転生したら没落貴族だったので、【呪言】を極めて家族を救います</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>作画：アマセケイ 原作：メソポ・たみあ</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第5話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>外れスキル《木の実マスター》 ～スキルの実(食べたら死ぬ)を無限に食べられるようになった件について～</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>漫画：松琴エア 原作：はにゅう キャラクター原案：イセ川ヤスタカ</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第29話　ライトと救いの子④</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>最凶貴族は死亡フラグを覆す</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>作画：sudekuma 原作：塚上</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第5話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>弱小国家の英雄王子　～最強の魔術師だけど、さっさと国出て自由に生きてぇぇ！～</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>友山アキ（漫画） 楓原こうた（原作） トモゼロ（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第3話　第一皇女護衛戦Ⅱ（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>この冒険者、人類史最強です～外れスキル『鑑定』が『継承』に覚醒したので、数多の英雄たちの力を受け継ぎ無双する～</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>日之影ソラ みやけりく エシュアル</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第27話①双子の錬金術師</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>元勇者、今はアイドルのドライバーやってます</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>十本スイ(原作) 舞鶴山画太郎(漫画)</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第5話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>傷口と包帯</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>七井海星</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第13話　ドキドキ手当て②</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>ストラテジックラバーズ</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>三色網戸。(著者)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>Move53 ダーク・スクエア②</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>ジゼルの錬金飴</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>漫画： katoson 原作：斯波 キャラクター原案：LINO</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>単行本 告知</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+          <t>生徒会にも穴はある！</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>zunta(作画) はらわたさいぞう(原作)</t>
+          <t>むちまろ</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第30話：一秒の奪い合い①</t>
+          <t>第130話	皆で夜遊び（集合編）</t>
         </is>
       </c>
     </row>
@@ -1573,17 +2615,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>光永康則</t>
+          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第６７話『六花停止』①</t>
+          <t>第76話その1</t>
         </is>
       </c>
     </row>
@@ -1593,17 +2635,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+          <t>実は俺、最強でした？</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>マツモトケンゴ</t>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第５９話　筋トレの戦いが始まった（２）</t>
+          <t>第120話　四騎戦決勝戦!!・前編</t>
         </is>
       </c>
     </row>
@@ -1613,17 +2655,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第3話 前編</t>
+          <t>第126話　戦争を終わらせてみるⅡ（前編）</t>
         </is>
       </c>
     </row>
@@ -1633,17 +2675,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>板垣恵介 猪原賽 陸井栄史</t>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第75話　大気の雷(いかづち)</t>
+          <t>第31話 独身貴族はヒラメが大事（3）</t>
         </is>
       </c>
     </row>
@@ -1653,17 +2695,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>異世界食堂　洋食のねこや</t>
+          <t>聖者無双</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>犬塚惇平(ヒーロー文庫／イマジカインフォス)(原作) ヤミザワ(漫画) モロザワ(漫画) エナミカツミ(キャラクター原案)</t>
+          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第39話②</t>
+          <t>第90話　研究者や技術者の故郷（前半）</t>
         </is>
       </c>
     </row>
@@ -1673,17 +2715,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
+          <t>オタクに優しいギャルはいない!?</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>板垣恵介 林たかあき</t>
+          <t>のりしろちゃん魚住さかな</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第49話 日常</t>
+          <t>【#146】最強ギャルズ結成秘話!?</t>
         </is>
       </c>
     </row>
@@ -1693,17 +2735,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>10年ぶりに再会したクソガキは清純美少女JKに成長していた</t>
+          <t>魔法少女リリカルなのは EXCEEDS</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>緑青黒羽（漫画） 館西夕木（原作） ひげ猫（キャラクター原案）</t>
+          <t>都築真紀 川上修一</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第5話　嫉妬、そして嫉妬（前編）</t>
+          <t>第３話②</t>
         </is>
       </c>
     </row>
@@ -1713,17 +2755,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ハズレ枠の【状態異常スキル】で最強になった俺がすべてを蹂躙するまで</t>
+          <t>生徒会役員共</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>鵜吉しょう（作画） 内々けやき（構成） 篠崎 芳（原作） KWKM（キャラクター原案）</t>
+          <t>氏家ト全</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第55話　壁外決戦</t>
+          <t>#403</t>
         </is>
       </c>
     </row>
@@ -1733,17 +2775,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>絶対死なないステラ姫</t>
+          <t>カナン様はあくまでチョロい</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>光永康則 大高稲</t>
+          <t>nonco</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第１３話　絶対巣穴に入らない・解（４）</t>
+          <t>第140話	カナンの文化祭フィナーレ！</t>
         </is>
       </c>
     </row>
@@ -1753,17 +2795,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+          <t>FPSゲームのコーチを引き受けたら依頼主が人気VTuberの美少女だった</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>漫画/すたひろ 原作/Y.A</t>
+          <t>漫画：真広吏希 原作：すかいふぁーむ キャラクター原案：みすみ</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>chapter65【34話②】</t>
+          <t>第7話</t>
         </is>
       </c>
     </row>
@@ -1773,17 +2815,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>ひとりぼっちの異世界攻略</t>
+          <t>ひげを剃る。そして女子高生を拾う。</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>びび（漫画） 五示正司（原作）</t>
+          <t>足立いまる(漫画) しめさば(原作) ぶーた(キャラクター原案)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第225話　俺がもし使い物にならなくなったら…</t>
+          <t>第64話その2</t>
         </is>
       </c>
     </row>
@@ -1793,17 +2835,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>暗殺者である俺のステータスが勇者よりも明らかに強いのだが</t>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>合鴨ひろゆき（漫画） 赤井まつり（原作） 東西（キャラクター原案）</t>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第33話　ブルート迷宮Ⅲ</t>
+          <t>第3話 前編</t>
         </is>
       </c>
     </row>
@@ -1813,17 +2855,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>クラス転移に巻き込まれたコンビニ店員のおっさん、勇者には必要なかった余り物スキルを駆使して最強となるようです。　コミック版</t>
+          <t>魔王討伐したあと、目立ちたくないのでギルドマスターになった</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>漫画：結城焔 原作：Narrative Works　日浦あやせ キャラクター原案：鱈</t>
+          <t>ＲＯＨＧＵＮ(作画) 朱月十話(原作) 鳴瀬ひろふみ(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>chapter49【23話②】</t>
+          <t>第65話-①</t>
         </is>
       </c>
     </row>
@@ -1833,17 +2875,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>彼女を奪ったイケメン美少女がなぜか俺まで狙ってくる</t>
+          <t>勇者は魔王が好きらしい</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>鹿もみじ(漫画) 福田週人(原作) さなだケイスイ(キャラクター原案)</t>
+          <t>赤槻コウ(著者)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第9話</t>
+          <t>第4話-1：激闘！サキュバス戦！</t>
         </is>
       </c>
     </row>
@@ -1853,17 +2895,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ネットの『推し』とリアルの『推し』が隣に引っ越してきた</t>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>カタケイ（漫画） 遥 透子（原作） 秋乃える（キャラクター原案）</t>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第17話　誤解を紐解く回</t>
+          <t>第30話：一秒の奪い合い①</t>
         </is>
       </c>
     </row>
@@ -1873,17 +2915,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>蜘蛛ですが、なにか？</t>
+          <t>すべての人類を破壊する。それらは再生できない。</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>かかし朝浩(著者) 馬場翁(原作) 輝竜司(キャラクター原案)</t>
+          <t>横田卓馬(漫画) 伊瀬勝良(原作)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第75話その2</t>
+          <t>第66話その1</t>
         </is>
       </c>
     </row>
@@ -1893,17 +2935,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>元最強探索者のおじさん。美少女配信者を助けて大バズりしてしまった。</t>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>かなたろー(原作) 草壁レイ(漫画)</t>
+          <t>光永康則</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第3話　美少女、おじさんにハメられる。②</t>
+          <t>第６７話『六花停止』①</t>
         </is>
       </c>
     </row>
@@ -1913,17 +2955,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ダウナー系お姉さんに毎日カスの嘘を流し込まれる話</t>
+          <t>転生したらスライムだった件 番外編 ～とある休暇の過ごし方～</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>生倉のゑる(著者) はるばーど屋(原作者)</t>
+          <t>伏瀬 高田裕三 みっつばー</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>10話 おまけ</t>
+          <t>最終話　帰りなんイザ！！（2）</t>
         </is>
       </c>
     </row>
@@ -1933,17 +2975,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>序盤で死ぬ最強のサブキャラに転生したので、ゲーム知識で無双する</t>
+          <t>よわよわ先生</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>作画：マエD 原作：新人</t>
+          <t>福地カミオ</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第4話(2)</t>
+          <t>第105話	よわよわの母②</t>
         </is>
       </c>
     </row>
@@ -1953,17 +2995,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>異世界魔法は遅れてる！</t>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>COMTA（漫画） 樋辻臥命（原作）</t>
+          <t>マツモトケンゴ</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第61話　新月の夜にⅢ</t>
+          <t>第５９話　筋トレの戦いが始まった（２）</t>
         </is>
       </c>
     </row>
@@ -1973,17 +3015,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>肥満令嬢は細くなり、後は傾国の美女（物理）として生きるのみ@COMIC</t>
+          <t>織田家の長男に生まれました 〜戦国時代に転生したけど、死にたくないので改革を起こします〜</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>宇斗リクツ（漫画） 八針来夏（原作） 輝竜司（キャラクター原案）</t>
+          <t>大沼田伊勢彦 逸見兎歌 平沢下戸</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>【7/1コミックス第１巻発売!!】</t>
+          <t>第32話「不忠者」②</t>
         </is>
       </c>
     </row>
@@ -1993,17 +3035,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>異世界マンチキン　―HP1のままで最強最速ダンジョン攻略―</t>
+          <t>ネクストライフ</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>原作／志瑞 祐 漫画／青桐 良</t>
+          <t>相野仁（ヒーロー文庫／イマジカインフォス）(原作) 市倉とかげ(漫画) 鵜飼沙樹・マニャ子(キャラクター原案)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>ページ127 多くの援軍</t>
+          <t>第66章-2</t>
         </is>
       </c>
     </row>
@@ -2013,17 +3055,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ハニートラップ・シェアハウス</t>
+          <t>外れスキル「世界図書館」による異世界の知識と始める『産業革命』 ～ファイアーアロー？ うるせえ、こっちはライフルだ!!～</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>久慈マサムネ(原作) 神月洸壱(作画)</t>
+          <t>©︎高野ケイ 藤井ふじこ riritto</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第38話「芸能界にスパイは潜む」①</t>
+          <t>第16話 ガラテアの秘策・ヴァーミリオンの流儀②</t>
         </is>
       </c>
     </row>
@@ -2033,17 +3075,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>竜と歩む成り上がり冒険者道～用済みとしてSランクパーティから追放された回復魔術師、捨てられた先で最強の神竜を復活させてしまう ～　コミック版</t>
+          <t>辰巳ヶ原さんの愛からは逃げられない</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>漫画/＠カリカリうめ 原作/岸本和葉 キャラクター原案/シソ</t>
+          <t>槙田ナル(著者)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>chapter49【25話①】</t>
+          <t>コミックス告知</t>
         </is>
       </c>
     </row>
@@ -2053,17 +3095,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>魔王様の街づくり！～最強のダンジョンは近代都市～</t>
+          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>吉川英朗（漫画） 月夜 涙（GAノベル/SBクリエイティブ刊）　（原作）</t>
+          <t>板垣恵介 猪原賽 陸井栄史</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第72話　【炎】の弔い</t>
+          <t>第75話　大気の雷(いかづち)</t>
         </is>
       </c>
     </row>
@@ -2073,17 +3115,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>帰ってください！ 阿久津さん</t>
+          <t>百瀬アキラの初恋破綻中。</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>長岡太一(著者)</t>
+          <t>晴川シンタ</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第191話</t>
+          <t>第29話 一つ屋根の下、雨中。</t>
         </is>
       </c>
     </row>
@@ -2093,17 +3135,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>農学博士の異世界無双～禁忌の知識で築くモンスター娘ハーレム～</t>
+          <t>303号室の神さま</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>インド僧(原作) ヤスウミ(作画)</t>
+          <t>ふに・無9(著者)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>コミックス告知</t>
+          <t>Episode. 17</t>
         </is>
       </c>
     </row>
@@ -2113,17 +3155,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>世界最速のレベルアップ</t>
+          <t>昔滅びた魔王城で拾った犬は、実は伝説の魔獣でした ～隠れ最強職《羊飼い》な貴族の三男坊、いずれ、百魔獣の王となる～</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>鈴見敦(漫画) 八又ナガト(原作) fame(キャラクター原案)</t>
+          <t>あまうい白一 鍋島テツヒロ 松本蓮士</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第47話②</t>
+          <t>第11話 呪いに対する提案</t>
         </is>
       </c>
     </row>
@@ -2133,17 +3175,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>黒の召喚士</t>
+          <t>俺だけ使える古代魔法 ～基礎すら使えないと追放された俺の魔法は、実は1万年前に失われた伝説魔法でした～</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>天羽 銀（漫画） 迷井豆腐（原作） 黒銀（DIGS）（キャラクター原案）</t>
+          <t>原作／アトハ 漫画／川上ニナ キャラクター原案／片倉響</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第143話　聖槍イクリプスⅣ</t>
+          <t>第1話</t>
         </is>
       </c>
     </row>
@@ -2153,17 +3195,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>恋人のフリのフリ</t>
+          <t>異世界食堂　洋食のねこや</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>むねひろ(著者)</t>
+          <t>犬塚惇平(ヒーロー文庫／イマジカインフォス)(原作) ヤミザワ(漫画) モロザワ(漫画) エナミカツミ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第7話①</t>
+          <t>第39話②</t>
         </is>
       </c>
     </row>
@@ -2173,17 +3215,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>勇者パーティを追放された【スキルサポーター】、仲間のスキルを解放して最強に成り上がる</t>
+          <t>10年ぶりに再会したクソガキは清純美少女JKに成長していた</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>作画：なかお 原作：前田氏</t>
+          <t>緑青黒羽（漫画） 館西夕木（原作） ひげ猫（キャラクター原案）</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第5話(1)</t>
+          <t>第5話　嫉妬、そして嫉妬（前編）</t>
         </is>
       </c>
     </row>
@@ -2193,17 +3235,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>最強の少年聖騎士、転生者を狩る</t>
+          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>作画：御塩 原作：宇奈木ユラ</t>
+          <t>板垣恵介 林たかあき</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第5話(1)</t>
+          <t>第49話 日常</t>
         </is>
       </c>
     </row>
@@ -2213,17 +3255,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>行き着く先は勇者か魔王か　元・廃プレイヤーが征く異世界攻略記</t>
+          <t>ガリ勉くんと裏アカさん　散々お世話になっているエロ系裏垢女子の正体がクラスのアイドルだった件</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>輔艮（漫画） ニト（原作） ゆーにっと（原作イラスト）</t>
+          <t>花咲まひる(著者) 鈴木えんぺら(原作) 小花雪(キャラクター原案)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第19話　地球</t>
+          <t>第8話②</t>
         </is>
       </c>
     </row>
@@ -2233,17 +3275,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>俺だけ使える古代魔法 ～基礎すら使えないと追放された俺の魔法は、実は1万年前に失われた伝説魔法でした～</t>
+          <t>妹はカノジョにできないのに</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>原作／アトハ 漫画／川上ニナ キャラクター原案／片倉響</t>
+          <t>ちくわ。(作画) 鏡遊(原作) 三九呂(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第1話</t>
+          <t>第28話②</t>
         </is>
       </c>
     </row>
@@ -2253,17 +3295,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>ギャルゲーマーに褒められたい</t>
+          <t>蜘蛛ですが、なにか？</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>げしゅまろ(著者)</t>
+          <t>かかし朝浩(著者) 馬場翁(原作) 輝竜司(キャラクター原案)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>35話</t>
+          <t>第75話その2</t>
         </is>
       </c>
     </row>
@@ -2273,17 +3315,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ラーメン大好き小泉さん</t>
+          <t>ハズレ枠の【状態異常スキル】で最強になった俺がすべてを蹂躙するまで</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>鳴見なる</t>
+          <t>鵜吉しょう（作画） 内々けやき（構成） 篠崎 芳（原作） KWKM（キャラクター原案）</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>14杯目 赤or白</t>
+          <t>第55話　壁外決戦</t>
         </is>
       </c>
     </row>
@@ -2293,17 +3335,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ゲーム　オブ　ファミリア-家族戦記-</t>
+          <t>千年英雄</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Ｄ．Ｐ(作画) 山口ミコト(原作)</t>
+          <t>原作/福島航平 作画/中村ゆきひろ</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第73話①</t>
+          <t>14話</t>
         </is>
       </c>
     </row>
@@ -2313,17 +3355,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>やり直し令嬢は竜帝陛下を攻略中</t>
+          <t>彼女を奪ったイケメン美少女がなぜか俺まで狙ってくる</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>柚アンコ(漫画) 永瀬さらさ（角川ビーンズ文庫）(原作) 藤未都也(キャラクター原案)</t>
+          <t>鹿もみじ(漫画) 福田週人(原作) さなだケイスイ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Episode40-3</t>
+          <t>第9話</t>
         </is>
       </c>
     </row>
@@ -2333,17 +3375,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>衛宮さんちの今日のごはん</t>
+          <t>絶対死なないステラ姫</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>TAa(漫画) 只野まこと(料理監修) ＴＹＰＥ－ＭＯＯＮ(原作)</t>
+          <t>光永康則 大高稲</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第74話</t>
+          <t>第１３話　絶対巣穴に入らない・解（４）</t>
         </is>
       </c>
     </row>
@@ -2353,17 +3395,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>無能の中の無能王子　スキル【無能】を授かりましたが、周りの女性は【傾国】【傾城】【奸婦】【毒婦】【悪婦】【妖婦】とかです</t>
+          <t>暗殺者である俺のステータスが勇者よりも明らかに強いのだが</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>漫画/一夢 原作/福朗 キャラクター原案/菊池政治</t>
+          <t>合鴨ひろゆき（漫画） 赤井まつり（原作） 東西（キャラクター原案）</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>chapter8【5話①】</t>
+          <t>第33話　ブルート迷宮Ⅲ</t>
         </is>
       </c>
     </row>
@@ -2373,17 +3415,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>転生したら没落貴族だったので、【呪言】を極めて家族を救います</t>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>作画：アマセケイ 原作：メソポ・たみあ</t>
+          <t>漫画/すたひろ 原作/Y.A</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第5話(1)</t>
+          <t>chapter65【34話②】</t>
         </is>
       </c>
     </row>
@@ -2393,17 +3435,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>外れスキル《木の実マスター》 ～スキルの実(食べたら死ぬ)を無限に食べられるようになった件について～</t>
+          <t>クラス転移に巻き込まれたコンビニ店員のおっさん、勇者には必要なかった余り物スキルを駆使して最強となるようです。　コミック版</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>漫画：松琴エア 原作：はにゅう キャラクター原案：イセ川ヤスタカ</t>
+          <t>漫画：結城焔 原作：Narrative Works　日浦あやせ キャラクター原案：鱈</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第29話　ライトと救いの子④</t>
+          <t>chapter49【23話②】</t>
         </is>
       </c>
     </row>
@@ -2413,17 +3455,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>最凶貴族は死亡フラグを覆す</t>
+          <t>ひとりぼっちの異世界攻略</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>作画：sudekuma 原作：塚上</t>
+          <t>びび（漫画） 五示正司（原作）</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第5話(1)</t>
+          <t>第225話　俺がもし使い物にならなくなったら…</t>
         </is>
       </c>
     </row>
@@ -2433,17 +3475,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>弱小国家の英雄王子　～最強の魔術師だけど、さっさと国出て自由に生きてぇぇ！～</t>
+          <t>ネットの『推し』とリアルの『推し』が隣に引っ越してきた</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>友山アキ（漫画） 楓原こうた（原作） トモゼロ（キャラクター原案）</t>
+          <t>カタケイ（漫画） 遥 透子（原作） 秋乃える（キャラクター原案）</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第3話　第一皇女護衛戦Ⅱ（前編）</t>
+          <t>第17話　誤解を紐解く回</t>
         </is>
       </c>
     </row>
@@ -2453,17 +3495,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>この冒険者、人類史最強です～外れスキル『鑑定』が『継承』に覚醒したので、数多の英雄たちの力を受け継ぎ無双する～</t>
+          <t>ダウナー系お姉さんに毎日カスの嘘を流し込まれる話</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>日之影ソラ みやけりく エシュアル</t>
+          <t>生倉のゑる(著者) はるばーど屋(原作者)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第27話①双子の錬金術師</t>
+          <t>10話 おまけ</t>
         </is>
       </c>
     </row>
@@ -2473,17 +3515,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>元勇者、今はアイドルのドライバーやってます</t>
+          <t>帰ってください！ 阿久津さん</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>十本スイ(原作) 舞鶴山画太郎(漫画)</t>
+          <t>長岡太一(著者)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第5話-2</t>
+          <t>第191話</t>
         </is>
       </c>
     </row>
@@ -2493,17 +3535,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>傷口と包帯</t>
+          <t>異世界おじさん</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>七井海星</t>
+          <t>殆ど死んでいる(著者)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第13話　ドキドキ手当て②</t>
+          <t>第69話</t>
         </is>
       </c>
     </row>
@@ -2513,17 +3555,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>ストラテジックラバーズ</t>
+          <t>アンゴルモア 元寇合戦記　【博多編】</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>三色網戸。(著者)</t>
+          <t>たかぎ七彦(著者)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Move53 ダーク・スクエア②</t>
+          <t>第四十四話その三</t>
         </is>
       </c>
     </row>
@@ -2533,17 +3575,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>ジゼルの錬金飴</t>
+          <t>カッコウの許嫁</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>漫画： katoson 原作：斯波 キャラクター原案：LINO</t>
+          <t>吉河美希</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>単行本 告知</t>
+          <t>第253話	4時間しか寝てなくない!?</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-07-04
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -18,6 +18,7 @@
     <sheet name="2025-07-01" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="2025-07-02" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="2025-07-03" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="2025-07-04" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -2590,22 +2591,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>生徒会にも穴はある！</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>むちまろ</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第130話	皆で夜遊び（集合編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第76話その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第120話　四騎戦決勝戦!!・前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第126話　戦争を終わらせてみるⅡ（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第31話 独身貴族はヒラメが大事（3）</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>聖者無双</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第90話　研究者や技術者の故郷（前半）</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>オタクに優しいギャルはいない!?</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>のりしろちゃん魚住さかな</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>【#146】最強ギャルズ結成秘話!?</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>魔法少女リリカルなのは EXCEEDS</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>都築真紀 川上修一</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第３話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>生徒会役員共</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>氏家ト全</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>#403</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>カナン様はあくまでチョロい</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>nonco</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第140話	カナンの文化祭フィナーレ！</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>FPSゲームのコーチを引き受けたら依頼主が人気VTuberの美少女だった</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>漫画：真広吏希 原作：すかいふぁーむ キャラクター原案：みすみ</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第7話</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>ひげを剃る。そして女子高生を拾う。</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>足立いまる(漫画) しめさば(原作) ぶーた(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第64話その2</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第3話 前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>魔王討伐したあと、目立ちたくないのでギルドマスターになった</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>ＲＯＨＧＵＮ(作画) 朱月十話(原作) 鳴瀬ひろふみ(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第65話-①</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>勇者は魔王が好きらしい</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>赤槻コウ(著者)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第4話-1：激闘！サキュバス戦！</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第30話：一秒の奪い合い①</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>すべての人類を破壊する。それらは再生できない。</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>横田卓馬(漫画) 伊瀬勝良(原作)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第66話その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第６７話『六花停止』①</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>転生したらスライムだった件 番外編 ～とある休暇の過ごし方～</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>伏瀬 高田裕三 みっつばー</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>最終話　帰りなんイザ！！（2）</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>よわよわ先生</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>福地カミオ</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第105話	よわよわの母②</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>マツモトケンゴ</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第５９話　筋トレの戦いが始まった（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>織田家の長男に生まれました 〜戦国時代に転生したけど、死にたくないので改革を起こします〜</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>大沼田伊勢彦 逸見兎歌 平沢下戸</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第32話「不忠者」②</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>ネクストライフ</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>相野仁（ヒーロー文庫／イマジカインフォス）(原作) 市倉とかげ(漫画) 鵜飼沙樹・マニャ子(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第66章-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>外れスキル「世界図書館」による異世界の知識と始める『産業革命』 ～ファイアーアロー？ うるせえ、こっちはライフルだ!!～</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>©︎高野ケイ 藤井ふじこ riritto</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第16話 ガラテアの秘策・ヴァーミリオンの流儀②</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>辰巳ヶ原さんの愛からは逃げられない</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>槙田ナル(著者)</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>コミックス告知</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>板垣恵介 猪原賽 陸井栄史</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第75話　大気の雷(いかづち)</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>百瀬アキラの初恋破綻中。</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>晴川シンタ</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第29話 一つ屋根の下、雨中。</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>303号室の神さま</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>ふに・無9(著者)</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>Episode. 17</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>昔滅びた魔王城で拾った犬は、実は伝説の魔獣でした ～隠れ最強職《羊飼い》な貴族の三男坊、いずれ、百魔獣の王となる～</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>あまうい白一 鍋島テツヒロ 松本蓮士</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第11話 呪いに対する提案</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>俺だけ使える古代魔法 ～基礎すら使えないと追放された俺の魔法は、実は1万年前に失われた伝説魔法でした～</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>原作／アトハ 漫画／川上ニナ キャラクター原案／片倉響</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第1話</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>異世界食堂　洋食のねこや</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>犬塚惇平(ヒーロー文庫／イマジカインフォス)(原作) ヤミザワ(漫画) モロザワ(漫画) エナミカツミ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第39話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>10年ぶりに再会したクソガキは清純美少女JKに成長していた</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>緑青黒羽（漫画） 館西夕木（原作） ひげ猫（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第5話　嫉妬、そして嫉妬（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>板垣恵介 林たかあき</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第49話 日常</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>ガリ勉くんと裏アカさん　散々お世話になっているエロ系裏垢女子の正体がクラスのアイドルだった件</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>花咲まひる(著者) 鈴木えんぺら(原作) 小花雪(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第8話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>妹はカノジョにできないのに</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>ちくわ。(作画) 鏡遊(原作) 三九呂(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第28話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>蜘蛛ですが、なにか？</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>かかし朝浩(著者) 馬場翁(原作) 輝竜司(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第75話その2</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>ハズレ枠の【状態異常スキル】で最強になった俺がすべてを蹂躙するまで</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>鵜吉しょう（作画） 内々けやき（構成） 篠崎 芳（原作） KWKM（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第55話　壁外決戦</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>千年英雄</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>原作/福島航平 作画/中村ゆきひろ</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>14話</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>彼女を奪ったイケメン美少女がなぜか俺まで狙ってくる</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>鹿もみじ(漫画) 福田週人(原作) さなだケイスイ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第9話</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>絶対死なないステラ姫</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>光永康則 大高稲</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第１３話　絶対巣穴に入らない・解（４）</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>暗殺者である俺のステータスが勇者よりも明らかに強いのだが</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>合鴨ひろゆき（漫画） 赤井まつり（原作） 東西（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第33話　ブルート迷宮Ⅲ</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>漫画/すたひろ 原作/Y.A</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>chapter65【34話②】</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>クラス転移に巻き込まれたコンビニ店員のおっさん、勇者には必要なかった余り物スキルを駆使して最強となるようです。　コミック版</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>漫画：結城焔 原作：Narrative Works　日浦あやせ キャラクター原案：鱈</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>chapter49【23話②】</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>ひとりぼっちの異世界攻略</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>びび（漫画） 五示正司（原作）</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第225話　俺がもし使い物にならなくなったら…</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>ネットの『推し』とリアルの『推し』が隣に引っ越してきた</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>カタケイ（漫画） 遥 透子（原作） 秋乃える（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第17話　誤解を紐解く回</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>ダウナー系お姉さんに毎日カスの嘘を流し込まれる話</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>生倉のゑる(著者) はるばーど屋(原作者)</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>10話 おまけ</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>帰ってください！ 阿久津さん</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>長岡太一(著者)</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第191話</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>異世界おじさん</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>殆ど死んでいる(著者)</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第69話</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>アンゴルモア 元寇合戦記　【博多編】</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>たかぎ七彦(著者)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第四十四話その三</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>カッコウの許嫁</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>吉河美希</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第253話	4時間しか寝てなくない!?</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>生徒会にも穴はある！</t>
+          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>むちまろ</t>
+          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第130話	皆で夜遊び（集合編）</t>
+          <t>第10話</t>
         </is>
       </c>
     </row>
@@ -2615,17 +3657,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
+          <t>戸賀 環 坂木持丸 riritto</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第76話その1</t>
+          <t>第48話②　お祭りを楽しんでみた</t>
         </is>
       </c>
     </row>
@@ -2635,17 +3677,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>実は俺、最強でした？</t>
+          <t>ライドンキング</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>原作：澄守 彩 漫画：高橋 愛</t>
+          <t>馬場康誌</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第120話　四騎戦決勝戦!!・前編</t>
+          <t>第80話 大統領と白の魔導師（後編）</t>
         </is>
       </c>
     </row>
@@ -2655,17 +3697,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>異世界魔王と召喚少女の奴隷魔術</t>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+          <t>村上よしゆき 茨木野 あるてら</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第126話　戦争を終わらせてみるⅡ（前編）</t>
+          <t>第４０話　勇者、聖女と元聖騎士と再会し、魚人を追っ払う（３）</t>
         </is>
       </c>
     </row>
@@ -2675,17 +3717,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+          <t>英雄女騎士に有能とバレた俺の美人ハーレム騎士団 ガイカク・ヒクメの奇術騎士団</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+          <t>明石六郎(原作) 太盛(作画) 氷室しゅんすけ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第31話 独身貴族はヒラメが大事（3）</t>
+          <t>第9話</t>
         </is>
       </c>
     </row>
@@ -2695,17 +3737,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>聖者無双</t>
+          <t>ライブダンジョン！</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
+          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第90話　研究者や技術者の故郷（前半）</t>
+          <t>第87話後半</t>
         </is>
       </c>
     </row>
@@ -2715,17 +3757,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>オタクに優しいギャルはいない!?</t>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>のりしろちゃん魚住さかな</t>
+          <t>空野進 sorani ファルまろ</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>【#146】最強ギャルズ結成秘話!?</t>
+          <t>番外編　最弱貴族、寝込む</t>
         </is>
       </c>
     </row>
@@ -2735,17 +3777,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>魔法少女リリカルなのは EXCEEDS</t>
+          <t>黄金の経験値</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>都築真紀 川上修一</t>
+          <t>原純(原作) 霜月汐(作画) fixro2n(キャラクター原案)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第３話②</t>
+          <t>第16話（後編）</t>
         </is>
       </c>
     </row>
@@ -2755,17 +3797,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>生徒会役員共</t>
+          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>氏家ト全</t>
+          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>#403</t>
+          <t>第1話③</t>
         </is>
       </c>
     </row>
@@ -2775,17 +3817,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>カナン様はあくまでチョロい</t>
+          <t>じつは義妹でした。～最近できた義理の弟の距離感がやたら近いわけ～</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>nonco</t>
+          <t>堺しょうきち(著者) 白井ムク(原作) 千種みのり(キャラクター原案)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第140話	カナンの文化祭フィナーレ！</t>
+          <t>第35話-2</t>
         </is>
       </c>
     </row>
@@ -2795,17 +3837,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>FPSゲームのコーチを引き受けたら依頼主が人気VTuberの美少女だった</t>
+          <t>私、蜘蛛なモンスターをテイムしたので、スパイダーシルクで裁縫を頑張ります！</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>漫画：真広吏希 原作：すかいふぁーむ キャラクター原案：みすみ</t>
+          <t>あきさけ(原作) さんねこ(作画) タムラヨウ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第7話</t>
+          <t>第5話</t>
         </is>
       </c>
     </row>
@@ -2815,17 +3857,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>ひげを剃る。そして女子高生を拾う。</t>
+          <t>貧乏騎士に嫁入りしたはずが!? ~野人令嬢は皇太子妃になっても竜を狩りたい~</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>足立いまる(漫画) しめさば(原作) ぶーた(キャラクター原案)</t>
+          <t>漫画：夏川そぞろ 原作：宮前葵 キャラクター原案：ののまろ</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第64話その2</t>
+          <t>第10話②皇太子妃（仮）</t>
         </is>
       </c>
     </row>
@@ -2835,17 +3877,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+          <t>となりの席のヤツがそういう目で見てくる</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+          <t>mmk</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第3話 前編</t>
+          <t>第39話 聞きたいこと</t>
         </is>
       </c>
     </row>
@@ -2855,17 +3897,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>魔王討伐したあと、目立ちたくないのでギルドマスターになった</t>
+          <t>【悲報】清楚系で売っていた底辺配信者、うっかり配信を切り忘れたままSS級モンスターを拳で殴り飛ばしてしまう</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>ＲＯＨＧＵＮ(作画) 朱月十話(原作) 鳴瀬ひろふみ(キャラクターデザイン)</t>
+          <t>アトハ NEO草野 pupps</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第65話-①</t>
+          <t>第４話　【悲報】ご乱行⁉ ダンジョンシーカー・アカデミー！（２）</t>
         </is>
       </c>
     </row>
@@ -2875,17 +3917,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>勇者は魔王が好きらしい</t>
+          <t>生徒会にも穴はある！</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>赤槻コウ(著者)</t>
+          <t>むちまろ</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第4話-1：激闘！サキュバス戦！</t>
+          <t>第130話	皆で夜遊び（集合編）</t>
         </is>
       </c>
     </row>
@@ -2895,17 +3937,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+          <t>規格外のダンジョン攻略者、実は異世界帰りの元勇者</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>zunta(作画) はらわたさいぞう(原作)</t>
+          <t>作画：やまざき君 原作：榊与一</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第30話：一秒の奪い合い①</t>
+          <t>第3話(3)</t>
         </is>
       </c>
     </row>
@@ -2915,17 +3957,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>すべての人類を破壊する。それらは再生できない。</t>
+          <t>僕は今すぐ前世の記憶を捨てたい。～憧れの田舎は人外魔境でした～@COMIC</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>横田卓馬(漫画) 伊瀬勝良(原作)</t>
+          <t>大島つむぎ （漫画） 星畑旭（原作） スズキイオリ （キャラクター原案）</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第66話その1</t>
+          <t>第18話 ②</t>
         </is>
       </c>
     </row>
@@ -2935,17 +3977,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+          <t>ようこそ『追放者ギルド』へ ～無能なＳランクパーティがどんどん有能な冒険者を追放するので、最弱を集めて最強ギルドを創ります～</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>光永康則</t>
+          <t>荒木佑輔(作画) メソポ・たみあ(原作) U助(キャラクター原案)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第６７話『六花停止』①</t>
+          <t>第40話</t>
         </is>
       </c>
     </row>
@@ -2955,17 +3997,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>転生したらスライムだった件 番外編 ～とある休暇の過ごし方～</t>
+          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>伏瀬 高田裕三 みっつばー</t>
+          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>最終話　帰りなんイザ！！（2）</t>
+          <t>第76話その1</t>
         </is>
       </c>
     </row>
@@ -2975,17 +4017,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>よわよわ先生</t>
+          <t>誰が勇者を殺したか</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>福地カミオ</t>
+          <t>石田あきら(漫画) 駄犬(原作) toi8(キャラクター原案)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第105話	よわよわの母②</t>
+          <t>第5話</t>
         </is>
       </c>
     </row>
@@ -2995,17 +4037,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+          <t>実は俺、最強でした？</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>マツモトケンゴ</t>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第５９話　筋トレの戦いが始まった（２）</t>
+          <t>第120話　四騎戦決勝戦!!・前編</t>
         </is>
       </c>
     </row>
@@ -3015,17 +4057,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>織田家の長男に生まれました 〜戦国時代に転生したけど、死にたくないので改革を起こします〜</t>
+          <t>ギルド追放された雑用係の下剋上～超万能な生活スキルで世界最強～</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>大沼田伊勢彦 逸見兎歌 平沢下戸</t>
+          <t>原作／夜桜ユノ 漫画／柳輪 ネーム構成／ユーキあきら</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第32話「不忠者」②</t>
+          <t>第62話</t>
         </is>
       </c>
     </row>
@@ -3035,17 +4077,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ネクストライフ</t>
+          <t>ギャルゲーマーに褒められたい</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>相野仁（ヒーロー文庫／イマジカインフォス）(原作) 市倉とかげ(漫画) 鵜飼沙樹・マニャ子(キャラクター原案)</t>
+          <t>げしゅまろ(著者)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第66章-2</t>
+          <t>36話</t>
         </is>
       </c>
     </row>
@@ -3055,17 +4097,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>外れスキル「世界図書館」による異世界の知識と始める『産業革命』 ～ファイアーアロー？ うるせえ、こっちはライフルだ!!～</t>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>©︎高野ケイ 藤井ふじこ riritto</t>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第16話 ガラテアの秘策・ヴァーミリオンの流儀②</t>
+          <t>第126話　戦争を終わらせてみるⅡ（前編）</t>
         </is>
       </c>
     </row>
@@ -3075,17 +4117,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>辰巳ヶ原さんの愛からは逃げられない</t>
+          <t>ルパン三世 異世界の姫君（ネイバーワールドプリンセス）</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>槙田ナル(著者)</t>
+          <t>モンキー・パンチ／エム・ピー・ワークス 内々けやき 佐伯庸介 白狼</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>コミックス告知</t>
+          <t>第99話：泥棒、心を盗めど縛りはせず❷</t>
         </is>
       </c>
     </row>
@@ -3095,17 +4137,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
+          <t>自分の事を主人公だと信じてやまない踏み台が、主人公を踏み台だと勘違いして、優勝してしまうお話です@COMIC</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>板垣恵介 猪原賽 陸井栄史</t>
+          <t>KYO=H（漫画） 流石ユユシタ（原作） 卵の黄身（キャラクター原案）</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第75話　大気の雷(いかづち)</t>
+          <t>第4話</t>
         </is>
       </c>
     </row>
@@ -3115,17 +4157,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>百瀬アキラの初恋破綻中。</t>
+          <t>直径3cmの召喚陣&lt;リミットリング&gt;で「雑魚すら呼べない」と蔑まれた底辺召喚士が頂点に立つまで</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>晴川シンタ</t>
+          <t>作画：まっつー 原作：空松蓮司</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第29話 一つ屋根の下、雨中。</t>
+          <t>第3話(3)</t>
         </is>
       </c>
     </row>
@@ -3135,17 +4177,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>303号室の神さま</t>
+          <t>聖者無双</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ふに・無9(著者)</t>
+          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Episode. 17</t>
+          <t>第90話　研究者や技術者の故郷（前半）</t>
         </is>
       </c>
     </row>
@@ -3155,17 +4197,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>昔滅びた魔王城で拾った犬は、実は伝説の魔獣でした ～隠れ最強職《羊飼い》な貴族の三男坊、いずれ、百魔獣の王となる～</t>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>あまうい白一 鍋島テツヒロ 松本蓮士</t>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第11話 呪いに対する提案</t>
+          <t>第31話 独身貴族はヒラメが大事（3）</t>
         </is>
       </c>
     </row>
@@ -3175,17 +4217,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>俺だけ使える古代魔法 ～基礎すら使えないと追放された俺の魔法は、実は1万年前に失われた伝説魔法でした～</t>
+          <t>FPSゲームのコーチを引き受けたら依頼主が人気VTuberの美少女だった</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>原作／アトハ 漫画／川上ニナ キャラクター原案／片倉響</t>
+          <t>漫画：真広吏希 原作：すかいふぁーむ キャラクター原案：みすみ</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第1話</t>
+          <t>単行本1巻発売告知</t>
         </is>
       </c>
     </row>
@@ -3195,17 +4237,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>異世界食堂　洋食のねこや</t>
+          <t>君の刀が折れるまで ~月宮まつりの恋難き~</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>犬塚惇平(ヒーロー文庫／イマジカインフォス)(原作) ヤミザワ(漫画) モロザワ(漫画) エナミカツミ(キャラクター原案)</t>
+          <t>イノウエ</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第39話②</t>
+          <t>第37話 日永のこと</t>
         </is>
       </c>
     </row>
@@ -3215,17 +4257,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>10年ぶりに再会したクソガキは清純美少女JKに成長していた</t>
+          <t>ゲーム内最強の『裏ボス』に転生したので、主人公の代わりに最速クリアを目指します！</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>緑青黒羽（漫画） 館西夕木（原作） ひげ猫（キャラクター原案）</t>
+          <t>作画：こめぐ 原作：迅空也</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第5話　嫉妬、そして嫉妬（前編）</t>
+          <t>第3話(3)</t>
         </is>
       </c>
     </row>
@@ -3235,17 +4277,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
+          <t>魔法少女リリカルなのは EXCEEDS</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>板垣恵介 林たかあき</t>
+          <t>都築真紀 川上修一</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第49話 日常</t>
+          <t>第３話②</t>
         </is>
       </c>
     </row>
@@ -3255,17 +4297,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ガリ勉くんと裏アカさん　散々お世話になっているエロ系裏垢女子の正体がクラスのアイドルだった件</t>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>花咲まひる(著者) 鈴木えんぺら(原作) 小花雪(キャラクター原案)</t>
+          <t>光永康則</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第8話②</t>
+          <t>第６７話『六花停止』①</t>
         </is>
       </c>
     </row>
@@ -3275,17 +4317,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>妹はカノジョにできないのに</t>
+          <t>金色の文字使い ―勇者四人に巻き込まれたユニークチート―</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>ちくわ。(作画) 鏡遊(原作) 三九呂(キャラクターデザイン)</t>
+          <t>尾崎祐介(作画) 十本スイ(原作) すまき俊悟(キャラクター原案)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第28話②</t>
+          <t>第117話</t>
         </is>
       </c>
     </row>
@@ -3295,17 +4337,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>蜘蛛ですが、なにか？</t>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>かかし朝浩(著者) 馬場翁(原作) 輝竜司(キャラクター原案)</t>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第75話その2</t>
+          <t>第30話：一秒の奪い合い①</t>
         </is>
       </c>
     </row>
@@ -3315,17 +4357,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ハズレ枠の【状態異常スキル】で最強になった俺がすべてを蹂躙するまで</t>
+          <t>冒険者アル あいつの魔法はおかしい@COMIC</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>鵜吉しょう（作画） 内々けやき（構成） 篠崎 芳（原作） KWKM（キャラクター原案）</t>
+          <t>山﨑と子（漫画） れもん（原作） sime（キャラクター原案）</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第55話　壁外決戦</t>
+          <t>第14話 ①</t>
         </is>
       </c>
     </row>
@@ -3345,7 +4387,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>14話</t>
+          <t>15話</t>
         </is>
       </c>
     </row>
@@ -3355,17 +4397,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>彼女を奪ったイケメン美少女がなぜか俺まで狙ってくる</t>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>鹿もみじ(漫画) 福田週人(原作) さなだケイスイ(キャラクター原案)</t>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第9話</t>
+          <t>第3話 前編</t>
         </is>
       </c>
     </row>
@@ -3375,17 +4417,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>絶対死なないステラ姫</t>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>光永康則 大高稲</t>
+          <t>マツモトケンゴ</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第１３話　絶対巣穴に入らない・解（４）</t>
+          <t>第５９話　筋トレの戦いが始まった（２）</t>
         </is>
       </c>
     </row>
@@ -3395,17 +4437,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>暗殺者である俺のステータスが勇者よりも明らかに強いのだが</t>
+          <t>オタクに優しいギャルはいない!?</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>合鴨ひろゆき（漫画） 赤井まつり（原作） 東西（キャラクター原案）</t>
+          <t>のりしろちゃん魚住さかな</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第33話　ブルート迷宮Ⅲ</t>
+          <t>【#146】最強ギャルズ結成秘話!?</t>
         </is>
       </c>
     </row>
@@ -3415,17 +4457,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+          <t>カナン様はあくまでチョロい</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>漫画/すたひろ 原作/Y.A</t>
+          <t>nonco</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>chapter65【34話②】</t>
+          <t>第140話	カナンの文化祭フィナーレ！</t>
         </is>
       </c>
     </row>
@@ -3435,17 +4477,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>クラス転移に巻き込まれたコンビニ店員のおっさん、勇者には必要なかった余り物スキルを駆使して最強となるようです。　コミック版</t>
+          <t>黒魔法寮の三悪人</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>漫画：結城焔 原作：Narrative Works　日浦あやせ キャラクター原案：鱈</t>
+          <t>斎藤キミオ</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>chapter49【23話②】</t>
+          <t>第39話 黒魔法寮生のクッキングだよ♪</t>
         </is>
       </c>
     </row>
@@ -3455,17 +4497,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ひとりぼっちの異世界攻略</t>
+          <t>生徒会役員共</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>びび（漫画） 五示正司（原作）</t>
+          <t>氏家ト全</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第225話　俺がもし使い物にならなくなったら…</t>
+          <t>#403</t>
         </is>
       </c>
     </row>
@@ -3475,17 +4517,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ネットの『推し』とリアルの『推し』が隣に引っ越してきた</t>
+          <t>ひげを剃る。そして女子高生を拾う。</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>カタケイ（漫画） 遥 透子（原作） 秋乃える（キャラクター原案）</t>
+          <t>足立いまる(漫画) しめさば(原作) ぶーた(キャラクター原案)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第17話　誤解を紐解く回</t>
+          <t>第64話その2</t>
         </is>
       </c>
     </row>
@@ -3495,17 +4537,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>ダウナー系お姉さんに毎日カスの嘘を流し込まれる話</t>
+          <t>無能と蔑まれた【勇気ある者】が、実は伝説の【勇者】でした~500年前の仲間＆魔王の娘と一緒に今度こそ世界を救います~</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>生倉のゑる(著者) はるばーど屋(原作者)</t>
+          <t>作画：シグチサトシ 原作：やすくん</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>10話 おまけ</t>
+          <t>第3話(3)</t>
         </is>
       </c>
     </row>
@@ -3515,17 +4557,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>帰ってください！ 阿久津さん</t>
+          <t>俺だけ使える古代魔法 ～基礎すら使えないと追放された俺の魔法は、実は1万年前に失われた伝説魔法でした～</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>長岡太一(著者)</t>
+          <t>原作／アトハ 漫画／川上ニナ キャラクター原案／片倉響</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第191話</t>
+          <t>第1話</t>
         </is>
       </c>
     </row>
@@ -3535,17 +4577,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>異世界おじさん</t>
+          <t>勇者は魔王が好きらしい</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>殆ど死んでいる(著者)</t>
+          <t>赤槻コウ(著者)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第69話</t>
+          <t>第4話-1：激闘！サキュバス戦！</t>
         </is>
       </c>
     </row>
@@ -3555,17 +4597,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>アンゴルモア 元寇合戦記　【博多編】</t>
+          <t>魔王討伐したあと、目立ちたくないのでギルドマスターになった</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>たかぎ七彦(著者)</t>
+          <t>ＲＯＨＧＵＮ(作画) 朱月十話(原作) 鳴瀬ひろふみ(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第四十四話その三</t>
+          <t>第65話-①</t>
         </is>
       </c>
     </row>
@@ -3575,17 +4617,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>カッコウの許嫁</t>
+          <t>蜘蛛ですが、なにか？</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>吉河美希</t>
+          <t>かかし朝浩(著者) 馬場翁(原作) 輝竜司(キャラクター原案)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第253話	4時間しか寝てなくない!?</t>
+          <t>第75話その2</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-07-05
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -19,6 +19,7 @@
     <sheet name="2025-07-02" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="2025-07-03" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="2025-07-04" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="2025-07-05" sheetId="14" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -3632,22 +3633,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第10話</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>戸賀 環 坂木持丸 riritto</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第48話②　お祭りを楽しんでみた</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>ライドンキング</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>馬場康誌</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第80話 大統領と白の魔導師（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>村上よしゆき 茨木野 あるてら</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第４０話　勇者、聖女と元聖騎士と再会し、魚人を追っ払う（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>英雄女騎士に有能とバレた俺の美人ハーレム騎士団 ガイカク・ヒクメの奇術騎士団</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>明石六郎(原作) 太盛(作画) 氷室しゅんすけ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第9話</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>ライブダンジョン！</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第87話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>空野進 sorani ファルまろ</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>番外編　最弱貴族、寝込む</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>黄金の経験値</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>原純(原作) 霜月汐(作画) fixro2n(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第16話（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第1話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>じつは義妹でした。～最近できた義理の弟の距離感がやたら近いわけ～</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>堺しょうきち(著者) 白井ムク(原作) 千種みのり(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第35話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>私、蜘蛛なモンスターをテイムしたので、スパイダーシルクで裁縫を頑張ります！</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>あきさけ(原作) さんねこ(作画) タムラヨウ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>貧乏騎士に嫁入りしたはずが!? ~野人令嬢は皇太子妃になっても竜を狩りたい~</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>漫画：夏川そぞろ 原作：宮前葵 キャラクター原案：ののまろ</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第10話②皇太子妃（仮）</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>となりの席のヤツがそういう目で見てくる</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>mmk</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第39話 聞きたいこと</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>【悲報】清楚系で売っていた底辺配信者、うっかり配信を切り忘れたままSS級モンスターを拳で殴り飛ばしてしまう</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>アトハ NEO草野 pupps</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第４話　【悲報】ご乱行⁉ ダンジョンシーカー・アカデミー！（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>生徒会にも穴はある！</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>むちまろ</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第130話	皆で夜遊び（集合編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>規格外のダンジョン攻略者、実は異世界帰りの元勇者</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>作画：やまざき君 原作：榊与一</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第3話(3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>僕は今すぐ前世の記憶を捨てたい。～憧れの田舎は人外魔境でした～@COMIC</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>大島つむぎ （漫画） 星畑旭（原作） スズキイオリ （キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第18話 ②</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>ようこそ『追放者ギルド』へ ～無能なＳランクパーティがどんどん有能な冒険者を追放するので、最弱を集めて最強ギルドを創ります～</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>荒木佑輔(作画) メソポ・たみあ(原作) U助(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第40話</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第76話その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>誰が勇者を殺したか</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>石田あきら(漫画) 駄犬(原作) toi8(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第120話　四騎戦決勝戦!!・前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>ギルド追放された雑用係の下剋上～超万能な生活スキルで世界最強～</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>原作／夜桜ユノ 漫画／柳輪 ネーム構成／ユーキあきら</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第62話</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>ギャルゲーマーに褒められたい</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>げしゅまろ(著者)</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>36話</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第126話　戦争を終わらせてみるⅡ（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>ルパン三世 異世界の姫君（ネイバーワールドプリンセス）</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>モンキー・パンチ／エム・ピー・ワークス 内々けやき 佐伯庸介 白狼</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第99話：泥棒、心を盗めど縛りはせず❷</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>自分の事を主人公だと信じてやまない踏み台が、主人公を踏み台だと勘違いして、優勝してしまうお話です@COMIC</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>KYO=H（漫画） 流石ユユシタ（原作） 卵の黄身（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第4話</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>直径3cmの召喚陣&lt;リミットリング&gt;で「雑魚すら呼べない」と蔑まれた底辺召喚士が頂点に立つまで</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>作画：まっつー 原作：空松蓮司</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第3話(3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>聖者無双</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第90話　研究者や技術者の故郷（前半）</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第31話 独身貴族はヒラメが大事（3）</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>FPSゲームのコーチを引き受けたら依頼主が人気VTuberの美少女だった</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>漫画：真広吏希 原作：すかいふぁーむ キャラクター原案：みすみ</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>単行本1巻発売告知</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>君の刀が折れるまで ~月宮まつりの恋難き~</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>イノウエ</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第37話 日永のこと</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>ゲーム内最強の『裏ボス』に転生したので、主人公の代わりに最速クリアを目指します！</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>作画：こめぐ 原作：迅空也</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第3話(3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>魔法少女リリカルなのは EXCEEDS</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>都築真紀 川上修一</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第３話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第６７話『六花停止』①</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>金色の文字使い ―勇者四人に巻き込まれたユニークチート―</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>尾崎祐介(作画) 十本スイ(原作) すまき俊悟(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第117話</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第30話：一秒の奪い合い①</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>冒険者アル あいつの魔法はおかしい@COMIC</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>山﨑と子（漫画） れもん（原作） sime（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第14話 ①</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>千年英雄</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>原作/福島航平 作画/中村ゆきひろ</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>15話</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第3話 前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>マツモトケンゴ</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第５９話　筋トレの戦いが始まった（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>オタクに優しいギャルはいない!?</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>のりしろちゃん魚住さかな</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>【#146】最強ギャルズ結成秘話!?</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>カナン様はあくまでチョロい</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>nonco</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第140話	カナンの文化祭フィナーレ！</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>黒魔法寮の三悪人</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>斎藤キミオ</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第39話 黒魔法寮生のクッキングだよ♪</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>生徒会役員共</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>氏家ト全</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>#403</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>ひげを剃る。そして女子高生を拾う。</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>足立いまる(漫画) しめさば(原作) ぶーた(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第64話その2</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>無能と蔑まれた【勇気ある者】が、実は伝説の【勇者】でした~500年前の仲間＆魔王の娘と一緒に今度こそ世界を救います~</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>作画：シグチサトシ 原作：やすくん</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第3話(3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>俺だけ使える古代魔法 ～基礎すら使えないと追放された俺の魔法は、実は1万年前に失われた伝説魔法でした～</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>原作／アトハ 漫画／川上ニナ キャラクター原案／片倉響</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第1話</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>勇者は魔王が好きらしい</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>赤槻コウ(著者)</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第4話-1：激闘！サキュバス戦！</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>魔王討伐したあと、目立ちたくないのでギルドマスターになった</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>ＲＯＨＧＵＮ(作画) 朱月十話(原作) 鳴瀬ひろふみ(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第65話-①</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>蜘蛛ですが、なにか？</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>かかし朝浩(著者) 馬場翁(原作) 輝竜司(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第75話その2</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
+          <t>王子様の友達</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
+          <t>すけろく(著者)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第10話</t>
+          <t>第28話</t>
         </is>
       </c>
     </row>
@@ -3657,17 +4699,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+          <t>魔のものたちは企てる</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>戸賀 環 坂木持丸 riritto</t>
+          <t>加藤拓弐(原作) ガしガし(作画)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第48話②　お祭りを楽しんでみた</t>
+          <t>第27.5話</t>
         </is>
       </c>
     </row>
@@ -3677,17 +4719,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ライドンキング</t>
+          <t>よくわからないけれど異世界に転生していたようです</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>馬場康誌</t>
+          <t>内々けやき あし カオミン</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第80話 大統領と白の魔導師（後編）</t>
+          <t>第135話 よくわからないけれど導かれてしまったようです（１）</t>
         </is>
       </c>
     </row>
@@ -3697,17 +4739,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+          <t>小林さんちのメイドラゴン</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>村上よしゆき 茨木野 あるてら</t>
+          <t>クール教信者</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第４０話　勇者、聖女と元聖騎士と再会し、魚人を追っ払う（３）</t>
+          <t>外伝 後編</t>
         </is>
       </c>
     </row>
@@ -3717,17 +4759,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>英雄女騎士に有能とバレた俺の美人ハーレム騎士団 ガイカク・ヒクメの奇術騎士団</t>
+          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>明石六郎(原作) 太盛(作画) 氷室しゅんすけ(キャラクター原案)</t>
+          <t>六志麻あさ 業務用餅 kisui</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第9話</t>
+          <t>第６８話</t>
         </is>
       </c>
     </row>
@@ -3737,17 +4779,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ライブダンジョン！</t>
+          <t>くらいあの子としたいこと</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
+          <t>碇マナツ(著者)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第87話後半</t>
+          <t>第79話</t>
         </is>
       </c>
     </row>
@@ -3757,17 +4799,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+          <t>理想のヒモ生活</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>空野進 sorani ファルまろ</t>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>番外編　最弱貴族、寝込む</t>
+          <t>第85話　その3</t>
         </is>
       </c>
     </row>
@@ -3777,17 +4819,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>黄金の経験値</t>
+          <t>経験値貯蓄でのんびり傷心旅行 ～勇者と恋人に追放された戦士の無自覚ざまぁ～</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>原純(原作) 霜月汐(作画) fixro2n(キャラクター原案)</t>
+          <t>奏ヨシキ(著者) 徳川レモン(原作) riritto(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第16話（後編）</t>
+          <t>第36話-2</t>
         </is>
       </c>
     </row>
@@ -3797,17 +4839,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
+          <t>最強勇者パーティーは愛が知りたい</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
+          <t>山田肌襦袢</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第1話③</t>
+          <t>第26話「祭りは踊ったほうがいい」</t>
         </is>
       </c>
     </row>
@@ -3817,17 +4859,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>じつは義妹でした。～最近できた義理の弟の距離感がやたら近いわけ～</t>
+          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>堺しょうきち(著者) 白井ムク(原作) 千種みのり(キャラクター原案)</t>
+          <t>神原絵理華(漫画) 一森一輝(原作)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第35話-2</t>
+          <t>第17話③</t>
         </is>
       </c>
     </row>
@@ -3837,17 +4879,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>私、蜘蛛なモンスターをテイムしたので、スパイダーシルクで裁縫を頑張ります！</t>
+          <t>ゲーセン少女と異文化交流</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>あきさけ(原作) さんねこ(作画) タムラヨウ(キャラクター原案)</t>
+          <t>安原宏和(著者)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第5話</t>
+          <t>125.5話</t>
         </is>
       </c>
     </row>
@@ -3857,17 +4899,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>貧乏騎士に嫁入りしたはずが!? ~野人令嬢は皇太子妃になっても竜を狩りたい~</t>
+          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>漫画：夏川そぞろ 原作：宮前葵 キャラクター原案：ののまろ</t>
+          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第10話②皇太子妃（仮）</t>
+          <t>第73話　大阪LOVER</t>
         </is>
       </c>
     </row>
@@ -3877,17 +4919,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>となりの席のヤツがそういう目で見てくる</t>
+          <t>ベヒモスの花婿</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>mmk</t>
+          <t>鈴音ことら(原作) 月並甲介(漫画)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第39話 聞きたいこと</t>
+          <t>第7話①</t>
         </is>
       </c>
     </row>
@@ -3897,17 +4939,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>【悲報】清楚系で売っていた底辺配信者、うっかり配信を切り忘れたままSS級モンスターを拳で殴り飛ばしてしまう</t>
+          <t>一万倍の聖女が教える聖教育</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>アトハ NEO草野 pupps</t>
+          <t>MIGCHIP(著者)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第４話　【悲報】ご乱行⁉ ダンジョンシーカー・アカデミー！（２）</t>
+          <t>最終話</t>
         </is>
       </c>
     </row>
@@ -3917,17 +4959,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>生徒会にも穴はある！</t>
+          <t>カノジョに浮気されていた俺が、小悪魔な後輩に懐かれています</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>むちまろ</t>
+          <t>香澤陽平(漫画) えーる(キャラクター原案) 御宮ゆう(原作)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第130話	皆で夜遊び（集合編）</t>
+          <t>第31話</t>
         </is>
       </c>
     </row>
@@ -3937,17 +4979,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>規格外のダンジョン攻略者、実は異世界帰りの元勇者</t>
+          <t>推しにささげるダンジョングルメ ～最強探索者VTuberになる～</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>作画：やまざき君 原作：榊与一</t>
+          <t>モノクロウサギ(原作) 藍川蓮(漫画)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第3話(3)</t>
+          <t>CHAPTER　10-2</t>
         </is>
       </c>
     </row>
@@ -3957,17 +4999,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>僕は今すぐ前世の記憶を捨てたい。～憧れの田舎は人外魔境でした～@COMIC</t>
+          <t>顔に出ない柏田さんと顔に出る太田君＋</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>大島つむぎ （漫画） 星畑旭（原作） スズキイオリ （キャラクター原案）</t>
+          <t>東ふゆ(著者)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第18話 ②</t>
+          <t>第29話 愛田さんと宿泊研修</t>
         </is>
       </c>
     </row>
@@ -3977,17 +5019,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ようこそ『追放者ギルド』へ ～無能なＳランクパーティがどんどん有能な冒険者を追放するので、最弱を集めて最強ギルドを創ります～</t>
+          <t>修羅幼女の英雄譚～半端者と言われた傭兵、幼女に転生して成り上がる～</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>荒木佑輔(作画) メソポ・たみあ(原作) U助(キャラクター原案)</t>
+          <t>作画：むらたん 原作：沙城流</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第40話</t>
+          <t>第6話(3)</t>
         </is>
       </c>
     </row>
@@ -3997,17 +5039,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
+          <t>ヤンデレかと思ったらもっとヤベー女だった</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
+          <t>八木戸マト</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第76話その1</t>
+          <t>第65話　どうしても彼氏を家に連れこみたいヤンデレ彼女</t>
         </is>
       </c>
     </row>
@@ -4017,17 +5059,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>誰が勇者を殺したか</t>
+          <t>スキルがなければレベルを上げる～９９がカンストの世界でレベル800万からスタート～</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>石田あきら(漫画) 駄犬(原作) toi8(キャラクター原案)</t>
+          <t>倉橋ユウス(漫画) 岡沢六十四(原作)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第5話</t>
+          <t>第51話①</t>
         </is>
       </c>
     </row>
@@ -4037,17 +5079,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>実は俺、最強でした？</t>
+          <t>なぜかS級美女達の話題に俺があがる件</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>原作：澄守 彩 漫画：高橋 愛</t>
+          <t>ジョN(著者) 脇岡こなつ(原作) magako(キャラクター原案)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第120話　四騎戦決勝戦!!・前編</t>
+          <t>第9話-1</t>
         </is>
       </c>
     </row>
@@ -4057,17 +5099,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ギルド追放された雑用係の下剋上～超万能な生活スキルで世界最強～</t>
+          <t>底辺冒険者だけど魔法を極めてみることにした ～無能スキルから神スキルに進化した【魔法創造】と【アイテム作成】で無双する～</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>原作／夜桜ユノ 漫画／柳輪 ネーム構成／ユーキあきら</t>
+          <t>蒼乃白兎 坂野杏梨 かわく</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第62話</t>
+          <t>第43話(後編) アーティフィカルモンスター</t>
         </is>
       </c>
     </row>
@@ -4077,17 +5119,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ギャルゲーマーに褒められたい</t>
+          <t>ダウナーお姉さんは遊びたい</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>げしゅまろ(著者)</t>
+          <t>山鷹景</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>36話</t>
+          <t>第12話</t>
         </is>
       </c>
     </row>
@@ -4097,17 +5139,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>異世界魔王と召喚少女の奴隷魔術</t>
+          <t>異世界転移したら愛犬が最強になりました～シルバーフェンリルと俺が異世界暮らしを始めたら～</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+          <t>漫画：一花ハナ 原作：龍央 キャラクター原案：りりんら</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第126話　戦争を終わらせてみるⅡ（前編）</t>
+          <t>第36話前半</t>
         </is>
       </c>
     </row>
@@ -4117,17 +5159,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ルパン三世 異世界の姫君（ネイバーワールドプリンセス）</t>
+          <t>パワハラギルマスをぶん殴ってブラック聖剣ギルドをクビになったので、辺境で聖剣工房を開くことにした</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>モンキー・パンチ／エム・ピー・ワークス 内々けやき 佐伯庸介 白狼</t>
+          <t>だいたいねむい(原作) まお(漫画)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第99話：泥棒、心を盗めど縛りはせず❷</t>
+          <t>第9話③</t>
         </is>
       </c>
     </row>
@@ -4137,17 +5179,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>自分の事を主人公だと信じてやまない踏み台が、主人公を踏み台だと勘違いして、優勝してしまうお話です@COMIC</t>
+          <t>つぐもも</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>KYO=H（漫画） 流石ユユシタ（原作） 卵の黄身（キャラクター原案）</t>
+          <t>浜田よしかづ</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第4話</t>
+          <t>第172話</t>
         </is>
       </c>
     </row>
@@ -4157,17 +5199,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>直径3cmの召喚陣&lt;リミットリング&gt;で「雑魚すら呼べない」と蔑まれた底辺召喚士が頂点に立つまで</t>
+          <t>傭兵団の愛し子 ～死にかけ孤児は最強師匠たちに育てられる～</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>作画：まっつー 原作：空松蓮司</t>
+          <t>柿野レイ(漫画) 天野雪人(原作) 黒井ススム(キャラクター原案)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第3話(3)</t>
+          <t>第6話前編：召喚士ウィル</t>
         </is>
       </c>
     </row>
@@ -4177,17 +5219,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>聖者無双</t>
+          <t>クラスメイトは異世界で勇者になったけど、俺だけ現代日本に置き去りにされました</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
+          <t>カボチャマスク(原作) 仲紙(漫画)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第90話　研究者や技術者の故郷（前半）</t>
+          <t>第9話-3</t>
         </is>
       </c>
     </row>
@@ -4197,17 +5239,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+          <t>限界超えの天賦は、転生者にしか扱えない ― オーバーリミット・スキルホルダー ―</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+          <t>長月みそか(漫画) 三上康明(原作) 大槍葦人(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第31話 独身貴族はヒラメが大事（3）</t>
+          <t>第3章［13］前半</t>
         </is>
       </c>
     </row>
@@ -4217,17 +5259,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>FPSゲームのコーチを引き受けたら依頼主が人気VTuberの美少女だった</t>
+          <t>勇者パーティから追い出された不遇職【罠士】、ユニークスキル【矢印】で最強になる</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>漫画：真広吏希 原作：すかいふぁーむ キャラクター原案：みすみ</t>
+          <t>作画：たつひこ 原作：白石 有希</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>単行本1巻発売告知</t>
+          <t>第6話(3)</t>
         </is>
       </c>
     </row>
@@ -4237,17 +5279,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>君の刀が折れるまで ~月宮まつりの恋難き~</t>
+          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>イノウエ</t>
+          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第37話 日永のこと</t>
+          <t>第10話</t>
         </is>
       </c>
     </row>
@@ -4257,17 +5299,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ゲーム内最強の『裏ボス』に転生したので、主人公の代わりに最速クリアを目指します！</t>
+          <t>レベル1で挑む縛りプレイ!</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>作画：こめぐ 原作：迅空也</t>
+          <t>北川ニキタ 大鐘いしや 刀 彼方</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第3話(3)</t>
+          <t>第20話 尋問②</t>
         </is>
       </c>
     </row>
@@ -4277,17 +5319,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>魔法少女リリカルなのは EXCEEDS</t>
+          <t>やっぱ人間やめて正解だわ</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>都築真紀 川上修一</t>
+          <t>偽BEなんとか</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第３話②</t>
+          <t>第14話（後編）とりあえず超をつける所から進化を始める</t>
         </is>
       </c>
     </row>
@@ -4297,17 +5339,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>光永康則</t>
+          <t>戸賀 環 坂木持丸 riritto</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第６７話『六花停止』①</t>
+          <t>第48話②　お祭りを楽しんでみた</t>
         </is>
       </c>
     </row>
@@ -4317,17 +5359,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>金色の文字使い ―勇者四人に巻き込まれたユニークチート―</t>
+          <t>おねえさんと猫を飼う</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>尾崎祐介(作画) 十本スイ(原作) すまき俊悟(キャラクター原案)</t>
+          <t>上杉響士郎(著者)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第117話</t>
+          <t>第1話：おねえさんと猫を拾う</t>
         </is>
       </c>
     </row>
@@ -4337,17 +5379,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+          <t>瞳ちゃんは人見知り</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>zunta(作画) はらわたさいぞう(原作)</t>
+          <t>夏海ちょりすけ</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第30話：一秒の奪い合い①</t>
+          <t>第135話</t>
         </is>
       </c>
     </row>
@@ -4357,17 +5399,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>冒険者アル あいつの魔法はおかしい@COMIC</t>
+          <t>ブレイド＆バスタード</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>山﨑と子（漫画） れもん（原作） sime（キャラクター原案）</t>
+          <t>漫画/楓月 誠 原作/蝸牛くも キャラクター原案/so-bin</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第14話 ①</t>
+          <t>第10話（1）</t>
         </is>
       </c>
     </row>
@@ -4377,17 +5419,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>千年英雄</t>
+          <t>カバンの勇者の異世界のんびり旅 ～実は「カバン」は何でも吸収できるし、日本から何でも取り寄せができるチート武器でした～</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>原作/福島航平 作画/中村ゆきひろ</t>
+          <t>きしだしき(漫画) 茨木野(原作) キャラクターデザイン(いずみけい)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>15話</t>
+          <t>第4話</t>
         </is>
       </c>
     </row>
@@ -4397,17 +5439,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+          <t>神々に育てられしもの、最強となる</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+          <t>九野十弥(漫画) 羽田遼亮(原作) fame(キャラクター原案)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第3話 前編</t>
+          <t>第56話</t>
         </is>
       </c>
     </row>
@@ -4417,17 +5459,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+          <t>やめてくれ、強いのは俺じゃなくて剣なんだ……！</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>マツモトケンゴ</t>
+          <t>漫画/廃狼 原作/馬路まんじ キャラクター原案/かぼちゃ</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第５９話　筋トレの戦いが始まった（２）</t>
+          <t>第7話（2）</t>
         </is>
       </c>
     </row>
@@ -4437,17 +5479,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>オタクに優しいギャルはいない!?</t>
+          <t>錬金術師の辺境再生スローライフ～S級パーティーで孤立した少女をかばったら追放されたので、一緒に幸せに暮らします～</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>のりしろちゃん魚住さかな</t>
+          <t>作画：弥永扇 原作：三月菫</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>【#146】最強ギャルズ結成秘話!?</t>
+          <t>第6話(3)</t>
         </is>
       </c>
     </row>
@@ -4457,17 +5499,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>カナン様はあくまでチョロい</t>
+          <t>英雄女騎士に有能とバレた俺の美人ハーレム騎士団 ガイカク・ヒクメの奇術騎士団</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>nonco</t>
+          <t>明石六郎(原作) 太盛(作画) 氷室しゅんすけ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第140話	カナンの文化祭フィナーレ！</t>
+          <t>第9話</t>
         </is>
       </c>
     </row>
@@ -4477,17 +5519,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>黒魔法寮の三悪人</t>
+          <t>ギルドを追放された回復術士、実は魔力無限だったので規格外の回復魔法で伝説となる</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>斎藤キミオ</t>
+          <t>漫画：坂下コウ 原作：霞杏檎</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第39話 黒魔法寮生のクッキングだよ♪</t>
+          <t>第3話(2)</t>
         </is>
       </c>
     </row>
@@ -4497,17 +5539,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>生徒会役員共</t>
+          <t>転生社畜のチート菜園　～万能スキルと便利な使い魔妖精を駆使してたら、気づけば大陸一の生産拠点ができていた～</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>氏家ト全</t>
+          <t>桃花台とぅる(著者) 可換環(原作) riritto(キャラクター原案)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>#403</t>
+          <t>第21話前半「砂糖革命前夜」</t>
         </is>
       </c>
     </row>
@@ -4517,17 +5559,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ひげを剃る。そして女子高生を拾う。</t>
+          <t>ライドンキング</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>足立いまる(漫画) しめさば(原作) ぶーた(キャラクター原案)</t>
+          <t>馬場康誌</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第64話その2</t>
+          <t>第80話 大統領と白の魔導師（後編）</t>
         </is>
       </c>
     </row>
@@ -4537,17 +5579,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>無能と蔑まれた【勇気ある者】が、実は伝説の【勇者】でした~500年前の仲間＆魔王の娘と一緒に今度こそ世界を救います~</t>
+          <t>母をたずねて、異世界に。</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>作画：シグチサトシ 原作：やすくん</t>
+          <t>藤原 祐(原作) 吉北ぽぷり(漫画) しの(キャラクター原案)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第3話(3)</t>
+          <t>第10話-2</t>
         </is>
       </c>
     </row>
@@ -4557,17 +5599,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>俺だけ使える古代魔法 ～基礎すら使えないと追放された俺の魔法は、実は1万年前に失われた伝説魔法でした～</t>
+          <t>隠居暮らしのおっさん、女王陛下の剣となる</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>原作／アトハ 漫画／川上ニナ キャラクター原案／片倉響</t>
+          <t>漫画/半二合 原作/天酒之瓢 キャラクター原案/みことあけみ</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第1話</t>
+          <t>第5話（1）</t>
         </is>
       </c>
     </row>
@@ -4577,17 +5619,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>勇者は魔王が好きらしい</t>
+          <t>影の英雄の日常譚 勇者の裏で暗躍していた最強のエージェント。組織が解体されたので、正体隠して人並みの日常を謳歌する。</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>赤槻コウ(著者)</t>
+          <t>kanco(漫画) 坂石遊作(原作) TYONE(キャラクター原案)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第4話-1：激闘！サキュバス戦！</t>
+          <t>Episode32-2</t>
         </is>
       </c>
     </row>
@@ -4597,17 +5639,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>魔王討伐したあと、目立ちたくないのでギルドマスターになった</t>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>ＲＯＨＧＵＮ(作画) 朱月十話(原作) 鳴瀬ひろふみ(キャラクターデザイン)</t>
+          <t>村上よしゆき 茨木野 あるてら</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第65話-①</t>
+          <t>第４０話　勇者、聖女と元聖騎士と再会し、魚人を追っ払う（３）</t>
         </is>
       </c>
     </row>
@@ -4617,17 +5659,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>蜘蛛ですが、なにか？</t>
+          <t>追放されたおっさんタンク、実は防御力最強だったのでダメージゼロで無双する</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>かかし朝浩(著者) 馬場翁(原作) 輝竜司(キャラクター原案)</t>
+          <t>漫画：化野九十九 原作：あけちともあき</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第75話その2</t>
+          <t>第3話(2)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-07-06
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -20,6 +20,7 @@
     <sheet name="2025-07-03" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="2025-07-04" sheetId="13" state="visible" r:id="rId13"/>
     <sheet name="2025-07-05" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="2025-07-06" sheetId="15" state="visible" r:id="rId15"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -4674,22 +4675,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>王子様の友達</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>すけろく(著者)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第28話</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>魔のものたちは企てる</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>加藤拓弐(原作) ガしガし(作画)</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第27.5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第135話 よくわからないけれど導かれてしまったようです（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>小林さんちのメイドラゴン</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>クール教信者</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>外伝 後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>六志麻あさ 業務用餅 kisui</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第６８話</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>くらいあの子としたいこと</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>碇マナツ(著者)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第79話</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>理想のヒモ生活</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第85話　その3</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>経験値貯蓄でのんびり傷心旅行 ～勇者と恋人に追放された戦士の無自覚ざまぁ～</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>奏ヨシキ(著者) 徳川レモン(原作) riritto(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第36話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>最強勇者パーティーは愛が知りたい</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>山田肌襦袢</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第26話「祭りは踊ったほうがいい」</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>神原絵理華(漫画) 一森一輝(原作)</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第17話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>ゲーセン少女と異文化交流</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>安原宏和(著者)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>125.5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第73話　大阪LOVER</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>ベヒモスの花婿</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>鈴音ことら(原作) 月並甲介(漫画)</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第7話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>一万倍の聖女が教える聖教育</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>MIGCHIP(著者)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>最終話</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>カノジョに浮気されていた俺が、小悪魔な後輩に懐かれています</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>香澤陽平(漫画) えーる(キャラクター原案) 御宮ゆう(原作)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第31話</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>推しにささげるダンジョングルメ ～最強探索者VTuberになる～</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>モノクロウサギ(原作) 藍川蓮(漫画)</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>CHAPTER　10-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>顔に出ない柏田さんと顔に出る太田君＋</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>東ふゆ(著者)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第29話 愛田さんと宿泊研修</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>修羅幼女の英雄譚～半端者と言われた傭兵、幼女に転生して成り上がる～</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>作画：むらたん 原作：沙城流</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第6話(3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>ヤンデレかと思ったらもっとヤベー女だった</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>八木戸マト</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第65話　どうしても彼氏を家に連れこみたいヤンデレ彼女</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>スキルがなければレベルを上げる～９９がカンストの世界でレベル800万からスタート～</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>倉橋ユウス(漫画) 岡沢六十四(原作)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第51話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>なぜかS級美女達の話題に俺があがる件</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>ジョN(著者) 脇岡こなつ(原作) magako(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第9話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>底辺冒険者だけど魔法を極めてみることにした ～無能スキルから神スキルに進化した【魔法創造】と【アイテム作成】で無双する～</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>蒼乃白兎 坂野杏梨 かわく</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第43話(後編) アーティフィカルモンスター</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>ダウナーお姉さんは遊びたい</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>山鷹景</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第12話</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>異世界転移したら愛犬が最強になりました～シルバーフェンリルと俺が異世界暮らしを始めたら～</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>漫画：一花ハナ 原作：龍央 キャラクター原案：りりんら</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第36話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>パワハラギルマスをぶん殴ってブラック聖剣ギルドをクビになったので、辺境で聖剣工房を開くことにした</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>だいたいねむい(原作) まお(漫画)</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第9話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>つぐもも</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>浜田よしかづ</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第172話</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>傭兵団の愛し子 ～死にかけ孤児は最強師匠たちに育てられる～</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>柿野レイ(漫画) 天野雪人(原作) 黒井ススム(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第6話前編：召喚士ウィル</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>クラスメイトは異世界で勇者になったけど、俺だけ現代日本に置き去りにされました</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>カボチャマスク(原作) 仲紙(漫画)</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第9話-3</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>限界超えの天賦は、転生者にしか扱えない ― オーバーリミット・スキルホルダー ―</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>長月みそか(漫画) 三上康明(原作) 大槍葦人(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第3章［13］前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティから追い出された不遇職【罠士】、ユニークスキル【矢印】で最強になる</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>作画：たつひこ 原作：白石 有希</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第6話(3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第10話</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>レベル1で挑む縛りプレイ!</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>北川ニキタ 大鐘いしや 刀 彼方</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第20話 尋問②</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>やっぱ人間やめて正解だわ</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>偽BEなんとか</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第14話（後編）とりあえず超をつける所から進化を始める</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>戸賀 環 坂木持丸 riritto</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第48話②　お祭りを楽しんでみた</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>おねえさんと猫を飼う</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>上杉響士郎(著者)</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第1話：おねえさんと猫を拾う</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>瞳ちゃんは人見知り</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>夏海ちょりすけ</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第135話</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>ブレイド＆バスタード</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>漫画/楓月 誠 原作/蝸牛くも キャラクター原案/so-bin</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第10話（1）</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>カバンの勇者の異世界のんびり旅 ～実は「カバン」は何でも吸収できるし、日本から何でも取り寄せができるチート武器でした～</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>きしだしき(漫画) 茨木野(原作) キャラクターデザイン(いずみけい)</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第4話</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>神々に育てられしもの、最強となる</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>九野十弥(漫画) 羽田遼亮(原作) fame(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第56話</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>やめてくれ、強いのは俺じゃなくて剣なんだ……！</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>漫画/廃狼 原作/馬路まんじ キャラクター原案/かぼちゃ</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第7話（2）</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>錬金術師の辺境再生スローライフ～S級パーティーで孤立した少女をかばったら追放されたので、一緒に幸せに暮らします～</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>作画：弥永扇 原作：三月菫</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第6話(3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>英雄女騎士に有能とバレた俺の美人ハーレム騎士団 ガイカク・ヒクメの奇術騎士団</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>明石六郎(原作) 太盛(作画) 氷室しゅんすけ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第9話</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>ギルドを追放された回復術士、実は魔力無限だったので規格外の回復魔法で伝説となる</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>漫画：坂下コウ 原作：霞杏檎</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第3話(2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>転生社畜のチート菜園　～万能スキルと便利な使い魔妖精を駆使してたら、気づけば大陸一の生産拠点ができていた～</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>桃花台とぅる(著者) 可換環(原作) riritto(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第21話前半「砂糖革命前夜」</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>ライドンキング</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>馬場康誌</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第80話 大統領と白の魔導師（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>母をたずねて、異世界に。</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>藤原 祐(原作) 吉北ぽぷり(漫画) しの(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第10話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>隠居暮らしのおっさん、女王陛下の剣となる</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>漫画/半二合 原作/天酒之瓢 キャラクター原案/みことあけみ</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第5話（1）</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>影の英雄の日常譚 勇者の裏で暗躍していた最強のエージェント。組織が解体されたので、正体隠して人並みの日常を謳歌する。</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>kanco(漫画) 坂石遊作(原作) TYONE(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>Episode32-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>村上よしゆき 茨木野 あるてら</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第４０話　勇者、聖女と元聖騎士と再会し、魚人を追っ払う（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>追放されたおっさんタンク、実は防御力最強だったのでダメージゼロで無双する</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>漫画：化野九十九 原作：あけちともあき</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第3話(2)</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>王子様の友達</t>
+          <t>いとこのこ</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>すけろく(著者)</t>
+          <t>いぬちく(著者)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第28話</t>
+          <t>第35.5話</t>
         </is>
       </c>
     </row>
@@ -4699,17 +5741,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>魔のものたちは企てる</t>
+          <t>ぽんドロイド！ はまさん</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>加藤拓弐(原作) ガしガし(作画)</t>
+          <t>はれやまはれぞう(著者)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第27.5話</t>
+          <t>第3話</t>
         </is>
       </c>
     </row>
@@ -4719,17 +5761,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>よくわからないけれど異世界に転生していたようです</t>
+          <t>このヒーラー、めんどくさい</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>内々けやき あし カオミン</t>
+          <t>丹念に発酵(著者)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第135話 よくわからないけれど導かれてしまったようです（１）</t>
+          <t>第88話：ゴブリンの罠</t>
         </is>
       </c>
     </row>
@@ -4739,17 +5781,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>小林さんちのメイドラゴン</t>
+          <t>リビルドワールド</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>クール教信者</t>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>外伝 後編</t>
+          <t>第70話④</t>
         </is>
       </c>
     </row>
@@ -4759,17 +5801,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
+          <t>リアデイルの大地にて</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>六志麻あさ 業務用餅 kisui</t>
+          <t>月見だしお(著者) Ceez(原作) てんまそ(キャラクター原案) 涼風涼(構成)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第６８話</t>
+          <t>第39章-2</t>
         </is>
       </c>
     </row>
@@ -4779,17 +5821,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>くらいあの子としたいこと</t>
+          <t>アイドル辞めるけど結婚してくれますか!?</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>碇マナツ(著者)</t>
+          <t>三吉汐美(著者)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第79話</t>
+          <t>第16話前半</t>
         </is>
       </c>
     </row>
@@ -4799,17 +5841,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>理想のヒモ生活</t>
+          <t>まったく最近の探偵ときたら</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+          <t>五十嵐正邦(著者)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第85話　その3</t>
+          <t>第113話</t>
         </is>
       </c>
     </row>
@@ -4819,17 +5861,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>経験値貯蓄でのんびり傷心旅行 ～勇者と恋人に追放された戦士の無自覚ざまぁ～</t>
+          <t>氷結令嬢さまをフォローしたら、メチャメチャ溺愛されてしまった件@comic</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>奏ヨシキ(著者) 徳川レモン(原作) riritto(キャラクターデザイン)</t>
+          <t>漫画：ハレノチアメ 原作：愛坂タカト キャラクター原案：Bcoca</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第36話-2</t>
+          <t>1話扉イラスト案大公開！</t>
         </is>
       </c>
     </row>
@@ -4839,17 +5881,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>最強勇者パーティーは愛が知りたい</t>
+          <t>三枝さんはメガネ先輩と恋を描く</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>山田肌襦袢</t>
+          <t>セレビィ量産型(著者)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第26話「祭りは踊ったほうがいい」</t>
+          <t>特別編</t>
         </is>
       </c>
     </row>
@@ -4859,17 +5901,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
+          <t>ダメ人間の愛しかた</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>神原絵理華(漫画) 一森一輝(原作)</t>
+          <t>岩葉(著者)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第17話③</t>
+          <t>第18話前編　ダメ人間とお姉ちゃんと彼女</t>
         </is>
       </c>
     </row>
@@ -4879,17 +5921,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ゲーセン少女と異文化交流</t>
+          <t>モテはるねえ蘆屋くん</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>安原宏和(著者)</t>
+          <t>栗原和明(原作) 寺井赤音(作画)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>125.5話</t>
+          <t>第15話後半</t>
         </is>
       </c>
     </row>
@@ -4899,17 +5941,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
+          <t>理想の彼女</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
+          <t>もりまりも(著者)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第73話　大阪LOVER</t>
+          <t>第22話</t>
         </is>
       </c>
     </row>
@@ -4919,17 +5961,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ベヒモスの花婿</t>
+          <t>王子様の友達</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>鈴音ことら(原作) 月並甲介(漫画)</t>
+          <t>すけろく(著者)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第7話①</t>
+          <t>第28話</t>
         </is>
       </c>
     </row>
@@ -4939,17 +5981,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>一万倍の聖女が教える聖教育</t>
+          <t>魔都精兵のスレイブ</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>MIGCHIP(著者)</t>
+          <t>原作:タカヒロ　漫画:竹村洋平</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>最終話</t>
+          <t>第156話　神隠し</t>
         </is>
       </c>
     </row>
@@ -4959,17 +6001,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>カノジョに浮気されていた俺が、小悪魔な後輩に懐かれています</t>
+          <t>無敵商人の異世界成り上がり物語 ～現代の製品を自在に取り寄せるスキルがあるので異世界では楽勝です～</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>香澤陽平(漫画) えーる(キャラクター原案) 御宮ゆう(原作)</t>
+          <t>隆原ヒロタ(漫画) 青山有(原作) ぷきゅのすけ(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第31話</t>
+          <t>第34話④</t>
         </is>
       </c>
     </row>
@@ -4979,17 +6021,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>推しにささげるダンジョングルメ ～最強探索者VTuberになる～</t>
+          <t>転生してあらゆるモノに好かれながら異世界で好きな事をして生きて行く</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>モノクロウサギ(原作) 藍川蓮(漫画)</t>
+          <t>都尾琉(漫画) 御峰。(原作)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>CHAPTER　10-2</t>
+          <t>第26話①</t>
         </is>
       </c>
     </row>
@@ -4999,17 +6041,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>顔に出ない柏田さんと顔に出る太田君＋</t>
+          <t>王立魔術学院の鬼畜講師</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>東ふゆ(著者)</t>
+          <t>実々みみず(漫画) 急川回レ(原作) zunta(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第29話 愛田さんと宿泊研修</t>
+          <t>第19話二</t>
         </is>
       </c>
     </row>
@@ -5019,17 +6061,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>修羅幼女の英雄譚～半端者と言われた傭兵、幼女に転生して成り上がる～</t>
+          <t>アラサーがVTuberになった話。</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>作画：むらたん 原作：沙城流</t>
+          <t>犬威赤彦(漫画) とくめい(原作) カラスBTK(キャラクター原案)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第6話(3)</t>
+          <t>第22話</t>
         </is>
       </c>
     </row>
@@ -5039,17 +6081,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ヤンデレかと思ったらもっとヤベー女だった</t>
+          <t>オトナを知りたい女友達</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>八木戸マト</t>
+          <t>望公太(原作) ぷよちゃ(作画)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第65話　どうしても彼氏を家に連れこみたいヤンデレ彼女</t>
+          <t>コミックス告知</t>
         </is>
       </c>
     </row>
@@ -5059,17 +6101,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>スキルがなければレベルを上げる～９９がカンストの世界でレベル800万からスタート～</t>
+          <t>俺堕ちスレイブヒーローコレクション</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>倉橋ユウス(漫画) 岡沢六十四(原作)</t>
+          <t>ゆっ栗栖(著者)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第51話①</t>
+          <t>第10話後半</t>
         </is>
       </c>
     </row>
@@ -5079,17 +6121,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>なぜかS級美女達の話題に俺があがる件</t>
+          <t>チュートリアルが始まる前に ボスキャラ達を破滅させない為に俺ができる幾つかの事</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>ジョN(著者) 脇岡こなつ(原作) magako(キャラクター原案)</t>
+          <t>横山コウヂ(漫画) 髙橋炬燵(原作) カカオ・ランタン(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第9話-1</t>
+          <t>第13話①</t>
         </is>
       </c>
     </row>
@@ -5099,17 +6141,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>底辺冒険者だけど魔法を極めてみることにした ～無能スキルから神スキルに進化した【魔法創造】と【アイテム作成】で無双する～</t>
+          <t>愚かな天使は悪魔と踊る</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>蒼乃白兎 坂野杏梨 かわく</t>
+          <t>アズマサワヨシ(著者)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第43話(後編) アーティフィカルモンスター</t>
+          <t>第99話④</t>
         </is>
       </c>
     </row>
@@ -5119,17 +6161,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ダウナーお姉さんは遊びたい</t>
+          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>山鷹景</t>
+          <t>六志麻あさ 業務用餅 kisui</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第12話</t>
+          <t>第６８話</t>
         </is>
       </c>
     </row>
@@ -5139,17 +6181,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>異世界転移したら愛犬が最強になりました～シルバーフェンリルと俺が異世界暮らしを始めたら～</t>
+          <t>ハーレムより平穏を！異世界で静かにニート姫させてくれ</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>漫画：一花ハナ 原作：龍央 キャラクター原案：りりんら</t>
+          <t>さかたはるき(原作) かわやばぐ(作画)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第36話前半</t>
+          <t>第13話前半</t>
         </is>
       </c>
     </row>
@@ -5159,17 +6201,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>パワハラギルマスをぶん殴ってブラック聖剣ギルドをクビになったので、辺境で聖剣工房を開くことにした</t>
+          <t>魔のものたちは企てる</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>だいたいねむい(原作) まお(漫画)</t>
+          <t>加藤拓弐(原作) ガしガし(作画)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第9話③</t>
+          <t>第27.5話</t>
         </is>
       </c>
     </row>
@@ -5179,17 +6221,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>つぐもも</t>
+          <t>ギャルゲーマーに褒められたい</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>浜田よしかづ</t>
+          <t>げしゅまろ(著者)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第172話</t>
+          <t>38話</t>
         </is>
       </c>
     </row>
@@ -5199,17 +6241,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>傭兵団の愛し子 ～死にかけ孤児は最強師匠たちに育てられる～</t>
+          <t>よくわからないけれど異世界に転生していたようです</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>柿野レイ(漫画) 天野雪人(原作) 黒井ススム(キャラクター原案)</t>
+          <t>内々けやき あし カオミン</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第6話前編：召喚士ウィル</t>
+          <t>第135話 よくわからないけれど導かれてしまったようです（１）</t>
         </is>
       </c>
     </row>
@@ -5219,17 +6261,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>クラスメイトは異世界で勇者になったけど、俺だけ現代日本に置き去りにされました</t>
+          <t>きみの願いが叶うまで</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>カボチャマスク(原作) 仲紙(漫画)</t>
+          <t>浅月のりと(著者)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第9話-3</t>
+          <t>第3話-1</t>
         </is>
       </c>
     </row>
@@ -5239,17 +6281,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>限界超えの天賦は、転生者にしか扱えない ― オーバーリミット・スキルホルダー ―</t>
+          <t>豚のレバーは加熱しろ</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>長月みそか(漫画) 三上康明(原作) 大槍葦人(キャラクターデザイン)</t>
+          <t>みなみ(漫画) 逆井卓馬(原作) 遠坂あさぎ(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第3章［13］前半</t>
+          <t>第41話②</t>
         </is>
       </c>
     </row>
@@ -5259,17 +6301,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>勇者パーティから追い出された不遇職【罠士】、ユニークスキル【矢印】で最強になる</t>
+          <t>小林さんちのメイドラゴン</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>作画：たつひこ 原作：白石 有希</t>
+          <t>クール教信者</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第6話(3)</t>
+          <t>外伝 後編</t>
         </is>
       </c>
     </row>
@@ -5279,17 +6321,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
+          <t>おねえさんと猫を飼う</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
+          <t>上杉響士郎(著者)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第10話</t>
+          <t>第1話：おねえさんと猫を拾う</t>
         </is>
       </c>
     </row>
@@ -5299,17 +6341,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>レベル1で挑む縛りプレイ!</t>
+          <t>くらいあの子としたいこと</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>北川ニキタ 大鐘いしや 刀 彼方</t>
+          <t>碇マナツ(著者)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第20話 尋問②</t>
+          <t>第79話</t>
         </is>
       </c>
     </row>
@@ -5319,17 +6361,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>やっぱ人間やめて正解だわ</t>
+          <t>経験値貯蓄でのんびり傷心旅行 ～勇者と恋人に追放された戦士の無自覚ざまぁ～</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>偽BEなんとか</t>
+          <t>奏ヨシキ(著者) 徳川レモン(原作) riritto(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第14話（後編）とりあえず超をつける所から進化を始める</t>
+          <t>第36話-2</t>
         </is>
       </c>
     </row>
@@ -5339,17 +6381,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+          <t>理想のヒモ生活</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>戸賀 環 坂木持丸 riritto</t>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第48話②　お祭りを楽しんでみた</t>
+          <t>第85話　その3</t>
         </is>
       </c>
     </row>
@@ -5359,17 +6401,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>おねえさんと猫を飼う</t>
+          <t>おっさん、転生して天才役者になる</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>上杉響士郎(著者)</t>
+          <t>芽々ノ圭(漫画) ほえ太郎(原作)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第1話：おねえさんと猫を拾う</t>
+          <t>第36.5話</t>
         </is>
       </c>
     </row>
@@ -5379,17 +6421,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>瞳ちゃんは人見知り</t>
+          <t>最強勇者パーティーは愛が知りたい</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>夏海ちょりすけ</t>
+          <t>山田肌襦袢</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第135話</t>
+          <t>第26話「祭りは踊ったほうがいい」</t>
         </is>
       </c>
     </row>
@@ -5399,17 +6441,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ブレイド＆バスタード</t>
+          <t>怪異部～M県Y市の怪現象について～</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>漫画/楓月 誠 原作/蝸牛くも キャラクター原案/so-bin</t>
+          <t>さりい・Ｂ(著者)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第10話（1）</t>
+          <t>File.5</t>
         </is>
       </c>
     </row>
@@ -5419,17 +6461,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>カバンの勇者の異世界のんびり旅 ～実は「カバン」は何でも吸収できるし、日本から何でも取り寄せができるチート武器でした～</t>
+          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>きしだしき(漫画) 茨木野(原作) キャラクターデザイン(いずみけい)</t>
+          <t>神原絵理華(漫画) 一森一輝(原作)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第4話</t>
+          <t>第17話③</t>
         </is>
       </c>
     </row>
@@ -5439,17 +6481,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>神々に育てられしもの、最強となる</t>
+          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>九野十弥(漫画) 羽田遼亮(原作) fame(キャラクター原案)</t>
+          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第56話</t>
+          <t>第73話　大阪LOVER</t>
         </is>
       </c>
     </row>
@@ -5459,17 +6501,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>やめてくれ、強いのは俺じゃなくて剣なんだ……！</t>
+          <t>終末ツーリング</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>漫画/廃狼 原作/馬路まんじ キャラクター原案/かぼちゃ</t>
+          <t>さいとー栄(著者)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第7話（2）</t>
+          <t>第48話 三沢基地　その４①</t>
         </is>
       </c>
     </row>
@@ -5479,17 +6521,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>錬金術師の辺境再生スローライフ～S級パーティーで孤立した少女をかばったら追放されたので、一緒に幸せに暮らします～</t>
+          <t>千年英雄</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>作画：弥永扇 原作：三月菫</t>
+          <t>原作/福島航平 作画/中村ゆきひろ</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第6話(3)</t>
+          <t>16話②</t>
         </is>
       </c>
     </row>
@@ -5499,17 +6541,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>英雄女騎士に有能とバレた俺の美人ハーレム騎士団 ガイカク・ヒクメの奇術騎士団</t>
+          <t>カノジョに浮気されていた俺が、小悪魔な後輩に懐かれています</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>明石六郎(原作) 太盛(作画) 氷室しゅんすけ(キャラクター原案)</t>
+          <t>香澤陽平(漫画) えーる(キャラクター原案) 御宮ゆう(原作)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第9話</t>
+          <t>第31話</t>
         </is>
       </c>
     </row>
@@ -5519,17 +6561,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>ギルドを追放された回復術士、実は魔力無限だったので規格外の回復魔法で伝説となる</t>
+          <t>ゲーセン少女と異文化交流</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>漫画：坂下コウ 原作：霞杏檎</t>
+          <t>安原宏和(著者)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第3話(2)</t>
+          <t>125.5話</t>
         </is>
       </c>
     </row>
@@ -5539,17 +6581,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>転生社畜のチート菜園　～万能スキルと便利な使い魔妖精を駆使してたら、気づけば大陸一の生産拠点ができていた～</t>
+          <t>一万倍の聖女が教える聖教育</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>桃花台とぅる(著者) 可換環(原作) riritto(キャラクター原案)</t>
+          <t>MIGCHIP(著者)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第21話前半「砂糖革命前夜」</t>
+          <t>最終話</t>
         </is>
       </c>
     </row>
@@ -5559,17 +6601,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ライドンキング</t>
+          <t>ベヒモスの花婿</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>馬場康誌</t>
+          <t>鈴音ことら(原作) 月並甲介(漫画)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第80話 大統領と白の魔導師（後編）</t>
+          <t>第7話①</t>
         </is>
       </c>
     </row>
@@ -5579,17 +6621,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>母をたずねて、異世界に。</t>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>藤原 祐(原作) 吉北ぽぷり(漫画) しの(キャラクター原案)</t>
+          <t>戸賀 環 坂木持丸 riritto</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第10話-2</t>
+          <t>第48話②　お祭りを楽しんでみた</t>
         </is>
       </c>
     </row>
@@ -5599,17 +6641,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>隠居暮らしのおっさん、女王陛下の剣となる</t>
+          <t>底辺冒険者だけど魔法を極めてみることにした ～無能スキルから神スキルに進化した【魔法創造】と【アイテム作成】で無双する～</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>漫画/半二合 原作/天酒之瓢 キャラクター原案/みことあけみ</t>
+          <t>蒼乃白兎 坂野杏梨 かわく</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第5話（1）</t>
+          <t>第43話(後編) アーティフィカルモンスター</t>
         </is>
       </c>
     </row>
@@ -5619,17 +6661,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>影の英雄の日常譚 勇者の裏で暗躍していた最強のエージェント。組織が解体されたので、正体隠して人並みの日常を謳歌する。</t>
+          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>kanco(漫画) 坂石遊作(原作) TYONE(キャラクター原案)</t>
+          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Episode32-2</t>
+          <t>第10話</t>
         </is>
       </c>
     </row>
@@ -5639,17 +6681,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+          <t>顔に出ない柏田さんと顔に出る太田君＋</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>村上よしゆき 茨木野 あるてら</t>
+          <t>東ふゆ(著者)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第４０話　勇者、聖女と元聖騎士と再会し、魚人を追っ払う（３）</t>
+          <t>第29話 愛田さんと宿泊研修</t>
         </is>
       </c>
     </row>
@@ -5659,17 +6701,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>追放されたおっさんタンク、実は防御力最強だったのでダメージゼロで無双する</t>
+          <t>ダウナーお姉さんは遊びたい</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>漫画：化野九十九 原作：あけちともあき</t>
+          <t>山鷹景</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第3話(2)</t>
+          <t>第12話</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-07-07
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -21,6 +21,7 @@
     <sheet name="2025-07-04" sheetId="13" state="visible" r:id="rId13"/>
     <sheet name="2025-07-05" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="2025-07-06" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="2025-07-07" sheetId="16" state="visible" r:id="rId16"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -5716,22 +5717,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>いとこのこ</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>いぬちく(著者)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第35.5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>ぽんドロイド！ はまさん</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>はれやまはれぞう(著者)</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第3話</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>このヒーラー、めんどくさい</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>丹念に発酵(著者)</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第88話：ゴブリンの罠</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第70話④</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>リアデイルの大地にて</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>月見だしお(著者) Ceez(原作) てんまそ(キャラクター原案) 涼風涼(構成)</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第39章-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>アイドル辞めるけど結婚してくれますか!?</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>三吉汐美(著者)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第16話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>まったく最近の探偵ときたら</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>五十嵐正邦(著者)</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第113話</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>氷結令嬢さまをフォローしたら、メチャメチャ溺愛されてしまった件@comic</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>漫画：ハレノチアメ 原作：愛坂タカト キャラクター原案：Bcoca</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>1話扉イラスト案大公開！</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>三枝さんはメガネ先輩と恋を描く</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>セレビィ量産型(著者)</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>特別編</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>ダメ人間の愛しかた</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>岩葉(著者)</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第18話前編　ダメ人間とお姉ちゃんと彼女</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>モテはるねえ蘆屋くん</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>栗原和明(原作) 寺井赤音(作画)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第15話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>理想の彼女</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>もりまりも(著者)</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第22話</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>王子様の友達</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>すけろく(著者)</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第28話</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>魔都精兵のスレイブ</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>原作:タカヒロ　漫画:竹村洋平</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第156話　神隠し</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>無敵商人の異世界成り上がり物語 ～現代の製品を自在に取り寄せるスキルがあるので異世界では楽勝です～</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>隆原ヒロタ(漫画) 青山有(原作) ぷきゅのすけ(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第34話④</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>転生してあらゆるモノに好かれながら異世界で好きな事をして生きて行く</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>都尾琉(漫画) 御峰。(原作)</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第26話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>王立魔術学院の鬼畜講師</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>実々みみず(漫画) 急川回レ(原作) zunta(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第19話二</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>アラサーがVTuberになった話。</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>犬威赤彦(漫画) とくめい(原作) カラスBTK(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第22話</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>オトナを知りたい女友達</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>望公太(原作) ぷよちゃ(作画)</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>コミックス告知</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>俺堕ちスレイブヒーローコレクション</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>ゆっ栗栖(著者)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第10話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>チュートリアルが始まる前に ボスキャラ達を破滅させない為に俺ができる幾つかの事</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>横山コウヂ(漫画) 髙橋炬燵(原作) カカオ・ランタン(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第13話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>愚かな天使は悪魔と踊る</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>アズマサワヨシ(著者)</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第99話④</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>六志麻あさ 業務用餅 kisui</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第６８話</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>ハーレムより平穏を！異世界で静かにニート姫させてくれ</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>さかたはるき(原作) かわやばぐ(作画)</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第13話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>魔のものたちは企てる</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>加藤拓弐(原作) ガしガし(作画)</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第27.5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>ギャルゲーマーに褒められたい</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>げしゅまろ(著者)</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>38話</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第135話 よくわからないけれど導かれてしまったようです（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>きみの願いが叶うまで</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>浅月のりと(著者)</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第3話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>豚のレバーは加熱しろ</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>みなみ(漫画) 逆井卓馬(原作) 遠坂あさぎ(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第41話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>小林さんちのメイドラゴン</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>クール教信者</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>外伝 後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>おねえさんと猫を飼う</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>上杉響士郎(著者)</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第1話：おねえさんと猫を拾う</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>くらいあの子としたいこと</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>碇マナツ(著者)</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第79話</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>経験値貯蓄でのんびり傷心旅行 ～勇者と恋人に追放された戦士の無自覚ざまぁ～</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>奏ヨシキ(著者) 徳川レモン(原作) riritto(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第36話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>理想のヒモ生活</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第85話　その3</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>おっさん、転生して天才役者になる</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>芽々ノ圭(漫画) ほえ太郎(原作)</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第36.5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>最強勇者パーティーは愛が知りたい</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>山田肌襦袢</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第26話「祭りは踊ったほうがいい」</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>怪異部～M県Y市の怪現象について～</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>さりい・Ｂ(著者)</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>File.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>神原絵理華(漫画) 一森一輝(原作)</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第17話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第73話　大阪LOVER</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>終末ツーリング</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>さいとー栄(著者)</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第48話 三沢基地　その４①</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>千年英雄</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>原作/福島航平 作画/中村ゆきひろ</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>16話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>カノジョに浮気されていた俺が、小悪魔な後輩に懐かれています</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>香澤陽平(漫画) えーる(キャラクター原案) 御宮ゆう(原作)</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第31話</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>ゲーセン少女と異文化交流</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>安原宏和(著者)</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>125.5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>一万倍の聖女が教える聖教育</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>MIGCHIP(著者)</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>最終話</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>ベヒモスの花婿</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>鈴音ことら(原作) 月並甲介(漫画)</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第7話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>戸賀 環 坂木持丸 riritto</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第48話②　お祭りを楽しんでみた</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>底辺冒険者だけど魔法を極めてみることにした ～無能スキルから神スキルに進化した【魔法創造】と【アイテム作成】で無双する～</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>蒼乃白兎 坂野杏梨 かわく</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第43話(後編) アーティフィカルモンスター</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第10話</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>顔に出ない柏田さんと顔に出る太田君＋</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>東ふゆ(著者)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第29話 愛田さんと宿泊研修</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>ダウナーお姉さんは遊びたい</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>山鷹景</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第12話</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>いとこのこ</t>
+          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>いぬちく(著者)</t>
+          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第35.5話</t>
+          <t>第4話-1：師匠と弟子の新生活</t>
         </is>
       </c>
     </row>
@@ -5741,17 +6783,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ぽんドロイド！ はまさん</t>
+          <t>姫様“拷問”の時間です</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>はれやまはれぞう(著者)</t>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第3話</t>
+          <t>拷問144</t>
         </is>
       </c>
     </row>
@@ -5761,17 +6803,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>このヒーラー、めんどくさい</t>
+          <t>窓際編集とバカにされた俺が、双子ＪＫと同居することになった</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>丹念に発酵(著者)</t>
+          <t>うさおとめ(著者) 茨木野(原作) トモゼロ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第88話：ゴブリンの罠</t>
+          <t>第4話①</t>
         </is>
       </c>
     </row>
@@ -5781,17 +6823,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>リビルドワールド</t>
+          <t>いとこのこ</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+          <t>いぬちく(著者)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第70話④</t>
+          <t>第35.5話</t>
         </is>
       </c>
     </row>
@@ -5801,17 +6843,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>リアデイルの大地にて</t>
+          <t>スキル【万物支配】に目覚めたおっさんは、ダンジョンで生計を立てることにしました～無職から始める支配者無双～</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>月見だしお(著者) Ceez(原作) てんまそ(キャラクター原案) 涼風涼(構成)</t>
+          <t>岸本和葉 原田 臙 シミズヒロノリ 吉武</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第39章-2</t>
+          <t>第3話　パーティ結成‼</t>
         </is>
       </c>
     </row>
@@ -5821,17 +6863,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>アイドル辞めるけど結婚してくれますか!?</t>
+          <t>悪役貴族として必要なそれ</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>三吉汐美(著者)</t>
+          <t>まさこりん(原作) 夏野うみ(作画) 村カルキ(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第16話前半</t>
+          <t>第17話①</t>
         </is>
       </c>
     </row>
@@ -5841,17 +6883,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>まったく最近の探偵ときたら</t>
+          <t>アイドル辞めるけど結婚してくれますか!?</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>五十嵐正邦(著者)</t>
+          <t>三吉汐美(著者)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第113話</t>
+          <t>第16話前半</t>
         </is>
       </c>
     </row>
@@ -5861,17 +6903,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>氷結令嬢さまをフォローしたら、メチャメチャ溺愛されてしまった件@comic</t>
+          <t>おんなのこのけんをてにいれた</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>漫画：ハレノチアメ 原作：愛坂タカト キャラクター原案：Bcoca</t>
+          <t>福岡太朗(著者)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1話扉イラスト案大公開！</t>
+          <t>13本目</t>
         </is>
       </c>
     </row>
@@ -5881,17 +6923,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>三枝さんはメガネ先輩と恋を描く</t>
+          <t>ぽんドロイド！ はまさん</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>セレビィ量産型(著者)</t>
+          <t>はれやまはれぞう(著者)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>特別編</t>
+          <t>第3話</t>
         </is>
       </c>
     </row>
@@ -5901,17 +6943,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ダメ人間の愛しかた</t>
+          <t>このヒーラー、めんどくさい</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>岩葉(著者)</t>
+          <t>丹念に発酵(著者)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第18話前編　ダメ人間とお姉ちゃんと彼女</t>
+          <t>第88話：ゴブリンの罠</t>
         </is>
       </c>
     </row>
@@ -5921,17 +6963,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>モテはるねえ蘆屋くん</t>
+          <t>ギャルゲーマーに褒められたい</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>栗原和明(原作) 寺井赤音(作画)</t>
+          <t>げしゅまろ(著者)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第15話後半</t>
+          <t>38話</t>
         </is>
       </c>
     </row>
@@ -5941,17 +6983,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>理想の彼女</t>
+          <t>まったく最近の探偵ときたら</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>もりまりも(著者)</t>
+          <t>五十嵐正邦(著者)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第22話</t>
+          <t>第113話</t>
         </is>
       </c>
     </row>
@@ -5961,17 +7003,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>王子様の友達</t>
+          <t>リアデイルの大地にて</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>すけろく(著者)</t>
+          <t>月見だしお(著者) Ceez(原作) てんまそ(キャラクター原案) 涼風涼(構成)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第28話</t>
+          <t>第39章-2</t>
         </is>
       </c>
     </row>
@@ -5981,17 +7023,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>魔都精兵のスレイブ</t>
+          <t>零細奴隷商人、一人も奴隷が売れなかったので売れ残り少女たちと辺境でスローライフをする</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>原作:タカヒロ　漫画:竹村洋平</t>
+          <t>原作：夜分長文 原案：はにゅう 漫画：もっつん*</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第156話　神隠し</t>
+          <t>第4話</t>
         </is>
       </c>
     </row>
@@ -6001,17 +7043,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>無敵商人の異世界成り上がり物語 ～現代の製品を自在に取り寄せるスキルがあるので異世界では楽勝です～</t>
+          <t>ダメ人間の愛しかた</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>隆原ヒロタ(漫画) 青山有(原作) ぷきゅのすけ(キャラクターデザイン)</t>
+          <t>岩葉(著者)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第34話④</t>
+          <t>第18話前編　ダメ人間とお姉ちゃんと彼女</t>
         </is>
       </c>
     </row>
@@ -6021,17 +7063,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>転生してあらゆるモノに好かれながら異世界で好きな事をして生きて行く</t>
+          <t>リビルドワールド</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>都尾琉(漫画) 御峰。(原作)</t>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第26話①</t>
+          <t>第70話④</t>
         </is>
       </c>
     </row>
@@ -6041,17 +7083,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>王立魔術学院の鬼畜講師</t>
+          <t>「先日救っていただいたドラゴンです」～押しかけ女房してきた美少女と、隠居した元Sランクオッサン冒険者による辺境スローライフ～</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>実々みみず(漫画) 急川回レ(原作) zunta(キャラクターデザイン)</t>
+          <t>漫画：紀乃なつき 原作：虎戸リア キャラクター原案：シソ</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第19話二</t>
+          <t>第7話</t>
         </is>
       </c>
     </row>
@@ -6061,17 +7103,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>アラサーがVTuberになった話。</t>
+          <t>モテはるねえ蘆屋くん</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>犬威赤彦(漫画) とくめい(原作) カラスBTK(キャラクター原案)</t>
+          <t>栗原和明(原作) 寺井赤音(作画)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第22話</t>
+          <t>第15話後半</t>
         </is>
       </c>
     </row>
@@ -6081,17 +7123,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>オトナを知りたい女友達</t>
+          <t>ナナシの器用貧乏</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>望公太(原作) ぷよちゃ(作画)</t>
+          <t>原作：高球 漫画：葉原辰月 キャラクター原案：KeG</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>コミックス告知</t>
+          <t>第4話</t>
         </is>
       </c>
     </row>
@@ -6101,17 +7143,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>俺堕ちスレイブヒーローコレクション</t>
+          <t>王子様の友達</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ゆっ栗栖(著者)</t>
+          <t>すけろく(著者)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第10話後半</t>
+          <t>第28話</t>
         </is>
       </c>
     </row>
@@ -6121,17 +7163,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>チュートリアルが始まる前に ボスキャラ達を破滅させない為に俺ができる幾つかの事</t>
+          <t>三枝さんはメガネ先輩と恋を描く</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>横山コウヂ(漫画) 髙橋炬燵(原作) カカオ・ランタン(キャラクターデザイン)</t>
+          <t>セレビィ量産型(著者)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第13話①</t>
+          <t>特別編</t>
         </is>
       </c>
     </row>
@@ -6141,17 +7183,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>愚かな天使は悪魔と踊る</t>
+          <t>氷結令嬢さまをフォローしたら、メチャメチャ溺愛されてしまった件@comic</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>アズマサワヨシ(著者)</t>
+          <t>漫画：ハレノチアメ 原作：愛坂タカト キャラクター原案：Bcoca</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第99話④</t>
+          <t>1話扉イラスト案大公開！</t>
         </is>
       </c>
     </row>
@@ -6161,17 +7203,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>六志麻あさ 業務用餅 kisui</t>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第６８話</t>
+          <t>第3話 前編</t>
         </is>
       </c>
     </row>
@@ -6181,17 +7223,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ハーレムより平穏を！異世界で静かにニート姫させてくれ</t>
+          <t>理想の彼女</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>さかたはるき(原作) かわやばぐ(作画)</t>
+          <t>もりまりも(著者)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第13話前半</t>
+          <t>第22話</t>
         </is>
       </c>
     </row>
@@ -6201,17 +7243,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>魔のものたちは企てる</t>
+          <t>異世界迷宮のオーパーツ</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>加藤拓弐(原作) ガしガし(作画)</t>
+          <t>三狛ハル(著者)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第27.5話</t>
+          <t>第2話-①：立派な棒と革と玉</t>
         </is>
       </c>
     </row>
@@ -6221,17 +7263,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ギャルゲーマーに褒められたい</t>
+          <t>魔都精兵のスレイブ</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>げしゅまろ(著者)</t>
+          <t>原作:タカヒロ　漫画:竹村洋平</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>38話</t>
+          <t>第156話　神隠し</t>
         </is>
       </c>
     </row>
@@ -6241,17 +7283,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>よくわからないけれど異世界に転生していたようです</t>
+          <t>半人前の恋人</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>内々けやき あし カオミン</t>
+          <t>川田大智</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第135話 よくわからないけれど導かれてしまったようです（１）</t>
+          <t>第47話</t>
         </is>
       </c>
     </row>
@@ -6261,17 +7303,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>きみの願いが叶うまで</t>
+          <t>千年英雄</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>浅月のりと(著者)</t>
+          <t>原作/福島航平 作画/中村ゆきひろ</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第3話-1</t>
+          <t>17話</t>
         </is>
       </c>
     </row>
@@ -6281,17 +7323,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>豚のレバーは加熱しろ</t>
+          <t>オトナを知りたい女友達</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>みなみ(漫画) 逆井卓馬(原作) 遠坂あさぎ(キャラクターデザイン)</t>
+          <t>望公太(原作) ぷよちゃ(作画)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第41話②</t>
+          <t>コミックス告知</t>
         </is>
       </c>
     </row>
@@ -6301,17 +7343,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>小林さんちのメイドラゴン</t>
+          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>クール教信者</t>
+          <t>六志麻あさ 業務用餅 kisui</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>外伝 後編</t>
+          <t>第６８話</t>
         </is>
       </c>
     </row>
@@ -6321,17 +7363,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>おねえさんと猫を飼う</t>
+          <t>よくわからないけれど異世界に転生していたようです</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>上杉響士郎(著者)</t>
+          <t>内々けやき あし カオミン</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第1話：おねえさんと猫を拾う</t>
+          <t>第135話 よくわからないけれど導かれてしまったようです（１）</t>
         </is>
       </c>
     </row>
@@ -6341,17 +7383,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>くらいあの子としたいこと</t>
+          <t>無敵商人の異世界成り上がり物語 ～現代の製品を自在に取り寄せるスキルがあるので異世界では楽勝です～</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>碇マナツ(著者)</t>
+          <t>隆原ヒロタ(漫画) 青山有(原作) ぷきゅのすけ(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第79話</t>
+          <t>第34話④</t>
         </is>
       </c>
     </row>
@@ -6361,17 +7403,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>経験値貯蓄でのんびり傷心旅行 ～勇者と恋人に追放された戦士の無自覚ざまぁ～</t>
+          <t>アラサーがVTuberになった話。</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>奏ヨシキ(著者) 徳川レモン(原作) riritto(キャラクターデザイン)</t>
+          <t>犬威赤彦(漫画) とくめい(原作) カラスBTK(キャラクター原案)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第36話-2</t>
+          <t>第22話</t>
         </is>
       </c>
     </row>
@@ -6381,17 +7423,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>理想のヒモ生活</t>
+          <t>魔のものたちは企てる</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+          <t>加藤拓弐(原作) ガしガし(作画)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第85話　その3</t>
+          <t>第27.5話</t>
         </is>
       </c>
     </row>
@@ -6401,17 +7443,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>おっさん、転生して天才役者になる</t>
+          <t>俺堕ちスレイブヒーローコレクション</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>芽々ノ圭(漫画) ほえ太郎(原作)</t>
+          <t>ゆっ栗栖(著者)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第36.5話</t>
+          <t>第10話後半</t>
         </is>
       </c>
     </row>
@@ -6421,17 +7463,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>最強勇者パーティーは愛が知りたい</t>
+          <t>王立魔術学院の鬼畜講師</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>山田肌襦袢</t>
+          <t>実々みみず(漫画) 急川回レ(原作) zunta(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第26話「祭りは踊ったほうがいい」</t>
+          <t>第19話二</t>
         </is>
       </c>
     </row>
@@ -6441,17 +7483,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>怪異部～M県Y市の怪現象について～</t>
+          <t>呪わないで！ 呪崎さん</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>さりい・Ｂ(著者)</t>
+          <t>依澄れい(著者)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>File.5</t>
+          <t>第２話</t>
         </is>
       </c>
     </row>
@@ -6461,17 +7503,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
+          <t>ハーレムより平穏を！異世界で静かにニート姫させてくれ</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>神原絵理華(漫画) 一森一輝(原作)</t>
+          <t>さかたはるき(原作) かわやばぐ(作画)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第17話③</t>
+          <t>第13話前半</t>
         </is>
       </c>
     </row>
@@ -6481,17 +7523,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
+          <t>元魔王様の南国スローライフ ～部下に裏切られたので、モフモフ達と楽しくスローライフするのじゃ～</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
+          <t>原作：十一屋翠 漫画：高羽ツバサ キャラクター原案：ファルまろ</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第73話　大阪LOVER</t>
+          <t>第10話</t>
         </is>
       </c>
     </row>
@@ -6501,17 +7543,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>終末ツーリング</t>
+          <t>世界の終わりの世界録(アンコール)</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>さいとー栄(著者)</t>
+          <t>雨水龍(著者) 細音啓(原作) ふゆの春秋(キャラクター原案)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第48話 三沢基地　その４①</t>
+          <t>第95話①</t>
         </is>
       </c>
     </row>
@@ -6521,17 +7563,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>千年英雄</t>
+          <t>育成上手な冒険者、幼女を拾い、セカンドライフを育児に捧げる</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>原作/福島航平 作画/中村ゆきひろ</t>
+          <t>原作／リズ 漫画／森見明日</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>16話②</t>
+          <t>第14話</t>
         </is>
       </c>
     </row>
@@ -6541,17 +7583,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>カノジョに浮気されていた俺が、小悪魔な後輩に懐かれています</t>
+          <t>ウィル様は今日も魔法で遊んでいます。ねくすと！</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>香澤陽平(漫画) えーる(キャラクター原案) 御宮ゆう(原作)</t>
+          <t>原作：綾河ららら 漫画：秋嶋うおと キャラクター原案：ネコメガネ</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第31話</t>
+          <t>第35話</t>
         </is>
       </c>
     </row>
@@ -6561,17 +7603,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>ゲーセン少女と異文化交流</t>
+          <t>小林さんちのメイドラゴン</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>安原宏和(著者)</t>
+          <t>クール教信者</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>125.5話</t>
+          <t>外伝 後編</t>
         </is>
       </c>
     </row>
@@ -6581,17 +7623,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>一万倍の聖女が教える聖教育</t>
+          <t>転生してあらゆるモノに好かれながら異世界で好きな事をして生きて行く</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>MIGCHIP(著者)</t>
+          <t>都尾琉(漫画) 御峰。(原作)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>最終話</t>
+          <t>第26話①</t>
         </is>
       </c>
     </row>
@@ -6601,17 +7643,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ベヒモスの花婿</t>
+          <t>愚かな天使は悪魔と踊る</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>鈴音ことら(原作) 月並甲介(漫画)</t>
+          <t>アズマサワヨシ(著者)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第7話①</t>
+          <t>第99話④</t>
         </is>
       </c>
     </row>
@@ -6621,17 +7663,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+          <t>経験値貯蓄でのんびり傷心旅行 ～勇者と恋人に追放された戦士の無自覚ざまぁ～</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>戸賀 環 坂木持丸 riritto</t>
+          <t>奏ヨシキ(著者) 徳川レモン(原作) riritto(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第48話②　お祭りを楽しんでみた</t>
+          <t>第36話-2</t>
         </is>
       </c>
     </row>
@@ -6641,17 +7683,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>底辺冒険者だけど魔法を極めてみることにした ～無能スキルから神スキルに進化した【魔法創造】と【アイテム作成】で無双する～</t>
+          <t>底辺ハンターが【リターン】スキルで現代最強 ～前世の知識と死に戻りを駆使して、人類最速レベルアップ～</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>蒼乃白兎 坂野杏梨 かわく</t>
+          <t>原作：萩鵜アキ 漫画：仲間友 キャラクター原案：gunkan</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第43話(後編) アーティフィカルモンスター</t>
+          <t>第18話</t>
         </is>
       </c>
     </row>
@@ -6661,17 +7703,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
+          <t>チュートリアルが始まる前に ボスキャラ達を破滅させない為に俺ができる幾つかの事</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
+          <t>横山コウヂ(漫画) 髙橋炬燵(原作) カカオ・ランタン(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第10話</t>
+          <t>第13話①</t>
         </is>
       </c>
     </row>
@@ -6681,17 +7723,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>顔に出ない柏田さんと顔に出る太田君＋</t>
+          <t>くらいあの子としたいこと</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>東ふゆ(著者)</t>
+          <t>碇マナツ(著者)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第29話 愛田さんと宿泊研修</t>
+          <t>第79話</t>
         </is>
       </c>
     </row>
@@ -6701,17 +7743,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>ダウナーお姉さんは遊びたい</t>
+          <t>理想のヒモ生活</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>山鷹景</t>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第12話</t>
+          <t>第85話　その3</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-07-08
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -22,6 +22,7 @@
     <sheet name="2025-07-05" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="2025-07-06" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="2025-07-07" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="2025-07-08" sheetId="17" state="visible" r:id="rId17"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -6758,22 +6759,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第4話-1：師匠と弟子の新生活</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>姫様“拷問”の時間です</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>拷問144</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>窓際編集とバカにされた俺が、双子ＪＫと同居することになった</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>うさおとめ(著者) 茨木野(原作) トモゼロ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第4話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>いとこのこ</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>いぬちく(著者)</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第35.5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>スキル【万物支配】に目覚めたおっさんは、ダンジョンで生計を立てることにしました～無職から始める支配者無双～</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>岸本和葉 原田 臙 シミズヒロノリ 吉武</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第3話　パーティ結成‼</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>悪役貴族として必要なそれ</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>まさこりん(原作) 夏野うみ(作画) 村カルキ(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第17話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>アイドル辞めるけど結婚してくれますか!?</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>三吉汐美(著者)</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第16話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>おんなのこのけんをてにいれた</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>福岡太朗(著者)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>13本目</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>ぽんドロイド！ はまさん</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>はれやまはれぞう(著者)</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第3話</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>このヒーラー、めんどくさい</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>丹念に発酵(著者)</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第88話：ゴブリンの罠</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>ギャルゲーマーに褒められたい</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>げしゅまろ(著者)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>38話</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>まったく最近の探偵ときたら</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>五十嵐正邦(著者)</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第113話</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>リアデイルの大地にて</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>月見だしお(著者) Ceez(原作) てんまそ(キャラクター原案) 涼風涼(構成)</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第39章-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>零細奴隷商人、一人も奴隷が売れなかったので売れ残り少女たちと辺境でスローライフをする</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>原作：夜分長文 原案：はにゅう 漫画：もっつん*</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第4話</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>ダメ人間の愛しかた</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>岩葉(著者)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第18話前編　ダメ人間とお姉ちゃんと彼女</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第70話④</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>「先日救っていただいたドラゴンです」～押しかけ女房してきた美少女と、隠居した元Sランクオッサン冒険者による辺境スローライフ～</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>漫画：紀乃なつき 原作：虎戸リア キャラクター原案：シソ</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第7話</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>モテはるねえ蘆屋くん</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>栗原和明(原作) 寺井赤音(作画)</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第15話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>ナナシの器用貧乏</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>原作：高球 漫画：葉原辰月 キャラクター原案：KeG</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第4話</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>王子様の友達</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>すけろく(著者)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第28話</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>三枝さんはメガネ先輩と恋を描く</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>セレビィ量産型(著者)</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>特別編</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>氷結令嬢さまをフォローしたら、メチャメチャ溺愛されてしまった件@comic</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>漫画：ハレノチアメ 原作：愛坂タカト キャラクター原案：Bcoca</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>1話扉イラスト案大公開！</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第3話 前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>理想の彼女</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>もりまりも(著者)</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第22話</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>異世界迷宮のオーパーツ</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>三狛ハル(著者)</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第2話-①：立派な棒と革と玉</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>魔都精兵のスレイブ</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>原作:タカヒロ　漫画:竹村洋平</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第156話　神隠し</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>半人前の恋人</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>川田大智</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第47話</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>千年英雄</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>原作/福島航平 作画/中村ゆきひろ</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>17話</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>オトナを知りたい女友達</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>望公太(原作) ぷよちゃ(作画)</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>コミックス告知</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>六志麻あさ 業務用餅 kisui</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第６８話</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第135話 よくわからないけれど導かれてしまったようです（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>無敵商人の異世界成り上がり物語 ～現代の製品を自在に取り寄せるスキルがあるので異世界では楽勝です～</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>隆原ヒロタ(漫画) 青山有(原作) ぷきゅのすけ(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第34話④</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>アラサーがVTuberになった話。</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>犬威赤彦(漫画) とくめい(原作) カラスBTK(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第22話</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>魔のものたちは企てる</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>加藤拓弐(原作) ガしガし(作画)</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第27.5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>俺堕ちスレイブヒーローコレクション</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>ゆっ栗栖(著者)</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第10話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>王立魔術学院の鬼畜講師</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>実々みみず(漫画) 急川回レ(原作) zunta(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第19話二</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>呪わないで！ 呪崎さん</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>依澄れい(著者)</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第２話</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>ハーレムより平穏を！異世界で静かにニート姫させてくれ</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>さかたはるき(原作) かわやばぐ(作画)</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第13話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>元魔王様の南国スローライフ ～部下に裏切られたので、モフモフ達と楽しくスローライフするのじゃ～</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>原作：十一屋翠 漫画：高羽ツバサ キャラクター原案：ファルまろ</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第10話</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>世界の終わりの世界録(アンコール)</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>雨水龍(著者) 細音啓(原作) ふゆの春秋(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第95話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>育成上手な冒険者、幼女を拾い、セカンドライフを育児に捧げる</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>原作／リズ 漫画／森見明日</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第14話</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>ウィル様は今日も魔法で遊んでいます。ねくすと！</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>原作：綾河ららら 漫画：秋嶋うおと キャラクター原案：ネコメガネ</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第35話</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>小林さんちのメイドラゴン</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>クール教信者</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>外伝 後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>転生してあらゆるモノに好かれながら異世界で好きな事をして生きて行く</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>都尾琉(漫画) 御峰。(原作)</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第26話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>愚かな天使は悪魔と踊る</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>アズマサワヨシ(著者)</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第99話④</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>経験値貯蓄でのんびり傷心旅行 ～勇者と恋人に追放された戦士の無自覚ざまぁ～</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>奏ヨシキ(著者) 徳川レモン(原作) riritto(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第36話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>底辺ハンターが【リターン】スキルで現代最強 ～前世の知識と死に戻りを駆使して、人類最速レベルアップ～</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>原作：萩鵜アキ 漫画：仲間友 キャラクター原案：gunkan</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第18話</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>チュートリアルが始まる前に ボスキャラ達を破滅させない為に俺ができる幾つかの事</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>横山コウヂ(漫画) 髙橋炬燵(原作) カカオ・ランタン(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第13話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>くらいあの子としたいこと</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>碇マナツ(著者)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第79話</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>理想のヒモ生活</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第85話　その3</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
+          <t>食い詰め傭兵の幻想奇譚</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
+          <t>原作／まいん キャラクター原案／peroshi 漫画／池宮アレア</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第4話-1：師匠と弟子の新生活</t>
+          <t>第28話</t>
         </is>
       </c>
     </row>
@@ -6783,17 +7825,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>姫様“拷問”の時間です</t>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>拷問144</t>
+          <t>第５０話　雌雄を決する器用貧乏（１）</t>
         </is>
       </c>
     </row>
@@ -6803,17 +7845,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>窓際編集とバカにされた俺が、双子ＪＫと同居することになった</t>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>うさおとめ(著者) 茨木野(原作) トモゼロ(キャラクター原案)</t>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第4話①</t>
+          <t>第２２食　ユクシーさんの覚悟、すごいのですわ！（１）</t>
         </is>
       </c>
     </row>
@@ -6823,17 +7865,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>いとこのこ</t>
+          <t>異世界メイドの三ツ星グルメ ～現代ごはん作ったら王宮で大バズリしました～</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>いぬちく(著者)</t>
+          <t>モリタ Ｕ４ nima</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第35.5話</t>
+          <t>第12話（６）　恋焦がれ！黄金色の実りと、握るはふっくら銀のシャリ（６）</t>
         </is>
       </c>
     </row>
@@ -6843,17 +7885,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>スキル【万物支配】に目覚めたおっさんは、ダンジョンで生計を立てることにしました～無職から始める支配者無双～</t>
+          <t>濁る瞳で何を願う ハイセルク戦記</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>岸本和葉 原田 臙 シミズヒロノリ 吉武</t>
+          <t>トルトネン 創-taro 斎藤八呑</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第3話　パーティ結成‼</t>
+          <t>第31話 大暴走</t>
         </is>
       </c>
     </row>
@@ -6863,17 +7905,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>悪役貴族として必要なそれ</t>
+          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>まさこりん(原作) 夏野うみ(作画) 村カルキ(キャラクターデザイン)</t>
+          <t>KAKERU</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第17話①</t>
+          <t>第66話「東アイギス」（前半）</t>
         </is>
       </c>
     </row>
@@ -6883,17 +7925,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>アイドル辞めるけど結婚してくれますか!?</t>
+          <t>ガチャを回して仲間を増やす 最強の美少女軍団を作り上げろ</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>三吉汐美(著者)</t>
+          <t>漫画：晴野しゅー 原作：ちんくるり キャラクター原案：イセ川ヤスタカ</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第16話前半</t>
+          <t>第71話前半</t>
         </is>
       </c>
     </row>
@@ -6903,17 +7945,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>おんなのこのけんをてにいれた</t>
+          <t>いつでも自宅に帰れる俺は、異世界で行商人をはじめました</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>福岡太朗(著者)</t>
+          <t>漫画／明地雫 原作／霜月緋色 キャラクター原案／いわさきたかし</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>13本目</t>
+          <t>第58話</t>
         </is>
       </c>
     </row>
@@ -6923,17 +7965,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ぽんドロイド！ はまさん</t>
+          <t>王都ワンオペゴーレムマスター。まさかの追放！？～自由の身になったので弟子の美人勇者たちと一緒に最強ゴーレム作ります。戻ってこいと言われてももう知らん！～@COMIC</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>はれやまはれぞう(著者)</t>
+          <t>阿住 周（漫画） レルクス（原作） 布施龍太（キャラクター原案）</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第3話</t>
+          <t>第8話</t>
         </is>
       </c>
     </row>
@@ -6943,17 +7985,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>このヒーラー、めんどくさい</t>
+          <t>異世界のすみっこで快適ものづくり生活 ～女神さまのくれた工房はちょっとやりすぎ性能だった～</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>丹念に発酵(著者)</t>
+          <t>西山アラタ(漫画) 長田信織(原作) 東上文(キャラクター原案)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第88話：ゴブリンの罠</t>
+          <t>EP.19①</t>
         </is>
       </c>
     </row>
@@ -6963,17 +8005,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ギャルゲーマーに褒められたい</t>
+          <t>ポーション頼みで生き延びます！ 続</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>げしゅまろ(著者)</t>
+          <t>原作：FUNA 漫画：園心ふつう キャラクター原案：すきま</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>38話</t>
+          <t>第63話　長いお別れ Ⅱ</t>
         </is>
       </c>
     </row>
@@ -6983,17 +8025,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>まったく最近の探偵ときたら</t>
+          <t>江戸前エルフ</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>五十嵐正邦(著者)</t>
+          <t>樋口彰彦</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第113話</t>
+          <t>#112</t>
         </is>
       </c>
     </row>
@@ -7003,17 +8045,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>リアデイルの大地にて</t>
+          <t>ブチ切れ令嬢は報復を誓いました。 ～魔導書の力で祖国を叩き潰します～</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>月見だしお(著者) Ceez(原作) てんまそ(キャラクター原案) 涼風涼(構成)</t>
+          <t>漫画：おおのいも 原作：はぐれメタボ キャラクター原案：昌未</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第39章-2</t>
+          <t>第47話</t>
         </is>
       </c>
     </row>
@@ -7023,17 +8065,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>零細奴隷商人、一人も奴隷が売れなかったので売れ残り少女たちと辺境でスローライフをする</t>
+          <t>創造錬金術師は自由を謳歌する 故郷を追放されたら、魔王のお膝元で超絶効果のマジックアイテム作り放題になりました</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>原作：夜分長文 原案：はにゅう 漫画：もっつん*</t>
+          <t>姫乃タカ(漫画) 千月さかき(原作) かぼちゃ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第4話</t>
+          <t>第19話-2</t>
         </is>
       </c>
     </row>
@@ -7043,17 +8085,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ダメ人間の愛しかた</t>
+          <t>クラス最安値で売られた俺は、実は最強パラメーター</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>岩葉(著者)</t>
+          <t>カンブリア爆発太郎(漫画) RYOMA(原作) 黒井ススム(キャラクター原案)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第18話前編　ダメ人間とお姉ちゃんと彼女</t>
+          <t>第35話-3</t>
         </is>
       </c>
     </row>
@@ -7063,17 +8105,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>リビルドワールド</t>
+          <t>ロメリア戦記～伯爵令嬢、魔王を倒した後も人類やばそうだから軍隊組織する～</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+          <t>漫画：上戸 亮 原作：有山リョウ(小学館「ガガガブックス」刊) キャラクター原案：コダマ</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第70話④</t>
+          <t>第13話「助けてくれる人々」②</t>
         </is>
       </c>
     </row>
@@ -7083,17 +8125,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>「先日救っていただいたドラゴンです」～押しかけ女房してきた美少女と、隠居した元Sランクオッサン冒険者による辺境スローライフ～</t>
+          <t>孤児院テイマー</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>漫画：紀乃なつき 原作：虎戸リア キャラクター原案：シソ</t>
+          <t>漫画：倉崎もろこ 原作：安藤正樹 キャラクター原案：イシバシヨウスケ</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第7話</t>
+          <t>第60話</t>
         </is>
       </c>
     </row>
@@ -7103,17 +8145,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>モテはるねえ蘆屋くん</t>
+          <t>断れない会長は友江くんにだけしてあげたい</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>栗原和明(原作) 寺井赤音(作画)</t>
+          <t>沼地どろまる(著者)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第15話後半</t>
+          <t>コミックス第２巻発売記念！生徒会総選挙！</t>
         </is>
       </c>
     </row>
@@ -7123,17 +8165,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ナナシの器用貧乏</t>
+          <t>アレクサンダー英雄戦記～最強の土魔術士～</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>原作：高球 漫画：葉原辰月 キャラクター原案：KeG</t>
+          <t>マツオカヨシノリ るれくちぇ なんじゃもんじゃ</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第4話</t>
+          <t>第10話（後編）</t>
         </is>
       </c>
     </row>
@@ -7143,17 +8185,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>王子様の友達</t>
+          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>すけろく(著者)</t>
+          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第28話</t>
+          <t>第4話-1：師匠と弟子の新生活</t>
         </is>
       </c>
     </row>
@@ -7163,17 +8205,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>三枝さんはメガネ先輩と恋を描く</t>
+          <t>え、テイマーは使えないってパーティから追放したよね？ ～実は世界唯一の【精霊使い】だと判明した途端に手のひらを返されても遅い。精霊の王女様にめちゃくちゃ溺愛されながら、僕はマイペースに最強を目指すので</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>セレビィ量産型(著者)</t>
+          <t>漫画：最中なつめ 原作：茨木野</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>特別編</t>
+          <t>第30話 特性と代償(後編)</t>
         </is>
       </c>
     </row>
@@ -7183,17 +8225,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>氷結令嬢さまをフォローしたら、メチャメチャ溺愛されてしまった件@comic</t>
+          <t>神の庭付き楠木邸</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>漫画：ハレノチアメ 原作：愛坂タカト キャラクター原案：Bcoca</t>
+          <t>安斎アキラ(著者) えんじゅ(原作) ox(キャラクター原案)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1話扉イラスト案大公開！</t>
+          <t>第32話</t>
         </is>
       </c>
     </row>
@@ -7203,17 +8245,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+          <t>姫様“拷問”の時間です</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第3話 前編</t>
+          <t>拷問144</t>
         </is>
       </c>
     </row>
@@ -7223,17 +8265,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>理想の彼女</t>
+          <t>Ｒｅ：ゼロから始める異世界生活 第四章 聖域と強欲の魔女</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>もりまりも(著者)</t>
+          <t>花鶏ハルノ(作画) 相川有(構成) 長月達平(原作) 大塚真一郎(キャラクター原案)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第22話</t>
+          <t>第61話①　エリオール大森林の永久凍土</t>
         </is>
       </c>
     </row>
@@ -7243,17 +8285,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>異世界迷宮のオーパーツ</t>
+          <t>迷宮ブラックカンパニー</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>三狛ハル(著者)</t>
+          <t>安村洋平</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第2話-①：立派な棒と革と玉</t>
+          <t>第50話　落花流水（前編）</t>
         </is>
       </c>
     </row>
@@ -7263,17 +8305,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>魔都精兵のスレイブ</t>
+          <t>ジゼルの錬金飴</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>原作:タカヒロ　漫画:竹村洋平</t>
+          <t>漫画： katoson 原作：斯波 キャラクター原案：LINO</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第156話　神隠し</t>
+          <t>第8話</t>
         </is>
       </c>
     </row>
@@ -7283,17 +8325,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>半人前の恋人</t>
+          <t>いとこのこ</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>川田大智</t>
+          <t>いぬちく(著者)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第47話</t>
+          <t>第35.5話</t>
         </is>
       </c>
     </row>
@@ -7303,17 +8345,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>千年英雄</t>
+          <t>追放されたギルド職員は、世界最強の召喚士@COMIC</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>原作/福島航平 作画/中村ゆきひろ</t>
+          <t>原作：月島秀一 漫画：あづち涼 キャラクター原案：チワワ丸</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>17話</t>
+          <t>第9話②「伏魔殿ダラスの惨劇」</t>
         </is>
       </c>
     </row>
@@ -7323,17 +8365,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>オトナを知りたい女友達</t>
+          <t>コボルト無双、モフモフな最弱噛ませ犬だけど世界最強を目指す！</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>望公太(原作) ぷよちゃ(作画)</t>
+          <t>赤志木ひの乃 shiba</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>コミックス告知</t>
+          <t>第十三話 帰還</t>
         </is>
       </c>
     </row>
@@ -7343,17 +8385,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
+          <t>少年マールの転生冒険記</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>六志麻あさ 業務用餅 kisui</t>
+          <t>漫画家：あわや 原作：月ノ宮マクラ キャラクター原案：まっちょこ</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第６８話</t>
+          <t>第17話</t>
         </is>
       </c>
     </row>
@@ -7363,17 +8405,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>よくわからないけれど異世界に転生していたようです</t>
+          <t>無能は不要と言われ『時計使い』の僕は職人ギルドから追い出されるも、ダンジョンの深部で真の力に覚醒する</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>内々けやき あし カオミン</t>
+          <t>漫画：さらさみさ 小説： 桜霧琥珀 キャラ原案： 福きつね</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第135話 よくわからないけれど導かれてしまったようです（１）</t>
+          <t>第19話前半</t>
         </is>
       </c>
     </row>
@@ -7383,17 +8425,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>無敵商人の異世界成り上がり物語 ～現代の製品を自在に取り寄せるスキルがあるので異世界では楽勝です～</t>
+          <t>魔物ノ森ノ少女ノヴァ</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>隆原ヒロタ(漫画) 青山有(原作) ぷきゅのすけ(キャラクターデザイン)</t>
+          <t>kamatama</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第34話④</t>
+          <t>第6話「ロスタイム」後編</t>
         </is>
       </c>
     </row>
@@ -7403,17 +8445,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>アラサーがVTuberになった話。</t>
+          <t>このヒーラー、めんどくさい</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>犬威赤彦(漫画) とくめい(原作) カラスBTK(キャラクター原案)</t>
+          <t>丹念に発酵(著者)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第22話</t>
+          <t>第88話：ゴブリンの罠</t>
         </is>
       </c>
     </row>
@@ -7423,17 +8465,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>魔のものたちは企てる</t>
+          <t>安達としまむら</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>加藤拓弐(原作) ガしガし(作画)</t>
+          <t>柚原もけ(漫画) 入間人間(原作) のん(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第27.5話</t>
+          <t>第48話「最初の旅の端１」①</t>
         </is>
       </c>
     </row>
@@ -7443,17 +8485,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>俺堕ちスレイブヒーローコレクション</t>
+          <t>スキル【万物支配】に目覚めたおっさんは、ダンジョンで生計を立てることにしました～無職から始める支配者無双～</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>ゆっ栗栖(著者)</t>
+          <t>岸本和葉 原田 臙 シミズヒロノリ 吉武</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第10話後半</t>
+          <t>第3話　パーティ結成‼</t>
         </is>
       </c>
     </row>
@@ -7463,17 +8505,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>王立魔術学院の鬼畜講師</t>
+          <t>ポンコツスキルしか使えない悪役魔女だけど、テイムしたパリピなスライムたちと強く生きます！</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>実々みみず(漫画) 急川回レ(原作) zunta(キャラクターデザイン)</t>
+          <t>漫画：鈴木イゾ 原作：雨傘ヒョウゴ キャラクター原案：朝日川日和</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第19話二</t>
+          <t>第8話</t>
         </is>
       </c>
     </row>
@@ -7483,17 +8525,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>呪わないで！ 呪崎さん</t>
+          <t>ぽんドロイド！ はまさん</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>依澄れい(著者)</t>
+          <t>はれやまはれぞう(著者)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第２話</t>
+          <t>第3話</t>
         </is>
       </c>
     </row>
@@ -7503,17 +8545,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ハーレムより平穏を！異世界で静かにニート姫させてくれ</t>
+          <t>ニャイト・オブ・ザ・リビングキャット</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>さかたはるき(原作) かわやばぐ(作画)</t>
+          <t>原作：ホークマン 作画：メカルーツ</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第13話前半</t>
+          <t>Chapter15　ニャンペイジ（後編）</t>
         </is>
       </c>
     </row>
@@ -7523,17 +8565,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>元魔王様の南国スローライフ ～部下に裏切られたので、モフモフ達と楽しくスローライフするのじゃ～</t>
+          <t>異世界で最強のスキルを生み出せたので、ひたすら無双することにしました。　～俺だけがスキルの数値を勝手に操作～</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>原作：十一屋翠 漫画：高羽ツバサ キャラクター原案：ファルまろ</t>
+          <t>漫画：星トマジロウ 原作：ヒゲ抜き地蔵 キャラクター原案：山椒魚</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第10話</t>
+          <t>第9話 ②</t>
         </is>
       </c>
     </row>
@@ -7543,17 +8585,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>世界の終わりの世界録(アンコール)</t>
+          <t>アラフォーおっさんはスローライフの夢を見るか？</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>雨水龍(著者) 細音啓(原作) ふゆの春秋(キャラクター原案)</t>
+          <t>漫画：大関詠詞 原作：サイトウアユム キャラクター原案： ジョンディー</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第95話①</t>
+          <t>第14話</t>
         </is>
       </c>
     </row>
@@ -7563,17 +8605,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>育成上手な冒険者、幼女を拾い、セカンドライフを育児に捧げる</t>
+          <t>アイドル辞めるけど結婚してくれますか!?</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>原作／リズ 漫画／森見明日</t>
+          <t>三吉汐美(著者)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第14話</t>
+          <t>第16話前半</t>
         </is>
       </c>
     </row>
@@ -7583,17 +8625,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>ウィル様は今日も魔法で遊んでいます。ねくすと！</t>
+          <t>まったく最近の探偵ときたら</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>原作：綾河ららら 漫画：秋嶋うおと キャラクター原案：ネコメガネ</t>
+          <t>五十嵐正邦(著者)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第35話</t>
+          <t>第113話</t>
         </is>
       </c>
     </row>
@@ -7603,17 +8645,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>小林さんちのメイドラゴン</t>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>クール教信者</t>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>外伝 後編</t>
+          <t>第3話 前編</t>
         </is>
       </c>
     </row>
@@ -7623,17 +8665,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>転生してあらゆるモノに好かれながら異世界で好きな事をして生きて行く</t>
+          <t>エンドロールの後には最高の旅を</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>都尾琉(漫画) 御峰。(原作)</t>
+          <t>リキタケ</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第26話①</t>
+          <t>最終話 最高の旅を②</t>
         </is>
       </c>
     </row>
@@ -7643,17 +8685,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>愚かな天使は悪魔と踊る</t>
+          <t>千年英雄</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>アズマサワヨシ(著者)</t>
+          <t>原作/福島航平 作画/中村ゆきひろ</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第99話④</t>
+          <t>18話①</t>
         </is>
       </c>
     </row>
@@ -7663,17 +8705,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>経験値貯蓄でのんびり傷心旅行 ～勇者と恋人に追放された戦士の無自覚ざまぁ～</t>
+          <t>さんしょく弁当</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>奏ヨシキ(著者) 徳川レモン(原作) riritto(キャラクターデザイン)</t>
+          <t>兎月あい(著者)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第36話-2</t>
+          <t>第18話#3</t>
         </is>
       </c>
     </row>
@@ -7683,17 +8725,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>底辺ハンターが【リターン】スキルで現代最強 ～前世の知識と死に戻りを駆使して、人類最速レベルアップ～</t>
+          <t>リアデイルの大地にて</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>原作：萩鵜アキ 漫画：仲間友 キャラクター原案：gunkan</t>
+          <t>月見だしお(著者) Ceez(原作) てんまそ(キャラクター原案) 涼風涼(構成)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第18話</t>
+          <t>第39章-2</t>
         </is>
       </c>
     </row>
@@ -7703,17 +8745,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>チュートリアルが始まる前に ボスキャラ達を破滅させない為に俺ができる幾つかの事</t>
+          <t>異世界創造のすゝめ～スマホアプリで惑星を創ってしまった俺は神となり世界を巡る～@COMIC</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>横山コウヂ(漫画) 髙橋炬燵(原作) カカオ・ランタン(キャラクターデザイン)</t>
+          <t>漫画：岩戸あきら 原作：たまごかけキャンディー キャラクター原案：かれい</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第13話①</t>
+          <t>第11話 ①</t>
         </is>
       </c>
     </row>
@@ -7723,17 +8765,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>くらいあの子としたいこと</t>
+          <t>王子様の友達</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>碇マナツ(著者)</t>
+          <t>すけろく(著者)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第79話</t>
+          <t>第28話</t>
         </is>
       </c>
     </row>
@@ -7743,17 +8785,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>理想のヒモ生活</t>
+          <t>クソ女に幸あれ</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+          <t>岸川瑞樹</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第85話　その3</t>
+          <t>第59話</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-07-09
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -23,6 +23,7 @@
     <sheet name="2025-07-06" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="2025-07-07" sheetId="16" state="visible" r:id="rId16"/>
     <sheet name="2025-07-08" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="2025-07-09" sheetId="18" state="visible" r:id="rId18"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -7800,22 +7801,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>食い詰め傭兵の幻想奇譚</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>原作／まいん キャラクター原案／peroshi 漫画／池宮アレア</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第28話</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第５０話　雌雄を決する器用貧乏（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第２２食　ユクシーさんの覚悟、すごいのですわ！（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>異世界メイドの三ツ星グルメ ～現代ごはん作ったら王宮で大バズリしました～</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>モリタ Ｕ４ nima</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第12話（６）　恋焦がれ！黄金色の実りと、握るはふっくら銀のシャリ（６）</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>濁る瞳で何を願う ハイセルク戦記</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>トルトネン 創-taro 斎藤八呑</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第31話 大暴走</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>KAKERU</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第66話「東アイギス」（前半）</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>ガチャを回して仲間を増やす 最強の美少女軍団を作り上げろ</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>漫画：晴野しゅー 原作：ちんくるり キャラクター原案：イセ川ヤスタカ</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第71話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>いつでも自宅に帰れる俺は、異世界で行商人をはじめました</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>漫画／明地雫 原作／霜月緋色 キャラクター原案／いわさきたかし</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第58話</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>王都ワンオペゴーレムマスター。まさかの追放！？～自由の身になったので弟子の美人勇者たちと一緒に最強ゴーレム作ります。戻ってこいと言われてももう知らん！～@COMIC</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>阿住 周（漫画） レルクス（原作） 布施龍太（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第8話</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>異世界のすみっこで快適ものづくり生活 ～女神さまのくれた工房はちょっとやりすぎ性能だった～</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>西山アラタ(漫画) 長田信織(原作) 東上文(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>EP.19①</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>ポーション頼みで生き延びます！ 続</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>原作：FUNA 漫画：園心ふつう キャラクター原案：すきま</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第63話　長いお別れ Ⅱ</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>江戸前エルフ</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>樋口彰彦</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>#112</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>ブチ切れ令嬢は報復を誓いました。 ～魔導書の力で祖国を叩き潰します～</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>漫画：おおのいも 原作：はぐれメタボ キャラクター原案：昌未</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第47話</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>創造錬金術師は自由を謳歌する 故郷を追放されたら、魔王のお膝元で超絶効果のマジックアイテム作り放題になりました</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>姫乃タカ(漫画) 千月さかき(原作) かぼちゃ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第19話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>クラス最安値で売られた俺は、実は最強パラメーター</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>カンブリア爆発太郎(漫画) RYOMA(原作) 黒井ススム(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第35話-3</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>ロメリア戦記～伯爵令嬢、魔王を倒した後も人類やばそうだから軍隊組織する～</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>漫画：上戸 亮 原作：有山リョウ(小学館「ガガガブックス」刊) キャラクター原案：コダマ</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第13話「助けてくれる人々」②</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>孤児院テイマー</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>漫画：倉崎もろこ 原作：安藤正樹 キャラクター原案：イシバシヨウスケ</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第60話</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>断れない会長は友江くんにだけしてあげたい</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>沼地どろまる(著者)</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>コミックス第２巻発売記念！生徒会総選挙！</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>アレクサンダー英雄戦記～最強の土魔術士～</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>マツオカヨシノリ るれくちぇ なんじゃもんじゃ</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第10話（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第4話-1：師匠と弟子の新生活</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>え、テイマーは使えないってパーティから追放したよね？ ～実は世界唯一の【精霊使い】だと判明した途端に手のひらを返されても遅い。精霊の王女様にめちゃくちゃ溺愛されながら、僕はマイペースに最強を目指すので</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>漫画：最中なつめ 原作：茨木野</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第30話 特性と代償(後編)</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>神の庭付き楠木邸</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>安斎アキラ(著者) えんじゅ(原作) ox(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第32話</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>姫様“拷問”の時間です</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>拷問144</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>Ｒｅ：ゼロから始める異世界生活 第四章 聖域と強欲の魔女</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>花鶏ハルノ(作画) 相川有(構成) 長月達平(原作) 大塚真一郎(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第61話①　エリオール大森林の永久凍土</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>迷宮ブラックカンパニー</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>安村洋平</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第50話　落花流水（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>ジゼルの錬金飴</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>漫画： katoson 原作：斯波 キャラクター原案：LINO</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第8話</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>いとこのこ</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>いぬちく(著者)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第35.5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>追放されたギルド職員は、世界最強の召喚士@COMIC</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>原作：月島秀一 漫画：あづち涼 キャラクター原案：チワワ丸</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第9話②「伏魔殿ダラスの惨劇」</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>コボルト無双、モフモフな最弱噛ませ犬だけど世界最強を目指す！</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>赤志木ひの乃 shiba</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第十三話 帰還</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>少年マールの転生冒険記</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>漫画家：あわや 原作：月ノ宮マクラ キャラクター原案：まっちょこ</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第17話</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>無能は不要と言われ『時計使い』の僕は職人ギルドから追い出されるも、ダンジョンの深部で真の力に覚醒する</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>漫画：さらさみさ 小説： 桜霧琥珀 キャラ原案： 福きつね</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第19話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>魔物ノ森ノ少女ノヴァ</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>kamatama</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第6話「ロスタイム」後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>このヒーラー、めんどくさい</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>丹念に発酵(著者)</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第88話：ゴブリンの罠</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>安達としまむら</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>柚原もけ(漫画) 入間人間(原作) のん(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第48話「最初の旅の端１」①</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>スキル【万物支配】に目覚めたおっさんは、ダンジョンで生計を立てることにしました～無職から始める支配者無双～</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>岸本和葉 原田 臙 シミズヒロノリ 吉武</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第3話　パーティ結成‼</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>ポンコツスキルしか使えない悪役魔女だけど、テイムしたパリピなスライムたちと強く生きます！</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>漫画：鈴木イゾ 原作：雨傘ヒョウゴ キャラクター原案：朝日川日和</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第8話</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>ぽんドロイド！ はまさん</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>はれやまはれぞう(著者)</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第3話</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>ニャイト・オブ・ザ・リビングキャット</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>原作：ホークマン 作画：メカルーツ</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>Chapter15　ニャンペイジ（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>異世界で最強のスキルを生み出せたので、ひたすら無双することにしました。　～俺だけがスキルの数値を勝手に操作～</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>漫画：星トマジロウ 原作：ヒゲ抜き地蔵 キャラクター原案：山椒魚</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第9話 ②</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>アラフォーおっさんはスローライフの夢を見るか？</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>漫画：大関詠詞 原作：サイトウアユム キャラクター原案： ジョンディー</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第14話</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>アイドル辞めるけど結婚してくれますか!?</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>三吉汐美(著者)</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第16話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>まったく最近の探偵ときたら</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>五十嵐正邦(著者)</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第113話</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第3話 前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>エンドロールの後には最高の旅を</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>リキタケ</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>最終話 最高の旅を②</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>千年英雄</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>原作/福島航平 作画/中村ゆきひろ</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>18話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>さんしょく弁当</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>兎月あい(著者)</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第18話#3</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>リアデイルの大地にて</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>月見だしお(著者) Ceez(原作) てんまそ(キャラクター原案) 涼風涼(構成)</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第39章-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>異世界創造のすゝめ～スマホアプリで惑星を創ってしまった俺は神となり世界を巡る～@COMIC</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>漫画：岩戸あきら 原作：たまごかけキャンディー キャラクター原案：かれい</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第11話 ①</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>王子様の友達</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>すけろく(著者)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第28話</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>クソ女に幸あれ</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>岸川瑞樹</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第59話</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>食い詰め傭兵の幻想奇譚</t>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>原作／まいん キャラクター原案／peroshi 漫画／池宮アレア</t>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第28話</t>
+          <t>第30話：一秒の奪い合い②</t>
         </is>
       </c>
     </row>
@@ -7825,17 +8867,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+          <t>マツモトケンゴ</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第５０話　雌雄を決する器用貧乏（１）</t>
+          <t>第６０話　じゃない方の戦いが始まった（１）</t>
         </is>
       </c>
     </row>
@@ -7845,17 +8887,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>島知宏 音速炒飯 有都あらゆる</t>
+          <t>光永康則</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第２２食　ユクシーさんの覚悟、すごいのですわ！（１）</t>
+          <t>第６６話『六花停止』②</t>
         </is>
       </c>
     </row>
@@ -7865,17 +8907,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>異世界メイドの三ツ星グルメ ～現代ごはん作ったら王宮で大バズリしました～</t>
+          <t>塔の管理をしてみよう</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>モリタ Ｕ４ nima</t>
+          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第12話（６）　恋焦がれ！黄金色の実りと、握るはふっくら銀のシャリ（６）</t>
+          <t>第90話後編</t>
         </is>
       </c>
     </row>
@@ -7885,17 +8927,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>濁る瞳で何を願う ハイセルク戦記</t>
+          <t>ラスボス討伐後に始める二周目冒険者ライフ はじまりの街でワケあり美少女たちがめちゃくちゃ懐いてきます</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>トルトネン 創-taro 斎藤八呑</t>
+          <t>鬼麻正明(漫画) 朱月十話(原作) ファルまろ(キャラ原案)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第31話 大暴走</t>
+          <t>第4話-1</t>
         </is>
       </c>
     </row>
@@ -7905,17 +8947,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
+          <t>残念女幹部ブラックジェネラルさん</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>KAKERU</t>
+          <t>jin(著者)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第66話「東アイギス」（前半）</t>
+          <t>第百九十九話</t>
         </is>
       </c>
     </row>
@@ -7925,17 +8967,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ガチャを回して仲間を増やす 最強の美少女軍団を作り上げろ</t>
+          <t>ひとりぼっちの異世界攻略</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>漫画：晴野しゅー 原作：ちんくるり キャラクター原案：イセ川ヤスタカ</t>
+          <t>びび（漫画） 五示正司（原作）</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第71話前半</t>
+          <t>第226話　人ではなくなった…？</t>
         </is>
       </c>
     </row>
@@ -7945,17 +8987,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>いつでも自宅に帰れる俺は、異世界で行商人をはじめました</t>
+          <t>女子高生の無駄づかい</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>漫画／明地雫 原作／霜月緋色 キャラクター原案／いわさきたかし</t>
+          <t>ビーノ(著者)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第58話</t>
+          <t>ばんがいへん</t>
         </is>
       </c>
     </row>
@@ -7965,17 +9007,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>王都ワンオペゴーレムマスター。まさかの追放！？～自由の身になったので弟子の美人勇者たちと一緒に最強ゴーレム作ります。戻ってこいと言われてももう知らん！～@COMIC</t>
+          <t>異世界でスローライフを（願望）</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>阿住 周（漫画） レルクス（原作） 布施龍太（キャラクター原案）</t>
+          <t>長頼（漫画） シゲ（原作） オウカ（キャラクター原案）</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第8話</t>
+          <t>第53話　王都観光</t>
         </is>
       </c>
     </row>
@@ -7985,17 +9027,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>異世界のすみっこで快適ものづくり生活 ～女神さまのくれた工房はちょっとやりすぎ性能だった～</t>
+          <t>煽り系ゲーム配信者（20歳）、配信の切り忘れによりいい人バレする。</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>西山アラタ(漫画) 長田信織(原作) 東上文(キャラクター原案)</t>
+          <t>流嘉（漫画） 夏乃実（原作） 麦うさぎ（キャラクター原案）</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>EP.19①</t>
+          <t>第4話　サブ垢（前編）</t>
         </is>
       </c>
     </row>
@@ -8005,17 +9047,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ポーション頼みで生き延びます！ 続</t>
+          <t>追放者食堂へようこそ！　～最強パーティーを追放された料理人（Lv.99）は、田舎で念願の冒険者食堂を開きます！～</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>原作：FUNA 漫画：園心ふつう キャラクター原案：すきま</t>
+          <t>つむみ（漫画） 君川優樹（原作）</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第63話　長いお別れ Ⅱ</t>
+          <t>第52話　真心XIII（前編）</t>
         </is>
       </c>
     </row>
@@ -8025,17 +9067,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>江戸前エルフ</t>
+          <t>サラリーマンが異世界に行ったら四天王になった話</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>樋口彰彦</t>
+          <t>漫画：村光 原作：ベニガシラ</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>#112</t>
+          <t>第87話　氷の捕食</t>
         </is>
       </c>
     </row>
@@ -8045,17 +9087,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ブチ切れ令嬢は報復を誓いました。 ～魔導書の力で祖国を叩き潰します～</t>
+          <t>ある日、惰眠を貪っていたら一族から追放されて森に捨てられました そのまま寝てたら周りが勝手に魔物の国を作ってたけど、私は気にせず今日も眠ります　コミック版</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>漫画：おおのいも 原作：はぐれメタボ キャラクター原案：昌未</t>
+          <t>漫画/伊草さゆ 原作/白波ハクア キャラクター原案/まさよ</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第47話</t>
+          <t>chapter51【27話①】</t>
         </is>
       </c>
     </row>
@@ -8065,17 +9107,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>創造錬金術師は自由を謳歌する 故郷を追放されたら、魔王のお膝元で超絶効果のマジックアイテム作り放題になりました</t>
+          <t>聖女に嘘は通じない</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>姫乃タカ(漫画) 千月さかき(原作) かぼちゃ(キャラクター原案)</t>
+          <t>日向 夏 浅見よう しんいし智歩</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第19話-2</t>
+          <t>第25話①　あと二日で</t>
         </is>
       </c>
     </row>
@@ -8085,17 +9127,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>クラス最安値で売られた俺は、実は最強パラメーター</t>
+          <t>この素晴らしい世界に祝福を！</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>カンブリア爆発太郎(漫画) RYOMA(原作) 黒井ススム(キャラクター原案)</t>
+          <t>渡真仁(作画) 三嶋くろね(キャラクター原案) 暁なつめ(原作)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第35話-3</t>
+          <t>第129話-2　この偉大なる姉のために名誉回復を！</t>
         </is>
       </c>
     </row>
@@ -8105,17 +9147,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ロメリア戦記～伯爵令嬢、魔王を倒した後も人類やばそうだから軍隊組織する～</t>
+          <t>元最強探索者のおじさん。美少女配信者を助けて大バズりしてしまった。</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>漫画：上戸 亮 原作：有山リョウ(小学館「ガガガブックス」刊) キャラクター原案：コダマ</t>
+          <t>かなたろー(原作) 草壁レイ(漫画)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第13話「助けてくれる人々」②</t>
+          <t>第3話　美少女、おじさんにハメられる。③</t>
         </is>
       </c>
     </row>
@@ -8125,17 +9167,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>孤児院テイマー</t>
+          <t>ガヴリールドロップアウト</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>漫画：倉崎もろこ 原作：安藤正樹 キャラクター原案：イシバシヨウスケ</t>
+          <t>うかみ(著者)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第60話</t>
+          <t>第124話</t>
         </is>
       </c>
     </row>
@@ -8145,17 +9187,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>断れない会長は友江くんにだけしてあげたい</t>
+          <t>序盤で死ぬ最強のサブキャラに転生したので、ゲーム知識で無双する</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>沼地どろまる(著者)</t>
+          <t>作画：マエD 原作：新人</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>コミックス第２巻発売記念！生徒会総選挙！</t>
+          <t>第4話(3)</t>
         </is>
       </c>
     </row>
@@ -8165,17 +9207,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>アレクサンダー英雄戦記～最強の土魔術士～</t>
+          <t>江戸前エルフ</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>マツオカヨシノリ るれくちぇ なんじゃもんじゃ</t>
+          <t>樋口彰彦</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第10話（後編）</t>
+          <t>#113</t>
         </is>
       </c>
     </row>
@@ -8185,17 +9227,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
+          <t>宮廷魔導師、追放される　～無能だと追い出された最巧の魔導師は、部下を引き連れて冒険者クランを始めるようです～</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
+          <t>きつね丸（漫画） しんこせい（原作） ろこ（キャラクター原案）</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第4話-1：師匠と弟子の新生活</t>
+          <t>第1話　宮廷魔導師、追放される</t>
         </is>
       </c>
     </row>
@@ -8205,17 +9247,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>え、テイマーは使えないってパーティから追放したよね？ ～実は世界唯一の【精霊使い】だと判明した途端に手のひらを返されても遅い。精霊の王女様にめちゃくちゃ溺愛されながら、僕はマイペースに最強を目指すので</t>
+          <t>絶対に働きたくないダンジョンマスターが惰眠をむさぼるまで</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>漫画：最中なつめ 原作：茨木野</t>
+          <t>七六（漫画） 鬼影スパナ（原作） よう太（キャラクター原案）</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第30話 特性と代償(後編)</t>
+          <t>第65章　総力戦の行方（前編）</t>
         </is>
       </c>
     </row>
@@ -8225,17 +9267,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>神の庭付き楠木邸</t>
+          <t>ラーメン大好き小泉さん</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>安斎アキラ(著者) えんじゅ(原作) ox(キャラクター原案)</t>
+          <t>鳴見なる</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第32話</t>
+          <t>15杯目 豚野郎</t>
         </is>
       </c>
     </row>
@@ -8245,17 +9287,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>姫様“拷問”の時間です</t>
+          <t>みだりに憑かせてはなりません</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+          <t>栗田あぐり(著者)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>拷問144</t>
+          <t>第8話①</t>
         </is>
       </c>
     </row>
@@ -8265,17 +9307,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Ｒｅ：ゼロから始める異世界生活 第四章 聖域と強欲の魔女</t>
+          <t>勇者パーティを追放された【スキルサポーター】、仲間のスキルを解放して最強に成り上がる</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>花鶏ハルノ(作画) 相川有(構成) 長月達平(原作) 大塚真一郎(キャラクター原案)</t>
+          <t>作画：なかお 原作：前田氏</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第61話①　エリオール大森林の永久凍土</t>
+          <t>第5話(2)</t>
         </is>
       </c>
     </row>
@@ -8285,17 +9327,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>迷宮ブラックカンパニー</t>
+          <t>死ぬ運命にある悪役令嬢の兄に転生したので、妹を育てて未来を変えたいと思います　～世界最強はオレだけど、世界最カワは妹に違いない～</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>安村洋平</t>
+          <t>石見翔子(漫画） 泉里侑希（原作） タムラヨウ（キャラクター原案）</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第50話　落花流水（前編）</t>
+          <t>第3話　新入りメイド・シオン（後編）</t>
         </is>
       </c>
     </row>
@@ -8305,17 +9347,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ジゼルの錬金飴</t>
+          <t>米原くんはつよつよギャルから離れられない</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>漫画： katoson 原作：斯波 キャラクター原案：LINO</t>
+          <t>川村拓(著者)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第8話</t>
+          <t>第14話</t>
         </is>
       </c>
     </row>
@@ -8325,17 +9367,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>いとこのこ</t>
+          <t>悪役一家の奥方、死に戻りして心を入れ替える。</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>いぬちく(著者)</t>
+          <t>鏡(漫画) 丘野優(原作) TEDDY(キャラクター原案)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第35.5話</t>
+          <t>第31話②</t>
         </is>
       </c>
     </row>
@@ -8345,17 +9387,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>追放されたギルド職員は、世界最強の召喚士@COMIC</t>
+          <t>食い詰め傭兵の幻想奇譚</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>原作：月島秀一 漫画：あづち涼 キャラクター原案：チワワ丸</t>
+          <t>原作／まいん キャラクター原案／peroshi 漫画／池宮アレア</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第9話②「伏魔殿ダラスの惨劇」</t>
+          <t>第28話</t>
         </is>
       </c>
     </row>
@@ -8365,17 +9407,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>コボルト無双、モフモフな最弱噛ませ犬だけど世界最強を目指す！</t>
+          <t>ゲーム　オブ　ファミリア-家族戦記-</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>赤志木ひの乃 shiba</t>
+          <t>Ｄ．Ｐ(作画) 山口ミコト(原作)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第十三話 帰還</t>
+          <t>第73話②</t>
         </is>
       </c>
     </row>
@@ -8385,17 +9427,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>少年マールの転生冒険記</t>
+          <t>最強の少年聖騎士、転生者を狩る</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>漫画家：あわや 原作：月ノ宮マクラ キャラクター原案：まっちょこ</t>
+          <t>作画：御塩 原作：宇奈木ユラ</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第17話</t>
+          <t>第5話(2)</t>
         </is>
       </c>
     </row>
@@ -8405,17 +9447,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>無能は不要と言われ『時計使い』の僕は職人ギルドから追い出されるも、ダンジョンの深部で真の力に覚醒する</t>
+          <t>異世界のすみっこで快適ものづくり生活 ～女神さまのくれた工房はちょっとやりすぎ性能だった～</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>漫画：さらさみさ 小説： 桜霧琥珀 キャラ原案： 福きつね</t>
+          <t>西山アラタ(漫画) 長田信織(原作) 東上文(キャラクター原案)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第19話前半</t>
+          <t>EP.19①</t>
         </is>
       </c>
     </row>
@@ -8425,17 +9467,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>魔物ノ森ノ少女ノヴァ</t>
+          <t>ギャルゲーマーに褒められたい</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>kamatama</t>
+          <t>げしゅまろ(著者)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第6話「ロスタイム」後編</t>
+          <t>39話</t>
         </is>
       </c>
     </row>
@@ -8445,17 +9487,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>このヒーラー、めんどくさい</t>
+          <t>初歩魔法しか使わない謎の老魔法使いが旅をする</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>丹念に発酵(著者)</t>
+          <t>山代カゲツ(漫画) やまだのぼる(原作) にじまあるく(キャラクター原案)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第88話：ゴブリンの罠</t>
+          <t>第4話③</t>
         </is>
       </c>
     </row>
@@ -8465,17 +9507,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>安達としまむら</t>
+          <t>二周目チートの転生魔導士～最強が1000年後に転生したら、人生余裕すぎました～</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>柚原もけ(漫画) 入間人間(原作) のん(キャラクターデザイン)</t>
+          <t>石後千鳥 鬱沢色素 りいちゅ</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第48話「最初の旅の端１」①</t>
+          <t>第31話　合同授業（後編）</t>
         </is>
       </c>
     </row>
@@ -8485,17 +9527,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>スキル【万物支配】に目覚めたおっさんは、ダンジョンで生計を立てることにしました～無職から始める支配者無双～</t>
+          <t>オークの酒杯に祝福を</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>岸本和葉 原田 臙 シミズヒロノリ 吉武</t>
+          <t>かなどめはじめ</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第3話　パーティ結成‼</t>
+          <t>第42話　リベンジマッチ</t>
         </is>
       </c>
     </row>
@@ -8505,17 +9547,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>ポンコツスキルしか使えない悪役魔女だけど、テイムしたパリピなスライムたちと強く生きます！</t>
+          <t>ちゃんと吸えない吸血鬼ちゃん</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>漫画：鈴木イゾ 原作：雨傘ヒョウゴ キャラクター原案：朝日川日和</t>
+          <t>二式恭介(著者)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第8話</t>
+          <t>第100話：吸血鬼ちゃんのおまもり④</t>
         </is>
       </c>
     </row>
@@ -8525,17 +9567,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ぽんドロイド！ はまさん</t>
+          <t>数分後の未来が分かるようになったけど、女心は分からない。</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>はれやまはれぞう(著者)</t>
+          <t>You2(漫画) mty(原作)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第3話</t>
+          <t>第10話-1</t>
         </is>
       </c>
     </row>
@@ -8545,17 +9587,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ニャイト・オブ・ザ・リビングキャット</t>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>原作：ホークマン 作画：メカルーツ</t>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Chapter15　ニャンペイジ（後編）</t>
+          <t>第５０話　雌雄を決する器用貧乏（１）</t>
         </is>
       </c>
     </row>
@@ -8565,17 +9607,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>異世界で最強のスキルを生み出せたので、ひたすら無双することにしました。　～俺だけがスキルの数値を勝手に操作～</t>
+          <t>濁る瞳で何を願う ハイセルク戦記</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>漫画：星トマジロウ 原作：ヒゲ抜き地蔵 キャラクター原案：山椒魚</t>
+          <t>トルトネン 創-taro 斎藤八呑</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第9話 ②</t>
+          <t>第31話 大暴走</t>
         </is>
       </c>
     </row>
@@ -8585,17 +9627,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>アラフォーおっさんはスローライフの夢を見るか？</t>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>漫画：大関詠詞 原作：サイトウアユム キャラクター原案： ジョンディー</t>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第14話</t>
+          <t>第２２食　ユクシーさんの覚悟、すごいのですわ！（１）</t>
         </is>
       </c>
     </row>
@@ -8605,17 +9647,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>アイドル辞めるけど結婚してくれますか!?</t>
+          <t>転生したら没落貴族だったので、【呪言】を極めて家族を救います</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>三吉汐美(著者)</t>
+          <t>作画：アマセケイ 原作：メソポ・たみあ</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第16話前半</t>
+          <t>第5話(2)</t>
         </is>
       </c>
     </row>
@@ -8625,17 +9667,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>まったく最近の探偵ときたら</t>
+          <t>二度追放された冒険者、激レアスキル駆使して美少女軍団を育成中！　コミック版</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>五十嵐正邦(著者)</t>
+          <t>漫画/青木千尋 原作/南野雪花</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第113話</t>
+          <t>chapter66【34話①】</t>
         </is>
       </c>
     </row>
@@ -8645,17 +9687,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+          <t>異世界メイドの三ツ星グルメ ～現代ごはん作ったら王宮で大バズリしました～</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+          <t>モリタ Ｕ４ nima</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第3話 前編</t>
+          <t>第12話（６）　恋焦がれ！黄金色の実りと、握るはふっくら銀のシャリ（６）</t>
         </is>
       </c>
     </row>
@@ -8665,17 +9707,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>エンドロールの後には最高の旅を</t>
+          <t>宮廷をクビになった植物魔導師はスローライフを謳歌する～のんびり世界樹を育てたら、最強領地ができました～</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>リキタケ</t>
+          <t>蛙田アメコ 十三木考 又市マタロー</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>最終話 最高の旅を②</t>
+          <t>第22話②フニクリ村</t>
         </is>
       </c>
     </row>
@@ -8685,17 +9727,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>千年英雄</t>
+          <t>最凶貴族は死亡フラグを覆す</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>原作/福島航平 作画/中村ゆきひろ</t>
+          <t>作画：sudekuma 原作：塚上</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>18話①</t>
+          <t>第5話(2)</t>
         </is>
       </c>
     </row>
@@ -8705,17 +9747,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>さんしょく弁当</t>
+          <t>黒幕一家に転生したけど原作無視して独立する</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>兎月あい(著者)</t>
+          <t>空野進 赤村晃人 笠間三四郎 るろお</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第18話#3</t>
+          <t>【単行本発売記念】告知です！</t>
         </is>
       </c>
     </row>
@@ -8725,17 +9767,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>リアデイルの大地にて</t>
+          <t>傷口と包帯</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>月見だしお(著者) Ceez(原作) てんまそ(キャラクター原案) 涼風涼(構成)</t>
+          <t>七井海星</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第39章-2</t>
+          <t>第13.5話 たまには静かに</t>
         </is>
       </c>
     </row>
@@ -8745,17 +9787,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>異世界創造のすゝめ～スマホアプリで惑星を創ってしまった俺は神となり世界を巡る～@COMIC</t>
+          <t>転生悪魔の最強勇者育成計画</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>漫画：岩戸あきら 原作：たまごかけキャンディー キャラクター原案：かれい</t>
+          <t>瀬川 竜（漫画） たまごかけキャンディー（原作） 長浜めぐみ（原作イラスト）</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第11話 ①</t>
+          <t>第10話　勇気の灯火（後編）</t>
         </is>
       </c>
     </row>
@@ -8765,17 +9807,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>王子様の友達</t>
+          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>すけろく(著者)</t>
+          <t>KAKERU</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第28話</t>
+          <t>第66話「東アイギス」（前半）</t>
         </is>
       </c>
     </row>
@@ -8785,17 +9827,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>クソ女に幸あれ</t>
+          <t>ぽんドロイド！ はまさん</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>岸川瑞樹</t>
+          <t>はれやまはれぞう(著者)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第59話</t>
+          <t>第3話</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-07-10
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -24,6 +24,7 @@
     <sheet name="2025-07-07" sheetId="16" state="visible" r:id="rId16"/>
     <sheet name="2025-07-08" sheetId="17" state="visible" r:id="rId17"/>
     <sheet name="2025-07-09" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="2025-07-10" sheetId="19" state="visible" r:id="rId19"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -8842,22 +8843,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第30話：一秒の奪い合い②</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>マツモトケンゴ</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第６０話　じゃない方の戦いが始まった（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第６６話『六花停止』②</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>塔の管理をしてみよう</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第90話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>ラスボス討伐後に始める二周目冒険者ライフ はじまりの街でワケあり美少女たちがめちゃくちゃ懐いてきます</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>鬼麻正明(漫画) 朱月十話(原作) ファルまろ(キャラ原案)</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第4話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>残念女幹部ブラックジェネラルさん</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>jin(著者)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第百九十九話</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>ひとりぼっちの異世界攻略</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>びび（漫画） 五示正司（原作）</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第226話　人ではなくなった…？</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>女子高生の無駄づかい</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>ビーノ(著者)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>ばんがいへん</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>異世界でスローライフを（願望）</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>長頼（漫画） シゲ（原作） オウカ（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第53話　王都観光</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>煽り系ゲーム配信者（20歳）、配信の切り忘れによりいい人バレする。</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>流嘉（漫画） 夏乃実（原作） 麦うさぎ（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第4話　サブ垢（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>追放者食堂へようこそ！　～最強パーティーを追放された料理人（Lv.99）は、田舎で念願の冒険者食堂を開きます！～</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>つむみ（漫画） 君川優樹（原作）</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第52話　真心XIII（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>サラリーマンが異世界に行ったら四天王になった話</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>漫画：村光 原作：ベニガシラ</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第87話　氷の捕食</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>ある日、惰眠を貪っていたら一族から追放されて森に捨てられました そのまま寝てたら周りが勝手に魔物の国を作ってたけど、私は気にせず今日も眠ります　コミック版</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>漫画/伊草さゆ 原作/白波ハクア キャラクター原案/まさよ</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>chapter51【27話①】</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>聖女に嘘は通じない</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>日向 夏 浅見よう しんいし智歩</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第25話①　あと二日で</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>この素晴らしい世界に祝福を！</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>渡真仁(作画) 三嶋くろね(キャラクター原案) 暁なつめ(原作)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第129話-2　この偉大なる姉のために名誉回復を！</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>元最強探索者のおじさん。美少女配信者を助けて大バズりしてしまった。</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>かなたろー(原作) 草壁レイ(漫画)</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第3話　美少女、おじさんにハメられる。③</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>ガヴリールドロップアウト</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>うかみ(著者)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第124話</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>序盤で死ぬ最強のサブキャラに転生したので、ゲーム知識で無双する</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>作画：マエD 原作：新人</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第4話(3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>江戸前エルフ</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>樋口彰彦</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>#113</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>宮廷魔導師、追放される　～無能だと追い出された最巧の魔導師は、部下を引き連れて冒険者クランを始めるようです～</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>きつね丸（漫画） しんこせい（原作） ろこ（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第1話　宮廷魔導師、追放される</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>絶対に働きたくないダンジョンマスターが惰眠をむさぼるまで</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>七六（漫画） 鬼影スパナ（原作） よう太（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第65章　総力戦の行方（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>ラーメン大好き小泉さん</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>鳴見なる</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>15杯目 豚野郎</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>みだりに憑かせてはなりません</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>栗田あぐり(著者)</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第8話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追放された【スキルサポーター】、仲間のスキルを解放して最強に成り上がる</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>作画：なかお 原作：前田氏</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第5話(2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>死ぬ運命にある悪役令嬢の兄に転生したので、妹を育てて未来を変えたいと思います　～世界最強はオレだけど、世界最カワは妹に違いない～</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>石見翔子(漫画） 泉里侑希（原作） タムラヨウ（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第3話　新入りメイド・シオン（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>米原くんはつよつよギャルから離れられない</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>川村拓(著者)</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第14話</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>悪役一家の奥方、死に戻りして心を入れ替える。</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>鏡(漫画) 丘野優(原作) TEDDY(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第31話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>食い詰め傭兵の幻想奇譚</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>原作／まいん キャラクター原案／peroshi 漫画／池宮アレア</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第28話</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>ゲーム　オブ　ファミリア-家族戦記-</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>Ｄ．Ｐ(作画) 山口ミコト(原作)</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第73話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>最強の少年聖騎士、転生者を狩る</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>作画：御塩 原作：宇奈木ユラ</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第5話(2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>異世界のすみっこで快適ものづくり生活 ～女神さまのくれた工房はちょっとやりすぎ性能だった～</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>西山アラタ(漫画) 長田信織(原作) 東上文(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>EP.19①</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>ギャルゲーマーに褒められたい</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>げしゅまろ(著者)</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>39話</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>初歩魔法しか使わない謎の老魔法使いが旅をする</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>山代カゲツ(漫画) やまだのぼる(原作) にじまあるく(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第4話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>二周目チートの転生魔導士～最強が1000年後に転生したら、人生余裕すぎました～</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>石後千鳥 鬱沢色素 りいちゅ</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第31話　合同授業（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>オークの酒杯に祝福を</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>かなどめはじめ</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第42話　リベンジマッチ</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>ちゃんと吸えない吸血鬼ちゃん</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>二式恭介(著者)</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第100話：吸血鬼ちゃんのおまもり④</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>数分後の未来が分かるようになったけど、女心は分からない。</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>You2(漫画) mty(原作)</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第10話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第５０話　雌雄を決する器用貧乏（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>濁る瞳で何を願う ハイセルク戦記</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>トルトネン 創-taro 斎藤八呑</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第31話 大暴走</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第２２食　ユクシーさんの覚悟、すごいのですわ！（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>転生したら没落貴族だったので、【呪言】を極めて家族を救います</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>作画：アマセケイ 原作：メソポ・たみあ</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第5話(2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>二度追放された冒険者、激レアスキル駆使して美少女軍団を育成中！　コミック版</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>漫画/青木千尋 原作/南野雪花</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>chapter66【34話①】</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>異世界メイドの三ツ星グルメ ～現代ごはん作ったら王宮で大バズリしました～</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>モリタ Ｕ４ nima</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第12話（６）　恋焦がれ！黄金色の実りと、握るはふっくら銀のシャリ（６）</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>宮廷をクビになった植物魔導師はスローライフを謳歌する～のんびり世界樹を育てたら、最強領地ができました～</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>蛙田アメコ 十三木考 又市マタロー</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第22話②フニクリ村</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>最凶貴族は死亡フラグを覆す</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>作画：sudekuma 原作：塚上</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第5話(2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>黒幕一家に転生したけど原作無視して独立する</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>空野進 赤村晃人 笠間三四郎 るろお</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>【単行本発売記念】告知です！</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>傷口と包帯</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>七井海星</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第13.5話 たまには静かに</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>転生悪魔の最強勇者育成計画</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>瀬川 竜（漫画） たまごかけキャンディー（原作） 長浜めぐみ（原作イラスト）</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第10話　勇気の灯火（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>KAKERU</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第66話「東アイギス」（前半）</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>ぽんドロイド！ はまさん</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>はれやまはれぞう(著者)</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第3話</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>zunta(作画) はらわたさいぞう(原作)</t>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第30話：一秒の奪い合い②</t>
+          <t>第33話②</t>
         </is>
       </c>
     </row>
@@ -8867,17 +9909,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>マツモトケンゴ</t>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第６０話　じゃない方の戦いが始まった（１）</t>
+          <t>第9話-1</t>
         </is>
       </c>
     </row>
@@ -8887,17 +9929,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+          <t>実は俺、最強でした？</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>光永康則</t>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第６６話『六花停止』②</t>
+          <t>第120話　四騎戦決勝戦!!・後編</t>
         </is>
       </c>
     </row>
@@ -8907,17 +9949,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>塔の管理をしてみよう</t>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第90話後編</t>
+          <t>第126話　戦争を終わらせてみるⅡ（中編）</t>
         </is>
       </c>
     </row>
@@ -8927,17 +9969,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ラスボス討伐後に始める二周目冒険者ライフ はじまりの街でワケあり美少女たちがめちゃくちゃ懐いてきます</t>
+          <t>アザミヤコを好きになる</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>鬼麻正明(漫画) 朱月十話(原作) ファルまろ(キャラ原案)</t>
+          <t>ユニティコング(原作) ツノニガウ(作画)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第4話-1</t>
+          <t>第8話</t>
         </is>
       </c>
     </row>
@@ -8947,17 +9989,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>残念女幹部ブラックジェネラルさん</t>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>jin(著者)</t>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第百九十九話</t>
+          <t>第31話 独身貴族はヒラメが大事（4）</t>
         </is>
       </c>
     </row>
@@ -8967,17 +10009,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ひとりぼっちの異世界攻略</t>
+          <t>黒幕一家に転生したけど原作無視して独立する</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>びび（漫画） 五示正司（原作）</t>
+          <t>空野進 赤村晃人 笠間三四郎 るろお</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第226話　人ではなくなった…？</t>
+          <t>【単行本発売記念】告知です！</t>
         </is>
       </c>
     </row>
@@ -8987,17 +10029,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>女子高生の無駄づかい</t>
+          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ビーノ(著者)</t>
+          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>ばんがいへん</t>
+          <t>重版決定記念イラスト</t>
         </is>
       </c>
     </row>
@@ -9007,17 +10049,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>異世界でスローライフを（願望）</t>
+          <t>隣の席のヤンキー清水さんが髪を黒く染めてきた</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>長頼（漫画） シゲ（原作） オウカ（キャラクター原案）</t>
+          <t>底花(原作) 真田若楓(漫画) ハム(キャラクター原案)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第53話　王都観光</t>
+          <t>第10話-1</t>
         </is>
       </c>
     </row>
@@ -9027,17 +10069,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>煽り系ゲーム配信者（20歳）、配信の切り忘れによりいい人バレする。</t>
+          <t>ダンジョン・シェルパ　迷宮道先案内人</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>流嘉（漫画） 夏乃実（原作） 麦うさぎ（キャラクター原案）</t>
+          <t>原作/加茂セイ 漫画/刀坂アキラ</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第4話　サブ垢（前編）</t>
+          <t>潜行：59(後編)</t>
         </is>
       </c>
     </row>
@@ -9047,17 +10089,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>追放者食堂へようこそ！　～最強パーティーを追放された料理人（Lv.99）は、田舎で念願の冒険者食堂を開きます！～</t>
+          <t>すだちの魔王城</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>つむみ（漫画） 君川優樹（原作）</t>
+          <t>森下真</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第52話　真心XIII（前編）</t>
+          <t>第44話　渡る鴉の縁結び（前編）</t>
         </is>
       </c>
     </row>
@@ -9067,17 +10109,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>サラリーマンが異世界に行ったら四天王になった話</t>
+          <t>オタクに優しいギャルはいない!?</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>漫画：村光 原作：ベニガシラ</t>
+          <t>のりしろちゃん 魚住さかな</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第87話　氷の捕食</t>
+          <t>【#147】ある春の日</t>
         </is>
       </c>
     </row>
@@ -9087,17 +10129,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ある日、惰眠を貪っていたら一族から追放されて森に捨てられました そのまま寝てたら周りが勝手に魔物の国を作ってたけど、私は気にせず今日も眠ります　コミック版</t>
+          <t>29歳独身は異世界で自由に生きた……かった。</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>漫画/伊草さゆ 原作/白波ハクア キャラクター原案/まさよ</t>
+          <t>オオハマイコ(漫画) リュート(原作) 桑島黎音(キャラクター原案)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>chapter51【27話①】</t>
+          <t>第40話-4①</t>
         </is>
       </c>
     </row>
@@ -9107,17 +10149,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>聖女に嘘は通じない</t>
+          <t>スキル【万物支配】に目覚めたおっさんは、ダンジョンで生計を立てることにしました～無職から始める支配者無双～</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>日向 夏 浅見よう しんいし智歩</t>
+          <t>岸本和葉 原田 臙 シミズヒロノリ 吉武</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第25話①　あと二日で</t>
+          <t>第4話　穴熊商店(前編)</t>
         </is>
       </c>
     </row>
@@ -9127,17 +10169,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>この素晴らしい世界に祝福を！</t>
+          <t>ポンコツ風紀委員とスカート丈が不適切なＪＫの話</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>渡真仁(作画) 三嶋くろね(キャラクター原案) 暁なつめ(原作)</t>
+          <t>横田卓馬</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第129話-2　この偉大なる姉のために名誉回復を！</t>
+          <t>第90話　ポンコツ保健委員と図書委員が動き出す話</t>
         </is>
       </c>
     </row>
@@ -9147,17 +10189,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>元最強探索者のおじさん。美少女配信者を助けて大バズりしてしまった。</t>
+          <t>生徒会役員共</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>かなたろー(原作) 草壁レイ(漫画)</t>
+          <t>氏家ト全</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第3話　美少女、おじさんにハメられる。③</t>
+          <t>#404</t>
         </is>
       </c>
     </row>
@@ -9167,17 +10209,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ガヴリールドロップアウト</t>
+          <t>カナン様はあくまでチョロい</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>うかみ(著者)</t>
+          <t>nonco</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第124話</t>
+          <t>第141話	カナンの寒暖差デレ</t>
         </is>
       </c>
     </row>
@@ -9187,17 +10229,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>序盤で死ぬ最強のサブキャラに転生したので、ゲーム知識で無双する</t>
+          <t>田舎のホームセンター男の自由な異世界生活</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>作画：マエD 原作：新人</t>
+          <t>うさぴょん(原作) 古来歩(漫画) 市丸きすけ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第4話(3)</t>
+          <t>第75話その2</t>
         </is>
       </c>
     </row>
@@ -9207,17 +10249,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>江戸前エルフ</t>
+          <t>姫騎士は蛮族の嫁</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>樋口彰彦</t>
+          <t>コトバノリアキ</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>#113</t>
+          <t>第52話① 浮船は未見の故郷</t>
         </is>
       </c>
     </row>
@@ -9227,17 +10269,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>宮廷魔導師、追放される　～無能だと追い出された最巧の魔導師は、部下を引き連れて冒険者クランを始めるようです～</t>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>きつね丸（漫画） しんこせい（原作） ろこ（キャラクター原案）</t>
+          <t>マツモトケンゴ</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第1話　宮廷魔導師、追放される</t>
+          <t>第６０話　じゃない方の戦いが始まった（１）</t>
         </is>
       </c>
     </row>
@@ -9247,17 +10289,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>絶対に働きたくないダンジョンマスターが惰眠をむさぼるまで</t>
+          <t>すべての人類を破壊する。それらは再生できない。</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>七六（漫画） 鬼影スパナ（原作） よう太（キャラクター原案）</t>
+          <t>横田卓馬(漫画) 伊瀬勝良(原作)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第65章　総力戦の行方（前編）</t>
+          <t>第66話その2</t>
         </is>
       </c>
     </row>
@@ -9267,17 +10309,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ラーメン大好き小泉さん</t>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>鳴見なる</t>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>15杯目 豚野郎</t>
+          <t>第30話：一秒の奪い合い②</t>
         </is>
       </c>
     </row>
@@ -9287,17 +10329,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>みだりに憑かせてはなりません</t>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>栗田あぐり(著者)</t>
+          <t>光永康則</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第8話①</t>
+          <t>第６６話『六花停止』②</t>
         </is>
       </c>
     </row>
@@ -9307,17 +10349,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>勇者パーティを追放された【スキルサポーター】、仲間のスキルを解放して最強に成り上がる</t>
+          <t>転生錬金少女のスローライフ</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>作画：なかお 原作：前田氏</t>
+          <t>里町(漫画) 夜想庭園(原作) potg(キャラクター原案)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第5話(2)</t>
+          <t>第16話-2</t>
         </is>
       </c>
     </row>
@@ -9327,17 +10369,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>死ぬ運命にある悪役令嬢の兄に転生したので、妹を育てて未来を変えたいと思います　～世界最強はオレだけど、世界最カワは妹に違いない～</t>
+          <t>よわよわ先生</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>石見翔子(漫画） 泉里侑希（原作） タムラヨウ（キャラクター原案）</t>
+          <t>福地カミオ</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第3話　新入りメイド・シオン（後編）</t>
+          <t>第106話	もじもじの特訓</t>
         </is>
       </c>
     </row>
@@ -9347,17 +10389,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>米原くんはつよつよギャルから離れられない</t>
+          <t>チート薬師のスローライフ ～異世界に作ろうドラッグストア～</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>川村拓(著者)</t>
+          <t>ケンノジ 春乃えり</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第14話</t>
+          <t>67本目　気持ちを形に[前半]</t>
         </is>
       </c>
     </row>
@@ -9367,17 +10409,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>悪役一家の奥方、死に戻りして心を入れ替える。</t>
+          <t>異世界チート魔術師</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>鏡(漫画) 丘野優(原作) TEDDY(キャラクター原案)</t>
+          <t>内田健（ヒーロー文庫／イマジカインフォス）(原作) 鈴羅木かりん(漫画) Ｎａｒｄａｃｋ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第31話②</t>
+          <t>第92話-1</t>
         </is>
       </c>
     </row>
@@ -9387,17 +10429,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>食い詰め傭兵の幻想奇譚</t>
+          <t>百瀬アキラの初恋破綻中。</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>原作／まいん キャラクター原案／peroshi 漫画／池宮アレア</t>
+          <t>晴川シンタ</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第28話</t>
+          <t>第30話 辿り着いた、暗中。</t>
         </is>
       </c>
     </row>
@@ -9407,17 +10449,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ゲーム　オブ　ファミリア-家族戦記-</t>
+          <t>勇者パーティーの荷物持ち</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Ｄ．Ｐ(作画) 山口ミコト(原作)</t>
+          <t>原作：河本ほむら／作画：八嶋諒</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第73話②</t>
+          <t>第24話 荷物持ちと勇者パーティーの魔法使い①</t>
         </is>
       </c>
     </row>
@@ -9427,17 +10469,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>最強の少年聖騎士、転生者を狩る</t>
+          <t>303号室の神さま</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>作画：御塩 原作：宇奈木ユラ</t>
+          <t>ふに・無9(著者)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第5話(2)</t>
+          <t>Episode. 18</t>
         </is>
       </c>
     </row>
@@ -9447,17 +10489,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>異世界のすみっこで快適ものづくり生活 ～女神さまのくれた工房はちょっとやりすぎ性能だった～</t>
+          <t>H村へようこそ！</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>西山アラタ(漫画) 長田信織(原作) 東上文(キャラクター原案)</t>
+          <t>額縁あいこ(著者)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>EP.19①</t>
+          <t>第11話</t>
         </is>
       </c>
     </row>
@@ -9467,17 +10509,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ギャルゲーマーに褒められたい</t>
+          <t>我が焔炎にひれ伏せ世界</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>げしゅまろ(著者)</t>
+          <t>すめらぎひよこ(原作) こゆき(作画) Mika Pikazo(キャラクター原案) mocha(背景画)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>39話</t>
+          <t>コミックス告知</t>
         </is>
       </c>
     </row>
@@ -9487,17 +10529,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>初歩魔法しか使わない謎の老魔法使いが旅をする</t>
+          <t>ジェノヴァの弟子～10秒しか戦えない魔術師、のちの『魔王』を育てる～</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>山代カゲツ(漫画) やまだのぼる(原作) にじまあるく(キャラクター原案)</t>
+          <t>原作：妹尾尻尾 漫画：魚塚じゃこ キャラクター原案：赤嶺直樹</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第4話③</t>
+          <t>第21話</t>
         </is>
       </c>
     </row>
@@ -9507,17 +10549,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>二周目チートの転生魔導士～最強が1000年後に転生したら、人生余裕すぎました～</t>
+          <t>シャドウ・アサシンズ・ワールド ～影は薄いけど、最強忍者やってます～</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>石後千鳥 鬱沢色素 りいちゅ</t>
+          <t>空山トキ 五色安未 泉乃せん 伍長</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第31話　合同授業（後編）</t>
+          <t>第10話　少女と本当の自分１（2）</t>
         </is>
       </c>
     </row>
@@ -9527,17 +10569,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>オークの酒杯に祝福を</t>
+          <t>ラスボス討伐後に始める二周目冒険者ライフ はじまりの街でワケあり美少女たちがめちゃくちゃ懐いてきます</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>かなどめはじめ</t>
+          <t>鬼麻正明(漫画) 朱月十話(原作) ファルまろ(キャラ原案)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第42話　リベンジマッチ</t>
+          <t>第4話-1</t>
         </is>
       </c>
     </row>
@@ -9547,17 +10589,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>ちゃんと吸えない吸血鬼ちゃん</t>
+          <t>女子高生の無駄づかい</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>二式恭介(著者)</t>
+          <t>ビーノ(著者)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第100話：吸血鬼ちゃんのおまもり④</t>
+          <t>ばんがいへん</t>
         </is>
       </c>
     </row>
@@ -9567,17 +10609,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>数分後の未来が分かるようになったけど、女心は分からない。</t>
+          <t>葉木莉さんは君だけの死神になりたい</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>You2(漫画) mty(原作)</t>
+          <t>３５まち</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第10話-1</t>
+          <t>第５話　葉木莉さん相手だ――間違っても間違いなんて起きないけど</t>
         </is>
       </c>
     </row>
@@ -9587,17 +10629,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+          <t>人生逆転ダンジョン</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+          <t>尾張 ニコ どすこい花丸様</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第５０話　雌雄を決する器用貧乏（１）</t>
+          <t>第3-1話	穴は使いよう</t>
         </is>
       </c>
     </row>
@@ -9607,17 +10649,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>濁る瞳で何を願う ハイセルク戦記</t>
+          <t>塔の管理をしてみよう</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>トルトネン 創-taro 斎藤八呑</t>
+          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第31話 大暴走</t>
+          <t>第90話後編</t>
         </is>
       </c>
     </row>
@@ -9627,17 +10669,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+          <t>残念女幹部ブラックジェネラルさん</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>島知宏 音速炒飯 有都あらゆる</t>
+          <t>jin(著者)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第２２食　ユクシーさんの覚悟、すごいのですわ！（１）</t>
+          <t>第百九十九話</t>
         </is>
       </c>
     </row>
@@ -9647,17 +10689,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>転生したら没落貴族だったので、【呪言】を極めて家族を救います</t>
+          <t>煽り系ゲーム配信者（20歳）、配信の切り忘れによりいい人バレする。</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>作画：アマセケイ 原作：メソポ・たみあ</t>
+          <t>流嘉（漫画） 夏乃実（原作） 麦うさぎ（キャラクター原案）</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第5話(2)</t>
+          <t>第4話　サブ垢（前編）</t>
         </is>
       </c>
     </row>
@@ -9667,17 +10709,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>二度追放された冒険者、激レアスキル駆使して美少女軍団を育成中！　コミック版</t>
+          <t>ひとりぼっちの異世界攻略</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>漫画/青木千尋 原作/南野雪花</t>
+          <t>びび（漫画） 五示正司（原作）</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>chapter66【34話①】</t>
+          <t>第226話　人ではなくなった…？</t>
         </is>
       </c>
     </row>
@@ -9687,17 +10729,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>異世界メイドの三ツ星グルメ ～現代ごはん作ったら王宮で大バズリしました～</t>
+          <t>異世界でスローライフを（願望）</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>モリタ Ｕ４ nima</t>
+          <t>長頼（漫画） シゲ（原作） オウカ（キャラクター原案）</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第12話（６）　恋焦がれ！黄金色の実りと、握るはふっくら銀のシャリ（６）</t>
+          <t>第53話　王都観光</t>
         </is>
       </c>
     </row>
@@ -9707,17 +10749,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>宮廷をクビになった植物魔導師はスローライフを謳歌する～のんびり世界樹を育てたら、最強領地ができました～</t>
+          <t>シルバーマウンテン</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>蛙田アメコ 十三木考 又市マタロー</t>
+          <t>藤田 和日郎</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第22話②フニクリ村</t>
+          <t>5．第一章「仙境＜螺界＞」 其ノ四 腰痛の竜</t>
         </is>
       </c>
     </row>
@@ -9727,17 +10769,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>最凶貴族は死亡フラグを覆す</t>
+          <t>アンゴルモア 元寇合戦記　【博多編】</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>作画：sudekuma 原作：塚上</t>
+          <t>たかぎ七彦(著者)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第5話(2)</t>
+          <t>第四十四話その四</t>
         </is>
       </c>
     </row>
@@ -9747,17 +10789,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>黒幕一家に転生したけど原作無視して独立する</t>
+          <t>終焉の魔女と世界の旅</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>空野進 赤村晃人 笠間三四郎 るろお</t>
+          <t>片岡とんち</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>【単行本発売記念】告知です！</t>
+          <t>第13話①	終焉の魔女と魔王メリア</t>
         </is>
       </c>
     </row>
@@ -9767,17 +10809,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>傷口と包帯</t>
+          <t>序盤で死ぬ最強のサブキャラに転生したので、ゲーム知識で無双する</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>七井海星</t>
+          <t>作画：マエD 原作：新人</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第13.5話 たまには静かに</t>
+          <t>第4話(3)</t>
         </is>
       </c>
     </row>
@@ -9787,17 +10829,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>転生悪魔の最強勇者育成計画</t>
+          <t>追放者食堂へようこそ！　～最強パーティーを追放された料理人（Lv.99）は、田舎で念願の冒険者食堂を開きます！～</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>瀬川 竜（漫画） たまごかけキャンディー（原作） 長浜めぐみ（原作イラスト）</t>
+          <t>つむみ（漫画） 君川優樹（原作）</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第10話　勇気の灯火（後編）</t>
+          <t>第52話　真心XIII（前編）</t>
         </is>
       </c>
     </row>
@@ -9807,17 +10849,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
+          <t>サラリーマンが異世界に行ったら四天王になった話</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>KAKERU</t>
+          <t>漫画：村光 原作：ベニガシラ</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第66話「東アイギス」（前半）</t>
+          <t>第87話　氷の捕食</t>
         </is>
       </c>
     </row>
@@ -9827,17 +10869,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>ぽんドロイド！ はまさん</t>
+          <t>この素晴らしい世界に祝福を！</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>はれやまはれぞう(著者)</t>
+          <t>渡真仁(作画) 三嶋くろね(キャラクター原案) 暁なつめ(原作)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第3話</t>
+          <t>第129話-2　この偉大なる姉のために名誉回復を！</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-07-11
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -25,6 +25,7 @@
     <sheet name="2025-07-08" sheetId="17" state="visible" r:id="rId17"/>
     <sheet name="2025-07-09" sheetId="18" state="visible" r:id="rId18"/>
     <sheet name="2025-07-10" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="2025-07-11" sheetId="20" state="visible" r:id="rId20"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -9884,1000 +9885,1000 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="0" t="inlineStr">
         <is>
           <t>クラスで２番目に可愛い女の子と友だちになった</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="0" t="inlineStr">
         <is>
           <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="0" t="inlineStr">
         <is>
           <t>第33話②</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="0" t="inlineStr">
         <is>
           <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="0" t="inlineStr">
         <is>
           <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" s="0" t="inlineStr">
         <is>
           <t>第9話-1</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="0" t="inlineStr">
         <is>
           <t>実は俺、最強でした？</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="0" t="inlineStr">
         <is>
           <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" s="0" t="inlineStr">
         <is>
           <t>第120話　四騎戦決勝戦!!・後編</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="0" t="inlineStr">
         <is>
           <t>異世界魔王と召喚少女の奴隷魔術</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="0" t="inlineStr">
         <is>
           <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D5" s="0" t="inlineStr">
         <is>
           <t>第126話　戦争を終わらせてみるⅡ（中編）</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="0" t="inlineStr">
         <is>
           <t>アザミヤコを好きになる</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" s="0" t="inlineStr">
         <is>
           <t>ユニティコング(原作) ツノニガウ(作画)</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D6" s="0" t="inlineStr">
         <is>
           <t>第8話</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="0" t="inlineStr">
         <is>
           <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="0" t="inlineStr">
         <is>
           <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D7" s="0" t="inlineStr">
         <is>
           <t>第31話 独身貴族はヒラメが大事（4）</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" s="0" t="inlineStr">
         <is>
           <t>黒幕一家に転生したけど原作無視して独立する</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" s="0" t="inlineStr">
         <is>
           <t>空野進 赤村晃人 笠間三四郎 るろお</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D8" s="0" t="inlineStr">
         <is>
           <t>【単行本発売記念】告知です！</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="0" t="inlineStr">
         <is>
           <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" s="0" t="inlineStr">
         <is>
           <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D9" s="0" t="inlineStr">
         <is>
           <t>重版決定記念イラスト</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" s="0" t="inlineStr">
         <is>
           <t>隣の席のヤンキー清水さんが髪を黒く染めてきた</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" s="0" t="inlineStr">
         <is>
           <t>底花(原作) 真田若楓(漫画) ハム(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D10" s="0" t="inlineStr">
         <is>
           <t>第10話-1</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" s="0" t="inlineStr">
         <is>
           <t>ダンジョン・シェルパ　迷宮道先案内人</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" s="0" t="inlineStr">
         <is>
           <t>原作/加茂セイ 漫画/刀坂アキラ</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D11" s="0" t="inlineStr">
         <is>
           <t>潜行：59(後編)</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
+      <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" s="0" t="inlineStr">
         <is>
           <t>すだちの魔王城</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" s="0" t="inlineStr">
         <is>
           <t>森下真</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D12" s="0" t="inlineStr">
         <is>
           <t>第44話　渡る鴉の縁結び（前編）</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
+      <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" s="0" t="inlineStr">
         <is>
           <t>オタクに優しいギャルはいない!?</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" s="0" t="inlineStr">
         <is>
           <t>のりしろちゃん 魚住さかな</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D13" s="0" t="inlineStr">
         <is>
           <t>【#147】ある春の日</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
+      <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B14" s="0" t="inlineStr">
         <is>
           <t>29歳独身は異世界で自由に生きた……かった。</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C14" s="0" t="inlineStr">
         <is>
           <t>オオハマイコ(漫画) リュート(原作) 桑島黎音(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D14" s="0" t="inlineStr">
         <is>
           <t>第40話-4①</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
+      <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B15" s="0" t="inlineStr">
         <is>
           <t>スキル【万物支配】に目覚めたおっさんは、ダンジョンで生計を立てることにしました～無職から始める支配者無双～</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C15" s="0" t="inlineStr">
         <is>
           <t>岸本和葉 原田 臙 シミズヒロノリ 吉武</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D15" s="0" t="inlineStr">
         <is>
           <t>第4話　穴熊商店(前編)</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
+      <c r="A16" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B16" s="0" t="inlineStr">
         <is>
           <t>ポンコツ風紀委員とスカート丈が不適切なＪＫの話</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C16" s="0" t="inlineStr">
         <is>
           <t>横田卓馬</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="D16" s="0" t="inlineStr">
         <is>
           <t>第90話　ポンコツ保健委員と図書委員が動き出す話</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
+      <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B17" s="0" t="inlineStr">
         <is>
           <t>生徒会役員共</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C17" s="0" t="inlineStr">
         <is>
           <t>氏家ト全</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="D17" s="0" t="inlineStr">
         <is>
           <t>#404</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
+      <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B18" s="0" t="inlineStr">
         <is>
           <t>カナン様はあくまでチョロい</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C18" s="0" t="inlineStr">
         <is>
           <t>nonco</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="D18" s="0" t="inlineStr">
         <is>
           <t>第141話	カナンの寒暖差デレ</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
+      <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B19" s="0" t="inlineStr">
         <is>
           <t>田舎のホームセンター男の自由な異世界生活</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C19" s="0" t="inlineStr">
         <is>
           <t>うさぴょん(原作) 古来歩(漫画) 市丸きすけ(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="D19" s="0" t="inlineStr">
         <is>
           <t>第75話その2</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
+      <c r="A20" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B20" s="0" t="inlineStr">
         <is>
           <t>姫騎士は蛮族の嫁</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C20" s="0" t="inlineStr">
         <is>
           <t>コトバノリアキ</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="D20" s="0" t="inlineStr">
         <is>
           <t>第52話① 浮船は未見の故郷</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
+      <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B21" s="0" t="inlineStr">
         <is>
           <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C21" s="0" t="inlineStr">
         <is>
           <t>マツモトケンゴ</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="D21" s="0" t="inlineStr">
         <is>
           <t>第６０話　じゃない方の戦いが始まった（１）</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
+      <c r="A22" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B22" s="0" t="inlineStr">
         <is>
           <t>すべての人類を破壊する。それらは再生できない。</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C22" s="0" t="inlineStr">
         <is>
           <t>横田卓馬(漫画) 伊瀬勝良(原作)</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="D22" s="0" t="inlineStr">
         <is>
           <t>第66話その2</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="n">
+      <c r="A23" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B23" s="0" t="inlineStr">
         <is>
           <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C23" s="0" t="inlineStr">
         <is>
           <t>zunta(作画) はらわたさいぞう(原作)</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="D23" s="0" t="inlineStr">
         <is>
           <t>第30話：一秒の奪い合い②</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="n">
+      <c r="A24" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B24" s="0" t="inlineStr">
         <is>
           <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="C24" s="0" t="inlineStr">
         <is>
           <t>光永康則</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="D24" s="0" t="inlineStr">
         <is>
           <t>第６６話『六花停止』②</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="n">
+      <c r="A25" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="B25" s="0" t="inlineStr">
         <is>
           <t>転生錬金少女のスローライフ</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C25" s="0" t="inlineStr">
         <is>
           <t>里町(漫画) 夜想庭園(原作) potg(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="D25" s="0" t="inlineStr">
         <is>
           <t>第16話-2</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="n">
+      <c r="A26" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="B26" s="0" t="inlineStr">
         <is>
           <t>よわよわ先生</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="C26" s="0" t="inlineStr">
         <is>
           <t>福地カミオ</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="D26" s="0" t="inlineStr">
         <is>
           <t>第106話	もじもじの特訓</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="n">
+      <c r="A27" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="B27" s="0" t="inlineStr">
         <is>
           <t>チート薬師のスローライフ ～異世界に作ろうドラッグストア～</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="C27" s="0" t="inlineStr">
         <is>
           <t>ケンノジ 春乃えり</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="D27" s="0" t="inlineStr">
         <is>
           <t>67本目　気持ちを形に[前半]</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="n">
+      <c r="A28" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B28" s="0" t="inlineStr">
         <is>
           <t>異世界チート魔術師</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C28" s="0" t="inlineStr">
         <is>
           <t>内田健（ヒーロー文庫／イマジカインフォス）(原作) 鈴羅木かりん(漫画) Ｎａｒｄａｃｋ(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="D28" s="0" t="inlineStr">
         <is>
           <t>第92話-1</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="n">
+      <c r="A29" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="B29" s="0" t="inlineStr">
         <is>
           <t>百瀬アキラの初恋破綻中。</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="C29" s="0" t="inlineStr">
         <is>
           <t>晴川シンタ</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="D29" s="0" t="inlineStr">
         <is>
           <t>第30話 辿り着いた、暗中。</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="n">
+      <c r="A30" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="B30" s="0" t="inlineStr">
         <is>
           <t>勇者パーティーの荷物持ち</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="C30" s="0" t="inlineStr">
         <is>
           <t>原作：河本ほむら／作画：八嶋諒</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="D30" s="0" t="inlineStr">
         <is>
           <t>第24話 荷物持ちと勇者パーティーの魔法使い①</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="n">
+      <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="B31" s="0" t="inlineStr">
         <is>
           <t>303号室の神さま</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="C31" s="0" t="inlineStr">
         <is>
           <t>ふに・無9(著者)</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="D31" s="0" t="inlineStr">
         <is>
           <t>Episode. 18</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="n">
+      <c r="A32" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="B32" s="0" t="inlineStr">
         <is>
           <t>H村へようこそ！</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="C32" s="0" t="inlineStr">
         <is>
           <t>額縁あいこ(著者)</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="D32" s="0" t="inlineStr">
         <is>
           <t>第11話</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="n">
+      <c r="A33" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="B33" s="0" t="inlineStr">
         <is>
           <t>我が焔炎にひれ伏せ世界</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="C33" s="0" t="inlineStr">
         <is>
           <t>すめらぎひよこ(原作) こゆき(作画) Mika Pikazo(キャラクター原案) mocha(背景画)</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="D33" s="0" t="inlineStr">
         <is>
           <t>コミックス告知</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="n">
+      <c r="A34" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B34" s="0" t="inlineStr">
         <is>
           <t>ジェノヴァの弟子～10秒しか戦えない魔術師、のちの『魔王』を育てる～</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="C34" s="0" t="inlineStr">
         <is>
           <t>原作：妹尾尻尾 漫画：魚塚じゃこ キャラクター原案：赤嶺直樹</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="D34" s="0" t="inlineStr">
         <is>
           <t>第21話</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="n">
+      <c r="A35" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="B35" s="0" t="inlineStr">
         <is>
           <t>シャドウ・アサシンズ・ワールド ～影は薄いけど、最強忍者やってます～</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="C35" s="0" t="inlineStr">
         <is>
           <t>空山トキ 五色安未 泉乃せん 伍長</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="D35" s="0" t="inlineStr">
         <is>
           <t>第10話　少女と本当の自分１（2）</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="n">
+      <c r="A36" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="B36" s="0" t="inlineStr">
         <is>
           <t>ラスボス討伐後に始める二周目冒険者ライフ はじまりの街でワケあり美少女たちがめちゃくちゃ懐いてきます</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="C36" s="0" t="inlineStr">
         <is>
           <t>鬼麻正明(漫画) 朱月十話(原作) ファルまろ(キャラ原案)</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="D36" s="0" t="inlineStr">
         <is>
           <t>第4話-1</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="n">
+      <c r="A37" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="B37" s="0" t="inlineStr">
         <is>
           <t>女子高生の無駄づかい</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="C37" s="0" t="inlineStr">
         <is>
           <t>ビーノ(著者)</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
+      <c r="D37" s="0" t="inlineStr">
         <is>
           <t>ばんがいへん</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="n">
+      <c r="A38" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="B38" s="0" t="inlineStr">
         <is>
           <t>葉木莉さんは君だけの死神になりたい</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
+      <c r="C38" s="0" t="inlineStr">
         <is>
           <t>３５まち</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
+      <c r="D38" s="0" t="inlineStr">
         <is>
           <t>第５話　葉木莉さん相手だ――間違っても間違いなんて起きないけど</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="n">
+      <c r="A39" s="0" t="n">
         <v>38</v>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="B39" s="0" t="inlineStr">
         <is>
           <t>人生逆転ダンジョン</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="C39" s="0" t="inlineStr">
         <is>
           <t>尾張 ニコ どすこい花丸様</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
+      <c r="D39" s="0" t="inlineStr">
         <is>
           <t>第3-1話	穴は使いよう</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="n">
+      <c r="A40" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="B40" s="0" t="inlineStr">
         <is>
           <t>塔の管理をしてみよう</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="C40" s="0" t="inlineStr">
         <is>
           <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="D40" s="0" t="inlineStr">
         <is>
           <t>第90話後編</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="n">
+      <c r="A41" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="B41" s="0" t="inlineStr">
         <is>
           <t>残念女幹部ブラックジェネラルさん</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="C41" s="0" t="inlineStr">
         <is>
           <t>jin(著者)</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
+      <c r="D41" s="0" t="inlineStr">
         <is>
           <t>第百九十九話</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="n">
+      <c r="A42" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="B42" s="0" t="inlineStr">
         <is>
           <t>煽り系ゲーム配信者（20歳）、配信の切り忘れによりいい人バレする。</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="C42" s="0" t="inlineStr">
         <is>
           <t>流嘉（漫画） 夏乃実（原作） 麦うさぎ（キャラクター原案）</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
+      <c r="D42" s="0" t="inlineStr">
         <is>
           <t>第4話　サブ垢（前編）</t>
         </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="n">
+      <c r="A43" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B43" s="0" t="inlineStr">
         <is>
           <t>ひとりぼっちの異世界攻略</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="C43" s="0" t="inlineStr">
         <is>
           <t>びび（漫画） 五示正司（原作）</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
+      <c r="D43" s="0" t="inlineStr">
         <is>
           <t>第226話　人ではなくなった…？</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="n">
+      <c r="A44" s="0" t="n">
         <v>43</v>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="B44" s="0" t="inlineStr">
         <is>
           <t>異世界でスローライフを（願望）</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="C44" s="0" t="inlineStr">
         <is>
           <t>長頼（漫画） シゲ（原作） オウカ（キャラクター原案）</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
+      <c r="D44" s="0" t="inlineStr">
         <is>
           <t>第53話　王都観光</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="n">
+      <c r="A45" s="0" t="n">
         <v>44</v>
       </c>
-      <c r="B45" t="inlineStr">
+      <c r="B45" s="0" t="inlineStr">
         <is>
           <t>シルバーマウンテン</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="C45" s="0" t="inlineStr">
         <is>
           <t>藤田 和日郎</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
+      <c r="D45" s="0" t="inlineStr">
         <is>
           <t>5．第一章「仙境＜螺界＞」 其ノ四 腰痛の竜</t>
         </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="n">
+      <c r="A46" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="B46" t="inlineStr">
+      <c r="B46" s="0" t="inlineStr">
         <is>
           <t>アンゴルモア 元寇合戦記　【博多編】</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="C46" s="0" t="inlineStr">
         <is>
           <t>たかぎ七彦(著者)</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
+      <c r="D46" s="0" t="inlineStr">
         <is>
           <t>第四十四話その四</t>
         </is>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="n">
+      <c r="A47" s="0" t="n">
         <v>46</v>
       </c>
-      <c r="B47" t="inlineStr">
+      <c r="B47" s="0" t="inlineStr">
         <is>
           <t>終焉の魔女と世界の旅</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="C47" s="0" t="inlineStr">
         <is>
           <t>片岡とんち</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
+      <c r="D47" s="0" t="inlineStr">
         <is>
           <t>第13話①	終焉の魔女と魔王メリア</t>
         </is>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="n">
+      <c r="A48" s="0" t="n">
         <v>47</v>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="B48" s="0" t="inlineStr">
         <is>
           <t>序盤で死ぬ最強のサブキャラに転生したので、ゲーム知識で無双する</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
+      <c r="C48" s="0" t="inlineStr">
         <is>
           <t>作画：マエD 原作：新人</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
+      <c r="D48" s="0" t="inlineStr">
         <is>
           <t>第4話(3)</t>
         </is>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="n">
+      <c r="A49" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="B49" s="0" t="inlineStr">
         <is>
           <t>追放者食堂へようこそ！　～最強パーティーを追放された料理人（Lv.99）は、田舎で念願の冒険者食堂を開きます！～</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="C49" s="0" t="inlineStr">
         <is>
           <t>つむみ（漫画） 君川優樹（原作）</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
+      <c r="D49" s="0" t="inlineStr">
         <is>
           <t>第52話　真心XIII（前編）</t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="n">
+      <c r="A50" s="0" t="n">
         <v>49</v>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="B50" s="0" t="inlineStr">
         <is>
           <t>サラリーマンが異世界に行ったら四天王になった話</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="C50" s="0" t="inlineStr">
         <is>
           <t>漫画：村光 原作：ベニガシラ</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
+      <c r="D50" s="0" t="inlineStr">
         <is>
           <t>第87話　氷の捕食</t>
         </is>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="n">
+      <c r="A51" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="B51" s="0" t="inlineStr">
         <is>
           <t>この素晴らしい世界に祝福を！</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="C51" s="0" t="inlineStr">
         <is>
           <t>渡真仁(作画) 三嶋くろね(キャラクター原案) 暁なつめ(原作)</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
+      <c r="D51" s="0" t="inlineStr">
         <is>
           <t>第129話-2　この偉大なる姉のために名誉回復を！</t>
         </is>
@@ -11929,6 +11930,1047 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>不徳のギルド</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>河添太一</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>第９６話：分福</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>辺境モブ貴族のウチに嫁いできた悪役令嬢が、めちゃくちゃできる良い嫁なんだが？</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>tera(原作) 朝倉はやて(作画) 徹田(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>第9話</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>村上よしゆき 茨木野 あるてら</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>第４０話　勇者、聖女と元聖騎士と再会し、魚人を追っ払う（４）</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>魔王になったので、ダンジョン造って人外娘とほのぼのする</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>遠野ノオト(作画) 流優(原作) だぶ竜(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>第1話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>俺以外誰も採取できない素材なのに「素材採取率が低い」とパワハラする幼馴染錬金術師と絶縁した専属魔導士、辺境の町でスローライフを送りたい。</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>狐御前(原作) 西岡知三(作画) ＮＯＣＯ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>第23話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>バーサス</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>第26話 惨事（1）</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ゲーム悪役貴族に転生した俺は、チート筋肉で無双する</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>昼行燈（原作） しいたけ元帥（漫画）</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>第25話</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>空野進 sorani ファルまろ</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>第10話　最弱貴族、部下を信じる（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>俺は全てを【パリイ】する　～逆勘違いの世界最強は冒険者になりたい～</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>原作：鍋敷・カワグチ 漫画：KRSG</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>第24話</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>無職の英雄　別にスキルなんか要らなかったんだが</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>原作：九頭七尾・上田夢人 漫画：名苗秋緒</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>第50話</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ディーふらぐ！</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>春野友矢(著者)</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>第171話</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>転生したらスライムだった件 異聞 ～魔国暮らしのトリニティ～</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>伏瀬 戸野タエ みっつばー</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>第106話　開国祭開幕［その１］</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>双子まとめて『カノジョ』にしない？</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>飴色みそ(漫画) 白井ムク(原作) 千種みのり(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>第13話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>クラスメイトの元アイドルが、とにかく挙動不審なんです。</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>となりける(作画) こりんさん(原作) ｋｒ木(キャラクター原案) マイクロマガジン社(監修)</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>第24話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>第1話④</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>貧乏騎士に嫁入りしたはずが!? ~野人令嬢は皇太子妃になっても竜を狩りたい~</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>漫画：夏川そぞろ 原作：宮前葵 キャラクター原案：ののまろ</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>第10話③皇太子妃（仮）</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>幼馴染のS級パーティーから追放された聖獣使い。万能支援魔法と仲間を増やして最強へ！</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>黒田高祥(作画) かなりつ(原作) 転(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>第51話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>となりの席のヤツがそういう目で見てくる</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>mmk</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>第40話 誘惑</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>転生してハイエルフになりましたが、スローライフは１２０年で飽きました</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>原作：らる鳥・しあびす 漫画：成田コウ</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>第40話</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>【悲報】清楚系で売っていた底辺配信者、うっかり配信を切り忘れたままSS級モンスターを拳で殴り飛ばしてしまう</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>アトハ NEO草野 pupps</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>第４話　【悲報】ご乱行⁉ ダンジョンシーカー・アカデミー！（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>実家に帰ったら甘やかされ生活が始まりました</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>漫画：幹藻ねずみ 原作：月夜乃古狸 キャラクター原案：うなさか</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>第23話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>戦隊レッド 異世界で冒険者になる</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>中吉虎吉</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>第41話「悠戯のブイダラ（前編）」</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>クラスメイトの美少女四人に頼まれたので、VRMMO内で専属料理人をはじめました</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>斗樹稼多利(原作) 幾夜大黒堂(漫画) 中林ずん(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>第6話</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>ヘルモード ～やり込み好きのゲーマーは廃設定の異世界で無双する～ はじまりの召喚士</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>原作：ハム男・藻 漫画：鉄田猿児</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>GAME 081　戦姫</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>フルメタル・パニック！　Family</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>賀東招二(原作) 神反ヲ鬚(作画) 四季童子(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>第6話　東京都江東区のタワマン39階②-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>第33話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>規格外のダンジョン攻略者、実は異世界帰りの元勇者</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>作画：やまざき君 原作：榊与一</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>第4話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>アザミヤコを好きになる</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>ユニティコング(原作) ツノニガウ(作画)</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>第8話</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>俺の死亡フラグが留まるところを知らない</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>漫画：乙須ミツヤ 原作：泉</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>フラグ68 フリエリ</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>第9話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>今日も絵に描いた餅が美味い@COMIC</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>漫画：梅渡飛鳥 原作：もちもち物質 キャラクター原案：転</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>第41話</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>ギャルゲーマーに褒められたい</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>げしゅまろ(著者)</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>40話</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>斎藤義龍に生まれ変わったので、織田信長に国譲りして長生きするのを目指します！</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>巽未頼 田村ゆうき マキムラシュンスケ</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>第71話「日々の積み重ねこそ」</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>第120話　四騎戦決勝戦!!・後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>戦姫サバイバルサガ-異世界の運命をかけた無人島フジュン異性交遊-</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>OTOSAMA(著者)</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>第17話</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>無能なナナ</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>原作 るーすぼーい 作画 古屋庵</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>第78話 兄弟PART2</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>殺されたらゾンビになったので、進化しまくって無双しようと思います</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>漫画：朝ケ夜 原作：幸運ピエロ キャラクター原案：東西</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>第15話(後半)暴走ドラゴンと魔剣②</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>ルパン三世 異世界の姫君（ネイバーワールドプリンセス）</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>モンキー・パンチ／エム・ピー・ワークス 内々けやき 佐伯庸介 白狼</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>第100話：金毛羊の星空</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>モブ高生の俺でも冒険者になればリア充になれますか？</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>原作：百均 漫画：さぎやまれん キャラクター原案：hai</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>第29.5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>第126話　戦争を終わらせてみるⅡ（中編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>直径3cmの召喚陣&lt;リミットリング&gt;で「雑魚すら呼べない」と蔑まれた底辺召喚士が頂点に立つまで</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>作画：まっつー 原作：空松蓮司</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>第4話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>おねえさんと猫を飼う</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>上杉響士郎(著者)</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>第2話：おねえさんと猫の部屋</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>六姫は神護衛に恋をする　～最強の守護騎士、転生して魔法学園に行く～</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>漫画:加古山 寿 原案:朱月 十話 キャラクター原案:てつぶた</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>第122話　声</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>隣の席のヤンキー清水さんが髪を黒く染めてきた</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>底花(原作) 真田若楓(漫画) ハム(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>第10話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>第31話 独身貴族はヒラメが大事（4）</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>かつての暗殺者は来世で違う生き方をする</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>ツネ(漫画) 丘野優(原作) つなかわ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>第4話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>廃嫡王子の華麗なる逃亡劇 ~手段を選ばない最強クズ魔術師は自堕落に生きたい~</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>出雲大吉(原作) 岡野むろ(作画) ゆのひと(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>第9話</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>スキル【万物支配】に目覚めたおっさんは、ダンジョンで生計を立てることにしました～無職から始める支配者無双～</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>岸本和葉 原田 臙 シミズヒロノリ 吉武</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>第4話　穴熊商店(前編)</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>重版決定記念イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>ゲーム内最強の『裏ボス』に転生したので、主人公の代わりに最速クリアを目指します！</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>作画：こめぐ 原作：迅空也</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>第4話(1)</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Add ranking data for 2025-07-12
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -26,6 +26,7 @@
     <sheet name="2025-07-09" sheetId="18" state="visible" r:id="rId18"/>
     <sheet name="2025-07-10" sheetId="19" state="visible" r:id="rId19"/>
     <sheet name="2025-07-11" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="2025-07-12" sheetId="21" state="visible" r:id="rId21"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -11967,22 +11968,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>不徳のギルド</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>河添太一</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第９６話：分福</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>辺境モブ貴族のウチに嫁いできた悪役令嬢が、めちゃくちゃできる良い嫁なんだが？</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>tera(原作) 朝倉はやて(作画) 徹田(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第9話</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>村上よしゆき 茨木野 あるてら</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第４０話　勇者、聖女と元聖騎士と再会し、魚人を追っ払う（４）</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>魔王になったので、ダンジョン造って人外娘とほのぼのする</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>遠野ノオト(作画) 流優(原作) だぶ竜(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第1話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>俺以外誰も採取できない素材なのに「素材採取率が低い」とパワハラする幼馴染錬金術師と絶縁した専属魔導士、辺境の町でスローライフを送りたい。</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>狐御前(原作) 西岡知三(作画) ＮＯＣＯ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第23話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>バーサス</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第26話 惨事（1）</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>ゲーム悪役貴族に転生した俺は、チート筋肉で無双する</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>昼行燈（原作） しいたけ元帥（漫画）</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第25話</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>空野進 sorani ファルまろ</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第10話　最弱貴族、部下を信じる（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>俺は全てを【パリイ】する　～逆勘違いの世界最強は冒険者になりたい～</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>原作：鍋敷・カワグチ 漫画：KRSG</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第24話</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>無職の英雄　別にスキルなんか要らなかったんだが</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>原作：九頭七尾・上田夢人 漫画：名苗秋緒</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第50話</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>ディーふらぐ！</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>春野友矢(著者)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第171話</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>転生したらスライムだった件 異聞 ～魔国暮らしのトリニティ～</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>伏瀬 戸野タエ みっつばー</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第106話　開国祭開幕［その１］</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>双子まとめて『カノジョ』にしない？</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>飴色みそ(漫画) 白井ムク(原作) 千種みのり(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第13話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>クラスメイトの元アイドルが、とにかく挙動不審なんです。</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>となりける(作画) こりんさん(原作) ｋｒ木(キャラクター原案) マイクロマガジン社(監修)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第24話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第1話④</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>貧乏騎士に嫁入りしたはずが!? ~野人令嬢は皇太子妃になっても竜を狩りたい~</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>漫画：夏川そぞろ 原作：宮前葵 キャラクター原案：ののまろ</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第10話③皇太子妃（仮）</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>幼馴染のS級パーティーから追放された聖獣使い。万能支援魔法と仲間を増やして最強へ！</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>黒田高祥(作画) かなりつ(原作) 転(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第51話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>となりの席のヤツがそういう目で見てくる</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>mmk</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第40話 誘惑</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>転生してハイエルフになりましたが、スローライフは１２０年で飽きました</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>原作：らる鳥・しあびす 漫画：成田コウ</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第40話</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>【悲報】清楚系で売っていた底辺配信者、うっかり配信を切り忘れたままSS級モンスターを拳で殴り飛ばしてしまう</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>アトハ NEO草野 pupps</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第４話　【悲報】ご乱行⁉ ダンジョンシーカー・アカデミー！（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>実家に帰ったら甘やかされ生活が始まりました</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>漫画：幹藻ねずみ 原作：月夜乃古狸 キャラクター原案：うなさか</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第23話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>戦隊レッド 異世界で冒険者になる</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>中吉虎吉</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第41話「悠戯のブイダラ（前編）」</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>クラスメイトの美少女四人に頼まれたので、VRMMO内で専属料理人をはじめました</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>斗樹稼多利(原作) 幾夜大黒堂(漫画) 中林ずん(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第6話</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>ヘルモード ～やり込み好きのゲーマーは廃設定の異世界で無双する～ はじまりの召喚士</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>原作：ハム男・藻 漫画：鉄田猿児</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>GAME 081　戦姫</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>フルメタル・パニック！　Family</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>賀東招二(原作) 神反ヲ鬚(作画) 四季童子(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第6話　東京都江東区のタワマン39階②-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第33話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>規格外のダンジョン攻略者、実は異世界帰りの元勇者</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>作画：やまざき君 原作：榊与一</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第4話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>アザミヤコを好きになる</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>ユニティコング(原作) ツノニガウ(作画)</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第8話</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>俺の死亡フラグが留まるところを知らない</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>漫画：乙須ミツヤ 原作：泉</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>フラグ68 フリエリ</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第9話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>今日も絵に描いた餅が美味い@COMIC</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>漫画：梅渡飛鳥 原作：もちもち物質 キャラクター原案：転</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第41話</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>ギャルゲーマーに褒められたい</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>げしゅまろ(著者)</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>40話</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>斎藤義龍に生まれ変わったので、織田信長に国譲りして長生きするのを目指します！</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>巽未頼 田村ゆうき マキムラシュンスケ</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第71話「日々の積み重ねこそ」</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第120話　四騎戦決勝戦!!・後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>戦姫サバイバルサガ-異世界の運命をかけた無人島フジュン異性交遊-</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>OTOSAMA(著者)</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第17話</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>無能なナナ</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>原作 るーすぼーい 作画 古屋庵</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第78話 兄弟PART2</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>殺されたらゾンビになったので、進化しまくって無双しようと思います</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>漫画：朝ケ夜 原作：幸運ピエロ キャラクター原案：東西</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第15話(後半)暴走ドラゴンと魔剣②</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>ルパン三世 異世界の姫君（ネイバーワールドプリンセス）</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>モンキー・パンチ／エム・ピー・ワークス 内々けやき 佐伯庸介 白狼</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第100話：金毛羊の星空</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>モブ高生の俺でも冒険者になればリア充になれますか？</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>原作：百均 漫画：さぎやまれん キャラクター原案：hai</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第29.5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第126話　戦争を終わらせてみるⅡ（中編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>直径3cmの召喚陣&lt;リミットリング&gt;で「雑魚すら呼べない」と蔑まれた底辺召喚士が頂点に立つまで</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>作画：まっつー 原作：空松蓮司</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第4話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>おねえさんと猫を飼う</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>上杉響士郎(著者)</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第2話：おねえさんと猫の部屋</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>六姫は神護衛に恋をする　～最強の守護騎士、転生して魔法学園に行く～</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>漫画:加古山 寿 原案:朱月 十話 キャラクター原案:てつぶた</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第122話　声</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>隣の席のヤンキー清水さんが髪を黒く染めてきた</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>底花(原作) 真田若楓(漫画) ハム(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第10話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第31話 独身貴族はヒラメが大事（4）</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>かつての暗殺者は来世で違う生き方をする</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>ツネ(漫画) 丘野優(原作) つなかわ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第4話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>廃嫡王子の華麗なる逃亡劇 ~手段を選ばない最強クズ魔術師は自堕落に生きたい~</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>出雲大吉(原作) 岡野むろ(作画) ゆのひと(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第9話</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>スキル【万物支配】に目覚めたおっさんは、ダンジョンで生計を立てることにしました～無職から始める支配者無双～</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>岸本和葉 原田 臙 シミズヒロノリ 吉武</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第4話　穴熊商店(前編)</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>重版決定記念イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>ゲーム内最強の『裏ボス』に転生したので、主人公の代わりに最速クリアを目指します！</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>作画：こめぐ 原作：迅空也</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第4話(1)</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>不徳のギルド</t>
+          <t>魔術師クノンは見えている</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>河添太一</t>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第９６話：分福</t>
+          <t>第38話②</t>
         </is>
       </c>
     </row>
@@ -11992,17 +13034,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>辺境モブ貴族のウチに嫁いできた悪役令嬢が、めちゃくちゃできる良い嫁なんだが？</t>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>tera(原作) 朝倉はやて(作画) 徹田(キャラクター原案)</t>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第9話</t>
+          <t>「名もなき英雄譚」前半</t>
         </is>
       </c>
     </row>
@@ -12012,17 +13054,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+          <t>勇者に全部奪われた俺は勇者の母親とパーティを組みました！</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>村上よしゆき 茨木野 あるてら</t>
+          <t>久遠まこと(著者) 石のやっさん(原作)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第４０話　勇者、聖女と元聖騎士と再会し、魚人を追っ払う（４）</t>
+          <t>第28話</t>
         </is>
       </c>
     </row>
@@ -12032,17 +13074,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>魔王になったので、ダンジョン造って人外娘とほのぼのする</t>
+          <t>ダンジョンの幼なじみ</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>遠野ノオト(作画) 流優(原作) だぶ竜(キャラクター原案)</t>
+          <t>久真やすひさ(著者)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第1話後半</t>
+          <t>第55話</t>
         </is>
       </c>
     </row>
@@ -12052,17 +13094,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>俺以外誰も採取できない素材なのに「素材採取率が低い」とパワハラする幼馴染錬金術師と絶縁した専属魔導士、辺境の町でスローライフを送りたい。</t>
+          <t>金属スライムを倒しまくった俺が【黒鋼の王】と呼ばれるまで</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>狐御前(原作) 西岡知三(作画) ＮＯＣＯ(キャラクター原案)</t>
+          <t>藤屋いずこ(著者) 温泉カピバラ(原作) 山椒魚(キャラクター原案)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第23話-2</t>
+          <t>第13章-2</t>
         </is>
       </c>
     </row>
@@ -12072,17 +13114,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>バーサス</t>
+          <t>淫獄団地</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第26話 惨事（1）</t>
+          <t>第48話（後編）</t>
         </is>
       </c>
     </row>
@@ -12092,17 +13134,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ゲーム悪役貴族に転生した俺は、チート筋肉で無双する</t>
+          <t>まんきつしたい常連さん</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>昼行燈（原作） しいたけ元帥（漫画）</t>
+          <t>しんみりん(著者)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第25話</t>
+          <t>第45話後編</t>
         </is>
       </c>
     </row>
@@ -12112,17 +13154,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+          <t>女友達は頼めば意外とヤらせてくれる</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>空野進 sorani ファルまろ</t>
+          <t>ろくろ(漫画) 鏡遊(原作)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第10話　最弱貴族、部下を信じる（１）</t>
+          <t>特別イラスト</t>
         </is>
       </c>
     </row>
@@ -12132,17 +13174,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>俺は全てを【パリイ】する　～逆勘違いの世界最強は冒険者になりたい～</t>
+          <t>美人女上司滝沢さん</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>原作：鍋敷・カワグチ 漫画：KRSG</t>
+          <t>やんBARU(著者)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第24話</t>
+          <t>第201話</t>
         </is>
       </c>
     </row>
@@ -12152,17 +13194,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>無職の英雄　別にスキルなんか要らなかったんだが</t>
+          <t>よくわからないけれど異世界に転生していたようです</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>原作：九頭七尾・上田夢人 漫画：名苗秋緒</t>
+          <t>内々けやき あし カオミン</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第50話</t>
+          <t>第135話 よくわからないけれど導かれてしまったようです（２）</t>
         </is>
       </c>
     </row>
@@ -12172,17 +13214,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ディーふらぐ！</t>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>春野友矢(著者)</t>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第171話</t>
+          <t>第80話その2</t>
         </is>
       </c>
     </row>
@@ -12192,17 +13234,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>転生したらスライムだった件 異聞 ～魔国暮らしのトリニティ～</t>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>伏瀬 戸野タエ みっつばー</t>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第106話　開国祭開幕［その１］</t>
+          <t>第70話(後編) 特別報酬ミッション</t>
         </is>
       </c>
     </row>
@@ -12212,17 +13254,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>双子まとめて『カノジョ』にしない？</t>
+          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>飴色みそ(漫画) 白井ムク(原作) 千種みのり(キャラクター原案)</t>
+          <t>FUNA 東西 モトエ恵介</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第13話①</t>
+          <t>第119話　会談［その4］</t>
         </is>
       </c>
     </row>
@@ -12232,17 +13274,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>クラスメイトの元アイドルが、とにかく挙動不審なんです。</t>
+          <t>陰キャの俺が席替えでS級美少女に囲まれたら秘密の関係が始まった。</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>となりける(作画) こりんさん(原作) ｋｒ木(キャラクター原案) マイクロマガジン社(監修)</t>
+          <t>星野 星野(原作) バラマツヒトミ(漫画) 黒兎 ゆう(キャラクター原案)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第24話-2</t>
+          <t>第3話</t>
         </is>
       </c>
     </row>
@@ -12252,17 +13294,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
+          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
+          <t>神原絵理華(漫画) 一森一輝(原作)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第1話④</t>
+          <t>第17話④</t>
         </is>
       </c>
     </row>
@@ -12272,17 +13314,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>貧乏騎士に嫁入りしたはずが!? ~野人令嬢は皇太子妃になっても竜を狩りたい~</t>
+          <t>不徳のギルド</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>漫画：夏川そぞろ 原作：宮前葵 キャラクター原案：ののまろ</t>
+          <t>河添太一</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第10話③皇太子妃（仮）</t>
+          <t>第９６話：分福</t>
         </is>
       </c>
     </row>
@@ -12292,17 +13334,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>幼馴染のS級パーティーから追放された聖獣使い。万能支援魔法と仲間を増やして最強へ！</t>
+          <t>ホームセンターごと呼び出された私の大迷宮リノベーション！</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>黒田高祥(作画) かなりつ(原作) 転(キャラクター原案)</t>
+          <t>ばたっち(漫画) 星崎崑(原作) 志田(キャラクター原案)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第51話-1</t>
+          <t>第4話後編</t>
         </is>
       </c>
     </row>
@@ -12312,17 +13354,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>となりの席のヤツがそういう目で見てくる</t>
+          <t>仕事帰り、独身の美人上司に頼まれて</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>mmk</t>
+          <t>望公太(原作) とんのすけ(作画) しの(キャラクター原案)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第40話 誘惑</t>
+          <t>第19話-2</t>
         </is>
       </c>
     </row>
@@ -12332,17 +13374,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>転生してハイエルフになりましたが、スローライフは１２０年で飽きました</t>
+          <t>ダウナーお姉さんは遊びたい</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>原作：らる鳥・しあびす 漫画：成田コウ</t>
+          <t>山鷹景</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第40話</t>
+          <t>第13話</t>
         </is>
       </c>
     </row>
@@ -12352,17 +13394,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>【悲報】清楚系で売っていた底辺配信者、うっかり配信を切り忘れたままSS級モンスターを拳で殴り飛ばしてしまう</t>
+          <t>農学博士の異世界無双～禁忌の知識で築くモンスター娘ハーレム～</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>アトハ NEO草野 pupps</t>
+          <t>インド僧(原作) ヤスウミ(作画)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第４話　【悲報】ご乱行⁉ ダンジョンシーカー・アカデミー！（３）</t>
+          <t>第24話</t>
         </is>
       </c>
     </row>
@@ -12372,17 +13414,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>実家に帰ったら甘やかされ生活が始まりました</t>
+          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>漫画：幹藻ねずみ 原作：月夜乃古狸 キャラクター原案：うなさか</t>
+          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第23話後半</t>
+          <t>休載マンガ</t>
         </is>
       </c>
     </row>
@@ -12392,17 +13434,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>戦隊レッド 異世界で冒険者になる</t>
+          <t>センパイ、自宅警備員の雇用はいかがですか？</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>中吉虎吉</t>
+          <t>漫画：コブラサナギ 原作：二上圭 キャラ原案：日向あずり</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第41話「悠戯のブイダラ（前編）」</t>
+          <t>第5話前半</t>
         </is>
       </c>
     </row>
@@ -12412,17 +13454,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>クラスメイトの美少女四人に頼まれたので、VRMMO内で専属料理人をはじめました</t>
+          <t>修羅幼女の英雄譚～半端者と言われた傭兵、幼女に転生して成り上がる～</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>斗樹稼多利(原作) 幾夜大黒堂(漫画) 中林ずん(キャラクター原案)</t>
+          <t>作画：むらたん 原作：沙城流</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第6話</t>
+          <t>第7話(1)</t>
         </is>
       </c>
     </row>
@@ -12432,17 +13474,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ヘルモード ～やり込み好きのゲーマーは廃設定の異世界で無双する～ はじまりの召喚士</t>
+          <t>ある日突然、ギャルの許嫁ができた</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>原作：ハム男・藻 漫画：鉄田猿児</t>
+          <t>窪茶(漫画) 泉谷一樹(原作) なかむら(文庫イラスト) まめぇ(原作イラスト)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>GAME 081　戦姫</t>
+          <t>第12話</t>
         </is>
       </c>
     </row>
@@ -12452,17 +13494,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>フルメタル・パニック！　Family</t>
+          <t>僕のいけずな婚約者</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>賀東招二(原作) 神反ヲ鬚(作画) 四季童子(キャラクター原案)</t>
+          <t>冬谷リク(漫画)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第6話　東京都江東区のタワマン39階②-1</t>
+          <t>第7話</t>
         </is>
       </c>
     </row>
@@ -12472,17 +13514,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+          <t>異世界はスマートフォンとともに。</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+          <t>そと(漫画) 冬原パトラ(原作) 兎塚エイジ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第33話②</t>
+          <t>EPISODE:102‐②</t>
         </is>
       </c>
     </row>
@@ -12492,17 +13534,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>規格外のダンジョン攻略者、実は異世界帰りの元勇者</t>
+          <t>スキルがなければレベルを上げる～９９がカンストの世界でレベル800万からスタート～</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>作画：やまざき君 原作：榊与一</t>
+          <t>倉橋ユウス(漫画) 岡沢六十四(原作)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第4話(1)</t>
+          <t>第51話②</t>
         </is>
       </c>
     </row>
@@ -12512,17 +13554,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>アザミヤコを好きになる</t>
+          <t>ヤンデレかと思ったらもっとヤベー女だった</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ユニティコング(原作) ツノニガウ(作画)</t>
+          <t>八木戸マト</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第8話</t>
+          <t>第66話　最後に彼氏の全てが欲しいヤンデレ彼女</t>
         </is>
       </c>
     </row>
@@ -12532,17 +13574,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>俺の死亡フラグが留まるところを知らない</t>
+          <t>時森さんが無防備です!!</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>漫画：乙須ミツヤ 原作：泉</t>
+          <t>たざわ</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>フラグ68 フリエリ</t>
+          <t>第62話</t>
         </is>
       </c>
     </row>
@@ -12552,17 +13594,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+          <t>不老不死少女の苗床旅行記</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+          <t>ふじはん(漫画) ルナ・ウサギ(原作)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第9話-1</t>
+          <t>第16話前編</t>
         </is>
       </c>
     </row>
@@ -12572,17 +13614,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>今日も絵に描いた餅が美味い@COMIC</t>
+          <t>ゴミ以下だと追放された使用人、実は前世賢者です　～史上最強の賢者、世界最高峰の学園に通う～</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>漫画：梅渡飛鳥 原作：もちもち物質 キャラクター原案：転</t>
+          <t>原作：夜分長文 漫画：矢部利恩 キャラクター原案：蔓木鋼音</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第41話</t>
+          <t>第14話 魔女対策（１）</t>
         </is>
       </c>
     </row>
@@ -12592,17 +13634,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ギャルゲーマーに褒められたい</t>
+          <t>辺境モブ貴族のウチに嫁いできた悪役令嬢が、めちゃくちゃできる良い嫁なんだが？</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>げしゅまろ(著者)</t>
+          <t>tera(原作) 朝倉はやて(作画) 徹田(キャラクター原案)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>40話</t>
+          <t>第9話</t>
         </is>
       </c>
     </row>
@@ -12612,17 +13654,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>斎藤義龍に生まれ変わったので、織田信長に国譲りして長生きするのを目指します！</t>
+          <t>断れない会長は友江くんにだけしてあげたい</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>巽未頼 田村ゆうき マキムラシュンスケ</t>
+          <t>沼地どろまる(著者)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第71話「日々の積み重ねこそ」</t>
+          <t>休載漫画</t>
         </is>
       </c>
     </row>
@@ -12632,17 +13674,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>実は俺、最強でした？</t>
+          <t>くじ引き特賞：無双ハーレム権</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>原作：澄守 彩 漫画：高橋 愛</t>
+          <t>原作／三木なずな（GA文庫／SBクリエイティブ刊） 漫画／長谷見亮 キャラクター原案／瑠奈璃亜</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第120話　四騎戦決勝戦!!・後編</t>
+          <t>第58話-01　新たな王女たちへ、受け継がれし慈愛の心！</t>
         </is>
       </c>
     </row>
@@ -12652,17 +13694,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>戦姫サバイバルサガ-異世界の運命をかけた無人島フジュン異性交遊-</t>
+          <t>脱稿するまでオチません</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>OTOSAMA(著者)</t>
+          <t>ヨシラギ(著者)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第17話</t>
+          <t>第32話前半</t>
         </is>
       </c>
     </row>
@@ -12672,17 +13714,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>無能なナナ</t>
+          <t>義妹生活</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>原作 るーすぼーい 作画 古屋庵</t>
+          <t>三河ごーすと(原作) 奏ユミカ(漫画) Hiten(キャラクター原案)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第78話 兄弟PART2</t>
+          <t>第30話-1</t>
         </is>
       </c>
     </row>
@@ -12692,17 +13734,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>殺されたらゾンビになったので、進化しまくって無双しようと思います</t>
+          <t>クラスメイトは異世界で勇者になったけど、俺だけ現代日本に置き去りにされました</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>漫画：朝ケ夜 原作：幸運ピエロ キャラクター原案：東西</t>
+          <t>カボチャマスク(原作) 仲紙(漫画)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第15話(後半)暴走ドラゴンと魔剣②</t>
+          <t>第9話-4</t>
         </is>
       </c>
     </row>
@@ -12712,17 +13754,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ルパン三世 異世界の姫君（ネイバーワールドプリンセス）</t>
+          <t>俺の愛娘は悪役令嬢</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>モンキー・パンチ／エム・ピー・ワークス 内々けやき 佐伯庸介 白狼</t>
+          <t>かわもり かぐら(原作) ほづみりや(漫画) 縞(キャラクター原案)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第100話：金毛羊の星空</t>
+          <t>第4話-1</t>
         </is>
       </c>
     </row>
@@ -12732,17 +13774,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>モブ高生の俺でも冒険者になればリア充になれますか？</t>
+          <t>俺の『全自動支援（フルオートバフ）』で仲間たちが世界最強 ～そこにいるだけ無自覚無双～</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>原作：百均 漫画：さぎやまれん キャラクター原案：hai</t>
+          <t>IプルT(著者) epina(原作) 片倉響(キャラクター原案)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第29.5話</t>
+          <t>第３３話「砂浜の盗賊たち」</t>
         </is>
       </c>
     </row>
@@ -12752,17 +13794,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>異世界魔王と召喚少女の奴隷魔術</t>
+          <t>勇者パーティから追い出された不遇職【罠士】、ユニークスキル【矢印】で最強になる</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+          <t>作画：たつひこ 原作：白石 有希</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第126話　戦争を終わらせてみるⅡ（中編）</t>
+          <t>第7話(1)</t>
         </is>
       </c>
     </row>
@@ -12772,17 +13814,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>直径3cmの召喚陣&lt;リミットリング&gt;で「雑魚すら呼べない」と蔑まれた底辺召喚士が頂点に立つまで</t>
+          <t>その冒険者、取り扱い注意。 ～正体は無敵の下僕たちを統べる異世界最強の魔導王～</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>作画：まっつー 原作：空松蓮司</t>
+          <t>満月シオン(作画) Sin Guilty(ツギクル)(原作) M.B(キャラクター原案)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第4話(1)</t>
+          <t>56章　はじまりの愚か者②　前編</t>
         </is>
       </c>
     </row>
@@ -12792,17 +13834,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>おねえさんと猫を飼う</t>
+          <t>モブ高生の俺でも冒険者になればリア充になれますか？</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>上杉響士郎(著者)</t>
+          <t>原作：百均 漫画：さぎやまれん キャラクター原案：hai</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第2話：おねえさんと猫の部屋</t>
+          <t>第29.5話</t>
         </is>
       </c>
     </row>
@@ -12812,17 +13854,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>六姫は神護衛に恋をする　～最強の守護騎士、転生して魔法学園に行く～</t>
+          <t>クロの戦記Ⅱ 異世界転移した僕が最強なのはベッドの上だけのようです</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>漫画:加古山 寿 原案:朱月 十話 キャラクター原案:てつぶた</t>
+          <t>サイトウアユム(原作) ユリシロ(漫画) むつみまさと(キャラクター原案)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第122話　声</t>
+          <t>第22話-1</t>
         </is>
       </c>
     </row>
@@ -12832,17 +13874,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>隣の席のヤンキー清水さんが髪を黒く染めてきた</t>
+          <t>ぽんドロイド！ はまさん</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>底花(原作) 真田若楓(漫画) ハム(キャラクター原案)</t>
+          <t>はれやまはれぞう(著者)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第10話-1</t>
+          <t>第3話</t>
         </is>
       </c>
     </row>
@@ -12852,17 +13894,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+          <t>ギルドを追放された回復術士、実は魔力無限だったので規格外の回復魔法で伝説となる</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+          <t>漫画：坂下コウ 原作：霞杏檎</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第31話 独身貴族はヒラメが大事（4）</t>
+          <t>第3話(3)</t>
         </is>
       </c>
     </row>
@@ -12872,17 +13914,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>かつての暗殺者は来世で違う生き方をする</t>
+          <t>聖剣が最強の世界で、少年は弓に愛される～封印された魔王がくれた力で聖剣士たちを援護します～</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>ツネ(漫画) 丘野優(原作) つなかわ(キャラクター原案)</t>
+          <t>さとう(原作) 貞清カズヒコ(漫画)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第4話①</t>
+          <t>第13話①</t>
         </is>
       </c>
     </row>
@@ -12892,17 +13934,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>廃嫡王子の華麗なる逃亡劇 ~手段を選ばない最強クズ魔術師は自堕落に生きたい~</t>
+          <t>おじ転生</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>出雲大吉(原作) 岡野むろ(作画) ゆのひと(キャラクター原案)</t>
+          <t>相葉キョウコ</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第9話</t>
+          <t>第14話</t>
         </is>
       </c>
     </row>
@@ -12912,17 +13954,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>スキル【万物支配】に目覚めたおっさんは、ダンジョンで生計を立てることにしました～無職から始める支配者無双～</t>
+          <t>俺以外誰も採取できない素材なのに「素材採取率が低い」とパワハラする幼馴染錬金術師と絶縁した専属魔導士、辺境の町でスローライフを送りたい。</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>岸本和葉 原田 臙 シミズヒロノリ 吉武</t>
+          <t>狐御前(原作) 西岡知三(作画) ＮＯＣＯ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第4話　穴熊商店(前編)</t>
+          <t>第23話-2</t>
         </is>
       </c>
     </row>
@@ -12932,17 +13974,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
+          <t>村上よしゆき 茨木野 あるてら</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>重版決定記念イラスト</t>
+          <t>第４０話　勇者、聖女と元聖騎士と再会し、魚人を追っ払う（４）</t>
         </is>
       </c>
     </row>
@@ -12952,17 +13994,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>ゲーム内最強の『裏ボス』に転生したので、主人公の代わりに最速クリアを目指します！</t>
+          <t>最も嫌われている最凶の悪役に転生</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>作画：こめぐ 原作：迅空也</t>
+          <t>灰色の鼠(原作) 沢田かに(漫画)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第4話(1)</t>
+          <t>第17話①</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-07-13
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -27,6 +27,7 @@
     <sheet name="2025-07-10" sheetId="19" state="visible" r:id="rId19"/>
     <sheet name="2025-07-11" sheetId="20" state="visible" r:id="rId20"/>
     <sheet name="2025-07-12" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="2025-07-13" sheetId="22" state="visible" r:id="rId22"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -13009,22 +13010,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>魔術師クノンは見えている</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第38話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>「名もなき英雄譚」前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>勇者に全部奪われた俺は勇者の母親とパーティを組みました！</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>久遠まこと(著者) 石のやっさん(原作)</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第28話</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>ダンジョンの幼なじみ</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>久真やすひさ(著者)</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第55話</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>金属スライムを倒しまくった俺が【黒鋼の王】と呼ばれるまで</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>藤屋いずこ(著者) 温泉カピバラ(原作) 山椒魚(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第13章-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>淫獄団地</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第48話（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>まんきつしたい常連さん</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>しんみりん(著者)</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第45話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>女友達は頼めば意外とヤらせてくれる</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>ろくろ(漫画) 鏡遊(原作)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>特別イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>美人女上司滝沢さん</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>やんBARU(著者)</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第201話</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第135話 よくわからないけれど導かれてしまったようです（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第80話その2</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第70話(後編) 特別報酬ミッション</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>FUNA 東西 モトエ恵介</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第119話　会談［その4］</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>陰キャの俺が席替えでS級美少女に囲まれたら秘密の関係が始まった。</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>星野 星野(原作) バラマツヒトミ(漫画) 黒兎 ゆう(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第3話</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>神原絵理華(漫画) 一森一輝(原作)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第17話④</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>不徳のギルド</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>河添太一</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第９６話：分福</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>ホームセンターごと呼び出された私の大迷宮リノベーション！</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>ばたっち(漫画) 星崎崑(原作) 志田(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第4話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>仕事帰り、独身の美人上司に頼まれて</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>望公太(原作) とんのすけ(作画) しの(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第19話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>ダウナーお姉さんは遊びたい</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>山鷹景</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第13話</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>農学博士の異世界無双～禁忌の知識で築くモンスター娘ハーレム～</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>インド僧(原作) ヤスウミ(作画)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第24話</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>休載マンガ</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>センパイ、自宅警備員の雇用はいかがですか？</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>漫画：コブラサナギ 原作：二上圭 キャラ原案：日向あずり</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第5話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>修羅幼女の英雄譚～半端者と言われた傭兵、幼女に転生して成り上がる～</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>作画：むらたん 原作：沙城流</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第7話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>ある日突然、ギャルの許嫁ができた</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>窪茶(漫画) 泉谷一樹(原作) なかむら(文庫イラスト) まめぇ(原作イラスト)</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第12話</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>僕のいけずな婚約者</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>冬谷リク(漫画)</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第7話</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>異世界はスマートフォンとともに。</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>そと(漫画) 冬原パトラ(原作) 兎塚エイジ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>EPISODE:102‐②</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>スキルがなければレベルを上げる～９９がカンストの世界でレベル800万からスタート～</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>倉橋ユウス(漫画) 岡沢六十四(原作)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第51話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>ヤンデレかと思ったらもっとヤベー女だった</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>八木戸マト</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第66話　最後に彼氏の全てが欲しいヤンデレ彼女</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>時森さんが無防備です!!</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>たざわ</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第62話</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>不老不死少女の苗床旅行記</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>ふじはん(漫画) ルナ・ウサギ(原作)</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第16話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>ゴミ以下だと追放された使用人、実は前世賢者です　～史上最強の賢者、世界最高峰の学園に通う～</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>原作：夜分長文 漫画：矢部利恩 キャラクター原案：蔓木鋼音</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第14話 魔女対策（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>辺境モブ貴族のウチに嫁いできた悪役令嬢が、めちゃくちゃできる良い嫁なんだが？</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>tera(原作) 朝倉はやて(作画) 徹田(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第9話</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>断れない会長は友江くんにだけしてあげたい</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>沼地どろまる(著者)</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>休載漫画</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>くじ引き特賞：無双ハーレム権</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>原作／三木なずな（GA文庫／SBクリエイティブ刊） 漫画／長谷見亮 キャラクター原案／瑠奈璃亜</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第58話-01　新たな王女たちへ、受け継がれし慈愛の心！</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>脱稿するまでオチません</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>ヨシラギ(著者)</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第32話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>義妹生活</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>三河ごーすと(原作) 奏ユミカ(漫画) Hiten(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第30話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>クラスメイトは異世界で勇者になったけど、俺だけ現代日本に置き去りにされました</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>カボチャマスク(原作) 仲紙(漫画)</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第9話-4</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>俺の愛娘は悪役令嬢</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>かわもり かぐら(原作) ほづみりや(漫画) 縞(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第4話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>俺の『全自動支援（フルオートバフ）』で仲間たちが世界最強 ～そこにいるだけ無自覚無双～</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>IプルT(著者) epina(原作) 片倉響(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第３３話「砂浜の盗賊たち」</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティから追い出された不遇職【罠士】、ユニークスキル【矢印】で最強になる</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>作画：たつひこ 原作：白石 有希</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第7話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>その冒険者、取り扱い注意。 ～正体は無敵の下僕たちを統べる異世界最強の魔導王～</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>満月シオン(作画) Sin Guilty(ツギクル)(原作) M.B(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>56章　はじまりの愚か者②　前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>モブ高生の俺でも冒険者になればリア充になれますか？</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>原作：百均 漫画：さぎやまれん キャラクター原案：hai</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第29.5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>クロの戦記Ⅱ 異世界転移した僕が最強なのはベッドの上だけのようです</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>サイトウアユム(原作) ユリシロ(漫画) むつみまさと(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第22話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>ぽんドロイド！ はまさん</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>はれやまはれぞう(著者)</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第3話</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>ギルドを追放された回復術士、実は魔力無限だったので規格外の回復魔法で伝説となる</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>漫画：坂下コウ 原作：霞杏檎</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第3話(3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>聖剣が最強の世界で、少年は弓に愛される～封印された魔王がくれた力で聖剣士たちを援護します～</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>さとう(原作) 貞清カズヒコ(漫画)</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第13話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>おじ転生</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>相葉キョウコ</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第14話</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>俺以外誰も採取できない素材なのに「素材採取率が低い」とパワハラする幼馴染錬金術師と絶縁した専属魔導士、辺境の町でスローライフを送りたい。</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>狐御前(原作) 西岡知三(作画) ＮＯＣＯ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第23話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>村上よしゆき 茨木野 あるてら</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第４０話　勇者、聖女と元聖騎士と再会し、魚人を追っ払う（４）</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>最も嫌われている最凶の悪役に転生</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>灰色の鼠(原作) 沢田かに(漫画)</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第17話①</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>魔術師クノンは見えている</t>
+          <t>寿司ガキ</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+          <t>ichika(著者)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第38話②</t>
+          <t>第9話</t>
         </is>
       </c>
     </row>
@@ -13034,17 +14076,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+          <t>不純な彼女達は懺悔しない</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+          <t>ポロロッカ(著者)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>「名もなき英雄譚」前半</t>
+          <t>第28話</t>
         </is>
       </c>
     </row>
@@ -13054,17 +14096,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>勇者に全部奪われた俺は勇者の母親とパーティを組みました！</t>
+          <t>クセ強彼女は床にいざなう</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>久遠まこと(著者) 石のやっさん(原作)</t>
+          <t>須河篤志(著者)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第28話</t>
+          <t>第13話後半</t>
         </is>
       </c>
     </row>
@@ -13074,17 +14116,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ダンジョンの幼なじみ</t>
+          <t>リビルドワールド</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>久真やすひさ(著者)</t>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第55話</t>
+          <t>第71話①</t>
         </is>
       </c>
     </row>
@@ -13094,17 +14136,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>金属スライムを倒しまくった俺が【黒鋼の王】と呼ばれるまで</t>
+          <t>ぽんドロイド！ はまさん</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>藤屋いずこ(著者) 温泉カピバラ(原作) 山椒魚(キャラクター原案)</t>
+          <t>はれやまはれぞう(著者)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第13章-2</t>
+          <t>第4話</t>
         </is>
       </c>
     </row>
@@ -13114,17 +14156,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>淫獄団地</t>
+          <t>おとなりのダウナーさんは無理させない</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+          <t>瑠璃いろ(著者)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第48話（後編）</t>
+          <t>第12話</t>
         </is>
       </c>
     </row>
@@ -13134,17 +14176,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>まんきつしたい常連さん</t>
+          <t>サーシャちゃんとクラスメイトオタクくん</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>しんみりん(著者)</t>
+          <t>はぐはぐ(著者)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第45話後編</t>
+          <t>第5話</t>
         </is>
       </c>
     </row>
@@ -13154,17 +14196,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>女友達は頼めば意外とヤらせてくれる</t>
+          <t>地味子な三葉さんが僕を誘惑する</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ろくろ(漫画) 鏡遊(原作)</t>
+          <t>はぶらえる(著者)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>特別イラスト</t>
+          <t>第10話前半</t>
         </is>
       </c>
     </row>
@@ -13174,17 +14216,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>美人女上司滝沢さん</t>
+          <t>男子高校生だけどギャルにTSしました</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>やんBARU(著者)</t>
+          <t>太陽まりい(著者)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第201話</t>
+          <t>第18話前編</t>
         </is>
       </c>
     </row>
@@ -13194,17 +14236,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>よくわからないけれど異世界に転生していたようです</t>
+          <t>田舎の黒ギャルJKと結婚しました</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>内々けやき あし カオミン</t>
+          <t>カヅチ(著者)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第135話 よくわからないけれど導かれてしまったようです（２）</t>
+          <t>第17話前半</t>
         </is>
       </c>
     </row>
@@ -13214,17 +14256,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+          <t>魔術師クノンは見えている</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第80話その2</t>
+          <t>第38話②</t>
         </is>
       </c>
     </row>
@@ -13234,17 +14276,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+          <t>オトナを知りたい女友達</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+          <t>望公太(原作) ぷよちゃ(作画)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第70話(後編) 特別報酬ミッション</t>
+          <t>第7話 後半</t>
         </is>
       </c>
     </row>
@@ -13254,17 +14296,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>FUNA 東西 モトエ恵介</t>
+          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第119話　会談［その4］</t>
+          <t>第1話④</t>
         </is>
       </c>
     </row>
@@ -13274,17 +14316,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>陰キャの俺が席替えでS級美少女に囲まれたら秘密の関係が始まった。</t>
+          <t>勇者に全部奪われた俺は勇者の母親とパーティを組みました！</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>星野 星野(原作) バラマツヒトミ(漫画) 黒兎 ゆう(キャラクター原案)</t>
+          <t>久遠まこと(著者) 石のやっさん(原作)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第3話</t>
+          <t>第28話</t>
         </is>
       </c>
     </row>
@@ -13294,17 +14336,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
+          <t>ミルク搾りハンターの異世界搾乳記～農家の冴えない男があらゆる種族の地区Bを弄び虜にする～</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>神原絵理華(漫画) 一森一輝(原作)</t>
+          <t>空詠大智(著者)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第17話④</t>
+          <t>第16話</t>
         </is>
       </c>
     </row>
@@ -13314,17 +14356,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>不徳のギルド</t>
+          <t>リモート授業になったらクラス１の美少女と同居することになった</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>河添太一</t>
+          <t>原作：三萩せんや(GA文庫／SBクリエイティブ刊)　漫画：jaguchi　キャラクター原案：さとうぽて</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第９６話：分福</t>
+          <t>第11話</t>
         </is>
       </c>
     </row>
@@ -13334,17 +14376,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ホームセンターごと呼び出された私の大迷宮リノベーション！</t>
+          <t>女友達は頼めば意外とヤらせてくれる</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>ばたっち(漫画) 星崎崑(原作) 志田(キャラクター原案)</t>
+          <t>ろくろ(漫画) 鏡遊(原作)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第4話後編</t>
+          <t>特別イラスト</t>
         </is>
       </c>
     </row>
@@ -13354,17 +14396,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>仕事帰り、独身の美人上司に頼まれて</t>
+          <t>聖液鍛冶屋のエロランタ</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>望公太(原作) とんのすけ(作画) しの(キャラクター原案)</t>
+          <t>しげきっくす(著者)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第19話-2</t>
+          <t>休載イラスト</t>
         </is>
       </c>
     </row>
@@ -13374,17 +14416,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ダウナーお姉さんは遊びたい</t>
+          <t>リアリスト魔王による聖域なき異世界改革</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>山鷹景</t>
+          <t>鈴木マナツ(漫画) 羽田遼亮(原作) ゆーげん(キャラクターデザイン) ひたきゆう(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第13話</t>
+          <t>第67幕①</t>
         </is>
       </c>
     </row>
@@ -13394,17 +14436,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>農学博士の異世界無双～禁忌の知識で築くモンスター娘ハーレム～</t>
+          <t>転生してあらゆるモノに好かれながら異世界で好きな事をして生きて行く</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>インド僧(原作) ヤスウミ(作画)</t>
+          <t>都尾琉(漫画) 御峰。(原作)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第24話</t>
+          <t>第26話②</t>
         </is>
       </c>
     </row>
@@ -13414,17 +14456,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
+          <t>淫獄団地</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>休載マンガ</t>
+          <t>第48話（後編）</t>
         </is>
       </c>
     </row>
@@ -13434,17 +14476,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>センパイ、自宅警備員の雇用はいかがですか？</t>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>漫画：コブラサナギ 原作：二上圭 キャラ原案：日向あずり</t>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第5話前半</t>
+          <t>「名もなき英雄譚」前半</t>
         </is>
       </c>
     </row>
@@ -13454,17 +14496,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>修羅幼女の英雄譚～半端者と言われた傭兵、幼女に転生して成り上がる～</t>
+          <t>金属スライムを倒しまくった俺が【黒鋼の王】と呼ばれるまで</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>作画：むらたん 原作：沙城流</t>
+          <t>藤屋いずこ(著者) 温泉カピバラ(原作) 山椒魚(キャラクター原案)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第7話(1)</t>
+          <t>第13章-2</t>
         </is>
       </c>
     </row>
@@ -13474,17 +14516,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ある日突然、ギャルの許嫁ができた</t>
+          <t>チュートリアルが始まる前に ボスキャラ達を破滅させない為に俺ができる幾つかの事</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>窪茶(漫画) 泉谷一樹(原作) なかむら(文庫イラスト) まめぇ(原作イラスト)</t>
+          <t>横山コウヂ(漫画) 髙橋炬燵(原作) カカオ・ランタン(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第12話</t>
+          <t>第13話②</t>
         </is>
       </c>
     </row>
@@ -13494,17 +14536,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>僕のいけずな婚約者</t>
+          <t>ダンジョンの幼なじみ</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>冬谷リク(漫画)</t>
+          <t>久真やすひさ(著者)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第7話</t>
+          <t>第55話</t>
         </is>
       </c>
     </row>
@@ -13514,17 +14556,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>異世界はスマートフォンとともに。</t>
+          <t>まんきつしたい常連さん</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>そと(漫画) 冬原パトラ(原作) 兎塚エイジ(キャラクター原案)</t>
+          <t>しんみりん(著者)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>EPISODE:102‐②</t>
+          <t>第45話後編</t>
         </is>
       </c>
     </row>
@@ -13534,17 +14576,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>スキルがなければレベルを上げる～９９がカンストの世界でレベル800万からスタート～</t>
+          <t>愚かな天使は悪魔と踊る</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>倉橋ユウス(漫画) 岡沢六十四(原作)</t>
+          <t>アズマサワヨシ(著者)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第51話②</t>
+          <t>第100話①</t>
         </is>
       </c>
     </row>
@@ -13554,17 +14596,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ヤンデレかと思ったらもっとヤベー女だった</t>
+          <t>殺されて井戸に捨てられた聖女がチート怨霊になりました</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>八木戸マト</t>
+          <t>原作　谷尾銀　漫画　七清水くらげ　ネーム構成　桜井竜矢</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第66話　最後に彼氏の全てが欲しいヤンデレ彼女</t>
+          <t>第7話　出産④</t>
         </is>
       </c>
     </row>
@@ -13574,17 +14616,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>時森さんが無防備です!!</t>
+          <t>美人女上司滝沢さん</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>たざわ</t>
+          <t>やんBARU(著者)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第62話</t>
+          <t>第201話</t>
         </is>
       </c>
     </row>
@@ -13594,17 +14636,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>不老不死少女の苗床旅行記</t>
+          <t>ギャルゲーマーに褒められたい</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>ふじはん(漫画) ルナ・ウサギ(原作)</t>
+          <t>げしゅまろ(著者)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第16話前編</t>
+          <t>42話</t>
         </is>
       </c>
     </row>
@@ -13614,17 +14656,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ゴミ以下だと追放された使用人、実は前世賢者です　～史上最強の賢者、世界最高峰の学園に通う～</t>
+          <t>よくわからないけれど異世界に転生していたようです</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>原作：夜分長文 漫画：矢部利恩 キャラクター原案：蔓木鋼音</t>
+          <t>内々けやき あし カオミン</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第14話 魔女対策（１）</t>
+          <t>第135話 よくわからないけれど導かれてしまったようです（２）</t>
         </is>
       </c>
     </row>
@@ -13634,17 +14676,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>辺境モブ貴族のウチに嫁いできた悪役令嬢が、めちゃくちゃできる良い嫁なんだが？</t>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>tera(原作) 朝倉はやて(作画) 徹田(キャラクター原案)</t>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第9話</t>
+          <t>第70話(後編) 特別報酬ミッション</t>
         </is>
       </c>
     </row>
@@ -13654,17 +14696,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>断れない会長は友江くんにだけしてあげたい</t>
+          <t>陰キャの俺が席替えでS級美少女に囲まれたら秘密の関係が始まった。</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>沼地どろまる(著者)</t>
+          <t>星野 星野(原作) バラマツヒトミ(漫画) 黒兎 ゆう(キャラクター原案)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>休載漫画</t>
+          <t>第3話</t>
         </is>
       </c>
     </row>
@@ -13674,17 +14716,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>くじ引き特賞：無双ハーレム権</t>
+          <t>女装男と男装女</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>原作／三木なずな（GA文庫／SBクリエイティブ刊） 漫画／長谷見亮 キャラクター原案／瑠奈璃亜</t>
+          <t>たけみつ(著者)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第58話-01　新たな王女たちへ、受け継がれし慈愛の心！</t>
+          <t>読み切り</t>
         </is>
       </c>
     </row>
@@ -13694,17 +14736,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>脱稿するまでオチません</t>
+          <t>不徳のギルド</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>ヨシラギ(著者)</t>
+          <t>河添太一</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第32話前半</t>
+          <t>第９６話：分福</t>
         </is>
       </c>
     </row>
@@ -13714,17 +14756,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>義妹生活</t>
+          <t>本物のカノジョにしたくなるまで、私で試していいよ。</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>三河ごーすと(原作) 奏ユミカ(漫画) Hiten(キャラクター原案)</t>
+          <t>wano(漫画) 有丈ほえる(原作) 緋月ひぐれ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第30話-1</t>
+          <t>第8話①</t>
         </is>
       </c>
     </row>
@@ -13734,17 +14776,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>クラスメイトは異世界で勇者になったけど、俺だけ現代日本に置き去りにされました</t>
+          <t>ステータス・オール∞（インフィニティ） ∞使いの最強能力者、異世界を自由気ままに暮らします！</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>カボチャマスク(原作) 仲紙(漫画)</t>
+          <t>漫画：三津屋みやこ 原作：八又ナガト</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第9話-4</t>
+          <t>第62話</t>
         </is>
       </c>
     </row>
@@ -13754,17 +14796,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>俺の愛娘は悪役令嬢</t>
+          <t>ダウナーお姉さんは遊びたい</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>かわもり かぐら(原作) ほづみりや(漫画) 縞(キャラクター原案)</t>
+          <t>山鷹景</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第4話-1</t>
+          <t>第13話</t>
         </is>
       </c>
     </row>
@@ -13774,17 +14816,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>俺の『全自動支援（フルオートバフ）』で仲間たちが世界最強 ～そこにいるだけ無自覚無双～</t>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>IプルT(著者) epina(原作) 片倉響(キャラクター原案)</t>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第３３話「砂浜の盗賊たち」</t>
+          <t>第80話その2</t>
         </is>
       </c>
     </row>
@@ -13794,17 +14836,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>勇者パーティから追い出された不遇職【罠士】、ユニークスキル【矢印】で最強になる</t>
+          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>作画：たつひこ 原作：白石 有希</t>
+          <t>FUNA 東西 モトエ恵介</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第7話(1)</t>
+          <t>第119話　会談［その4］</t>
         </is>
       </c>
     </row>
@@ -13814,17 +14856,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>その冒険者、取り扱い注意。 ～正体は無敵の下僕たちを統べる異世界最強の魔導王～</t>
+          <t>異種族追放コンカフェ</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>満月シオン(作画) Sin Guilty(ツギクル)(原作) M.B(キャラクター原案)</t>
+          <t>佐々木マサヒト(著者)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>56章　はじまりの愚か者②　前編</t>
+          <t>第16話</t>
         </is>
       </c>
     </row>
@@ -13834,17 +14876,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>モブ高生の俺でも冒険者になればリア充になれますか？</t>
+          <t>おっさん、転生して天才役者になる</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>原作：百均 漫画：さぎやまれん キャラクター原案：hai</t>
+          <t>芽々ノ圭(漫画) ほえ太郎(原作)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第29.5話</t>
+          <t>第37話①</t>
         </is>
       </c>
     </row>
@@ -13854,17 +14896,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>クロの戦記Ⅱ 異世界転移した僕が最強なのはベッドの上だけのようです</t>
+          <t>傭兵団の料理番</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>サイトウアユム(原作) ユリシロ(漫画) むつみまさと(キャラクター原案)</t>
+          <t>梅木泰祐(漫画) 川井昂(原作) 四季童子(キャラクター原案)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第22話-1</t>
+          <t>第9話-1</t>
         </is>
       </c>
     </row>
@@ -13874,17 +14916,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ぽんドロイド！ はまさん</t>
+          <t>ラスボスたちの隠し仔　～魔王城に転生した元社畜プログラマーは自由気ままに『魔導言語《マジックコード》』を開発する～</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>はれやまはれぞう(著者)</t>
+          <t>森清士郎(漫画) 熊乃げん骨(原作)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第3話</t>
+          <t>第14話①</t>
         </is>
       </c>
     </row>
@@ -13894,17 +14936,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ギルドを追放された回復術士、実は魔力無限だったので規格外の回復魔法で伝説となる</t>
+          <t>りゅうとあまがみ</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>漫画：坂下コウ 原作：霞杏檎</t>
+          <t>角丸柴朗(著者)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第3話(3)</t>
+          <t>第一話・魚嫌いのウィル</t>
         </is>
       </c>
     </row>
@@ -13914,17 +14956,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>聖剣が最強の世界で、少年は弓に愛される～封印された魔王がくれた力で聖剣士たちを援護します～</t>
+          <t>辺境モブ貴族のウチに嫁いできた悪役令嬢が、めちゃくちゃできる良い嫁なんだが？</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>さとう(原作) 貞清カズヒコ(漫画)</t>
+          <t>tera(原作) 朝倉はやて(作画) 徹田(キャラクター原案)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第13話①</t>
+          <t>第9話</t>
         </is>
       </c>
     </row>
@@ -13934,17 +14976,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>おじ転生</t>
+          <t>ホームセンターごと呼び出された私の大迷宮リノベーション！</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>相葉キョウコ</t>
+          <t>ばたっち(漫画) 星崎崑(原作) 志田(キャラクター原案)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第14話</t>
+          <t>第4話後編</t>
         </is>
       </c>
     </row>
@@ -13954,17 +14996,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>俺以外誰も採取できない素材なのに「素材採取率が低い」とパワハラする幼馴染錬金術師と絶縁した専属魔導士、辺境の町でスローライフを送りたい。</t>
+          <t>仕事帰り、独身の美人上司に頼まれて</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>狐御前(原作) 西岡知三(作画) ＮＯＣＯ(キャラクター原案)</t>
+          <t>望公太(原作) とんのすけ(作画) しの(キャラクター原案)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第23話-2</t>
+          <t>第19話-2</t>
         </is>
       </c>
     </row>
@@ -13974,17 +15016,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>村上よしゆき 茨木野 あるてら</t>
+          <t>神原絵理華(漫画) 一森一輝(原作)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第４０話　勇者、聖女と元聖騎士と再会し、魚人を追っ払う（４）</t>
+          <t>第17話④</t>
         </is>
       </c>
     </row>
@@ -13994,17 +15036,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>最も嫌われている最凶の悪役に転生</t>
+          <t>八男って、それはないでしょう！　みそっかす</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>灰色の鼠(原作) 沢田かに(漫画)</t>
+          <t>ながを(漫画) Ｙ．Ａ(原作) 藤ちょこ(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第17話①</t>
+          <t>episode.エリーゼ 第4話②</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-07-14
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -28,6 +28,7 @@
     <sheet name="2025-07-11" sheetId="20" state="visible" r:id="rId20"/>
     <sheet name="2025-07-12" sheetId="21" state="visible" r:id="rId21"/>
     <sheet name="2025-07-13" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="2025-07-14" sheetId="23" state="visible" r:id="rId23"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -14051,6 +14052,1047 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>寿司ガキ</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>ichika(著者)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第9話</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>不純な彼女達は懺悔しない</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>ポロロッカ(著者)</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第28話</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>クセ強彼女は床にいざなう</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>須河篤志(著者)</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第13話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第71話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>ぽんドロイド！ はまさん</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>はれやまはれぞう(著者)</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第4話</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>おとなりのダウナーさんは無理させない</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>瑠璃いろ(著者)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第12話</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>サーシャちゃんとクラスメイトオタクくん</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>はぐはぐ(著者)</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>地味子な三葉さんが僕を誘惑する</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>はぶらえる(著者)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第10話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>男子高校生だけどギャルにTSしました</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>太陽まりい(著者)</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第18話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>田舎の黒ギャルJKと結婚しました</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>カヅチ(著者)</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第17話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>魔術師クノンは見えている</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第38話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>オトナを知りたい女友達</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>望公太(原作) ぷよちゃ(作画)</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第7話 後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第1話④</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>勇者に全部奪われた俺は勇者の母親とパーティを組みました！</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>久遠まこと(著者) 石のやっさん(原作)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第28話</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>ミルク搾りハンターの異世界搾乳記～農家の冴えない男があらゆる種族の地区Bを弄び虜にする～</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>空詠大智(著者)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第16話</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>リモート授業になったらクラス１の美少女と同居することになった</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>原作：三萩せんや(GA文庫／SBクリエイティブ刊)　漫画：jaguchi　キャラクター原案：さとうぽて</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第11話</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>女友達は頼めば意外とヤらせてくれる</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>ろくろ(漫画) 鏡遊(原作)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>特別イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>聖液鍛冶屋のエロランタ</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>しげきっくす(著者)</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>休載イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>リアリスト魔王による聖域なき異世界改革</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>鈴木マナツ(漫画) 羽田遼亮(原作) ゆーげん(キャラクターデザイン) ひたきゆう(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第67幕①</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>転生してあらゆるモノに好かれながら異世界で好きな事をして生きて行く</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>都尾琉(漫画) 御峰。(原作)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第26話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>淫獄団地</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第48話（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>「名もなき英雄譚」前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>金属スライムを倒しまくった俺が【黒鋼の王】と呼ばれるまで</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>藤屋いずこ(著者) 温泉カピバラ(原作) 山椒魚(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第13章-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>チュートリアルが始まる前に ボスキャラ達を破滅させない為に俺ができる幾つかの事</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>横山コウヂ(漫画) 髙橋炬燵(原作) カカオ・ランタン(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第13話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>ダンジョンの幼なじみ</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>久真やすひさ(著者)</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第55話</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>まんきつしたい常連さん</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>しんみりん(著者)</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第45話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>愚かな天使は悪魔と踊る</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>アズマサワヨシ(著者)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第100話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>殺されて井戸に捨てられた聖女がチート怨霊になりました</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>原作　谷尾銀　漫画　七清水くらげ　ネーム構成　桜井竜矢</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第7話　出産④</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>美人女上司滝沢さん</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>やんBARU(著者)</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第201話</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>ギャルゲーマーに褒められたい</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>げしゅまろ(著者)</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>42話</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第135話 よくわからないけれど導かれてしまったようです（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第70話(後編) 特別報酬ミッション</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>陰キャの俺が席替えでS級美少女に囲まれたら秘密の関係が始まった。</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>星野 星野(原作) バラマツヒトミ(漫画) 黒兎 ゆう(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第3話</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>女装男と男装女</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>たけみつ(著者)</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>読み切り</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>不徳のギルド</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>河添太一</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第９６話：分福</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>本物のカノジョにしたくなるまで、私で試していいよ。</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>wano(漫画) 有丈ほえる(原作) 緋月ひぐれ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第8話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>ステータス・オール∞（インフィニティ） ∞使いの最強能力者、異世界を自由気ままに暮らします！</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>漫画：三津屋みやこ 原作：八又ナガト</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第62話</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>ダウナーお姉さんは遊びたい</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>山鷹景</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第13話</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第80話その2</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>FUNA 東西 モトエ恵介</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第119話　会談［その4］</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>異種族追放コンカフェ</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>佐々木マサヒト(著者)</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第16話</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>おっさん、転生して天才役者になる</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>芽々ノ圭(漫画) ほえ太郎(原作)</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第37話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>傭兵団の料理番</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>梅木泰祐(漫画) 川井昂(原作) 四季童子(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第9話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>ラスボスたちの隠し仔　～魔王城に転生した元社畜プログラマーは自由気ままに『魔導言語《マジックコード》』を開発する～</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>森清士郎(漫画) 熊乃げん骨(原作)</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第14話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>りゅうとあまがみ</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>角丸柴朗(著者)</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第一話・魚嫌いのウィル</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>辺境モブ貴族のウチに嫁いできた悪役令嬢が、めちゃくちゃできる良い嫁なんだが？</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>tera(原作) 朝倉はやて(作画) 徹田(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第9話</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>ホームセンターごと呼び出された私の大迷宮リノベーション！</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>ばたっち(漫画) 星崎崑(原作) 志田(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第4話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>仕事帰り、独身の美人上司に頼まれて</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>望公太(原作) とんのすけ(作画) しの(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第19話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>神原絵理華(漫画) 一森一輝(原作)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第17話④</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>八男って、それはないでしょう！　みそっかす</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>ながを(漫画) Ｙ．Ａ(原作) 藤ちょこ(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>episode.エリーゼ 第4話②</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
@@ -14116,17 +15158,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>リビルドワールド</t>
+          <t>ぽんドロイド！ はまさん</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+          <t>はれやまはれぞう(著者)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第71話①</t>
+          <t>第4話</t>
         </is>
       </c>
     </row>
@@ -14136,17 +15178,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ぽんドロイド！ はまさん</t>
+          <t>おんなのこのけんをてにいれた</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>はれやまはれぞう(著者)</t>
+          <t>福岡太朗(著者)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第4話</t>
+          <t>14本目</t>
         </is>
       </c>
     </row>
@@ -14156,17 +15198,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>おとなりのダウナーさんは無理させない</t>
+          <t>女装男と男装女</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>瑠璃いろ(著者)</t>
+          <t>たけみつ(著者)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第12話</t>
+          <t>読み切り</t>
         </is>
       </c>
     </row>
@@ -14176,17 +15218,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>サーシャちゃんとクラスメイトオタクくん</t>
+          <t>おとなりのダウナーさんは無理させない</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>はぐはぐ(著者)</t>
+          <t>瑠璃いろ(著者)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第5話</t>
+          <t>第12話</t>
         </is>
       </c>
     </row>
@@ -14196,17 +15238,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>地味子な三葉さんが僕を誘惑する</t>
+          <t>はずれスキル念動力（ただしレベルＭＡＸ）で無双する～手をかざすだけです。詠唱とか必殺技とかいりません。念じるだけで倒せます～</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>はぶらえる(著者)</t>
+          <t>さとう うなぽっぽ トダフミト</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第10話前半</t>
+          <t>9話②</t>
         </is>
       </c>
     </row>
@@ -14216,17 +15258,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>男子高校生だけどギャルにTSしました</t>
+          <t>ギャルゲーマーに褒められたい</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>太陽まりい(著者)</t>
+          <t>げしゅまろ(著者)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第18話前編</t>
+          <t>42話</t>
         </is>
       </c>
     </row>
@@ -14236,17 +15278,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>田舎の黒ギャルJKと結婚しました</t>
+          <t>リビルドワールド</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>カヅチ(著者)</t>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第17話前半</t>
+          <t>第71話①</t>
         </is>
       </c>
     </row>
@@ -14256,17 +15298,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>魔術師クノンは見えている</t>
+          <t>地味子な三葉さんが僕を誘惑する</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+          <t>はぶらえる(著者)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第38話②</t>
+          <t>第10話前半</t>
         </is>
       </c>
     </row>
@@ -14276,17 +15318,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>オトナを知りたい女友達</t>
+          <t>サーシャちゃんとクラスメイトオタクくん</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>望公太(原作) ぷよちゃ(作画)</t>
+          <t>はぐはぐ(著者)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第7話 後半</t>
+          <t>第5話</t>
         </is>
       </c>
     </row>
@@ -14296,17 +15338,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
+          <t>どれだけ努力しても経験値が入らず万年レベル０の俺は追放された</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
+          <t>原作：蓮池タロウ 漫画：そらモチ</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第1話④</t>
+          <t>第12話</t>
         </is>
       </c>
     </row>
@@ -14316,17 +15358,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>勇者に全部奪われた俺は勇者の母親とパーティを組みました！</t>
+          <t>魔術師クノンは見えている</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>久遠まこと(著者) 石のやっさん(原作)</t>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第28話</t>
+          <t>第38話②</t>
         </is>
       </c>
     </row>
@@ -14336,17 +15378,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ミルク搾りハンターの異世界搾乳記～農家の冴えない男があらゆる種族の地区Bを弄び虜にする～</t>
+          <t>勇者に全部奪われた俺は勇者の母親とパーティを組みました！</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>空詠大智(著者)</t>
+          <t>久遠まこと(著者) 石のやっさん(原作)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第16話</t>
+          <t>第28話</t>
         </is>
       </c>
     </row>
@@ -14356,17 +15398,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>リモート授業になったらクラス１の美少女と同居することになった</t>
+          <t>田舎の黒ギャルJKと結婚しました</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>原作：三萩せんや(GA文庫／SBクリエイティブ刊)　漫画：jaguchi　キャラクター原案：さとうぽて</t>
+          <t>カヅチ(著者)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第11話</t>
+          <t>第17話前半</t>
         </is>
       </c>
     </row>
@@ -14376,17 +15418,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>女友達は頼めば意外とヤらせてくれる</t>
+          <t>オトナを知りたい女友達</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>ろくろ(漫画) 鏡遊(原作)</t>
+          <t>望公太(原作) ぷよちゃ(作画)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>特別イラスト</t>
+          <t>第7話 後半</t>
         </is>
       </c>
     </row>
@@ -14396,17 +15438,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>聖液鍛冶屋のエロランタ</t>
+          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>しげきっくす(著者)</t>
+          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>休載イラスト</t>
+          <t>第1話④</t>
         </is>
       </c>
     </row>
@@ -14416,17 +15458,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>リアリスト魔王による聖域なき異世界改革</t>
+          <t>男子高校生だけどギャルにTSしました</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>鈴木マナツ(漫画) 羽田遼亮(原作) ゆーげん(キャラクターデザイン) ひたきゆう(キャラクターデザイン)</t>
+          <t>太陽まりい(著者)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第67幕①</t>
+          <t>第18話前編</t>
         </is>
       </c>
     </row>
@@ -14436,17 +15478,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>転生してあらゆるモノに好かれながら異世界で好きな事をして生きて行く</t>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>都尾琉(漫画) 御峰。(原作)</t>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第26話②</t>
+          <t>「名もなき英雄譚」前半</t>
         </is>
       </c>
     </row>
@@ -14456,17 +15498,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>淫獄団地</t>
+          <t>金属スライムを倒しまくった俺が【黒鋼の王】と呼ばれるまで</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+          <t>藤屋いずこ(著者) 温泉カピバラ(原作) 山椒魚(キャラクター原案)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第48話（後編）</t>
+          <t>第13章-2</t>
         </is>
       </c>
     </row>
@@ -14476,17 +15518,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+          <t>女友達は頼めば意外とヤらせてくれる</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+          <t>ろくろ(漫画) 鏡遊(原作)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>「名もなき英雄譚」前半</t>
+          <t>特別イラスト</t>
         </is>
       </c>
     </row>
@@ -14496,17 +15538,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>金属スライムを倒しまくった俺が【黒鋼の王】と呼ばれるまで</t>
+          <t>淫獄団地</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>藤屋いずこ(著者) 温泉カピバラ(原作) 山椒魚(キャラクター原案)</t>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第13章-2</t>
+          <t>第48話（後編）</t>
         </is>
       </c>
     </row>
@@ -14516,17 +15558,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>チュートリアルが始まる前に ボスキャラ達を破滅させない為に俺ができる幾つかの事</t>
+          <t>リモート授業になったらクラス１の美少女と同居することになった</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>横山コウヂ(漫画) 髙橋炬燵(原作) カカオ・ランタン(キャラクターデザイン)</t>
+          <t>原作：三萩せんや(GA文庫／SBクリエイティブ刊)　漫画：jaguchi　キャラクター原案：さとうぽて</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第13話②</t>
+          <t>第11話</t>
         </is>
       </c>
     </row>
@@ -14536,17 +15578,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ダンジョンの幼なじみ</t>
+          <t>ミルク搾りハンターの異世界搾乳記～農家の冴えない男があらゆる種族の地区Bを弄び虜にする～</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>久真やすひさ(著者)</t>
+          <t>空詠大智(著者)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第55話</t>
+          <t>第16話</t>
         </is>
       </c>
     </row>
@@ -14556,17 +15598,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>まんきつしたい常連さん</t>
+          <t>不徳のギルド</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>しんみりん(著者)</t>
+          <t>河添太一</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第45話後編</t>
+          <t>第９６話：分福</t>
         </is>
       </c>
     </row>
@@ -14576,17 +15618,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>愚かな天使は悪魔と踊る</t>
+          <t>聖液鍛冶屋のエロランタ</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>アズマサワヨシ(著者)</t>
+          <t>しげきっくす(著者)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第100話①</t>
+          <t>休載イラスト</t>
         </is>
       </c>
     </row>
@@ -14596,17 +15638,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>殺されて井戸に捨てられた聖女がチート怨霊になりました</t>
+          <t>ダンジョンの幼なじみ</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>原作　谷尾銀　漫画　七清水くらげ　ネーム構成　桜井竜矢</t>
+          <t>久真やすひさ(著者)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第7話　出産④</t>
+          <t>第55話</t>
         </is>
       </c>
     </row>
@@ -14616,17 +15658,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>美人女上司滝沢さん</t>
+          <t>まんきつしたい常連さん</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>やんBARU(著者)</t>
+          <t>しんみりん(著者)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第201話</t>
+          <t>第45話後編</t>
         </is>
       </c>
     </row>
@@ -14636,17 +15678,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ギャルゲーマーに褒められたい</t>
+          <t>ソードアート・オンライン Re:Aincrad</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>げしゅまろ(著者)</t>
+          <t>樹深(作画) 佐藤ミト(構成) 川原礫(原作) ａｂｅｃ(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>42話</t>
+          <t>第40話①</t>
         </is>
       </c>
     </row>
@@ -14656,17 +15698,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>よくわからないけれど異世界に転生していたようです</t>
+          <t>スライムテイマーの異世界ライフ</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>内々けやき あし カオミン</t>
+          <t>作画：チイチ 原作：穴の空いた靴下</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第135話 よくわからないけれど導かれてしまったようです（２）</t>
+          <t>第7話(1)</t>
         </is>
       </c>
     </row>
@@ -14676,17 +15718,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+          <t>よくわからないけれど異世界に転生していたようです</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+          <t>内々けやき あし カオミン</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第70話(後編) 特別報酬ミッション</t>
+          <t>第135話 よくわからないけれど導かれてしまったようです（２）</t>
         </is>
       </c>
     </row>
@@ -14696,17 +15738,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>陰キャの俺が席替えでS級美少女に囲まれたら秘密の関係が始まった。</t>
+          <t>リアリスト魔王による聖域なき異世界改革</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>星野 星野(原作) バラマツヒトミ(漫画) 黒兎 ゆう(キャラクター原案)</t>
+          <t>鈴木マナツ(漫画) 羽田遼亮(原作) ゆーげん(キャラクターデザイン) ひたきゆう(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第3話</t>
+          <t>第67幕①</t>
         </is>
       </c>
     </row>
@@ -14716,17 +15758,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>女装男と男装女</t>
+          <t>美人女上司滝沢さん</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>たけみつ(著者)</t>
+          <t>やんBARU(著者)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>読み切り</t>
+          <t>第201話</t>
         </is>
       </c>
     </row>
@@ -14736,17 +15778,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>不徳のギルド</t>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>河添太一</t>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第９６話：分福</t>
+          <t>第70話(後編) 特別報酬ミッション</t>
         </is>
       </c>
     </row>
@@ -14756,17 +15798,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>本物のカノジョにしたくなるまで、私で試していいよ。</t>
+          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>wano(漫画) 有丈ほえる(原作) 緋月ひぐれ(キャラクター原案)</t>
+          <t>FUNA 東西 モトエ恵介</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第8話①</t>
+          <t>第119話　会談［その4］</t>
         </is>
       </c>
     </row>
@@ -14776,17 +15818,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ステータス・オール∞（インフィニティ） ∞使いの最強能力者、異世界を自由気ままに暮らします！</t>
+          <t>陰キャの俺が席替えでS級美少女に囲まれたら秘密の関係が始まった。</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>漫画：三津屋みやこ 原作：八又ナガト</t>
+          <t>星野 星野(原作) バラマツヒトミ(漫画) 黒兎 ゆう(キャラクター原案)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第62話</t>
+          <t>第3話</t>
         </is>
       </c>
     </row>
@@ -14796,17 +15838,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ダウナーお姉さんは遊びたい</t>
+          <t>辺境モブ貴族のウチに嫁いできた悪役令嬢が、めちゃくちゃできる良い嫁なんだが？</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>山鷹景</t>
+          <t>tera(原作) 朝倉はやて(作画) 徹田(キャラクター原案)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第13話</t>
+          <t>第9話</t>
         </is>
       </c>
     </row>
@@ -14816,17 +15858,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+          <t>チュートリアルが始まる前に ボスキャラ達を破滅させない為に俺ができる幾つかの事</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+          <t>横山コウヂ(漫画) 髙橋炬燵(原作) カカオ・ランタン(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第80話その2</t>
+          <t>第13話②</t>
         </is>
       </c>
     </row>
@@ -14836,17 +15878,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+          <t>転生してあらゆるモノに好かれながら異世界で好きな事をして生きて行く</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>FUNA 東西 モトエ恵介</t>
+          <t>都尾琉(漫画) 御峰。(原作)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第119話　会談［その4］</t>
+          <t>第26話②</t>
         </is>
       </c>
     </row>
@@ -14856,17 +15898,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>異種族追放コンカフェ</t>
+          <t>時森さんが無防備です!!</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>佐々木マサヒト(著者)</t>
+          <t>たざわ</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第16話</t>
+          <t>第62話</t>
         </is>
       </c>
     </row>
@@ -14876,17 +15918,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>おっさん、転生して天才役者になる</t>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>芽々ノ圭(漫画) ほえ太郎(原作)</t>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第37話①</t>
+          <t>第80話その2</t>
         </is>
       </c>
     </row>
@@ -14896,17 +15938,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>傭兵団の料理番</t>
+          <t>愚かな天使は悪魔と踊る</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>梅木泰祐(漫画) 川井昂(原作) 四季童子(キャラクター原案)</t>
+          <t>アズマサワヨシ(著者)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第9話-1</t>
+          <t>第100話①</t>
         </is>
       </c>
     </row>
@@ -14916,17 +15958,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ラスボスたちの隠し仔　～魔王城に転生した元社畜プログラマーは自由気ままに『魔導言語《マジックコード》』を開発する～</t>
+          <t>本物のカノジョにしたくなるまで、私で試していいよ。</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>森清士郎(漫画) 熊乃げん骨(原作)</t>
+          <t>wano(漫画) 有丈ほえる(原作) 緋月ひぐれ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第14話①</t>
+          <t>第8話①</t>
         </is>
       </c>
     </row>
@@ -14936,17 +15978,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>りゅうとあまがみ</t>
+          <t>ナマケモノ学</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>角丸柴朗(著者)</t>
+          <t>ハリ</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第一話・魚嫌いのウィル</t>
+          <t>第19話　モフモフ断罪裁判</t>
         </is>
       </c>
     </row>
@@ -14956,17 +15998,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>辺境モブ貴族のウチに嫁いできた悪役令嬢が、めちゃくちゃできる良い嫁なんだが？</t>
+          <t>ダメ人間の愛しかた</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>tera(原作) 朝倉はやて(作画) 徹田(キャラクター原案)</t>
+          <t>岩葉(著者)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第9話</t>
+          <t>第18話前編　ダメ人間とお姉ちゃんと彼女</t>
         </is>
       </c>
     </row>
@@ -14976,17 +16018,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>ホームセンターごと呼び出された私の大迷宮リノベーション！</t>
+          <t>小さめの魔法師匠と大きめの魔法少女。report：3</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>ばたっち(漫画) 星崎崑(原作) 志田(キャラクター原案)</t>
+          <t>とりから</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第4話後編</t>
+          <t>第37話の2</t>
         </is>
       </c>
     </row>
@@ -14996,17 +16038,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>仕事帰り、独身の美人上司に頼まれて</t>
+          <t>ホームセンターごと呼び出された私の大迷宮リノベーション！</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>望公太(原作) とんのすけ(作画) しの(キャラクター原案)</t>
+          <t>ばたっち(漫画) 星崎崑(原作) 志田(キャラクター原案)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第19話-2</t>
+          <t>第4話後編</t>
         </is>
       </c>
     </row>
@@ -15016,17 +16058,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
+          <t>殺されて井戸に捨てられた聖女がチート怨霊になりました</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>神原絵理華(漫画) 一森一輝(原作)</t>
+          <t>原作　谷尾銀　漫画　七清水くらげ　ネーム構成　桜井竜矢</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第17話④</t>
+          <t>第7話　出産④</t>
         </is>
       </c>
     </row>
@@ -15036,17 +16078,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>八男って、それはないでしょう！　みそっかす</t>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>ながを(漫画) Ｙ．Ａ(原作) 藤ちょこ(キャラクターデザイン)</t>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>episode.エリーゼ 第4話②</t>
+          <t>第33話②</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-07-15
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -29,6 +29,7 @@
     <sheet name="2025-07-12" sheetId="21" state="visible" r:id="rId21"/>
     <sheet name="2025-07-13" sheetId="22" state="visible" r:id="rId22"/>
     <sheet name="2025-07-14" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="2025-07-15" sheetId="24" state="visible" r:id="rId24"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -15093,22 +15094,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>寿司ガキ</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>ichika(著者)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第9話</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>不純な彼女達は懺悔しない</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>ポロロッカ(著者)</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第28話</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>クセ強彼女は床にいざなう</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>須河篤志(著者)</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第13話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>ぽんドロイド！ はまさん</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>はれやまはれぞう(著者)</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第4話</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>おんなのこのけんをてにいれた</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>福岡太朗(著者)</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>14本目</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>女装男と男装女</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>たけみつ(著者)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>読み切り</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>おとなりのダウナーさんは無理させない</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>瑠璃いろ(著者)</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第12話</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>はずれスキル念動力（ただしレベルＭＡＸ）で無双する～手をかざすだけです。詠唱とか必殺技とかいりません。念じるだけで倒せます～</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>さとう うなぽっぽ トダフミト</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>9話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>ギャルゲーマーに褒められたい</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>げしゅまろ(著者)</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>42話</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第71話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>地味子な三葉さんが僕を誘惑する</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>はぶらえる(著者)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第10話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>サーシャちゃんとクラスメイトオタクくん</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>はぐはぐ(著者)</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>どれだけ努力しても経験値が入らず万年レベル０の俺は追放された</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>原作：蓮池タロウ 漫画：そらモチ</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第12話</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>魔術師クノンは見えている</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第38話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>勇者に全部奪われた俺は勇者の母親とパーティを組みました！</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>久遠まこと(著者) 石のやっさん(原作)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第28話</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>田舎の黒ギャルJKと結婚しました</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>カヅチ(著者)</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第17話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>オトナを知りたい女友達</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>望公太(原作) ぷよちゃ(作画)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第7話 後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第1話④</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>男子高校生だけどギャルにTSしました</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>太陽まりい(著者)</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第18話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>「名もなき英雄譚」前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>金属スライムを倒しまくった俺が【黒鋼の王】と呼ばれるまで</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>藤屋いずこ(著者) 温泉カピバラ(原作) 山椒魚(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第13章-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>女友達は頼めば意外とヤらせてくれる</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>ろくろ(漫画) 鏡遊(原作)</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>特別イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>淫獄団地</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第48話（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>リモート授業になったらクラス１の美少女と同居することになった</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>原作：三萩せんや(GA文庫／SBクリエイティブ刊)　漫画：jaguchi　キャラクター原案：さとうぽて</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第11話</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>ミルク搾りハンターの異世界搾乳記～農家の冴えない男があらゆる種族の地区Bを弄び虜にする～</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>空詠大智(著者)</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第16話</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>不徳のギルド</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>河添太一</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第９６話：分福</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>聖液鍛冶屋のエロランタ</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>しげきっくす(著者)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>休載イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>ダンジョンの幼なじみ</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>久真やすひさ(著者)</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第55話</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>まんきつしたい常連さん</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>しんみりん(著者)</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第45話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>ソードアート・オンライン Re:Aincrad</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>樹深(作画) 佐藤ミト(構成) 川原礫(原作) ａｂｅｃ(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第40話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>スライムテイマーの異世界ライフ</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>作画：チイチ 原作：穴の空いた靴下</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第7話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第135話 よくわからないけれど導かれてしまったようです（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>リアリスト魔王による聖域なき異世界改革</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>鈴木マナツ(漫画) 羽田遼亮(原作) ゆーげん(キャラクターデザイン) ひたきゆう(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第67幕①</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>美人女上司滝沢さん</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>やんBARU(著者)</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第201話</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第70話(後編) 特別報酬ミッション</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>FUNA 東西 モトエ恵介</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第119話　会談［その4］</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>陰キャの俺が席替えでS級美少女に囲まれたら秘密の関係が始まった。</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>星野 星野(原作) バラマツヒトミ(漫画) 黒兎 ゆう(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第3話</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>辺境モブ貴族のウチに嫁いできた悪役令嬢が、めちゃくちゃできる良い嫁なんだが？</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>tera(原作) 朝倉はやて(作画) 徹田(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第9話</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>チュートリアルが始まる前に ボスキャラ達を破滅させない為に俺ができる幾つかの事</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>横山コウヂ(漫画) 髙橋炬燵(原作) カカオ・ランタン(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第13話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>転生してあらゆるモノに好かれながら異世界で好きな事をして生きて行く</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>都尾琉(漫画) 御峰。(原作)</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第26話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>時森さんが無防備です!!</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>たざわ</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第62話</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第80話その2</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>愚かな天使は悪魔と踊る</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>アズマサワヨシ(著者)</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第100話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>本物のカノジョにしたくなるまで、私で試していいよ。</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>wano(漫画) 有丈ほえる(原作) 緋月ひぐれ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第8話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>ナマケモノ学</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>ハリ</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第19話　モフモフ断罪裁判</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>ダメ人間の愛しかた</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>岩葉(著者)</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第18話前編　ダメ人間とお姉ちゃんと彼女</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>小さめの魔法師匠と大きめの魔法少女。report：3</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>とりから</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第37話の2</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>ホームセンターごと呼び出された私の大迷宮リノベーション！</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>ばたっち(漫画) 星崎崑(原作) 志田(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第4話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>殺されて井戸に捨てられた聖女がチート怨霊になりました</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>原作　谷尾銀　漫画　七清水くらげ　ネーム構成　桜井竜矢</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第7話　出産④</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第33話②</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>寿司ガキ</t>
+          <t>帰ってください！ 阿久津さん</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ichika(著者)</t>
+          <t>長岡太一(著者)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第9話</t>
+          <t>第192話</t>
         </is>
       </c>
     </row>
@@ -15118,17 +16160,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>不純な彼女達は懺悔しない</t>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ポロロッカ(著者)</t>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第28話</t>
+          <t>第５０話　雌雄を決する器用貧乏（２）</t>
         </is>
       </c>
     </row>
@@ -15138,17 +16180,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>クセ強彼女は床にいざなう</t>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>須河篤志(著者)</t>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第13話後半</t>
+          <t>第２２食　ユクシーさんの覚悟、すごいのですわ！（２）</t>
         </is>
       </c>
     </row>
@@ -15158,17 +16200,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ぽんドロイド！ はまさん</t>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>はれやまはれぞう(著者)</t>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第4話</t>
+          <t>第47話 魔導具師とつながれたもの②</t>
         </is>
       </c>
     </row>
@@ -15178,17 +16220,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>おんなのこのけんをてにいれた</t>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>福岡太朗(著者)</t>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>14本目</t>
+          <t>第１８話②</t>
         </is>
       </c>
     </row>
@@ -15198,17 +16240,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>女装男と男装女</t>
+          <t>異世界でも無難に生きたい症候群</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>たけみつ(著者)</t>
+          <t>原作：安泰（一二三書房刊） 漫画：笹峰コウ キャラクター原案：ひたきゆう</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>読み切り</t>
+          <t>第30話①</t>
         </is>
       </c>
     </row>
@@ -15218,17 +16260,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>おとなりのダウナーさんは無理させない</t>
+          <t>ギャルとダンジョンと周回遅れの探索英雄譚</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>瑠璃いろ(著者)</t>
+          <t>漫画家： 水田ケンジ 原作：榊一郎 キャラクター原案：黒獅子</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第12話</t>
+          <t>第1話</t>
         </is>
       </c>
     </row>
@@ -15238,17 +16280,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>はずれスキル念動力（ただしレベルＭＡＸ）で無双する～手をかざすだけです。詠唱とか必殺技とかいりません。念じるだけで倒せます～</t>
+          <t>賢者の孫</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>さとう うなぽっぽ トダフミト</t>
+          <t>緒方俊輔(漫画) 吉岡剛(原作) 菊池政治(キャラクター原案)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>9話②</t>
+          <t>第94話-2</t>
         </is>
       </c>
     </row>
@@ -15258,17 +16300,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ギャルゲーマーに褒められたい</t>
+          <t>めっちゃ召喚された件 THE COMIC</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>げしゅまろ(著者)</t>
+          <t>漫画：六甲島カモメ 原作：さいとうさ キャラクター原案：ツグトク</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>42話</t>
+          <t>第46話②</t>
         </is>
       </c>
     </row>
@@ -15278,17 +16320,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>リビルドワールド</t>
+          <t>レベル１だけどユニークスキルで最強です</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+          <t>漫画：真綿 原作：三木なずな キャラクター原案：すばち</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第71話①</t>
+          <t>第７２話　インドール救援作戦 大成功!?（１）</t>
         </is>
       </c>
     </row>
@@ -15298,17 +16340,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>地味子な三葉さんが僕を誘惑する</t>
+          <t>異世界建国記</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>はぶらえる(著者)</t>
+          <t>ＫＯＩＺＵＭＩ(漫画) 桜木桜(原作) 屡那(キャラクター原案)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第10話前半</t>
+          <t>第77話</t>
         </is>
       </c>
     </row>
@@ -15318,17 +16360,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>サーシャちゃんとクラスメイトオタクくん</t>
+          <t>外れスキル『レベルアップ』のせいでパーティーを追放された少年は、レベルを上げて物理で殴る</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>はぐはぐ(著者)</t>
+          <t>しんこせい 大橋ウルオ てんまそ</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第5話</t>
+          <t>第18話 ミヤダケ（前編）</t>
         </is>
       </c>
     </row>
@@ -15338,17 +16380,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>どれだけ努力しても経験値が入らず万年レベル０の俺は追放された</t>
+          <t>大学入学時から噂されていた美少女三姉妹、生き別れていた義妹だった。</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>原作：蓮池タロウ 漫画：そらモチ</t>
+          <t>こすずめ(著者) 夏乃実(原作) ポメ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第12話</t>
+          <t>今週はスペシャルイラスト！！</t>
         </is>
       </c>
     </row>
@@ -15358,17 +16400,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>魔術師クノンは見えている</t>
+          <t>無能と呼ばれた『精霊たらし』～実は異能で、精霊界では伝説的ヒーローでした～＠COMIC</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+          <t>原作：佐藤謙羊 漫画：タバタグランドキャニオン</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第38話②</t>
+          <t>第27話「求職は総合人材ギルドで」①</t>
         </is>
       </c>
     </row>
@@ -15378,17 +16420,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>勇者に全部奪われた俺は勇者の母親とパーティを組みました！</t>
+          <t>人外姫様、始めました　-Free Life Fantasy Online-</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>久遠まこと(著者) 石のやっさん(原作)</t>
+          <t>園原アオ 割田コマ 子日あきすず Sherry</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第28話</t>
+          <t>第５９話　再チャレンジと思ったら、まさかの冥府へ！（２）</t>
         </is>
       </c>
     </row>
@@ -15398,17 +16440,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>田舎の黒ギャルJKと結婚しました</t>
+          <t>器用貧乏、城を建てる～開拓学園の劣等生なのに、 上級職のスキルと魔法がすべて使えます～＠COMIC</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>カヅチ(著者)</t>
+          <t>原作：佐藤謙羊 漫画：スガン</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第17話前半</t>
+          <t>第21話②「ルールの代償」</t>
         </is>
       </c>
     </row>
@@ -15418,17 +16460,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>オトナを知りたい女友達</t>
+          <t>尾守つみきと奇日常。</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>望公太(原作) ぷよちゃ(作画)</t>
+          <t>森下みゆ</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第7話 後半</t>
+          <t>第58話 雷漸会長と雷。</t>
         </is>
       </c>
     </row>
@@ -15438,17 +16480,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
+          <t>転生少女はまず一歩からはじめたい～魔物がいるとか聞いてない！～</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
+          <t>原作：カヤ 漫画：岡村アユム キャラクター原案：那流</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第1話④</t>
+          <t>第37話 お屋敷での日々①</t>
         </is>
       </c>
     </row>
@@ -15458,17 +16500,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>男子高校生だけどギャルにTSしました</t>
+          <t>魔眼の悪役に転生したので推しキャラを見守るモブを目指します</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>太陽まりい(著者)</t>
+          <t>在間りしん(漫画) 瀧岡くるじ(原作) 福きつね(キャラクター原案)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第18話前編</t>
+          <t>第10話②</t>
         </is>
       </c>
     </row>
@@ -15478,17 +16520,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+          <t>没落予定の貴族だけど、暇だったから魔法を極めてみた@COMIC</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+          <t>漫画：秋咲りお 原作：三木なずな キャラクター原案：かぼちゃ</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>「名もなき英雄譚」前半</t>
+          <t>第52話</t>
         </is>
       </c>
     </row>
@@ -15498,17 +16540,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>金属スライムを倒しまくった俺が【黒鋼の王】と呼ばれるまで</t>
+          <t>レベル１から始まる召喚無双</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>藤屋いずこ(著者) 温泉カピバラ(原作) 山椒魚(キャラクター原案)</t>
+          <t>漫画：七桃りお 原作：白石新 キャラクター原案：夕薙</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第13章-2</t>
+          <t>第32話後半</t>
         </is>
       </c>
     </row>
@@ -15518,17 +16560,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>女友達は頼めば意外とヤらせてくれる</t>
+          <t>狂戦士なモブ、無自覚に本編を破壊する</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>ろくろ(漫画) 鏡遊(原作)</t>
+          <t>漫画：佐藤良亮 原作：なるのるな キャラクター原案：霜月えいと</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>特別イラスト</t>
+          <t>第11話 ②</t>
         </is>
       </c>
     </row>
@@ -15538,17 +16580,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>淫獄団地</t>
+          <t>超!!! 天才発明令嬢のパワフル領地改革</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+          <t>漫画：katoson 原作：守雨</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第48話（後編）</t>
+          <t>第46話</t>
         </is>
       </c>
     </row>
@@ -15558,17 +16600,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>リモート授業になったらクラス１の美少女と同居することになった</t>
+          <t>元最強の剣士は、異世界魔法に憧れる</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>原作：三萩せんや(GA文庫／SBクリエイティブ刊)　漫画：jaguchi　キャラクター原案：さとうぽて</t>
+          <t>漫画：天乃ちはる 原作：紅月シン キャラクター原案：necömi</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第11話</t>
+          <t>第72話後半</t>
         </is>
       </c>
     </row>
@@ -15578,17 +16620,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ミルク搾りハンターの異世界搾乳記～農家の冴えない男があらゆる種族の地区Bを弄び虜にする～</t>
+          <t>アラフォーになった最強の英雄たち、再び戦場で無双する!!</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>空詠大智(著者)</t>
+          <t>漫画：戸田泰成 原作：岸馬きらく 構成協力：森小太郎 キャラクター原案：peroshi</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第16話</t>
+          <t>第23話 後編</t>
         </is>
       </c>
     </row>
@@ -15598,17 +16640,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>不徳のギルド</t>
+          <t>女神から『孵化』のスキルを授かった俺が、なぜか幻獣や神獣を従える最強テイマーになるまで</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>河添太一</t>
+          <t>漫画家：春夏冬 唯人 原作：まるせい</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第９６話：分福</t>
+          <t>第15話</t>
         </is>
       </c>
     </row>
@@ -15618,17 +16660,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>聖液鍛冶屋のエロランタ</t>
+          <t>S級パーティーから追放された狩人、実は世界最強 ～射程9999の男、帝国の狙撃手として無双する～</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>しげきっくす(著者)</t>
+          <t>漫画：カズミヤアキラ 原作：茨木野 キャラクター原案：へいろー</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>休載イラスト</t>
+          <t>第9話 ①</t>
         </is>
       </c>
     </row>
@@ -15638,17 +16680,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ダンジョンの幼なじみ</t>
+          <t>異世界のんびり開拓記  -平凡サラリーマン、万能自在のビルド&amp;クラフトスキルで、気ままなスローライフ 開拓始めます! -</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>久真やすひさ(著者)</t>
+          <t>漫画：しょうじひでまさ 原作：タライ和治 キャラクター原案：イシバシヨウスケ</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第55話</t>
+          <t>第22話 後編</t>
         </is>
       </c>
     </row>
@@ -15658,17 +16700,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>まんきつしたい常連さん</t>
+          <t>寿司ガキ</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>しんみりん(著者)</t>
+          <t>ichika(著者)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第45話後編</t>
+          <t>第9話</t>
         </is>
       </c>
     </row>
@@ -15678,17 +16720,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ソードアート・オンライン Re:Aincrad</t>
+          <t>不純な彼女達は懺悔しない</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>樹深(作画) 佐藤ミト(構成) 川原礫(原作) ａｂｅｃ(キャラクターデザイン)</t>
+          <t>ポロロッカ(著者)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第40話①</t>
+          <t>第28話</t>
         </is>
       </c>
     </row>
@@ -15698,17 +16740,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>スライムテイマーの異世界ライフ</t>
+          <t>クセ強彼女は床にいざなう</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>作画：チイチ 原作：穴の空いた靴下</t>
+          <t>須河篤志(著者)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第7話(1)</t>
+          <t>第13話後半</t>
         </is>
       </c>
     </row>
@@ -15718,17 +16760,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>よくわからないけれど異世界に転生していたようです</t>
+          <t>忌み子と呼ばれた召喚士@COMIC</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>内々けやき あし カオミン</t>
+          <t>漫画：コイシ 原作：緑黄色野菜 キャラクター原案：こよいみつき</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第135話 よくわからないけれど導かれてしまったようです（２）</t>
+          <t>第40話 ②</t>
         </is>
       </c>
     </row>
@@ -15738,17 +16780,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>リアリスト魔王による聖域なき異世界改革</t>
+          <t>ダンジョンバンド</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>鈴木マナツ(漫画) 羽田遼亮(原作) ゆーげん(キャラクターデザイン) ひたきゆう(キャラクターデザイン)</t>
+          <t>新挑限(著者)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第67幕①</t>
+          <t>♯７SPEED TUBE ①</t>
         </is>
       </c>
     </row>
@@ -15758,17 +16800,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>美人女上司滝沢さん</t>
+          <t>ぽんドロイド！ はまさん</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>やんBARU(著者)</t>
+          <t>はれやまはれぞう(著者)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第201話</t>
+          <t>第4話</t>
         </is>
       </c>
     </row>
@@ -15778,17 +16820,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+          <t>ヘテロゲニア リンギスティコ ～異種族言語学入門～</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+          <t>瀬野反人(著者)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第70話(後編) 特別報酬ミッション</t>
+          <t>第56話</t>
         </is>
       </c>
     </row>
@@ -15798,17 +16840,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+          <t>ちはるくんは女装をしたくない！</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>FUNA 東西 モトエ恵介</t>
+          <t>翁丸ジョン</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第119話　会談［その4］</t>
+          <t>【第20話】男装宗と交流したくない！その二</t>
         </is>
       </c>
     </row>
@@ -15818,17 +16860,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>陰キャの俺が席替えでS級美少女に囲まれたら秘密の関係が始まった。</t>
+          <t>千年英雄</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>星野 星野(原作) バラマツヒトミ(漫画) 黒兎 ゆう(キャラクター原案)</t>
+          <t>原作/福島航平 作画/中村ゆきひろ</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第3話</t>
+          <t>18話②</t>
         </is>
       </c>
     </row>
@@ -15838,17 +16880,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>辺境モブ貴族のウチに嫁いできた悪役令嬢が、めちゃくちゃできる良い嫁なんだが？</t>
+          <t>おとなりのダウナーさんは無理させない</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>tera(原作) 朝倉はやて(作画) 徹田(キャラクター原案)</t>
+          <t>瑠璃いろ(著者)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第9話</t>
+          <t>第12話</t>
         </is>
       </c>
     </row>
@@ -15858,17 +16900,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>チュートリアルが始まる前に ボスキャラ達を破滅させない為に俺ができる幾つかの事</t>
+          <t>スライムテイマーの異世界ライフ</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>横山コウヂ(漫画) 髙橋炬燵(原作) カカオ・ランタン(キャラクターデザイン)</t>
+          <t>作画：チイチ 原作：穴の空いた靴下</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第13話②</t>
+          <t>第7話(1)</t>
         </is>
       </c>
     </row>
@@ -15878,17 +16920,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>転生してあらゆるモノに好かれながら異世界で好きな事をして生きて行く</t>
+          <t>魔術師クノンは見えている</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>都尾琉(漫画) 御峰。(原作)</t>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第26話②</t>
+          <t>第38話②</t>
         </is>
       </c>
     </row>
@@ -15898,17 +16940,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>時森さんが無防備です!!</t>
+          <t>リビルドワールド</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>たざわ</t>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第62話</t>
+          <t>第71話①</t>
         </is>
       </c>
     </row>
@@ -15918,17 +16960,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+          <t>地味子な三葉さんが僕を誘惑する</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+          <t>はぶらえる(著者)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第80話その2</t>
+          <t>第10話前半</t>
         </is>
       </c>
     </row>
@@ -15938,17 +16980,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>愚かな天使は悪魔と踊る</t>
+          <t>勇者に全部奪われた俺は勇者の母親とパーティを組みました！</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>アズマサワヨシ(著者)</t>
+          <t>久遠まこと(著者) 石のやっさん(原作)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第100話①</t>
+          <t>第28話</t>
         </is>
       </c>
     </row>
@@ -15958,17 +17000,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>本物のカノジョにしたくなるまで、私で試していいよ。</t>
+          <t>サーシャちゃんとクラスメイトオタクくん</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>wano(漫画) 有丈ほえる(原作) 緋月ひぐれ(キャラクター原案)</t>
+          <t>はぐはぐ(著者)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第8話①</t>
+          <t>第5話</t>
         </is>
       </c>
     </row>
@@ -15978,17 +17020,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ナマケモノ学</t>
+          <t>勇者ディンは2.5回殺せ</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>ハリ</t>
+          <t>ナゲク 福留のりひろ</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第19話　モフモフ断罪裁判</t>
+          <t>第4話「その死は必然」②</t>
         </is>
       </c>
     </row>
@@ -15998,17 +17040,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>ダメ人間の愛しかた</t>
+          <t>女友達は頼めば意外とヤらせてくれる</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>岩葉(著者)</t>
+          <t>ろくろ(漫画) 鏡遊(原作)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第18話前編　ダメ人間とお姉ちゃんと彼女</t>
+          <t>特別イラスト</t>
         </is>
       </c>
     </row>
@@ -16018,17 +17060,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>小さめの魔法師匠と大きめの魔法少女。report：3</t>
+          <t>わたしのために脱ぎなさいっ！</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>とりから</t>
+          <t>九郎(著者)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第37話の2</t>
+          <t>第83話</t>
         </is>
       </c>
     </row>
@@ -16038,17 +17080,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ホームセンターごと呼び出された私の大迷宮リノベーション！</t>
+          <t>淫獄団地</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>ばたっち(漫画) 星崎崑(原作) 志田(キャラクター原案)</t>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第4話後編</t>
+          <t>第48話（後編）</t>
         </is>
       </c>
     </row>
@@ -16058,17 +17100,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>殺されて井戸に捨てられた聖女がチート怨霊になりました</t>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>原作　谷尾銀　漫画　七清水くらげ　ネーム構成　桜井竜矢</t>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第7話　出産④</t>
+          <t>「名もなき英雄譚」前半</t>
         </is>
       </c>
     </row>
@@ -16078,17 +17120,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+          <t>冒険者ギルドが十二歳からしか入れなかったので、サバよみました。</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+          <t>GUNP（漫画） KAME （原作） ox （キャラクター原案）</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第33話②</t>
+          <t>第12話後半</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-07-16
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -30,6 +30,7 @@
     <sheet name="2025-07-13" sheetId="22" state="visible" r:id="rId22"/>
     <sheet name="2025-07-14" sheetId="23" state="visible" r:id="rId23"/>
     <sheet name="2025-07-15" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="2025-07-16" sheetId="25" state="visible" r:id="rId25"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -16135,22 +16136,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>帰ってください！ 阿久津さん</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>長岡太一(著者)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第192話</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第５０話　雌雄を決する器用貧乏（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第２２食　ユクシーさんの覚悟、すごいのですわ！（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第47話 魔導具師とつながれたもの②</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第１８話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>異世界でも無難に生きたい症候群</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>原作：安泰（一二三書房刊） 漫画：笹峰コウ キャラクター原案：ひたきゆう</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第30話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>ギャルとダンジョンと周回遅れの探索英雄譚</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>漫画家： 水田ケンジ 原作：榊一郎 キャラクター原案：黒獅子</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第1話</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>賢者の孫</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>緒方俊輔(漫画) 吉岡剛(原作) 菊池政治(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第94話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>めっちゃ召喚された件 THE COMIC</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>漫画：六甲島カモメ 原作：さいとうさ キャラクター原案：ツグトク</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第46話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>レベル１だけどユニークスキルで最強です</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>漫画：真綿 原作：三木なずな キャラクター原案：すばち</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第７２話　インドール救援作戦 大成功!?（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>異世界建国記</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>ＫＯＩＺＵＭＩ(漫画) 桜木桜(原作) 屡那(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第77話</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>外れスキル『レベルアップ』のせいでパーティーを追放された少年は、レベルを上げて物理で殴る</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>しんこせい 大橋ウルオ てんまそ</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第18話 ミヤダケ（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>大学入学時から噂されていた美少女三姉妹、生き別れていた義妹だった。</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>こすずめ(著者) 夏乃実(原作) ポメ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>今週はスペシャルイラスト！！</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>無能と呼ばれた『精霊たらし』～実は異能で、精霊界では伝説的ヒーローでした～＠COMIC</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>原作：佐藤謙羊 漫画：タバタグランドキャニオン</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第27話「求職は総合人材ギルドで」①</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>人外姫様、始めました　-Free Life Fantasy Online-</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>園原アオ 割田コマ 子日あきすず Sherry</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第５９話　再チャレンジと思ったら、まさかの冥府へ！（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>器用貧乏、城を建てる～開拓学園の劣等生なのに、 上級職のスキルと魔法がすべて使えます～＠COMIC</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>原作：佐藤謙羊 漫画：スガン</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第21話②「ルールの代償」</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>尾守つみきと奇日常。</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>森下みゆ</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第58話 雷漸会長と雷。</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>転生少女はまず一歩からはじめたい～魔物がいるとか聞いてない！～</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>原作：カヤ 漫画：岡村アユム キャラクター原案：那流</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第37話 お屋敷での日々①</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>魔眼の悪役に転生したので推しキャラを見守るモブを目指します</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>在間りしん(漫画) 瀧岡くるじ(原作) 福きつね(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第10話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>没落予定の貴族だけど、暇だったから魔法を極めてみた@COMIC</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>漫画：秋咲りお 原作：三木なずな キャラクター原案：かぼちゃ</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第52話</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>レベル１から始まる召喚無双</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>漫画：七桃りお 原作：白石新 キャラクター原案：夕薙</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第32話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>狂戦士なモブ、無自覚に本編を破壊する</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>漫画：佐藤良亮 原作：なるのるな キャラクター原案：霜月えいと</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第11話 ②</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>超!!! 天才発明令嬢のパワフル領地改革</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>漫画：katoson 原作：守雨</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第46話</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>元最強の剣士は、異世界魔法に憧れる</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>漫画：天乃ちはる 原作：紅月シン キャラクター原案：necömi</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第72話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>アラフォーになった最強の英雄たち、再び戦場で無双する!!</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>漫画：戸田泰成 原作：岸馬きらく 構成協力：森小太郎 キャラクター原案：peroshi</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第23話 後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>女神から『孵化』のスキルを授かった俺が、なぜか幻獣や神獣を従える最強テイマーになるまで</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>漫画家：春夏冬 唯人 原作：まるせい</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第15話</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>S級パーティーから追放された狩人、実は世界最強 ～射程9999の男、帝国の狙撃手として無双する～</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>漫画：カズミヤアキラ 原作：茨木野 キャラクター原案：へいろー</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第9話 ①</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>異世界のんびり開拓記  -平凡サラリーマン、万能自在のビルド&amp;クラフトスキルで、気ままなスローライフ 開拓始めます! -</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>漫画：しょうじひでまさ 原作：タライ和治 キャラクター原案：イシバシヨウスケ</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第22話 後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>寿司ガキ</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>ichika(著者)</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第9話</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>不純な彼女達は懺悔しない</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>ポロロッカ(著者)</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第28話</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>クセ強彼女は床にいざなう</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>須河篤志(著者)</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第13話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>忌み子と呼ばれた召喚士@COMIC</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>漫画：コイシ 原作：緑黄色野菜 キャラクター原案：こよいみつき</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第40話 ②</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>ダンジョンバンド</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>新挑限(著者)</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>♯７SPEED TUBE ①</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>ぽんドロイド！ はまさん</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>はれやまはれぞう(著者)</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第4話</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>ヘテロゲニア リンギスティコ ～異種族言語学入門～</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>瀬野反人(著者)</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第56話</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>ちはるくんは女装をしたくない！</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>翁丸ジョン</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>【第20話】男装宗と交流したくない！その二</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>千年英雄</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>原作/福島航平 作画/中村ゆきひろ</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>18話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>おとなりのダウナーさんは無理させない</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>瑠璃いろ(著者)</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第12話</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>スライムテイマーの異世界ライフ</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>作画：チイチ 原作：穴の空いた靴下</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第7話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>魔術師クノンは見えている</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第38話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第71話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>地味子な三葉さんが僕を誘惑する</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>はぶらえる(著者)</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第10話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>勇者に全部奪われた俺は勇者の母親とパーティを組みました！</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>久遠まこと(著者) 石のやっさん(原作)</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第28話</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>サーシャちゃんとクラスメイトオタクくん</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>はぐはぐ(著者)</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>勇者ディンは2.5回殺せ</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>ナゲク 福留のりひろ</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第4話「その死は必然」②</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>女友達は頼めば意外とヤらせてくれる</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>ろくろ(漫画) 鏡遊(原作)</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>特別イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>わたしのために脱ぎなさいっ！</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>九郎(著者)</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第83話</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>淫獄団地</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第48話（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>「名もなき英雄譚」前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>冒険者ギルドが十二歳からしか入れなかったので、サバよみました。</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>GUNP（漫画） KAME （原作） ox （キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第12話後半</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>帰ってください！ 阿久津さん</t>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>長岡太一(著者)</t>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第192話</t>
+          <t>第30話：一秒の奪い合い③</t>
         </is>
       </c>
     </row>
@@ -16160,17 +17202,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+          <t>光永康則</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第５０話　雌雄を決する器用貧乏（２）</t>
+          <t>第６６話『六花停止』③</t>
         </is>
       </c>
     </row>
@@ -16180,17 +17222,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>島知宏 音速炒飯 有都あらゆる</t>
+          <t>マツモトケンゴ</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第２２食　ユクシーさんの覚悟、すごいのですわ！（２）</t>
+          <t>第６０話　じゃない方の戦いが始まった（２）</t>
         </is>
       </c>
     </row>
@@ -16200,17 +17242,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第47話 魔導具師とつながれたもの②</t>
+          <t>第3話 後編</t>
         </is>
       </c>
     </row>
@@ -16220,17 +17262,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+          <t>板垣恵介 猪原賽 陸井栄史</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第１８話②</t>
+          <t>第76話　海皇戦争</t>
         </is>
       </c>
     </row>
@@ -16240,17 +17282,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>異世界でも無難に生きたい症候群</t>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>原作：安泰（一二三書房刊） 漫画：笹峰コウ キャラクター原案：ひたきゆう</t>
+          <t>戸賀 環 坂木持丸 riritto</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第30話①</t>
+          <t>第49話①　城のパーティーに参加してみた</t>
         </is>
       </c>
     </row>
@@ -16260,17 +17302,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ギャルとダンジョンと周回遅れの探索英雄譚</t>
+          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>漫画家： 水田ケンジ 原作：榊一郎 キャラクター原案：黒獅子</t>
+          <t>板垣恵介 林たかあき</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第1話</t>
+          <t>第50話 愛の試練</t>
         </is>
       </c>
     </row>
@@ -16280,17 +17322,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>賢者の孫</t>
+          <t>10年ぶりに再会したクソガキは清純美少女JKに成長していた</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>緒方俊輔(漫画) 吉岡剛(原作) 菊池政治(キャラクター原案)</t>
+          <t>緑青黒羽（漫画） 館西夕木（原作） ひげ猫（キャラクター原案）</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第94話-2</t>
+          <t>第5話　嫉妬、そして嫉妬（後編）</t>
         </is>
       </c>
     </row>
@@ -16300,17 +17342,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>めっちゃ召喚された件 THE COMIC</t>
+          <t>俺は星間国家の悪徳領主！</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>漫画：六甲島カモメ 原作：さいとうさ キャラクター原案：ツグトク</t>
+          <t>灘島かい（漫画） 三嶋与夢（原作） 高峰ナダレ（キャラクター原案）</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第46話②</t>
+          <t>第39話　自惚れ</t>
         </is>
       </c>
     </row>
@@ -16320,17 +17362,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>レベル１だけどユニークスキルで最強です</t>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>漫画：真綿 原作：三木なずな キャラクター原案：すばち</t>
+          <t>漫画/すたひろ 原作/Y.A</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第７２話　インドール救援作戦 大成功!?（１）</t>
+          <t>chapter66【35話①】</t>
         </is>
       </c>
     </row>
@@ -16340,17 +17382,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>異世界建国記</t>
+          <t>絶対死なないステラ姫</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ＫＯＩＺＵＭＩ(漫画) 桜木桜(原作) 屡那(キャラクター原案)</t>
+          <t>光永康則 大高稲</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第77話</t>
+          <t>第１４話　絶対旅立たない（１）</t>
         </is>
       </c>
     </row>
@@ -16360,17 +17402,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>外れスキル『レベルアップ』のせいでパーティーを追放された少年は、レベルを上げて物理で殴る</t>
+          <t>ひとりぼっちの異世界攻略</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>しんこせい 大橋ウルオ てんまそ</t>
+          <t>びび（漫画） 五示正司（原作）</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第18話 ミヤダケ（前編）</t>
+          <t>第227話　自業自得です</t>
         </is>
       </c>
     </row>
@@ -16380,17 +17422,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>大学入学時から噂されていた美少女三姉妹、生き別れていた義妹だった。</t>
+          <t>サラリーマンが異世界に行ったら四天王になった話</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>こすずめ(著者) 夏乃実(原作) ポメ(キャラクター原案)</t>
+          <t>漫画：村光 原作：ベニガシラ</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>今週はスペシャルイラスト！！</t>
+          <t>第88話　王のシステム</t>
         </is>
       </c>
     </row>
@@ -16400,17 +17442,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>無能と呼ばれた『精霊たらし』～実は異能で、精霊界では伝説的ヒーローでした～＠COMIC</t>
+          <t>世界最強の騎士は、必ず死ぬヒロインを救うため異世界でも最強の騎士となる〜両手に花を、両手に剣を〜</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>原作：佐藤謙羊 漫画：タバタグランドキャニオン</t>
+          <t>KAZU（原作） イソベカズマ（漫画） moino（メカデザイン協力）</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第27話「求職は総合人材ギルドで」①</t>
+          <t>第13話（後編）決断</t>
         </is>
       </c>
     </row>
@@ -16420,17 +17462,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>人外姫様、始めました　-Free Life Fantasy Online-</t>
+          <t>追放者食堂へようこそ！　～最強パーティーを追放された料理人（Lv.99）は、田舎で念願の冒険者食堂を開きます！～</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>園原アオ 割田コマ 子日あきすず Sherry</t>
+          <t>つむみ（漫画） 君川優樹（原作）</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第５９話　再チャレンジと思ったら、まさかの冥府へ！（２）</t>
+          <t>第52話　真心XIII（後編）</t>
         </is>
       </c>
     </row>
@@ -16440,17 +17482,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>器用貧乏、城を建てる～開拓学園の劣等生なのに、 上級職のスキルと魔法がすべて使えます～＠COMIC</t>
+          <t>元最強探索者のおじさん。美少女配信者を助けて大バズりしてしまった。</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>原作：佐藤謙羊 漫画：スガン</t>
+          <t>かなたろー(原作) 草壁レイ(漫画)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第21話②「ルールの代償」</t>
+          <t>第3話　美少女、おじさんにハメられる。④</t>
         </is>
       </c>
     </row>
@@ -16460,17 +17502,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>尾守つみきと奇日常。</t>
+          <t>勇者と魔物の運び屋さん</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>森下みゆ</t>
+          <t>大河原</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第58話 雷漸会長と雷。</t>
+          <t>終章１２</t>
         </is>
       </c>
     </row>
@@ -16480,17 +17522,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>転生少女はまず一歩からはじめたい～魔物がいるとか聞いてない！～</t>
+          <t>江戸前エルフ</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>原作：カヤ 漫画：岡村アユム キャラクター原案：那流</t>
+          <t>樋口彰彦</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第37話 お屋敷での日々①</t>
+          <t>#114</t>
         </is>
       </c>
     </row>
@@ -16500,17 +17542,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>魔眼の悪役に転生したので推しキャラを見守るモブを目指します</t>
+          <t>序盤で死ぬ最強のサブキャラに転生したので、ゲーム知識で無双する</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>在間りしん(漫画) 瀧岡くるじ(原作) 福きつね(キャラクター原案)</t>
+          <t>作画：マエD 原作：新人</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第10話②</t>
+          <t>第4話(4)</t>
         </is>
       </c>
     </row>
@@ -16520,17 +17562,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>没落予定の貴族だけど、暇だったから魔法を極めてみた@COMIC</t>
+          <t>D級冒険者の俺、なぜか勇者パーティーに勧誘されたあげく、王女につきまとわれてる</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>漫画：秋咲りお 原作：三木なずな キャラクター原案：かぼちゃ</t>
+          <t>舘津テト（漫画） 白青虎猫（原作） りいちゅ（キャラクター原案）</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第52話</t>
+          <t>第33話　なぜかどこに逃げても見つかってしまう</t>
         </is>
       </c>
     </row>
@@ -16540,17 +17582,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>レベル１から始まる召喚無双</t>
+          <t>最後のエルフ</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>漫画：七桃りお 原作：白石新 キャラクター原案：夕薙</t>
+          <t>サワノアキラ（漫画）</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第32話後半</t>
+          <t>第9章　竜の眠る地（前編）</t>
         </is>
       </c>
     </row>
@@ -16560,17 +17602,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>狂戦士なモブ、無自覚に本編を破壊する</t>
+          <t>ハニートラップ・シェアハウス</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>漫画：佐藤良亮 原作：なるのるな キャラクター原案：霜月えいと</t>
+          <t>久慈マサムネ(原作) 神月洸壱(作画)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第11話 ②</t>
+          <t>第38話「芸能界にスパイは潜む」②</t>
         </is>
       </c>
     </row>
@@ -16580,17 +17622,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>超!!! 天才発明令嬢のパワフル領地改革</t>
+          <t>絶対に働きたくないダンジョンマスターが惰眠をむさぼるまで</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>漫画：katoson 原作：守雨</t>
+          <t>七六（漫画） 鬼影スパナ（原作） よう太（キャラクター原案）</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第46話</t>
+          <t>第65章　総力戦の行方（後編）</t>
         </is>
       </c>
     </row>
@@ -16600,17 +17642,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>元最強の剣士は、異世界魔法に憧れる</t>
+          <t>エロゲ転生 運命に抗う金豚貴族の奮闘記</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>漫画：天乃ちはる 原作：紅月シン キャラクター原案：necömi</t>
+          <t>奈々鎌土（漫画） 名無しの権兵衛（原作） 星夕（キャラクター原案）</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第72話後半</t>
+          <t>最終フラグ　True End</t>
         </is>
       </c>
     </row>
@@ -16620,17 +17662,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>アラフォーになった最強の英雄たち、再び戦場で無双する!!</t>
+          <t>黒の召喚士</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>漫画：戸田泰成 原作：岸馬きらく 構成協力：森小太郎 キャラクター原案：peroshi</t>
+          <t>天羽 銀（漫画） 迷井豆腐（原作） 黒銀（DIGS）（キャラクター原案）</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第23話 後編</t>
+          <t>第144話　聖槍イクリプスⅤ</t>
         </is>
       </c>
     </row>
@@ -16640,17 +17682,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>女神から『孵化』のスキルを授かった俺が、なぜか幻獣や神獣を従える最強テイマーになるまで</t>
+          <t>帰ってください！ 阿久津さん</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>漫画家：春夏冬 唯人 原作：まるせい</t>
+          <t>長岡太一(著者)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第15話</t>
+          <t>第192話</t>
         </is>
       </c>
     </row>
@@ -16660,17 +17702,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>S級パーティーから追放された狩人、実は世界最強 ～射程9999の男、帝国の狙撃手として無双する～</t>
+          <t>恋人のフリのフリ</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>漫画：カズミヤアキラ 原作：茨木野 キャラクター原案：へいろー</t>
+          <t>むねひろ(著者)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第9話 ①</t>
+          <t>第7話②</t>
         </is>
       </c>
     </row>
@@ -16680,17 +17722,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>異世界のんびり開拓記  -平凡サラリーマン、万能自在のビルド&amp;クラフトスキルで、気ままなスローライフ 開拓始めます! -</t>
+          <t>ゲーム　オブ　ファミリア-家族戦記-</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>漫画：しょうじひでまさ 原作：タライ和治 キャラクター原案：イシバシヨウスケ</t>
+          <t>Ｄ．Ｐ(作画) 山口ミコト(原作)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第22話 後編</t>
+          <t>第73話③</t>
         </is>
       </c>
     </row>
@@ -16700,17 +17742,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>寿司ガキ</t>
+          <t>ギャルゲーマーに褒められたい</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ichika(著者)</t>
+          <t>げしゅまろ(著者)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第9話</t>
+          <t>43話</t>
         </is>
       </c>
     </row>
@@ -16720,17 +17762,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>不純な彼女達は懺悔しない</t>
+          <t>勇者パーティを追放された【スキルサポーター】、仲間のスキルを解放して最強に成り上がる</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>ポロロッカ(著者)</t>
+          <t>作画：なかお 原作：前田氏</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第28話</t>
+          <t>第5話(3)</t>
         </is>
       </c>
     </row>
@@ -16740,17 +17782,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>クセ強彼女は床にいざなう</t>
+          <t>最強の少年聖騎士、転生者を狩る</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>須河篤志(著者)</t>
+          <t>作画：御塩 原作：宇奈木ユラ</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第13話後半</t>
+          <t>第5話(3)</t>
         </is>
       </c>
     </row>
@@ -16760,17 +17802,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>忌み子と呼ばれた召喚士@COMIC</t>
+          <t>ラーメン大好き小泉さん</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>漫画：コイシ 原作：緑黄色野菜 キャラクター原案：こよいみつき</t>
+          <t>鳴見なる</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第40話 ②</t>
+          <t>16杯目 コンビニ</t>
         </is>
       </c>
     </row>
@@ -16780,17 +17822,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ダンジョンバンド</t>
+          <t>傷口と包帯</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>新挑限(著者)</t>
+          <t>七井海星</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>♯７SPEED TUBE ①</t>
+          <t>第14話　新章開幕！　お嬢のマジニー</t>
         </is>
       </c>
     </row>
@@ -16800,17 +17842,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ぽんドロイド！ はまさん</t>
+          <t>ネトゲの嫁が人気アイドルだった　～クール系の彼女は現実でも嫁のつもりでいる～</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>はれやまはれぞう(著者)</t>
+          <t>もっつぉ（漫画） あボーン（原作） 館田ダン（キャラクター原案）</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第4話</t>
+          <t>第30話　人気アイドルと手を繋ぎたい</t>
         </is>
       </c>
     </row>
@@ -16820,17 +17862,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>ヘテロゲニア リンギスティコ ～異種族言語学入門～</t>
+          <t>オークの酒杯に祝福を</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>瀬野反人(著者)</t>
+          <t>かなどめはじめ</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第56話</t>
+          <t>第43話　略奪</t>
         </is>
       </c>
     </row>
@@ -16840,17 +17882,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>ちはるくんは女装をしたくない！</t>
+          <t>無能の中の無能王子　スキル【無能】を授かりましたが、周りの女性は【傾国】【傾城】【奸婦】【毒婦】【悪婦】【妖婦】とかです</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>翁丸ジョン</t>
+          <t>漫画/一夢 原作/福朗 キャラクター原案/菊池政治</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>【第20話】男装宗と交流したくない！その二</t>
+          <t>chapter9【5話②】</t>
         </is>
       </c>
     </row>
@@ -16860,17 +17902,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>千年英雄</t>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>原作/福島航平 作画/中村ゆきひろ</t>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>18話②</t>
+          <t>第５０話　雌雄を決する器用貧乏（２）</t>
         </is>
       </c>
     </row>
@@ -16880,17 +17922,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>おとなりのダウナーさんは無理させない</t>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>瑠璃いろ(著者)</t>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第12話</t>
+          <t>第２２食　ユクシーさんの覚悟、すごいのですわ！（２）</t>
         </is>
       </c>
     </row>
@@ -16900,17 +17942,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>スライムテイマーの異世界ライフ</t>
+          <t>おしかけ勇者嫁 勇者は放逐されたおっさんを追いかけ、スローライフを応援する　コミック版</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>作画：チイチ 原作：穴の空いた靴下</t>
+          <t>漫画/珠洲城くるみ 原作/日富美信吾 キャラクター原案/白井鋭利</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第7話(1)</t>
+          <t>chapter32【16話①】</t>
         </is>
       </c>
     </row>
@@ -16920,17 +17962,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>魔術師クノンは見えている</t>
+          <t>転生したら没落貴族だったので、【呪言】を極めて家族を救います</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+          <t>作画：アマセケイ 原作：メソポ・たみあ</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第38話②</t>
+          <t>第5話(3)</t>
         </is>
       </c>
     </row>
@@ -16940,17 +17982,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>リビルドワールド</t>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第71話①</t>
+          <t>第47話 魔導具師とつながれたもの②</t>
         </is>
       </c>
     </row>
@@ -16960,17 +18002,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>地味子な三葉さんが僕を誘惑する</t>
+          <t>宮廷魔導師、追放される　～無能だと追い出された最巧の魔導師は、部下を引き連れて冒険者クランを始めるようです～</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>はぶらえる(著者)</t>
+          <t>きつね丸（漫画） しんこせい（原作） ろこ（キャラクター原案）</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第10話前半</t>
+          <t>第2話　憧れの人（前編）</t>
         </is>
       </c>
     </row>
@@ -16980,17 +18022,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>勇者に全部奪われた俺は勇者の母親とパーティを組みました！</t>
+          <t>この冒険者、人類史最強です～外れスキル『鑑定』が『継承』に覚醒したので、数多の英雄たちの力を受け継ぎ無双する～</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>久遠まこと(著者) 石のやっさん(原作)</t>
+          <t>日之影ソラ みやけりく エシュアル</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第28話</t>
+          <t>第27話②双子の錬金術師</t>
         </is>
       </c>
     </row>
@@ -17000,17 +18042,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>サーシャちゃんとクラスメイトオタクくん</t>
+          <t>最凶貴族は死亡フラグを覆す</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>はぐはぐ(著者)</t>
+          <t>作画：sudekuma 原作：塚上</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第5話</t>
+          <t>第5話(3)</t>
         </is>
       </c>
     </row>
@@ -17020,17 +18062,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>勇者ディンは2.5回殺せ</t>
+          <t>信者ゼロの女神サマと始める異世界攻略</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>ナゲク 福留のりひろ</t>
+          <t>しろいはくと（漫画） 大崎アイル（原作） Tam-U（キャラクター原案）</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第4話「その死は必然」②</t>
+          <t>第43話　桜井リョウスケの思い出</t>
         </is>
       </c>
     </row>
@@ -17040,17 +18082,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>女友達は頼めば意外とヤらせてくれる</t>
+          <t>弱小国家の英雄王子　～最強の魔術師だけど、さっさと国出て自由に生きてぇぇ！～</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>ろくろ(漫画) 鏡遊(原作)</t>
+          <t>友山アキ（漫画） 楓原こうた（原作） トモゼロ（キャラクター原案）</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>特別イラスト</t>
+          <t>第3話　第一皇女護衛戦Ⅱ（後編）</t>
         </is>
       </c>
     </row>
@@ -17060,17 +18102,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>わたしのために脱ぎなさいっ！</t>
+          <t>俺の前世の知識で底辺職テイマーが上級職になってしまいそうな件</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>九郎(著者)</t>
+          <t>にわリズム（漫画） 可換 環（原作） カット（キャラクター原案）</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第83話</t>
+          <t>第45話　予想外の参加者がいた！</t>
         </is>
       </c>
     </row>
@@ -17080,17 +18122,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>淫獄団地</t>
+          <t>元勇者、今はアイドルのドライバーやってます</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+          <t>十本スイ(原作) 舞鶴山画太郎(漫画)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第48話（後編）</t>
+          <t>第6話-1</t>
         </is>
       </c>
     </row>
@@ -17100,17 +18142,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+          <t>無気力ニートな元神童、冒険者になる</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+          <t>緑茶こいめ（漫画） ぺもぺもさん（原作） 福きつね（原作イラスト）</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>「名もなき英雄譚」前半</t>
+          <t>第50話　スタンピード！Ⅰ</t>
         </is>
       </c>
     </row>
@@ -17120,17 +18162,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>冒険者ギルドが十二歳からしか入れなかったので、サバよみました。</t>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>GUNP（漫画） KAME （原作） ox （キャラクター原案）</t>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第12話後半</t>
+          <t>第１８話②</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-07-17
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -31,6 +31,7 @@
     <sheet name="2025-07-14" sheetId="23" state="visible" r:id="rId23"/>
     <sheet name="2025-07-15" sheetId="24" state="visible" r:id="rId24"/>
     <sheet name="2025-07-16" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="2025-07-17" sheetId="26" state="visible" r:id="rId26"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -17177,22 +17178,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第30話：一秒の奪い合い③</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第６６話『六花停止』③</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>マツモトケンゴ</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第６０話　じゃない方の戦いが始まった（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第3話 後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>板垣恵介 猪原賽 陸井栄史</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第76話　海皇戦争</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>戸賀 環 坂木持丸 riritto</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第49話①　城のパーティーに参加してみた</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>板垣恵介 林たかあき</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第50話 愛の試練</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>10年ぶりに再会したクソガキは清純美少女JKに成長していた</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>緑青黒羽（漫画） 館西夕木（原作） ひげ猫（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第5話　嫉妬、そして嫉妬（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>俺は星間国家の悪徳領主！</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>灘島かい（漫画） 三嶋与夢（原作） 高峰ナダレ（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第39話　自惚れ</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>漫画/すたひろ 原作/Y.A</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>chapter66【35話①】</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>絶対死なないステラ姫</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>光永康則 大高稲</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第１４話　絶対旅立たない（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>ひとりぼっちの異世界攻略</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>びび（漫画） 五示正司（原作）</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第227話　自業自得です</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>サラリーマンが異世界に行ったら四天王になった話</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>漫画：村光 原作：ベニガシラ</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第88話　王のシステム</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>世界最強の騎士は、必ず死ぬヒロインを救うため異世界でも最強の騎士となる〜両手に花を、両手に剣を〜</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>KAZU（原作） イソベカズマ（漫画） moino（メカデザイン協力）</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第13話（後編）決断</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>追放者食堂へようこそ！　～最強パーティーを追放された料理人（Lv.99）は、田舎で念願の冒険者食堂を開きます！～</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>つむみ（漫画） 君川優樹（原作）</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第52話　真心XIII（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>元最強探索者のおじさん。美少女配信者を助けて大バズりしてしまった。</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>かなたろー(原作) 草壁レイ(漫画)</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第3話　美少女、おじさんにハメられる。④</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>勇者と魔物の運び屋さん</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>大河原</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>終章１２</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>江戸前エルフ</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>樋口彰彦</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>#114</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>序盤で死ぬ最強のサブキャラに転生したので、ゲーム知識で無双する</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>作画：マエD 原作：新人</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第4話(4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>D級冒険者の俺、なぜか勇者パーティーに勧誘されたあげく、王女につきまとわれてる</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>舘津テト（漫画） 白青虎猫（原作） りいちゅ（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第33話　なぜかどこに逃げても見つかってしまう</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>最後のエルフ</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>サワノアキラ（漫画）</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第9章　竜の眠る地（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>ハニートラップ・シェアハウス</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>久慈マサムネ(原作) 神月洸壱(作画)</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第38話「芸能界にスパイは潜む」②</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>絶対に働きたくないダンジョンマスターが惰眠をむさぼるまで</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>七六（漫画） 鬼影スパナ（原作） よう太（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第65章　総力戦の行方（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>エロゲ転生 運命に抗う金豚貴族の奮闘記</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>奈々鎌土（漫画） 名無しの権兵衛（原作） 星夕（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>最終フラグ　True End</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>黒の召喚士</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>天羽 銀（漫画） 迷井豆腐（原作） 黒銀（DIGS）（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第144話　聖槍イクリプスⅤ</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>帰ってください！ 阿久津さん</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>長岡太一(著者)</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第192話</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>恋人のフリのフリ</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>むねひろ(著者)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第7話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>ゲーム　オブ　ファミリア-家族戦記-</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>Ｄ．Ｐ(作画) 山口ミコト(原作)</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第73話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>ギャルゲーマーに褒められたい</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>げしゅまろ(著者)</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>43話</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追放された【スキルサポーター】、仲間のスキルを解放して最強に成り上がる</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>作画：なかお 原作：前田氏</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第5話(3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>最強の少年聖騎士、転生者を狩る</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>作画：御塩 原作：宇奈木ユラ</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第5話(3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>ラーメン大好き小泉さん</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>鳴見なる</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>16杯目 コンビニ</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>傷口と包帯</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>七井海星</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第14話　新章開幕！　お嬢のマジニー</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>ネトゲの嫁が人気アイドルだった　～クール系の彼女は現実でも嫁のつもりでいる～</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>もっつぉ（漫画） あボーン（原作） 館田ダン（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第30話　人気アイドルと手を繋ぎたい</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>オークの酒杯に祝福を</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>かなどめはじめ</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第43話　略奪</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>無能の中の無能王子　スキル【無能】を授かりましたが、周りの女性は【傾国】【傾城】【奸婦】【毒婦】【悪婦】【妖婦】とかです</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>漫画/一夢 原作/福朗 キャラクター原案/菊池政治</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>chapter9【5話②】</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第５０話　雌雄を決する器用貧乏（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第２２食　ユクシーさんの覚悟、すごいのですわ！（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>おしかけ勇者嫁 勇者は放逐されたおっさんを追いかけ、スローライフを応援する　コミック版</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>漫画/珠洲城くるみ 原作/日富美信吾 キャラクター原案/白井鋭利</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>chapter32【16話①】</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>転生したら没落貴族だったので、【呪言】を極めて家族を救います</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>作画：アマセケイ 原作：メソポ・たみあ</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第5話(3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第47話 魔導具師とつながれたもの②</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>宮廷魔導師、追放される　～無能だと追い出された最巧の魔導師は、部下を引き連れて冒険者クランを始めるようです～</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>きつね丸（漫画） しんこせい（原作） ろこ（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第2話　憧れの人（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>この冒険者、人類史最強です～外れスキル『鑑定』が『継承』に覚醒したので、数多の英雄たちの力を受け継ぎ無双する～</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>日之影ソラ みやけりく エシュアル</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第27話②双子の錬金術師</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>最凶貴族は死亡フラグを覆す</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>作画：sudekuma 原作：塚上</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第5話(3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>信者ゼロの女神サマと始める異世界攻略</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>しろいはくと（漫画） 大崎アイル（原作） Tam-U（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第43話　桜井リョウスケの思い出</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>弱小国家の英雄王子　～最強の魔術師だけど、さっさと国出て自由に生きてぇぇ！～</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>友山アキ（漫画） 楓原こうた（原作） トモゼロ（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第3話　第一皇女護衛戦Ⅱ（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>俺の前世の知識で底辺職テイマーが上級職になってしまいそうな件</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>にわリズム（漫画） 可換 環（原作） カット（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第45話　予想外の参加者がいた！</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>元勇者、今はアイドルのドライバーやってます</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>十本スイ(原作) 舞鶴山画太郎(漫画)</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第6話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>無気力ニートな元神童、冒険者になる</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>緑茶こいめ（漫画） ぺもぺもさん（原作） 福きつね（原作イラスト）</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第50話　スタンピード！Ⅰ</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第１８話②</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+          <t>異世界おじさん</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>zunta(作画) はらわたさいぞう(原作)</t>
+          <t>殆ど死んでいる(著者)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第30話：一秒の奪い合い③</t>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
@@ -17202,17 +18244,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>光永康則</t>
+          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第６６話『六花停止』③</t>
+          <t>第76話その2</t>
         </is>
       </c>
     </row>
@@ -17222,17 +18264,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>マツモトケンゴ</t>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第６０話　じゃない方の戦いが始まった（２）</t>
+          <t>第126話　戦争を終わらせてみるⅡ（後編）</t>
         </is>
       </c>
     </row>
@@ -17242,17 +18284,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+          <t>実は俺、最強でした？</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第3話 後編</t>
+          <t>おまけ63</t>
         </is>
       </c>
     </row>
@@ -17262,17 +18304,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>板垣恵介 猪原賽 陸井栄史</t>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第76話　海皇戦争</t>
+          <t>第32話 独身貴族は森で写真を撮る（1）</t>
         </is>
       </c>
     </row>
@@ -17282,17 +18324,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+          <t>聖者無双</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>戸賀 環 坂木持丸 riritto</t>
+          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第49話①　城のパーティーに参加してみた</t>
+          <t>第90話　研究者や技術者の故郷（後半）</t>
         </is>
       </c>
     </row>
@@ -17302,17 +18344,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
+          <t>王子様の友達</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>板垣恵介 林たかあき</t>
+          <t>すけろく(著者)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第50話 愛の試練</t>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
@@ -17322,17 +18364,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>10年ぶりに再会したクソガキは清純美少女JKに成長していた</t>
+          <t>生徒会にも穴はある！</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>緑青黒羽（漫画） 館西夕木（原作） ひげ猫（キャラクター原案）</t>
+          <t>むちまろ</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第5話　嫉妬、そして嫉妬（後編）</t>
+          <t>第131話	ありす大ピンチ！（デジャブ編）</t>
         </is>
       </c>
     </row>
@@ -17342,17 +18384,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>俺は星間国家の悪徳領主！</t>
+          <t>オタクに優しいギャルはいない!?</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>灘島かい（漫画） 三嶋与夢（原作） 高峰ナダレ（キャラクター原案）</t>
+          <t>のりしろちゃん 魚住さかな</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第39話　自惚れ</t>
+          <t>【#148】氷の笑み</t>
         </is>
       </c>
     </row>
@@ -17362,17 +18404,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+          <t>魔法少女リリカルなのは EXCEEDS</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>漫画/すたひろ 原作/Y.A</t>
+          <t>都築真紀 川上修一</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>chapter66【35話①】</t>
+          <t>第４話①</t>
         </is>
       </c>
     </row>
@@ -17382,17 +18424,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>絶対死なないステラ姫</t>
+          <t>脇役に転生したはずが、いつの間にか伝説の錬金術師になってた～仲間たちが英雄でも俺は支援職なんだが～</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>光永康則 大高稲</t>
+          <t>神無月みり 相野 仁</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第１４話　絶対旅立たない（１）</t>
+          <t>第２６話　脇役、目論見を見破る（１）</t>
         </is>
       </c>
     </row>
@@ -17402,17 +18444,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>ひとりぼっちの異世界攻略</t>
+          <t>ひげを剃る。そして女子高生を拾う。</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>びび（漫画） 五示正司（原作）</t>
+          <t>足立いまる(漫画) しめさば(原作) ぶーた(キャラクター原案)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第227話　自業自得です</t>
+          <t>第65話その1</t>
         </is>
       </c>
     </row>
@@ -17422,17 +18464,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>サラリーマンが異世界に行ったら四天王になった話</t>
+          <t>カナン様はあくまでチョロい</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>漫画：村光 原作：ベニガシラ</t>
+          <t>nonco</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第88話　王のシステム</t>
+          <t>第142話	アミのパジャマパーティ女子会</t>
         </is>
       </c>
     </row>
@@ -17442,17 +18484,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>世界最強の騎士は、必ず死ぬヒロインを救うため異世界でも最強の騎士となる〜両手に花を、両手に剣を〜</t>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>KAZU（原作） イソベカズマ（漫画） moino（メカデザイン協力）</t>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第13話（後編）決断</t>
+          <t>第3話 後編</t>
         </is>
       </c>
     </row>
@@ -17462,17 +18504,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>追放者食堂へようこそ！　～最強パーティーを追放された料理人（Lv.99）は、田舎で念願の冒険者食堂を開きます！～</t>
+          <t>魔王討伐したあと、目立ちたくないのでギルドマスターになった</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>つむみ（漫画） 君川優樹（原作）</t>
+          <t>ＲＯＨＧＵＮ(作画) 朱月十話(原作) 鳴瀬ひろふみ(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第52話　真心XIII（後編）</t>
+          <t>第65話-②</t>
         </is>
       </c>
     </row>
@@ -17482,17 +18524,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>元最強探索者のおじさん。美少女配信者を助けて大バズりしてしまった。</t>
+          <t>すべての人類を破壊する。それらは再生できない。</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>かなたろー(原作) 草壁レイ(漫画)</t>
+          <t>横田卓馬(漫画) 伊瀬勝良(原作)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第3話　美少女、おじさんにハメられる。④</t>
+          <t>第66話その3</t>
         </is>
       </c>
     </row>
@@ -17502,17 +18544,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>勇者と魔物の運び屋さん</t>
+          <t>勇者は魔王が好きらしい</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>大河原</t>
+          <t>赤槻コウ(著者)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>終章１２</t>
+          <t>第4話-2：激闘！サキュバス戦！</t>
         </is>
       </c>
     </row>
@@ -17522,17 +18564,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>江戸前エルフ</t>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>樋口彰彦</t>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>#114</t>
+          <t>第30話：一秒の奪い合い③</t>
         </is>
       </c>
     </row>
@@ -17542,17 +18584,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>序盤で死ぬ最強のサブキャラに転生したので、ゲーム知識で無双する</t>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>作画：マエD 原作：新人</t>
+          <t>光永康則</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第4話(4)</t>
+          <t>第６６話『六花停止』③</t>
         </is>
       </c>
     </row>
@@ -17562,17 +18604,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>D級冒険者の俺、なぜか勇者パーティーに勧誘されたあげく、王女につきまとわれてる</t>
+          <t>よわよわ先生</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>舘津テト（漫画） 白青虎猫（原作） りいちゅ（キャラクター原案）</t>
+          <t>福地カミオ</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第33話　なぜかどこに逃げても見つかってしまう</t>
+          <t>第107話	ゆりゆりとドヘンタイと真実</t>
         </is>
       </c>
     </row>
@@ -17582,17 +18624,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>最後のエルフ</t>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>サワノアキラ（漫画）</t>
+          <t>マツモトケンゴ</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第9章　竜の眠る地（前編）</t>
+          <t>第６０話　じゃない方の戦いが始まった（２）</t>
         </is>
       </c>
     </row>
@@ -17602,17 +18644,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ハニートラップ・シェアハウス</t>
+          <t>善人おっさん、生まれ変わったらSSSランク人生が確定した</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>久慈マサムネ(原作) 神月洸壱(作画)</t>
+          <t>原作／三木なずな 漫画／ゆづましろ キャラクター原案／伍長</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第38話「芸能界にスパイは潜む」②</t>
+          <t>第133話</t>
         </is>
       </c>
     </row>
@@ -17622,17 +18664,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>絶対に働きたくないダンジョンマスターが惰眠をむさぼるまで</t>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>七六（漫画） 鬼影スパナ（原作） よう太（キャラクター原案）</t>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第65章　総力戦の行方（後編）</t>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
@@ -17642,17 +18684,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>エロゲ転生 運命に抗う金豚貴族の奮闘記</t>
+          <t>織田家の長男に生まれました 〜戦国時代に転生したけど、死にたくないので改革を起こします〜</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>奈々鎌土（漫画） 名無しの権兵衛（原作） 星夕（キャラクター原案）</t>
+          <t>大沼田伊勢彦 逸見兎歌 平沢下戸</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>最終フラグ　True End</t>
+          <t>第33話「私的な会話」①</t>
         </is>
       </c>
     </row>
@@ -17662,17 +18704,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>黒の召喚士</t>
+          <t>百瀬アキラの初恋破綻中。</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>天羽 銀（漫画） 迷井豆腐（原作） 黒銀（DIGS）（キャラクター原案）</t>
+          <t>晴川シンタ</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第144話　聖槍イクリプスⅤ</t>
+          <t>第31話 2つの危機に対面中。</t>
         </is>
       </c>
     </row>
@@ -17682,17 +18724,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>帰ってください！ 阿久津さん</t>
+          <t>昔滅びた魔王城で拾った犬は、実は伝説の魔獣でした ～隠れ最強職《羊飼い》な貴族の三男坊、いずれ、百魔獣の王となる～</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>長岡太一(著者)</t>
+          <t>あまうい白一 鍋島テツヒロ 松本蓮士</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第192話</t>
+          <t>第12話  殲滅するものと、抗うもの</t>
         </is>
       </c>
     </row>
@@ -17702,17 +18744,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>恋人のフリのフリ</t>
+          <t>生徒会役員共</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>むねひろ(著者)</t>
+          <t>氏家ト全</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第7話②</t>
+          <t>#405</t>
         </is>
       </c>
     </row>
@@ -17722,17 +18764,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ゲーム　オブ　ファミリア-家族戦記-</t>
+          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Ｄ．Ｐ(作画) 山口ミコト(原作)</t>
+          <t>板垣恵介 猪原賽 陸井栄史</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第73話③</t>
+          <t>第76話　海皇戦争</t>
         </is>
       </c>
     </row>
@@ -17742,17 +18784,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ギャルゲーマーに褒められたい</t>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>げしゅまろ(著者)</t>
+          <t>戸賀 環 坂木持丸 riritto</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>43話</t>
+          <t>第49話①　城のパーティーに参加してみた</t>
         </is>
       </c>
     </row>
@@ -17762,17 +18804,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>勇者パーティを追放された【スキルサポーター】、仲間のスキルを解放して最強に成り上がる</t>
+          <t>303号室の神さま</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>作画：なかお 原作：前田氏</t>
+          <t>ふに・無9(著者)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第5話(3)</t>
+          <t>Episode. 19</t>
         </is>
       </c>
     </row>
@@ -17782,17 +18824,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>最強の少年聖騎士、転生者を狩る</t>
+          <t>10年ぶりに再会したクソガキは清純美少女JKに成長していた</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>作画：御塩 原作：宇奈木ユラ</t>
+          <t>緑青黒羽（漫画） 館西夕木（原作） ひげ猫（キャラクター原案）</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第5話(3)</t>
+          <t>第5話　嫉妬、そして嫉妬（後編）</t>
         </is>
       </c>
     </row>
@@ -17802,17 +18844,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ラーメン大好き小泉さん</t>
+          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>鳴見なる</t>
+          <t>板垣恵介 林たかあき</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>16杯目 コンビニ</t>
+          <t>第50話 愛の試練</t>
         </is>
       </c>
     </row>
@@ -17822,17 +18864,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>傷口と包帯</t>
+          <t>学食ガール</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>七井海星</t>
+          <t>杉本 萌</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第14話　新章開幕！　お嬢のマジニー</t>
+          <t>＃01タルタルソースとコールスロー</t>
         </is>
       </c>
     </row>
@@ -17842,17 +18884,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ネトゲの嫁が人気アイドルだった　～クール系の彼女は現実でも嫁のつもりでいる～</t>
+          <t>勇者と魔物の運び屋さん</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>もっつぉ（漫画） あボーン（原作） 館田ダン（キャラクター原案）</t>
+          <t>大河原</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第30話　人気アイドルと手を繋ぎたい</t>
+          <t>終章１２</t>
         </is>
       </c>
     </row>
@@ -17862,17 +18904,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>オークの酒杯に祝福を</t>
+          <t>俺は星間国家の悪徳領主！</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>かなどめはじめ</t>
+          <t>灘島かい（漫画） 三嶋与夢（原作） 高峰ナダレ（キャラクター原案）</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第43話　略奪</t>
+          <t>第39話　自惚れ</t>
         </is>
       </c>
     </row>
@@ -17882,17 +18924,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>無能の中の無能王子　スキル【無能】を授かりましたが、周りの女性は【傾国】【傾城】【奸婦】【毒婦】【悪婦】【妖婦】とかです</t>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>漫画/一夢 原作/福朗 キャラクター原案/菊池政治</t>
+          <t>漫画/すたひろ 原作/Y.A</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>chapter9【5話②】</t>
+          <t>chapter66【35話①】</t>
         </is>
       </c>
     </row>
@@ -17902,17 +18944,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+          <t>絶対死なないステラ姫</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+          <t>光永康則 大高稲</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第５０話　雌雄を決する器用貧乏（２）</t>
+          <t>第１４話　絶対旅立たない（１）</t>
         </is>
       </c>
     </row>
@@ -17922,17 +18964,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+          <t>ひとりぼっちの異世界攻略</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>島知宏 音速炒飯 有都あらゆる</t>
+          <t>びび（漫画） 五示正司（原作）</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第２２食　ユクシーさんの覚悟、すごいのですわ！（２）</t>
+          <t>第227話　自業自得です</t>
         </is>
       </c>
     </row>
@@ -17942,17 +18984,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>おしかけ勇者嫁 勇者は放逐されたおっさんを追いかけ、スローライフを応援する　コミック版</t>
+          <t>アンゴルモア 元寇合戦記　【博多編】</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>漫画/珠洲城くるみ 原作/日富美信吾 キャラクター原案/白井鋭利</t>
+          <t>たかぎ七彦(著者)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>chapter32【16話①】</t>
+          <t>第四十四話その五</t>
         </is>
       </c>
     </row>
@@ -17962,17 +19004,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>転生したら没落貴族だったので、【呪言】を極めて家族を救います</t>
+          <t>ゴリラ女子高生</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>作画：アマセケイ 原作：メソポ・たみあ</t>
+          <t>大友しゅうま(著者)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第5話(3)</t>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
@@ -17982,17 +19024,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
+          <t>サラリーマンが異世界に行ったら四天王になった話</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
+          <t>漫画：村光 原作：ベニガシラ</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第47話 魔導具師とつながれたもの②</t>
+          <t>第88話　王のシステム</t>
         </is>
       </c>
     </row>
@@ -18002,17 +19044,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>宮廷魔導師、追放される　～無能だと追い出された最巧の魔導師は、部下を引き連れて冒険者クランを始めるようです～</t>
+          <t>帰ってください！ 阿久津さん</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>きつね丸（漫画） しんこせい（原作） ろこ（キャラクター原案）</t>
+          <t>長岡太一(著者)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第2話　憧れの人（前編）</t>
+          <t>第192話</t>
         </is>
       </c>
     </row>
@@ -18022,17 +19064,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>この冒険者、人類史最強です～外れスキル『鑑定』が『継承』に覚醒したので、数多の英雄たちの力を受け継ぎ無双する～</t>
+          <t>ロードマギアの弟子</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>日之影ソラ みやけりく エシュアル</t>
+          <t>FLIPFLOPs</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第27話②双子の錬金術師</t>
+          <t>第18話 魔術師の戦い (前編)</t>
         </is>
       </c>
     </row>
@@ -18042,17 +19084,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>最凶貴族は死亡フラグを覆す</t>
+          <t>黒月のイェルクナハト</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>作画：sudekuma 原作：塚上</t>
+          <t>スズモトコウ</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第5話(3)</t>
+          <t>第5話	思いの儘に</t>
         </is>
       </c>
     </row>
@@ -18062,17 +19104,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>信者ゼロの女神サマと始める異世界攻略</t>
+          <t>序盤で死ぬ最強のサブキャラに転生したので、ゲーム知識で無双する</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>しろいはくと（漫画） 大崎アイル（原作） Tam-U（キャラクター原案）</t>
+          <t>作画：マエD 原作：新人</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第43話　桜井リョウスケの思い出</t>
+          <t>第4話(4)</t>
         </is>
       </c>
     </row>
@@ -18082,17 +19124,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>弱小国家の英雄王子　～最強の魔術師だけど、さっさと国出て自由に生きてぇぇ！～</t>
+          <t>世界最強の騎士は、必ず死ぬヒロインを救うため異世界でも最強の騎士となる〜両手に花を、両手に剣を〜</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>友山アキ（漫画） 楓原こうた（原作） トモゼロ（キャラクター原案）</t>
+          <t>KAZU（原作） イソベカズマ（漫画） moino（メカデザイン協力）</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第3話　第一皇女護衛戦Ⅱ（後編）</t>
+          <t>第13話（後編）決断</t>
         </is>
       </c>
     </row>
@@ -18102,17 +19144,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>俺の前世の知識で底辺職テイマーが上級職になってしまいそうな件</t>
+          <t>最後のエルフ</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>にわリズム（漫画） 可換 環（原作） カット（キャラクター原案）</t>
+          <t>サワノアキラ（漫画）</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第45話　予想外の参加者がいた！</t>
+          <t>第9章　竜の眠る地（前編）</t>
         </is>
       </c>
     </row>
@@ -18122,17 +19164,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>元勇者、今はアイドルのドライバーやってます</t>
+          <t>追放者食堂へようこそ！　～最強パーティーを追放された料理人（Lv.99）は、田舎で念願の冒険者食堂を開きます！～</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>十本スイ(原作) 舞鶴山画太郎(漫画)</t>
+          <t>つむみ（漫画） 君川優樹（原作）</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第6話-1</t>
+          <t>第52話　真心XIII（後編）</t>
         </is>
       </c>
     </row>
@@ -18142,17 +19184,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>無気力ニートな元神童、冒険者になる</t>
+          <t>色憑くモノクローム</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>緑茶こいめ（漫画） ぺもぺもさん（原作） 福きつね（原作イラスト）</t>
+          <t>内山敦司</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第50話　スタンピード！Ⅰ</t>
+          <t>第37話	猫娘と勝負!!</t>
         </is>
       </c>
     </row>
@@ -18162,17 +19204,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+          <t>元最強探索者のおじさん。美少女配信者を助けて大バズりしてしまった。</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+          <t>かなたろー(原作) 草壁レイ(漫画)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第１８話②</t>
+          <t>第3話　美少女、おじさんにハメられる。④</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-07-18
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -32,6 +32,7 @@
     <sheet name="2025-07-15" sheetId="24" state="visible" r:id="rId24"/>
     <sheet name="2025-07-16" sheetId="25" state="visible" r:id="rId25"/>
     <sheet name="2025-07-17" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="2025-07-18" sheetId="27" state="visible" r:id="rId27"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -18219,22 +18220,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>異世界おじさん</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>殆ど死んでいる(著者)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第76話その2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第126話　戦争を終わらせてみるⅡ（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>おまけ63</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第32話 独身貴族は森で写真を撮る（1）</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>聖者無双</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第90話　研究者や技術者の故郷（後半）</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>王子様の友達</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>すけろく(著者)</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>生徒会にも穴はある！</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>むちまろ</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第131話	ありす大ピンチ！（デジャブ編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>オタクに優しいギャルはいない!?</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>のりしろちゃん 魚住さかな</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>【#148】氷の笑み</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>魔法少女リリカルなのは EXCEEDS</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>都築真紀 川上修一</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第４話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>脇役に転生したはずが、いつの間にか伝説の錬金術師になってた～仲間たちが英雄でも俺は支援職なんだが～</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>神無月みり 相野 仁</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第２６話　脇役、目論見を見破る（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>ひげを剃る。そして女子高生を拾う。</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>足立いまる(漫画) しめさば(原作) ぶーた(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第65話その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>カナン様はあくまでチョロい</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>nonco</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第142話	アミのパジャマパーティ女子会</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第3話 後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>魔王討伐したあと、目立ちたくないのでギルドマスターになった</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>ＲＯＨＧＵＮ(作画) 朱月十話(原作) 鳴瀬ひろふみ(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第65話-②</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>すべての人類を破壊する。それらは再生できない。</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>横田卓馬(漫画) 伊瀬勝良(原作)</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第66話その3</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>勇者は魔王が好きらしい</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>赤槻コウ(著者)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第4話-2：激闘！サキュバス戦！</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第30話：一秒の奪い合い③</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第６６話『六花停止』③</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>よわよわ先生</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>福地カミオ</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第107話	ゆりゆりとドヘンタイと真実</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>マツモトケンゴ</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第６０話　じゃない方の戦いが始まった（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>善人おっさん、生まれ変わったらSSSランク人生が確定した</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>原作／三木なずな 漫画／ゆづましろ キャラクター原案／伍長</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第133話</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>織田家の長男に生まれました 〜戦国時代に転生したけど、死にたくないので改革を起こします〜</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>大沼田伊勢彦 逸見兎歌 平沢下戸</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第33話「私的な会話」①</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>百瀬アキラの初恋破綻中。</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>晴川シンタ</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第31話 2つの危機に対面中。</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>昔滅びた魔王城で拾った犬は、実は伝説の魔獣でした ～隠れ最強職《羊飼い》な貴族の三男坊、いずれ、百魔獣の王となる～</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>あまうい白一 鍋島テツヒロ 松本蓮士</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第12話  殲滅するものと、抗うもの</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>生徒会役員共</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>氏家ト全</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>#405</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>板垣恵介 猪原賽 陸井栄史</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第76話　海皇戦争</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>戸賀 環 坂木持丸 riritto</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第49話①　城のパーティーに参加してみた</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>303号室の神さま</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>ふに・無9(著者)</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>Episode. 19</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>10年ぶりに再会したクソガキは清純美少女JKに成長していた</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>緑青黒羽（漫画） 館西夕木（原作） ひげ猫（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第5話　嫉妬、そして嫉妬（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>板垣恵介 林たかあき</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第50話 愛の試練</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>学食ガール</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>杉本 萌</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>＃01タルタルソースとコールスロー</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>勇者と魔物の運び屋さん</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>大河原</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>終章１２</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>俺は星間国家の悪徳領主！</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>灘島かい（漫画） 三嶋与夢（原作） 高峰ナダレ（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第39話　自惚れ</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>漫画/すたひろ 原作/Y.A</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>chapter66【35話①】</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>絶対死なないステラ姫</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>光永康則 大高稲</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第１４話　絶対旅立たない（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>ひとりぼっちの異世界攻略</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>びび（漫画） 五示正司（原作）</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第227話　自業自得です</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>アンゴルモア 元寇合戦記　【博多編】</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>たかぎ七彦(著者)</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第四十四話その五</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>ゴリラ女子高生</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>大友しゅうま(著者)</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>サラリーマンが異世界に行ったら四天王になった話</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>漫画：村光 原作：ベニガシラ</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第88話　王のシステム</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>帰ってください！ 阿久津さん</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>長岡太一(著者)</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第192話</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>ロードマギアの弟子</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>FLIPFLOPs</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第18話 魔術師の戦い (前編)</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>黒月のイェルクナハト</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>スズモトコウ</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第5話	思いの儘に</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>序盤で死ぬ最強のサブキャラに転生したので、ゲーム知識で無双する</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>作画：マエD 原作：新人</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第4話(4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>世界最強の騎士は、必ず死ぬヒロインを救うため異世界でも最強の騎士となる〜両手に花を、両手に剣を〜</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>KAZU（原作） イソベカズマ（漫画） moino（メカデザイン協力）</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第13話（後編）決断</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>最後のエルフ</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>サワノアキラ（漫画）</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第9章　竜の眠る地（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>追放者食堂へようこそ！　～最強パーティーを追放された料理人（Lv.99）は、田舎で念願の冒険者食堂を開きます！～</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>つむみ（漫画） 君川優樹（原作）</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第52話　真心XIII（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>色憑くモノクローム</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>内山敦司</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第37話	猫娘と勝負!!</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>元最強探索者のおじさん。美少女配信者を助けて大バズりしてしまった。</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>かなたろー(原作) 草壁レイ(漫画)</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第3話　美少女、おじさんにハメられる。④</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>異世界おじさん</t>
+          <t>生徒会にも穴はある！</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>殆ど死んでいる(著者)</t>
+          <t>むちまろ</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+          <t>第131話	ありす大ピンチ！（デジャブ編）</t>
         </is>
       </c>
     </row>
@@ -18244,17 +19286,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
+          <t>村上よしゆき 茨木野 あるてら</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第76話その2</t>
+          <t>第４０話　勇者、聖女と元聖騎士と再会し、魚人を追っ払う（５）</t>
         </is>
       </c>
     </row>
@@ -18264,17 +19306,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>異世界魔王と召喚少女の奴隷魔術</t>
+          <t>ライドンキング</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+          <t>馬場康誌</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第126話　戦争を終わらせてみるⅡ（後編）</t>
+          <t>第81話 大統領と失われた神器（前編）</t>
         </is>
       </c>
     </row>
@@ -18284,17 +19326,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>実は俺、最強でした？</t>
+          <t>ライブダンジョン！</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>原作：澄守 彩 漫画：高橋 愛</t>
+          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>おまけ63</t>
+          <t>第88話前半</t>
         </is>
       </c>
     </row>
@@ -18304,17 +19346,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+          <t>空野進 sorani ファルまろ</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第32話 独身貴族は森で写真を撮る（1）</t>
+          <t>第10話　最弱貴族、部下を信じる（２）</t>
         </is>
       </c>
     </row>
@@ -18324,17 +19366,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>聖者無双</t>
+          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
+          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第90話　研究者や技術者の故郷（後半）</t>
+          <t>第2話①</t>
         </is>
       </c>
     </row>
@@ -18344,17 +19386,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>王子様の友達</t>
+          <t>デスゲームに巻き込まれた山本さん、気ままにゲームバランスを崩壊させる</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>すけろく(著者)</t>
+          <t>ぽち(原作) カモトタツヤ(作画) 久賀フーナ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+          <t>休載イラスト</t>
         </is>
       </c>
     </row>
@@ -18364,17 +19406,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>生徒会にも穴はある！</t>
+          <t>極振り拒否して手探りスタート！　特化しないヒーラー、仲間と別れて旅に出る</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>むちまろ</t>
+          <t>蒼井一秀(作画) 刻一(原作) MIYA*KI(キャラクター原案)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第131話	ありす大ピンチ！（デジャブ編）</t>
+          <t>第64話</t>
         </is>
       </c>
     </row>
@@ -18384,17 +19426,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>オタクに優しいギャルはいない!?</t>
+          <t>異世界おじさん</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>のりしろちゃん 魚住さかな</t>
+          <t>殆ど死んでいる(著者)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>【#148】氷の笑み</t>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
@@ -18404,17 +19446,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>魔法少女リリカルなのは EXCEEDS</t>
+          <t>生徒会役員共</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>都築真紀 川上修一</t>
+          <t>氏家ト全</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第４話①</t>
+          <t>#405</t>
         </is>
       </c>
     </row>
@@ -18424,17 +19466,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>脇役に転生したはずが、いつの間にか伝説の錬金術師になってた～仲間たちが英雄でも俺は支援職なんだが～</t>
+          <t>貧乏騎士に嫁入りしたはずが!? ~野人令嬢は皇太子妃になっても竜を狩りたい~</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>神無月みり 相野 仁</t>
+          <t>漫画：夏川そぞろ 原作：宮前葵 キャラクター原案：ののまろ</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第２６話　脇役、目論見を見破る（１）</t>
+          <t>第10話④皇太子妃（仮）</t>
         </is>
       </c>
     </row>
@@ -18444,17 +19486,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>ひげを剃る。そして女子高生を拾う。</t>
+          <t>【悲報】清楚系で売っていた底辺配信者、うっかり配信を切り忘れたままSS級モンスターを拳で殴り飛ばしてしまう</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>足立いまる(漫画) しめさば(原作) ぶーた(キャラクター原案)</t>
+          <t>アトハ NEO草野 pupps</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第65話その1</t>
+          <t>第５話　【悲報】ゆきのんとのコラボ配信、ワンパン撃破！？（１）</t>
         </is>
       </c>
     </row>
@@ -18464,17 +19506,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>カナン様はあくまでチョロい</t>
+          <t>となりの席のヤツがそういう目で見てくる</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>nonco</t>
+          <t>mmk</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第142話	アミのパジャマパーティ女子会</t>
+          <t>第41話 教えたくない？</t>
         </is>
       </c>
     </row>
@@ -18484,17 +19526,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+          <t>規格外のダンジョン攻略者、実は異世界帰りの元勇者</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+          <t>作画：やまざき君 原作：榊与一</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第3話 後編</t>
+          <t>第4話(2)</t>
         </is>
       </c>
     </row>
@@ -18504,17 +19546,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>魔王討伐したあと、目立ちたくないのでギルドマスターになった</t>
+          <t>町人Aは悪役令嬢をどうしても救いたい　～どぶと空と氷の姫君～</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ＲＯＨＧＵＮ(作画) 朱月十話(原作) 鳴瀬ひろふみ(キャラクターデザイン)</t>
+          <t>原作：一色孝太郎・Parum 漫画：目黒三吉</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第65話-②</t>
+          <t>第38話 攻撃開始</t>
         </is>
       </c>
     </row>
@@ -18524,17 +19566,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>すべての人類を破壊する。それらは再生できない。</t>
+          <t>継母の連れ子が元カノだった</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>横田卓馬(漫画) 伊瀬勝良(原作)</t>
+          <t>草壁レイ(作画) 紙城境介(原作) たかやKi(キャラクター原案)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第66話その3</t>
+          <t>第61話前半</t>
         </is>
       </c>
     </row>
@@ -18544,17 +19586,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>勇者は魔王が好きらしい</t>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>赤槻コウ(著者)</t>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第4話-2：激闘！サキュバス戦！</t>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
@@ -18564,17 +19606,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+          <t>異世界に転移したら山の中だった。反動で強さよりも快適さを選びました。</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>zunta(作画) はらわたさいぞう(原作)</t>
+          <t>原作/じゃがバター(ツギクルブックス) 漫画/蔦屋空 キャラクター原案/岩崎美奈子</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第30話：一秒の奪い合い③</t>
+          <t>第32話</t>
         </is>
       </c>
     </row>
@@ -18584,17 +19626,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>光永康則</t>
+          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第６６話『六花停止』③</t>
+          <t>第76話その2</t>
         </is>
       </c>
     </row>
@@ -18604,17 +19646,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>よわよわ先生</t>
+          <t>ギャルゲーマーに褒められたい</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>福地カミオ</t>
+          <t>げしゅまろ(著者)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第107話	ゆりゆりとドヘンタイと真実</t>
+          <t>44話</t>
         </is>
       </c>
     </row>
@@ -18624,17 +19666,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+          <t>りゅうとあまがみ</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>マツモトケンゴ</t>
+          <t>角丸柴朗(著者)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第６０話　じゃない方の戦いが始まった（２）</t>
+          <t>第一話・魚嫌いのウィル</t>
         </is>
       </c>
     </row>
@@ -18644,17 +19686,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>善人おっさん、生まれ変わったらSSSランク人生が確定した</t>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>原作／三木なずな 漫画／ゆづましろ キャラクター原案／伍長</t>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第133話</t>
+          <t>第126話　戦争を終わらせてみるⅡ（後編）</t>
         </is>
       </c>
     </row>
@@ -18664,17 +19706,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+          <t>実は俺、最強でした？</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+          <t>おまけ63</t>
         </is>
       </c>
     </row>
@@ -18684,17 +19726,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>織田家の長男に生まれました 〜戦国時代に転生したけど、死にたくないので改革を起こします〜</t>
+          <t>ルパン三世 異世界の姫君（ネイバーワールドプリンセス）</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>大沼田伊勢彦 逸見兎歌 平沢下戸</t>
+          <t>モンキー・パンチ／エム・ピー・ワークス 内々けやき 佐伯庸介 白狼</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第33話「私的な会話」①</t>
+          <t>第101話：マッスルタの魔犬❶</t>
         </is>
       </c>
     </row>
@@ -18704,17 +19746,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>百瀬アキラの初恋破綻中。</t>
+          <t>直径3cmの召喚陣&lt;リミットリング&gt;で「雑魚すら呼べない」と蔑まれた底辺召喚士が頂点に立つまで</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>晴川シンタ</t>
+          <t>作画：まっつー 原作：空松蓮司</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第31話 2つの危機に対面中。</t>
+          <t>第4話(2)</t>
         </is>
       </c>
     </row>
@@ -18724,17 +19766,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>昔滅びた魔王城で拾った犬は、実は伝説の魔獣でした ～隠れ最強職《羊飼い》な貴族の三男坊、いずれ、百魔獣の王となる～</t>
+          <t>やり込んだ乙女ゲームの悪役モブですが、断罪は嫌なので真っ当に生きます@COMIC</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>あまうい白一 鍋島テツヒロ 松本蓮士</t>
+          <t>戸張ちょも（漫画） MIZUNA（原作） Ruki（キャラクター原案）</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第12話  殲滅するものと、抗うもの</t>
+          <t>第18話</t>
         </is>
       </c>
     </row>
@@ -18744,17 +19786,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>生徒会役員共</t>
+          <t>僕のカノジョ先生</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>氏家ト全</t>
+          <t>星河蟹(作画) 孟倫（ＳＤｗｉｎｇ）(構成) 鏡遊(原作) おりょう(キャラクター原案)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>#405</t>
+          <t>75時間目-1</t>
         </is>
       </c>
     </row>
@@ -18764,17 +19806,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
+          <t>聖者無双</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>板垣恵介 猪原賽 陸井栄史</t>
+          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第76話　海皇戦争</t>
+          <t>第90話　研究者や技術者の故郷（後半）</t>
         </is>
       </c>
     </row>
@@ -18784,17 +19826,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>戸賀 環 坂木持丸 riritto</t>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第49話①　城のパーティーに参加してみた</t>
+          <t>第32話 独身貴族は森で写真を撮る（1）</t>
         </is>
       </c>
     </row>
@@ -18804,17 +19846,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>303号室の神さま</t>
+          <t>FPSゲームのコーチを引き受けたら依頼主が人気VTuberの美少女だった</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>ふに・無9(著者)</t>
+          <t>漫画：真広吏希 原作：すかいふぁーむ キャラクター原案：みすみ</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Episode. 19</t>
+          <t>第8話</t>
         </is>
       </c>
     </row>
@@ -18824,17 +19866,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>10年ぶりに再会したクソガキは清純美少女JKに成長していた</t>
+          <t>王子様の友達</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>緑青黒羽（漫画） 館西夕木（原作） ひげ猫（キャラクター原案）</t>
+          <t>すけろく(著者)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第5話　嫉妬、そして嫉妬（後編）</t>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
@@ -18844,17 +19886,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
+          <t>かつての暗殺者は来世で違う生き方をする</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>板垣恵介 林たかあき</t>
+          <t>ツネ(漫画) 丘野優(原作) つなかわ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第50話 愛の試練</t>
+          <t>第4話②</t>
         </is>
       </c>
     </row>
@@ -18864,17 +19906,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>学食ガール</t>
+          <t>君の刀が折れるまで ~月宮まつりの恋難き~</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>杉本 萌</t>
+          <t>イノウエ</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>＃01タルタルソースとコールスロー</t>
+          <t>第38話 家族のこと</t>
         </is>
       </c>
     </row>
@@ -18884,17 +19926,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>勇者と魔物の運び屋さん</t>
+          <t>ゲーム内最強の『裏ボス』に転生したので、主人公の代わりに最速クリアを目指します！</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>大河原</t>
+          <t>作画：こめぐ 原作：迅空也</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>終章１２</t>
+          <t>第4話(2)</t>
         </is>
       </c>
     </row>
@@ -18904,17 +19946,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>俺は星間国家の悪徳領主！</t>
+          <t>金色の文字使い ―勇者四人に巻き込まれたユニークチート―</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>灘島かい（漫画） 三嶋与夢（原作） 高峰ナダレ（キャラクター原案）</t>
+          <t>尾崎祐介(作画) 十本スイ(原作) すまき俊悟(キャラクター原案)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第39話　自惚れ</t>
+          <t>第119話</t>
         </is>
       </c>
     </row>
@@ -18924,17 +19966,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+          <t>冒険者アル あいつの魔法はおかしい@COMIC</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>漫画/すたひろ 原作/Y.A</t>
+          <t>山﨑と子（漫画） れもん（原作） sime（キャラクター原案）</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>chapter66【35話①】</t>
+          <t>第14話 ②</t>
         </is>
       </c>
     </row>
@@ -18944,17 +19986,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>絶対死なないステラ姫</t>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>光永康則 大高稲</t>
+          <t>光永康則</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第１４話　絶対旅立たない（１）</t>
+          <t>第６６話『六花停止』③</t>
         </is>
       </c>
     </row>
@@ -18964,17 +20006,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ひとりぼっちの異世界攻略</t>
+          <t>魔法少女リリカルなのは EXCEEDS</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>びび（漫画） 五示正司（原作）</t>
+          <t>都築真紀 川上修一</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第227話　自業自得です</t>
+          <t>第４話①</t>
         </is>
       </c>
     </row>
@@ -18984,17 +20026,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>アンゴルモア 元寇合戦記　【博多編】</t>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>たかぎ七彦(著者)</t>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第四十四話その五</t>
+          <t>第3話 後編</t>
         </is>
       </c>
     </row>
@@ -19004,17 +20046,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>ゴリラ女子高生</t>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>大友しゅうま(著者)</t>
+          <t>マツモトケンゴ</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+          <t>第６０話　じゃない方の戦いが始まった（２）</t>
         </is>
       </c>
     </row>
@@ -19024,17 +20066,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>サラリーマンが異世界に行ったら四天王になった話</t>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>漫画：村光 原作：ベニガシラ</t>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第88話　王のシステム</t>
+          <t>第30話：一秒の奪い合い③</t>
         </is>
       </c>
     </row>
@@ -19044,17 +20086,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>帰ってください！ 阿久津さん</t>
+          <t>黒魔法寮の三悪人</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>長岡太一(著者)</t>
+          <t>斎藤キミオ</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第192話</t>
+          <t>第41話 星家vs善寿賀家!だよ♪</t>
         </is>
       </c>
     </row>
@@ -19064,17 +20106,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>ロードマギアの弟子</t>
+          <t>オタクに優しいギャルはいない!?</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>FLIPFLOPs</t>
+          <t>のりしろちゃん 魚住さかな</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第18話 魔術師の戦い (前編)</t>
+          <t>【#148】氷の笑み</t>
         </is>
       </c>
     </row>
@@ -19084,17 +20126,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>黒月のイェルクナハト</t>
+          <t>カナン様はあくまでチョロい</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>スズモトコウ</t>
+          <t>nonco</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第5話	思いの儘に</t>
+          <t>第142話	アミのパジャマパーティ女子会</t>
         </is>
       </c>
     </row>
@@ -19104,17 +20146,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>序盤で死ぬ最強のサブキャラに転生したので、ゲーム知識で無双する</t>
+          <t>ひげを剃る。そして女子高生を拾う。</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>作画：マエD 原作：新人</t>
+          <t>足立いまる(漫画) しめさば(原作) ぶーた(キャラクター原案)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第4話(4)</t>
+          <t>第65話その1</t>
         </is>
       </c>
     </row>
@@ -19124,17 +20166,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>世界最強の騎士は、必ず死ぬヒロインを救うため異世界でも最強の騎士となる〜両手に花を、両手に剣を〜</t>
+          <t>学食ガール</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>KAZU（原作） イソベカズマ（漫画） moino（メカデザイン協力）</t>
+          <t>杉本 萌</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第13話（後編）決断</t>
+          <t>＃01タルタルソースとコールスロー</t>
         </is>
       </c>
     </row>
@@ -19144,17 +20186,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>最後のエルフ</t>
+          <t>無能と蔑まれた【勇気ある者】が、実は伝説の【勇者】でした~500年前の仲間＆魔王の娘と一緒に今度こそ世界を救います~</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>サワノアキラ（漫画）</t>
+          <t>作画：シグチサトシ 原作：やすくん</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第9章　竜の眠る地（前編）</t>
+          <t>第4話(2)</t>
         </is>
       </c>
     </row>
@@ -19164,17 +20206,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>追放者食堂へようこそ！　～最強パーティーを追放された料理人（Lv.99）は、田舎で念願の冒険者食堂を開きます！～</t>
+          <t>脇役に転生したはずが、いつの間にか伝説の錬金術師になってた～仲間たちが英雄でも俺は支援職なんだが～</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>つむみ（漫画） 君川優樹（原作）</t>
+          <t>神無月みり 相野 仁</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第52話　真心XIII（後編）</t>
+          <t>第２６話　脇役、目論見を見破る（１）</t>
         </is>
       </c>
     </row>
@@ -19184,17 +20226,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>色憑くモノクローム</t>
+          <t>すべての人類を破壊する。それらは再生できない。</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>内山敦司</t>
+          <t>横田卓馬(漫画) 伊瀬勝良(原作)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第37話	猫娘と勝負!!</t>
+          <t>第66話その3</t>
         </is>
       </c>
     </row>
@@ -19204,17 +20246,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>元最強探索者のおじさん。美少女配信者を助けて大バズりしてしまった。</t>
+          <t>カッコウの許嫁</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>かなたろー(原作) 草壁レイ(漫画)</t>
+          <t>吉河美希</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第3話　美少女、おじさんにハメられる。④</t>
+          <t>第255話	二人きりになれる場所…？</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-07-19
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -33,6 +33,7 @@
     <sheet name="2025-07-16" sheetId="25" state="visible" r:id="rId25"/>
     <sheet name="2025-07-17" sheetId="26" state="visible" r:id="rId26"/>
     <sheet name="2025-07-18" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="2025-07-19" sheetId="28" state="visible" r:id="rId28"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -19261,22 +19262,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>生徒会にも穴はある！</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>むちまろ</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第131話	ありす大ピンチ！（デジャブ編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>村上よしゆき 茨木野 あるてら</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第４０話　勇者、聖女と元聖騎士と再会し、魚人を追っ払う（５）</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>ライドンキング</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>馬場康誌</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第81話 大統領と失われた神器（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>ライブダンジョン！</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第88話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>空野進 sorani ファルまろ</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第10話　最弱貴族、部下を信じる（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第2話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>デスゲームに巻き込まれた山本さん、気ままにゲームバランスを崩壊させる</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>ぽち(原作) カモトタツヤ(作画) 久賀フーナ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>休載イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>極振り拒否して手探りスタート！　特化しないヒーラー、仲間と別れて旅に出る</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>蒼井一秀(作画) 刻一(原作) MIYA*KI(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第64話</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>異世界おじさん</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>殆ど死んでいる(著者)</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>生徒会役員共</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>氏家ト全</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>#405</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>貧乏騎士に嫁入りしたはずが!? ~野人令嬢は皇太子妃になっても竜を狩りたい~</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>漫画：夏川そぞろ 原作：宮前葵 キャラクター原案：ののまろ</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第10話④皇太子妃（仮）</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>【悲報】清楚系で売っていた底辺配信者、うっかり配信を切り忘れたままSS級モンスターを拳で殴り飛ばしてしまう</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>アトハ NEO草野 pupps</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第５話　【悲報】ゆきのんとのコラボ配信、ワンパン撃破！？（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>となりの席のヤツがそういう目で見てくる</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>mmk</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第41話 教えたくない？</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>規格外のダンジョン攻略者、実は異世界帰りの元勇者</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>作画：やまざき君 原作：榊与一</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第4話(2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>町人Aは悪役令嬢をどうしても救いたい　～どぶと空と氷の姫君～</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>原作：一色孝太郎・Parum 漫画：目黒三吉</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第38話 攻撃開始</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>継母の連れ子が元カノだった</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>草壁レイ(作画) 紙城境介(原作) たかやKi(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第61話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>異世界に転移したら山の中だった。反動で強さよりも快適さを選びました。</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>原作/じゃがバター(ツギクルブックス) 漫画/蔦屋空 キャラクター原案/岩崎美奈子</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第32話</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第76話その2</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>ギャルゲーマーに褒められたい</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>げしゅまろ(著者)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>44話</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>りゅうとあまがみ</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>角丸柴朗(著者)</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第一話・魚嫌いのウィル</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第126話　戦争を終わらせてみるⅡ（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>おまけ63</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>ルパン三世 異世界の姫君（ネイバーワールドプリンセス）</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>モンキー・パンチ／エム・ピー・ワークス 内々けやき 佐伯庸介 白狼</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第101話：マッスルタの魔犬❶</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>直径3cmの召喚陣&lt;リミットリング&gt;で「雑魚すら呼べない」と蔑まれた底辺召喚士が頂点に立つまで</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>作画：まっつー 原作：空松蓮司</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第4話(2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>やり込んだ乙女ゲームの悪役モブですが、断罪は嫌なので真っ当に生きます@COMIC</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>戸張ちょも（漫画） MIZUNA（原作） Ruki（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第18話</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>僕のカノジョ先生</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>星河蟹(作画) 孟倫（ＳＤｗｉｎｇ）(構成) 鏡遊(原作) おりょう(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>75時間目-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>聖者無双</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第90話　研究者や技術者の故郷（後半）</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第32話 独身貴族は森で写真を撮る（1）</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>FPSゲームのコーチを引き受けたら依頼主が人気VTuberの美少女だった</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>漫画：真広吏希 原作：すかいふぁーむ キャラクター原案：みすみ</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第8話</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>王子様の友達</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>すけろく(著者)</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>かつての暗殺者は来世で違う生き方をする</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>ツネ(漫画) 丘野優(原作) つなかわ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第4話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>君の刀が折れるまで ~月宮まつりの恋難き~</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>イノウエ</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第38話 家族のこと</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>ゲーム内最強の『裏ボス』に転生したので、主人公の代わりに最速クリアを目指します！</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>作画：こめぐ 原作：迅空也</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第4話(2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>金色の文字使い ―勇者四人に巻き込まれたユニークチート―</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>尾崎祐介(作画) 十本スイ(原作) すまき俊悟(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第119話</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>冒険者アル あいつの魔法はおかしい@COMIC</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>山﨑と子（漫画） れもん（原作） sime（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第14話 ②</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第６６話『六花停止』③</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>魔法少女リリカルなのは EXCEEDS</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>都築真紀 川上修一</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第４話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第3話 後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>マツモトケンゴ</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第６０話　じゃない方の戦いが始まった（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第30話：一秒の奪い合い③</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>黒魔法寮の三悪人</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>斎藤キミオ</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第41話 星家vs善寿賀家!だよ♪</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>オタクに優しいギャルはいない!?</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>のりしろちゃん 魚住さかな</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>【#148】氷の笑み</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>カナン様はあくまでチョロい</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>nonco</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第142話	アミのパジャマパーティ女子会</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>ひげを剃る。そして女子高生を拾う。</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>足立いまる(漫画) しめさば(原作) ぶーた(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第65話その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>学食ガール</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>杉本 萌</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>＃01タルタルソースとコールスロー</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>無能と蔑まれた【勇気ある者】が、実は伝説の【勇者】でした~500年前の仲間＆魔王の娘と一緒に今度こそ世界を救います~</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>作画：シグチサトシ 原作：やすくん</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第4話(2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>脇役に転生したはずが、いつの間にか伝説の錬金術師になってた～仲間たちが英雄でも俺は支援職なんだが～</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>神無月みり 相野 仁</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第２６話　脇役、目論見を見破る（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>すべての人類を破壊する。それらは再生できない。</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>横田卓馬(漫画) 伊瀬勝良(原作)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第66話その3</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>カッコウの許嫁</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>吉河美希</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第255話	二人きりになれる場所…？</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>生徒会にも穴はある！</t>
+          <t>宇崎ちゃんは遊びたい！</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>むちまろ</t>
+          <t>丈(著者)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第131話	ありす大ピンチ！（デジャブ編）</t>
+          <t>第125話</t>
         </is>
       </c>
     </row>
@@ -19286,17 +20328,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+          <t>よくわからないけれど異世界に転生していたようです</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>村上よしゆき 茨木野 あるてら</t>
+          <t>内々けやき あし カオミン</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第４０話　勇者、聖女と元聖騎士と再会し、魚人を追っ払う（５）</t>
+          <t>第136話 よくわからないけれどスカウトされたみたいです（１）</t>
         </is>
       </c>
     </row>
@@ -19306,17 +20348,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ライドンキング</t>
+          <t>くらいあの子としたいこと</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>馬場康誌</t>
+          <t>碇マナツ(著者)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第81話 大統領と失われた神器（前編）</t>
+          <t>第80話</t>
         </is>
       </c>
     </row>
@@ -19326,17 +20368,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ライブダンジョン！</t>
+          <t>小林さんちのメイドラゴン</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
+          <t>クール教信者</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第88話前半</t>
+          <t>第146話</t>
         </is>
       </c>
     </row>
@@ -19346,17 +20388,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+          <t>理想のヒモ生活</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>空野進 sorani ファルまろ</t>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第10話　最弱貴族、部下を信じる（２）</t>
+          <t>第86話　その1</t>
         </is>
       </c>
     </row>
@@ -19366,17 +20408,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
+          <t>最強勇者パーティーは愛が知りたい</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
+          <t>山田肌襦袢</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第2話①</t>
+          <t>第27話「エッチな祭りを始めたい」</t>
         </is>
       </c>
     </row>
@@ -19386,17 +20428,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>デスゲームに巻き込まれた山本さん、気ままにゲームバランスを崩壊させる</t>
+          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ぽち(原作) カモトタツヤ(作画) 久賀フーナ(キャラクター原案)</t>
+          <t>神原絵理華(漫画) 一森一輝(原作)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>休載イラスト</t>
+          <t>第18話①</t>
         </is>
       </c>
     </row>
@@ -19406,17 +20448,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>極振り拒否して手探りスタート！　特化しないヒーラー、仲間と別れて旅に出る</t>
+          <t>ゲーセン少女と異文化交流</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>蒼井一秀(作画) 刻一(原作) MIYA*KI(キャラクター原案)</t>
+          <t>安原宏和(著者)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第64話</t>
+          <t>第126話</t>
         </is>
       </c>
     </row>
@@ -19426,17 +20468,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>異世界おじさん</t>
+          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>殆ど死んでいる(著者)</t>
+          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+          <t>第74話 トワイライト</t>
         </is>
       </c>
     </row>
@@ -19446,17 +20488,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>生徒会役員共</t>
+          <t>ヤンデレかと思ったらもっとヤベー女だった</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>氏家ト全</t>
+          <t>八木戸マト</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>#405</t>
+          <t>第67話　全てを間違えたヤンデレ彼女</t>
         </is>
       </c>
     </row>
@@ -19466,17 +20508,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>貧乏騎士に嫁入りしたはずが!? ~野人令嬢は皇太子妃になっても竜を狩りたい~</t>
+          <t>王都の外れの錬金術師 ～ハズレ職業だったので、のんびりお店経営します～</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>漫画：夏川そぞろ 原作：宮前葵 キャラクター原案：ののまろ</t>
+          <t>あさなや(著者) yocco(原作) 純粋(キャラクター原案)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第10話④皇太子妃（仮）</t>
+          <t>element.49</t>
         </is>
       </c>
     </row>
@@ -19486,17 +20528,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>【悲報】清楚系で売っていた底辺配信者、うっかり配信を切り忘れたままSS級モンスターを拳で殴り飛ばしてしまう</t>
+          <t>ベヒモスの花婿</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>アトハ NEO草野 pupps</t>
+          <t>鈴音ことら(原作) 月並甲介(漫画)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第５話　【悲報】ゆきのんとのコラボ配信、ワンパン撃破！？（１）</t>
+          <t>第7話②</t>
         </is>
       </c>
     </row>
@@ -19506,17 +20548,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>となりの席のヤツがそういう目で見てくる</t>
+          <t>異世界おじさん</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>mmk</t>
+          <t>殆ど死んでいる(著者)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第41話 教えたくない？</t>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
@@ -19526,17 +20568,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>規格外のダンジョン攻略者、実は異世界帰りの元勇者</t>
+          <t>修羅幼女の英雄譚～半端者と言われた傭兵、幼女に転生して成り上がる～</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>作画：やまざき君 原作：榊与一</t>
+          <t>作画：むらたん 原作：沙城流</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第4話(2)</t>
+          <t>第7話(2)</t>
         </is>
       </c>
     </row>
@@ -19546,17 +20588,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>町人Aは悪役令嬢をどうしても救いたい　～どぶと空と氷の姫君～</t>
+          <t>推しにささげるダンジョングルメ ～最強探索者VTuberになる～</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>原作：一色孝太郎・Parum 漫画：目黒三吉</t>
+          <t>モノクロウサギ(原作) 藍川蓮(漫画)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第38話 攻撃開始</t>
+          <t>CHAPTER　10-3</t>
         </is>
       </c>
     </row>
@@ -19566,17 +20608,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>継母の連れ子が元カノだった</t>
+          <t>顔に出ない柏田さんと顔に出る太田君＋</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>草壁レイ(作画) 紙城境介(原作) たかやKi(キャラクター原案)</t>
+          <t>東ふゆ(著者)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第61話前半</t>
+          <t>第30話 田沼先生の秘密</t>
         </is>
       </c>
     </row>
@@ -19586,17 +20628,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+          <t>生活魔法使いの下剋上</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+          <t>保志レンジ(著者) 月汰元(原作) ｈｉｍｅｓｕｚ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+          <t>第26話-2</t>
         </is>
       </c>
     </row>
@@ -19606,17 +20648,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>異世界に転移したら山の中だった。反動で強さよりも快適さを選びました。</t>
+          <t>なぜかS級美女達の話題に俺があがる件</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>原作/じゃがバター(ツギクルブックス) 漫画/蔦屋空 キャラクター原案/岩崎美奈子</t>
+          <t>ジョN(著者) 脇岡こなつ(原作) magako(キャラクター原案)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第32話</t>
+          <t>第9話-2</t>
         </is>
       </c>
     </row>
@@ -19626,17 +20668,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
+          <t>スキルがなければレベルを上げる～９９がカンストの世界でレベル800万からスタート～</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
+          <t>倉橋ユウス(漫画) 岡沢六十四(原作)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第76話その2</t>
+          <t>第51話③</t>
         </is>
       </c>
     </row>
@@ -19646,17 +20688,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>ギャルゲーマーに褒められたい</t>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>げしゅまろ(著者)</t>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>44話</t>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
@@ -19666,17 +20708,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>りゅうとあまがみ</t>
+          <t>お前妹じゃなくて許嫁だったのかよ!?</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>角丸柴朗(著者)</t>
+          <t>湯猫子(漫画) 未来人A(原作)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第一話・魚嫌いのウィル</t>
+          <t>第28話</t>
         </is>
       </c>
     </row>
@@ -19686,17 +20728,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>異世界魔王と召喚少女の奴隷魔術</t>
+          <t>パワハラギルマスをぶん殴ってブラック聖剣ギルドをクビになったので、辺境で聖剣工房を開くことにした</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+          <t>だいたいねむい(原作) まお(漫画)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第126話　戦争を終わらせてみるⅡ（後編）</t>
+          <t>第9話④</t>
         </is>
       </c>
     </row>
@@ -19706,17 +20748,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>実は俺、最強でした？</t>
+          <t>底辺冒険者だけど魔法を極めてみることにした ～無能スキルから神スキルに進化した【魔法創造】と【アイテム作成】で無双する～</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>原作：澄守 彩 漫画：高橋 愛</t>
+          <t>蒼乃白兎 坂野杏梨 かわく</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>おまけ63</t>
+          <t>第44話(前編) 救世主</t>
         </is>
       </c>
     </row>
@@ -19726,17 +20768,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ルパン三世 異世界の姫君（ネイバーワールドプリンセス）</t>
+          <t>異世界転移したら愛犬が最強になりました～シルバーフェンリルと俺が異世界暮らしを始めたら～</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>モンキー・パンチ／エム・ピー・ワークス 内々けやき 佐伯庸介 白狼</t>
+          <t>漫画：一花ハナ 原作：龍央 キャラクター原案：りりんら</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第101話：マッスルタの魔犬❶</t>
+          <t>第36話後半</t>
         </is>
       </c>
     </row>
@@ -19746,17 +20788,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>直径3cmの召喚陣&lt;リミットリング&gt;で「雑魚すら呼べない」と蔑まれた底辺召喚士が頂点に立つまで</t>
+          <t>ダウナーお姉さんは遊びたい</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>作画：まっつー 原作：空松蓮司</t>
+          <t>山鷹景</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第4話(2)</t>
+          <t>第14話</t>
         </is>
       </c>
     </row>
@@ -19766,17 +20808,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>やり込んだ乙女ゲームの悪役モブですが、断罪は嫌なので真っ当に生きます@COMIC</t>
+          <t>傭兵団の愛し子 ～死にかけ孤児は最強師匠たちに育てられる～</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>戸張ちょも（漫画） MIZUNA（原作） Ruki（キャラクター原案）</t>
+          <t>柿野レイ(漫画) 天野雪人(原作) 黒井ススム(キャラクター原案)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第18話</t>
+          <t>第6話後編：召喚士ウィル</t>
         </is>
       </c>
     </row>
@@ -19786,17 +20828,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>僕のカノジョ先生</t>
+          <t>限界超えの天賦は、転生者にしか扱えない ― オーバーリミット・スキルホルダー ―</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>星河蟹(作画) 孟倫（ＳＤｗｉｎｇ）(構成) 鏡遊(原作) おりょう(キャラクター原案)</t>
+          <t>長月みそか(漫画) 三上康明(原作) 大槍葦人(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>75時間目-1</t>
+          <t>第3章［13］後半</t>
         </is>
       </c>
     </row>
@@ -19806,17 +20848,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>聖者無双</t>
+          <t>クラスの大嫌いな女子と結婚することになった。</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
+          <t>天乃聖樹(原作) もすこんぶ(漫画)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第90話　研究者や技術者の故郷（後半）</t>
+          <t>第44話-1</t>
         </is>
       </c>
     </row>
@@ -19826,17 +20868,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+          <t>勇者パーティから追い出された不遇職【罠士】、ユニークスキル【矢印】で最強になる</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+          <t>作画：たつひこ 原作：白石 有希</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第32話 独身貴族は森で写真を撮る（1）</t>
+          <t>第7話(2)</t>
         </is>
       </c>
     </row>
@@ -19846,17 +20888,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>FPSゲームのコーチを引き受けたら依頼主が人気VTuberの美少女だった</t>
+          <t>義妹生活</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>漫画：真広吏希 原作：すかいふぁーむ キャラクター原案：みすみ</t>
+          <t>三河ごーすと(原作) 奏ユミカ(漫画) Hiten(キャラクター原案)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第8話</t>
+          <t>第30話-2</t>
         </is>
       </c>
     </row>
@@ -19866,17 +20908,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>王子様の友達</t>
+          <t>やっぱ人間やめて正解だわ</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>すけろく(著者)</t>
+          <t>偽BEなんとか</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+          <t>第15話　こちら世界の中心からお届け</t>
         </is>
       </c>
     </row>
@@ -19886,17 +20928,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>かつての暗殺者は来世で違う生き方をする</t>
+          <t>レベル1で挑む縛りプレイ!</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>ツネ(漫画) 丘野優(原作) つなかわ(キャラクター原案)</t>
+          <t>北川ニキタ 大鐘いしや 刀 彼方</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第4話②</t>
+          <t>最終話 最高の気分①</t>
         </is>
       </c>
     </row>
@@ -19906,17 +20948,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>君の刀が折れるまで ~月宮まつりの恋難き~</t>
+          <t>双子の姉が神子として引き取られて、私は捨てられたけど多分私が神子である。</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>イノウエ</t>
+          <t>雪(著者) 池中織奈(原作) カット(キャラクター原案)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第38話 家族のこと</t>
+          <t>第32話前編</t>
         </is>
       </c>
     </row>
@@ -19926,17 +20968,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ゲーム内最強の『裏ボス』に転生したので、主人公の代わりに最速クリアを目指します！</t>
+          <t>生徒会にも穴はある！</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>作画：こめぐ 原作：迅空也</t>
+          <t>むちまろ</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第4話(2)</t>
+          <t>第131話	ありす大ピンチ！（デジャブ編）</t>
         </is>
       </c>
     </row>
@@ -19946,17 +20988,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>金色の文字使い ―勇者四人に巻き込まれたユニークチート―</t>
+          <t>ブレイド＆バスタード</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>尾崎祐介(作画) 十本スイ(原作) すまき俊悟(キャラクター原案)</t>
+          <t>漫画/楓月 誠 原作/蝸牛くも キャラクター原案/so-bin</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第119話</t>
+          <t>第10話（2）</t>
         </is>
       </c>
     </row>
@@ -19966,17 +21008,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>冒険者アル あいつの魔法はおかしい@COMIC</t>
+          <t>ちびっこ賢者、Lv.1から異世界でがんばります！</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>山﨑と子（漫画） れもん（原作） sime（キャラクター原案）</t>
+          <t>みさき樹里(漫画) 彩戸ゆめ(原作) 竹花ノート(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第14話 ②</t>
+          <t>第37話</t>
         </is>
       </c>
     </row>
@@ -19986,17 +21028,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+          <t>やめてくれ、強いのは俺じゃなくて剣なんだ……！</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>光永康則</t>
+          <t>漫画/廃狼 原作/馬路まんじ キャラクター原案/かぼちゃ</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第６６話『六花停止』③</t>
+          <t>第7話（3）</t>
         </is>
       </c>
     </row>
@@ -20006,17 +21048,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>魔法少女リリカルなのは EXCEEDS</t>
+          <t>チンチンデビルを追え！</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>都築真紀 川上修一</t>
+          <t>くぼたふみお</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第４話①</t>
+          <t>第３０話　仲間のため振るう力…！</t>
         </is>
       </c>
     </row>
@@ -20026,17 +21068,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+          <t>異世界のんびり農家の日常</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+          <t>ユウズィ(著者) 内藤騎之介(原作) やすも(キャラクター原案)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第3話 後編</t>
+          <t>収穫その36</t>
         </is>
       </c>
     </row>
@@ -20046,17 +21088,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+          <t>ライドンキング</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>マツモトケンゴ</t>
+          <t>馬場康誌</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第６０話　じゃない方の戦いが始まった（２）</t>
+          <t>第81話 大統領と失われた神器（前編）</t>
         </is>
       </c>
     </row>
@@ -20066,17 +21108,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+          <t>ギルドを追放された回復術士、実は魔力無限だったので規格外の回復魔法で伝説となる</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>zunta(作画) はらわたさいぞう(原作)</t>
+          <t>漫画：坂下コウ 原作：霞杏檎</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第30話：一秒の奪い合い③</t>
+          <t>第4話(1)</t>
         </is>
       </c>
     </row>
@@ -20086,17 +21128,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>黒魔法寮の三悪人</t>
+          <t>魔王学園の反逆者 ～人類初の魔王候補、眷属少女と王座を目指して成り上がる～</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>斎藤キミオ</t>
+          <t>溝口ぜらちん(作画) 久慈マサムネ(原作) ｋａｋａｏ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第41話 星家vs善寿賀家!だよ♪</t>
+          <t>最終話</t>
         </is>
       </c>
     </row>
@@ -20106,17 +21148,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>オタクに優しいギャルはいない!?</t>
+          <t>瞳ちゃんは人見知り</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>のりしろちゃん 魚住さかな</t>
+          <t>夏海ちょりすけ</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>【#148】氷の笑み</t>
+          <t>第136話</t>
         </is>
       </c>
     </row>
@@ -20126,17 +21168,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>カナン様はあくまでチョロい</t>
+          <t>隠居暮らしのおっさん、女王陛下の剣となる</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>nonco</t>
+          <t>漫画/半二合 原作/天酒之瓢 キャラクター原案/みことあけみ</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第142話	アミのパジャマパーティ女子会</t>
+          <t>第5話（2）</t>
         </is>
       </c>
     </row>
@@ -20146,17 +21188,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ひげを剃る。そして女子高生を拾う。</t>
+          <t>転生して成長チートを手に入れたら、最凶スキルもついたのですが!?</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>足立いまる(漫画) しめさば(原作) ぶーた(キャラクター原案)</t>
+          <t>やま ゆずもと 我美蘭</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第65話その1</t>
+          <t>第10話</t>
         </is>
       </c>
     </row>
@@ -20166,17 +21208,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>学食ガール</t>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>杉本 萌</t>
+          <t>村上よしゆき 茨木野 あるてら</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>＃01タルタルソースとコールスロー</t>
+          <t>第４０話　勇者、聖女と元聖騎士と再会し、魚人を追っ払う（５）</t>
         </is>
       </c>
     </row>
@@ -20186,17 +21228,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>無能と蔑まれた【勇気ある者】が、実は伝説の【勇者】でした~500年前の仲間＆魔王の娘と一緒に今度こそ世界を救います~</t>
+          <t>錬金術師の辺境再生スローライフ～S級パーティーで孤立した少女をかばったら追放されたので、一緒に幸せに暮らします～</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>作画：シグチサトシ 原作：やすくん</t>
+          <t>作画：弥永扇 原作：三月菫</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第4話(2)</t>
+          <t>第7話(2)</t>
         </is>
       </c>
     </row>
@@ -20206,17 +21248,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>脇役に転生したはずが、いつの間にか伝説の錬金術師になってた～仲間たちが英雄でも俺は支援職なんだが～</t>
+          <t>影の英雄の日常譚 勇者の裏で暗躍していた最強のエージェント。組織が解体されたので、正体隠して人並みの日常を謳歌する。</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>神無月みり 相野 仁</t>
+          <t>kanco(漫画) 坂石遊作(原作) TYONE(キャラクター原案)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第２６話　脇役、目論見を見破る（１）</t>
+          <t>Episode32-3</t>
         </is>
       </c>
     </row>
@@ -20226,17 +21268,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>すべての人類を破壊する。それらは再生できない。</t>
+          <t>ライブダンジョン！</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>横田卓馬(漫画) 伊瀬勝良(原作)</t>
+          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第66話その3</t>
+          <t>第88話前半</t>
         </is>
       </c>
     </row>
@@ -20246,17 +21288,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>カッコウの許嫁</t>
+          <t>追放されたおっさんタンク、実は防御力最強だったのでダメージゼロで無双する</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>吉河美希</t>
+          <t>漫画：化野九十九 原作：あけちともあき</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第255話	二人きりになれる場所…？</t>
+          <t>第4話(1)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-07-20
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -34,6 +34,7 @@
     <sheet name="2025-07-17" sheetId="26" state="visible" r:id="rId26"/>
     <sheet name="2025-07-18" sheetId="27" state="visible" r:id="rId27"/>
     <sheet name="2025-07-19" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="2025-07-20" sheetId="29" state="visible" r:id="rId29"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -20303,22 +20304,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>宇崎ちゃんは遊びたい！</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>丈(著者)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第125話</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第136話 よくわからないけれどスカウトされたみたいです（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>くらいあの子としたいこと</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>碇マナツ(著者)</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第80話</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>小林さんちのメイドラゴン</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>クール教信者</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第146話</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>理想のヒモ生活</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第86話　その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>最強勇者パーティーは愛が知りたい</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>山田肌襦袢</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第27話「エッチな祭りを始めたい」</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>神原絵理華(漫画) 一森一輝(原作)</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第18話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>ゲーセン少女と異文化交流</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>安原宏和(著者)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第126話</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第74話 トワイライト</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>ヤンデレかと思ったらもっとヤベー女だった</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>八木戸マト</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第67話　全てを間違えたヤンデレ彼女</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>王都の外れの錬金術師 ～ハズレ職業だったので、のんびりお店経営します～</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>あさなや(著者) yocco(原作) 純粋(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>element.49</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>ベヒモスの花婿</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>鈴音ことら(原作) 月並甲介(漫画)</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第7話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>異世界おじさん</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>殆ど死んでいる(著者)</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>修羅幼女の英雄譚～半端者と言われた傭兵、幼女に転生して成り上がる～</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>作画：むらたん 原作：沙城流</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第7話(2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>推しにささげるダンジョングルメ ～最強探索者VTuberになる～</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>モノクロウサギ(原作) 藍川蓮(漫画)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>CHAPTER　10-3</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>顔に出ない柏田さんと顔に出る太田君＋</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>東ふゆ(著者)</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第30話 田沼先生の秘密</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>生活魔法使いの下剋上</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>保志レンジ(著者) 月汰元(原作) ｈｉｍｅｓｕｚ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第26話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>なぜかS級美女達の話題に俺があがる件</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>ジョN(著者) 脇岡こなつ(原作) magako(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第9話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>スキルがなければレベルを上げる～９９がカンストの世界でレベル800万からスタート～</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>倉橋ユウス(漫画) 岡沢六十四(原作)</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第51話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>お前妹じゃなくて許嫁だったのかよ!?</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>湯猫子(漫画) 未来人A(原作)</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第28話</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>パワハラギルマスをぶん殴ってブラック聖剣ギルドをクビになったので、辺境で聖剣工房を開くことにした</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>だいたいねむい(原作) まお(漫画)</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第9話④</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>底辺冒険者だけど魔法を極めてみることにした ～無能スキルから神スキルに進化した【魔法創造】と【アイテム作成】で無双する～</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>蒼乃白兎 坂野杏梨 かわく</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第44話(前編) 救世主</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>異世界転移したら愛犬が最強になりました～シルバーフェンリルと俺が異世界暮らしを始めたら～</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>漫画：一花ハナ 原作：龍央 キャラクター原案：りりんら</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第36話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>ダウナーお姉さんは遊びたい</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>山鷹景</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第14話</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>傭兵団の愛し子 ～死にかけ孤児は最強師匠たちに育てられる～</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>柿野レイ(漫画) 天野雪人(原作) 黒井ススム(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第6話後編：召喚士ウィル</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>限界超えの天賦は、転生者にしか扱えない ― オーバーリミット・スキルホルダー ―</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>長月みそか(漫画) 三上康明(原作) 大槍葦人(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第3章［13］後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>クラスの大嫌いな女子と結婚することになった。</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>天乃聖樹(原作) もすこんぶ(漫画)</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第44話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティから追い出された不遇職【罠士】、ユニークスキル【矢印】で最強になる</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>作画：たつひこ 原作：白石 有希</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第7話(2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>義妹生活</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>三河ごーすと(原作) 奏ユミカ(漫画) Hiten(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第30話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>やっぱ人間やめて正解だわ</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>偽BEなんとか</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第15話　こちら世界の中心からお届け</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>レベル1で挑む縛りプレイ!</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>北川ニキタ 大鐘いしや 刀 彼方</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>最終話 最高の気分①</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>双子の姉が神子として引き取られて、私は捨てられたけど多分私が神子である。</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>雪(著者) 池中織奈(原作) カット(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第32話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>生徒会にも穴はある！</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>むちまろ</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第131話	ありす大ピンチ！（デジャブ編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>ブレイド＆バスタード</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>漫画/楓月 誠 原作/蝸牛くも キャラクター原案/so-bin</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第10話（2）</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>ちびっこ賢者、Lv.1から異世界でがんばります！</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>みさき樹里(漫画) 彩戸ゆめ(原作) 竹花ノート(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第37話</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>やめてくれ、強いのは俺じゃなくて剣なんだ……！</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>漫画/廃狼 原作/馬路まんじ キャラクター原案/かぼちゃ</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第7話（3）</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>チンチンデビルを追え！</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>くぼたふみお</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第３０話　仲間のため振るう力…！</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>異世界のんびり農家の日常</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>ユウズィ(著者) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>収穫その36</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>ライドンキング</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>馬場康誌</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第81話 大統領と失われた神器（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>ギルドを追放された回復術士、実は魔力無限だったので規格外の回復魔法で伝説となる</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>漫画：坂下コウ 原作：霞杏檎</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第4話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>魔王学園の反逆者 ～人類初の魔王候補、眷属少女と王座を目指して成り上がる～</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>溝口ぜらちん(作画) 久慈マサムネ(原作) ｋａｋａｏ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>最終話</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>瞳ちゃんは人見知り</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>夏海ちょりすけ</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第136話</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>隠居暮らしのおっさん、女王陛下の剣となる</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>漫画/半二合 原作/天酒之瓢 キャラクター原案/みことあけみ</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第5話（2）</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>転生して成長チートを手に入れたら、最凶スキルもついたのですが!?</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>やま ゆずもと 我美蘭</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第10話</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>村上よしゆき 茨木野 あるてら</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第４０話　勇者、聖女と元聖騎士と再会し、魚人を追っ払う（５）</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>錬金術師の辺境再生スローライフ～S級パーティーで孤立した少女をかばったら追放されたので、一緒に幸せに暮らします～</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>作画：弥永扇 原作：三月菫</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第7話(2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>影の英雄の日常譚 勇者の裏で暗躍していた最強のエージェント。組織が解体されたので、正体隠して人並みの日常を謳歌する。</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>kanco(漫画) 坂石遊作(原作) TYONE(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>Episode32-3</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>ライブダンジョン！</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第88話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>追放されたおっさんタンク、実は防御力最強だったのでダメージゼロで無双する</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>漫画：化野九十九 原作：あけちともあき</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第4話(1)</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>宇崎ちゃんは遊びたい！</t>
+          <t>いとこのこ</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>丈(著者)</t>
+          <t>いぬちく(著者)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第125話</t>
+          <t>休載イラスト</t>
         </is>
       </c>
     </row>
@@ -20328,17 +21370,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>よくわからないけれど異世界に転生していたようです</t>
+          <t>リビルドワールド</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>内々けやき あし カオミン</t>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第136話 よくわからないけれどスカウトされたみたいです（１）</t>
+          <t>第71話②</t>
         </is>
       </c>
     </row>
@@ -20348,17 +21390,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>くらいあの子としたいこと</t>
+          <t>宇崎ちゃんは遊びたい！</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>碇マナツ(著者)</t>
+          <t>丈(著者)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第80話</t>
+          <t>第125話</t>
         </is>
       </c>
     </row>
@@ -20368,17 +21410,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>小林さんちのメイドラゴン</t>
+          <t>アイドル辞めるけど結婚してくれますか!?</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>クール教信者</t>
+          <t>三吉汐美(著者)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第146話</t>
+          <t>第16話後半</t>
         </is>
       </c>
     </row>
@@ -20388,17 +21430,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>理想のヒモ生活</t>
+          <t>ダメ人間の愛しかた</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+          <t>岩葉(著者)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第86話　その1</t>
+          <t>第18話後編　ダメ人間とお姉ちゃんと彼女</t>
         </is>
       </c>
     </row>
@@ -20408,17 +21450,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>最強勇者パーティーは愛が知りたい</t>
+          <t>魔都精兵のスレイブ</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>山田肌襦袢</t>
+          <t>原作:タカヒロ　漫画:竹村洋平</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第27話「エッチな祭りを始めたい」</t>
+          <t>第157話　神域へ</t>
         </is>
       </c>
     </row>
@@ -20428,17 +21470,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
+          <t>理想の彼女</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>神原絵理華(漫画) 一森一輝(原作)</t>
+          <t>もりまりも(著者)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第18話①</t>
+          <t>番外編4</t>
         </is>
       </c>
     </row>
@@ -20448,17 +21490,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ゲーセン少女と異文化交流</t>
+          <t>宮廷鍛冶師の幸せな日常 ～ブラックな職場を追放されたが、隣国で公爵令嬢に溺愛されながらホワイトな生活送ります～</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>安原宏和(著者)</t>
+          <t>上林眞(著者) 木嶋隆太(原作) a20(キャラクター原案)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第126話</t>
+          <t>第2話-②</t>
         </is>
       </c>
     </row>
@@ -20468,17 +21510,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
+          <t>無敵商人の異世界成り上がり物語 ～現代の製品を自在に取り寄せるスキルがあるので異世界では楽勝です～</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
+          <t>隆原ヒロタ(漫画) 青山有(原作) ぷきゅのすけ(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第74話 トワイライト</t>
+          <t>第35話①</t>
         </is>
       </c>
     </row>
@@ -20488,17 +21530,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ヤンデレかと思ったらもっとヤベー女だった</t>
+          <t>転生してあらゆるモノに好かれながら異世界で好きな事をして生きて行く</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>八木戸マト</t>
+          <t>都尾琉(漫画) 御峰。(原作)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第67話　全てを間違えたヤンデレ彼女</t>
+          <t>第26話③</t>
         </is>
       </c>
     </row>
@@ -20508,17 +21550,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>王都の外れの錬金術師 ～ハズレ職業だったので、のんびりお店経営します～</t>
+          <t>異世界おじさん</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>あさなや(著者) yocco(原作) 純粋(キャラクター原案)</t>
+          <t>殆ど死んでいる(著者)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>element.49</t>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
@@ -20528,17 +21570,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>ベヒモスの花婿</t>
+          <t>リアリスト魔王による聖域なき異世界改革</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>鈴音ことら(原作) 月並甲介(漫画)</t>
+          <t>鈴木マナツ(漫画) 羽田遼亮(原作) ゆーげん(キャラクターデザイン) ひたきゆう(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第7話②</t>
+          <t>第67幕②</t>
         </is>
       </c>
     </row>
@@ -20548,17 +21590,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>異世界おじさん</t>
+          <t>アラサーがVTuberになった話。</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>殆ど死んでいる(著者)</t>
+          <t>犬威赤彦(漫画) とくめい(原作) カラスBTK(キャラクター原案)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+          <t>第23話</t>
         </is>
       </c>
     </row>
@@ -20568,17 +21610,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>修羅幼女の英雄譚～半端者と言われた傭兵、幼女に転生して成り上がる～</t>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>作画：むらたん 原作：沙城流</t>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第7話(2)</t>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
@@ -20588,17 +21630,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>推しにささげるダンジョングルメ ～最強探索者VTuberになる～</t>
+          <t>俺堕ちスレイブヒーローコレクション</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>モノクロウサギ(原作) 藍川蓮(漫画)</t>
+          <t>ゆっ栗栖(著者)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>CHAPTER　10-3</t>
+          <t>第11話前半</t>
         </is>
       </c>
     </row>
@@ -20608,17 +21650,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>顔に出ない柏田さんと顔に出る太田君＋</t>
+          <t>貴方は猫（わたし）の下僕です ～ねことげぼくのヒミツなカンケイ～</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>東ふゆ(著者)</t>
+          <t>大田優一(著者)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第30話 田沼先生の秘密</t>
+          <t>第14話前半</t>
         </is>
       </c>
     </row>
@@ -20628,17 +21670,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>生活魔法使いの下剋上</t>
+          <t>チュートリアルが始まる前に ボスキャラ達を破滅させない為に俺ができる幾つかの事</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>保志レンジ(著者) 月汰元(原作) ｈｉｍｅｓｕｚ(キャラクター原案)</t>
+          <t>横山コウヂ(漫画) 髙橋炬燵(原作) カカオ・ランタン(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第26話-2</t>
+          <t>第13話③</t>
         </is>
       </c>
     </row>
@@ -20648,17 +21690,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>なぜかS級美女達の話題に俺があがる件</t>
+          <t>王様ランキング200話～</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>ジョN(著者) 脇岡こなつ(原作) magako(キャラクター原案)</t>
+          <t>十日草輔（とおかそうすけ）</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第9話-2</t>
+          <t>第261話</t>
         </is>
       </c>
     </row>
@@ -20668,17 +21710,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>スキルがなければレベルを上げる～９９がカンストの世界でレベル800万からスタート～</t>
+          <t>ハーレムより平穏を！異世界で静かにニート姫させてくれ</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>倉橋ユウス(漫画) 岡沢六十四(原作)</t>
+          <t>さかたはるき(原作) かわやばぐ(作画)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第51話③</t>
+          <t>第13話後半</t>
         </is>
       </c>
     </row>
@@ -20688,17 +21730,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+          <t>愚かな天使は悪魔と踊る</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+          <t>アズマサワヨシ(著者)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+          <t>第100話②</t>
         </is>
       </c>
     </row>
@@ -20708,17 +21750,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>お前妹じゃなくて許嫁だったのかよ!?</t>
+          <t>くらいあの子としたいこと</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>湯猫子(漫画) 未来人A(原作)</t>
+          <t>碇マナツ(著者)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第28話</t>
+          <t>第80話</t>
         </is>
       </c>
     </row>
@@ -20728,17 +21770,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>パワハラギルマスをぶん殴ってブラック聖剣ギルドをクビになったので、辺境で聖剣工房を開くことにした</t>
+          <t>よくわからないけれど異世界に転生していたようです</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>だいたいねむい(原作) まお(漫画)</t>
+          <t>内々けやき あし カオミン</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第9話④</t>
+          <t>第136話 よくわからないけれどスカウトされたみたいです（１）</t>
         </is>
       </c>
     </row>
@@ -20748,17 +21790,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>底辺冒険者だけど魔法を極めてみることにした ～無能スキルから神スキルに進化した【魔法創造】と【アイテム作成】で無双する～</t>
+          <t>きみの願いが叶うまで</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>蒼乃白兎 坂野杏梨 かわく</t>
+          <t>浅月のりと(著者)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第44話(前編) 救世主</t>
+          <t>第3話-2</t>
         </is>
       </c>
     </row>
@@ -20768,17 +21810,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>異世界転移したら愛犬が最強になりました～シルバーフェンリルと俺が異世界暮らしを始めたら～</t>
+          <t>小林さんちのメイドラゴン</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>漫画：一花ハナ 原作：龍央 キャラクター原案：りりんら</t>
+          <t>クール教信者</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第36話後半</t>
+          <t>第146話</t>
         </is>
       </c>
     </row>
@@ -20788,17 +21830,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ダウナーお姉さんは遊びたい</t>
+          <t>豚のレバーは加熱しろ</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>山鷹景</t>
+          <t>みなみ(漫画) 逆井卓馬(原作) 遠坂あさぎ(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第14話</t>
+          <t>第42話①</t>
         </is>
       </c>
     </row>
@@ -20808,17 +21850,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>傭兵団の愛し子 ～死にかけ孤児は最強師匠たちに育てられる～</t>
+          <t>理想のヒモ生活</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>柿野レイ(漫画) 天野雪人(原作) 黒井ススム(キャラクター原案)</t>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第6話後編：召喚士ウィル</t>
+          <t>第86話　その1</t>
         </is>
       </c>
     </row>
@@ -20828,17 +21870,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>限界超えの天賦は、転生者にしか扱えない ― オーバーリミット・スキルホルダー ―</t>
+          <t>おっさん、転生して天才役者になる</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>長月みそか(漫画) 三上康明(原作) 大槍葦人(キャラクターデザイン)</t>
+          <t>芽々ノ圭(漫画) ほえ太郎(原作)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第3章［13］後半</t>
+          <t>第37話②</t>
         </is>
       </c>
     </row>
@@ -20848,17 +21890,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>クラスの大嫌いな女子と結婚することになった。</t>
+          <t>最強勇者パーティーは愛が知りたい</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>天乃聖樹(原作) もすこんぶ(漫画)</t>
+          <t>山田肌襦袢</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第44話-1</t>
+          <t>第27話「エッチな祭りを始めたい」</t>
         </is>
       </c>
     </row>
@@ -20868,17 +21910,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>勇者パーティから追い出された不遇職【罠士】、ユニークスキル【矢印】で最強になる</t>
+          <t>怪異部～M県Y市の怪現象について～</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>作画：たつひこ 原作：白石 有希</t>
+          <t>さりい・Ｂ(著者)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第7話(2)</t>
+          <t>File.6</t>
         </is>
       </c>
     </row>
@@ -20888,17 +21930,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>義妹生活</t>
+          <t>ゲーセン少女と異文化交流</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>三河ごーすと(原作) 奏ユミカ(漫画) Hiten(キャラクター原案)</t>
+          <t>安原宏和(著者)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第30話-2</t>
+          <t>第126話</t>
         </is>
       </c>
     </row>
@@ -20908,17 +21950,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>やっぱ人間やめて正解だわ</t>
+          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>偽BEなんとか</t>
+          <t>神原絵理華(漫画) 一森一輝(原作)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第15話　こちら世界の中心からお届け</t>
+          <t>第18話①</t>
         </is>
       </c>
     </row>
@@ -20928,17 +21970,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>レベル1で挑む縛りプレイ!</t>
+          <t>終末ツーリング</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>北川ニキタ 大鐘いしや 刀 彼方</t>
+          <t>さいとー栄(著者)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>最終話 最高の気分①</t>
+          <t>第48話 三沢基地　その４②</t>
         </is>
       </c>
     </row>
@@ -20948,17 +21990,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>双子の姉が神子として引き取られて、私は捨てられたけど多分私が神子である。</t>
+          <t>王都の外れの錬金術師 ～ハズレ職業だったので、のんびりお店経営します～</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>雪(著者) 池中織奈(原作) カット(キャラクター原案)</t>
+          <t>あさなや(著者) yocco(原作) 純粋(キャラクター原案)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第32話前編</t>
+          <t>element.49</t>
         </is>
       </c>
     </row>
@@ -20968,17 +22010,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>生徒会にも穴はある！</t>
+          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>むちまろ</t>
+          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第131話	ありす大ピンチ！（デジャブ編）</t>
+          <t>第74話 トワイライト</t>
         </is>
       </c>
     </row>
@@ -20988,17 +22030,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>ブレイド＆バスタード</t>
+          <t>魔王学園の反逆者 ～人類初の魔王候補、眷属少女と王座を目指して成り上がる～</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>漫画/楓月 誠 原作/蝸牛くも キャラクター原案/so-bin</t>
+          <t>溝口ぜらちん(作画) 久慈マサムネ(原作) ｋａｋａｏ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第10話（2）</t>
+          <t>最終話</t>
         </is>
       </c>
     </row>
@@ -21008,17 +22050,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>ちびっこ賢者、Lv.1から異世界でがんばります！</t>
+          <t>お前妹じゃなくて許嫁だったのかよ!?</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>みさき樹里(漫画) 彩戸ゆめ(原作) 竹花ノート(キャラクターデザイン)</t>
+          <t>湯猫子(漫画) 未来人A(原作)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第37話</t>
+          <t>第28話</t>
         </is>
       </c>
     </row>
@@ -21028,17 +22070,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>やめてくれ、強いのは俺じゃなくて剣なんだ……！</t>
+          <t>ヤンデレかと思ったらもっとヤベー女だった</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>漫画/廃狼 原作/馬路まんじ キャラクター原案/かぼちゃ</t>
+          <t>八木戸マト</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第7話（3）</t>
+          <t>第67話　全てを間違えたヤンデレ彼女</t>
         </is>
       </c>
     </row>
@@ -21048,17 +22090,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>チンチンデビルを追え！</t>
+          <t>顔に出ない柏田さんと顔に出る太田君＋</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>くぼたふみお</t>
+          <t>東ふゆ(著者)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第３０話　仲間のため振るう力…！</t>
+          <t>第30話 田沼先生の秘密</t>
         </is>
       </c>
     </row>
@@ -21068,17 +22110,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>異世界のんびり農家の日常</t>
+          <t>ベヒモスの花婿</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>ユウズィ(著者) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+          <t>鈴音ことら(原作) 月並甲介(漫画)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>収穫その36</t>
+          <t>第7話②</t>
         </is>
       </c>
     </row>
@@ -21088,17 +22130,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>ライドンキング</t>
+          <t>パワハラギルマスをぶん殴ってブラック聖剣ギルドをクビになったので、辺境で聖剣工房を開くことにした</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>馬場康誌</t>
+          <t>だいたいねむい(原作) まお(漫画)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第81話 大統領と失われた神器（前編）</t>
+          <t>第9話④</t>
         </is>
       </c>
     </row>
@@ -21108,17 +22150,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>ギルドを追放された回復術士、実は魔力無限だったので規格外の回復魔法で伝説となる</t>
+          <t>異世界たぬき</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>漫画：坂下コウ 原作：霞杏檎</t>
+          <t>小林安曇</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第4話(1)</t>
+          <t>第1話</t>
         </is>
       </c>
     </row>
@@ -21128,17 +22170,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>魔王学園の反逆者 ～人類初の魔王候補、眷属少女と王座を目指して成り上がる～</t>
+          <t>底辺冒険者だけど魔法を極めてみることにした ～無能スキルから神スキルに進化した【魔法創造】と【アイテム作成】で無双する～</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>溝口ぜらちん(作画) 久慈マサムネ(原作) ｋａｋａｏ(キャラクター原案)</t>
+          <t>蒼乃白兎 坂野杏梨 かわく</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>最終話</t>
+          <t>第44話(前編) 救世主</t>
         </is>
       </c>
     </row>
@@ -21148,17 +22190,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>瞳ちゃんは人見知り</t>
+          <t>生徒会にも穴はある！</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>夏海ちょりすけ</t>
+          <t>むちまろ</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第136話</t>
+          <t>第131話	ありす大ピンチ！（デジャブ編）</t>
         </is>
       </c>
     </row>
@@ -21168,17 +22210,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>隠居暮らしのおっさん、女王陛下の剣となる</t>
+          <t>生活魔法使いの下剋上</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>漫画/半二合 原作/天酒之瓢 キャラクター原案/みことあけみ</t>
+          <t>保志レンジ(著者) 月汰元(原作) ｈｉｍｅｓｕｚ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第5話（2）</t>
+          <t>第26話-2</t>
         </is>
       </c>
     </row>
@@ -21188,17 +22230,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>転生して成長チートを手に入れたら、最凶スキルもついたのですが!?</t>
+          <t>なぜかS級美女達の話題に俺があがる件</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>やま ゆずもと 我美蘭</t>
+          <t>ジョN(著者) 脇岡こなつ(原作) magako(キャラクター原案)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第10話</t>
+          <t>第9話-2</t>
         </is>
       </c>
     </row>
@@ -21208,17 +22250,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+          <t>ダウナーお姉さんは遊びたい</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>村上よしゆき 茨木野 あるてら</t>
+          <t>山鷹景</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第４０話　勇者、聖女と元聖騎士と再会し、魚人を追っ払う（５）</t>
+          <t>第14話</t>
         </is>
       </c>
     </row>
@@ -21228,12 +22270,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>錬金術師の辺境再生スローライフ～S級パーティーで孤立した少女をかばったら追放されたので、一緒に幸せに暮らします～</t>
+          <t>修羅幼女の英雄譚～半端者と言われた傭兵、幼女に転生して成り上がる～</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>作画：弥永扇 原作：三月菫</t>
+          <t>作画：むらたん 原作：沙城流</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -21248,17 +22290,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>影の英雄の日常譚 勇者の裏で暗躍していた最強のエージェント。組織が解体されたので、正体隠して人並みの日常を謳歌する。</t>
+          <t>異世界転移したら愛犬が最強になりました～シルバーフェンリルと俺が異世界暮らしを始めたら～</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>kanco(漫画) 坂石遊作(原作) TYONE(キャラクター原案)</t>
+          <t>漫画：一花ハナ 原作：龍央 キャラクター原案：りりんら</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Episode32-3</t>
+          <t>第36話後半</t>
         </is>
       </c>
     </row>
@@ -21268,17 +22310,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>ライブダンジョン！</t>
+          <t>クラスの大嫌いな女子と結婚することになった。</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
+          <t>天乃聖樹(原作) もすこんぶ(漫画)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第88話前半</t>
+          <t>第44話-1</t>
         </is>
       </c>
     </row>
@@ -21288,17 +22330,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>追放されたおっさんタンク、実は防御力最強だったのでダメージゼロで無双する</t>
+          <t>やっぱ人間やめて正解だわ</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>漫画：化野九十九 原作：あけちともあき</t>
+          <t>偽BEなんとか</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第4話(1)</t>
+          <t>第15話　こちら世界の中心からお届け</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-07-21
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -35,6 +35,7 @@
     <sheet name="2025-07-18" sheetId="27" state="visible" r:id="rId27"/>
     <sheet name="2025-07-19" sheetId="28" state="visible" r:id="rId28"/>
     <sheet name="2025-07-20" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="2025-07-21" sheetId="30" state="visible" r:id="rId30"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -21345,1000 +21346,1000 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="0" t="inlineStr">
         <is>
           <t>いとこのこ</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="0" t="inlineStr">
         <is>
           <t>いぬちく(著者)</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="0" t="inlineStr">
         <is>
           <t>休載イラスト</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="0" t="inlineStr">
         <is>
           <t>リビルドワールド</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="0" t="inlineStr">
         <is>
           <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" s="0" t="inlineStr">
         <is>
           <t>第71話②</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="0" t="inlineStr">
         <is>
           <t>宇崎ちゃんは遊びたい！</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="0" t="inlineStr">
         <is>
           <t>丈(著者)</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" s="0" t="inlineStr">
         <is>
           <t>第125話</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="0" t="inlineStr">
         <is>
           <t>アイドル辞めるけど結婚してくれますか!?</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="0" t="inlineStr">
         <is>
           <t>三吉汐美(著者)</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D5" s="0" t="inlineStr">
         <is>
           <t>第16話後半</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="0" t="inlineStr">
         <is>
           <t>ダメ人間の愛しかた</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" s="0" t="inlineStr">
         <is>
           <t>岩葉(著者)</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D6" s="0" t="inlineStr">
         <is>
           <t>第18話後編　ダメ人間とお姉ちゃんと彼女</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="0" t="inlineStr">
         <is>
           <t>魔都精兵のスレイブ</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="0" t="inlineStr">
         <is>
           <t>原作:タカヒロ　漫画:竹村洋平</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D7" s="0" t="inlineStr">
         <is>
           <t>第157話　神域へ</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" s="0" t="inlineStr">
         <is>
           <t>理想の彼女</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" s="0" t="inlineStr">
         <is>
           <t>もりまりも(著者)</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D8" s="0" t="inlineStr">
         <is>
           <t>番外編4</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="0" t="inlineStr">
         <is>
           <t>宮廷鍛冶師の幸せな日常 ～ブラックな職場を追放されたが、隣国で公爵令嬢に溺愛されながらホワイトな生活送ります～</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" s="0" t="inlineStr">
         <is>
           <t>上林眞(著者) 木嶋隆太(原作) a20(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D9" s="0" t="inlineStr">
         <is>
           <t>第2話-②</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" s="0" t="inlineStr">
         <is>
           <t>無敵商人の異世界成り上がり物語 ～現代の製品を自在に取り寄せるスキルがあるので異世界では楽勝です～</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" s="0" t="inlineStr">
         <is>
           <t>隆原ヒロタ(漫画) 青山有(原作) ぷきゅのすけ(キャラクターデザイン)</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D10" s="0" t="inlineStr">
         <is>
           <t>第35話①</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" s="0" t="inlineStr">
         <is>
           <t>転生してあらゆるモノに好かれながら異世界で好きな事をして生きて行く</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" s="0" t="inlineStr">
         <is>
           <t>都尾琉(漫画) 御峰。(原作)</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D11" s="0" t="inlineStr">
         <is>
           <t>第26話③</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
+      <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" s="0" t="inlineStr">
         <is>
           <t>異世界おじさん</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" s="0" t="inlineStr">
         <is>
           <t>殆ど死んでいる(著者)</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D12" s="0" t="inlineStr">
         <is>
           <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
+      <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" s="0" t="inlineStr">
         <is>
           <t>リアリスト魔王による聖域なき異世界改革</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" s="0" t="inlineStr">
         <is>
           <t>鈴木マナツ(漫画) 羽田遼亮(原作) ゆーげん(キャラクターデザイン) ひたきゆう(キャラクターデザイン)</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D13" s="0" t="inlineStr">
         <is>
           <t>第67幕②</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
+      <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B14" s="0" t="inlineStr">
         <is>
           <t>アラサーがVTuberになった話。</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C14" s="0" t="inlineStr">
         <is>
           <t>犬威赤彦(漫画) とくめい(原作) カラスBTK(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D14" s="0" t="inlineStr">
         <is>
           <t>第23話</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
+      <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B15" s="0" t="inlineStr">
         <is>
           <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C15" s="0" t="inlineStr">
         <is>
           <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D15" s="0" t="inlineStr">
         <is>
           <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
+      <c r="A16" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B16" s="0" t="inlineStr">
         <is>
           <t>俺堕ちスレイブヒーローコレクション</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C16" s="0" t="inlineStr">
         <is>
           <t>ゆっ栗栖(著者)</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="D16" s="0" t="inlineStr">
         <is>
           <t>第11話前半</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
+      <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B17" s="0" t="inlineStr">
         <is>
           <t>貴方は猫（わたし）の下僕です ～ねことげぼくのヒミツなカンケイ～</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C17" s="0" t="inlineStr">
         <is>
           <t>大田優一(著者)</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="D17" s="0" t="inlineStr">
         <is>
           <t>第14話前半</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
+      <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B18" s="0" t="inlineStr">
         <is>
           <t>チュートリアルが始まる前に ボスキャラ達を破滅させない為に俺ができる幾つかの事</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C18" s="0" t="inlineStr">
         <is>
           <t>横山コウヂ(漫画) 髙橋炬燵(原作) カカオ・ランタン(キャラクターデザイン)</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="D18" s="0" t="inlineStr">
         <is>
           <t>第13話③</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
+      <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B19" s="0" t="inlineStr">
         <is>
           <t>王様ランキング200話～</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C19" s="0" t="inlineStr">
         <is>
           <t>十日草輔（とおかそうすけ）</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="D19" s="0" t="inlineStr">
         <is>
           <t>第261話</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
+      <c r="A20" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B20" s="0" t="inlineStr">
         <is>
           <t>ハーレムより平穏を！異世界で静かにニート姫させてくれ</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C20" s="0" t="inlineStr">
         <is>
           <t>さかたはるき(原作) かわやばぐ(作画)</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="D20" s="0" t="inlineStr">
         <is>
           <t>第13話後半</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
+      <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B21" s="0" t="inlineStr">
         <is>
           <t>愚かな天使は悪魔と踊る</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C21" s="0" t="inlineStr">
         <is>
           <t>アズマサワヨシ(著者)</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="D21" s="0" t="inlineStr">
         <is>
           <t>第100話②</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
+      <c r="A22" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B22" s="0" t="inlineStr">
         <is>
           <t>くらいあの子としたいこと</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C22" s="0" t="inlineStr">
         <is>
           <t>碇マナツ(著者)</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="D22" s="0" t="inlineStr">
         <is>
           <t>第80話</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="n">
+      <c r="A23" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B23" s="0" t="inlineStr">
         <is>
           <t>よくわからないけれど異世界に転生していたようです</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C23" s="0" t="inlineStr">
         <is>
           <t>内々けやき あし カオミン</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="D23" s="0" t="inlineStr">
         <is>
           <t>第136話 よくわからないけれどスカウトされたみたいです（１）</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="n">
+      <c r="A24" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B24" s="0" t="inlineStr">
         <is>
           <t>きみの願いが叶うまで</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="C24" s="0" t="inlineStr">
         <is>
           <t>浅月のりと(著者)</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="D24" s="0" t="inlineStr">
         <is>
           <t>第3話-2</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="n">
+      <c r="A25" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="B25" s="0" t="inlineStr">
         <is>
           <t>小林さんちのメイドラゴン</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C25" s="0" t="inlineStr">
         <is>
           <t>クール教信者</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="D25" s="0" t="inlineStr">
         <is>
           <t>第146話</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="n">
+      <c r="A26" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="B26" s="0" t="inlineStr">
         <is>
           <t>豚のレバーは加熱しろ</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="C26" s="0" t="inlineStr">
         <is>
           <t>みなみ(漫画) 逆井卓馬(原作) 遠坂あさぎ(キャラクターデザイン)</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="D26" s="0" t="inlineStr">
         <is>
           <t>第42話①</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="n">
+      <c r="A27" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="B27" s="0" t="inlineStr">
         <is>
           <t>理想のヒモ生活</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="C27" s="0" t="inlineStr">
         <is>
           <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="D27" s="0" t="inlineStr">
         <is>
           <t>第86話　その1</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="n">
+      <c r="A28" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B28" s="0" t="inlineStr">
         <is>
           <t>おっさん、転生して天才役者になる</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C28" s="0" t="inlineStr">
         <is>
           <t>芽々ノ圭(漫画) ほえ太郎(原作)</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="D28" s="0" t="inlineStr">
         <is>
           <t>第37話②</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="n">
+      <c r="A29" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="B29" s="0" t="inlineStr">
         <is>
           <t>最強勇者パーティーは愛が知りたい</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="C29" s="0" t="inlineStr">
         <is>
           <t>山田肌襦袢</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="D29" s="0" t="inlineStr">
         <is>
           <t>第27話「エッチな祭りを始めたい」</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="n">
+      <c r="A30" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="B30" s="0" t="inlineStr">
         <is>
           <t>怪異部～M県Y市の怪現象について～</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="C30" s="0" t="inlineStr">
         <is>
           <t>さりい・Ｂ(著者)</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="D30" s="0" t="inlineStr">
         <is>
           <t>File.6</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="n">
+      <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="B31" s="0" t="inlineStr">
         <is>
           <t>ゲーセン少女と異文化交流</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="C31" s="0" t="inlineStr">
         <is>
           <t>安原宏和(著者)</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="D31" s="0" t="inlineStr">
         <is>
           <t>第126話</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="n">
+      <c r="A32" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="B32" s="0" t="inlineStr">
         <is>
           <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="C32" s="0" t="inlineStr">
         <is>
           <t>神原絵理華(漫画) 一森一輝(原作)</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="D32" s="0" t="inlineStr">
         <is>
           <t>第18話①</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="n">
+      <c r="A33" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="B33" s="0" t="inlineStr">
         <is>
           <t>終末ツーリング</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="C33" s="0" t="inlineStr">
         <is>
           <t>さいとー栄(著者)</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="D33" s="0" t="inlineStr">
         <is>
           <t>第48話 三沢基地　その４②</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="n">
+      <c r="A34" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B34" s="0" t="inlineStr">
         <is>
           <t>王都の外れの錬金術師 ～ハズレ職業だったので、のんびりお店経営します～</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="C34" s="0" t="inlineStr">
         <is>
           <t>あさなや(著者) yocco(原作) 純粋(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="D34" s="0" t="inlineStr">
         <is>
           <t>element.49</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="n">
+      <c r="A35" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="B35" s="0" t="inlineStr">
         <is>
           <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="C35" s="0" t="inlineStr">
         <is>
           <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="D35" s="0" t="inlineStr">
         <is>
           <t>第74話 トワイライト</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="n">
+      <c r="A36" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="B36" s="0" t="inlineStr">
         <is>
           <t>魔王学園の反逆者 ～人類初の魔王候補、眷属少女と王座を目指して成り上がる～</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="C36" s="0" t="inlineStr">
         <is>
           <t>溝口ぜらちん(作画) 久慈マサムネ(原作) ｋａｋａｏ(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="D36" s="0" t="inlineStr">
         <is>
           <t>最終話</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="n">
+      <c r="A37" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="B37" s="0" t="inlineStr">
         <is>
           <t>お前妹じゃなくて許嫁だったのかよ!?</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="C37" s="0" t="inlineStr">
         <is>
           <t>湯猫子(漫画) 未来人A(原作)</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
+      <c r="D37" s="0" t="inlineStr">
         <is>
           <t>第28話</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="n">
+      <c r="A38" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="B38" s="0" t="inlineStr">
         <is>
           <t>ヤンデレかと思ったらもっとヤベー女だった</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
+      <c r="C38" s="0" t="inlineStr">
         <is>
           <t>八木戸マト</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
+      <c r="D38" s="0" t="inlineStr">
         <is>
           <t>第67話　全てを間違えたヤンデレ彼女</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="n">
+      <c r="A39" s="0" t="n">
         <v>38</v>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="B39" s="0" t="inlineStr">
         <is>
           <t>顔に出ない柏田さんと顔に出る太田君＋</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="C39" s="0" t="inlineStr">
         <is>
           <t>東ふゆ(著者)</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
+      <c r="D39" s="0" t="inlineStr">
         <is>
           <t>第30話 田沼先生の秘密</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="n">
+      <c r="A40" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="B40" s="0" t="inlineStr">
         <is>
           <t>ベヒモスの花婿</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="C40" s="0" t="inlineStr">
         <is>
           <t>鈴音ことら(原作) 月並甲介(漫画)</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="D40" s="0" t="inlineStr">
         <is>
           <t>第7話②</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="n">
+      <c r="A41" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="B41" s="0" t="inlineStr">
         <is>
           <t>パワハラギルマスをぶん殴ってブラック聖剣ギルドをクビになったので、辺境で聖剣工房を開くことにした</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="C41" s="0" t="inlineStr">
         <is>
           <t>だいたいねむい(原作) まお(漫画)</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
+      <c r="D41" s="0" t="inlineStr">
         <is>
           <t>第9話④</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="n">
+      <c r="A42" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="B42" s="0" t="inlineStr">
         <is>
           <t>異世界たぬき</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="C42" s="0" t="inlineStr">
         <is>
           <t>小林安曇</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
+      <c r="D42" s="0" t="inlineStr">
         <is>
           <t>第1話</t>
         </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="n">
+      <c r="A43" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B43" s="0" t="inlineStr">
         <is>
           <t>底辺冒険者だけど魔法を極めてみることにした ～無能スキルから神スキルに進化した【魔法創造】と【アイテム作成】で無双する～</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="C43" s="0" t="inlineStr">
         <is>
           <t>蒼乃白兎 坂野杏梨 かわく</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
+      <c r="D43" s="0" t="inlineStr">
         <is>
           <t>第44話(前編) 救世主</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="n">
+      <c r="A44" s="0" t="n">
         <v>43</v>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="B44" s="0" t="inlineStr">
         <is>
           <t>生徒会にも穴はある！</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="C44" s="0" t="inlineStr">
         <is>
           <t>むちまろ</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
+      <c r="D44" s="0" t="inlineStr">
         <is>
           <t>第131話	ありす大ピンチ！（デジャブ編）</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="n">
+      <c r="A45" s="0" t="n">
         <v>44</v>
       </c>
-      <c r="B45" t="inlineStr">
+      <c r="B45" s="0" t="inlineStr">
         <is>
           <t>生活魔法使いの下剋上</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="C45" s="0" t="inlineStr">
         <is>
           <t>保志レンジ(著者) 月汰元(原作) ｈｉｍｅｓｕｚ(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
+      <c r="D45" s="0" t="inlineStr">
         <is>
           <t>第26話-2</t>
         </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="n">
+      <c r="A46" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="B46" t="inlineStr">
+      <c r="B46" s="0" t="inlineStr">
         <is>
           <t>なぜかS級美女達の話題に俺があがる件</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="C46" s="0" t="inlineStr">
         <is>
           <t>ジョN(著者) 脇岡こなつ(原作) magako(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
+      <c r="D46" s="0" t="inlineStr">
         <is>
           <t>第9話-2</t>
         </is>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="n">
+      <c r="A47" s="0" t="n">
         <v>46</v>
       </c>
-      <c r="B47" t="inlineStr">
+      <c r="B47" s="0" t="inlineStr">
         <is>
           <t>ダウナーお姉さんは遊びたい</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="C47" s="0" t="inlineStr">
         <is>
           <t>山鷹景</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
+      <c r="D47" s="0" t="inlineStr">
         <is>
           <t>第14話</t>
         </is>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="n">
+      <c r="A48" s="0" t="n">
         <v>47</v>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="B48" s="0" t="inlineStr">
         <is>
           <t>修羅幼女の英雄譚～半端者と言われた傭兵、幼女に転生して成り上がる～</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
+      <c r="C48" s="0" t="inlineStr">
         <is>
           <t>作画：むらたん 原作：沙城流</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
+      <c r="D48" s="0" t="inlineStr">
         <is>
           <t>第7話(2)</t>
         </is>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="n">
+      <c r="A49" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="B49" s="0" t="inlineStr">
         <is>
           <t>異世界転移したら愛犬が最強になりました～シルバーフェンリルと俺が異世界暮らしを始めたら～</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="C49" s="0" t="inlineStr">
         <is>
           <t>漫画：一花ハナ 原作：龍央 キャラクター原案：りりんら</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
+      <c r="D49" s="0" t="inlineStr">
         <is>
           <t>第36話後半</t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="n">
+      <c r="A50" s="0" t="n">
         <v>49</v>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="B50" s="0" t="inlineStr">
         <is>
           <t>クラスの大嫌いな女子と結婚することになった。</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="C50" s="0" t="inlineStr">
         <is>
           <t>天乃聖樹(原作) もすこんぶ(漫画)</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
+      <c r="D50" s="0" t="inlineStr">
         <is>
           <t>第44話-1</t>
         </is>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="n">
+      <c r="A51" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="B51" s="0" t="inlineStr">
         <is>
           <t>やっぱ人間やめて正解だわ</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="C51" s="0" t="inlineStr">
         <is>
           <t>偽BEなんとか</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
+      <c r="D51" s="0" t="inlineStr">
         <is>
           <t>第15話　こちら世界の中心からお届け</t>
         </is>
@@ -23390,6 +23391,1047 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>姫様“拷問”の時間です</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>拷問145</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>第4話-2：師匠と弟子の新生活</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>窓際編集とバカにされた俺が、双子ＪＫと同居することになった</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>うさおとめ(著者) 茨木野(原作) トモゼロ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>第4話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>宇崎ちゃんは遊びたい！</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>丈(著者)</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>第125話</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>異世界おじさん</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>殆ど死んでいる(著者)</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>悪役貴族として必要なそれ</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>まさこりん(原作) 夏野うみ(作画) 村カルキ(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>第17話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>いとこのこ</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>いぬちく(著者)</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>休載イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>おんなのこのけんをてにいれた</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>福岡太朗(著者)</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>15本目</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>アイドル辞めるけど結婚してくれますか!?</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>三吉汐美(著者)</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>第16話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>第71話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>「才能の器」で目指す迷宮最深部 スキル横伸ばしのはずが、万能チートだった!</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>漫画：かくばやしつよし 原作：とんび キャラクター原案： りりんら</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>第39話</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ダメ人間の愛しかた</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>岩葉(著者)</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>第18話後編　ダメ人間とお姉ちゃんと彼女</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>異世界迷宮のオーパーツ</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>三狛ハル(著者)</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>第2話-②：立派な棒と革と玉</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>理想の彼女</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>もりまりも(著者)</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>番外編4</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>魔都精兵のスレイブ</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>原作:タカヒロ　漫画:竹村洋平</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>第157話　神域へ</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>追放された付与魔法使いの成り上がり ～勇者パーティを陰から支えていたと知らなかったので戻って来い？【剣聖】と【賢者】の美少女たちに囲まれて幸せなので戻りません～</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>原作：蒼月浩二 漫画：伊香透 キャラクター原案：nima</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>第23話</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>宮廷鍛冶師の幸せな日常 ～ブラックな職場を追放されたが、隣国で公爵令嬢に溺愛されながらホワイトな生活送ります～</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>上林眞(著者) 木嶋隆太(原作) a20(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>第2話-②</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>半人前の恋人</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>川田大智</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>第48話</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>無敵商人の異世界成り上がり物語 ～現代の製品を自在に取り寄せるスキルがあるので異世界では楽勝です～</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>隆原ヒロタ(漫画) 青山有(原作) ぷきゅのすけ(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>第35話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>貴方は猫（わたし）の下僕です ～ねことげぼくのヒミツなカンケイ～</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>大田優一(著者)</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>第14話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>リアリスト魔王による聖域なき異世界改革</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>鈴木マナツ(漫画) 羽田遼亮(原作) ゆーげん(キャラクターデザイン) ひたきゆう(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>第67幕②</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>俺堕ちスレイブヒーローコレクション</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>ゆっ栗栖(著者)</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>第11話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>第136話 よくわからないけれどスカウトされたみたいです（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>アラサーがVTuberになった話。</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>犬威赤彦(漫画) とくめい(原作) カラスBTK(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>第23話</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>世界の終わりの世界録(アンコール)</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>雨水龍(著者) 細音啓(原作) ふゆの春秋(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>第95話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>転生してあらゆるモノに好かれながら異世界で好きな事をして生きて行く</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>都尾琉(漫画) 御峰。(原作)</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>第26話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>転生して成長チートを手に入れたら、最凶スキルもついたのですが!?</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>やま ゆずもと 我美蘭</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>第10話</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>くらいあの子としたいこと</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>碇マナツ(著者)</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>第80話</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>ダンジョンシーカーズ ～スマホアプリからはじまる現代ダンジョン制圧録～</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>原作：七篠康晴 漫画：くりきまる キャラクター原案：冬野ユウキ</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>第6話</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>ハーレムより平穏を！異世界で静かにニート姫させてくれ</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>さかたはるき(原作) かわやばぐ(作画)</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>第13話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>きみの願いが叶うまで</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>浅月のりと(著者)</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>第3話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>小林さんちのメイドラゴン</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>クール教信者</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>第146話</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>チュートリアルが始まる前に ボスキャラ達を破滅させない為に俺ができる幾つかの事</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>横山コウヂ(漫画) 髙橋炬燵(原作) カカオ・ランタン(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>第13話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>理想のヒモ生活</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>第86話　その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>陰々に鬼灯の咲く</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>絹江おばあちゃんの暴れパスタ祭り</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>第2話・土御門ハルネ</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>愚かな天使は悪魔と踊る</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>アズマサワヨシ(著者)</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>第100話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>ゲーセン少女と異文化交流</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>安原宏和(著者)</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>第126話</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>小さめの魔法師匠と大きめの魔法少女。report：3</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>とりから</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>第37話の8</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>最強勇者パーティーは愛が知りたい</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>山田肌襦袢</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>第27話「エッチな祭りを始めたい」</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>生徒会にも穴はある！</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>むちまろ</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>第131話	ありす大ピンチ！（デジャブ編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>豚のレバーは加熱しろ</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>みなみ(漫画) 逆井卓馬(原作) 遠坂あさぎ(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>第42話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>私たちはカケちがっている</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>みなもと悠</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>第1話</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>第3話 後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>第74話 トワイライト</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>王様ランキング200話～</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>十日草輔（とおかそうすけ）</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>第261話</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>王都の外れの錬金術師 ～ハズレ職業だったので、のんびりお店経営します～</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>あさなや(著者) yocco(原作) 純粋(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>element.49</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>神原絵理華(漫画) 一森一輝(原作)</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>第18話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>お前妹じゃなくて許嫁だったのかよ!?</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>湯猫子(漫画) 未来人A(原作)</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>第28話</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>第６６話『六花停止』③</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Add ranking data for 2025-07-22
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -36,6 +36,7 @@
     <sheet name="2025-07-19" sheetId="28" state="visible" r:id="rId28"/>
     <sheet name="2025-07-20" sheetId="29" state="visible" r:id="rId29"/>
     <sheet name="2025-07-21" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="2025-07-22" sheetId="31" state="visible" r:id="rId31"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -23428,22 +23429,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>姫様“拷問”の時間です</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>拷問145</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第4話-2：師匠と弟子の新生活</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>窓際編集とバカにされた俺が、双子ＪＫと同居することになった</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>うさおとめ(著者) 茨木野(原作) トモゼロ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第4話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>宇崎ちゃんは遊びたい！</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>丈(著者)</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第125話</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>異世界おじさん</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>殆ど死んでいる(著者)</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>悪役貴族として必要なそれ</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>まさこりん(原作) 夏野うみ(作画) 村カルキ(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第17話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>いとこのこ</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>いぬちく(著者)</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>休載イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>おんなのこのけんをてにいれた</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>福岡太朗(著者)</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>15本目</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>アイドル辞めるけど結婚してくれますか!?</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>三吉汐美(著者)</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第16話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第71話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>「才能の器」で目指す迷宮最深部 スキル横伸ばしのはずが、万能チートだった!</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>漫画：かくばやしつよし 原作：とんび キャラクター原案： りりんら</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第39話</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>ダメ人間の愛しかた</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>岩葉(著者)</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第18話後編　ダメ人間とお姉ちゃんと彼女</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>異世界迷宮のオーパーツ</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>三狛ハル(著者)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第2話-②：立派な棒と革と玉</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>理想の彼女</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>もりまりも(著者)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>番外編4</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>魔都精兵のスレイブ</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>原作:タカヒロ　漫画:竹村洋平</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第157話　神域へ</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>追放された付与魔法使いの成り上がり ～勇者パーティを陰から支えていたと知らなかったので戻って来い？【剣聖】と【賢者】の美少女たちに囲まれて幸せなので戻りません～</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>原作：蒼月浩二 漫画：伊香透 キャラクター原案：nima</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第23話</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>宮廷鍛冶師の幸せな日常 ～ブラックな職場を追放されたが、隣国で公爵令嬢に溺愛されながらホワイトな生活送ります～</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>上林眞(著者) 木嶋隆太(原作) a20(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第2話-②</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>半人前の恋人</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>川田大智</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第48話</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>無敵商人の異世界成り上がり物語 ～現代の製品を自在に取り寄せるスキルがあるので異世界では楽勝です～</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>隆原ヒロタ(漫画) 青山有(原作) ぷきゅのすけ(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第35話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>貴方は猫（わたし）の下僕です ～ねことげぼくのヒミツなカンケイ～</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>大田優一(著者)</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第14話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>リアリスト魔王による聖域なき異世界改革</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>鈴木マナツ(漫画) 羽田遼亮(原作) ゆーげん(キャラクターデザイン) ひたきゆう(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第67幕②</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>俺堕ちスレイブヒーローコレクション</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>ゆっ栗栖(著者)</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第11話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第136話 よくわからないけれどスカウトされたみたいです（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>アラサーがVTuberになった話。</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>犬威赤彦(漫画) とくめい(原作) カラスBTK(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第23話</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>世界の終わりの世界録(アンコール)</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>雨水龍(著者) 細音啓(原作) ふゆの春秋(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第95話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>転生してあらゆるモノに好かれながら異世界で好きな事をして生きて行く</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>都尾琉(漫画) 御峰。(原作)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第26話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>転生して成長チートを手に入れたら、最凶スキルもついたのですが!?</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>やま ゆずもと 我美蘭</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第10話</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>くらいあの子としたいこと</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>碇マナツ(著者)</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第80話</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>ダンジョンシーカーズ ～スマホアプリからはじまる現代ダンジョン制圧録～</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>原作：七篠康晴 漫画：くりきまる キャラクター原案：冬野ユウキ</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第6話</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>ハーレムより平穏を！異世界で静かにニート姫させてくれ</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>さかたはるき(原作) かわやばぐ(作画)</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第13話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>きみの願いが叶うまで</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>浅月のりと(著者)</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第3話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>小林さんちのメイドラゴン</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>クール教信者</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第146話</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>チュートリアルが始まる前に ボスキャラ達を破滅させない為に俺ができる幾つかの事</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>横山コウヂ(漫画) 髙橋炬燵(原作) カカオ・ランタン(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第13話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>理想のヒモ生活</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第86話　その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>陰々に鬼灯の咲く</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>絹江おばあちゃんの暴れパスタ祭り</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第2話・土御門ハルネ</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>愚かな天使は悪魔と踊る</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>アズマサワヨシ(著者)</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第100話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>ゲーセン少女と異文化交流</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>安原宏和(著者)</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第126話</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>小さめの魔法師匠と大きめの魔法少女。report：3</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>とりから</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第37話の8</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>最強勇者パーティーは愛が知りたい</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>山田肌襦袢</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第27話「エッチな祭りを始めたい」</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>生徒会にも穴はある！</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>むちまろ</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第131話	ありす大ピンチ！（デジャブ編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>豚のレバーは加熱しろ</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>みなみ(漫画) 逆井卓馬(原作) 遠坂あさぎ(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第42話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>私たちはカケちがっている</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>みなもと悠</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第1話</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第3話 後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第74話 トワイライト</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>王様ランキング200話～</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>十日草輔（とおかそうすけ）</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第261話</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>王都の外れの錬金術師 ～ハズレ職業だったので、のんびりお店経営します～</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>あさなや(著者) yocco(原作) 純粋(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>element.49</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>神原絵理華(漫画) 一森一輝(原作)</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第18話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>お前妹じゃなくて許嫁だったのかよ!?</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>湯猫子(漫画) 未来人A(原作)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第28話</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第６６話『六花停止』③</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>姫様“拷問”の時間です</t>
+          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>拷問145</t>
+          <t>第69話</t>
         </is>
       </c>
     </row>
@@ -23453,17 +24495,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第4話-2：師匠と弟子の新生活</t>
+          <t>第５０話　雌雄を決する器用貧乏（３）</t>
         </is>
       </c>
     </row>
@@ -23473,17 +24515,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>窓際編集とバカにされた俺が、双子ＪＫと同居することになった</t>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>うさおとめ(著者) 茨木野(原作) トモゼロ(キャラクター原案)</t>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第4話②</t>
+          <t>第２２食　ユクシーさんの覚悟、すごいのですわ！（３）</t>
         </is>
       </c>
     </row>
@@ -23493,17 +24535,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>宇崎ちゃんは遊びたい！</t>
+          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>丈(著者)</t>
+          <t>KAKERU</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第125話</t>
+          <t>第66話「東アイギス」（後半）</t>
         </is>
       </c>
     </row>
@@ -23513,17 +24555,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>異世界おじさん</t>
+          <t>回復術士のやり直し</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>殆ど死んでいる(著者)</t>
+          <t>月夜涙(原作) 羽賀ソウケン(漫画) しおこんぶ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+          <t>第72話-1</t>
         </is>
       </c>
     </row>
@@ -23533,17 +24575,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>悪役貴族として必要なそれ</t>
+          <t>異世界のすみっこで快適ものづくり生活 ～女神さまのくれた工房はちょっとやりすぎ性能だった～</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>まさこりん(原作) 夏野うみ(作画) 村カルキ(キャラクターデザイン)</t>
+          <t>西山アラタ(漫画) 長田信織(原作) 東上文(キャラクター原案)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第17話②</t>
+          <t>EP.19②</t>
         </is>
       </c>
     </row>
@@ -23553,17 +24595,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>いとこのこ</t>
+          <t>肥満令嬢は細くなり、後は傾国の美女（物理）として生きるのみ@COMIC</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>いぬちく(著者)</t>
+          <t>宇斗リクツ（漫画） 八針来夏（原作） 輝竜司（キャラクター原案）</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>休載イラスト</t>
+          <t>第5話</t>
         </is>
       </c>
     </row>
@@ -23573,17 +24615,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+          <t>世界最高の暗殺者、異世界貴族に転生する</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+          <t>月夜涙(原作) 皇ハマオ(漫画) れい亜(キャラクター原案)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+          <t>第38話-2</t>
         </is>
       </c>
     </row>
@@ -23593,17 +24635,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>おんなのこのけんをてにいれた</t>
+          <t>ガチャを回して仲間を増やす 最強の美少女軍団を作り上げろ</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>福岡太朗(著者)</t>
+          <t>漫画：晴野しゅー 原作：ちんくるり キャラクター原案：イセ川ヤスタカ</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>15本目</t>
+          <t>第71話後半</t>
         </is>
       </c>
     </row>
@@ -23613,17 +24655,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>アイドル辞めるけど結婚してくれますか!?</t>
+          <t>大学入学時から噂されていた美少女三姉妹、生き別れていた義妹だった。</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>三吉汐美(著者)</t>
+          <t>こすずめ(著者) 夏乃実(原作) ポメ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第16話後半</t>
+          <t>第9話①</t>
         </is>
       </c>
     </row>
@@ -23633,17 +24675,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>リビルドワールド</t>
+          <t>ポーション頼みで生き延びます！ 続</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+          <t>原作：FUNA 漫画：園心ふつう キャラクター原案：すきま</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第71話②</t>
+          <t>第64話　長いお別れ Ⅲ</t>
         </is>
       </c>
     </row>
@@ -23653,17 +24695,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>「才能の器」で目指す迷宮最深部 スキル横伸ばしのはずが、万能チートだった!</t>
+          <t>宇崎ちゃんは遊びたい！</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>漫画：かくばやしつよし 原作：とんび キャラクター原案： りりんら</t>
+          <t>丈(著者)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第39話</t>
+          <t>第125話</t>
         </is>
       </c>
     </row>
@@ -23673,17 +24715,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ダメ人間の愛しかた</t>
+          <t>ゴリラ女子高生</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>岩葉(著者)</t>
+          <t>大友しゅうま(著者)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第18話後編　ダメ人間とお姉ちゃんと彼女</t>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
@@ -23693,17 +24735,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>異世界迷宮のオーパーツ</t>
+          <t>王子様の友達</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>三狛ハル(著者)</t>
+          <t>すけろく(著者)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第2話-②：立派な棒と革と玉</t>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
@@ -23713,17 +24755,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>理想の彼女</t>
+          <t>ラブコメと怪獣退治の不文律</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>もりまりも(著者)</t>
+          <t>御池慧（漫画） 上代務（原作） TMSLab（原作）</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>番外編4</t>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
@@ -23733,17 +24775,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>魔都精兵のスレイブ</t>
+          <t>ロメリア戦記～伯爵令嬢、魔王を倒した後も人類やばそうだから軍隊組織する～</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>原作:タカヒロ　漫画:竹村洋平</t>
+          <t>漫画：上戸 亮 原作：有山リョウ(小学館「ガガガブックス」刊) キャラクター原案：コダマ</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第157話　神域へ</t>
+          <t>第13話「助けてくれる人々」③</t>
         </is>
       </c>
     </row>
@@ -23753,17 +24795,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>追放された付与魔法使いの成り上がり ～勇者パーティを陰から支えていたと知らなかったので戻って来い？【剣聖】と【賢者】の美少女たちに囲まれて幸せなので戻りません～</t>
+          <t>姫様“拷問”の時間です</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>原作：蒼月浩二 漫画：伊香透 キャラクター原案：nima</t>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第23話</t>
+          <t>拷問145</t>
         </is>
       </c>
     </row>
@@ -23773,17 +24815,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>宮廷鍛冶師の幸せな日常 ～ブラックな職場を追放されたが、隣国で公爵令嬢に溺愛されながらホワイトな生活送ります～</t>
+          <t>無慈悲な悪役貴族に転生した僕は掌握魔法を駆使して魔法世界の頂点に立つ 〜ヒロインなんていないと諦めていたら向こうから勝手に寄ってきました〜</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>上林眞(著者) 木嶋隆太(原作) a20(キャラクター原案)</t>
+          <t>坂井オイ(漫画) びゃくし(原作) ファルまろ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第2話-②</t>
+          <t>コミックス第1巻発売告知</t>
         </is>
       </c>
     </row>
@@ -23793,17 +24835,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>半人前の恋人</t>
+          <t>アレクサンダー英雄戦記～最強の土魔術士～</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>川田大智</t>
+          <t>マツオカヨシノリ るれくちぇ なんじゃもんじゃ</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第48話</t>
+          <t>第11話（前編）</t>
         </is>
       </c>
     </row>
@@ -23813,17 +24855,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>無敵商人の異世界成り上がり物語 ～現代の製品を自在に取り寄せるスキルがあるので異世界では楽勝です～</t>
+          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>隆原ヒロタ(漫画) 青山有(原作) ぷきゅのすけ(キャラクターデザイン)</t>
+          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第35話①</t>
+          <t>第4話-2：師匠と弟子の新生活</t>
         </is>
       </c>
     </row>
@@ -23833,17 +24875,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>貴方は猫（わたし）の下僕です ～ねことげぼくのヒミツなカンケイ～</t>
+          <t>特殊性癖教室へようこそ</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>大田優一(著者)</t>
+          <t>紫苑寺七瀬(原作) 能呂やすとき(漫画) 魔太郎(キャラクター原案)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第14話前半</t>
+          <t>13限目-1</t>
         </is>
       </c>
     </row>
@@ -23853,17 +24895,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>リアリスト魔王による聖域なき異世界改革</t>
+          <t>Ｒｅ：ゼロから始める異世界生活 第四章 聖域と強欲の魔女</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>鈴木マナツ(漫画) 羽田遼亮(原作) ゆーげん(キャラクターデザイン) ひたきゆう(キャラクターデザイン)</t>
+          <t>花鶏ハルノ(作画) 相川有(構成) 長月達平(原作) 大塚真一郎(キャラクター原案)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第67幕②</t>
+          <t>第61話②　エリオール大森林の永久凍土</t>
         </is>
       </c>
     </row>
@@ -23873,17 +24915,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>俺堕ちスレイブヒーローコレクション</t>
+          <t>迷宮ブラックカンパニー</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ゆっ栗栖(著者)</t>
+          <t>安村洋平</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第11話前半</t>
+          <t>第50話　落花流水（中編）</t>
         </is>
       </c>
     </row>
@@ -23893,17 +24935,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>よくわからないけれど異世界に転生していたようです</t>
+          <t>異世界たぬき</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>内々けやき あし カオミン</t>
+          <t>小林安曇</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第136話 よくわからないけれどスカウトされたみたいです（１）</t>
+          <t>第2話①</t>
         </is>
       </c>
     </row>
@@ -23913,17 +24955,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>アラサーがVTuberになった話。</t>
+          <t>SSSランクダンジョンでナイフ一本手渡され追放された白魔導師 ユグドラシルの呪いにより弱点である魔力不足を克服し世界最強へと至る</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>犬威赤彦(漫画) とくめい(原作) カラスBTK(キャラクター原案)</t>
+          <t>上下瑞樹(漫画) カミトイチ(原作) 眠介(キャラクター原案)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第23話</t>
+          <t>第22話-2</t>
         </is>
       </c>
     </row>
@@ -23933,17 +24975,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>世界の終わりの世界録(アンコール)</t>
+          <t>ケイヤクシマイ</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>雨水龍(著者) 細音啓(原作) ふゆの春秋(キャラクター原案)</t>
+          <t>ヒジキ(著者)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第95話②</t>
+          <t>第26話後編</t>
         </is>
       </c>
     </row>
@@ -23953,17 +24995,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>転生してあらゆるモノに好かれながら異世界で好きな事をして生きて行く</t>
+          <t>追放されたギルド職員は、世界最強の召喚士@COMIC</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>都尾琉(漫画) 御峰。(原作)</t>
+          <t>原作：月島秀一 漫画：あづち涼 キャラクター原案：チワワ丸</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第26話③</t>
+          <t>第9話③「伏魔殿ダラスの惨劇」</t>
         </is>
       </c>
     </row>
@@ -23973,17 +25015,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>転生して成長チートを手に入れたら、最凶スキルもついたのですが!?</t>
+          <t>無能は不要と言われ『時計使い』の僕は職人ギルドから追い出されるも、ダンジョンの深部で真の力に覚醒する</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>やま ゆずもと 我美蘭</t>
+          <t>漫画：さらさみさ 小説： 桜霧琥珀 キャラ原案： 福きつね</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第10話</t>
+          <t>第19話後半</t>
         </is>
       </c>
     </row>
@@ -23993,17 +25035,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>くらいあの子としたいこと</t>
+          <t>余命一年の公爵子息は、旅をしたい</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>碇マナツ(著者)</t>
+          <t>漫画：Gisces 原作：サンボン</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第80話</t>
+          <t>第1話 ③</t>
         </is>
       </c>
     </row>
@@ -24013,17 +25055,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ダンジョンシーカーズ ～スマホアプリからはじまる現代ダンジョン制圧録～</t>
+          <t>安達としまむら</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>原作：七篠康晴 漫画：くりきまる キャラクター原案：冬野ユウキ</t>
+          <t>柚原もけ(漫画) 入間人間(原作) のん(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第6話</t>
+          <t>第48話「最初の旅の端１」②</t>
         </is>
       </c>
     </row>
@@ -24033,17 +25075,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ハーレムより平穏を！異世界で静かにニート姫させてくれ</t>
+          <t>ニャイト・オブ・ザ・リビングキャット</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>さかたはるき(原作) かわやばぐ(作画)</t>
+          <t>原作：ホークマン 作画：メカルーツ</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第13話後半</t>
+          <t>Chapter16　トランスフォーミャー～キャット覚醒～（前編）</t>
         </is>
       </c>
     </row>
@@ -24053,17 +25095,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>きみの願いが叶うまで</t>
+          <t>いとこのこ</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>浅月のりと(著者)</t>
+          <t>いぬちく(著者)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第3話-2</t>
+          <t>休載イラスト</t>
         </is>
       </c>
     </row>
@@ -24073,17 +25115,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>小林さんちのメイドラゴン</t>
+          <t>貰った三つの外れスキル、合わせたら最強でした</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>クール教信者</t>
+          <t>漫画：七谷八尋 原作：雪ノ狐 キャラクター原案：増田幹生</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第146話</t>
+          <t>第11話</t>
         </is>
       </c>
     </row>
@@ -24093,17 +25135,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>チュートリアルが始まる前に ボスキャラ達を破滅させない為に俺ができる幾つかの事</t>
+          <t>異世界で最強のスキルを生み出せたので、ひたすら無双することにしました。　～俺だけがスキルの数値を勝手に操作～</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>横山コウヂ(漫画) 髙橋炬燵(原作) カカオ・ランタン(キャラクターデザイン)</t>
+          <t>漫画：星トマジロウ 原作：ヒゲ抜き地蔵 キャラクター原案：山椒魚</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第13話③</t>
+          <t>第9話 ③</t>
         </is>
       </c>
     </row>
@@ -24113,17 +25155,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>理想のヒモ生活</t>
+          <t>ダメ人間の愛しかた</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+          <t>岩葉(著者)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第86話　その1</t>
+          <t>第18話後編　ダメ人間とお姉ちゃんと彼女</t>
         </is>
       </c>
     </row>
@@ -24133,17 +25175,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>陰々に鬼灯の咲く</t>
+          <t>異世界おじさん</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>絹江おばあちゃんの暴れパスタ祭り</t>
+          <t>殆ど死んでいる(著者)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第2話・土御門ハルネ</t>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
@@ -24153,17 +25195,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>愚かな天使は悪魔と踊る</t>
+          <t>千年英雄</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>アズマサワヨシ(著者)</t>
+          <t>原作/福島航平 作画/中村ゆきひろ</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第100話②</t>
+          <t>19話①</t>
         </is>
       </c>
     </row>
@@ -24173,17 +25215,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ゲーセン少女と異文化交流</t>
+          <t>クソ女に幸あれ</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>安原宏和(著者)</t>
+          <t>岸川瑞樹</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第126話</t>
+          <t>第60話</t>
         </is>
       </c>
     </row>
@@ -24193,17 +25235,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>小さめの魔法師匠と大きめの魔法少女。report：3</t>
+          <t>異世界創造のすゝめ～スマホアプリで惑星を創ってしまった俺は神となり世界を巡る～@COMIC</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>とりから</t>
+          <t>漫画：岩戸あきら 原作：たまごかけキャンディー キャラクター原案：かれい</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第37話の8</t>
+          <t>第11話 ②</t>
         </is>
       </c>
     </row>
@@ -24213,17 +25255,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>最強勇者パーティーは愛が知りたい</t>
+          <t>アイドル辞めるけど結婚してくれますか!?</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>山田肌襦袢</t>
+          <t>三吉汐美(著者)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第27話「エッチな祭りを始めたい」</t>
+          <t>第16話後半</t>
         </is>
       </c>
     </row>
@@ -24233,17 +25275,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>生徒会にも穴はある！</t>
+          <t>リビルドワールド</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>むちまろ</t>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第131話	ありす大ピンチ！（デジャブ編）</t>
+          <t>第71話②</t>
         </is>
       </c>
     </row>
@@ -24253,17 +25295,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>豚のレバーは加熱しろ</t>
+          <t>窓際編集とバカにされた俺が、双子ＪＫと同居することになった</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>みなみ(漫画) 逆井卓馬(原作) 遠坂あさぎ(キャラクターデザイン)</t>
+          <t>うさおとめ(著者) 茨木野(原作) トモゼロ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第42話①</t>
+          <t>第4話②</t>
         </is>
       </c>
     </row>
@@ -24273,17 +25315,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>私たちはカケちがっている</t>
+          <t>直径3cmの召喚陣&lt;リミットリング&gt;で「雑魚すら呼べない」と蔑まれた底辺召喚士が頂点に立つまで</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>みなもと悠</t>
+          <t>作画：まっつー 原作：空松蓮司</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第1話</t>
+          <t>第4話(2)</t>
         </is>
       </c>
     </row>
@@ -24293,17 +25335,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+          <t>異世界転生スラム街からの成り上がり～採取や猟をしてご飯食べてスローライフするんだ～</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+          <t>漫画：幾夜大黒堂 原作：滝川海老郎 キャラクター原案：沖史慈宴</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第3話 後編</t>
+          <t>第12話 ②</t>
         </is>
       </c>
     </row>
@@ -24313,17 +25355,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第74話 トワイライト</t>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
@@ -24333,17 +25375,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>王様ランキング200話～</t>
+          <t>転生前はドラゴンでした</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>十日草輔（とおかそうすけ）</t>
+          <t>甘井ヤドラキ</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第261話</t>
+          <t>第43話</t>
         </is>
       </c>
     </row>
@@ -24353,17 +25395,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>王都の外れの錬金術師 ～ハズレ職業だったので、のんびりお店経営します～</t>
+          <t>おんなのこのけんをてにいれた</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>あさなや(著者) yocco(原作) 純粋(キャラクター原案)</t>
+          <t>福岡太朗(著者)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>element.49</t>
+          <t>15本目</t>
         </is>
       </c>
     </row>
@@ -24373,17 +25415,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
+          <t>魔王様のバグトラップ迷宮制作記</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>神原絵理華(漫画) 一森一輝(原作)</t>
+          <t>あまがえる</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第18話①</t>
+          <t>第10話 偏愛バンシー②</t>
         </is>
       </c>
     </row>
@@ -24393,17 +25435,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>お前妹じゃなくて許嫁だったのかよ!?</t>
+          <t>理想の彼女</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>湯猫子(漫画) 未来人A(原作)</t>
+          <t>もりまりも(著者)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第28話</t>
+          <t>番外編4</t>
         </is>
       </c>
     </row>
@@ -24413,17 +25455,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+          <t>悪役貴族として必要なそれ</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>光永康則</t>
+          <t>まさこりん(原作) 夏野うみ(作画) 村カルキ(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第６６話『六花停止』③</t>
+          <t>第17話②</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-07-23
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -37,6 +37,7 @@
     <sheet name="2025-07-20" sheetId="29" state="visible" r:id="rId29"/>
     <sheet name="2025-07-21" sheetId="30" state="visible" r:id="rId30"/>
     <sheet name="2025-07-22" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="2025-07-23" sheetId="32" state="visible" r:id="rId32"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -24470,22 +24471,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第69話</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第５０話　雌雄を決する器用貧乏（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第２２食　ユクシーさんの覚悟、すごいのですわ！（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>KAKERU</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第66話「東アイギス」（後半）</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>回復術士のやり直し</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>月夜涙(原作) 羽賀ソウケン(漫画) しおこんぶ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第72話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>異世界のすみっこで快適ものづくり生活 ～女神さまのくれた工房はちょっとやりすぎ性能だった～</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>西山アラタ(漫画) 長田信織(原作) 東上文(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>EP.19②</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>肥満令嬢は細くなり、後は傾国の美女（物理）として生きるのみ@COMIC</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>宇斗リクツ（漫画） 八針来夏（原作） 輝竜司（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>世界最高の暗殺者、異世界貴族に転生する</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>月夜涙(原作) 皇ハマオ(漫画) れい亜(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第38話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>ガチャを回して仲間を増やす 最強の美少女軍団を作り上げろ</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>漫画：晴野しゅー 原作：ちんくるり キャラクター原案：イセ川ヤスタカ</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第71話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>大学入学時から噂されていた美少女三姉妹、生き別れていた義妹だった。</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>こすずめ(著者) 夏乃実(原作) ポメ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第9話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>ポーション頼みで生き延びます！ 続</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>原作：FUNA 漫画：園心ふつう キャラクター原案：すきま</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第64話　長いお別れ Ⅲ</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>宇崎ちゃんは遊びたい！</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>丈(著者)</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第125話</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>ゴリラ女子高生</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>大友しゅうま(著者)</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>王子様の友達</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>すけろく(著者)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>ラブコメと怪獣退治の不文律</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>御池慧（漫画） 上代務（原作） TMSLab（原作）</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>ロメリア戦記～伯爵令嬢、魔王を倒した後も人類やばそうだから軍隊組織する～</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>漫画：上戸 亮 原作：有山リョウ(小学館「ガガガブックス」刊) キャラクター原案：コダマ</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第13話「助けてくれる人々」③</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>姫様“拷問”の時間です</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>拷問145</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>無慈悲な悪役貴族に転生した僕は掌握魔法を駆使して魔法世界の頂点に立つ 〜ヒロインなんていないと諦めていたら向こうから勝手に寄ってきました〜</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>坂井オイ(漫画) びゃくし(原作) ファルまろ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>コミックス第1巻発売告知</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>アレクサンダー英雄戦記～最強の土魔術士～</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>マツオカヨシノリ るれくちぇ なんじゃもんじゃ</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第11話（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第4話-2：師匠と弟子の新生活</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>特殊性癖教室へようこそ</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>紫苑寺七瀬(原作) 能呂やすとき(漫画) 魔太郎(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>13限目-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>Ｒｅ：ゼロから始める異世界生活 第四章 聖域と強欲の魔女</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>花鶏ハルノ(作画) 相川有(構成) 長月達平(原作) 大塚真一郎(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第61話②　エリオール大森林の永久凍土</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>迷宮ブラックカンパニー</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>安村洋平</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第50話　落花流水（中編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>異世界たぬき</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>小林安曇</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第2話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>SSSランクダンジョンでナイフ一本手渡され追放された白魔導師 ユグドラシルの呪いにより弱点である魔力不足を克服し世界最強へと至る</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>上下瑞樹(漫画) カミトイチ(原作) 眠介(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第22話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>ケイヤクシマイ</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>ヒジキ(著者)</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第26話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>追放されたギルド職員は、世界最強の召喚士@COMIC</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>原作：月島秀一 漫画：あづち涼 キャラクター原案：チワワ丸</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第9話③「伏魔殿ダラスの惨劇」</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>無能は不要と言われ『時計使い』の僕は職人ギルドから追い出されるも、ダンジョンの深部で真の力に覚醒する</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>漫画：さらさみさ 小説： 桜霧琥珀 キャラ原案： 福きつね</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第19話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>余命一年の公爵子息は、旅をしたい</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>漫画：Gisces 原作：サンボン</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第1話 ③</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>安達としまむら</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>柚原もけ(漫画) 入間人間(原作) のん(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第48話「最初の旅の端１」②</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>ニャイト・オブ・ザ・リビングキャット</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>原作：ホークマン 作画：メカルーツ</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>Chapter16　トランスフォーミャー～キャット覚醒～（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>いとこのこ</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>いぬちく(著者)</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>休載イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>貰った三つの外れスキル、合わせたら最強でした</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>漫画：七谷八尋 原作：雪ノ狐 キャラクター原案：増田幹生</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第11話</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>異世界で最強のスキルを生み出せたので、ひたすら無双することにしました。　～俺だけがスキルの数値を勝手に操作～</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>漫画：星トマジロウ 原作：ヒゲ抜き地蔵 キャラクター原案：山椒魚</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第9話 ③</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>ダメ人間の愛しかた</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>岩葉(著者)</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第18話後編　ダメ人間とお姉ちゃんと彼女</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>異世界おじさん</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>殆ど死んでいる(著者)</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>千年英雄</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>原作/福島航平 作画/中村ゆきひろ</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>19話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>クソ女に幸あれ</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>岸川瑞樹</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第60話</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>異世界創造のすゝめ～スマホアプリで惑星を創ってしまった俺は神となり世界を巡る～@COMIC</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>漫画：岩戸あきら 原作：たまごかけキャンディー キャラクター原案：かれい</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第11話 ②</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>アイドル辞めるけど結婚してくれますか!?</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>三吉汐美(著者)</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第16話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第71話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>窓際編集とバカにされた俺が、双子ＪＫと同居することになった</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>うさおとめ(著者) 茨木野(原作) トモゼロ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第4話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>直径3cmの召喚陣&lt;リミットリング&gt;で「雑魚すら呼べない」と蔑まれた底辺召喚士が頂点に立つまで</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>作画：まっつー 原作：空松蓮司</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第4話(2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>異世界転生スラム街からの成り上がり～採取や猟をしてご飯食べてスローライフするんだ～</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>漫画：幾夜大黒堂 原作：滝川海老郎 キャラクター原案：沖史慈宴</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第12話 ②</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>転生前はドラゴンでした</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>甘井ヤドラキ</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第43話</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>おんなのこのけんをてにいれた</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>福岡太朗(著者)</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>15本目</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>魔王様のバグトラップ迷宮制作記</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>あまがえる</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第10話 偏愛バンシー②</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>理想の彼女</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>もりまりも(著者)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>番外編4</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>悪役貴族として必要なそれ</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>まさこりん(原作) 夏野うみ(作画) 村カルキ(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第17話②</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
+          <t>光永康則</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第69話</t>
+          <t>第６６話『六花停止』④</t>
         </is>
       </c>
     </row>
@@ -24495,17 +25537,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+          <t>マツモトケンゴ</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第５０話　雌雄を決する器用貧乏（３）</t>
+          <t>第６１話　偽彼氏の戦いが始まった</t>
         </is>
       </c>
     </row>
@@ -24515,17 +25557,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+          <t>いとこのこ</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>島知宏 音速炒飯 有都あらゆる</t>
+          <t>いぬちく(著者)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第２２食　ユクシーさんの覚悟、すごいのですわ！（３）</t>
+          <t>距離が近すぎる爽ちゃんと一緒に行きたい場所募集～！！【コメント募集企画】</t>
         </is>
       </c>
     </row>
@@ -24535,17 +25577,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>KAKERU</t>
+          <t>戸賀 環 坂木持丸 riritto</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第66話「東アイギス」（後半）</t>
+          <t>第49話②　城のパーティーに参加してみた</t>
         </is>
       </c>
     </row>
@@ -24555,17 +25597,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>回復術士のやり直し</t>
+          <t>ラスボス討伐後に始める二周目冒険者ライフ はじまりの街でワケあり美少女たちがめちゃくちゃ懐いてきます</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>月夜涙(原作) 羽賀ソウケン(漫画) しおこんぶ(キャラクター原案)</t>
+          <t>鬼麻正明(漫画) 朱月十話(原作) ファルまろ(キャラ原案)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第72話-1</t>
+          <t>第4話-2</t>
         </is>
       </c>
     </row>
@@ -24575,17 +25617,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>異世界のすみっこで快適ものづくり生活 ～女神さまのくれた工房はちょっとやりすぎ性能だった～</t>
+          <t>最果てのパラディン</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>西山アラタ(漫画) 長田信織(原作) 東上文(キャラクター原案)</t>
+          <t>奥橋睦（漫画） 柳野かなた（原作） 輪くすさが（キャラクター原案）</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>EP.19②</t>
+          <t>第66話　祝宴</t>
         </is>
       </c>
     </row>
@@ -24595,17 +25637,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>肥満令嬢は細くなり、後は傾国の美女（物理）として生きるのみ@COMIC</t>
+          <t>塔の管理をしてみよう</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>宇斗リクツ（漫画） 八針来夏（原作） 輝竜司（キャラクター原案）</t>
+          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第5話</t>
+          <t>第91話前編</t>
         </is>
       </c>
     </row>
@@ -24615,17 +25657,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>世界最高の暗殺者、異世界貴族に転生する</t>
+          <t>絶対死なないステラ姫</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>月夜涙(原作) 皇ハマオ(漫画) れい亜(キャラクター原案)</t>
+          <t>光永康則 大高稲</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第38話-2</t>
+          <t>第１４話　絶対旅立たない（２）</t>
         </is>
       </c>
     </row>
@@ -24635,17 +25677,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ガチャを回して仲間を増やす 最強の美少女軍団を作り上げろ</t>
+          <t>ひとりぼっちの異世界攻略</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>漫画：晴野しゅー 原作：ちんくるり キャラクター原案：イセ川ヤスタカ</t>
+          <t>びび（漫画） 五示正司（原作）</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第71話後半</t>
+          <t>第228話　弱肉強食</t>
         </is>
       </c>
     </row>
@@ -24655,17 +25697,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>大学入学時から噂されていた美少女三姉妹、生き別れていた義妹だった。</t>
+          <t>Sランク冒険者である俺の娘たちは重度のファザコンでした</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>こすずめ(著者) 夏乃実(原作) ポメ(キャラクター原案)</t>
+          <t>しゅにち（漫画） 友橋かめつ（原作） 希望つばめ（原作イラスト）</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第9話①</t>
+          <t>第46話　敵か、味方か</t>
         </is>
       </c>
     </row>
@@ -24675,17 +25717,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ポーション頼みで生き延びます！ 続</t>
+          <t>煽り系ゲーム配信者（20歳）、配信の切り忘れによりいい人バレする。</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>原作：FUNA 漫画：園心ふつう キャラクター原案：すきま</t>
+          <t>流嘉（漫画） 夏乃実（原作） 麦うさぎ（キャラクター原案）</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第64話　長いお別れ Ⅲ</t>
+          <t>第4話　サブ垢（後編）</t>
         </is>
       </c>
     </row>
@@ -24695,17 +25737,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>宇崎ちゃんは遊びたい！</t>
+          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>丈(著者)</t>
+          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第125話</t>
+          <t>第69話</t>
         </is>
       </c>
     </row>
@@ -24715,17 +25757,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ゴリラ女子高生</t>
+          <t>江戸前エルフ</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>大友しゅうま(著者)</t>
+          <t>樋口彰彦</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+          <t>#115</t>
         </is>
       </c>
     </row>
@@ -24735,17 +25777,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>王子様の友達</t>
+          <t>ある日、惰眠を貪っていたら一族から追放されて森に捨てられました そのまま寝てたら周りが勝手に魔物の国を作ってたけど、私は気にせず今日も眠ります　コミック版</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>すけろく(著者)</t>
+          <t>漫画/伊草さゆ 原作/白波ハクア キャラクター原案/まさよ</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+          <t>chapter52【27話②】</t>
         </is>
       </c>
     </row>
@@ -24755,17 +25797,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ラブコメと怪獣退治の不文律</t>
+          <t>履いてください、鷹峰さん</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>御池慧（漫画） 上代務（原作） TMSLab（原作）</t>
+          <t>柊裕一</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+          <t>第64話 当人同士で、どうぞ。(前編)</t>
         </is>
       </c>
     </row>
@@ -24775,17 +25817,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ロメリア戦記～伯爵令嬢、魔王を倒した後も人類やばそうだから軍隊組織する～</t>
+          <t>聖女に嘘は通じない</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>漫画：上戸 亮 原作：有山リョウ(小学館「ガガガブックス」刊) キャラクター原案：コダマ</t>
+          <t>日向 夏 浅見よう しんいし智歩</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第13話「助けてくれる人々」③</t>
+          <t>第25話②　あと二日で</t>
         </is>
       </c>
     </row>
@@ -24795,17 +25837,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>姫様“拷問”の時間です</t>
+          <t>ジャヒー様はくじけない！</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+          <t>昆布わかめ</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>拷問145</t>
+          <t>復興計画その99 ジャヒー様と大切なあの日</t>
         </is>
       </c>
     </row>
@@ -24815,17 +25857,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>無慈悲な悪役貴族に転生した僕は掌握魔法を駆使して魔法世界の頂点に立つ 〜ヒロインなんていないと諦めていたら向こうから勝手に寄ってきました〜</t>
+          <t>序盤で死ぬ最強のサブキャラに転生したので、ゲーム知識で無双する</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>坂井オイ(漫画) びゃくし(原作) ファルまろ(キャラクター原案)</t>
+          <t>作画：マエD 原作：新人</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>コミックス第1巻発売告知</t>
+          <t>第5話(1)</t>
         </is>
       </c>
     </row>
@@ -24835,17 +25877,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>アレクサンダー英雄戦記～最強の土魔術士～</t>
+          <t>ダウナー系お姉さんに毎日カスの嘘を流し込まれる話</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>マツオカヨシノリ るれくちぇ なんじゃもんじゃ</t>
+          <t>生倉のゑる(著者) はるばーど屋(原作者)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第11話（前編）</t>
+          <t>第11話</t>
         </is>
       </c>
     </row>
@@ -24855,17 +25897,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
+          <t>ゴリラ女子高生</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
+          <t>大友しゅうま(著者)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第4話-2：師匠と弟子の新生活</t>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
@@ -24875,17 +25917,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>特殊性癖教室へようこそ</t>
+          <t>ラブコメと怪獣退治の不文律</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>紫苑寺七瀬(原作) 能呂やすとき(漫画) 魔太郎(キャラクター原案)</t>
+          <t>御池慧（漫画） 上代務（原作） TMSLab（原作）</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>13限目-1</t>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
@@ -24895,17 +25937,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Ｒｅ：ゼロから始める異世界生活 第四章 聖域と強欲の魔女</t>
+          <t>王子様の友達</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>花鶏ハルノ(作画) 相川有(構成) 長月達平(原作) 大塚真一郎(キャラクター原案)</t>
+          <t>すけろく(著者)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第61話②　エリオール大森林の永久凍土</t>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
@@ -24915,17 +25957,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>迷宮ブラックカンパニー</t>
+          <t>ゲーム　オブ　ファミリア-家族戦記-</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>安村洋平</t>
+          <t>Ｄ．Ｐ(作画) 山口ミコト(原作)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第50話　落花流水（中編）</t>
+          <t>第73話④</t>
         </is>
       </c>
     </row>
@@ -24935,17 +25977,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>異世界たぬき</t>
+          <t>傭兵団の料理番</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>小林安曇</t>
+          <t>梅木泰祐(漫画) 川井昂(原作) 四季童子(キャラクター原案)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第2話①</t>
+          <t>第9話-2</t>
         </is>
       </c>
     </row>
@@ -24955,17 +25997,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>SSSランクダンジョンでナイフ一本手渡され追放された白魔導師 ユグドラシルの呪いにより弱点である魔力不足を克服し世界最強へと至る</t>
+          <t>みだりに憑かせてはなりません</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>上下瑞樹(漫画) カミトイチ(原作) 眠介(キャラクター原案)</t>
+          <t>栗田あぐり(著者)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第22話-2</t>
+          <t>第8話②</t>
         </is>
       </c>
     </row>
@@ -24975,17 +26017,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ケイヤクシマイ</t>
+          <t>宇崎ちゃんは遊びたい！</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>ヒジキ(著者)</t>
+          <t>丈(著者)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第26話後編</t>
+          <t>第125話</t>
         </is>
       </c>
     </row>
@@ -24995,17 +26037,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>追放されたギルド職員は、世界最強の召喚士@COMIC</t>
+          <t>高森くんを黙らせたいっ!!</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>原作：月島秀一 漫画：あづち涼 キャラクター原案：チワワ丸</t>
+          <t>春乃カミハル</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第9話③「伏魔殿ダラスの惨劇」</t>
+          <t>最終話</t>
         </is>
       </c>
     </row>
@@ -25015,17 +26057,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>無能は不要と言われ『時計使い』の僕は職人ギルドから追い出されるも、ダンジョンの深部で真の力に覚醒する</t>
+          <t>勇者パーティを追放された【スキルサポーター】、仲間のスキルを解放して最強に成り上がる</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>漫画：さらさみさ 小説： 桜霧琥珀 キャラ原案： 福きつね</t>
+          <t>作画：なかお 原作：前田氏</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第19話後半</t>
+          <t>第6話(1)</t>
         </is>
       </c>
     </row>
@@ -25035,17 +26077,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>余命一年の公爵子息は、旅をしたい</t>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>漫画：Gisces 原作：サンボン</t>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第1話 ③</t>
+          <t>第５０話　雌雄を決する器用貧乏（３）</t>
         </is>
       </c>
     </row>
@@ -25055,17 +26097,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>安達としまむら</t>
+          <t>米原くんはつよつよギャルから離れられない</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>柚原もけ(漫画) 入間人間(原作) のん(キャラクターデザイン)</t>
+          <t>川村拓(著者)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第48話「最初の旅の端１」②</t>
+          <t>第15話</t>
         </is>
       </c>
     </row>
@@ -25075,17 +26117,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ニャイト・オブ・ザ・リビングキャット</t>
+          <t>悪役一家の奥方、死に戻りして心を入れ替える。</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>原作：ホークマン 作画：メカルーツ</t>
+          <t>鏡(漫画) 丘野優(原作) TEDDY(キャラクター原案)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Chapter16　トランスフォーミャー～キャット覚醒～（前編）</t>
+          <t>第32話①</t>
         </is>
       </c>
     </row>
@@ -25095,17 +26137,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>いとこのこ</t>
+          <t>ラーメン大好き小泉さん</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>いぬちく(著者)</t>
+          <t>鳴見なる</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>休載イラスト</t>
+          <t>17杯目 家系</t>
         </is>
       </c>
     </row>
@@ -25115,17 +26157,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>貰った三つの外れスキル、合わせたら最強でした</t>
+          <t>最強の少年聖騎士、転生者を狩る</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>漫画：七谷八尋 原作：雪ノ狐 キャラクター原案：増田幹生</t>
+          <t>作画：御塩 原作：宇奈木ユラ</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第11話</t>
+          <t>第6話(1)</t>
         </is>
       </c>
     </row>
@@ -25135,17 +26177,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>異世界で最強のスキルを生み出せたので、ひたすら無双することにしました。　～俺だけがスキルの数値を勝手に操作～</t>
+          <t>数分後の未来が分かるようになったけど、女心は分からない。</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>漫画：星トマジロウ 原作：ヒゲ抜き地蔵 キャラクター原案：山椒魚</t>
+          <t>You2(漫画) mty(原作)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第9話 ③</t>
+          <t>第10話-2</t>
         </is>
       </c>
     </row>
@@ -25155,17 +26197,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>ダメ人間の愛しかた</t>
+          <t>オークの酒杯に祝福を</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>岩葉(著者)</t>
+          <t>かなどめはじめ</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第18話後編　ダメ人間とお姉ちゃんと彼女</t>
+          <t>第44話　冥土黒子</t>
         </is>
       </c>
     </row>
@@ -25175,17 +26217,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>異世界おじさん</t>
+          <t>初歩魔法しか使わない謎の老魔法使いが旅をする</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>殆ど死んでいる(著者)</t>
+          <t>山代カゲツ(漫画) やまだのぼる(原作) にじまあるく(キャラクター原案)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+          <t>第5話①</t>
         </is>
       </c>
     </row>
@@ -25195,17 +26237,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>千年英雄</t>
+          <t>8歳から始める魔法学</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>原作/福島航平 作画/中村ゆきひろ</t>
+          <t>ゆうなぎ（漫画） 上野夕陽（原作） 乃希（キャラクター原案）</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>19話①</t>
+          <t>第18話　意思交錯（前編）</t>
         </is>
       </c>
     </row>
@@ -25215,17 +26257,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>クソ女に幸あれ</t>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>岸川瑞樹</t>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第60話</t>
+          <t>第２２食　ユクシーさんの覚悟、すごいのですわ！（３）</t>
         </is>
       </c>
     </row>
@@ -25235,17 +26277,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>異世界創造のすゝめ～スマホアプリで惑星を創ってしまった俺は神となり世界を巡る～@COMIC</t>
+          <t>ちゃんと吸えない吸血鬼ちゃん</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>漫画：岩戸あきら 原作：たまごかけキャンディー キャラクター原案：かれい</t>
+          <t>二式恭介(著者)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第11話 ②</t>
+          <t>第101話：吸血鬼ちゃんのおまもり⑤</t>
         </is>
       </c>
     </row>
@@ -25255,17 +26297,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>アイドル辞めるけど結婚してくれますか!?</t>
+          <t>宮廷魔導師、追放される　～無能だと追い出された最巧の魔導師は、部下を引き連れて冒険者クランを始めるようです～</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>三吉汐美(著者)</t>
+          <t>きつね丸（漫画） しんこせい（原作） ろこ（キャラクター原案）</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第16話後半</t>
+          <t>第2話　憧れの人（後編）</t>
         </is>
       </c>
     </row>
@@ -25275,17 +26317,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>リビルドワールド</t>
+          <t>ギルドを追放された回復術士、実は魔力無限だったので規格外の回復魔法で伝説となる</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+          <t>漫画：坂下コウ 原作：霞杏檎</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第71話②</t>
+          <t>第4話(1)</t>
         </is>
       </c>
     </row>
@@ -25295,17 +26337,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>窓際編集とバカにされた俺が、双子ＪＫと同居することになった</t>
+          <t>二度追放された冒険者、激レアスキル駆使して美少女軍団を育成中！　コミック版</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>うさおとめ(著者) 茨木野(原作) トモゼロ(キャラクター原案)</t>
+          <t>漫画/青木千尋 原作/南野雪花</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第4話②</t>
+          <t>chapter67【34話②】</t>
         </is>
       </c>
     </row>
@@ -25315,17 +26357,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>直径3cmの召喚陣&lt;リミットリング&gt;で「雑魚すら呼べない」と蔑まれた底辺召喚士が頂点に立つまで</t>
+          <t>転生したら没落貴族だったので、【呪言】を極めて家族を救います</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>作画：まっつー 原作：空松蓮司</t>
+          <t>作画：アマセケイ 原作：メソポ・たみあ</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第4話(2)</t>
+          <t>第6話(1)</t>
         </is>
       </c>
     </row>
@@ -25335,17 +26377,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>異世界転生スラム街からの成り上がり～採取や猟をしてご飯食べてスローライフするんだ～</t>
+          <t>神猫ミーちゃんと猫用品召喚師の異世界奮闘記 ～目指すは、もふもふスローライフ！～</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>漫画：幾夜大黒堂 原作：滝川海老郎 キャラクター原案：沖史慈宴</t>
+          <t>にゃんたろう(原作) ねこのゆーま(作画) 岩崎美奈子(キャラクター原案)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第12話 ②</t>
+          <t>第4話①</t>
         </is>
       </c>
     </row>
@@ -25355,17 +26397,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+          <t>フシノカミ ～辺境から始める文明再生記～</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+          <t>黒杞よるの（漫画） 雨川水海（原作） 大熊まい（キャラクター原案）</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+          <t>第39話　蘇る歴史（前編）</t>
         </is>
       </c>
     </row>
@@ -25375,17 +26417,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>転生前はドラゴンでした</t>
+          <t>ダンジョン・バスターズ　～中年男ですが庭にダンジョンが出現したので世界を救います～</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>甘井ヤドラキ</t>
+          <t>蒼和 伸（漫画） 篠崎冬馬（原作） 千里GAN（キャラクター原案）</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第43話</t>
+          <t>第32話　始動へ</t>
         </is>
       </c>
     </row>
@@ -25395,17 +26437,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>おんなのこのけんをてにいれた</t>
+          <t>回復術士のやり直し</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>福岡太朗(著者)</t>
+          <t>月夜涙(原作) 羽賀ソウケン(漫画) しおこんぶ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>15本目</t>
+          <t>第72話-1</t>
         </is>
       </c>
     </row>
@@ -25415,17 +26457,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>魔王様のバグトラップ迷宮制作記</t>
+          <t>最凶貴族は死亡フラグを覆す</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>あまがえる</t>
+          <t>作画：sudekuma 原作：塚上</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第10話 偏愛バンシー②</t>
+          <t>第6話(1)</t>
         </is>
       </c>
     </row>
@@ -25435,17 +26477,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>理想の彼女</t>
+          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>もりまりも(著者)</t>
+          <t>KAKERU</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>番外編4</t>
+          <t>第66話「東アイギス」（後半）</t>
         </is>
       </c>
     </row>
@@ -25455,17 +26497,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>悪役貴族として必要なそれ</t>
+          <t>傷口と包帯</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>まさこりん(原作) 夏野うみ(作画) 村カルキ(キャラクターデザイン)</t>
+          <t>七井海星</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第17話②</t>
+          <t>第15話　新章開幕！　考える切谷</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-07-24
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -38,6 +38,7 @@
     <sheet name="2025-07-21" sheetId="30" state="visible" r:id="rId30"/>
     <sheet name="2025-07-22" sheetId="31" state="visible" r:id="rId31"/>
     <sheet name="2025-07-23" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="2025-07-24" sheetId="33" state="visible" r:id="rId33"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -25512,22 +25513,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第６６話『六花停止』④</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>マツモトケンゴ</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第６１話　偽彼氏の戦いが始まった</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>いとこのこ</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>いぬちく(著者)</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>距離が近すぎる爽ちゃんと一緒に行きたい場所募集～！！【コメント募集企画】</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>戸賀 環 坂木持丸 riritto</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第49話②　城のパーティーに参加してみた</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>ラスボス討伐後に始める二周目冒険者ライフ はじまりの街でワケあり美少女たちがめちゃくちゃ懐いてきます</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>鬼麻正明(漫画) 朱月十話(原作) ファルまろ(キャラ原案)</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第4話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>最果てのパラディン</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>奥橋睦（漫画） 柳野かなた（原作） 輪くすさが（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第66話　祝宴</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>塔の管理をしてみよう</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第91話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>絶対死なないステラ姫</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>光永康則 大高稲</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第１４話　絶対旅立たない（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>ひとりぼっちの異世界攻略</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>びび（漫画） 五示正司（原作）</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第228話　弱肉強食</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>Sランク冒険者である俺の娘たちは重度のファザコンでした</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>しゅにち（漫画） 友橋かめつ（原作） 希望つばめ（原作イラスト）</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第46話　敵か、味方か</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>煽り系ゲーム配信者（20歳）、配信の切り忘れによりいい人バレする。</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>流嘉（漫画） 夏乃実（原作） 麦うさぎ（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第4話　サブ垢（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第69話</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>江戸前エルフ</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>樋口彰彦</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>#115</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>ある日、惰眠を貪っていたら一族から追放されて森に捨てられました そのまま寝てたら周りが勝手に魔物の国を作ってたけど、私は気にせず今日も眠ります　コミック版</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>漫画/伊草さゆ 原作/白波ハクア キャラクター原案/まさよ</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>chapter52【27話②】</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>履いてください、鷹峰さん</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>柊裕一</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第64話 当人同士で、どうぞ。(前編)</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>聖女に嘘は通じない</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>日向 夏 浅見よう しんいし智歩</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第25話②　あと二日で</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>ジャヒー様はくじけない！</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>昆布わかめ</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>復興計画その99 ジャヒー様と大切なあの日</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>序盤で死ぬ最強のサブキャラに転生したので、ゲーム知識で無双する</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>作画：マエD 原作：新人</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第5話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>ダウナー系お姉さんに毎日カスの嘘を流し込まれる話</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>生倉のゑる(著者) はるばーど屋(原作者)</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第11話</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>ゴリラ女子高生</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>大友しゅうま(著者)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>ラブコメと怪獣退治の不文律</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>御池慧（漫画） 上代務（原作） TMSLab（原作）</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>王子様の友達</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>すけろく(著者)</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>ゲーム　オブ　ファミリア-家族戦記-</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>Ｄ．Ｐ(作画) 山口ミコト(原作)</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第73話④</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>傭兵団の料理番</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>梅木泰祐(漫画) 川井昂(原作) 四季童子(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第9話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>みだりに憑かせてはなりません</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>栗田あぐり(著者)</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第8話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>宇崎ちゃんは遊びたい！</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>丈(著者)</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第125話</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>高森くんを黙らせたいっ!!</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>春乃カミハル</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>最終話</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追放された【スキルサポーター】、仲間のスキルを解放して最強に成り上がる</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>作画：なかお 原作：前田氏</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第6話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第５０話　雌雄を決する器用貧乏（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>米原くんはつよつよギャルから離れられない</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>川村拓(著者)</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第15話</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>悪役一家の奥方、死に戻りして心を入れ替える。</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>鏡(漫画) 丘野優(原作) TEDDY(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第32話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>ラーメン大好き小泉さん</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>鳴見なる</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>17杯目 家系</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>最強の少年聖騎士、転生者を狩る</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>作画：御塩 原作：宇奈木ユラ</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第6話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>数分後の未来が分かるようになったけど、女心は分からない。</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>You2(漫画) mty(原作)</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第10話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>オークの酒杯に祝福を</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>かなどめはじめ</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第44話　冥土黒子</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>初歩魔法しか使わない謎の老魔法使いが旅をする</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>山代カゲツ(漫画) やまだのぼる(原作) にじまあるく(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第5話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>8歳から始める魔法学</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>ゆうなぎ（漫画） 上野夕陽（原作） 乃希（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第18話　意思交錯（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第２２食　ユクシーさんの覚悟、すごいのですわ！（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>ちゃんと吸えない吸血鬼ちゃん</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>二式恭介(著者)</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第101話：吸血鬼ちゃんのおまもり⑤</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>宮廷魔導師、追放される　～無能だと追い出された最巧の魔導師は、部下を引き連れて冒険者クランを始めるようです～</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>きつね丸（漫画） しんこせい（原作） ろこ（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第2話　憧れの人（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>ギルドを追放された回復術士、実は魔力無限だったので規格外の回復魔法で伝説となる</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>漫画：坂下コウ 原作：霞杏檎</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第4話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>二度追放された冒険者、激レアスキル駆使して美少女軍団を育成中！　コミック版</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>漫画/青木千尋 原作/南野雪花</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>chapter67【34話②】</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>転生したら没落貴族だったので、【呪言】を極めて家族を救います</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>作画：アマセケイ 原作：メソポ・たみあ</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第6話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>神猫ミーちゃんと猫用品召喚師の異世界奮闘記 ～目指すは、もふもふスローライフ！～</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>にゃんたろう(原作) ねこのゆーま(作画) 岩崎美奈子(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第4話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>フシノカミ ～辺境から始める文明再生記～</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>黒杞よるの（漫画） 雨川水海（原作） 大熊まい（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第39話　蘇る歴史（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>ダンジョン・バスターズ　～中年男ですが庭にダンジョンが出現したので世界を救います～</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>蒼和 伸（漫画） 篠崎冬馬（原作） 千里GAN（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第32話　始動へ</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>回復術士のやり直し</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>月夜涙(原作) 羽賀ソウケン(漫画) しおこんぶ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第72話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>最凶貴族は死亡フラグを覆す</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>作画：sudekuma 原作：塚上</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第6話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>KAKERU</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第66話「東アイギス」（後半）</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>傷口と包帯</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>七井海星</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第15話　新章開幕！　考える切谷</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>光永康則</t>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第６６話『六花停止』④</t>
+          <t>第34話①</t>
         </is>
       </c>
     </row>
@@ -25537,17 +26579,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>マツモトケンゴ</t>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第６１話　偽彼氏の戦いが始まった</t>
+          <t>第9話-2</t>
         </is>
       </c>
     </row>
@@ -25557,17 +26599,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>いとこのこ</t>
+          <t>実は俺、最強でした？</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>いぬちく(著者)</t>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>距離が近すぎる爽ちゃんと一緒に行きたい場所募集～！！【コメント募集企画】</t>
+          <t>第121話　王都の危機を守れ!!・前編</t>
         </is>
       </c>
     </row>
@@ -25577,17 +26619,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>戸賀 環 坂木持丸 riritto</t>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第49話②　城のパーティーに参加してみた</t>
+          <t>第32話 独身貴族は森で写真を撮る（2）</t>
         </is>
       </c>
     </row>
@@ -25597,17 +26639,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ラスボス討伐後に始める二周目冒険者ライフ はじまりの街でワケあり美少女たちがめちゃくちゃ懐いてきます</t>
+          <t>隣の席のヤンキー清水さんが髪を黒く染めてきた</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>鬼麻正明(漫画) 朱月十話(原作) ファルまろ(キャラ原案)</t>
+          <t>底花(原作) 真田若楓(漫画) ハム(キャラクター原案)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第4話-2</t>
+          <t>第10話-2</t>
         </is>
       </c>
     </row>
@@ -25617,17 +26659,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>最果てのパラディン</t>
+          <t>ダンジョン・シェルパ　迷宮道先案内人</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>奥橋睦（漫画） 柳野かなた（原作） 輪くすさが（キャラクター原案）</t>
+          <t>原作/加茂セイ 漫画/刀坂アキラ</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第66話　祝宴</t>
+          <t>潜行：60(前編)</t>
         </is>
       </c>
     </row>
@@ -25637,17 +26679,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>塔の管理をしてみよう</t>
+          <t>スキル【万物支配】に目覚めたおっさんは、ダンジョンで生計を立てることにしました～無職から始める支配者無双～</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
+          <t>岸本和葉 原田 臙 シミズヒロノリ 吉武</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第91話前編</t>
+          <t>第4話　穴熊商店(後編)</t>
         </is>
       </c>
     </row>
@@ -25657,17 +26699,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>絶対死なないステラ姫</t>
+          <t>すだちの魔王城</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>光永康則 大高稲</t>
+          <t>森下真</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第１４話　絶対旅立たない（２）</t>
+          <t>第44話　渡る鴉の縁結び（後編）</t>
         </is>
       </c>
     </row>
@@ -25677,17 +26719,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ひとりぼっちの異世界攻略</t>
+          <t>オタクに優しいギャルはいない!?</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>びび（漫画） 五示正司（原作）</t>
+          <t>のりしろちゃん 魚住さかな</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第228話　弱肉強食</t>
+          <t>【#149】心配ないさ</t>
         </is>
       </c>
     </row>
@@ -25697,17 +26739,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Sランク冒険者である俺の娘たちは重度のファザコンでした</t>
+          <t>生徒会役員共</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>しゅにち（漫画） 友橋かめつ（原作） 希望つばめ（原作イラスト）</t>
+          <t>氏家ト全</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第46話　敵か、味方か</t>
+          <t>#406</t>
         </is>
       </c>
     </row>
@@ -25717,17 +26759,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>煽り系ゲーム配信者（20歳）、配信の切り忘れによりいい人バレする。</t>
+          <t>姫騎士は蛮族の嫁</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>流嘉（漫画） 夏乃実（原作） 麦うさぎ（キャラクター原案）</t>
+          <t>コトバノリアキ</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第4話　サブ垢（後編）</t>
+          <t>第52話②	浮船は未見の故郷</t>
         </is>
       </c>
     </row>
@@ -25737,17 +26779,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
+          <t>29歳独身は異世界で自由に生きた……かった。</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
+          <t>オオハマイコ(漫画) リュート(原作) 桑島黎音(キャラクター原案)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第69話</t>
+          <t>第41話-1②</t>
         </is>
       </c>
     </row>
@@ -25757,17 +26799,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>江戸前エルフ</t>
+          <t>脇役に転生したはずが、いつの間にか伝説の錬金術師になってた～仲間たちが英雄でも俺は支援職なんだが～</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>樋口彰彦</t>
+          <t>神無月みり 相野 仁</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>#115</t>
+          <t>第２６話　脇役、目論見を見破る（２）</t>
         </is>
       </c>
     </row>
@@ -25777,17 +26819,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ある日、惰眠を貪っていたら一族から追放されて森に捨てられました そのまま寝てたら周りが勝手に魔物の国を作ってたけど、私は気にせず今日も眠ります　コミック版</t>
+          <t>カナン様はあくまでチョロい</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>漫画/伊草さゆ 原作/白波ハクア キャラクター原案/まさよ</t>
+          <t>nonco</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>chapter52【27話②】</t>
+          <t>第143話	ジャンヌのスマホデビュー</t>
         </is>
       </c>
     </row>
@@ -25797,17 +26839,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>履いてください、鷹峰さん</t>
+          <t>ポンコツ風紀委員とスカート丈が不適切なＪＫの話</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>柊裕一</t>
+          <t>横田卓馬</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第64話 当人同士で、どうぞ。(前編)</t>
+          <t>描き下ろし休載イラスト</t>
         </is>
       </c>
     </row>
@@ -25817,17 +26859,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>聖女に嘘は通じない</t>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>日向 夏 浅見よう しんいし智歩</t>
+          <t>光永康則</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第25話②　あと二日で</t>
+          <t>第６６話『六花停止』④</t>
         </is>
       </c>
     </row>
@@ -25837,17 +26879,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ジャヒー様はくじけない！</t>
+          <t>すべての人類を破壊する。それらは再生できない。</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>昆布わかめ</t>
+          <t>横田卓馬(漫画) 伊瀬勝良(原作)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>復興計画その99 ジャヒー様と大切なあの日</t>
+          <t>第66話その4</t>
         </is>
       </c>
     </row>
@@ -25857,17 +26899,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>序盤で死ぬ最強のサブキャラに転生したので、ゲーム知識で無双する</t>
+          <t>王子様の友達</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>作画：マエD 原作：新人</t>
+          <t>すけろく(著者)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第5話(1)</t>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
@@ -25877,17 +26919,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ダウナー系お姉さんに毎日カスの嘘を流し込まれる話</t>
+          <t>ゴリラ女子高生</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>生倉のゑる(著者) はるばーど屋(原作者)</t>
+          <t>大友しゅうま(著者)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第11話</t>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
@@ -25897,17 +26939,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>ゴリラ女子高生</t>
+          <t>ダメ人間の愛しかた</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>大友しゅうま(著者)</t>
+          <t>岩葉(著者)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+          <t>コミックス3巻告知記事</t>
         </is>
       </c>
     </row>
@@ -25937,17 +26979,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>王子様の友達</t>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>すけろく(著者)</t>
+          <t>マツモトケンゴ</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+          <t>第６１話　偽彼氏の戦いが始まった</t>
         </is>
       </c>
     </row>
@@ -25957,17 +26999,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ゲーム　オブ　ファミリア-家族戦記-</t>
+          <t>転生錬金少女のスローライフ</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Ｄ．Ｐ(作画) 山口ミコト(原作)</t>
+          <t>里町(漫画) 夜想庭園(原作) potg(キャラクター原案)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第73話④</t>
+          <t>第17話-1</t>
         </is>
       </c>
     </row>
@@ -25977,17 +27019,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>傭兵団の料理番</t>
+          <t>よわよわ先生</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>梅木泰祐(漫画) 川井昂(原作) 四季童子(キャラクター原案)</t>
+          <t>福地カミオ</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第9話-2</t>
+          <t>第108話	ミニミニのもみノート</t>
         </is>
       </c>
     </row>
@@ -25997,17 +27039,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>みだりに憑かせてはなりません</t>
+          <t>チート薬師のスローライフ ～異世界に作ろうドラッグストア～</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>栗田あぐり(著者)</t>
+          <t>ケンノジ 春乃えり</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第8話②</t>
+          <t>67本目　気持ちを形に[後半]</t>
         </is>
       </c>
     </row>
@@ -26017,17 +27059,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>宇崎ちゃんは遊びたい！</t>
+          <t>カット＆ペーストでこの世界を生きていく</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>丈(著者)</t>
+          <t>原作／咲夜(ツギクル) 漫画／加藤コウキ キャラクター原案／PiNe　乾和音　茶餅</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第125話</t>
+          <t>第119話　自由奔放</t>
         </is>
       </c>
     </row>
@@ -26037,17 +27079,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>高森くんを黙らせたいっ!!</t>
+          <t>いとこのこ</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>春乃カミハル</t>
+          <t>いぬちく(著者)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>最終話</t>
+          <t>距離が近すぎる爽ちゃんと一緒に行きたい場所募集～！！【コメント募集企画】</t>
         </is>
       </c>
     </row>
@@ -26057,17 +27099,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>勇者パーティを追放された【スキルサポーター】、仲間のスキルを解放して最強に成り上がる</t>
+          <t>ギルドを追放された回復術士、実は魔力無限だったので規格外の回復魔法で伝説となる</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>作画：なかお 原作：前田氏</t>
+          <t>漫画：坂下コウ 原作：霞杏檎</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第6話(1)</t>
+          <t>第4話(1)</t>
         </is>
       </c>
     </row>
@@ -26077,17 +27119,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+          <t>異世界チート魔術師</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+          <t>内田健（ヒーロー文庫／イマジカインフォス）(原作) 鈴羅木かりん(漫画) Ｎａｒｄａｃｋ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第５０話　雌雄を決する器用貧乏（３）</t>
+          <t>第92話-2</t>
         </is>
       </c>
     </row>
@@ -26097,17 +27139,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>米原くんはつよつよギャルから離れられない</t>
+          <t>百瀬アキラの初恋破綻中。</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>川村拓(著者)</t>
+          <t>晴川シンタ</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第15話</t>
+          <t>第32話 あの日の想いを追憶中。</t>
         </is>
       </c>
     </row>
@@ -26117,17 +27159,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>悪役一家の奥方、死に戻りして心を入れ替える。</t>
+          <t>勇者パーティーの荷物持ち</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>鏡(漫画) 丘野優(原作) TEDDY(キャラクター原案)</t>
+          <t>原作：河本ほむら／作画：八嶋諒</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第32話①</t>
+          <t>第24話 荷物持ちと勇者パーティーの魔法使い②</t>
         </is>
       </c>
     </row>
@@ -26137,17 +27179,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ラーメン大好き小泉さん</t>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>鳴見なる</t>
+          <t>戸賀 環 坂木持丸 riritto</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>17杯目 家系</t>
+          <t>第49話②　城のパーティーに参加してみた</t>
         </is>
       </c>
     </row>
@@ -26157,17 +27199,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>最強の少年聖騎士、転生者を狩る</t>
+          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>作画：御塩 原作：宇奈木ユラ</t>
+          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第6話(1)</t>
+          <t>第69話</t>
         </is>
       </c>
     </row>
@@ -26177,17 +27219,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>数分後の未来が分かるようになったけど、女心は分からない。</t>
+          <t>ラスボス討伐後に始める二周目冒険者ライフ はじまりの街でワケあり美少女たちがめちゃくちゃ懐いてきます</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>You2(漫画) mty(原作)</t>
+          <t>鬼麻正明(漫画) 朱月十話(原作) ファルまろ(キャラ原案)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第10話-2</t>
+          <t>第4話-2</t>
         </is>
       </c>
     </row>
@@ -26197,17 +27239,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>オークの酒杯に祝福を</t>
+          <t>ジェノヴァの弟子～10秒しか戦えない魔術師、のちの『魔王』を育てる～</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>かなどめはじめ</t>
+          <t>原作：妹尾尻尾 漫画：魚塚じゃこ キャラクター原案：赤嶺直樹</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第44話　冥土黒子</t>
+          <t>第22話</t>
         </is>
       </c>
     </row>
@@ -26217,17 +27259,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>初歩魔法しか使わない謎の老魔法使いが旅をする</t>
+          <t>シャドウ・アサシンズ・ワールド ～影は薄いけど、最強忍者やってます～</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>山代カゲツ(漫画) やまだのぼる(原作) にじまあるく(キャラクター原案)</t>
+          <t>空山トキ 五色安未 泉乃せん 伍長</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第5話①</t>
+          <t>第11話　少女と本当の自分２（1）</t>
         </is>
       </c>
     </row>
@@ -26237,17 +27279,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>8歳から始める魔法学</t>
+          <t>最果てのパラディン</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>ゆうなぎ（漫画） 上野夕陽（原作） 乃希（キャラクター原案）</t>
+          <t>奥橋睦（漫画） 柳野かなた（原作） 輪くすさが（キャラクター原案）</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第18話　意思交錯（前編）</t>
+          <t>第66話　祝宴</t>
         </is>
       </c>
     </row>
@@ -26257,17 +27299,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+          <t>宇崎ちゃんは遊びたい！</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>島知宏 音速炒飯 有都あらゆる</t>
+          <t>丈(著者)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第２２食　ユクシーさんの覚悟、すごいのですわ！（３）</t>
+          <t>第125話</t>
         </is>
       </c>
     </row>
@@ -26277,17 +27319,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>ちゃんと吸えない吸血鬼ちゃん</t>
+          <t>塔の管理をしてみよう</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>二式恭介(著者)</t>
+          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第101話：吸血鬼ちゃんのおまもり⑤</t>
+          <t>第91話前編</t>
         </is>
       </c>
     </row>
@@ -26297,17 +27339,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>宮廷魔導師、追放される　～無能だと追い出された最巧の魔導師は、部下を引き連れて冒険者クランを始めるようです～</t>
+          <t>絶対死なないステラ姫</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>きつね丸（漫画） しんこせい（原作） ろこ（キャラクター原案）</t>
+          <t>光永康則 大高稲</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第2話　憧れの人（後編）</t>
+          <t>第１４話　絶対旅立たない（２）</t>
         </is>
       </c>
     </row>
@@ -26317,17 +27359,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>ギルドを追放された回復術士、実は魔力無限だったので規格外の回復魔法で伝説となる</t>
+          <t>葉木莉さんは君だけの死神になりたい</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>漫画：坂下コウ 原作：霞杏檎</t>
+          <t>35まち</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第4話(1)</t>
+          <t>第６話　それは好きということでは？</t>
         </is>
       </c>
     </row>
@@ -26337,17 +27379,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>二度追放された冒険者、激レアスキル駆使して美少女軍団を育成中！　コミック版</t>
+          <t>人生逆転ダンジョン</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>漫画/青木千尋 原作/南野雪花</t>
+          <t>尾張 ニコ どすこい花丸様</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>chapter67【34話②】</t>
+          <t>第3-2話	穴は使いよう</t>
         </is>
       </c>
     </row>
@@ -26357,17 +27399,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>転生したら没落貴族だったので、【呪言】を極めて家族を救います</t>
+          <t>ひとりぼっちの異世界攻略</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>作画：アマセケイ 原作：メソポ・たみあ</t>
+          <t>びび（漫画） 五示正司（原作）</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第6話(1)</t>
+          <t>第228話　弱肉強食</t>
         </is>
       </c>
     </row>
@@ -26377,17 +27419,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>神猫ミーちゃんと猫用品召喚師の異世界奮闘記 ～目指すは、もふもふスローライフ！～</t>
+          <t>煽り系ゲーム配信者（20歳）、配信の切り忘れによりいい人バレする。</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>にゃんたろう(原作) ねこのゆーま(作画) 岩崎美奈子(キャラクター原案)</t>
+          <t>流嘉（漫画） 夏乃実（原作） 麦うさぎ（キャラクター原案）</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第4話①</t>
+          <t>第4話　サブ垢（後編）</t>
         </is>
       </c>
     </row>
@@ -26397,17 +27439,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>フシノカミ ～辺境から始める文明再生記～</t>
+          <t>ダウナー系お姉さんに毎日カスの嘘を流し込まれる話</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>黒杞よるの（漫画） 雨川水海（原作） 大熊まい（キャラクター原案）</t>
+          <t>生倉のゑる(著者) はるばーど屋(原作者)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第39話　蘇る歴史（前編）</t>
+          <t>第11話</t>
         </is>
       </c>
     </row>
@@ -26417,17 +27459,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>ダンジョン・バスターズ　～中年男ですが庭にダンジョンが出現したので世界を救います～</t>
+          <t>終焉の魔女と世界の旅</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>蒼和 伸（漫画） 篠崎冬馬（原作） 千里GAN（キャラクター原案）</t>
+          <t>片岡とんち</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第32話　始動へ</t>
+          <t>第13話②	終焉の魔女と魔王メリア</t>
         </is>
       </c>
     </row>
@@ -26437,17 +27479,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>回復術士のやり直し</t>
+          <t>Sランク冒険者である俺の娘たちは重度のファザコンでした</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>月夜涙(原作) 羽賀ソウケン(漫画) しおこんぶ(キャラクター原案)</t>
+          <t>しゅにち（漫画） 友橋かめつ（原作） 希望つばめ（原作イラスト）</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第72話-1</t>
+          <t>第46話　敵か、味方か</t>
         </is>
       </c>
     </row>
@@ -26457,17 +27499,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>最凶貴族は死亡フラグを覆す</t>
+          <t>履いてください、鷹峰さん</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>作画：sudekuma 原作：塚上</t>
+          <t>柊裕一</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第6話(1)</t>
+          <t>第64話 当人同士で、どうぞ。(前編)</t>
         </is>
       </c>
     </row>
@@ -26477,17 +27519,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
+          <t>アンゴルモア 元寇合戦記　【博多編】</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>KAKERU</t>
+          <t>たかぎ七彦(著者)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第66話「東アイギス」（後半）</t>
+          <t>第四十四話その六</t>
         </is>
       </c>
     </row>
@@ -26497,17 +27539,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>傷口と包帯</t>
+          <t>恋人以上友人未満</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>七井海星</t>
+          <t>yatoyato</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第15話　新章開幕！　考える切谷</t>
+          <t>第93話</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-07-25
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -39,6 +39,7 @@
     <sheet name="2025-07-22" sheetId="31" state="visible" r:id="rId31"/>
     <sheet name="2025-07-23" sheetId="32" state="visible" r:id="rId32"/>
     <sheet name="2025-07-24" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="2025-07-25" sheetId="34" state="visible" r:id="rId34"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -26554,22 +26555,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第34話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第9話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第121話　王都の危機を守れ!!・前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第32話 独身貴族は森で写真を撮る（2）</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>隣の席のヤンキー清水さんが髪を黒く染めてきた</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>底花(原作) 真田若楓(漫画) ハム(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第10話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>ダンジョン・シェルパ　迷宮道先案内人</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>原作/加茂セイ 漫画/刀坂アキラ</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>潜行：60(前編)</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>スキル【万物支配】に目覚めたおっさんは、ダンジョンで生計を立てることにしました～無職から始める支配者無双～</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>岸本和葉 原田 臙 シミズヒロノリ 吉武</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第4話　穴熊商店(後編)</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>すだちの魔王城</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>森下真</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第44話　渡る鴉の縁結び（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>オタクに優しいギャルはいない!?</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>のりしろちゃん 魚住さかな</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>【#149】心配ないさ</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>生徒会役員共</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>氏家ト全</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>#406</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>姫騎士は蛮族の嫁</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>コトバノリアキ</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第52話②	浮船は未見の故郷</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>29歳独身は異世界で自由に生きた……かった。</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>オオハマイコ(漫画) リュート(原作) 桑島黎音(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第41話-1②</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>脇役に転生したはずが、いつの間にか伝説の錬金術師になってた～仲間たちが英雄でも俺は支援職なんだが～</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>神無月みり 相野 仁</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第２６話　脇役、目論見を見破る（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>カナン様はあくまでチョロい</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>nonco</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第143話	ジャンヌのスマホデビュー</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>ポンコツ風紀委員とスカート丈が不適切なＪＫの話</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>横田卓馬</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>描き下ろし休載イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第６６話『六花停止』④</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>すべての人類を破壊する。それらは再生できない。</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>横田卓馬(漫画) 伊瀬勝良(原作)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第66話その4</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>王子様の友達</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>すけろく(著者)</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>ゴリラ女子高生</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>大友しゅうま(著者)</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>ダメ人間の愛しかた</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>岩葉(著者)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>コミックス3巻告知記事</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>ラブコメと怪獣退治の不文律</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>御池慧（漫画） 上代務（原作） TMSLab（原作）</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>マツモトケンゴ</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第６１話　偽彼氏の戦いが始まった</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>転生錬金少女のスローライフ</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>里町(漫画) 夜想庭園(原作) potg(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第17話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>よわよわ先生</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>福地カミオ</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第108話	ミニミニのもみノート</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>チート薬師のスローライフ ～異世界に作ろうドラッグストア～</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>ケンノジ 春乃えり</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>67本目　気持ちを形に[後半]</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>カット＆ペーストでこの世界を生きていく</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>原作／咲夜(ツギクル) 漫画／加藤コウキ キャラクター原案／PiNe　乾和音　茶餅</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第119話　自由奔放</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>いとこのこ</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>いぬちく(著者)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>距離が近すぎる爽ちゃんと一緒に行きたい場所募集～！！【コメント募集企画】</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>ギルドを追放された回復術士、実は魔力無限だったので規格外の回復魔法で伝説となる</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>漫画：坂下コウ 原作：霞杏檎</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第4話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>異世界チート魔術師</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>内田健（ヒーロー文庫／イマジカインフォス）(原作) 鈴羅木かりん(漫画) Ｎａｒｄａｃｋ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第92話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>百瀬アキラの初恋破綻中。</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>晴川シンタ</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第32話 あの日の想いを追憶中。</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティーの荷物持ち</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>原作：河本ほむら／作画：八嶋諒</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第24話 荷物持ちと勇者パーティーの魔法使い②</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>戸賀 環 坂木持丸 riritto</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第49話②　城のパーティーに参加してみた</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第69話</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>ラスボス討伐後に始める二周目冒険者ライフ はじまりの街でワケあり美少女たちがめちゃくちゃ懐いてきます</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>鬼麻正明(漫画) 朱月十話(原作) ファルまろ(キャラ原案)</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第4話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>ジェノヴァの弟子～10秒しか戦えない魔術師、のちの『魔王』を育てる～</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>原作：妹尾尻尾 漫画：魚塚じゃこ キャラクター原案：赤嶺直樹</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第22話</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>シャドウ・アサシンズ・ワールド ～影は薄いけど、最強忍者やってます～</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>空山トキ 五色安未 泉乃せん 伍長</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第11話　少女と本当の自分２（1）</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>最果てのパラディン</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>奥橋睦（漫画） 柳野かなた（原作） 輪くすさが（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第66話　祝宴</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>宇崎ちゃんは遊びたい！</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>丈(著者)</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第125話</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>塔の管理をしてみよう</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第91話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>絶対死なないステラ姫</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>光永康則 大高稲</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第１４話　絶対旅立たない（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>葉木莉さんは君だけの死神になりたい</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>35まち</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第６話　それは好きということでは？</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>人生逆転ダンジョン</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>尾張 ニコ どすこい花丸様</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第3-2話	穴は使いよう</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>ひとりぼっちの異世界攻略</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>びび（漫画） 五示正司（原作）</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第228話　弱肉強食</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>煽り系ゲーム配信者（20歳）、配信の切り忘れによりいい人バレする。</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>流嘉（漫画） 夏乃実（原作） 麦うさぎ（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第4話　サブ垢（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>ダウナー系お姉さんに毎日カスの嘘を流し込まれる話</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>生倉のゑる(著者) はるばーど屋(原作者)</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第11話</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>終焉の魔女と世界の旅</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>片岡とんち</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第13話②	終焉の魔女と魔王メリア</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>Sランク冒険者である俺の娘たちは重度のファザコンでした</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>しゅにち（漫画） 友橋かめつ（原作） 希望つばめ（原作イラスト）</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第46話　敵か、味方か</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>履いてください、鷹峰さん</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>柊裕一</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第64話 当人同士で、どうぞ。(前編)</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>アンゴルモア 元寇合戦記　【博多編】</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>たかぎ七彦(著者)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第四十四話その六</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>恋人以上友人未満</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>yatoyato</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第93話</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+          <t>ワンパンマン</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第34話①</t>
+          <t>206撃目</t>
         </is>
       </c>
     </row>
@@ -26579,17 +27621,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+          <t>ダークサモナーとデキている</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+          <t>車王(著者)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第9話-2</t>
+          <t>【コミックス第6巻発売記念】挟まるならどの衣装？コメント大募集！</t>
         </is>
       </c>
     </row>
@@ -26599,17 +27641,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>実は俺、最強でした？</t>
+          <t>最弱テイマーはゴミ拾いの旅を始めました。@COMIC</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>原作：澄守 彩 漫画：高橋 愛</t>
+          <t>漫画：蕗野 冬 原作：ほのぼのる500 キャラクター原案：なま</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第121話　王都の危機を守れ!!・前編</t>
+          <t>第26話</t>
         </is>
       </c>
     </row>
@@ -26619,17 +27661,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+          <t>魔王になったので、ダンジョン造って人外娘とほのぼのする</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+          <t>遠野ノオト(作画) 流優(原作) だぶ竜(キャラクター原案)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第32話 独身貴族は森で写真を撮る（2）</t>
+          <t>第82話後半</t>
         </is>
       </c>
     </row>
@@ -26639,17 +27681,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>隣の席のヤンキー清水さんが髪を黒く染めてきた</t>
+          <t>バーサス</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>底花(原作) 真田若楓(漫画) ハム(キャラクター原案)</t>
+          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第10話-2</t>
+          <t>第26話 惨事（2）</t>
         </is>
       </c>
     </row>
@@ -26659,17 +27701,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ダンジョン・シェルパ　迷宮道先案内人</t>
+          <t>魔石グルメ　魔物の力を食べたオレは最強！</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>原作/加茂セイ 漫画/刀坂アキラ</t>
+          <t>菅原健二(作画) 結城涼(原作) 成瀬ちさと(キャラクター原案)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>潜行：60(前編)</t>
+          <t>第67話前半</t>
         </is>
       </c>
     </row>
@@ -26679,17 +27721,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>スキル【万物支配】に目覚めたおっさんは、ダンジョンで生計を立てることにしました～無職から始める支配者無双～</t>
+          <t>ゲーム悪役貴族に転生した俺は、チート筋肉で無双する</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>岸本和葉 原田 臙 シミズヒロノリ 吉武</t>
+          <t>昼行燈（原作） しいたけ元帥（漫画）</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第4話　穴熊商店(後編)</t>
+          <t>第26話</t>
         </is>
       </c>
     </row>
@@ -26699,17 +27741,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>すだちの魔王城</t>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>森下真</t>
+          <t>空野進 sorani ファルまろ</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第44話　渡る鴉の縁結び（後編）</t>
+          <t>第10話　最弱貴族、部下を信じる（３）</t>
         </is>
       </c>
     </row>
@@ -26719,17 +27761,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>オタクに優しいギャルはいない!?</t>
+          <t>転生したらスライムだった件 異聞 ～魔国暮らしのトリニティ～</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>のりしろちゃん 魚住さかな</t>
+          <t>伏瀬 戸野タエ みっつばー</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>【#149】心配ないさ</t>
+          <t>第107話　開国祭開幕［その２］</t>
         </is>
       </c>
     </row>
@@ -26739,17 +27781,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>生徒会役員共</t>
+          <t>黄金の経験値</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>氏家ト全</t>
+          <t>原純(原作) 霜月汐(作画) fixro2n(キャラクター原案)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>#406</t>
+          <t>第17話（前編）</t>
         </is>
       </c>
     </row>
@@ -26759,17 +27801,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>姫騎士は蛮族の嫁</t>
+          <t>手に入れた催眠アプリで夢のハーレム生活を送りたい</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>コトバノリアキ</t>
+          <t>櫻ヨル(漫画) みょん(原作) マッパニナッタ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第52話②	浮船は未見の故郷</t>
+          <t>第10話①</t>
         </is>
       </c>
     </row>
@@ -26779,17 +27821,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>29歳独身は異世界で自由に生きた……かった。</t>
+          <t>デスマーチからはじまる異世界狂想曲</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>オオハマイコ(漫画) リュート(原作) 桑島黎音(キャラクター原案)</t>
+          <t>あやめぐむ(作画) 愛七ひろ(原作) ｓｈｒｉ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第41話-1②</t>
+          <t>第127話</t>
         </is>
       </c>
     </row>
@@ -26799,17 +27841,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>脇役に転生したはずが、いつの間にか伝説の錬金術師になってた～仲間たちが英雄でも俺は支援職なんだが～</t>
+          <t>野生のラスボスが現れた！ 黒翼の覇王</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>神無月みり 相野 仁</t>
+          <t>原作：炎頭・YahaKo 漫画：葉月翼</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第２６話　脇役、目論見を見破る（２）</t>
+          <t>第53話　水瓶座アクアリウス</t>
         </is>
       </c>
     </row>
@@ -26819,17 +27861,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>カナン様はあくまでチョロい</t>
+          <t>幼馴染のS級パーティーから追放された聖獣使い。万能支援魔法と仲間を増やして最強へ！</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>nonco</t>
+          <t>黒田高祥(作画) かなりつ(原作) 転(キャラクター原案)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第143話	ジャンヌのスマホデビュー</t>
+          <t>第51話-2</t>
         </is>
       </c>
     </row>
@@ -26839,17 +27881,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ポンコツ風紀委員とスカート丈が不適切なＪＫの話</t>
+          <t>フルメタル・パニック！　Family</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>横田卓馬</t>
+          <t>賀東招二(原作) 神反ヲ鬚(作画) 四季童子(キャラクター原案)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>描き下ろし休載イラスト</t>
+          <t>第6話　東京都江東区のタワマン39階②-2</t>
         </is>
       </c>
     </row>
@@ -26859,17 +27901,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+          <t>となりの席のヤツがそういう目で見てくる</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>光永康則</t>
+          <t>mmk</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第６６話『六花停止』④</t>
+          <t>第42話 名前</t>
         </is>
       </c>
     </row>
@@ -26879,17 +27921,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>すべての人類を破壊する。それらは再生できない。</t>
+          <t>【悲報】清楚系で売っていた底辺配信者、うっかり配信を切り忘れたままSS級モンスターを拳で殴り飛ばしてしまう</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>横田卓馬(漫画) 伊瀬勝良(原作)</t>
+          <t>アトハ NEO草野 pupps</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第66話その4</t>
+          <t>第５話　【悲報】ゆきのんとのコラボ配信、ワンパン撃破！？（２）</t>
         </is>
       </c>
     </row>
@@ -26899,17 +27941,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>王子様の友達</t>
+          <t>ヘルモード ～やり込み好きのゲーマーは廃設定の異世界で無双する～ はじまりの召喚士</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>すけろく(著者)</t>
+          <t>原作：ハム男・藻 漫画：鉄田猿児</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+          <t>GAME 082　マクリスの聖珠</t>
         </is>
       </c>
     </row>
@@ -26919,17 +27961,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ゴリラ女子高生</t>
+          <t>双子まとめて『カノジョ』にしない？</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>大友しゅうま(著者)</t>
+          <t>飴色みそ(漫画) 白井ムク(原作) 千種みのり(キャラクター原案)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+          <t>コミック第3巻発売告知！</t>
         </is>
       </c>
     </row>
@@ -26939,17 +27981,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>ダメ人間の愛しかた</t>
+          <t>どうやら私の身体は完全無敵のようですね</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>岩葉(著者)</t>
+          <t>さばねこ(作画) ちゃつふさ(原作) ふーみ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>コミックス3巻告知記事</t>
+          <t>休載イラスト</t>
         </is>
       </c>
     </row>
@@ -26959,17 +28001,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>ラブコメと怪獣退治の不文律</t>
+          <t>異世界ゆるっとサバイバル生活～学校の皆と異世界の無人島に転移したけど俺だけ楽勝です～</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>御池慧（漫画） 上代務（原作） TMSLab（原作）</t>
+          <t>西尾洋一(作画) 絢乃(原作) 乾和音(キャラクター原案) 株式会社一二三書房(監修)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+          <t>第49話-2</t>
         </is>
       </c>
     </row>
@@ -26979,17 +28021,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+          <t>仕事帰り、独身の美人上司に頼まれて</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>マツモトケンゴ</t>
+          <t>望公太(原作) とんのすけ(作画) しの(キャラクター原案)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第６１話　偽彼氏の戦いが始まった</t>
+          <t>休載イラスト</t>
         </is>
       </c>
     </row>
@@ -26999,17 +28041,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>転生錬金少女のスローライフ</t>
+          <t>放課後はケンカ最強のギャルに連れこまれる生活 彼女たちに好かれて、僕も最強に!?</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>里町(漫画) 夜想庭園(原作) potg(キャラクター原案)</t>
+          <t>亜逸(原作) あおやぎ孝夫(作画) ｋａｋａｏ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第17話-1</t>
+          <t>第16話</t>
         </is>
       </c>
     </row>
@@ -27019,17 +28061,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>よわよわ先生</t>
+          <t>王子様の友達</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>福地カミオ</t>
+          <t>すけろく(著者)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第108話	ミニミニのもみノート</t>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
@@ -27039,17 +28081,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>チート薬師のスローライフ ～異世界に作ろうドラッグストア～</t>
+          <t>ゴリラ女子高生</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ケンノジ 春乃えり</t>
+          <t>大友しゅうま(著者)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>67本目　気持ちを形に[後半]</t>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
@@ -27059,17 +28101,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>カット＆ペーストでこの世界を生きていく</t>
+          <t>ラブコメと怪獣退治の不文律</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>原作／咲夜(ツギクル) 漫画／加藤コウキ キャラクター原案／PiNe　乾和音　茶餅</t>
+          <t>御池慧（漫画） 上代務（原作） TMSLab（原作）</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第119話　自由奔放</t>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
@@ -27079,17 +28121,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>いとこのこ</t>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>いぬちく(著者)</t>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>距離が近すぎる爽ちゃんと一緒に行きたい場所募集～！！【コメント募集企画】</t>
+          <t>第34話①</t>
         </is>
       </c>
     </row>
@@ -27099,17 +28141,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ギルドを追放された回復術士、実は魔力無限だったので規格外の回復魔法で伝説となる</t>
+          <t>規格外のダンジョン攻略者、実は異世界帰りの元勇者</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>漫画：坂下コウ 原作：霞杏檎</t>
+          <t>作画：やまざき君 原作：榊与一</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第4話(1)</t>
+          <t>第4話(3)</t>
         </is>
       </c>
     </row>
@@ -27119,17 +28161,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>異世界チート魔術師</t>
+          <t>世界を救うために亜人と朝チュンできますか？</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>内田健（ヒーロー文庫／イマジカインフォス）(原作) 鈴羅木かりん(漫画) Ｎａｒｄａｃｋ(キャラクター原案)</t>
+          <t>音井れこ丸(作)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第92話-2</t>
+          <t>第46話-2</t>
         </is>
       </c>
     </row>
@@ -27139,17 +28181,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>百瀬アキラの初恋破綻中。</t>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>晴川シンタ</t>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第32話 あの日の想いを追憶中。</t>
+          <t>第9話-2</t>
         </is>
       </c>
     </row>
@@ -27159,17 +28201,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>勇者パーティーの荷物持ち</t>
+          <t>村人ですが何か？</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>原作：河本ほむら／作画：八嶋諒</t>
+          <t>鯖夢(作画) 白石新(原案・監修) 白蘇ふぁみ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第24話 荷物持ちと勇者パーティーの魔法使い②</t>
+          <t>第91話</t>
         </is>
       </c>
     </row>
@@ -27179,17 +28221,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>戸賀 環 坂木持丸 riritto</t>
+          <t>漫画/すたひろ 原作/Y.A</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第49話②　城のパーティーに参加してみた</t>
+          <t>chapter66【35話①】</t>
         </is>
       </c>
     </row>
@@ -27199,17 +28241,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
+          <t>「美人でお金持ちの彼女が欲しい」と言ったら、ワケあり女子がやってきた件。</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
+          <t>白鷺六羽(作画) 小宮地千々(原作) Re岳(キャラクター原案) マイクロマガジン社(監修)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第69話</t>
+          <t>第27話-2</t>
         </is>
       </c>
     </row>
@@ -27219,17 +28261,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ラスボス討伐後に始める二周目冒険者ライフ はじまりの街でワケあり美少女たちがめちゃくちゃ懐いてきます</t>
+          <t>戦姫サバイバルサガ-異世界の運命をかけた無人島フジュン異性交遊-</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>鬼麻正明(漫画) 朱月十話(原作) ファルまろ(キャラ原案)</t>
+          <t>OTOSAMA(著者)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第4話-2</t>
+          <t>第18話</t>
         </is>
       </c>
     </row>
@@ -27239,17 +28281,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>ジェノヴァの弟子～10秒しか戦えない魔術師、のちの『魔王』を育てる～</t>
+          <t>実は俺、最強でした？</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>原作：妹尾尻尾 漫画：魚塚じゃこ キャラクター原案：赤嶺直樹</t>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第22話</t>
+          <t>第121話　王都の危機を守れ!!・前編</t>
         </is>
       </c>
     </row>
@@ -27259,17 +28301,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>シャドウ・アサシンズ・ワールド ～影は薄いけど、最強忍者やってます～</t>
+          <t>異世界でスキルを解体したらチートな嫁が増殖しました 概念交差のストラクチャー</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>空山トキ 五色安未 泉乃せん 伍長</t>
+          <t>カタセミナミ(作画) 千月さかき(原作) 東西(キャラクター原案)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第11話　少女と本当の自分２（1）</t>
+          <t>第79話-2</t>
         </is>
       </c>
     </row>
@@ -27279,17 +28321,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>最果てのパラディン</t>
+          <t>ルパン三世 異世界の姫君（ネイバーワールドプリンセス）</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>奥橋睦（漫画） 柳野かなた（原作） 輪くすさが（キャラクター原案）</t>
+          <t>モンキー・パンチ／エム・ピー・ワークス 内々けやき 佐伯庸介 白狼</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第66話　祝宴</t>
+          <t>第102話：マッスルタの魔犬❷</t>
         </is>
       </c>
     </row>
@@ -27299,17 +28341,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>宇崎ちゃんは遊びたい！</t>
+          <t>斎藤義龍に生まれ変わったので、織田信長に国譲りして長生きするのを目指します！</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>丈(著者)</t>
+          <t>巽未頼 田村ゆうき マキムラシュンスケ</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第125話</t>
+          <t>第72話「信ずるか否かを決める」</t>
         </is>
       </c>
     </row>
@@ -27319,17 +28361,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>塔の管理をしてみよう</t>
+          <t>殺されたらゾンビになったので、進化しまくって無双しようと思います</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
+          <t>漫画：朝ケ夜 原作：幸運ピエロ キャラクター原案：東西</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第91話前編</t>
+          <t>第16話(前半)ダンジョン開放①</t>
         </is>
       </c>
     </row>
@@ -27339,17 +28381,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>絶対死なないステラ姫</t>
+          <t>六姫は神護衛に恋をする　～最強の守護騎士、転生して魔法学園に行く～</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>光永康則 大高稲</t>
+          <t>漫画:加古山 寿 原案:朱月 十話 キャラクター原案:てつぶた</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第１４話　絶対旅立たない（２）</t>
+          <t>第123話　未来</t>
         </is>
       </c>
     </row>
@@ -27359,17 +28401,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>葉木莉さんは君だけの死神になりたい</t>
+          <t>ポンコツ勇者パーティー、竜をひろう</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>35まち</t>
+          <t>優風(著者)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第６話　それは好きということでは？</t>
+          <t>第3話</t>
         </is>
       </c>
     </row>
@@ -27379,17 +28421,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>人生逆転ダンジョン</t>
+          <t>おねえさんと猫を飼う</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>尾張 ニコ どすこい花丸様</t>
+          <t>上杉響士郎(著者)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第3-2話	穴は使いよう</t>
+          <t>第3話：おねえさんと猫を洗う</t>
         </is>
       </c>
     </row>
@@ -27399,17 +28441,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>ひとりぼっちの異世界攻略</t>
+          <t>没落予定なので、鍛冶職人を目指す</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>びび（漫画） 五示正司（原作）</t>
+          <t>石田彩(作画) CK(原作) かわく(キャラクター原案)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第228話　弱肉強食</t>
+          <t>第100話-2</t>
         </is>
       </c>
     </row>
@@ -27419,17 +28461,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>煽り系ゲーム配信者（20歳）、配信の切り忘れによりいい人バレする。</t>
+          <t>直径3cmの召喚陣&lt;リミットリング&gt;で「雑魚すら呼べない」と蔑まれた底辺召喚士が頂点に立つまで</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>流嘉（漫画） 夏乃実（原作） 麦うさぎ（キャラクター原案）</t>
+          <t>作画：まっつー 原作：空松蓮司</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第4話　サブ垢（後編）</t>
+          <t>第4話(3)</t>
         </is>
       </c>
     </row>
@@ -27439,17 +28481,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ダウナー系お姉さんに毎日カスの嘘を流し込まれる話</t>
+          <t>僕のカノジョ先生</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>生倉のゑる(著者) はるばーど屋(原作者)</t>
+          <t>星河蟹(作画) 孟倫（ＳＤｗｉｎｇ）(構成) 鏡遊(原作) おりょう(キャラクター原案)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第11話</t>
+          <t>75時間目-2</t>
         </is>
       </c>
     </row>
@@ -27459,17 +28501,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>終焉の魔女と世界の旅</t>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>片岡とんち</t>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第13話②	終焉の魔女と魔王メリア</t>
+          <t>第32話 独身貴族は森で写真を撮る（2）</t>
         </is>
       </c>
     </row>
@@ -27479,17 +28521,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Sランク冒険者である俺の娘たちは重度のファザコンでした</t>
+          <t>モブだけど最強を目指します！　～ゲーム世界に転生した俺は自由に強さを追い求める～</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>しゅにち（漫画） 友橋かめつ（原作） 希望つばめ（原作イラスト）</t>
+          <t>反面教師(原作) 五條さやか(作画) 大熊猫介(キャラクター原案)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第46話　敵か、味方か</t>
+          <t>第12話-1</t>
         </is>
       </c>
     </row>
@@ -27499,17 +28541,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>履いてください、鷹峰さん</t>
+          <t>Only Sense Online ‐オンリーセンス・オンライン‐</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>柊裕一</t>
+          <t>羽仁倉雲(作画) アロハ座長(原作) ゆきさん(キャラクター原案)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第64話 当人同士で、どうぞ。(前編)</t>
+          <t>第128話-1</t>
         </is>
       </c>
     </row>
@@ -27519,17 +28561,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>アンゴルモア 元寇合戦記　【博多編】</t>
+          <t>隣の席のヤンキー清水さんが髪を黒く染めてきた</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>たかぎ七彦(著者)</t>
+          <t>底花(原作) 真田若楓(漫画) ハム(キャラクター原案)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第四十四話その六</t>
+          <t>第10話-2</t>
         </is>
       </c>
     </row>
@@ -27539,17 +28581,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>恋人以上友人未満</t>
+          <t>異種族追放コンカフェ</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>yatoyato</t>
+          <t>佐々木マサヒト(著者)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第93話</t>
+          <t>【投票企画】おまけ漫画を描いてほしいキャラ募集～！【2巻発売記念】</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-07-26
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -40,6 +40,7 @@
     <sheet name="2025-07-23" sheetId="32" state="visible" r:id="rId32"/>
     <sheet name="2025-07-24" sheetId="33" state="visible" r:id="rId33"/>
     <sheet name="2025-07-25" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="2025-07-26" sheetId="35" state="visible" r:id="rId35"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -27596,22 +27597,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>ワンパンマン</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>206撃目</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>ダークサモナーとデキている</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>車王(著者)</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>【コミックス第6巻発売記念】挟まるならどの衣装？コメント大募集！</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>最弱テイマーはゴミ拾いの旅を始めました。@COMIC</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>漫画：蕗野 冬 原作：ほのぼのる500 キャラクター原案：なま</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第26話</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>魔王になったので、ダンジョン造って人外娘とほのぼのする</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>遠野ノオト(作画) 流優(原作) だぶ竜(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第82話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>バーサス</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第26話 惨事（2）</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>魔石グルメ　魔物の力を食べたオレは最強！</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>菅原健二(作画) 結城涼(原作) 成瀬ちさと(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第67話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>ゲーム悪役貴族に転生した俺は、チート筋肉で無双する</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>昼行燈（原作） しいたけ元帥（漫画）</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第26話</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>空野進 sorani ファルまろ</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第10話　最弱貴族、部下を信じる（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>転生したらスライムだった件 異聞 ～魔国暮らしのトリニティ～</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>伏瀬 戸野タエ みっつばー</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第107話　開国祭開幕［その２］</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>黄金の経験値</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>原純(原作) 霜月汐(作画) fixro2n(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第17話（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>手に入れた催眠アプリで夢のハーレム生活を送りたい</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>櫻ヨル(漫画) みょん(原作) マッパニナッタ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第10話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>デスマーチからはじまる異世界狂想曲</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>あやめぐむ(作画) 愛七ひろ(原作) ｓｈｒｉ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第127話</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>野生のラスボスが現れた！ 黒翼の覇王</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>原作：炎頭・YahaKo 漫画：葉月翼</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第53話　水瓶座アクアリウス</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>幼馴染のS級パーティーから追放された聖獣使い。万能支援魔法と仲間を増やして最強へ！</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>黒田高祥(作画) かなりつ(原作) 転(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第51話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>フルメタル・パニック！　Family</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>賀東招二(原作) 神反ヲ鬚(作画) 四季童子(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第6話　東京都江東区のタワマン39階②-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>となりの席のヤツがそういう目で見てくる</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>mmk</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第42話 名前</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>【悲報】清楚系で売っていた底辺配信者、うっかり配信を切り忘れたままSS級モンスターを拳で殴り飛ばしてしまう</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>アトハ NEO草野 pupps</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第５話　【悲報】ゆきのんとのコラボ配信、ワンパン撃破！？（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>ヘルモード ～やり込み好きのゲーマーは廃設定の異世界で無双する～ はじまりの召喚士</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>原作：ハム男・藻 漫画：鉄田猿児</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>GAME 082　マクリスの聖珠</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>双子まとめて『カノジョ』にしない？</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>飴色みそ(漫画) 白井ムク(原作) 千種みのり(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>コミック第3巻発売告知！</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>どうやら私の身体は完全無敵のようですね</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>さばねこ(作画) ちゃつふさ(原作) ふーみ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>休載イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>異世界ゆるっとサバイバル生活～学校の皆と異世界の無人島に転移したけど俺だけ楽勝です～</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>西尾洋一(作画) 絢乃(原作) 乾和音(キャラクター原案) 株式会社一二三書房(監修)</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第49話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>仕事帰り、独身の美人上司に頼まれて</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>望公太(原作) とんのすけ(作画) しの(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>休載イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>放課後はケンカ最強のギャルに連れこまれる生活 彼女たちに好かれて、僕も最強に!?</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>亜逸(原作) あおやぎ孝夫(作画) ｋａｋａｏ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第16話</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>王子様の友達</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>すけろく(著者)</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>ゴリラ女子高生</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>大友しゅうま(著者)</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>ラブコメと怪獣退治の不文律</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>御池慧（漫画） 上代務（原作） TMSLab（原作）</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第34話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>規格外のダンジョン攻略者、実は異世界帰りの元勇者</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>作画：やまざき君 原作：榊与一</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第4話(3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>世界を救うために亜人と朝チュンできますか？</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>音井れこ丸(作)</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第46話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第9話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>村人ですが何か？</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>鯖夢(作画) 白石新(原案・監修) 白蘇ふぁみ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第91話</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>漫画/すたひろ 原作/Y.A</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>chapter66【35話①】</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>「美人でお金持ちの彼女が欲しい」と言ったら、ワケあり女子がやってきた件。</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>白鷺六羽(作画) 小宮地千々(原作) Re岳(キャラクター原案) マイクロマガジン社(監修)</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第27話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>戦姫サバイバルサガ-異世界の運命をかけた無人島フジュン異性交遊-</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>OTOSAMA(著者)</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第18話</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第121話　王都の危機を守れ!!・前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>異世界でスキルを解体したらチートな嫁が増殖しました 概念交差のストラクチャー</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>カタセミナミ(作画) 千月さかき(原作) 東西(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第79話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>ルパン三世 異世界の姫君（ネイバーワールドプリンセス）</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>モンキー・パンチ／エム・ピー・ワークス 内々けやき 佐伯庸介 白狼</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第102話：マッスルタの魔犬❷</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>斎藤義龍に生まれ変わったので、織田信長に国譲りして長生きするのを目指します！</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>巽未頼 田村ゆうき マキムラシュンスケ</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第72話「信ずるか否かを決める」</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>殺されたらゾンビになったので、進化しまくって無双しようと思います</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>漫画：朝ケ夜 原作：幸運ピエロ キャラクター原案：東西</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第16話(前半)ダンジョン開放①</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>六姫は神護衛に恋をする　～最強の守護騎士、転生して魔法学園に行く～</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>漫画:加古山 寿 原案:朱月 十話 キャラクター原案:てつぶた</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第123話　未来</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>ポンコツ勇者パーティー、竜をひろう</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>優風(著者)</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第3話</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>おねえさんと猫を飼う</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>上杉響士郎(著者)</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第3話：おねえさんと猫を洗う</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>没落予定なので、鍛冶職人を目指す</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>石田彩(作画) CK(原作) かわく(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第100話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>直径3cmの召喚陣&lt;リミットリング&gt;で「雑魚すら呼べない」と蔑まれた底辺召喚士が頂点に立つまで</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>作画：まっつー 原作：空松蓮司</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第4話(3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>僕のカノジョ先生</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>星河蟹(作画) 孟倫（ＳＤｗｉｎｇ）(構成) 鏡遊(原作) おりょう(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>75時間目-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第32話 独身貴族は森で写真を撮る（2）</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>モブだけど最強を目指します！　～ゲーム世界に転生した俺は自由に強さを追い求める～</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>反面教師(原作) 五條さやか(作画) 大熊猫介(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第12話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>Only Sense Online ‐オンリーセンス・オンライン‐</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>羽仁倉雲(作画) アロハ座長(原作) ゆきさん(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第128話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>隣の席のヤンキー清水さんが髪を黒く染めてきた</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>底花(原作) 真田若楓(漫画) ハム(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第10話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>異種族追放コンカフェ</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>佐々木マサヒト(著者)</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>【投票企画】おまけ漫画を描いてほしいキャラ募集～！【2巻発売記念】</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ワンパンマン</t>
+          <t>異世界おじさん</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>原作/ＯＮＥ 作画/村田雄介</t>
+          <t>殆ど死んでいる(著者)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>206撃目</t>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
@@ -27621,17 +28663,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ダークサモナーとデキている</t>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>車王(著者)</t>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>【コミックス第6巻発売記念】挟まるならどの衣装？コメント大募集！</t>
+          <t>「名もなき英雄譚」後半</t>
         </is>
       </c>
     </row>
@@ -27641,17 +28683,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>最弱テイマーはゴミ拾いの旅を始めました。@COMIC</t>
+          <t>淫獄団地</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>漫画：蕗野 冬 原作：ほのぼのる500 キャラクター原案：なま</t>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第26話</t>
+          <t>第49話（前編）</t>
         </is>
       </c>
     </row>
@@ -27661,17 +28703,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>魔王になったので、ダンジョン造って人外娘とほのぼのする</t>
+          <t>まんきつしたい常連さん</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>遠野ノオト(作画) 流優(原作) だぶ竜(キャラクター原案)</t>
+          <t>しんみりん(著者)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第82話後半</t>
+          <t>第46話前編</t>
         </is>
       </c>
     </row>
@@ -27681,17 +28723,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>バーサス</t>
+          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
+          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第26話 惨事（2）</t>
+          <t>第23話</t>
         </is>
       </c>
     </row>
@@ -27701,17 +28743,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>魔石グルメ　魔物の力を食べたオレは最強！</t>
+          <t>美人女上司滝沢さん</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>菅原健二(作画) 結城涼(原作) 成瀬ちさと(キャラクター原案)</t>
+          <t>やんBARU(著者)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第67話前半</t>
+          <t>第202話</t>
         </is>
       </c>
     </row>
@@ -27721,17 +28763,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ゲーム悪役貴族に転生した俺は、チート筋肉で無双する</t>
+          <t>よくわからないけれど異世界に転生していたようです</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>昼行燈（原作） しいたけ元帥（漫画）</t>
+          <t>内々けやき あし カオミン</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第26話</t>
+          <t>第136話 よくわからないけれどスカウトされたみたいです（２）</t>
         </is>
       </c>
     </row>
@@ -27741,17 +28783,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>空野進 sorani ファルまろ</t>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第10話　最弱貴族、部下を信じる（３）</t>
+          <t>第80話その3</t>
         </is>
       </c>
     </row>
@@ -27761,17 +28803,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>転生したらスライムだった件 異聞 ～魔国暮らしのトリニティ～</t>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>伏瀬 戸野タエ みっつばー</t>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第107話　開国祭開幕［その２］</t>
+          <t>第71話(前編) ダリエルVS.滾り</t>
         </is>
       </c>
     </row>
@@ -27781,17 +28823,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>黄金の経験値</t>
+          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>原純(原作) 霜月汐(作画) fixro2n(キャラクター原案)</t>
+          <t>FUNA 東西 モトエ恵介</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第17話（前編）</t>
+          <t>第120話　会談［その5］</t>
         </is>
       </c>
     </row>
@@ -27801,17 +28843,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>手に入れた催眠アプリで夢のハーレム生活を送りたい</t>
+          <t>天獄で悪魔がボクを魅惑する</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>櫻ヨル(漫画) みょん(原作) マッパニナッタ(キャラクター原案)</t>
+          <t>銀河味めてお(著者)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第10話①</t>
+          <t>第34話</t>
         </is>
       </c>
     </row>
@@ -27821,17 +28863,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>デスマーチからはじまる異世界狂想曲</t>
+          <t>ワンパンマン</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>あやめぐむ(作画) 愛七ひろ(原作) ｓｈｒｉ(キャラクター原案)</t>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第127話</t>
+          <t>206撃目</t>
         </is>
       </c>
     </row>
@@ -27841,17 +28883,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>野生のラスボスが現れた！ 黒翼の覇王</t>
+          <t>ずっと好きだった幼馴染と付き合い始めたら一途ビッチの性欲ジャンキーだったんだがどうすりゃいいですか？</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>原作：炎頭・YahaKo 漫画：葉月翼</t>
+          <t>原作：トラ子猫 作画：あらいぐま</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第53話　水瓶座アクアリウス</t>
+          <t>第3話</t>
         </is>
       </c>
     </row>
@@ -27861,17 +28903,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>幼馴染のS級パーティーから追放された聖獣使い。万能支援魔法と仲間を増やして最強へ！</t>
+          <t>冒険者絶対殺すダンジョン</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>黒田高祥(作画) かなりつ(原作) 転(キャラクター原案)</t>
+          <t>道満晴明(著者)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第51話-2</t>
+          <t>第34話</t>
         </is>
       </c>
     </row>
@@ -27881,17 +28923,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>フルメタル・パニック！　Family</t>
+          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>賀東招二(原作) 神反ヲ鬚(作画) 四季童子(キャラクター原案)</t>
+          <t>神原絵理華(漫画) 一森一輝(原作)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第6話　東京都江東区のタワマン39階②-2</t>
+          <t>第18話②</t>
         </is>
       </c>
     </row>
@@ -27901,17 +28943,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>となりの席のヤツがそういう目で見てくる</t>
+          <t>両親の借金を肩代わりしてもらう条件は日本一可愛い女子高生と一緒に暮らすことでした。</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>mmk</t>
+          <t>美月めいあ(漫画) 雨音恵(原作) ｋａｋａｏ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第42話 名前</t>
+          <t>第36話</t>
         </is>
       </c>
     </row>
@@ -27921,17 +28963,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>【悲報】清楚系で売っていた底辺配信者、うっかり配信を切り忘れたままSS級モンスターを拳で殴り飛ばしてしまう</t>
+          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>アトハ NEO草野 pupps</t>
+          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第５話　【悲報】ゆきのんとのコラボ配信、ワンパン撃破！？（２）</t>
+          <t>第75話 ゆめうつつ</t>
         </is>
       </c>
     </row>
@@ -27941,17 +28983,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ヘルモード ～やり込み好きのゲーマーは廃設定の異世界で無双する～ はじまりの召喚士</t>
+          <t>陰キャの僕に罰ゲームで告白してきたはずのギャルが、どう見ても僕にベタ惚れです</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>原作：ハム男・藻 漫画：鉄田猿児</t>
+          <t>神奈なごみ(漫画) 結石(原作) かがちさく(キャラクター原案)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>GAME 082　マクリスの聖珠</t>
+          <t>第26話</t>
         </is>
       </c>
     </row>
@@ -27961,17 +29003,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>双子まとめて『カノジョ』にしない？</t>
+          <t>修羅幼女の英雄譚～半端者と言われた傭兵、幼女に転生して成り上がる～</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>飴色みそ(漫画) 白井ムク(原作) 千種みのり(キャラクター原案)</t>
+          <t>作画：むらたん 原作：沙城流</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>コミック第3巻発売告知！</t>
+          <t>第7話(3)</t>
         </is>
       </c>
     </row>
@@ -27981,17 +29023,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>どうやら私の身体は完全無敵のようですね</t>
+          <t>ゴリラ女子高生</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>さばねこ(作画) ちゃつふさ(原作) ふーみ(キャラクター原案)</t>
+          <t>大友しゅうま(著者)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>休載イラスト</t>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
@@ -28001,17 +29043,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>異世界ゆるっとサバイバル生活～学校の皆と異世界の無人島に転移したけど俺だけ楽勝です～</t>
+          <t>王子様の友達</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>西尾洋一(作画) 絢乃(原作) 乾和音(キャラクター原案) 株式会社一二三書房(監修)</t>
+          <t>すけろく(著者)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第49話-2</t>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
@@ -28021,17 +29063,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>仕事帰り、独身の美人上司に頼まれて</t>
+          <t>ラブコメと怪獣退治の不文律</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>望公太(原作) とんのすけ(作画) しの(キャラクター原案)</t>
+          <t>御池慧（漫画） 上代務（原作） TMSLab（原作）</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>休載イラスト</t>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
@@ -28041,17 +29083,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>放課後はケンカ最強のギャルに連れこまれる生活 彼女たちに好かれて、僕も最強に!?</t>
+          <t>わたし、二番目の彼女でいいから。</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>亜逸(原作) あおやぎ孝夫(作画) ｋａｋａｏ(キャラクター原案)</t>
+          <t>にの子(漫画) 西条陽(原作) Re岳(キャラクター原案)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第16話</t>
+          <t>第10話③：カーテンのなか</t>
         </is>
       </c>
     </row>
@@ -28061,17 +29103,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>王子様の友達</t>
+          <t>ヤンデレかと思ったらもっとヤベー女だった</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>すけろく(著者)</t>
+          <t>八木戸マト</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+          <t>第68話　全てを失ったヤンデレ彼女</t>
         </is>
       </c>
     </row>
@@ -28081,17 +29123,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ゴリラ女子高生</t>
+          <t>センパイ、自宅警備員の雇用はいかがですか？</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>大友しゅうま(著者)</t>
+          <t>漫画：コブラサナギ 原作：二上圭 キャラ原案：日向あずり</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+          <t>第5話後半</t>
         </is>
       </c>
     </row>
@@ -28101,17 +29143,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ラブコメと怪獣退治の不文律</t>
+          <t>スキルがなければレベルを上げる～９９がカンストの世界でレベル800万からスタート～</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>御池慧（漫画） 上代務（原作） TMSLab（原作）</t>
+          <t>倉橋ユウス(漫画) 岡沢六十四(原作)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+          <t>第51話④</t>
         </is>
       </c>
     </row>
@@ -28121,17 +29163,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+          <t>時森さんが無防備です!!</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+          <t>たざわ</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第34話①</t>
+          <t>第63話</t>
         </is>
       </c>
     </row>
@@ -28141,17 +29183,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>規格外のダンジョン攻略者、実は異世界帰りの元勇者</t>
+          <t>不老不死少女の苗床旅行記</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>作画：やまざき君 原作：榊与一</t>
+          <t>ふじはん(漫画) ルナ・ウサギ(原作)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第4話(3)</t>
+          <t>第16話後編</t>
         </is>
       </c>
     </row>
@@ -28161,17 +29203,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>世界を救うために亜人と朝チュンできますか？</t>
+          <t>くじ引き特賞：無双ハーレム権</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>音井れこ丸(作)</t>
+          <t>原作／三木なずな（GA文庫／SBクリエイティブ刊） 漫画／長谷見亮 キャラクター原案／瑠奈璃亜</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第46話-2</t>
+          <t>第58話-02　新たな王女たちへ、受け継がれし慈愛の心！</t>
         </is>
       </c>
     </row>
@@ -28181,17 +29223,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+          <t>勇者のクズ</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+          <t>ナカシマ723</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第9話-2</t>
+          <t>第48話　勇者の矜持 II（前半）</t>
         </is>
       </c>
     </row>
@@ -28201,17 +29243,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>村人ですが何か？</t>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>鯖夢(作画) 白石新(原案・監修) 白蘇ふぁみ(キャラクター原案)</t>
+          <t>漫画/すたひろ 原作/Y.A</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第91話</t>
+          <t>chapter66【35話①】</t>
         </is>
       </c>
     </row>
@@ -28221,17 +29263,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+          <t>断れない会長は友江くんにだけしてあげたい</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>漫画/すたひろ 原作/Y.A</t>
+          <t>沼地どろまる(著者)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>chapter66【35話①】</t>
+          <t>休載漫画</t>
         </is>
       </c>
     </row>
@@ -28241,17 +29283,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>「美人でお金持ちの彼女が欲しい」と言ったら、ワケあり女子がやってきた件。</t>
+          <t>ダウナーお姉さんは遊びたい</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>白鷺六羽(作画) 小宮地千々(原作) Re岳(キャラクター原案) マイクロマガジン社(監修)</t>
+          <t>山鷹景</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第27話-2</t>
+          <t>第15話</t>
         </is>
       </c>
     </row>
@@ -28261,17 +29303,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>戦姫サバイバルサガ-異世界の運命をかけた無人島フジュン異性交遊-</t>
+          <t>聖騎士になったけど団長のおっぱいが凄すぎて心が清められない</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>OTOSAMA(著者)</t>
+          <t>木の芽(原作) 川喜田ミツオ(漫画) 雨傘ゆん(キャラクター原案)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第18話</t>
+          <t>コミックス6巻発売＆休載のお知らせ</t>
         </is>
       </c>
     </row>
@@ -28281,17 +29323,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>実は俺、最強でした？</t>
+          <t>脱稿するまでオチません</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>原作：澄守 彩 漫画：高橋 愛</t>
+          <t>ヨシラギ(著者)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第121話　王都の危機を守れ!!・前編</t>
+          <t>第32話後半</t>
         </is>
       </c>
     </row>
@@ -28301,17 +29343,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>異世界でスキルを解体したらチートな嫁が増殖しました 概念交差のストラクチャー</t>
+          <t>勇者パーティから追い出された不遇職【罠士】、ユニークスキル【矢印】で最強になる</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>カタセミナミ(作画) 千月さかき(原作) 東西(キャラクター原案)</t>
+          <t>作画：たつひこ 原作：白石 有希</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第79話-2</t>
+          <t>第7話(3)</t>
         </is>
       </c>
     </row>
@@ -28321,17 +29363,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ルパン三世 異世界の姫君（ネイバーワールドプリンセス）</t>
+          <t>クラスの大嫌いな女子と結婚することになった。</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>モンキー・パンチ／エム・ピー・ワークス 内々けやき 佐伯庸介 白狼</t>
+          <t>天乃聖樹(原作) もすこんぶ(漫画)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第102話：マッスルタの魔犬❷</t>
+          <t>第44話-2</t>
         </is>
       </c>
     </row>
@@ -28341,17 +29383,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>斎藤義龍に生まれ変わったので、織田信長に国譲りして長生きするのを目指します！</t>
+          <t>隣のクーデレラを甘やかしたら、ウチの合鍵を渡すことになった</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>巽未頼 田村ゆうき マキムラシュンスケ</t>
+          <t>青島かなえ(漫画) 雪仁(原作) かがちさく(キャラクター原案)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第72話「信ずるか否かを決める」</t>
+          <t>第38話</t>
         </is>
       </c>
     </row>
@@ -28361,17 +29403,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>殺されたらゾンビになったので、進化しまくって無双しようと思います</t>
+          <t>りんちゃんは据え膳したい</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>漫画：朝ケ夜 原作：幸運ピエロ キャラクター原案：東西</t>
+          <t>澄田佑貴(著者)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第16話(前半)ダンジョン開放①</t>
+          <t>第38話</t>
         </is>
       </c>
     </row>
@@ -28381,17 +29423,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>六姫は神護衛に恋をする　～最強の守護騎士、転生して魔法学園に行く～</t>
+          <t>ボクの理想の異世界生活 ～転生したらケモ耳娘だらけの世界でハーレムに～</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>漫画:加古山 寿 原案:朱月 十話 キャラクター原案:てつぶた</t>
+          <t>イチリ(原作) 空維深夜(作画)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第123話　未来</t>
+          <t>第15話前半：CALL</t>
         </is>
       </c>
     </row>
@@ -28401,17 +29443,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>ポンコツ勇者パーティー、竜をひろう</t>
+          <t>その冒険者、取り扱い注意。 ～正体は無敵の下僕たちを統べる異世界最強の魔導王～</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>優風(著者)</t>
+          <t>満月シオン(作画) Sin Guilty(ツギクル)(原作) M.B(キャラクター原案)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第3話</t>
+          <t>56章　はじまりの愚か者②　後編</t>
         </is>
       </c>
     </row>
@@ -28421,17 +29463,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>おねえさんと猫を飼う</t>
+          <t>俺の愛娘は悪役令嬢</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>上杉響士郎(著者)</t>
+          <t>かわもり かぐら(原作) ほづみりや(漫画) 縞(キャラクター原案)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第3話：おねえさんと猫を洗う</t>
+          <t>第4話-2</t>
         </is>
       </c>
     </row>
@@ -28441,17 +29483,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>没落予定なので、鍛冶職人を目指す</t>
+          <t>フルメタル・パニック！　Family</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>石田彩(作画) CK(原作) かわく(キャラクター原案)</t>
+          <t>賀東招二(原作) 神反ヲ鬚(作画) 四季童子(キャラクター原案)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第100話-2</t>
+          <t>第6話　東京都江東区のタワマン39階②-2</t>
         </is>
       </c>
     </row>
@@ -28461,17 +29503,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>直径3cmの召喚陣&lt;リミットリング&gt;で「雑魚すら呼べない」と蔑まれた底辺召喚士が頂点に立つまで</t>
+          <t>双子の姉が神子として引き取られて、私は捨てられたけど多分私が神子である。</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>作画：まっつー 原作：空松蓮司</t>
+          <t>雪(著者) 池中織奈(原作) カット(キャラクター原案)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第4話(3)</t>
+          <t>第32話後編</t>
         </is>
       </c>
     </row>
@@ -28481,17 +29523,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>僕のカノジョ先生</t>
+          <t>TRPGプレイヤーが異世界で最強ビルドを目指す ～ヘンダーソン氏の福音を～</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>星河蟹(作画) 孟倫（ＳＤｗｉｎｇ）(構成) 鏡遊(原作) おりょう(キャラクター原案)</t>
+          <t>内田テモ(漫画) Schuld(原作) ランサネ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>75時間目-2</t>
+          <t>第14話</t>
         </is>
       </c>
     </row>
@@ -28501,17 +29543,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+          <t>クロの戦記Ⅱ 異世界転移した僕が最強なのはベッドの上だけのようです</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+          <t>サイトウアユム(原作) ユリシロ(漫画) むつみまさと(キャラクター原案)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第32話 独身貴族は森で写真を撮る（2）</t>
+          <t>第22話-2</t>
         </is>
       </c>
     </row>
@@ -28521,17 +29563,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>モブだけど最強を目指します！　～ゲーム世界に転生した俺は自由に強さを追い求める～</t>
+          <t>ダークサモナーとデキている</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>反面教師(原作) 五條さやか(作画) 大熊猫介(キャラクター原案)</t>
+          <t>車王(著者)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第12話-1</t>
+          <t>【コミックス第6巻発売記念】挟まるならどの衣装？コメント大募集！</t>
         </is>
       </c>
     </row>
@@ -28541,17 +29583,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Only Sense Online ‐オンリーセンス・オンライン‐</t>
+          <t>ギルドを追放された回復術士、実は魔力無限だったので規格外の回復魔法で伝説となる</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>羽仁倉雲(作画) アロハ座長(原作) ゆきさん(キャラクター原案)</t>
+          <t>漫画：坂下コウ 原作：霞杏檎</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第128話-1</t>
+          <t>第4話(2)</t>
         </is>
       </c>
     </row>
@@ -28561,17 +29603,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>隣の席のヤンキー清水さんが髪を黒く染めてきた</t>
+          <t>チンチンデビルを追え！</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>底花(原作) 真田若楓(漫画) ハム(キャラクター原案)</t>
+          <t>くぼたふみお</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第10話-2</t>
+          <t>第３１話　激突！ アンとキュベレ！</t>
         </is>
       </c>
     </row>
@@ -28581,17 +29623,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>異種族追放コンカフェ</t>
+          <t>俺の『鑑定』スキルがチートすぎて ～伝説の勇者を読み“盗り”最強へ～</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>佐々木マサヒト(著者)</t>
+          <t>原作：澄守　彩 漫画：龍牙 翔</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>【投票企画】おまけ漫画を描いてほしいキャラ募集～！【2巻発売記念】</t>
+          <t>第33話ー③　迷宮の掃除番</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-07-27
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -41,6 +41,7 @@
     <sheet name="2025-07-24" sheetId="33" state="visible" r:id="rId33"/>
     <sheet name="2025-07-25" sheetId="34" state="visible" r:id="rId34"/>
     <sheet name="2025-07-26" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="2025-07-27" sheetId="36" state="visible" r:id="rId36"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -28638,22 +28639,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>異世界おじさん</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>殆ど死んでいる(著者)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>「名もなき英雄譚」後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>淫獄団地</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第49話（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>まんきつしたい常連さん</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>しんみりん(著者)</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第46話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第23話</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>美人女上司滝沢さん</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>やんBARU(著者)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第202話</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第136話 よくわからないけれどスカウトされたみたいです（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第80話その3</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第71話(前編) ダリエルVS.滾り</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>FUNA 東西 モトエ恵介</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第120話　会談［その5］</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>天獄で悪魔がボクを魅惑する</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>銀河味めてお(著者)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第34話</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>ワンパンマン</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>206撃目</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>ずっと好きだった幼馴染と付き合い始めたら一途ビッチの性欲ジャンキーだったんだがどうすりゃいいですか？</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>原作：トラ子猫 作画：あらいぐま</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第3話</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>冒険者絶対殺すダンジョン</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>道満晴明(著者)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第34話</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>神原絵理華(漫画) 一森一輝(原作)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第18話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>両親の借金を肩代わりしてもらう条件は日本一可愛い女子高生と一緒に暮らすことでした。</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>美月めいあ(漫画) 雨音恵(原作) ｋａｋａｏ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第36話</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第75話 ゆめうつつ</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>陰キャの僕に罰ゲームで告白してきたはずのギャルが、どう見ても僕にベタ惚れです</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>神奈なごみ(漫画) 結石(原作) かがちさく(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第26話</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>修羅幼女の英雄譚～半端者と言われた傭兵、幼女に転生して成り上がる～</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>作画：むらたん 原作：沙城流</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第7話(3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>ゴリラ女子高生</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>大友しゅうま(著者)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>王子様の友達</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>すけろく(著者)</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>ラブコメと怪獣退治の不文律</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>御池慧（漫画） 上代務（原作） TMSLab（原作）</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>わたし、二番目の彼女でいいから。</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>にの子(漫画) 西条陽(原作) Re岳(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第10話③：カーテンのなか</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>ヤンデレかと思ったらもっとヤベー女だった</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>八木戸マト</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第68話　全てを失ったヤンデレ彼女</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>センパイ、自宅警備員の雇用はいかがですか？</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>漫画：コブラサナギ 原作：二上圭 キャラ原案：日向あずり</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第5話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>スキルがなければレベルを上げる～９９がカンストの世界でレベル800万からスタート～</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>倉橋ユウス(漫画) 岡沢六十四(原作)</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第51話④</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>時森さんが無防備です!!</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>たざわ</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第63話</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>不老不死少女の苗床旅行記</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>ふじはん(漫画) ルナ・ウサギ(原作)</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第16話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>くじ引き特賞：無双ハーレム権</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>原作／三木なずな（GA文庫／SBクリエイティブ刊） 漫画／長谷見亮 キャラクター原案／瑠奈璃亜</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第58話-02　新たな王女たちへ、受け継がれし慈愛の心！</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>勇者のクズ</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>ナカシマ723</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第48話　勇者の矜持 II（前半）</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>漫画/すたひろ 原作/Y.A</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>chapter66【35話①】</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>断れない会長は友江くんにだけしてあげたい</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>沼地どろまる(著者)</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>休載漫画</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>ダウナーお姉さんは遊びたい</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>山鷹景</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第15話</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>聖騎士になったけど団長のおっぱいが凄すぎて心が清められない</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>木の芽(原作) 川喜田ミツオ(漫画) 雨傘ゆん(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>コミックス6巻発売＆休載のお知らせ</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>脱稿するまでオチません</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>ヨシラギ(著者)</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第32話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティから追い出された不遇職【罠士】、ユニークスキル【矢印】で最強になる</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>作画：たつひこ 原作：白石 有希</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第7話(3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>クラスの大嫌いな女子と結婚することになった。</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>天乃聖樹(原作) もすこんぶ(漫画)</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第44話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>隣のクーデレラを甘やかしたら、ウチの合鍵を渡すことになった</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>青島かなえ(漫画) 雪仁(原作) かがちさく(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第38話</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>りんちゃんは据え膳したい</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>澄田佑貴(著者)</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第38話</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>ボクの理想の異世界生活 ～転生したらケモ耳娘だらけの世界でハーレムに～</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>イチリ(原作) 空維深夜(作画)</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第15話前半：CALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>その冒険者、取り扱い注意。 ～正体は無敵の下僕たちを統べる異世界最強の魔導王～</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>満月シオン(作画) Sin Guilty(ツギクル)(原作) M.B(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>56章　はじまりの愚か者②　後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>俺の愛娘は悪役令嬢</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>かわもり かぐら(原作) ほづみりや(漫画) 縞(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第4話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>フルメタル・パニック！　Family</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>賀東招二(原作) 神反ヲ鬚(作画) 四季童子(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第6話　東京都江東区のタワマン39階②-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>双子の姉が神子として引き取られて、私は捨てられたけど多分私が神子である。</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>雪(著者) 池中織奈(原作) カット(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第32話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>TRPGプレイヤーが異世界で最強ビルドを目指す ～ヘンダーソン氏の福音を～</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>内田テモ(漫画) Schuld(原作) ランサネ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第14話</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>クロの戦記Ⅱ 異世界転移した僕が最強なのはベッドの上だけのようです</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>サイトウアユム(原作) ユリシロ(漫画) むつみまさと(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第22話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>ダークサモナーとデキている</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>車王(著者)</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>【コミックス第6巻発売記念】挟まるならどの衣装？コメント大募集！</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>ギルドを追放された回復術士、実は魔力無限だったので規格外の回復魔法で伝説となる</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>漫画：坂下コウ 原作：霞杏檎</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第4話(2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>チンチンデビルを追え！</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>くぼたふみお</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第３１話　激突！ アンとキュベレ！</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>俺の『鑑定』スキルがチートすぎて ～伝説の勇者を読み“盗り”最強へ～</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守　彩 漫画：龍牙 翔</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第33話ー③　迷宮の掃除番</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>異世界おじさん</t>
+          <t>クセ強彼女は床にいざなう</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>殆ど死んでいる(著者)</t>
+          <t>須河篤志(著者)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+          <t>第14話前半</t>
         </is>
       </c>
     </row>
@@ -28663,17 +29705,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+          <t>異世界のんびり農家</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>「名もなき英雄譚」後半</t>
+          <t>第302話</t>
         </is>
       </c>
     </row>
@@ -28683,17 +29725,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>淫獄団地</t>
+          <t>リビルドワールド</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第49話（前編）</t>
+          <t>第71話③</t>
         </is>
       </c>
     </row>
@@ -28703,17 +29745,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>まんきつしたい常連さん</t>
+          <t>氷結令嬢さまをフォローしたら、メチャメチャ溺愛されてしまった件@comic</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>しんみりん(著者)</t>
+          <t>漫画：ハレノチアメ 原作：愛坂タカト キャラクター原案：Bcoca</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第46話前編</t>
+          <t>第8話</t>
         </is>
       </c>
     </row>
@@ -28723,17 +29765,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
+          <t>ぽんドロイド！ はまさん</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
+          <t>はれやまはれぞう(著者)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第23話</t>
+          <t>第5話</t>
         </is>
       </c>
     </row>
@@ -28743,17 +29785,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>美人女上司滝沢さん</t>
+          <t>物語の黒幕に転生して</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>やんBARU(著者)</t>
+          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第202話</t>
+          <t>第32話</t>
         </is>
       </c>
     </row>
@@ -28763,17 +29805,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>よくわからないけれど異世界に転生していたようです</t>
+          <t>サーシャちゃんとクラスメイトオタクくん</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>内々けやき あし カオミン</t>
+          <t>はぐはぐ(著者)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第136話 よくわからないけれどスカウトされたみたいです（２）</t>
+          <t>第82話</t>
         </is>
       </c>
     </row>
@@ -28783,17 +29825,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+          <t>幼女戦記</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+          <t>東條チカ(漫画) カルロ・ゼン(原作) 篠月しのぶ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第80話その3</t>
+          <t>第百六章：ドードーバード航空戦Ⅰ</t>
         </is>
       </c>
     </row>
@@ -28803,17 +29845,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+          <t>三枝さんはメガネ先輩と恋を描く</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+          <t>セレビィ量産型(著者)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第71話(前編) ダリエルVS.滾り</t>
+          <t>第21話前半</t>
         </is>
       </c>
     </row>
@@ -28823,17 +29865,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+          <t>異世界おじさん</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>FUNA 東西 モトエ恵介</t>
+          <t>殆ど死んでいる(著者)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第120話　会談［その5］</t>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
@@ -28843,17 +29885,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>天獄で悪魔がボクを魅惑する</t>
+          <t>男子高校生だけどギャルにTSしました</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>銀河味めてお(著者)</t>
+          <t>太陽まりい(著者)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第34話</t>
+          <t>第18話後編</t>
         </is>
       </c>
     </row>
@@ -28863,17 +29905,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>ワンパンマン</t>
+          <t>モテはるねえ蘆屋くん</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>原作/ＯＮＥ 作画/村田雄介</t>
+          <t>栗原和明(原作) 寺井赤音(作画)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>206撃目</t>
+          <t>第16話前半</t>
         </is>
       </c>
     </row>
@@ -28883,17 +29925,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ずっと好きだった幼馴染と付き合い始めたら一途ビッチの性欲ジャンキーだったんだがどうすりゃいいですか？</t>
+          <t>田舎の黒ギャルJKと結婚しました</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>原作：トラ子猫 作画：あらいぐま</t>
+          <t>カヅチ(著者)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第3話</t>
+          <t>第17話後半</t>
         </is>
       </c>
     </row>
@@ -28903,17 +29945,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>冒険者絶対殺すダンジョン</t>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>道満晴明(著者)</t>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第34話</t>
+          <t>「名もなき英雄譚」後半</t>
         </is>
       </c>
     </row>
@@ -28923,17 +29965,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
+          <t>ミルク搾りハンターの異世界搾乳記～農家の冴えない男があらゆる種族の地区Bを弄び虜にする～</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>神原絵理華(漫画) 一森一輝(原作)</t>
+          <t>空詠大智(著者)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第18話②</t>
+          <t>第17話前半</t>
         </is>
       </c>
     </row>
@@ -28943,17 +29985,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>両親の借金を肩代わりしてもらう条件は日本一可愛い女子高生と一緒に暮らすことでした。</t>
+          <t>転生してあらゆるモノに好かれながら異世界で好きな事をして生きて行く</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>美月めいあ(漫画) 雨音恵(原作) ｋａｋａｏ(キャラクター原案)</t>
+          <t>都尾琉(漫画) 御峰。(原作)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第36話</t>
+          <t>第26話④</t>
         </is>
       </c>
     </row>
@@ -28963,17 +30005,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
+          <t>リアリスト魔王による聖域なき異世界改革</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
+          <t>鈴木マナツ(漫画) 羽田遼亮(原作) ゆーげん(キャラクターデザイン) ひたきゆう(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第75話 ゆめうつつ</t>
+          <t>第67幕③</t>
         </is>
       </c>
     </row>
@@ -28983,17 +30025,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>陰キャの僕に罰ゲームで告白してきたはずのギャルが、どう見ても僕にベタ惚れです</t>
+          <t>アラサーがVTuberになった話。</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>神奈なごみ(漫画) 結石(原作) かがちさく(キャラクター原案)</t>
+          <t>犬威赤彦(漫画) とくめい(原作) カラスBTK(キャラクター原案)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第26話</t>
+          <t>第24話</t>
         </is>
       </c>
     </row>
@@ -29003,17 +30045,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>修羅幼女の英雄譚～半端者と言われた傭兵、幼女に転生して成り上がる～</t>
+          <t>ずっと好きだった幼馴染と付き合い始めたら一途ビッチの性欲ジャンキーだったんだがどうすりゃいいですか？</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>作画：むらたん 原作：沙城流</t>
+          <t>原作：トラ子猫 作画：あらいぐま</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第7話(3)</t>
+          <t>第3話</t>
         </is>
       </c>
     </row>
@@ -29023,17 +30065,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>ゴリラ女子高生</t>
+          <t>ガルルガール</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>大友しゅうま(著者)</t>
+          <t>原聡志(著者)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+          <t>第15話</t>
         </is>
       </c>
     </row>
@@ -29043,17 +30085,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>王子様の友達</t>
+          <t>淫獄団地</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>すけろく(著者)</t>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+          <t>第49話（前編）</t>
         </is>
       </c>
     </row>
@@ -29063,17 +30105,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ラブコメと怪獣退治の不文律</t>
+          <t>まんきつしたい常連さん</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>御池慧（漫画） 上代務（原作） TMSLab（原作）</t>
+          <t>しんみりん(著者)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+          <t>第46話前編</t>
         </is>
       </c>
     </row>
@@ -29083,17 +30125,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>わたし、二番目の彼女でいいから。</t>
+          <t>愚かな天使は悪魔と踊る</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>にの子(漫画) 西条陽(原作) Re岳(キャラクター原案)</t>
+          <t>アズマサワヨシ(著者)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第10話③：カーテンのなか</t>
+          <t>第100話③</t>
         </is>
       </c>
     </row>
@@ -29103,17 +30145,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ヤンデレかと思ったらもっとヤベー女だった</t>
+          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>八木戸マト</t>
+          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第68話　全てを失ったヤンデレ彼女</t>
+          <t>第23話</t>
         </is>
       </c>
     </row>
@@ -29123,17 +30165,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>センパイ、自宅警備員の雇用はいかがですか？</t>
+          <t>王様ランキング200話～</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>漫画：コブラサナギ 原作：二上圭 キャラ原案：日向あずり</t>
+          <t>十日草輔（とおかそうすけ）</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第5話後半</t>
+          <t>第262話</t>
         </is>
       </c>
     </row>
@@ -29143,17 +30185,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>スキルがなければレベルを上げる～９９がカンストの世界でレベル800万からスタート～</t>
+          <t>よくわからないけれど異世界に転生していたようです</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>倉橋ユウス(漫画) 岡沢六十四(原作)</t>
+          <t>内々けやき あし カオミン</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第51話④</t>
+          <t>第136話 よくわからないけれどスカウトされたみたいです（２）</t>
         </is>
       </c>
     </row>
@@ -29163,17 +30205,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>時森さんが無防備です!!</t>
+          <t>美人女上司滝沢さん</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>たざわ</t>
+          <t>やんBARU(著者)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第63話</t>
+          <t>第202話</t>
         </is>
       </c>
     </row>
@@ -29183,17 +30225,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>不老不死少女の苗床旅行記</t>
+          <t>ワンパンマン</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ふじはん(漫画) ルナ・ウサギ(原作)</t>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第16話後編</t>
+          <t>206撃目</t>
         </is>
       </c>
     </row>
@@ -29203,17 +30245,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>くじ引き特賞：無双ハーレム権</t>
+          <t>ステータス・オール∞（インフィニティ） ∞使いの最強能力者、異世界を自由気ままに暮らします！</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>原作／三木なずな（GA文庫／SBクリエイティブ刊） 漫画／長谷見亮 キャラクター原案／瑠奈璃亜</t>
+          <t>漫画：三津屋みやこ 原作：八又ナガト</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第58話-02　新たな王女たちへ、受け継がれし慈愛の心！</t>
+          <t>第63話</t>
         </is>
       </c>
     </row>
@@ -29223,17 +30265,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>勇者のクズ</t>
+          <t>天獄で悪魔がボクを魅惑する</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>ナカシマ723</t>
+          <t>銀河味めてお(著者)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第48話　勇者の矜持 II（前半）</t>
+          <t>第34話</t>
         </is>
       </c>
     </row>
@@ -29243,17 +30285,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>漫画/すたひろ 原作/Y.A</t>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>chapter66【35話①】</t>
+          <t>第71話(前編) ダリエルVS.滾り</t>
         </is>
       </c>
     </row>
@@ -29263,17 +30305,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>断れない会長は友江くんにだけしてあげたい</t>
+          <t>本物のカノジョにしたくなるまで、私で試していいよ。</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>沼地どろまる(著者)</t>
+          <t>wano(漫画) 有丈ほえる(原作) 緋月ひぐれ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>休載漫画</t>
+          <t>第8話②</t>
         </is>
       </c>
     </row>
@@ -29283,17 +30325,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ダウナーお姉さんは遊びたい</t>
+          <t>異種族追放コンカフェ</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>山鷹景</t>
+          <t>佐々木マサヒト(著者)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第15話</t>
+          <t>第17話</t>
         </is>
       </c>
     </row>
@@ -29303,17 +30345,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>聖騎士になったけど団長のおっぱいが凄すぎて心が清められない</t>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>木の芽(原作) 川喜田ミツオ(漫画) 雨傘ゆん(キャラクター原案)</t>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>コミックス6巻発売＆休載のお知らせ</t>
+          <t>第80話その3</t>
         </is>
       </c>
     </row>
@@ -29323,17 +30365,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>脱稿するまでオチません</t>
+          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>ヨシラギ(著者)</t>
+          <t>FUNA 東西 モトエ恵介</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第32話後半</t>
+          <t>第120話　会談［その5］</t>
         </is>
       </c>
     </row>
@@ -29343,17 +30385,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>勇者パーティから追い出された不遇職【罠士】、ユニークスキル【矢印】で最強になる</t>
+          <t>おっさん、転生して天才役者になる</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>作画：たつひこ 原作：白石 有希</t>
+          <t>芽々ノ圭(漫画) ほえ太郎(原作)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第7話(3)</t>
+          <t>第37話③</t>
         </is>
       </c>
     </row>
@@ -29363,17 +30405,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>クラスの大嫌いな女子と結婚することになった。</t>
+          <t>ラスボスたちの隠し仔　～魔王城に転生した元社畜プログラマーは自由気ままに『魔導言語《マジックコード》』を開発する～</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>天乃聖樹(原作) もすこんぶ(漫画)</t>
+          <t>森清士郎(漫画) 熊乃げん骨(原作)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第44話-2</t>
+          <t>第14話②</t>
         </is>
       </c>
     </row>
@@ -29383,17 +30425,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>隣のクーデレラを甘やかしたら、ウチの合鍵を渡すことになった</t>
+          <t>母をたずねて、異世界に。</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>青島かなえ(漫画) 雪仁(原作) かがちさく(キャラクター原案)</t>
+          <t>藤原 祐(原作) 吉北ぽぷり(漫画) しの(キャラクター原案)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第38話</t>
+          <t>コミックス2巻発売告知</t>
         </is>
       </c>
     </row>
@@ -29403,17 +30445,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>りんちゃんは据え膳したい</t>
+          <t>ケロロ軍曹</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>澄田佑貴(著者)</t>
+          <t>吉崎観音(著者)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第38話</t>
+          <t>第355話　さらば、もう一人の桃華…の巻</t>
         </is>
       </c>
     </row>
@@ -29423,17 +30465,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>ボクの理想の異世界生活 ～転生したらケモ耳娘だらけの世界でハーレムに～</t>
+          <t>両親の借金を肩代わりしてもらう条件は日本一可愛い女子高生と一緒に暮らすことでした。</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>イチリ(原作) 空維深夜(作画)</t>
+          <t>美月めいあ(漫画) 雨音恵(原作) ｋａｋａｏ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第15話前半：CALL</t>
+          <t>第36話</t>
         </is>
       </c>
     </row>
@@ -29443,17 +30485,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>その冒険者、取り扱い注意。 ～正体は無敵の下僕たちを統べる異世界最強の魔導王～</t>
+          <t>わたし、二番目の彼女でいいから。</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>満月シオン(作画) Sin Guilty(ツギクル)(原作) M.B(キャラクター原案)</t>
+          <t>にの子(漫画) 西条陽(原作) Re岳(キャラクター原案)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>56章　はじまりの愚か者②　後編</t>
+          <t>第10話③：カーテンのなか</t>
         </is>
       </c>
     </row>
@@ -29463,17 +30505,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>俺の愛娘は悪役令嬢</t>
+          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>かわもり かぐら(原作) ほづみりや(漫画) 縞(キャラクター原案)</t>
+          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第4話-2</t>
+          <t>第75話 ゆめうつつ</t>
         </is>
       </c>
     </row>
@@ -29483,17 +30525,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>フルメタル・パニック！　Family</t>
+          <t>Dジェネシス　ダンジョンが出来て３年</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>賀東招二(原作) 神反ヲ鬚(作画) 四季童子(キャラクター原案)</t>
+          <t>平未夜(漫画) 之貫紀(原作) ttl(キャラクター原案)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第6話　東京都江東区のタワマン39階②-2</t>
+          <t>#3③</t>
         </is>
       </c>
     </row>
@@ -29503,17 +30545,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>双子の姉が神子として引き取られて、私は捨てられたけど多分私が神子である。</t>
+          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>雪(著者) 池中織奈(原作) カット(キャラクター原案)</t>
+          <t>神原絵理華(漫画) 一森一輝(原作)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第32話後編</t>
+          <t>第18話②</t>
         </is>
       </c>
     </row>
@@ -29523,17 +30565,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>TRPGプレイヤーが異世界で最強ビルドを目指す ～ヘンダーソン氏の福音を～</t>
+          <t>魔物喰らい ランキング最下位の冒険者は魔物の力で最強へ</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>内田テモ(漫画) Schuld(原作) ランサネ(キャラクター原案)</t>
+          <t>赤井ハコ(漫画) 緒二葉(原作) とよた瑣織(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第14話</t>
+          <t>第9話-1</t>
         </is>
       </c>
     </row>
@@ -29543,17 +30585,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>クロの戦記Ⅱ 異世界転移した僕が最強なのはベッドの上だけのようです</t>
+          <t>陰キャの僕に罰ゲームで告白してきたはずのギャルが、どう見ても僕にベタ惚れです</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>サイトウアユム(原作) ユリシロ(漫画) むつみまさと(キャラクター原案)</t>
+          <t>神奈なごみ(漫画) 結石(原作) かがちさく(キャラクター原案)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第22話-2</t>
+          <t>第26話</t>
         </is>
       </c>
     </row>
@@ -29563,17 +30605,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>ダークサモナーとデキている</t>
+          <t>人外教室の人間嫌い教師 ヒトマ先生、私たちに人間を教えてくれますか……？</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>車王(著者)</t>
+          <t>紅野あつ(漫画) 来栖夏芽(原作) 泉彩(キャラクター原案)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>【コミックス第6巻発売記念】挟まるならどの衣装？コメント大募集！</t>
+          <t>第28話（後半）</t>
         </is>
       </c>
     </row>
@@ -29583,17 +30625,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ギルドを追放された回復術士、実は魔力無限だったので規格外の回復魔法で伝説となる</t>
+          <t>冒険者絶対殺すダンジョン</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>漫画：坂下コウ 原作：霞杏檎</t>
+          <t>道満晴明(著者)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第4話(2)</t>
+          <t>第34話</t>
         </is>
       </c>
     </row>
@@ -29603,17 +30645,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>チンチンデビルを追え！</t>
+          <t>不老不死少女の苗床旅行記</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>くぼたふみお</t>
+          <t>ふじはん(漫画) ルナ・ウサギ(原作)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第３１話　激突！ アンとキュベレ！</t>
+          <t>第16話後編</t>
         </is>
       </c>
     </row>
@@ -29623,17 +30665,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>俺の『鑑定』スキルがチートすぎて ～伝説の勇者を読み“盗り”最強へ～</t>
+          <t>センパイ、自宅警備員の雇用はいかがですか？</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>原作：澄守　彩 漫画：龍牙 翔</t>
+          <t>漫画：コブラサナギ 原作：二上圭 キャラ原案：日向あずり</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第33話ー③　迷宮の掃除番</t>
+          <t>第5話後半</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-07-28
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -42,6 +42,7 @@
     <sheet name="2025-07-25" sheetId="34" state="visible" r:id="rId34"/>
     <sheet name="2025-07-26" sheetId="35" state="visible" r:id="rId35"/>
     <sheet name="2025-07-27" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="2025-07-28" sheetId="37" state="visible" r:id="rId37"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -29680,22 +29681,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>クセ強彼女は床にいざなう</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>須河篤志(著者)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第14話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>異世界のんびり農家</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第302話</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第71話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>氷結令嬢さまをフォローしたら、メチャメチャ溺愛されてしまった件@comic</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>漫画：ハレノチアメ 原作：愛坂タカト キャラクター原案：Bcoca</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第8話</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>ぽんドロイド！ はまさん</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>はれやまはれぞう(著者)</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>物語の黒幕に転生して</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第32話</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>サーシャちゃんとクラスメイトオタクくん</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>はぐはぐ(著者)</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第82話</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>幼女戦記</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>東條チカ(漫画) カルロ・ゼン(原作) 篠月しのぶ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第百六章：ドードーバード航空戦Ⅰ</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>三枝さんはメガネ先輩と恋を描く</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>セレビィ量産型(著者)</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第21話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>異世界おじさん</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>殆ど死んでいる(著者)</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>男子高校生だけどギャルにTSしました</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>太陽まりい(著者)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第18話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>モテはるねえ蘆屋くん</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>栗原和明(原作) 寺井赤音(作画)</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第16話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>田舎の黒ギャルJKと結婚しました</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>カヅチ(著者)</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第17話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>「名もなき英雄譚」後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>ミルク搾りハンターの異世界搾乳記～農家の冴えない男があらゆる種族の地区Bを弄び虜にする～</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>空詠大智(著者)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第17話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>転生してあらゆるモノに好かれながら異世界で好きな事をして生きて行く</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>都尾琉(漫画) 御峰。(原作)</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第26話④</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>リアリスト魔王による聖域なき異世界改革</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>鈴木マナツ(漫画) 羽田遼亮(原作) ゆーげん(キャラクターデザイン) ひたきゆう(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第67幕③</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>アラサーがVTuberになった話。</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>犬威赤彦(漫画) とくめい(原作) カラスBTK(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第24話</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>ずっと好きだった幼馴染と付き合い始めたら一途ビッチの性欲ジャンキーだったんだがどうすりゃいいですか？</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>原作：トラ子猫 作画：あらいぐま</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第3話</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>ガルルガール</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>原聡志(著者)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第15話</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>淫獄団地</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第49話（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>まんきつしたい常連さん</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>しんみりん(著者)</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第46話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>愚かな天使は悪魔と踊る</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>アズマサワヨシ(著者)</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第100話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第23話</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>王様ランキング200話～</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>十日草輔（とおかそうすけ）</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第262話</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第136話 よくわからないけれどスカウトされたみたいです（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>美人女上司滝沢さん</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>やんBARU(著者)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第202話</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>ワンパンマン</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>206撃目</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>ステータス・オール∞（インフィニティ） ∞使いの最強能力者、異世界を自由気ままに暮らします！</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>漫画：三津屋みやこ 原作：八又ナガト</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第63話</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>天獄で悪魔がボクを魅惑する</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>銀河味めてお(著者)</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第34話</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第71話(前編) ダリエルVS.滾り</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>本物のカノジョにしたくなるまで、私で試していいよ。</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>wano(漫画) 有丈ほえる(原作) 緋月ひぐれ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第8話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>異種族追放コンカフェ</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>佐々木マサヒト(著者)</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第17話</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第80話その3</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>FUNA 東西 モトエ恵介</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第120話　会談［その5］</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>おっさん、転生して天才役者になる</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>芽々ノ圭(漫画) ほえ太郎(原作)</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第37話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>ラスボスたちの隠し仔　～魔王城に転生した元社畜プログラマーは自由気ままに『魔導言語《マジックコード》』を開発する～</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>森清士郎(漫画) 熊乃げん骨(原作)</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第14話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>母をたずねて、異世界に。</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>藤原 祐(原作) 吉北ぽぷり(漫画) しの(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>コミックス2巻発売告知</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>ケロロ軍曹</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>吉崎観音(著者)</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第355話　さらば、もう一人の桃華…の巻</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>両親の借金を肩代わりしてもらう条件は日本一可愛い女子高生と一緒に暮らすことでした。</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>美月めいあ(漫画) 雨音恵(原作) ｋａｋａｏ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第36話</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>わたし、二番目の彼女でいいから。</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>にの子(漫画) 西条陽(原作) Re岳(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第10話③：カーテンのなか</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第75話 ゆめうつつ</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>Dジェネシス　ダンジョンが出来て３年</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>平未夜(漫画) 之貫紀(原作) ttl(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>#3③</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>神原絵理華(漫画) 一森一輝(原作)</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第18話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>魔物喰らい ランキング最下位の冒険者は魔物の力で最強へ</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>赤井ハコ(漫画) 緒二葉(原作) とよた瑣織(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第9話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>陰キャの僕に罰ゲームで告白してきたはずのギャルが、どう見ても僕にベタ惚れです</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>神奈なごみ(漫画) 結石(原作) かがちさく(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第26話</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>人外教室の人間嫌い教師 ヒトマ先生、私たちに人間を教えてくれますか……？</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>紅野あつ(漫画) 来栖夏芽(原作) 泉彩(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第28話（後半）</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>冒険者絶対殺すダンジョン</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>道満晴明(著者)</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第34話</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>不老不死少女の苗床旅行記</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>ふじはん(漫画) ルナ・ウサギ(原作)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第16話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>センパイ、自宅警備員の雇用はいかがですか？</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>漫画：コブラサナギ 原作：二上圭 キャラ原案：日向あずり</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第5話後半</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>クセ強彼女は床にいざなう</t>
+          <t>魔術師クノンは見えている</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>須河篤志(著者)</t>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第14話前半</t>
+          <t>第39話①</t>
         </is>
       </c>
     </row>
@@ -29705,17 +30747,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>異世界のんびり農家</t>
+          <t>ダンジョンの幼なじみ</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+          <t>久真やすひさ(著者)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第302話</t>
+          <t>お休みイラスト</t>
         </is>
       </c>
     </row>
@@ -29725,17 +30767,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>リビルドワールド</t>
+          <t>モブ高生の俺でも冒険者になればリア充になれますか？</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+          <t>原作：百均 漫画：さぎやまれん キャラクター原案：hai</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第71話③</t>
+          <t>第30話</t>
         </is>
       </c>
     </row>
@@ -29745,17 +30787,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>氷結令嬢さまをフォローしたら、メチャメチャ溺愛されてしまった件@comic</t>
+          <t>クセ強彼女は床にいざなう</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>漫画：ハレノチアメ 原作：愛坂タカト キャラクター原案：Bcoca</t>
+          <t>須河篤志(著者)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第8話</t>
+          <t>第14話前半</t>
         </is>
       </c>
     </row>
@@ -29765,17 +30807,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ぽんドロイド！ はまさん</t>
+          <t>悪役令嬢、俺</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>はれやまはれぞう(著者)</t>
+          <t>弥南せいら(漫画) 猫屋敷のあ(原作)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第5話</t>
+          <t>第1話</t>
         </is>
       </c>
     </row>
@@ -29785,17 +30827,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>物語の黒幕に転生して</t>
+          <t>異世界のんびり農家</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第32話</t>
+          <t>第302話</t>
         </is>
       </c>
     </row>
@@ -29805,17 +30847,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>サーシャちゃんとクラスメイトオタクくん</t>
+          <t>氷結令嬢さまをフォローしたら、メチャメチャ溺愛されてしまった件@comic</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>はぐはぐ(著者)</t>
+          <t>漫画：ハレノチアメ 原作：愛坂タカト キャラクター原案：Bcoca</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第82話</t>
+          <t>第8話</t>
         </is>
       </c>
     </row>
@@ -29825,17 +30867,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>幼女戦記</t>
+          <t>ぽんドロイド！ はまさん</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>東條チカ(漫画) カルロ・ゼン(原作) 篠月しのぶ(キャラクター原案)</t>
+          <t>はれやまはれぞう(著者)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第百六章：ドードーバード航空戦Ⅰ</t>
+          <t>第5話</t>
         </is>
       </c>
     </row>
@@ -29845,17 +30887,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>三枝さんはメガネ先輩と恋を描く</t>
+          <t>はずれスキル念動力（ただしレベルＭＡＸ）で無双する～手をかざすだけです。詠唱とか必殺技とかいりません。念じるだけで倒せます～</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>セレビィ量産型(著者)</t>
+          <t>さとう うなぽっぽ トダフミト</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第21話前半</t>
+          <t>9話③</t>
         </is>
       </c>
     </row>
@@ -29885,17 +30927,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>男子高校生だけどギャルにTSしました</t>
+          <t>物語の黒幕に転生して</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>太陽まりい(著者)</t>
+          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第18話後編</t>
+          <t>第32話</t>
         </is>
       </c>
     </row>
@@ -29905,17 +30947,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>モテはるねえ蘆屋くん</t>
+          <t>リビルドワールド</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>栗原和明(原作) 寺井赤音(作画)</t>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第16話前半</t>
+          <t>第71話③</t>
         </is>
       </c>
     </row>
@@ -29925,17 +30967,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>田舎の黒ギャルJKと結婚しました</t>
+          <t>転生貴族の異世界冒険録 ～カインのやりすぎギルド日記～</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>カヅチ(著者)</t>
+          <t>原作：夜州 漫画：佐々木あかね・香本セトラ キャラクター原案：藻</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第17話後半</t>
+          <t>第48話</t>
         </is>
       </c>
     </row>
@@ -29945,17 +30987,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+          <t>サーシャちゃんとクラスメイトオタクくん</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+          <t>はぐはぐ(著者)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>「名もなき英雄譚」後半</t>
+          <t>第82話</t>
         </is>
       </c>
     </row>
@@ -29965,17 +31007,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ミルク搾りハンターの異世界搾乳記～農家の冴えない男があらゆる種族の地区Bを弄び虜にする～</t>
+          <t>幼女戦記</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>空詠大智(著者)</t>
+          <t>東條チカ(漫画) カルロ・ゼン(原作) 篠月しのぶ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第17話前半</t>
+          <t>第百六章：ドードーバード航空戦Ⅰ</t>
         </is>
       </c>
     </row>
@@ -29985,17 +31027,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>転生してあらゆるモノに好かれながら異世界で好きな事をして生きて行く</t>
+          <t>俺だけ使える古代魔法 ～基礎すら使えないと追放された俺の魔法は、実は1万年前に失われた伝説魔法でした～</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>都尾琉(漫画) 御峰。(原作)</t>
+          <t>原作／アトハ 漫画／川上ニナ キャラクター原案／片倉響</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第26話④</t>
+          <t>第15話</t>
         </is>
       </c>
     </row>
@@ -30005,17 +31047,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>リアリスト魔王による聖域なき異世界改革</t>
+          <t>ナナシの器用貧乏</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>鈴木マナツ(漫画) 羽田遼亮(原作) ゆーげん(キャラクターデザイン) ひたきゆう(キャラクターデザイン)</t>
+          <t>原作：高球 漫画：葉原辰月 キャラクター原案：KeG</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第67幕③</t>
+          <t>第5話</t>
         </is>
       </c>
     </row>
@@ -30025,17 +31067,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>アラサーがVTuberになった話。</t>
+          <t>男子高校生だけどギャルにTSしました</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>犬威赤彦(漫画) とくめい(原作) カラスBTK(キャラクター原案)</t>
+          <t>太陽まりい(著者)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第24話</t>
+          <t>第18話後編</t>
         </is>
       </c>
     </row>
@@ -30045,17 +31087,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ずっと好きだった幼馴染と付き合い始めたら一途ビッチの性欲ジャンキーだったんだがどうすりゃいいですか？</t>
+          <t>田舎の黒ギャルJKと結婚しました</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>原作：トラ子猫 作画：あらいぐま</t>
+          <t>カヅチ(著者)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第3話</t>
+          <t>第17話後半</t>
         </is>
       </c>
     </row>
@@ -30065,17 +31107,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>ガルルガール</t>
+          <t>三枝さんはメガネ先輩と恋を描く</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>原聡志(著者)</t>
+          <t>セレビィ量産型(著者)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第15話</t>
+          <t>第21話前半</t>
         </is>
       </c>
     </row>
@@ -30085,17 +31127,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>淫獄団地</t>
+          <t>モテはるねえ蘆屋くん</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+          <t>栗原和明(原作) 寺井赤音(作画)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第49話（前編）</t>
+          <t>第16話前半</t>
         </is>
       </c>
     </row>
@@ -30105,17 +31147,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>まんきつしたい常連さん</t>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>しんみりん(著者)</t>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第46話前編</t>
+          <t>「名もなき英雄譚」後半</t>
         </is>
       </c>
     </row>
@@ -30125,17 +31167,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>愚かな天使は悪魔と踊る</t>
+          <t>ゆーち〇ーばー</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>アズマサワヨシ(著者)</t>
+          <t>ともお</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第100話③</t>
+          <t>第1話</t>
         </is>
       </c>
     </row>
@@ -30145,17 +31187,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
+          <t>ワンパンマン</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第23話</t>
+          <t>206撃目</t>
         </is>
       </c>
     </row>
@@ -30165,17 +31207,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>王様ランキング200話～</t>
+          <t>魔王令嬢の教育係 ～勇者学院を追放された平民教師は魔王の娘たちの家庭教師となる～</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>十日草輔（とおかそうすけ）</t>
+          <t>原作：新人 漫画：松原剛 キャラクター原案：巻羊</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第262話</t>
+          <t>第29話</t>
         </is>
       </c>
     </row>
@@ -30185,17 +31227,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>よくわからないけれど異世界に転生していたようです</t>
+          <t>淫獄団地</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>内々けやき あし カオミン</t>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第136話 よくわからないけれどスカウトされたみたいです（２）</t>
+          <t>第49話（前編）</t>
         </is>
       </c>
     </row>
@@ -30205,17 +31247,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>美人女上司滝沢さん</t>
+          <t>ミルク搾りハンターの異世界搾乳記～農家の冴えない男があらゆる種族の地区Bを弄び虜にする～</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>やんBARU(著者)</t>
+          <t>空詠大智(著者)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第202話</t>
+          <t>第17話前半</t>
         </is>
       </c>
     </row>
@@ -30225,17 +31267,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ワンパンマン</t>
+          <t>まんきつしたい常連さん</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>原作/ＯＮＥ 作画/村田雄介</t>
+          <t>しんみりん(著者)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>206撃目</t>
+          <t>第46話前編</t>
         </is>
       </c>
     </row>
@@ -30245,17 +31287,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ステータス・オール∞（インフィニティ） ∞使いの最強能力者、異世界を自由気ままに暮らします！</t>
+          <t>ソードアート・オンライン Re:Aincrad</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>漫画：三津屋みやこ 原作：八又ナガト</t>
+          <t>樹深(作画) 佐藤ミト(構成) 川原礫(原作) ａｂｅｃ(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第63話</t>
+          <t>第40話②</t>
         </is>
       </c>
     </row>
@@ -30265,17 +31307,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>天獄で悪魔がボクを魅惑する</t>
+          <t>よくわからないけれど異世界に転生していたようです</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>銀河味めてお(著者)</t>
+          <t>内々けやき あし カオミン</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第34話</t>
+          <t>第136話 よくわからないけれどスカウトされたみたいです（２）</t>
         </is>
       </c>
     </row>
@@ -30285,17 +31327,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+          <t>リアリスト魔王による聖域なき異世界改革</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+          <t>鈴木マナツ(漫画) 羽田遼亮(原作) ゆーげん(キャラクターデザイン) ひたきゆう(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第71話(前編) ダリエルVS.滾り</t>
+          <t>第67幕③</t>
         </is>
       </c>
     </row>
@@ -30305,17 +31347,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>本物のカノジョにしたくなるまで、私で試していいよ。</t>
+          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>wano(漫画) 有丈ほえる(原作) 緋月ひぐれ(キャラクター原案)</t>
+          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第8話②</t>
+          <t>第23話</t>
         </is>
       </c>
     </row>
@@ -30325,17 +31367,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>異種族追放コンカフェ</t>
+          <t>ガルルガール</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>佐々木マサヒト(著者)</t>
+          <t>原聡志(著者)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第17話</t>
+          <t>第15話</t>
         </is>
       </c>
     </row>
@@ -30345,17 +31387,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+          <t>最強ギフトで領地経営スローライフ ～辺境の村を開拓していたら英雄級の人材がわんさかやってきた！～</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+          <t>原作：音速炒飯 漫画：眠田瞼 キャラクター原案：riritto</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第80話その3</t>
+          <t>第28話</t>
         </is>
       </c>
     </row>
@@ -30365,17 +31407,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+          <t>アラサーがVTuberになった話。</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>FUNA 東西 モトエ恵介</t>
+          <t>犬威赤彦(漫画) とくめい(原作) カラスBTK(キャラクター原案)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第120話　会談［その5］</t>
+          <t>第24話</t>
         </is>
       </c>
     </row>
@@ -30385,17 +31427,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>おっさん、転生して天才役者になる</t>
+          <t>美人女上司滝沢さん</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>芽々ノ圭(漫画) ほえ太郎(原作)</t>
+          <t>やんBARU(著者)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第37話③</t>
+          <t>第202話</t>
         </is>
       </c>
     </row>
@@ -30405,17 +31447,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ラスボスたちの隠し仔　～魔王城に転生した元社畜プログラマーは自由気ままに『魔導言語《マジックコード》』を開発する～</t>
+          <t>転生してあらゆるモノに好かれながら異世界で好きな事をして生きて行く</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>森清士郎(漫画) 熊乃げん骨(原作)</t>
+          <t>都尾琉(漫画) 御峰。(原作)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第14話②</t>
+          <t>第26話④</t>
         </is>
       </c>
     </row>
@@ -30425,17 +31467,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>母をたずねて、異世界に。</t>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>藤原 祐(原作) 吉北ぽぷり(漫画) しの(キャラクター原案)</t>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>コミックス2巻発売告知</t>
+          <t>第71話(前編) ダリエルVS.滾り</t>
         </is>
       </c>
     </row>
@@ -30445,17 +31487,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>ケロロ軍曹</t>
+          <t>天獄で悪魔がボクを魅惑する</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>吉崎観音(著者)</t>
+          <t>銀河味めてお(著者)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第355話　さらば、もう一人の桃華…の巻</t>
+          <t>第34話</t>
         </is>
       </c>
     </row>
@@ -30465,17 +31507,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>両親の借金を肩代わりしてもらう条件は日本一可愛い女子高生と一緒に暮らすことでした。</t>
+          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>美月めいあ(漫画) 雨音恵(原作) ｋａｋａｏ(キャラクター原案)</t>
+          <t>FUNA 東西 モトエ恵介</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第36話</t>
+          <t>第120話　会談［その5］</t>
         </is>
       </c>
     </row>
@@ -30485,17 +31527,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>わたし、二番目の彼女でいいから。</t>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>にの子(漫画) 西条陽(原作) Re岳(キャラクター原案)</t>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第10話③：カーテンのなか</t>
+          <t>第80話その3</t>
         </is>
       </c>
     </row>
@@ -30505,17 +31547,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
+          <t>王様ランキング200話～</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
+          <t>十日草輔（とおかそうすけ）</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第75話 ゆめうつつ</t>
+          <t>第262話</t>
         </is>
       </c>
     </row>
@@ -30525,17 +31567,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Dジェネシス　ダンジョンが出来て３年</t>
+          <t>愚かな天使は悪魔と踊る</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>平未夜(漫画) 之貫紀(原作) ttl(キャラクター原案)</t>
+          <t>アズマサワヨシ(著者)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>#3③</t>
+          <t>第100話③</t>
         </is>
       </c>
     </row>
@@ -30545,17 +31587,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
+          <t>ひびワれこうじつ</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>神原絵理華(漫画) 一森一輝(原作)</t>
+          <t>ぺろぽねそす(著者)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第18話②</t>
+          <t>第1話</t>
         </is>
       </c>
     </row>
@@ -30565,17 +31607,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>魔物喰らい ランキング最下位の冒険者は魔物の力で最強へ</t>
+          <t>ずっと好きだった幼馴染と付き合い始めたら一途ビッチの性欲ジャンキーだったんだがどうすりゃいいですか？</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>赤井ハコ(漫画) 緒二葉(原作) とよた瑣織(キャラクターデザイン)</t>
+          <t>原作：トラ子猫 作画：あらいぐま</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第9話-1</t>
+          <t>第3話</t>
         </is>
       </c>
     </row>
@@ -30585,17 +31627,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>陰キャの僕に罰ゲームで告白してきたはずのギャルが、どう見ても僕にベタ惚れです</t>
+          <t>転生前はドラゴンでした</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>神奈なごみ(漫画) 結石(原作) かがちさく(キャラクター原案)</t>
+          <t>甘井ヤドラキ</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第26話</t>
+          <t>第44話+お知らせ</t>
         </is>
       </c>
     </row>
@@ -30605,17 +31647,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>人外教室の人間嫌い教師 ヒトマ先生、私たちに人間を教えてくれますか……？</t>
+          <t>両親の借金を肩代わりしてもらう条件は日本一可愛い女子高生と一緒に暮らすことでした。</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>紅野あつ(漫画) 来栖夏芽(原作) 泉彩(キャラクター原案)</t>
+          <t>美月めいあ(漫画) 雨音恵(原作) ｋａｋａｏ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第28話（後半）</t>
+          <t>第36話</t>
         </is>
       </c>
     </row>
@@ -30625,17 +31667,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>冒険者絶対殺すダンジョン</t>
+          <t>本物のカノジョにしたくなるまで、私で試していいよ。</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>道満晴明(著者)</t>
+          <t>wano(漫画) 有丈ほえる(原作) 緋月ひぐれ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第34話</t>
+          <t>第8話②</t>
         </is>
       </c>
     </row>
@@ -30645,17 +31687,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>不老不死少女の苗床旅行記</t>
+          <t>わたし、二番目の彼女でいいから。</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>ふじはん(漫画) ルナ・ウサギ(原作)</t>
+          <t>にの子(漫画) 西条陽(原作) Re岳(キャラクター原案)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第16話後編</t>
+          <t>第10話③：カーテンのなか</t>
         </is>
       </c>
     </row>
@@ -30665,17 +31707,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>センパイ、自宅警備員の雇用はいかがですか？</t>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>漫画：コブラサナギ 原作：二上圭 キャラ原案：日向あずり</t>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第5話後半</t>
+          <t>第34話①</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-07-29
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -43,6 +43,7 @@
     <sheet name="2025-07-26" sheetId="35" state="visible" r:id="rId35"/>
     <sheet name="2025-07-27" sheetId="36" state="visible" r:id="rId36"/>
     <sheet name="2025-07-28" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="2025-07-29" sheetId="38" state="visible" r:id="rId38"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -30722,22 +30723,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>魔術師クノンは見えている</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第39話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>ダンジョンの幼なじみ</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>久真やすひさ(著者)</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>お休みイラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>モブ高生の俺でも冒険者になればリア充になれますか？</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>原作：百均 漫画：さぎやまれん キャラクター原案：hai</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第30話</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>クセ強彼女は床にいざなう</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>須河篤志(著者)</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第14話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>悪役令嬢、俺</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>弥南せいら(漫画) 猫屋敷のあ(原作)</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第1話</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>異世界のんびり農家</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第302話</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>氷結令嬢さまをフォローしたら、メチャメチャ溺愛されてしまった件@comic</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>漫画：ハレノチアメ 原作：愛坂タカト キャラクター原案：Bcoca</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第8話</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>ぽんドロイド！ はまさん</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>はれやまはれぞう(著者)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>はずれスキル念動力（ただしレベルＭＡＸ）で無双する～手をかざすだけです。詠唱とか必殺技とかいりません。念じるだけで倒せます～</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>さとう うなぽっぽ トダフミト</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>9話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>異世界おじさん</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>殆ど死んでいる(著者)</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>物語の黒幕に転生して</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第32話</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第71話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>転生貴族の異世界冒険録 ～カインのやりすぎギルド日記～</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>原作：夜州 漫画：佐々木あかね・香本セトラ キャラクター原案：藻</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第48話</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>サーシャちゃんとクラスメイトオタクくん</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>はぐはぐ(著者)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第82話</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>幼女戦記</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>東條チカ(漫画) カルロ・ゼン(原作) 篠月しのぶ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第百六章：ドードーバード航空戦Ⅰ</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>俺だけ使える古代魔法 ～基礎すら使えないと追放された俺の魔法は、実は1万年前に失われた伝説魔法でした～</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>原作／アトハ 漫画／川上ニナ キャラクター原案／片倉響</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第15話</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>ナナシの器用貧乏</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>原作：高球 漫画：葉原辰月 キャラクター原案：KeG</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>男子高校生だけどギャルにTSしました</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>太陽まりい(著者)</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第18話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>田舎の黒ギャルJKと結婚しました</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>カヅチ(著者)</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第17話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>三枝さんはメガネ先輩と恋を描く</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>セレビィ量産型(著者)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第21話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>モテはるねえ蘆屋くん</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>栗原和明(原作) 寺井赤音(作画)</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第16話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>「名もなき英雄譚」後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>ゆーち〇ーばー</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>ともお</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第1話</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>ワンパンマン</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>206撃目</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>魔王令嬢の教育係 ～勇者学院を追放された平民教師は魔王の娘たちの家庭教師となる～</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>原作：新人 漫画：松原剛 キャラクター原案：巻羊</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第29話</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>淫獄団地</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第49話（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>ミルク搾りハンターの異世界搾乳記～農家の冴えない男があらゆる種族の地区Bを弄び虜にする～</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>空詠大智(著者)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第17話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>まんきつしたい常連さん</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>しんみりん(著者)</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第46話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>ソードアート・オンライン Re:Aincrad</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>樹深(作画) 佐藤ミト(構成) 川原礫(原作) ａｂｅｃ(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第40話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第136話 よくわからないけれどスカウトされたみたいです（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>リアリスト魔王による聖域なき異世界改革</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>鈴木マナツ(漫画) 羽田遼亮(原作) ゆーげん(キャラクターデザイン) ひたきゆう(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第67幕③</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第23話</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>ガルルガール</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>原聡志(著者)</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第15話</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>最強ギフトで領地経営スローライフ ～辺境の村を開拓していたら英雄級の人材がわんさかやってきた！～</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>原作：音速炒飯 漫画：眠田瞼 キャラクター原案：riritto</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第28話</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>アラサーがVTuberになった話。</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>犬威赤彦(漫画) とくめい(原作) カラスBTK(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第24話</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>美人女上司滝沢さん</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>やんBARU(著者)</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第202話</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>転生してあらゆるモノに好かれながら異世界で好きな事をして生きて行く</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>都尾琉(漫画) 御峰。(原作)</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第26話④</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第71話(前編) ダリエルVS.滾り</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>天獄で悪魔がボクを魅惑する</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>銀河味めてお(著者)</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第34話</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>FUNA 東西 モトエ恵介</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第120話　会談［その5］</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第80話その3</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>王様ランキング200話～</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>十日草輔（とおかそうすけ）</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第262話</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>愚かな天使は悪魔と踊る</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>アズマサワヨシ(著者)</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第100話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>ひびワれこうじつ</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>ぺろぽねそす(著者)</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第1話</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>ずっと好きだった幼馴染と付き合い始めたら一途ビッチの性欲ジャンキーだったんだがどうすりゃいいですか？</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>原作：トラ子猫 作画：あらいぐま</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第3話</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>転生前はドラゴンでした</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>甘井ヤドラキ</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第44話+お知らせ</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>両親の借金を肩代わりしてもらう条件は日本一可愛い女子高生と一緒に暮らすことでした。</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>美月めいあ(漫画) 雨音恵(原作) ｋａｋａｏ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第36話</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>本物のカノジョにしたくなるまで、私で試していいよ。</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>wano(漫画) 有丈ほえる(原作) 緋月ひぐれ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第8話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>わたし、二番目の彼女でいいから。</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>にの子(漫画) 西条陽(原作) Re岳(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第10話③：カーテンのなか</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第34話①</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>魔術師クノンは見えている</t>
+          <t>帰ってください！ 阿久津さん</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+          <t>長岡太一(著者)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第39話①</t>
+          <t>第193話</t>
         </is>
       </c>
     </row>
@@ -30747,17 +31789,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ダンジョンの幼なじみ</t>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>久真やすひさ(著者)</t>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>お休みイラスト</t>
+          <t>第５０話　雌雄を決する器用貧乏（４）</t>
         </is>
       </c>
     </row>
@@ -30767,17 +31809,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>モブ高生の俺でも冒険者になればリア充になれますか？</t>
+          <t>姫ヶ崎櫻子は今日も不憫可愛い</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>原作：百均 漫画：さぎやまれん キャラクター原案：hai</t>
+          <t>安田剛助(著者)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第30話</t>
+          <t>第49話</t>
         </is>
       </c>
     </row>
@@ -30787,17 +31829,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>クセ強彼女は床にいざなう</t>
+          <t>「おかえり、パパ」</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>須河篤志(著者)</t>
+          <t>蝉丸</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第14話前半</t>
+          <t>第26話　家族</t>
         </is>
       </c>
     </row>
@@ -30807,17 +31849,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>悪役令嬢、俺</t>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>弥南せいら(漫画) 猫屋敷のあ(原作)</t>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第1話</t>
+          <t>第47話 魔導具師とつながれたもの③</t>
         </is>
       </c>
     </row>
@@ -30827,17 +31869,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>異世界のんびり農家</t>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第302話</t>
+          <t>第１８話③</t>
         </is>
       </c>
     </row>
@@ -30847,17 +31889,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>氷結令嬢さまをフォローしたら、メチャメチャ溺愛されてしまった件@comic</t>
+          <t>異世界でも無難に生きたい症候群</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>漫画：ハレノチアメ 原作：愛坂タカト キャラクター原案：Bcoca</t>
+          <t>原作：安泰（一二三書房刊） 漫画：笹峰コウ キャラクター原案：ひたきゆう</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第8話</t>
+          <t>第30話②</t>
         </is>
       </c>
     </row>
@@ -30867,17 +31909,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ぽんドロイド！ はまさん</t>
+          <t>賢者の孫</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>はれやまはれぞう(著者)</t>
+          <t>緒方俊輔(漫画) 吉岡剛(原作) 菊池政治(キャラクター原案)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第5話</t>
+          <t>第94話-3</t>
         </is>
       </c>
     </row>
@@ -30887,17 +31929,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>はずれスキル念動力（ただしレベルＭＡＸ）で無双する～手をかざすだけです。詠唱とか必殺技とかいりません。念じるだけで倒せます～</t>
+          <t>めっちゃ召喚された件 THE COMIC</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>さとう うなぽっぽ トダフミト</t>
+          <t>漫画：六甲島カモメ 原作：さいとうさ キャラクター原案：ツグトク</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>9話③</t>
+          <t>第46話③</t>
         </is>
       </c>
     </row>
@@ -30907,17 +31949,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>異世界おじさん</t>
+          <t>魔術師クノンは見えている</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>殆ど死んでいる(著者)</t>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+          <t>第39話①</t>
         </is>
       </c>
     </row>
@@ -30927,17 +31969,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>物語の黒幕に転生して</t>
+          <t>レベル１だけどユニークスキルで最強です</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
+          <t>漫画：真綿 原作：三木なずな キャラクター原案：すばち</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第32話</t>
+          <t>第７２話　インドール救援作戦 大成功!?（２）</t>
         </is>
       </c>
     </row>
@@ -30947,17 +31989,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>リビルドワールド</t>
+          <t>北海道の現役ハンターが異世界に放り込まれてみた 〜エルフ嫁と巡る異世界狩猟ライフ〜</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+          <t>原作：ジュピタースタジオ「北海道の現役ハンターが異世界に放り込まれてみた」（小学館「ガガガブックス」刊） 漫画：カルトマ キャラクター原案：夕薙</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第71話③</t>
+          <t>第26話①</t>
         </is>
       </c>
     </row>
@@ -30967,17 +32009,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>転生貴族の異世界冒険録 ～カインのやりすぎギルド日記～</t>
+          <t>骨ドラゴンのマナ娘</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>原作：夜州 漫画：佐々木あかね・香本セトラ キャラクター原案：藻</t>
+          <t>雪白いち</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第48話</t>
+          <t>第38話②「祖先から継いだもの」</t>
         </is>
       </c>
     </row>
@@ -30987,17 +32029,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>サーシャちゃんとクラスメイトオタクくん</t>
+          <t>一億年ボタンを連打した俺は、気付いたら最強になっていた ～落第剣士の学院無双～</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>はぐはぐ(著者)</t>
+          <t>士土幽太郎(漫画) 月島秀一(原作) もきゅ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第82話</t>
+          <t>第40話-2</t>
         </is>
       </c>
     </row>
@@ -31007,17 +32049,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>幼女戦記</t>
+          <t>人外姫様、始めました　-Free Life Fantasy Online-</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>東條チカ(漫画) カルロ・ゼン(原作) 篠月しのぶ(キャラクター原案)</t>
+          <t>園原アオ 割田コマ 子日あきすず Sherry</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第百六章：ドードーバード航空戦Ⅰ</t>
+          <t>第６０話　常夜の城へ、突撃作戦！？</t>
         </is>
       </c>
     </row>
@@ -31027,17 +32069,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>俺だけ使える古代魔法 ～基礎すら使えないと追放された俺の魔法は、実は1万年前に失われた伝説魔法でした～</t>
+          <t>外れスキル『レベルアップ』のせいでパーティーを追放された少年は、レベルを上げて物理で殴る</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>原作／アトハ 漫画／川上ニナ キャラクター原案／片倉響</t>
+          <t>しんこせい 大橋ウルオ てんまそ</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第15話</t>
+          <t>第18話 ミヤダケ（後編）</t>
         </is>
       </c>
     </row>
@@ -31047,17 +32089,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ナナシの器用貧乏</t>
+          <t>無能と呼ばれた『精霊たらし』～実は異能で、精霊界では伝説的ヒーローでした～＠COMIC</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>原作：高球 漫画：葉原辰月 キャラクター原案：KeG</t>
+          <t>原作：佐藤謙羊 漫画：タバタグランドキャニオン</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第5話</t>
+          <t>第27話「求職は総合人材ギルドで」②</t>
         </is>
       </c>
     </row>
@@ -31067,17 +32109,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>男子高校生だけどギャルにTSしました</t>
+          <t>おっちゃん冒険者の千夜一夜</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>太陽まりい(著者)</t>
+          <t>キャラクター原案：戯々 漫画：栗橋伸祐 原作：金暮 銀</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第18話後編</t>
+          <t>第19話</t>
         </is>
       </c>
     </row>
@@ -31087,17 +32129,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>田舎の黒ギャルJKと結婚しました</t>
+          <t>国王である兄から辺境に追放されたけど平穏に暮らしたい ～目指せスローライフ～</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>カヅチ(著者)</t>
+          <t>おとら(原作) 西沢秀二(漫画) 夜ノみつき(キャラクター原案)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第17話後半</t>
+          <t>第11話-1</t>
         </is>
       </c>
     </row>
@@ -31107,17 +32149,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>三枝さんはメガネ先輩と恋を描く</t>
+          <t>ブチ切れ令嬢は報復を誓いました。 ～魔導書の力で祖国を叩き潰します～</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>セレビィ量産型(著者)</t>
+          <t>漫画：おおのいも 原作：はぐれメタボ キャラクター原案：昌未</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第21話前半</t>
+          <t>第48話</t>
         </is>
       </c>
     </row>
@@ -31127,17 +32169,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>モテはるねえ蘆屋くん</t>
+          <t>元カノ先生は、ちょっぴりエッチな家庭訪問できみとの愛を育みたい。</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>栗原和明(原作) 寺井赤音(作画)</t>
+          <t>漫画家：はづきけい 原作： 猫又ぬこ キャラクター原案： カット</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第16話前半</t>
+          <t>第9話</t>
         </is>
       </c>
     </row>
@@ -31147,17 +32189,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+          <t>器用貧乏、城を建てる～開拓学園の劣等生なのに、 上級職のスキルと魔法がすべて使えます～＠COMIC</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+          <t>原作：佐藤謙羊 漫画：スガン</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>「名もなき英雄譚」後半</t>
+          <t>第21話③「ルールの代償」</t>
         </is>
       </c>
     </row>
@@ -31167,17 +32209,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ゆーち〇ーばー</t>
+          <t>尾守つみきと奇日常。</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ともお</t>
+          <t>森下みゆ</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第1話</t>
+          <t>第59話 雷漸会長と約束。</t>
         </is>
       </c>
     </row>
@@ -31187,17 +32229,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ワンパンマン</t>
+          <t>クラス最安値で売られた俺は、実は最強パラメーター</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>原作/ＯＮＥ 作画/村田雄介</t>
+          <t>カンブリア爆発太郎(漫画) RYOMA(原作) 黒井ススム(キャラクター原案)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>206撃目</t>
+          <t>第36話-1</t>
         </is>
       </c>
     </row>
@@ -31207,17 +32249,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>魔王令嬢の教育係 ～勇者学院を追放された平民教師は魔王の娘たちの家庭教師となる～</t>
+          <t>転生少女はまず一歩からはじめたい～魔物がいるとか聞いてない！～</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>原作：新人 漫画：松原剛 キャラクター原案：巻羊</t>
+          <t>原作：カヤ 漫画：岡村アユム キャラクター原案：那流</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第29話</t>
+          <t>第37話 お屋敷での日々②</t>
         </is>
       </c>
     </row>
@@ -31227,17 +32269,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>淫獄団地</t>
+          <t>魔眼の悪役に転生したので推しキャラを見守るモブを目指します</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+          <t>在間りしん(漫画) 瀧岡くるじ(原作) 福きつね(キャラクター原案)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第49話（前編）</t>
+          <t>第11話①</t>
         </is>
       </c>
     </row>
@@ -31247,17 +32289,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ミルク搾りハンターの異世界搾乳記～農家の冴えない男があらゆる種族の地区Bを弄び虜にする～</t>
+          <t>拝啓…殺し屋さんと結婚しました</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>空詠大智(著者)</t>
+          <t>高坂曇天(著者)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第17話前半</t>
+          <t>第65話</t>
         </is>
       </c>
     </row>
@@ -31267,17 +32309,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>まんきつしたい常連さん</t>
+          <t>レベル１から始まる召喚無双</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>しんみりん(著者)</t>
+          <t>漫画：七桃りお 原作：白石新 キャラクター原案：夕薙</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第46話前編</t>
+          <t>第33話前半</t>
         </is>
       </c>
     </row>
@@ -31287,17 +32329,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ソードアート・オンライン Re:Aincrad</t>
+          <t>狂戦士なモブ、無自覚に本編を破壊する</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>樹深(作画) 佐藤ミト(構成) 川原礫(原作) ａｂｅｃ(キャラクターデザイン)</t>
+          <t>漫画：佐藤良亮 原作：なるのるな キャラクター原案：霜月えいと</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第40話②</t>
+          <t>第11話 ③</t>
         </is>
       </c>
     </row>
@@ -31307,17 +32349,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>よくわからないけれど異世界に転生していたようです</t>
+          <t>ネタキャラ転生とかあんまりだ！ THE COMIC</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>内々けやき あし カオミン</t>
+          <t>漫画：あまねかむらぎ 原作：音無奏 キャラクター原案：azuタロウ</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第136話 よくわからないけれどスカウトされたみたいです（２）</t>
+          <t>第30話②</t>
         </is>
       </c>
     </row>
@@ -31327,17 +32369,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>リアリスト魔王による聖域なき異世界改革</t>
+          <t>不遇皇子は天才錬金術師～皇帝なんて柄じゃないので弟妹を可愛がりたい～@COMIC</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>鈴木マナツ(漫画) 羽田遼亮(原作) ゆーげん(キャラクターデザイン) ひたきゆう(キャラクターデザイン)</t>
+          <t>長先ザワ（漫画） うめー（原作） 瑛来イチ（構成） 雨銛（構成） かわく（キャラクター原案）</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第67幕③</t>
+          <t>第8話 ②</t>
         </is>
       </c>
     </row>
@@ -31347,17 +32389,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
+          <t>ダンジョンの幼なじみ</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
+          <t>久真やすひさ(著者)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第23話</t>
+          <t>お休みイラスト</t>
         </is>
       </c>
     </row>
@@ -31367,17 +32409,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ガルルガール</t>
+          <t>ひきこもりの俺がかわいいギルドマスターに世話を焼かれまくったって別にいいだろう?</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>原聡志(著者)</t>
+          <t>漫画：ミト 原作：東條功一 イラスト：にもし</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第15話</t>
+          <t>第18話</t>
         </is>
       </c>
     </row>
@@ -31387,17 +32429,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>最強ギフトで領地経営スローライフ ～辺境の村を開拓していたら英雄級の人材がわんさかやってきた！～</t>
+          <t>２度目の人生、と思ったら、実は３度目だった。～歴史知識と内政努力で不幸な歴史の改変に挑みます～@COMIC</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>原作：音速炒飯 漫画：眠田瞼 キャラクター原案：riritto</t>
+          <t>麦こうちゃ（漫画） take4（原作） 桧野ひなこ（キャラクター原案）</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第28話</t>
+          <t>第9話 ①</t>
         </is>
       </c>
     </row>
@@ -31407,17 +32449,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>アラサーがVTuberになった話。</t>
+          <t>クセ強彼女は床にいざなう</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>犬威赤彦(漫画) とくめい(原作) カラスBTK(キャラクター原案)</t>
+          <t>須河篤志(著者)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第24話</t>
+          <t>第14話前半</t>
         </is>
       </c>
     </row>
@@ -31427,17 +32469,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>美人女上司滝沢さん</t>
+          <t>S級パーティーから追放された狩人、実は世界最強 ～射程9999の男、帝国の狙撃手として無双する～</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>やんBARU(著者)</t>
+          <t>漫画：カズミヤアキラ 原作：茨木野 キャラクター原案：へいろー</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第202話</t>
+          <t>第9話 ②</t>
         </is>
       </c>
     </row>
@@ -31447,17 +32489,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>転生してあらゆるモノに好かれながら異世界で好きな事をして生きて行く</t>
+          <t>コボルト無双、モフモフな最弱噛ませ犬だけど世界最強を目指す！</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>都尾琉(漫画) 御峰。(原作)</t>
+          <t>赤志木ひの乃 shiba</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第26話④</t>
+          <t>第十四話 約束</t>
         </is>
       </c>
     </row>
@@ -31467,17 +32509,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+          <t>異世界たぬき</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+          <t>小林安曇</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第71話(前編) ダリエルVS.滾り</t>
+          <t>第2話②</t>
         </is>
       </c>
     </row>
@@ -31487,17 +32529,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>天獄で悪魔がボクを魅惑する</t>
+          <t>ダンジョンバンド</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>銀河味めてお(著者)</t>
+          <t>新挑限(著者)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第34話</t>
+          <t>♯７SPEED TUBE ②</t>
         </is>
       </c>
     </row>
@@ -31507,17 +32549,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+          <t>能あるオーガは角を隠す</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>FUNA 東西 モトエ恵介</t>
+          <t>漫画家： 蒼葉 結 原作： 津野瀬 文</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第120話　会談［その5］</t>
+          <t>第9話 後編</t>
         </is>
       </c>
     </row>
@@ -31527,17 +32569,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+          <t>異世界おじさん</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+          <t>殆ど死んでいる(著者)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第80話その3</t>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
@@ -31547,17 +32589,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>王様ランキング200話～</t>
+          <t>異世界のんびり農家</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>十日草輔（とおかそうすけ）</t>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第262話</t>
+          <t>第302話</t>
         </is>
       </c>
     </row>
@@ -31567,17 +32609,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>愚かな天使は悪魔と踊る</t>
+          <t>ちはるくんは女装をしたくない！</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>アズマサワヨシ(著者)</t>
+          <t>翁丸ジョン</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第100話③</t>
+          <t>【第21話】男装宗と交流したくない！その三</t>
         </is>
       </c>
     </row>
@@ -31587,17 +32629,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ひびワれこうじつ</t>
+          <t>モブ高生の俺でも冒険者になればリア充になれますか？</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>ぺろぽねそす(著者)</t>
+          <t>原作：百均 漫画：さぎやまれん キャラクター原案：hai</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第1話</t>
+          <t>第30話</t>
         </is>
       </c>
     </row>
@@ -31607,17 +32649,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ずっと好きだった幼馴染と付き合い始めたら一途ビッチの性欲ジャンキーだったんだがどうすりゃいいですか？</t>
+          <t>氷結令嬢さまをフォローしたら、メチャメチャ溺愛されてしまった件@comic</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>原作：トラ子猫 作画：あらいぐま</t>
+          <t>漫画：ハレノチアメ 原作：愛坂タカト キャラクター原案：Bcoca</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第3話</t>
+          <t>第8話</t>
         </is>
       </c>
     </row>
@@ -31627,17 +32669,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>転生前はドラゴンでした</t>
+          <t>ぽんドロイド！ はまさん</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>甘井ヤドラキ</t>
+          <t>はれやまはれぞう(著者)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第44話+お知らせ</t>
+          <t>第5話</t>
         </is>
       </c>
     </row>
@@ -31647,17 +32689,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>両親の借金を肩代わりしてもらう条件は日本一可愛い女子高生と一緒に暮らすことでした。</t>
+          <t>千年英雄</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>美月めいあ(漫画) 雨音恵(原作) ｋａｋａｏ(キャラクター原案)</t>
+          <t>原作/福島航平 作画/中村ゆきひろ</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第36話</t>
+          <t>19話②</t>
         </is>
       </c>
     </row>
@@ -31667,17 +32709,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>本物のカノジョにしたくなるまで、私で試していいよ。</t>
+          <t>物語の黒幕に転生して</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>wano(漫画) 有丈ほえる(原作) 緋月ひぐれ(キャラクター原案)</t>
+          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第8話②</t>
+          <t>第32話</t>
         </is>
       </c>
     </row>
@@ -31687,17 +32729,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>わたし、二番目の彼女でいいから。</t>
+          <t>ワンパンマン</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>にの子(漫画) 西条陽(原作) Re岳(キャラクター原案)</t>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第10話③：カーテンのなか</t>
+          <t>207撃目</t>
         </is>
       </c>
     </row>
@@ -31707,17 +32749,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+          <t>リビルドワールド</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第34話①</t>
+          <t>第71話③</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-07-30
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -44,6 +44,7 @@
     <sheet name="2025-07-27" sheetId="36" state="visible" r:id="rId36"/>
     <sheet name="2025-07-28" sheetId="37" state="visible" r:id="rId37"/>
     <sheet name="2025-07-29" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="2025-07-30" sheetId="39" state="visible" r:id="rId39"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -31764,22 +31765,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>帰ってください！ 阿久津さん</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>長岡太一(著者)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第193話</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第５０話　雌雄を決する器用貧乏（４）</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>姫ヶ崎櫻子は今日も不憫可愛い</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>安田剛助(著者)</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第49話</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>「おかえり、パパ」</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>蝉丸</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第26話　家族</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第47話 魔導具師とつながれたもの③</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第１８話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>異世界でも無難に生きたい症候群</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>原作：安泰（一二三書房刊） 漫画：笹峰コウ キャラクター原案：ひたきゆう</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第30話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>賢者の孫</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>緒方俊輔(漫画) 吉岡剛(原作) 菊池政治(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第94話-3</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>めっちゃ召喚された件 THE COMIC</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>漫画：六甲島カモメ 原作：さいとうさ キャラクター原案：ツグトク</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第46話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>魔術師クノンは見えている</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第39話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>レベル１だけどユニークスキルで最強です</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>漫画：真綿 原作：三木なずな キャラクター原案：すばち</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第７２話　インドール救援作戦 大成功!?（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>北海道の現役ハンターが異世界に放り込まれてみた 〜エルフ嫁と巡る異世界狩猟ライフ〜</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>原作：ジュピタースタジオ「北海道の現役ハンターが異世界に放り込まれてみた」（小学館「ガガガブックス」刊） 漫画：カルトマ キャラクター原案：夕薙</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第26話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>骨ドラゴンのマナ娘</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>雪白いち</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第38話②「祖先から継いだもの」</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>一億年ボタンを連打した俺は、気付いたら最強になっていた ～落第剣士の学院無双～</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>士土幽太郎(漫画) 月島秀一(原作) もきゅ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第40話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>人外姫様、始めました　-Free Life Fantasy Online-</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>園原アオ 割田コマ 子日あきすず Sherry</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第６０話　常夜の城へ、突撃作戦！？</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>外れスキル『レベルアップ』のせいでパーティーを追放された少年は、レベルを上げて物理で殴る</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>しんこせい 大橋ウルオ てんまそ</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第18話 ミヤダケ（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>無能と呼ばれた『精霊たらし』～実は異能で、精霊界では伝説的ヒーローでした～＠COMIC</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>原作：佐藤謙羊 漫画：タバタグランドキャニオン</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第27話「求職は総合人材ギルドで」②</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>おっちゃん冒険者の千夜一夜</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>キャラクター原案：戯々 漫画：栗橋伸祐 原作：金暮 銀</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第19話</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>国王である兄から辺境に追放されたけど平穏に暮らしたい ～目指せスローライフ～</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>おとら(原作) 西沢秀二(漫画) 夜ノみつき(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第11話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>ブチ切れ令嬢は報復を誓いました。 ～魔導書の力で祖国を叩き潰します～</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>漫画：おおのいも 原作：はぐれメタボ キャラクター原案：昌未</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第48話</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>元カノ先生は、ちょっぴりエッチな家庭訪問できみとの愛を育みたい。</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>漫画家：はづきけい 原作： 猫又ぬこ キャラクター原案： カット</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第9話</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>器用貧乏、城を建てる～開拓学園の劣等生なのに、 上級職のスキルと魔法がすべて使えます～＠COMIC</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>原作：佐藤謙羊 漫画：スガン</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第21話③「ルールの代償」</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>尾守つみきと奇日常。</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>森下みゆ</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第59話 雷漸会長と約束。</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>クラス最安値で売られた俺は、実は最強パラメーター</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>カンブリア爆発太郎(漫画) RYOMA(原作) 黒井ススム(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第36話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>転生少女はまず一歩からはじめたい～魔物がいるとか聞いてない！～</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>原作：カヤ 漫画：岡村アユム キャラクター原案：那流</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第37話 お屋敷での日々②</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>魔眼の悪役に転生したので推しキャラを見守るモブを目指します</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>在間りしん(漫画) 瀧岡くるじ(原作) 福きつね(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第11話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>拝啓…殺し屋さんと結婚しました</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>高坂曇天(著者)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第65話</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>レベル１から始まる召喚無双</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>漫画：七桃りお 原作：白石新 キャラクター原案：夕薙</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第33話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>狂戦士なモブ、無自覚に本編を破壊する</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>漫画：佐藤良亮 原作：なるのるな キャラクター原案：霜月えいと</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第11話 ③</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>ネタキャラ転生とかあんまりだ！ THE COMIC</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>漫画：あまねかむらぎ 原作：音無奏 キャラクター原案：azuタロウ</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第30話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>不遇皇子は天才錬金術師～皇帝なんて柄じゃないので弟妹を可愛がりたい～@COMIC</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>長先ザワ（漫画） うめー（原作） 瑛来イチ（構成） 雨銛（構成） かわく（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第8話 ②</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>ダンジョンの幼なじみ</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>久真やすひさ(著者)</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>お休みイラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>ひきこもりの俺がかわいいギルドマスターに世話を焼かれまくったって別にいいだろう?</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>漫画：ミト 原作：東條功一 イラスト：にもし</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第18話</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>２度目の人生、と思ったら、実は３度目だった。～歴史知識と内政努力で不幸な歴史の改変に挑みます～@COMIC</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>麦こうちゃ（漫画） take4（原作） 桧野ひなこ（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第9話 ①</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>クセ強彼女は床にいざなう</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>須河篤志(著者)</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第14話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>S級パーティーから追放された狩人、実は世界最強 ～射程9999の男、帝国の狙撃手として無双する～</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>漫画：カズミヤアキラ 原作：茨木野 キャラクター原案：へいろー</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第9話 ②</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>コボルト無双、モフモフな最弱噛ませ犬だけど世界最強を目指す！</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>赤志木ひの乃 shiba</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第十四話 約束</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>異世界たぬき</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>小林安曇</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第2話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>ダンジョンバンド</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>新挑限(著者)</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>♯７SPEED TUBE ②</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>能あるオーガは角を隠す</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>漫画家： 蒼葉 結 原作： 津野瀬 文</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第9話 後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>異世界おじさん</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>殆ど死んでいる(著者)</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>異世界のんびり農家</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第302話</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>ちはるくんは女装をしたくない！</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>翁丸ジョン</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>【第21話】男装宗と交流したくない！その三</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>モブ高生の俺でも冒険者になればリア充になれますか？</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>原作：百均 漫画：さぎやまれん キャラクター原案：hai</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第30話</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>氷結令嬢さまをフォローしたら、メチャメチャ溺愛されてしまった件@comic</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>漫画：ハレノチアメ 原作：愛坂タカト キャラクター原案：Bcoca</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第8話</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>ぽんドロイド！ はまさん</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>はれやまはれぞう(著者)</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>千年英雄</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>原作/福島航平 作画/中村ゆきひろ</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>19話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>物語の黒幕に転生して</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第32話</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>ワンパンマン</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>207撃目</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第71話③</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>帰ってください！ 阿久津さん</t>
+          <t>異世界居酒屋「のぶ」</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>長岡太一(著者)</t>
+          <t>蝉川夏哉(原作) ヴァージニア二等兵(漫画) 転(キャラクター原案)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第193話</t>
+          <t>第123話</t>
         </is>
       </c>
     </row>
@@ -31789,17 +32831,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+          <t>戸賀 環 坂木持丸 riritto</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第５０話　雌雄を決する器用貧乏（４）</t>
+          <t>第50話①　祝われた家を探索してみた</t>
         </is>
       </c>
     </row>
@@ -31809,17 +32851,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>姫ヶ崎櫻子は今日も不憫可愛い</t>
+          <t>女子高生の無駄づかい</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>安田剛助(著者)</t>
+          <t>ビーノ(著者)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第49話</t>
+          <t>第133話　てこいれ</t>
         </is>
       </c>
     </row>
@@ -31829,17 +32871,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>「おかえり、パパ」</t>
+          <t>絶対死なないステラ姫</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>蝉丸</t>
+          <t>光永康則 大高稲</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第26話　家族</t>
+          <t>第１４話　絶対旅立たない（３）</t>
         </is>
       </c>
     </row>
@@ -31849,17 +32891,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
+          <t>ひとりぼっちの異世界攻略</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
+          <t>びび（漫画） 五示正司（原作）</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第47話 魔導具師とつながれたもの③</t>
+          <t>第229話　最初は良い感じだったよ…？</t>
         </is>
       </c>
     </row>
@@ -31869,17 +32911,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+          <t>江戸前エルフ</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+          <t>樋口彰彦</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第１８話③</t>
+          <t>#116</t>
         </is>
       </c>
     </row>
@@ -31889,17 +32931,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>異世界でも無難に生きたい症候群</t>
+          <t>序盤で死ぬ最強のサブキャラに転生したので、ゲーム知識で無双する</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>原作：安泰（一二三書房刊） 漫画：笹峰コウ キャラクター原案：ひたきゆう</t>
+          <t>作画：マエD 原作：新人</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第30話②</t>
+          <t>第5話(2)</t>
         </is>
       </c>
     </row>
@@ -31909,17 +32951,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>賢者の孫</t>
+          <t>最後のエルフ</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>緒方俊輔(漫画) 吉岡剛(原作) 菊池政治(キャラクター原案)</t>
+          <t>サワノアキラ（漫画）</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第94話-3</t>
+          <t>第9章　竜の眠る地（後編）</t>
         </is>
       </c>
     </row>
@@ -31929,17 +32971,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>めっちゃ召喚された件 THE COMIC</t>
+          <t>ダウナー系お姉さんに毎日カスの嘘を流し込まれる話</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>漫画：六甲島カモメ 原作：さいとうさ キャラクター原案：ツグトク</t>
+          <t>生倉のゑる(著者) はるばーど屋(原作者)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第46話③</t>
+          <t>11話 おまけ</t>
         </is>
       </c>
     </row>
@@ -31949,17 +32991,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>魔術師クノンは見えている</t>
+          <t>「おかえり、パパ」</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+          <t>蝉丸</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第39話①</t>
+          <t>第26話　家族</t>
         </is>
       </c>
     </row>
@@ -31969,17 +33011,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>レベル１だけどユニークスキルで最強です</t>
+          <t>一生働きたくない俺が、クラスメイトの大人気アイドルに懐かれたら</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>漫画：真綿 原作：三木なずな キャラクター原案：すばち</t>
+          <t>三崎弓（漫画） 岸本和葉（原作） みわべさくら（キャラクター原案）</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第７２話　インドール救援作戦 大成功!?（２）</t>
+          <t>第20話　悩む者たち</t>
         </is>
       </c>
     </row>
@@ -31989,17 +33031,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>北海道の現役ハンターが異世界に放り込まれてみた 〜エルフ嫁と巡る異世界狩猟ライフ〜</t>
+          <t>ブレイド＆バスタード</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>原作：ジュピタースタジオ「北海道の現役ハンターが異世界に放り込まれてみた」（小学館「ガガガブックス」刊） 漫画：カルトマ キャラクター原案：夕薙</t>
+          <t>漫画/楓月 誠 原作/蝸牛くも キャラクター原案/so-bin</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第26話①</t>
+          <t>第10話（2）</t>
         </is>
       </c>
     </row>
@@ -32009,17 +33051,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>骨ドラゴンのマナ娘</t>
+          <t>黒の召喚士</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>雪白いち</t>
+          <t>天羽 銀（漫画） 迷井豆腐（原作） 黒銀（DIGS）（キャラクター原案）</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第38話②「祖先から継いだもの」</t>
+          <t>第145話　聖槍イクリプスⅥ</t>
         </is>
       </c>
     </row>
@@ -32029,17 +33071,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>一億年ボタンを連打した俺は、気付いたら最強になっていた ～落第剣士の学院無双～</t>
+          <t>凡人探索者のたのしい現代ダンジョンライフ</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>士土幽太郎(漫画) 月島秀一(原作) もきゅ(キャラクター原案)</t>
+          <t>もちろんさん（漫画） しば犬部隊(原作） 諏訪真弘（キャラクター原案）</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第40話-2</t>
+          <t>第4話　夜の街に繰り出そう！（前編）</t>
         </is>
       </c>
     </row>
@@ -32049,17 +33091,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>人外姫様、始めました　-Free Life Fantasy Online-</t>
+          <t>帰ってください！ 阿久津さん</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>園原アオ 割田コマ 子日あきすず Sherry</t>
+          <t>長岡太一(著者)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第６０話　常夜の城へ、突撃作戦！？</t>
+          <t>第193話</t>
         </is>
       </c>
     </row>
@@ -32069,17 +33111,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>外れスキル『レベルアップ』のせいでパーティーを追放された少年は、レベルを上げて物理で殴る</t>
+          <t>死ぬ運命にある悪役令嬢の兄に転生したので、妹を育てて未来を変えたいと思います　～世界最強はオレだけど、世界最カワは妹に違いない～</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>しんこせい 大橋ウルオ てんまそ</t>
+          <t>石見翔子(漫画） 泉里侑希（原作） タムラヨウ（キャラクター原案）</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第18話 ミヤダケ（後編）</t>
+          <t>第4話　はじめてのお出かけ（前編）</t>
         </is>
       </c>
     </row>
@@ -32089,17 +33131,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>無能と呼ばれた『精霊たらし』～実は異能で、精霊界では伝説的ヒーローでした～＠COMIC</t>
+          <t>姫ヶ崎櫻子は今日も不憫可愛い</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>原作：佐藤謙羊 漫画：タバタグランドキャニオン</t>
+          <t>安田剛助(著者)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第27話「求職は総合人材ギルドで」②</t>
+          <t>第49話</t>
         </is>
       </c>
     </row>
@@ -32109,17 +33151,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>おっちゃん冒険者の千夜一夜</t>
+          <t>勇者パーティを追放された【スキルサポーター】、仲間のスキルを解放して最強に成り上がる</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>キャラクター原案：戯々 漫画：栗橋伸祐 原作：金暮 銀</t>
+          <t>作画：なかお 原作：前田氏</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第19話</t>
+          <t>第6話(2)</t>
         </is>
       </c>
     </row>
@@ -32129,17 +33171,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>国王である兄から辺境に追放されたけど平穏に暮らしたい ～目指せスローライフ～</t>
+          <t>ラーメン大好き小泉さん</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>おとら(原作) 西沢秀二(漫画) 夜ノみつき(キャラクター原案)</t>
+          <t>鳴見なる</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第11話-1</t>
+          <t>18杯目 未知味の拉麺</t>
         </is>
       </c>
     </row>
@@ -32149,17 +33191,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>ブチ切れ令嬢は報復を誓いました。 ～魔導書の力で祖国を叩き潰します～</t>
+          <t>亡びの国の征服者～魔王は世界を征服するようです～</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>漫画：おおのいも 原作：はぐれメタボ キャラクター原案：昌未</t>
+          <t>錆狗村昌（漫画） 不手折家（原作） toi8（キャラクター原案）</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第48話</t>
+          <t>第31話　正しい理解</t>
         </is>
       </c>
     </row>
@@ -32169,17 +33211,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>元カノ先生は、ちょっぴりエッチな家庭訪問できみとの愛を育みたい。</t>
+          <t>最強の少年聖騎士、転生者を狩る</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>漫画家：はづきけい 原作： 猫又ぬこ キャラクター原案： カット</t>
+          <t>作画：御塩 原作：宇奈木ユラ</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第9話</t>
+          <t>第6話(2)</t>
         </is>
       </c>
     </row>
@@ -32189,17 +33231,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>器用貧乏、城を建てる～開拓学園の劣等生なのに、 上級職のスキルと魔法がすべて使えます～＠COMIC</t>
+          <t>オークの酒杯に祝福を</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>原作：佐藤謙羊 漫画：スガン</t>
+          <t>かなどめはじめ</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第21話③「ルールの代償」</t>
+          <t>第45話　影瞬拳</t>
         </is>
       </c>
     </row>
@@ -32209,17 +33251,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>尾守つみきと奇日常。</t>
+          <t>転生したら没落貴族だったので、【呪言】を極めて家族を救います</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>森下みゆ</t>
+          <t>作画：アマセケイ 原作：メソポ・たみあ</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第59話 雷漸会長と約束。</t>
+          <t>第6話(2)</t>
         </is>
       </c>
     </row>
@@ -32229,17 +33271,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>クラス最安値で売られた俺は、実は最強パラメーター</t>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>カンブリア爆発太郎(漫画) RYOMA(原作) 黒井ススム(キャラクター原案)</t>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第36話-1</t>
+          <t>第５０話　雌雄を決する器用貧乏（４）</t>
         </is>
       </c>
     </row>
@@ -32249,17 +33291,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>転生少女はまず一歩からはじめたい～魔物がいるとか聞いてない！～</t>
+          <t>8歳から始める魔法学</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>原作：カヤ 漫画：岡村アユム キャラクター原案：那流</t>
+          <t>ゆうなぎ（漫画） 上野夕陽（原作） 乃希（キャラクター原案）</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第37話 お屋敷での日々②</t>
+          <t>第18話　意思交錯（後編）</t>
         </is>
       </c>
     </row>
@@ -32269,17 +33311,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>魔眼の悪役に転生したので推しキャラを見守るモブを目指します</t>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>在間りしん(漫画) 瀧岡くるじ(原作) 福きつね(キャラクター原案)</t>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第11話①</t>
+          <t>第47話 魔導具師とつながれたもの③</t>
         </is>
       </c>
     </row>
@@ -32289,17 +33331,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>拝啓…殺し屋さんと結婚しました</t>
+          <t>豚貴族は未来を切り開くようです</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>高坂曇天(著者)</t>
+          <t>大出リコ（漫画） しんこせい（原作） riritto（原作イラスト）</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第65話</t>
+          <t>第11話　仲間</t>
         </is>
       </c>
     </row>
@@ -32309,17 +33351,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>レベル１から始まる召喚無双</t>
+          <t>とある魔術の禁書目録外伝　とある科学の心理掌握</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>漫画：七桃りお 原作：白石新 キャラクター原案：夕薙</t>
+          <t>乃木康仁(漫画) 鎌池和馬(原作) はいむらきよたか(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第33話前半</t>
+          <t>第32話中編</t>
         </is>
       </c>
     </row>
@@ -32329,17 +33371,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>狂戦士なモブ、無自覚に本編を破壊する</t>
+          <t>フシノカミ ～辺境から始める文明再生記～</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>漫画：佐藤良亮 原作：なるのるな キャラクター原案：霜月えいと</t>
+          <t>黒杞よるの（漫画） 雨川水海（原作） 大熊まい（キャラクター原案）</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第11話 ③</t>
+          <t>第39話　蘇る歴史（後編）</t>
         </is>
       </c>
     </row>
@@ -32349,17 +33391,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ネタキャラ転生とかあんまりだ！ THE COMIC</t>
+          <t>魔術師クノンは見えている</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>漫画：あまねかむらぎ 原作：音無奏 キャラクター原案：azuタロウ</t>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第30話②</t>
+          <t>第39話①</t>
         </is>
       </c>
     </row>
@@ -32369,17 +33411,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>不遇皇子は天才錬金術師～皇帝なんて柄じゃないので弟妹を可愛がりたい～@COMIC</t>
+          <t>転生悪魔の最強勇者育成計画</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>長先ザワ（漫画） うめー（原作） 瑛来イチ（構成） 雨銛（構成） かわく（キャラクター原案）</t>
+          <t>瀬川 竜（漫画） たまごかけキャンディー（原作） 長浜めぐみ（原作イラスト）</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第8話 ②</t>
+          <t>第11話　親の背中</t>
         </is>
       </c>
     </row>
@@ -32389,17 +33431,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ダンジョンの幼なじみ</t>
+          <t>傷口と包帯</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>久真やすひさ(著者)</t>
+          <t>七井海星</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>お休みイラスト</t>
+          <t>第16話　2人の決意</t>
         </is>
       </c>
     </row>
@@ -32409,17 +33451,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ひきこもりの俺がかわいいギルドマスターに世話を焼かれまくったって別にいいだろう?</t>
+          <t>最凶貴族は死亡フラグを覆す</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>漫画：ミト 原作：東條功一 イラスト：にもし</t>
+          <t>作画：sudekuma 原作：塚上</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第18話</t>
+          <t>第6話(2)</t>
         </is>
       </c>
     </row>
@@ -32429,17 +33471,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>２度目の人生、と思ったら、実は３度目だった。～歴史知識と内政努力で不幸な歴史の改変に挑みます～@COMIC</t>
+          <t>この冒険者、人類史最強です～外れスキル『鑑定』が『継承』に覚醒したので、数多の英雄たちの力を受け継ぎ無双する～</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>麦こうちゃ（漫画） take4（原作） 桧野ひなこ（キャラクター原案）</t>
+          <t>日之影ソラ みやけりく エシュアル</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第9話 ①</t>
+          <t>第28話①もう一つ問題</t>
         </is>
       </c>
     </row>
@@ -32449,17 +33491,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>クセ強彼女は床にいざなう</t>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>須河篤志(著者)</t>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第14話前半</t>
+          <t>第１８話③</t>
         </is>
       </c>
     </row>
@@ -32469,17 +33511,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>S級パーティーから追放された狩人、実は世界最強 ～射程9999の男、帝国の狙撃手として無双する～</t>
+          <t>十歳の最強魔導師</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>漫画：カズミヤアキラ 原作：茨木野 キャラクター原案：へいろー</t>
+          <t>猫月 天乃聖樹</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第9話 ②</t>
+          <t>第1話</t>
         </is>
       </c>
     </row>
@@ -32489,17 +33531,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>コボルト無双、モフモフな最弱噛ませ犬だけど世界最強を目指す！</t>
+          <t>無能勇者の復讐譚 ～異世界で捨てられた少年は反逆を誓う～</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>赤志木ひの乃 shiba</t>
+          <t>作画：さんじろ♨ 原作：葵 咲九</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第十四話 約束</t>
+          <t>第6話(2)</t>
         </is>
       </c>
     </row>
@@ -32509,17 +33551,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>異世界たぬき</t>
+          <t>あたしは星間国家の英雄騎士！</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>小林安曇</t>
+          <t>石口 十（漫画） 三嶋与夢（原作） 高峰ナダレ（キャラクター原案）</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第2話②</t>
+          <t>第17話　新たな依頼（後編）</t>
         </is>
       </c>
     </row>
@@ -32529,17 +33571,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>ダンジョンバンド</t>
+          <t>異世界でも無難に生きたい症候群</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>新挑限(著者)</t>
+          <t>原作：安泰（一二三書房刊） 漫画：笹峰コウ キャラクター原案：ひたきゆう</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>♯７SPEED TUBE ②</t>
+          <t>第30話②</t>
         </is>
       </c>
     </row>
@@ -32549,17 +33591,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>能あるオーガは角を隠す</t>
+          <t>ワールド・ティーチャー 異世界式教育エージェント</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>漫画家： 蒼葉 結 原作： 津野瀬 文</t>
+          <t>吉乃そら（漫画） ネコ光一（原作） Nardack（キャラクター原案）</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第9話 後編</t>
+          <t>第80話　罪人達</t>
         </is>
       </c>
     </row>
@@ -32589,17 +33631,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>異世界のんびり農家</t>
+          <t>賢者の孫</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+          <t>緒方俊輔(漫画) 吉岡剛(原作) 菊池政治(キャラクター原案)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第302話</t>
+          <t>第94話-3</t>
         </is>
       </c>
     </row>
@@ -32609,17 +33651,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>ちはるくんは女装をしたくない！</t>
+          <t>めっちゃ召喚された件 THE COMIC</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>翁丸ジョン</t>
+          <t>漫画：六甲島カモメ 原作：さいとうさ キャラクター原案：ツグトク</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>【第21話】男装宗と交流したくない！その三</t>
+          <t>第46話③</t>
         </is>
       </c>
     </row>
@@ -32629,17 +33671,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>モブ高生の俺でも冒険者になればリア充になれますか？</t>
+          <t>影の宮廷魔術師 ～無能だと思われていた男、実は最強の軍師だった～</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>原作：百均 漫画：さぎやまれん キャラクター原案：hai</t>
+          <t>白石琴似（漫画） 羽田遼亮（原作） 黒井ススム（キャラクター原案）</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第30話</t>
+          <t>第47話　ジャンプからの踵落とし（後編）</t>
         </is>
       </c>
     </row>
@@ -32649,17 +33691,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>氷結令嬢さまをフォローしたら、メチャメチャ溺愛されてしまった件@comic</t>
+          <t>骨ドラゴンのマナ娘</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>漫画：ハレノチアメ 原作：愛坂タカト キャラクター原案：Bcoca</t>
+          <t>雪白いち</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第8話</t>
+          <t>第38話②「祖先から継いだもの」</t>
         </is>
       </c>
     </row>
@@ -32669,17 +33711,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>ぽんドロイド！ はまさん</t>
+          <t>追放されたダンジョン配信者、《マッピング》スキルで最強パーティーを目指します</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>はれやまはれぞう(著者)</t>
+          <t>作画：入逢夕 原作：瀬戸夏樹</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第5話</t>
+          <t>第6話(2)</t>
         </is>
       </c>
     </row>
@@ -32689,17 +33731,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>千年英雄</t>
+          <t>北海道の現役ハンターが異世界に放り込まれてみた 〜エルフ嫁と巡る異世界狩猟ライフ〜</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>原作/福島航平 作画/中村ゆきひろ</t>
+          <t>原作：ジュピタースタジオ「北海道の現役ハンターが異世界に放り込まれてみた」（小学館「ガガガブックス」刊） 漫画：カルトマ キャラクター原案：夕薙</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>19話②</t>
+          <t>第26話①</t>
         </is>
       </c>
     </row>
@@ -32709,17 +33751,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>物語の黒幕に転生して</t>
+          <t>外れスキル『レベルアップ』のせいでパーティーを追放された少年は、レベルを上げて物理で殴る</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
+          <t>しんこせい 大橋ウルオ てんまそ</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第32話</t>
+          <t>第18話 ミヤダケ（後編）</t>
         </is>
       </c>
     </row>
@@ -32729,17 +33771,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>ワンパンマン</t>
+          <t>レベル１だけどユニークスキルで最強です</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>原作/ＯＮＥ 作画/村田雄介</t>
+          <t>漫画：真綿 原作：三木なずな キャラクター原案：すばち</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>207撃目</t>
+          <t>第７２話　インドール救援作戦 大成功!?（２）</t>
         </is>
       </c>
     </row>
@@ -32749,17 +33791,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>リビルドワールド</t>
+          <t>ワンパンマン</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第71話③</t>
+          <t>207撃目</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-07-31
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -45,6 +45,7 @@
     <sheet name="2025-07-28" sheetId="37" state="visible" r:id="rId37"/>
     <sheet name="2025-07-29" sheetId="38" state="visible" r:id="rId38"/>
     <sheet name="2025-07-30" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="2025-07-31" sheetId="40" state="visible" r:id="rId40"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -32806,1000 +32807,1000 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="0" t="inlineStr">
         <is>
           <t>異世界居酒屋「のぶ」</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="0" t="inlineStr">
         <is>
           <t>蝉川夏哉(原作) ヴァージニア二等兵(漫画) 転(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="0" t="inlineStr">
         <is>
           <t>第123話</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="0" t="inlineStr">
         <is>
           <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="0" t="inlineStr">
         <is>
           <t>戸賀 環 坂木持丸 riritto</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" s="0" t="inlineStr">
         <is>
           <t>第50話①　祝われた家を探索してみた</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="0" t="inlineStr">
         <is>
           <t>女子高生の無駄づかい</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="0" t="inlineStr">
         <is>
           <t>ビーノ(著者)</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" s="0" t="inlineStr">
         <is>
           <t>第133話　てこいれ</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="0" t="inlineStr">
         <is>
           <t>絶対死なないステラ姫</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="0" t="inlineStr">
         <is>
           <t>光永康則 大高稲</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D5" s="0" t="inlineStr">
         <is>
           <t>第１４話　絶対旅立たない（３）</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="0" t="inlineStr">
         <is>
           <t>ひとりぼっちの異世界攻略</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" s="0" t="inlineStr">
         <is>
           <t>びび（漫画） 五示正司（原作）</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D6" s="0" t="inlineStr">
         <is>
           <t>第229話　最初は良い感じだったよ…？</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="0" t="inlineStr">
         <is>
           <t>江戸前エルフ</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="0" t="inlineStr">
         <is>
           <t>樋口彰彦</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D7" s="0" t="inlineStr">
         <is>
           <t>#116</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" s="0" t="inlineStr">
         <is>
           <t>序盤で死ぬ最強のサブキャラに転生したので、ゲーム知識で無双する</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" s="0" t="inlineStr">
         <is>
           <t>作画：マエD 原作：新人</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D8" s="0" t="inlineStr">
         <is>
           <t>第5話(2)</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="0" t="inlineStr">
         <is>
           <t>最後のエルフ</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" s="0" t="inlineStr">
         <is>
           <t>サワノアキラ（漫画）</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D9" s="0" t="inlineStr">
         <is>
           <t>第9章　竜の眠る地（後編）</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" s="0" t="inlineStr">
         <is>
           <t>ダウナー系お姉さんに毎日カスの嘘を流し込まれる話</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" s="0" t="inlineStr">
         <is>
           <t>生倉のゑる(著者) はるばーど屋(原作者)</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D10" s="0" t="inlineStr">
         <is>
           <t>11話 おまけ</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" s="0" t="inlineStr">
         <is>
           <t>「おかえり、パパ」</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" s="0" t="inlineStr">
         <is>
           <t>蝉丸</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D11" s="0" t="inlineStr">
         <is>
           <t>第26話　家族</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
+      <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" s="0" t="inlineStr">
         <is>
           <t>一生働きたくない俺が、クラスメイトの大人気アイドルに懐かれたら</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" s="0" t="inlineStr">
         <is>
           <t>三崎弓（漫画） 岸本和葉（原作） みわべさくら（キャラクター原案）</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D12" s="0" t="inlineStr">
         <is>
           <t>第20話　悩む者たち</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
+      <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" s="0" t="inlineStr">
         <is>
           <t>ブレイド＆バスタード</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" s="0" t="inlineStr">
         <is>
           <t>漫画/楓月 誠 原作/蝸牛くも キャラクター原案/so-bin</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D13" s="0" t="inlineStr">
         <is>
           <t>第10話（2）</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
+      <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B14" s="0" t="inlineStr">
         <is>
           <t>黒の召喚士</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C14" s="0" t="inlineStr">
         <is>
           <t>天羽 銀（漫画） 迷井豆腐（原作） 黒銀（DIGS）（キャラクター原案）</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D14" s="0" t="inlineStr">
         <is>
           <t>第145話　聖槍イクリプスⅥ</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
+      <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B15" s="0" t="inlineStr">
         <is>
           <t>凡人探索者のたのしい現代ダンジョンライフ</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C15" s="0" t="inlineStr">
         <is>
           <t>もちろんさん（漫画） しば犬部隊(原作） 諏訪真弘（キャラクター原案）</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D15" s="0" t="inlineStr">
         <is>
           <t>第4話　夜の街に繰り出そう！（前編）</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
+      <c r="A16" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B16" s="0" t="inlineStr">
         <is>
           <t>帰ってください！ 阿久津さん</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C16" s="0" t="inlineStr">
         <is>
           <t>長岡太一(著者)</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="D16" s="0" t="inlineStr">
         <is>
           <t>第193話</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
+      <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B17" s="0" t="inlineStr">
         <is>
           <t>死ぬ運命にある悪役令嬢の兄に転生したので、妹を育てて未来を変えたいと思います　～世界最強はオレだけど、世界最カワは妹に違いない～</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C17" s="0" t="inlineStr">
         <is>
           <t>石見翔子(漫画） 泉里侑希（原作） タムラヨウ（キャラクター原案）</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="D17" s="0" t="inlineStr">
         <is>
           <t>第4話　はじめてのお出かけ（前編）</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
+      <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B18" s="0" t="inlineStr">
         <is>
           <t>姫ヶ崎櫻子は今日も不憫可愛い</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C18" s="0" t="inlineStr">
         <is>
           <t>安田剛助(著者)</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="D18" s="0" t="inlineStr">
         <is>
           <t>第49話</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
+      <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B19" s="0" t="inlineStr">
         <is>
           <t>勇者パーティを追放された【スキルサポーター】、仲間のスキルを解放して最強に成り上がる</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C19" s="0" t="inlineStr">
         <is>
           <t>作画：なかお 原作：前田氏</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="D19" s="0" t="inlineStr">
         <is>
           <t>第6話(2)</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
+      <c r="A20" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B20" s="0" t="inlineStr">
         <is>
           <t>ラーメン大好き小泉さん</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C20" s="0" t="inlineStr">
         <is>
           <t>鳴見なる</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="D20" s="0" t="inlineStr">
         <is>
           <t>18杯目 未知味の拉麺</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
+      <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B21" s="0" t="inlineStr">
         <is>
           <t>亡びの国の征服者～魔王は世界を征服するようです～</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C21" s="0" t="inlineStr">
         <is>
           <t>錆狗村昌（漫画） 不手折家（原作） toi8（キャラクター原案）</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="D21" s="0" t="inlineStr">
         <is>
           <t>第31話　正しい理解</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
+      <c r="A22" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B22" s="0" t="inlineStr">
         <is>
           <t>最強の少年聖騎士、転生者を狩る</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C22" s="0" t="inlineStr">
         <is>
           <t>作画：御塩 原作：宇奈木ユラ</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="D22" s="0" t="inlineStr">
         <is>
           <t>第6話(2)</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="n">
+      <c r="A23" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B23" s="0" t="inlineStr">
         <is>
           <t>オークの酒杯に祝福を</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C23" s="0" t="inlineStr">
         <is>
           <t>かなどめはじめ</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="D23" s="0" t="inlineStr">
         <is>
           <t>第45話　影瞬拳</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="n">
+      <c r="A24" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B24" s="0" t="inlineStr">
         <is>
           <t>転生したら没落貴族だったので、【呪言】を極めて家族を救います</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="C24" s="0" t="inlineStr">
         <is>
           <t>作画：アマセケイ 原作：メソポ・たみあ</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="D24" s="0" t="inlineStr">
         <is>
           <t>第6話(2)</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="n">
+      <c r="A25" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="B25" s="0" t="inlineStr">
         <is>
           <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C25" s="0" t="inlineStr">
         <is>
           <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="D25" s="0" t="inlineStr">
         <is>
           <t>第５０話　雌雄を決する器用貧乏（４）</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="n">
+      <c r="A26" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="B26" s="0" t="inlineStr">
         <is>
           <t>8歳から始める魔法学</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="C26" s="0" t="inlineStr">
         <is>
           <t>ゆうなぎ（漫画） 上野夕陽（原作） 乃希（キャラクター原案）</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="D26" s="0" t="inlineStr">
         <is>
           <t>第18話　意思交錯（後編）</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="n">
+      <c r="A27" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="B27" s="0" t="inlineStr">
         <is>
           <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="C27" s="0" t="inlineStr">
         <is>
           <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="D27" s="0" t="inlineStr">
         <is>
           <t>第47話 魔導具師とつながれたもの③</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="n">
+      <c r="A28" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B28" s="0" t="inlineStr">
         <is>
           <t>豚貴族は未来を切り開くようです</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C28" s="0" t="inlineStr">
         <is>
           <t>大出リコ（漫画） しんこせい（原作） riritto（原作イラスト）</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="D28" s="0" t="inlineStr">
         <is>
           <t>第11話　仲間</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="n">
+      <c r="A29" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="B29" s="0" t="inlineStr">
         <is>
           <t>とある魔術の禁書目録外伝　とある科学の心理掌握</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="C29" s="0" t="inlineStr">
         <is>
           <t>乃木康仁(漫画) 鎌池和馬(原作) はいむらきよたか(キャラクターデザイン)</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="D29" s="0" t="inlineStr">
         <is>
           <t>第32話中編</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="n">
+      <c r="A30" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="B30" s="0" t="inlineStr">
         <is>
           <t>フシノカミ ～辺境から始める文明再生記～</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="C30" s="0" t="inlineStr">
         <is>
           <t>黒杞よるの（漫画） 雨川水海（原作） 大熊まい（キャラクター原案）</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="D30" s="0" t="inlineStr">
         <is>
           <t>第39話　蘇る歴史（後編）</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="n">
+      <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="B31" s="0" t="inlineStr">
         <is>
           <t>魔術師クノンは見えている</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="C31" s="0" t="inlineStr">
         <is>
           <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="D31" s="0" t="inlineStr">
         <is>
           <t>第39話①</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="n">
+      <c r="A32" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="B32" s="0" t="inlineStr">
         <is>
           <t>転生悪魔の最強勇者育成計画</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="C32" s="0" t="inlineStr">
         <is>
           <t>瀬川 竜（漫画） たまごかけキャンディー（原作） 長浜めぐみ（原作イラスト）</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="D32" s="0" t="inlineStr">
         <is>
           <t>第11話　親の背中</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="n">
+      <c r="A33" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="B33" s="0" t="inlineStr">
         <is>
           <t>傷口と包帯</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="C33" s="0" t="inlineStr">
         <is>
           <t>七井海星</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="D33" s="0" t="inlineStr">
         <is>
           <t>第16話　2人の決意</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="n">
+      <c r="A34" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B34" s="0" t="inlineStr">
         <is>
           <t>最凶貴族は死亡フラグを覆す</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="C34" s="0" t="inlineStr">
         <is>
           <t>作画：sudekuma 原作：塚上</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="D34" s="0" t="inlineStr">
         <is>
           <t>第6話(2)</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="n">
+      <c r="A35" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="B35" s="0" t="inlineStr">
         <is>
           <t>この冒険者、人類史最強です～外れスキル『鑑定』が『継承』に覚醒したので、数多の英雄たちの力を受け継ぎ無双する～</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="C35" s="0" t="inlineStr">
         <is>
           <t>日之影ソラ みやけりく エシュアル</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="D35" s="0" t="inlineStr">
         <is>
           <t>第28話①もう一つ問題</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="n">
+      <c r="A36" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="B36" s="0" t="inlineStr">
         <is>
           <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="C36" s="0" t="inlineStr">
         <is>
           <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="D36" s="0" t="inlineStr">
         <is>
           <t>第１８話③</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="n">
+      <c r="A37" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="B37" s="0" t="inlineStr">
         <is>
           <t>十歳の最強魔導師</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="C37" s="0" t="inlineStr">
         <is>
           <t>猫月 天乃聖樹</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
+      <c r="D37" s="0" t="inlineStr">
         <is>
           <t>第1話</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="n">
+      <c r="A38" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="B38" s="0" t="inlineStr">
         <is>
           <t>無能勇者の復讐譚 ～異世界で捨てられた少年は反逆を誓う～</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
+      <c r="C38" s="0" t="inlineStr">
         <is>
           <t>作画：さんじろ♨ 原作：葵 咲九</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
+      <c r="D38" s="0" t="inlineStr">
         <is>
           <t>第6話(2)</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="n">
+      <c r="A39" s="0" t="n">
         <v>38</v>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="B39" s="0" t="inlineStr">
         <is>
           <t>あたしは星間国家の英雄騎士！</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="C39" s="0" t="inlineStr">
         <is>
           <t>石口 十（漫画） 三嶋与夢（原作） 高峰ナダレ（キャラクター原案）</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
+      <c r="D39" s="0" t="inlineStr">
         <is>
           <t>第17話　新たな依頼（後編）</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="n">
+      <c r="A40" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="B40" s="0" t="inlineStr">
         <is>
           <t>異世界でも無難に生きたい症候群</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="C40" s="0" t="inlineStr">
         <is>
           <t>原作：安泰（一二三書房刊） 漫画：笹峰コウ キャラクター原案：ひたきゆう</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="D40" s="0" t="inlineStr">
         <is>
           <t>第30話②</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="n">
+      <c r="A41" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="B41" s="0" t="inlineStr">
         <is>
           <t>ワールド・ティーチャー 異世界式教育エージェント</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="C41" s="0" t="inlineStr">
         <is>
           <t>吉乃そら（漫画） ネコ光一（原作） Nardack（キャラクター原案）</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
+      <c r="D41" s="0" t="inlineStr">
         <is>
           <t>第80話　罪人達</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="n">
+      <c r="A42" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="B42" s="0" t="inlineStr">
         <is>
           <t>異世界おじさん</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="C42" s="0" t="inlineStr">
         <is>
           <t>殆ど死んでいる(著者)</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
+      <c r="D42" s="0" t="inlineStr">
         <is>
           <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="n">
+      <c r="A43" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B43" s="0" t="inlineStr">
         <is>
           <t>賢者の孫</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="C43" s="0" t="inlineStr">
         <is>
           <t>緒方俊輔(漫画) 吉岡剛(原作) 菊池政治(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
+      <c r="D43" s="0" t="inlineStr">
         <is>
           <t>第94話-3</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="n">
+      <c r="A44" s="0" t="n">
         <v>43</v>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="B44" s="0" t="inlineStr">
         <is>
           <t>めっちゃ召喚された件 THE COMIC</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="C44" s="0" t="inlineStr">
         <is>
           <t>漫画：六甲島カモメ 原作：さいとうさ キャラクター原案：ツグトク</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
+      <c r="D44" s="0" t="inlineStr">
         <is>
           <t>第46話③</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="n">
+      <c r="A45" s="0" t="n">
         <v>44</v>
       </c>
-      <c r="B45" t="inlineStr">
+      <c r="B45" s="0" t="inlineStr">
         <is>
           <t>影の宮廷魔術師 ～無能だと思われていた男、実は最強の軍師だった～</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="C45" s="0" t="inlineStr">
         <is>
           <t>白石琴似（漫画） 羽田遼亮（原作） 黒井ススム（キャラクター原案）</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
+      <c r="D45" s="0" t="inlineStr">
         <is>
           <t>第47話　ジャンプからの踵落とし（後編）</t>
         </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="n">
+      <c r="A46" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="B46" t="inlineStr">
+      <c r="B46" s="0" t="inlineStr">
         <is>
           <t>骨ドラゴンのマナ娘</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="C46" s="0" t="inlineStr">
         <is>
           <t>雪白いち</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
+      <c r="D46" s="0" t="inlineStr">
         <is>
           <t>第38話②「祖先から継いだもの」</t>
         </is>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="n">
+      <c r="A47" s="0" t="n">
         <v>46</v>
       </c>
-      <c r="B47" t="inlineStr">
+      <c r="B47" s="0" t="inlineStr">
         <is>
           <t>追放されたダンジョン配信者、《マッピング》スキルで最強パーティーを目指します</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="C47" s="0" t="inlineStr">
         <is>
           <t>作画：入逢夕 原作：瀬戸夏樹</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
+      <c r="D47" s="0" t="inlineStr">
         <is>
           <t>第6話(2)</t>
         </is>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="n">
+      <c r="A48" s="0" t="n">
         <v>47</v>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="B48" s="0" t="inlineStr">
         <is>
           <t>北海道の現役ハンターが異世界に放り込まれてみた 〜エルフ嫁と巡る異世界狩猟ライフ〜</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
+      <c r="C48" s="0" t="inlineStr">
         <is>
           <t>原作：ジュピタースタジオ「北海道の現役ハンターが異世界に放り込まれてみた」（小学館「ガガガブックス」刊） 漫画：カルトマ キャラクター原案：夕薙</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
+      <c r="D48" s="0" t="inlineStr">
         <is>
           <t>第26話①</t>
         </is>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="n">
+      <c r="A49" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="B49" s="0" t="inlineStr">
         <is>
           <t>外れスキル『レベルアップ』のせいでパーティーを追放された少年は、レベルを上げて物理で殴る</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="C49" s="0" t="inlineStr">
         <is>
           <t>しんこせい 大橋ウルオ てんまそ</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
+      <c r="D49" s="0" t="inlineStr">
         <is>
           <t>第18話 ミヤダケ（後編）</t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="n">
+      <c r="A50" s="0" t="n">
         <v>49</v>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="B50" s="0" t="inlineStr">
         <is>
           <t>レベル１だけどユニークスキルで最強です</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="C50" s="0" t="inlineStr">
         <is>
           <t>漫画：真綿 原作：三木なずな キャラクター原案：すばち</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
+      <c r="D50" s="0" t="inlineStr">
         <is>
           <t>第７２話　インドール救援作戦 大成功!?（２）</t>
         </is>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="n">
+      <c r="A51" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="B51" s="0" t="inlineStr">
         <is>
           <t>ワンパンマン</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="C51" s="0" t="inlineStr">
         <is>
           <t>原作/ＯＮＥ 作画/村田雄介</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
+      <c r="D51" s="0" t="inlineStr">
         <is>
           <t>207撃目</t>
         </is>
@@ -34851,6 +34852,1047 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>生徒会にも穴はある！</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>むちまろ</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>第132話	ありす大ピンチ！（バッドエンド編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>おまけ64</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>第32話 独身貴族は森で写真を撮る（3）</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>異世界食堂　洋食のねこや</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>犬塚惇平(ヒーロー文庫／イマジカインフォス)(原作) ヤミザワ(漫画) モロザワ(漫画) エナミカツミ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>第40話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>オタクに優しいギャルはいない!?</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>のりしろちゃん 魚住さかな</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>【#150】ひび割れ</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>生徒会役員共</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>氏家ト全</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>#407</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>脇役に転生したはずが、いつの間にか伝説の錬金術師になってた～仲間たちが英雄でも俺は支援職なんだが～</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>神無月みり 相野 仁</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>第２６話　脇役、目論見を見破る（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>♀ガキとおじさん</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>サラマンダ(著者)</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>第29話</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>カナン様はあくまでチョロい</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>nonco</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>第144話	リリイの仕返し恩返し</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ブレイド＆バスタード</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>漫画/楓月 誠 原作/蝸牛くも キャラクター原案/so-bin</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>第10話（2）</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>すべての人類を破壊する。それらは再生できない。</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>横田卓馬(漫画) 伊瀬勝良(原作)</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>第67話その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>色欲無双 ～変態スキルが暴走してヤリサーから追放された俺は、はからずも淫靡な力で最強になる～</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>あいのひとし 笠原巴 三九呂</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>第1話 ヤリサーを追放！？</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>よわよわ先生</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>福地カミオ</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>第109話	ほどほどのバレンタインデー</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>世界最速のレベルアップ</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>鈴見敦(漫画) 八又ナガト(原作) fame(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>第48話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>異世界居酒屋「のぶ」</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>蝉川夏哉(原作) ヴァージニア二等兵(漫画) 転(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>第123話</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>おかけになった呪文は現在使われておりません</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>ロケット商会 天宮ケイリ</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>第1話　婚活の呪文</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>善人おっさん、生まれ変わったらSSSランク人生が確定した</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>原作／三木なずな 漫画／ゆづましろ キャラクター原案／伍長</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>祝！単行本11巻発売！特別イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>ギャルゲーマーに褒められたい</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>げしゅまろ(著者)</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>45話</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>やり直し令嬢は竜帝陛下を攻略中</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>柚アンコ(漫画) 永瀬さらさ（角川ビーンズ文庫）(原作) 藤未都也(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Episode40.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>百瀬アキラの初恋破綻中。</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>晴川シンタ</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>第33話 あくまで公務を執行中。</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>漫画/すたひろ 原作/Y.A</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>chapter66【35話①】</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>え、社内システム全てワンオペしている私を解雇ですか？</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>漫画：伊於 原作：下城米雪 キャラクター原案：icchi</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>4巻発売告知漫画</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>ガリ勉くんと裏アカさん　散々お世話になっているエロ系裏垢女子の正体がクラスのアイドルだった件</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>花咲まひる(著者) 鈴木えんぺら(原作) 小花雪(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>第9話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>戸賀 環 坂木持丸 riritto</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>第50話①　祝われた家を探索してみた</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>女子高生の無駄づかい</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>ビーノ(著者)</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>第133話　てこいれ</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>奈落の底で生活して早三年、当時『白魔道士』だった私は『聖魔女』になっていた</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>雪葵ムラサキ(漫画) tani(原作) れんた(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>第7話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>妹はカノジョにできないのに</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>ちくわ。(作画) 鏡遊(原作) 三九呂(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>第29話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>黒月のイェルクナハト</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>スズモトコウ</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>第6話	生きる意味</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>ひとりぼっちの異世界攻略</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>びび（漫画） 五示正司（原作）</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>第229話　最初は良い感じだったよ…？</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>絶対死なないステラ姫</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>光永康則 大高稲</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>第１４話　絶対旅立たない（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>帰ってください！ 阿久津さん</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>長岡太一(著者)</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>第193話</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>ぽんドロイド！ はまさん</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>はれやまはれぞう(著者)</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>第5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>アンゴルモア 元寇合戦記　【博多編】</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>たかぎ七彦(著者)</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>第四十四話その七</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>「おかえり、パパ」</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>蝉丸</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>第26話　家族</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>最強の少年聖騎士、転生者を狩る</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>作画：御塩 原作：宇奈木ユラ</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>第6話(2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>ロードマギアの弟子</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>FLIPFLOPs</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>第19話 魔術師の戦い (後編)</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>姫ヶ崎櫻子は今日も不憫可愛い</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>安田剛助(著者)</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>第49話</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>ポーション、わが身を助ける</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>戸部淑 岩船晶</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>第1話</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>異世界おじさん</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>殆ど死んでいる(著者)</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>魔術師クノンは見えている</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>第39話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>カッコウの許嫁</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>吉河美希</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>第257話	また将来の選択肢が増えちゃった!</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>色憑くモノクローム</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>内山敦司</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>第39話	湧き上がる熱情</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>江戸前エルフ</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>樋口彰彦</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>#116</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>ダウナー系お姉さんに毎日カスの嘘を流し込まれる話</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>生倉のゑる(著者) はるばーど屋(原作者)</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>11話 おまけ</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>第５０話　雌雄を決する器用貧乏（４）</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>第47話 魔導具師とつながれたもの③</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>最後のエルフ</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>サワノアキラ（漫画）</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>第9章　竜の眠る地（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>帰ってきた元勇者</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>漫画：なるさわ景 原作：ニシ キャラクター原案：米白粕</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>第31話(3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>ゆめねこねくと</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>澤田コウ</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>第38こねくと	ゆめねこねくと</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>序盤で死ぬ最強のサブキャラに転生したので、ゲーム知識で無双する</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>作画：マエD 原作：新人</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>第5話(2)</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Add ranking data for 2025-08-01
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -46,6 +46,7 @@
     <sheet name="2025-07-29" sheetId="38" state="visible" r:id="rId38"/>
     <sheet name="2025-07-30" sheetId="39" state="visible" r:id="rId39"/>
     <sheet name="2025-07-31" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="2025-08-01" sheetId="41" state="visible" r:id="rId41"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -34889,22 +34890,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>生徒会にも穴はある！</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>むちまろ</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第132話	ありす大ピンチ！（バッドエンド編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>おまけ64</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第32話 独身貴族は森で写真を撮る（3）</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>異世界食堂　洋食のねこや</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>犬塚惇平(ヒーロー文庫／イマジカインフォス)(原作) ヤミザワ(漫画) モロザワ(漫画) エナミカツミ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第40話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>オタクに優しいギャルはいない!?</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>のりしろちゃん 魚住さかな</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>【#150】ひび割れ</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>生徒会役員共</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>氏家ト全</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>#407</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>脇役に転生したはずが、いつの間にか伝説の錬金術師になってた～仲間たちが英雄でも俺は支援職なんだが～</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>神無月みり 相野 仁</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第２６話　脇役、目論見を見破る（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>♀ガキとおじさん</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>サラマンダ(著者)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第29話</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>カナン様はあくまでチョロい</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>nonco</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第144話	リリイの仕返し恩返し</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>ブレイド＆バスタード</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>漫画/楓月 誠 原作/蝸牛くも キャラクター原案/so-bin</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第10話（2）</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>すべての人類を破壊する。それらは再生できない。</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>横田卓馬(漫画) 伊瀬勝良(原作)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第67話その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>色欲無双 ～変態スキルが暴走してヤリサーから追放された俺は、はからずも淫靡な力で最強になる～</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>あいのひとし 笠原巴 三九呂</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第1話 ヤリサーを追放！？</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>よわよわ先生</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>福地カミオ</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第109話	ほどほどのバレンタインデー</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>世界最速のレベルアップ</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>鈴見敦(漫画) 八又ナガト(原作) fame(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第48話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>異世界居酒屋「のぶ」</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>蝉川夏哉(原作) ヴァージニア二等兵(漫画) 転(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第123話</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>おかけになった呪文は現在使われておりません</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>ロケット商会 天宮ケイリ</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第1話　婚活の呪文</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>善人おっさん、生まれ変わったらSSSランク人生が確定した</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>原作／三木なずな 漫画／ゆづましろ キャラクター原案／伍長</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>祝！単行本11巻発売！特別イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>ギャルゲーマーに褒められたい</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>げしゅまろ(著者)</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>45話</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>やり直し令嬢は竜帝陛下を攻略中</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>柚アンコ(漫画) 永瀬さらさ（角川ビーンズ文庫）(原作) 藤未都也(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>Episode40.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>百瀬アキラの初恋破綻中。</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>晴川シンタ</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第33話 あくまで公務を執行中。</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>漫画/すたひろ 原作/Y.A</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>chapter66【35話①】</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>え、社内システム全てワンオペしている私を解雇ですか？</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>漫画：伊於 原作：下城米雪 キャラクター原案：icchi</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>4巻発売告知漫画</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>ガリ勉くんと裏アカさん　散々お世話になっているエロ系裏垢女子の正体がクラスのアイドルだった件</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>花咲まひる(著者) 鈴木えんぺら(原作) 小花雪(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第9話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>戸賀 環 坂木持丸 riritto</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第50話①　祝われた家を探索してみた</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>女子高生の無駄づかい</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>ビーノ(著者)</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第133話　てこいれ</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>奈落の底で生活して早三年、当時『白魔道士』だった私は『聖魔女』になっていた</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>雪葵ムラサキ(漫画) tani(原作) れんた(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第7話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>妹はカノジョにできないのに</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>ちくわ。(作画) 鏡遊(原作) 三九呂(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第29話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>黒月のイェルクナハト</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>スズモトコウ</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第6話	生きる意味</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>ひとりぼっちの異世界攻略</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>びび（漫画） 五示正司（原作）</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第229話　最初は良い感じだったよ…？</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>絶対死なないステラ姫</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>光永康則 大高稲</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第１４話　絶対旅立たない（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>帰ってください！ 阿久津さん</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>長岡太一(著者)</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第193話</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>ぽんドロイド！ はまさん</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>はれやまはれぞう(著者)</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>アンゴルモア 元寇合戦記　【博多編】</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>たかぎ七彦(著者)</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第四十四話その七</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>「おかえり、パパ」</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>蝉丸</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第26話　家族</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>最強の少年聖騎士、転生者を狩る</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>作画：御塩 原作：宇奈木ユラ</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第6話(2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>ロードマギアの弟子</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>FLIPFLOPs</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第19話 魔術師の戦い (後編)</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>姫ヶ崎櫻子は今日も不憫可愛い</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>安田剛助(著者)</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第49話</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>ポーション、わが身を助ける</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>戸部淑 岩船晶</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第1話</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>異世界おじさん</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>殆ど死んでいる(著者)</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>魔術師クノンは見えている</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第39話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>カッコウの許嫁</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>吉河美希</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第257話	また将来の選択肢が増えちゃった!</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>色憑くモノクローム</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>内山敦司</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第39話	湧き上がる熱情</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>江戸前エルフ</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>樋口彰彦</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>#116</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>ダウナー系お姉さんに毎日カスの嘘を流し込まれる話</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>生倉のゑる(著者) はるばーど屋(原作者)</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>11話 おまけ</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第５０話　雌雄を決する器用貧乏（４）</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第47話 魔導具師とつながれたもの③</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>最後のエルフ</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>サワノアキラ（漫画）</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第9章　竜の眠る地（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>帰ってきた元勇者</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>漫画：なるさわ景 原作：ニシ キャラクター原案：米白粕</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第31話(3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>ゆめねこねくと</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>澤田コウ</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第38こねくと	ゆめねこねくと</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>序盤で死ぬ最強のサブキャラに転生したので、ゲーム知識で無双する</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>作画：マエD 原作：新人</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第5話(2)</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>生徒会にも穴はある！</t>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>むちまろ</t>
+          <t>村上よしゆき 茨木野 あるてら</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第132話	ありす大ピンチ！（バッドエンド編）</t>
+          <t>第４１話　勇者、人魚王国を救い、歓迎される。あと、六邪神将が、全員来る（１）</t>
         </is>
       </c>
     </row>
@@ -34914,17 +35956,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>実は俺、最強でした？</t>
+          <t>ライブダンジョン！</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>原作：澄守 彩 漫画：高橋 愛</t>
+          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>おまけ64</t>
+          <t>第88話後半</t>
         </is>
       </c>
     </row>
@@ -34934,17 +35976,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第32話 独身貴族は森で写真を撮る（3）</t>
+          <t>第2話②</t>
         </is>
       </c>
     </row>
@@ -34954,17 +35996,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>異世界食堂　洋食のねこや</t>
+          <t>魔石グルメ　魔物の力を食べたオレは最強！</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>犬塚惇平(ヒーロー文庫／イマジカインフォス)(原作) ヤミザワ(漫画) モロザワ(漫画) エナミカツミ(キャラクター原案)</t>
+          <t>菅原健二(作画) 結城涼(原作) 成瀬ちさと(キャラクター原案)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第40話②</t>
+          <t>第67話後半</t>
         </is>
       </c>
     </row>
@@ -34974,17 +36016,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>オタクに優しいギャルはいない!?</t>
+          <t>生徒会にも穴はある！</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>のりしろちゃん 魚住さかな</t>
+          <t>むちまろ</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>【#150】ひび割れ</t>
+          <t>第132話	ありす大ピンチ！（バッドエンド編）</t>
         </is>
       </c>
     </row>
@@ -34994,17 +36036,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>生徒会役員共</t>
+          <t>貧乏騎士に嫁入りしたはずが!? ~野人令嬢は皇太子妃になっても竜を狩りたい~</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>氏家ト全</t>
+          <t>漫画：夏川そぞろ 原作：宮前葵 キャラクター原案：ののまろ</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>#407</t>
+          <t>第11話①皇族の責務</t>
         </is>
       </c>
     </row>
@@ -35014,17 +36056,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>脇役に転生したはずが、いつの間にか伝説の錬金術師になってた～仲間たちが英雄でも俺は支援職なんだが～</t>
+          <t>となりの席のヤツがそういう目で見てくる</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>神無月みり 相野 仁</t>
+          <t>mmk</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第２６話　脇役、目論見を見破る（３）</t>
+          <t>第43話 臨戦態勢</t>
         </is>
       </c>
     </row>
@@ -35034,17 +36076,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>♀ガキとおじさん</t>
+          <t>規格外のダンジョン攻略者、実は異世界帰りの元勇者</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>サラマンダ(著者)</t>
+          <t>作画：やまざき君 原作：榊与一</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第29話</t>
+          <t>第5話(1)</t>
         </is>
       </c>
     </row>
@@ -35054,17 +36096,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>カナン様はあくまでチョロい</t>
+          <t>色欲無双 ～変態スキルが暴走してヤリサーから追放された俺は、はからずも淫靡な力で最強になる～</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>nonco</t>
+          <t>あいのひとし 笠原巴 三九呂</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第144話	リリイの仕返し恩返し</t>
+          <t>第1話 ヤリサーを追放！？</t>
         </is>
       </c>
     </row>
@@ -35074,17 +36116,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ブレイド＆バスタード</t>
+          <t>僕は今すぐ前世の記憶を捨てたい。～憧れの田舎は人外魔境でした～@COMIC</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>漫画/楓月 誠 原作/蝸牛くも キャラクター原案/so-bin</t>
+          <t>大島つむぎ （漫画） 星畑旭（原作） スズキイオリ （キャラクター原案）</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第10話（2）</t>
+          <t>第19話 ①</t>
         </is>
       </c>
     </row>
@@ -35094,17 +36136,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>すべての人類を破壊する。それらは再生できない。</t>
+          <t>二番目な僕と一番の彼女</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>横田卓馬(漫画) 伊瀬勝良(原作)</t>
+          <t>ぬずタニ(漫画) 和尚(原作) ミュシャ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第67話その1</t>
+          <t>第1話</t>
         </is>
       </c>
     </row>
@@ -35114,17 +36156,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>色欲無双 ～変態スキルが暴走してヤリサーから追放された俺は、はからずも淫靡な力で最強になる～</t>
+          <t>継母の連れ子が元カノだった</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>あいのひとし 笠原巴 三九呂</t>
+          <t>草壁レイ(作画) 紙城境介(原作) たかやKi(キャラクター原案)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第1話 ヤリサーを追放！？</t>
+          <t>第61話後半</t>
         </is>
       </c>
     </row>
@@ -35134,17 +36176,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>よわよわ先生</t>
+          <t>え、社内システム全てワンオペしている私を解雇ですか？</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>福地カミオ</t>
+          <t>漫画：伊於 原作：下城米雪 キャラクター原案：icchi</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第109話	ほどほどのバレンタインデー</t>
+          <t>4巻発売告知漫画</t>
         </is>
       </c>
     </row>
@@ -35154,17 +36196,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>世界最速のレベルアップ</t>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>鈴見敦(漫画) 八又ナガト(原作) fame(キャラクター原案)</t>
+          <t>漫画/すたひろ 原作/Y.A</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第48話②</t>
+          <t>chapter66【35話①】</t>
         </is>
       </c>
     </row>
@@ -35174,17 +36216,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>異世界居酒屋「のぶ」</t>
+          <t>ギルド追放された雑用係の下剋上～超万能な生活スキルで世界最強～</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>蝉川夏哉(原作) ヴァージニア二等兵(漫画) 転(キャラクター原案)</t>
+          <t>原作／夜桜ユノ 漫画／柳輪 ネーム構成／ユーキあきら</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第123話</t>
+          <t>第63話</t>
         </is>
       </c>
     </row>
@@ -35194,17 +36236,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>おかけになった呪文は現在使われておりません</t>
+          <t>実は俺、最強でした？</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>ロケット商会 天宮ケイリ</t>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第1話　婚活の呪文</t>
+          <t>おまけ64</t>
         </is>
       </c>
     </row>
@@ -35214,17 +36256,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>善人おっさん、生まれ変わったらSSSランク人生が確定した</t>
+          <t>ルパン三世 異世界の姫君（ネイバーワールドプリンセス）</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>原作／三木なずな 漫画／ゆづましろ キャラクター原案／伍長</t>
+          <t>モンキー・パンチ／エム・ピー・ワークス 内々けやき 佐伯庸介 白狼</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>祝！単行本11巻発売！特別イラスト</t>
+          <t>第103話：マッスルタの魔犬❸</t>
         </is>
       </c>
     </row>
@@ -35234,17 +36276,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ギャルゲーマーに褒められたい</t>
+          <t>我が焔炎にひれ伏せ世界</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>げしゅまろ(著者)</t>
+          <t>すめらぎひよこ(原作) こゆき(作画) Mika Pikazo(キャラクター原案) mocha(背景画)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>45話</t>
+          <t>第12話</t>
         </is>
       </c>
     </row>
@@ -35254,17 +36296,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>やり直し令嬢は竜帝陛下を攻略中</t>
+          <t>自分の事を主人公だと信じてやまない踏み台が、主人公を踏み台だと勘違いして、優勝してしまうお話です@COMIC</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>柚アンコ(漫画) 永瀬さらさ（角川ビーンズ文庫）(原作) 藤未都也(キャラクター原案)</t>
+          <t>KYO=H（漫画） 流石ユユシタ（原作） 卵の黄身（キャラクター原案）</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Episode40.5</t>
+          <t>第5話</t>
         </is>
       </c>
     </row>
@@ -35274,17 +36316,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>百瀬アキラの初恋破綻中。</t>
+          <t>直径3cmの召喚陣&lt;リミットリング&gt;で「雑魚すら呼べない」と蔑まれた底辺召喚士が頂点に立つまで</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>晴川シンタ</t>
+          <t>作画：まっつー 原作：空松蓮司</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第33話 あくまで公務を執行中。</t>
+          <t>第5話(1)</t>
         </is>
       </c>
     </row>
@@ -35294,17 +36336,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+          <t>モブだけど最強を目指します！　～ゲーム世界に転生した俺は自由に強さを追い求める～</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>漫画/すたひろ 原作/Y.A</t>
+          <t>反面教師(原作) 五條さやか(作画) 大熊猫介(キャラクター原案)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>chapter66【35話①】</t>
+          <t>第12話-2</t>
         </is>
       </c>
     </row>
@@ -35314,17 +36356,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>え、社内システム全てワンオペしている私を解雇ですか？</t>
+          <t>異世界食堂　洋食のねこや</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>漫画：伊於 原作：下城米雪 キャラクター原案：icchi</t>
+          <t>犬塚惇平(ヒーロー文庫／イマジカインフォス)(原作) ヤミザワ(漫画) モロザワ(漫画) エナミカツミ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>4巻発売告知漫画</t>
+          <t>第40話②</t>
         </is>
       </c>
     </row>
@@ -35334,17 +36376,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ガリ勉くんと裏アカさん　散々お世話になっているエロ系裏垢女子の正体がクラスのアイドルだった件</t>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>花咲まひる(著者) 鈴木えんぺら(原作) 小花雪(キャラクター原案)</t>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第9話①</t>
+          <t>第32話 独身貴族は森で写真を撮る（3）</t>
         </is>
       </c>
     </row>
@@ -35354,17 +36396,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+          <t>君の刀が折れるまで ~月宮まつりの恋難き~</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>戸賀 環 坂木持丸 riritto</t>
+          <t>イノウエ</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第50話①　祝われた家を探索してみた</t>
+          <t>第39話 あの日のこと</t>
         </is>
       </c>
     </row>
@@ -35374,17 +36416,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>女子高生の無駄づかい</t>
+          <t>ブレイド＆バスタード</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ビーノ(著者)</t>
+          <t>漫画/楓月 誠 原作/蝸牛くも キャラクター原案/so-bin</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第133話　てこいれ</t>
+          <t>第11話（1）</t>
         </is>
       </c>
     </row>
@@ -35394,17 +36436,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>奈落の底で生活して早三年、当時『白魔道士』だった私は『聖魔女』になっていた</t>
+          <t>ゲーム内最強の『裏ボス』に転生したので、主人公の代わりに最速クリアを目指します！</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>雪葵ムラサキ(漫画) tani(原作) れんた(キャラクター原案)</t>
+          <t>作画：こめぐ 原作：迅空也</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第7話①</t>
+          <t>第5話(1)</t>
         </is>
       </c>
     </row>
@@ -35414,17 +36456,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>妹はカノジョにできないのに</t>
+          <t>金色の文字使い ―勇者四人に巻き込まれたユニークチート―</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>ちくわ。(作画) 鏡遊(原作) 三九呂(キャラクターデザイン)</t>
+          <t>尾崎祐介(作画) 十本スイ(原作) すまき俊悟(キャラクター原案)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第29話②</t>
+          <t>第121話</t>
         </is>
       </c>
     </row>
@@ -35434,17 +36476,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>黒月のイェルクナハト</t>
+          <t>異世界居酒屋「のぶ」</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>スズモトコウ</t>
+          <t>蝉川夏哉(原作) ヴァージニア二等兵(漫画) 転(キャラクター原案)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第6話	生きる意味</t>
+          <t>第123話</t>
         </is>
       </c>
     </row>
@@ -35454,17 +36496,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ひとりぼっちの異世界攻略</t>
+          <t>オタクに優しいギャルはいない!?</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>びび（漫画） 五示正司（原作）</t>
+          <t>のりしろちゃん 魚住さかな</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第229話　最初は良い感じだったよ…？</t>
+          <t>【#150】ひび割れ</t>
         </is>
       </c>
     </row>
@@ -35474,17 +36516,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>絶対死なないステラ姫</t>
+          <t>黒魔法寮の三悪人</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>光永康則 大高稲</t>
+          <t>斎藤キミオ</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第１４話　絶対旅立たない（３）</t>
+          <t>第43話 こんな寮があるからいけないのだよ!</t>
         </is>
       </c>
     </row>
@@ -35494,17 +36536,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>帰ってください！ 阿久津さん</t>
+          <t>♀ガキとおじさん</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>長岡太一(著者)</t>
+          <t>サラマンダ(著者)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第193話</t>
+          <t>第29話</t>
         </is>
       </c>
     </row>
@@ -35514,17 +36556,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ぽんドロイド！ はまさん</t>
+          <t>カナン様はあくまでチョロい</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>はれやまはれぞう(著者)</t>
+          <t>nonco</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第5話</t>
+          <t>第144話	リリイの仕返し恩返し</t>
         </is>
       </c>
     </row>
@@ -35534,17 +36576,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>アンゴルモア 元寇合戦記　【博多編】</t>
+          <t>無能と蔑まれた【勇気ある者】が、実は伝説の【勇者】でした~500年前の仲間＆魔王の娘と一緒に今度こそ世界を救います~</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>たかぎ七彦(著者)</t>
+          <t>作画：シグチサトシ 原作：やすくん</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第四十四話その七</t>
+          <t>第5話(1)</t>
         </is>
       </c>
     </row>
@@ -35554,17 +36596,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>「おかえり、パパ」</t>
+          <t>生徒会役員共</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>蝉丸</t>
+          <t>氏家ト全</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第26話　家族</t>
+          <t>#407</t>
         </is>
       </c>
     </row>
@@ -35574,17 +36616,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>最強の少年聖騎士、転生者を狩る</t>
+          <t>脇役に転生したはずが、いつの間にか伝説の錬金術師になってた～仲間たちが英雄でも俺は支援職なんだが～</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>作画：御塩 原作：宇奈木ユラ</t>
+          <t>神無月みり 相野 仁</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第6話(2)</t>
+          <t>第２６話　脇役、目論見を見破る（３）</t>
         </is>
       </c>
     </row>
@@ -35594,17 +36636,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>ロードマギアの弟子</t>
+          <t>不死王の息子</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>FLIPFLOPs</t>
+          <t>日向夏(原作) 小うどん(漫画) 大地幹(キャラクター原案)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第19話 魔術師の戦い (後編)</t>
+          <t>第2話-2</t>
         </is>
       </c>
     </row>
@@ -35614,17 +36656,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>姫ヶ崎櫻子は今日も不憫可愛い</t>
+          <t>よわよわ先生</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>安田剛助(著者)</t>
+          <t>福地カミオ</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第49話</t>
+          <t>第109話	ほどほどのバレンタインデー</t>
         </is>
       </c>
     </row>
@@ -35634,12 +36676,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ポーション、わが身を助ける</t>
+          <t>悪役令嬢、俺</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>戸部淑 岩船晶</t>
+          <t>弥南せいら(漫画) 猫屋敷のあ(原作)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -35654,17 +36696,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>異世界おじさん</t>
+          <t>すべての人類を破壊する。それらは再生できない。</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>殆ど死んでいる(著者)</t>
+          <t>横田卓馬(漫画) 伊瀬勝良(原作)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+          <t>第67話その1</t>
         </is>
       </c>
     </row>
@@ -35674,17 +36716,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>魔術師クノンは見えている</t>
+          <t>異世界おじさん</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+          <t>殆ど死んでいる(著者)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第39話①</t>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
         </is>
       </c>
     </row>
@@ -35694,17 +36736,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>カッコウの許嫁</t>
+          <t>女子高生の無駄づかい</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>吉河美希</t>
+          <t>ビーノ(著者)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第257話	また将来の選択肢が増えちゃった!</t>
+          <t>第133話　てこいれ</t>
         </is>
       </c>
     </row>
@@ -35714,17 +36756,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>色憑くモノクローム</t>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>内山敦司</t>
+          <t>戸賀 環 坂木持丸 riritto</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第39話	湧き上がる熱情</t>
+          <t>第50話①　祝われた家を探索してみた</t>
         </is>
       </c>
     </row>
@@ -35734,17 +36776,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>江戸前エルフ</t>
+          <t>極悪令嬢～令嬢に転生した最強老兵はスキル「魔弾」で無双する～</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>樋口彰彦</t>
+          <t>作画：月村月野 原作：ルクル</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>#116</t>
+          <t>第5話(1)</t>
         </is>
       </c>
     </row>
@@ -35754,17 +36796,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ダウナー系お姉さんに毎日カスの嘘を流し込まれる話</t>
+          <t>死に戻った最強勇者は、すべてを守り切る</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>生倉のゑる(著者) はるばーど屋(原作者)</t>
+          <t>作画：花門初海 原作：柚鼓ユズ</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>11話 おまけ</t>
+          <t>第5話(1)</t>
         </is>
       </c>
     </row>
@@ -35774,17 +36816,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+          <t>魔術師クノンは見えている</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第５０話　雌雄を決する器用貧乏（４）</t>
+          <t>第39話①</t>
         </is>
       </c>
     </row>
@@ -35794,17 +36836,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
+          <t>ポーション、わが身を助ける</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
+          <t>戸部淑 岩船晶</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第47話 魔導具師とつながれたもの③</t>
+          <t>第1話</t>
         </is>
       </c>
     </row>
@@ -35814,17 +36856,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>最後のエルフ</t>
+          <t>角と板と魔法記師 Tab.3</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>サワノアキラ（漫画）</t>
+          <t>とりから</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第9章　竜の眠る地（後編）</t>
+          <t>第25話の4</t>
         </is>
       </c>
     </row>
@@ -35834,17 +36876,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>帰ってきた元勇者</t>
+          <t>世界最速のレベルアップ</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>漫画：なるさわ景 原作：ニシ キャラクター原案：米白粕</t>
+          <t>鈴見敦(漫画) 八又ナガト(原作) fame(キャラクター原案)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第31話(3)</t>
+          <t>第48話②</t>
         </is>
       </c>
     </row>
@@ -35854,17 +36896,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>ゆめねこねくと</t>
+          <t>陰キャちゃん総長にされる「２枠目」</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>澤田コウ</t>
+          <t>紫野原広隆</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第38こねくと	ゆめねこねくと</t>
+          <t>第35話</t>
         </is>
       </c>
     </row>
@@ -35874,17 +36916,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>序盤で死ぬ最強のサブキャラに転生したので、ゲーム知識で無双する</t>
+          <t>やり直し令嬢は竜帝陛下を攻略中</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>作画：マエD 原作：新人</t>
+          <t>柚アンコ(漫画) 永瀬さらさ（角川ビーンズ文庫）(原作) 藤未都也(キャラクター原案)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第5話(2)</t>
+          <t>Episode40.5</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-08-02
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -47,6 +47,7 @@
     <sheet name="2025-07-30" sheetId="39" state="visible" r:id="rId39"/>
     <sheet name="2025-07-31" sheetId="40" state="visible" r:id="rId40"/>
     <sheet name="2025-08-01" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="2025-08-02" sheetId="42" state="visible" r:id="rId42"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -35931,22 +35932,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>村上よしゆき 茨木野 あるてら</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第４１話　勇者、人魚王国を救い、歓迎される。あと、六邪神将が、全員来る（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>ライブダンジョン！</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第88話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第2話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>魔石グルメ　魔物の力を食べたオレは最強！</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>菅原健二(作画) 結城涼(原作) 成瀬ちさと(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第67話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>生徒会にも穴はある！</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>むちまろ</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第132話	ありす大ピンチ！（バッドエンド編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>貧乏騎士に嫁入りしたはずが!? ~野人令嬢は皇太子妃になっても竜を狩りたい~</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>漫画：夏川そぞろ 原作：宮前葵 キャラクター原案：ののまろ</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第11話①皇族の責務</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>となりの席のヤツがそういう目で見てくる</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>mmk</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第43話 臨戦態勢</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>規格外のダンジョン攻略者、実は異世界帰りの元勇者</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>作画：やまざき君 原作：榊与一</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第5話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>色欲無双 ～変態スキルが暴走してヤリサーから追放された俺は、はからずも淫靡な力で最強になる～</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>あいのひとし 笠原巴 三九呂</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第1話 ヤリサーを追放！？</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>僕は今すぐ前世の記憶を捨てたい。～憧れの田舎は人外魔境でした～@COMIC</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>大島つむぎ （漫画） 星畑旭（原作） スズキイオリ （キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第19話 ①</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>二番目な僕と一番の彼女</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>ぬずタニ(漫画) 和尚(原作) ミュシャ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第1話</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>継母の連れ子が元カノだった</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>草壁レイ(作画) 紙城境介(原作) たかやKi(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第61話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>え、社内システム全てワンオペしている私を解雇ですか？</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>漫画：伊於 原作：下城米雪 キャラクター原案：icchi</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>4巻発売告知漫画</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>漫画/すたひろ 原作/Y.A</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>chapter66【35話①】</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>ギルド追放された雑用係の下剋上～超万能な生活スキルで世界最強～</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>原作／夜桜ユノ 漫画／柳輪 ネーム構成／ユーキあきら</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第63話</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>おまけ64</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>ルパン三世 異世界の姫君（ネイバーワールドプリンセス）</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>モンキー・パンチ／エム・ピー・ワークス 内々けやき 佐伯庸介 白狼</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第103話：マッスルタの魔犬❸</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>我が焔炎にひれ伏せ世界</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>すめらぎひよこ(原作) こゆき(作画) Mika Pikazo(キャラクター原案) mocha(背景画)</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第12話</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>自分の事を主人公だと信じてやまない踏み台が、主人公を踏み台だと勘違いして、優勝してしまうお話です@COMIC</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>KYO=H（漫画） 流石ユユシタ（原作） 卵の黄身（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>直径3cmの召喚陣&lt;リミットリング&gt;で「雑魚すら呼べない」と蔑まれた底辺召喚士が頂点に立つまで</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>作画：まっつー 原作：空松蓮司</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第5話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>モブだけど最強を目指します！　～ゲーム世界に転生した俺は自由に強さを追い求める～</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>反面教師(原作) 五條さやか(作画) 大熊猫介(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第12話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>異世界食堂　洋食のねこや</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>犬塚惇平(ヒーロー文庫／イマジカインフォス)(原作) ヤミザワ(漫画) モロザワ(漫画) エナミカツミ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第40話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第32話 独身貴族は森で写真を撮る（3）</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>君の刀が折れるまで ~月宮まつりの恋難き~</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>イノウエ</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第39話 あの日のこと</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>ブレイド＆バスタード</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>漫画/楓月 誠 原作/蝸牛くも キャラクター原案/so-bin</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第11話（1）</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>ゲーム内最強の『裏ボス』に転生したので、主人公の代わりに最速クリアを目指します！</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>作画：こめぐ 原作：迅空也</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第5話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>金色の文字使い ―勇者四人に巻き込まれたユニークチート―</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>尾崎祐介(作画) 十本スイ(原作) すまき俊悟(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第121話</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>異世界居酒屋「のぶ」</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>蝉川夏哉(原作) ヴァージニア二等兵(漫画) 転(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第123話</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>オタクに優しいギャルはいない!?</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>のりしろちゃん 魚住さかな</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>【#150】ひび割れ</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>黒魔法寮の三悪人</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>斎藤キミオ</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第43話 こんな寮があるからいけないのだよ!</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>♀ガキとおじさん</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>サラマンダ(著者)</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第29話</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>カナン様はあくまでチョロい</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>nonco</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第144話	リリイの仕返し恩返し</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>無能と蔑まれた【勇気ある者】が、実は伝説の【勇者】でした~500年前の仲間＆魔王の娘と一緒に今度こそ世界を救います~</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>作画：シグチサトシ 原作：やすくん</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第5話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>生徒会役員共</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>氏家ト全</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>#407</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>脇役に転生したはずが、いつの間にか伝説の錬金術師になってた～仲間たちが英雄でも俺は支援職なんだが～</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>神無月みり 相野 仁</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第２６話　脇役、目論見を見破る（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>不死王の息子</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>日向夏(原作) 小うどん(漫画) 大地幹(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第2話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>よわよわ先生</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>福地カミオ</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第109話	ほどほどのバレンタインデー</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>悪役令嬢、俺</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>弥南せいら(漫画) 猫屋敷のあ(原作)</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第1話</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>すべての人類を破壊する。それらは再生できない。</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>横田卓馬(漫画) 伊瀬勝良(原作)</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第67話その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>異世界おじさん</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>殆ど死んでいる(著者)</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>女子高生の無駄づかい</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>ビーノ(著者)</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第133話　てこいれ</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>戸賀 環 坂木持丸 riritto</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第50話①　祝われた家を探索してみた</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>極悪令嬢～令嬢に転生した最強老兵はスキル「魔弾」で無双する～</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>作画：月村月野 原作：ルクル</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第5話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>死に戻った最強勇者は、すべてを守り切る</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>作画：花門初海 原作：柚鼓ユズ</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第5話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>魔術師クノンは見えている</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第39話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>ポーション、わが身を助ける</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>戸部淑 岩船晶</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第1話</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>角と板と魔法記師 Tab.3</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>とりから</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第25話の4</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>世界最速のレベルアップ</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>鈴見敦(漫画) 八又ナガト(原作) fame(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第48話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>陰キャちゃん総長にされる「２枠目」</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>紫野原広隆</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第35話</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>やり直し令嬢は竜帝陛下を攻略中</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>柚アンコ(漫画) 永瀬さらさ（角川ビーンズ文庫）(原作) 藤未都也(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>Episode40.5</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+          <t>女友達は頼めば意外とヤらせてくれる</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>村上よしゆき 茨木野 あるてら</t>
+          <t>ろくろ(漫画) 鏡遊(原作)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第４１話　勇者、人魚王国を救い、歓迎される。あと、六邪神将が、全員来る（１）</t>
+          <t>第23話②</t>
         </is>
       </c>
     </row>
@@ -35956,17 +36998,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ライブダンジョン！</t>
+          <t>Ｓ級ギルドを追放されたけど、実は俺だけドラゴンの言葉がわかるので、気付いたときには竜騎士の頂点を極めてました。</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
+          <t>ひそな(漫画) 三木なずな(原作) 白狼(キャラクター原案)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第88話後半</t>
+          <t>第37話-2</t>
         </is>
       </c>
     </row>
@@ -35976,17 +37018,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
+          <t>魔のものたちは企てる</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
+          <t>加藤拓弐(原作) ガしガし(作画)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第2話②</t>
+          <t>第28話</t>
         </is>
       </c>
     </row>
@@ -35996,17 +37038,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>魔石グルメ　魔物の力を食べたオレは最強！</t>
+          <t>小林さんちのメイドラゴン</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>菅原健二(作画) 結城涼(原作) 成瀬ちさと(キャラクター原案)</t>
+          <t>クール教信者</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第67話後半</t>
+          <t>第147話</t>
         </is>
       </c>
     </row>
@@ -36016,17 +37058,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>生徒会にも穴はある！</t>
+          <t>遊遊じてき。</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>むちまろ</t>
+          <t>カンケー</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第132話	ありす大ピンチ！（バッドエンド編）</t>
+          <t>第1話</t>
         </is>
       </c>
     </row>
@@ -36036,17 +37078,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>貧乏騎士に嫁入りしたはずが!? ~野人令嬢は皇太子妃になっても竜を狩りたい~</t>
+          <t>くらいあの子としたいこと</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>漫画：夏川そぞろ 原作：宮前葵 キャラクター原案：ののまろ</t>
+          <t>碇マナツ(著者)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第11話①皇族の責務</t>
+          <t>第81話</t>
         </is>
       </c>
     </row>
@@ -36056,17 +37098,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>となりの席のヤツがそういう目で見てくる</t>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>mmk</t>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第43話 臨戦態勢</t>
+          <t>第81話その1</t>
         </is>
       </c>
     </row>
@@ -36076,17 +37118,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>規格外のダンジョン攻略者、実は異世界帰りの元勇者</t>
+          <t>理想のヒモ生活</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>作画：やまざき君 原作：榊与一</t>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第5話(1)</t>
+          <t>第86話　その2</t>
         </is>
       </c>
     </row>
@@ -36096,17 +37138,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>色欲無双 ～変態スキルが暴走してヤリサーから追放された俺は、はからずも淫靡な力で最強になる～</t>
+          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>あいのひとし 笠原巴 三九呂</t>
+          <t>六志麻あさ 業務用餅 kisui</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第1話 ヤリサーを追放！？</t>
+          <t>第６９話</t>
         </is>
       </c>
     </row>
@@ -36116,17 +37158,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>僕は今すぐ前世の記憶を捨てたい。～憧れの田舎は人外魔境でした～@COMIC</t>
+          <t>経験値貯蓄でのんびり傷心旅行 ～勇者と恋人に追放された戦士の無自覚ざまぁ～</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>大島つむぎ （漫画） 星畑旭（原作） スズキイオリ （キャラクター原案）</t>
+          <t>奏ヨシキ(著者) 徳川レモン(原作) riritto(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第19話 ①</t>
+          <t>第37話-2</t>
         </is>
       </c>
     </row>
@@ -36136,17 +37178,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>二番目な僕と一番の彼女</t>
+          <t>最強勇者パーティーは愛が知りたい</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ぬずタニ(漫画) 和尚(原作) ミュシャ(キャラクター原案)</t>
+          <t>山田肌襦袢</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第1話</t>
+          <t>第28話「最後はこぶしがあればいい」</t>
         </is>
       </c>
     </row>
@@ -36156,17 +37198,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>継母の連れ子が元カノだった</t>
+          <t>ゲーセン少女と異文化交流</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>草壁レイ(作画) 紙城境介(原作) たかやKi(キャラクター原案)</t>
+          <t>安原宏和(著者)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第61話後半</t>
+          <t>第127話</t>
         </is>
       </c>
     </row>
@@ -36176,17 +37218,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>え、社内システム全てワンオペしている私を解雇ですか？</t>
+          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>漫画：伊於 原作：下城米雪 キャラクター原案：icchi</t>
+          <t>神原絵理華(漫画) 一森一輝(原作)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>4巻発売告知漫画</t>
+          <t>第18話③</t>
         </is>
       </c>
     </row>
@@ -36196,17 +37238,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>漫画/すたひろ 原作/Y.A</t>
+          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>chapter66【35話①】</t>
+          <t>第76話 Change</t>
         </is>
       </c>
     </row>
@@ -36216,17 +37258,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ギルド追放された雑用係の下剋上～超万能な生活スキルで世界最強～</t>
+          <t>ホームセンターごと呼び出された私の大迷宮リノベーション！</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>原作／夜桜ユノ 漫画／柳輪 ネーム構成／ユーキあきら</t>
+          <t>ばたっち(漫画) 星崎崑(原作) 志田(キャラクター原案)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第63話</t>
+          <t>番外編①</t>
         </is>
       </c>
     </row>
@@ -36236,17 +37278,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>実は俺、最強でした？</t>
+          <t>顔に出ない柏田さんと顔に出る太田君＋</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>原作：澄守 彩 漫画：高橋 愛</t>
+          <t>東ふゆ(著者)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>おまけ64</t>
+          <t>第31話 柏田さんと太田君のすれ違い</t>
         </is>
       </c>
     </row>
@@ -36256,17 +37298,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ルパン三世 異世界の姫君（ネイバーワールドプリンセス）</t>
+          <t>道にスライムが捨てられていたから連れて帰りました ～おじさんとスライムのほのぼの冒険ライフ～</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>モンキー・パンチ／エム・ピー・ワークス 内々けやき 佐伯庸介 白狼</t>
+          <t>めぐお(漫画) イコ(原作) いもいち(キャラクター原案)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第103話：マッスルタの魔犬❸</t>
+          <t>第1話</t>
         </is>
       </c>
     </row>
@@ -36276,17 +37318,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>我が焔炎にひれ伏せ世界</t>
+          <t>修羅幼女の英雄譚～半端者と言われた傭兵、幼女に転生して成り上がる～</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>すめらぎひよこ(原作) こゆき(作画) Mika Pikazo(キャラクター原案) mocha(背景画)</t>
+          <t>作画：むらたん 原作：沙城流</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第12話</t>
+          <t>第8話(1)</t>
         </is>
       </c>
     </row>
@@ -36296,17 +37338,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>自分の事を主人公だと信じてやまない踏み台が、主人公を踏み台だと勘違いして、優勝してしまうお話です@COMIC</t>
+          <t>推しにささげるダンジョングルメ ～最強探索者VTuberになる～</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>KYO=H（漫画） 流石ユユシタ（原作） 卵の黄身（キャラクター原案）</t>
+          <t>モノクロウサギ(原作) 藍川蓮(漫画)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第5話</t>
+          <t>CHAPTER　10-4</t>
         </is>
       </c>
     </row>
@@ -36316,17 +37358,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>直径3cmの召喚陣&lt;リミットリング&gt;で「雑魚すら呼べない」と蔑まれた底辺召喚士が頂点に立つまで</t>
+          <t>底辺冒険者だけど魔法を極めてみることにした ～無能スキルから神スキルに進化した【魔法創造】と【アイテム作成】で無双する～</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>作画：まっつー 原作：空松蓮司</t>
+          <t>蒼乃白兎 坂野杏梨 かわく</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第5話(1)</t>
+          <t>第44話(後編) 深淵の魔印</t>
         </is>
       </c>
     </row>
@@ -36336,17 +37378,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>モブだけど最強を目指します！　～ゲーム世界に転生した俺は自由に強さを追い求める～</t>
+          <t>ヤンデレかと思ったらもっとヤベー女だった</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>反面教師(原作) 五條さやか(作画) 大熊猫介(キャラクター原案)</t>
+          <t>八木戸マト</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第12話-2</t>
+          <t>第69話　全てが終わるヤンデレ彼女</t>
         </is>
       </c>
     </row>
@@ -36356,17 +37398,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>異世界食堂　洋食のねこや</t>
+          <t>異世界はスマートフォンとともに。</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>犬塚惇平(ヒーロー文庫／イマジカインフォス)(原作) ヤミザワ(漫画) モロザワ(漫画) エナミカツミ(キャラクター原案)</t>
+          <t>そと(漫画) 冬原パトラ(原作) 兎塚エイジ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第40話②</t>
+          <t>EPISODE:103‐①</t>
         </is>
       </c>
     </row>
@@ -36376,17 +37418,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+          <t>スキルがなければレベルを上げる～９９がカンストの世界でレベル800万からスタート～</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+          <t>倉橋ユウス(漫画) 岡沢六十四(原作)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第32話 独身貴族は森で写真を撮る（3）</t>
+          <t>第52話①</t>
         </is>
       </c>
     </row>
@@ -36396,17 +37438,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>君の刀が折れるまで ~月宮まつりの恋難き~</t>
+          <t>ゴミ以下だと追放された使用人、実は前世賢者です　～史上最強の賢者、世界最高峰の学園に通う～</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>イノウエ</t>
+          <t>原作：夜分長文 漫画：矢部利恩 キャラクター原案：蔓木鋼音</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第39話 あの日のこと</t>
+          <t>第14話 魔女対策（２）</t>
         </is>
       </c>
     </row>
@@ -36416,17 +37458,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ブレイド＆バスタード</t>
+          <t>異世界転移したら愛犬が最強になりました～シルバーフェンリルと俺が異世界暮らしを始めたら～</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>漫画/楓月 誠 原作/蝸牛くも キャラクター原案/so-bin</t>
+          <t>漫画：一花ハナ 原作：龍央 キャラクター原案：りりんら</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第11話（1）</t>
+          <t>第37話前半</t>
         </is>
       </c>
     </row>
@@ -36436,17 +37478,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ゲーム内最強の『裏ボス』に転生したので、主人公の代わりに最速クリアを目指します！</t>
+          <t>ダウナーお姉さんは遊びたい</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>作画：こめぐ 原作：迅空也</t>
+          <t>山鷹景</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第5話(1)</t>
+          <t>第16話</t>
         </is>
       </c>
     </row>
@@ -36456,17 +37498,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>金色の文字使い ―勇者四人に巻き込まれたユニークチート―</t>
+          <t>つぐもも</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>尾崎祐介(作画) 十本スイ(原作) すまき俊悟(キャラクター原案)</t>
+          <t>浜田よしかづ</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第121話</t>
+          <t>第173話</t>
         </is>
       </c>
     </row>
@@ -36476,17 +37518,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>異世界居酒屋「のぶ」</t>
+          <t>傭兵団の愛し子 ～死にかけ孤児は最強師匠たちに育てられる～</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>蝉川夏哉(原作) ヴァージニア二等兵(漫画) 転(キャラクター原案)</t>
+          <t>柿野レイ(漫画) 天野雪人(原作) 黒井ススム(キャラクター原案)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第123話</t>
+          <t>第7話前編：問題児シャルノア</t>
         </is>
       </c>
     </row>
@@ -36496,17 +37538,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>オタクに優しいギャルはいない!?</t>
+          <t>え、社内システム全てワンオペしている私を解雇ですか？</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>のりしろちゃん 魚住さかな</t>
+          <t>漫画：伊於 原作：下城米雪 キャラクター原案：icchi</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>【#150】ひび割れ</t>
+          <t>4巻発売告知漫画</t>
         </is>
       </c>
     </row>
@@ -36516,17 +37558,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>黒魔法寮の三悪人</t>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>斎藤キミオ</t>
+          <t>漫画/すたひろ 原作/Y.A</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第43話 こんな寮があるからいけないのだよ!</t>
+          <t>chapter66【35話①】</t>
         </is>
       </c>
     </row>
@@ -36536,17 +37578,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>♀ガキとおじさん</t>
+          <t>限界超えの天賦は、転生者にしか扱えない ― オーバーリミット・スキルホルダー ―</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>サラマンダ(著者)</t>
+          <t>長月みそか(漫画) 三上康明(原作) 大槍葦人(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第29話</t>
+          <t>第3章［14］前半</t>
         </is>
       </c>
     </row>
@@ -36556,17 +37598,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>カナン様はあくまでチョロい</t>
+          <t>勇者パーティから追い出された不遇職【罠士】、ユニークスキル【矢印】で最強になる</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>nonco</t>
+          <t>作画：たつひこ 原作：白石 有希</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第144話	リリイの仕返し恩返し</t>
+          <t>第8話(1)</t>
         </is>
       </c>
     </row>
@@ -36576,17 +37618,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>無能と蔑まれた【勇気ある者】が、実は伝説の【勇者】でした~500年前の仲間＆魔王の娘と一緒に今度こそ世界を救います~</t>
+          <t>二番目な僕と一番の彼女</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>作画：シグチサトシ 原作：やすくん</t>
+          <t>ぬずタニ(漫画) 和尚(原作) ミュシャ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第5話(1)</t>
+          <t>第1話</t>
         </is>
       </c>
     </row>
@@ -36596,17 +37638,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>生徒会役員共</t>
+          <t>ブレイド＆バスタード</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>氏家ト全</t>
+          <t>漫画/楓月 誠 原作/蝸牛くも キャラクター原案/so-bin</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>#407</t>
+          <t>第11話（1）</t>
         </is>
       </c>
     </row>
@@ -36616,17 +37658,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>脇役に転生したはずが、いつの間にか伝説の錬金術師になってた～仲間たちが英雄でも俺は支援職なんだが～</t>
+          <t>レベル1で挑む縛りプレイ!</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>神無月みり 相野 仁</t>
+          <t>北川ニキタ 大鐘いしや 刀 彼方</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第２６話　脇役、目論見を見破る（３）</t>
+          <t>最終話 最高の気分②</t>
         </is>
       </c>
     </row>
@@ -36636,17 +37678,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>不死王の息子</t>
+          <t>やっぱ人間やめて正解だわ</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>日向夏(原作) 小うどん(漫画) 大地幹(キャラクター原案)</t>
+          <t>偽BEなんとか</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第2話-2</t>
+          <t>第16話（前編）　ちんちんな二人</t>
         </is>
       </c>
     </row>
@@ -36656,17 +37698,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>よわよわ先生</t>
+          <t>カバンの勇者の異世界のんびり旅 ～実は「カバン」は何でも吸収できるし、日本から何でも取り寄せができるチート武器でした～</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>福地カミオ</t>
+          <t>きしだしき(漫画) 茨木野(原作) キャラクターデザイン(いずみけい)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第109話	ほどほどのバレンタインデー</t>
+          <t>第5話</t>
         </is>
       </c>
     </row>
@@ -36676,17 +37718,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>悪役令嬢、俺</t>
+          <t>チンチンデビルを追え！</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>弥南せいら(漫画) 猫屋敷のあ(原作)</t>
+          <t>くぼたふみお</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第1話</t>
+          <t>第３２話　新たなる目標</t>
         </is>
       </c>
     </row>
@@ -36696,17 +37738,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>すべての人類を破壊する。それらは再生できない。</t>
+          <t>隠居暮らしのおっさん、女王陛下の剣となる</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>横田卓馬(漫画) 伊瀬勝良(原作)</t>
+          <t>漫画/半二合 原作/天酒之瓢 キャラクター原案/みことあけみ</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第67話その1</t>
+          <t>第5話（3）</t>
         </is>
       </c>
     </row>
@@ -36716,17 +37758,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>異世界おじさん</t>
+          <t>ギルドを追放された回復術士、実は魔力無限だったので規格外の回復魔法で伝説となる</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>殆ど死んでいる(著者)</t>
+          <t>漫画：坂下コウ 原作：霞杏檎</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>【マンガ総選挙出馬中】マニフェスト実現に向けて清き一票をお願いします！</t>
+          <t>第4話(3)</t>
         </is>
       </c>
     </row>
@@ -36736,17 +37778,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>女子高生の無駄づかい</t>
+          <t>やめてくれ、強いのは俺じゃなくて剣なんだ……！</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>ビーノ(著者)</t>
+          <t>漫画/廃狼 原作/馬路まんじ キャラクター原案/かぼちゃ</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第133話　てこいれ</t>
+          <t>第8話（1）</t>
         </is>
       </c>
     </row>
@@ -36756,17 +37798,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+          <t>影の英雄の日常譚 勇者の裏で暗躍していた最強のエージェント。組織が解体されたので、正体隠して人並みの日常を謳歌する。</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>戸賀 環 坂木持丸 riritto</t>
+          <t>kanco(漫画) 坂石遊作(原作) TYONE(キャラクター原案)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第50話①　祝われた家を探索してみた</t>
+          <t>Episode32-4</t>
         </is>
       </c>
     </row>
@@ -36776,17 +37818,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>極悪令嬢～令嬢に転生した最強老兵はスキル「魔弾」で無双する～</t>
+          <t>瞳ちゃんは人見知り</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>作画：月村月野 原作：ルクル</t>
+          <t>夏海ちょりすけ</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第5話(1)</t>
+          <t>第137話</t>
         </is>
       </c>
     </row>
@@ -36796,17 +37838,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>死に戻った最強勇者は、すべてを守り切る</t>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>作画：花門初海 原作：柚鼓ユズ</t>
+          <t>村上よしゆき 茨木野 あるてら</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第5話(1)</t>
+          <t>第４１話　勇者、人魚王国を救い、歓迎される。あと、六邪神将が、全員来る（１）</t>
         </is>
       </c>
     </row>
@@ -36816,17 +37858,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>魔術師クノンは見えている</t>
+          <t>錬金術師の辺境再生スローライフ～S級パーティーで孤立した少女をかばったら追放されたので、一緒に幸せに暮らします～</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+          <t>作画：弥永扇 原作：三月菫</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第39話①</t>
+          <t>第8話(1)</t>
         </is>
       </c>
     </row>
@@ -36836,17 +37878,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>ポーション、わが身を助ける</t>
+          <t>生徒会にも穴はある！</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>戸部淑 岩船晶</t>
+          <t>むちまろ</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第1話</t>
+          <t>第132話	ありす大ピンチ！（バッドエンド編）</t>
         </is>
       </c>
     </row>
@@ -36856,17 +37898,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>角と板と魔法記師 Tab.3</t>
+          <t>本能寺から始める信長との天下統一</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>とりから</t>
+          <t>村橋リョウ(作画) 常陸之介寛浩(原作) 茨乃(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第25話の4</t>
+          <t>第五十四話（上）</t>
         </is>
       </c>
     </row>
@@ -36876,17 +37918,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>世界最速のレベルアップ</t>
+          <t>ライブダンジョン！</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>鈴見敦(漫画) 八又ナガト(原作) fame(キャラクター原案)</t>
+          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第48話②</t>
+          <t>第88話後半</t>
         </is>
       </c>
     </row>
@@ -36896,17 +37938,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>陰キャちゃん総長にされる「２枠目」</t>
+          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>紫野原広隆</t>
+          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第35話</t>
+          <t>第2話②</t>
         </is>
       </c>
     </row>
@@ -36916,17 +37958,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>やり直し令嬢は竜帝陛下を攻略中</t>
+          <t>追放されたおっさんタンク、実は防御力最強だったのでダメージゼロで無双する</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>柚アンコ(漫画) 永瀬さらさ（角川ビーンズ文庫）(原作) 藤未都也(キャラクター原案)</t>
+          <t>漫画：化野九十九 原作：あけちともあき</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Episode40.5</t>
+          <t>第4話(3)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-08-03
</commit_message>
<xml_diff>
--- a/ranking_results.xlsx
+++ b/ranking_results.xlsx
@@ -48,6 +48,7 @@
     <sheet name="2025-07-31" sheetId="40" state="visible" r:id="rId40"/>
     <sheet name="2025-08-01" sheetId="41" state="visible" r:id="rId41"/>
     <sheet name="2025-08-02" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="2025-08-03" sheetId="43" state="visible" r:id="rId43"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -36973,22 +36974,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>女友達は頼めば意外とヤらせてくれる</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>ろくろ(漫画) 鏡遊(原作)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第23話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>Ｓ級ギルドを追放されたけど、実は俺だけドラゴンの言葉がわかるので、気付いたときには竜騎士の頂点を極めてました。</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>ひそな(漫画) 三木なずな(原作) 白狼(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第37話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>魔のものたちは企てる</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>加藤拓弐(原作) ガしガし(作画)</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第28話</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>小林さんちのメイドラゴン</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>クール教信者</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第147話</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>遊遊じてき。</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>カンケー</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第1話</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>くらいあの子としたいこと</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>碇マナツ(著者)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第81話</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第81話その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>理想のヒモ生活</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第86話　その2</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>六志麻あさ 業務用餅 kisui</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第６９話</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>経験値貯蓄でのんびり傷心旅行 ～勇者と恋人に追放された戦士の無自覚ざまぁ～</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>奏ヨシキ(著者) 徳川レモン(原作) riritto(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第37話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>最強勇者パーティーは愛が知りたい</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>山田肌襦袢</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第28話「最後はこぶしがあればいい」</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>ゲーセン少女と異文化交流</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>安原宏和(著者)</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第127話</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>神原絵理華(漫画) 一森一輝(原作)</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第18話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>最強で最速の無限レベルアップ ～スキル【経験値1000倍】と【レベルフリー】でレベル上限の枷が外れた俺は無双する～</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>シオヤマ琴 鳥羽田 航 トモゼロ</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第76話 Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>ホームセンターごと呼び出された私の大迷宮リノベーション！</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>ばたっち(漫画) 星崎崑(原作) 志田(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>番外編①</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>顔に出ない柏田さんと顔に出る太田君＋</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>東ふゆ(著者)</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第31話 柏田さんと太田君のすれ違い</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>道にスライムが捨てられていたから連れて帰りました ～おじさんとスライムのほのぼの冒険ライフ～</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>めぐお(漫画) イコ(原作) いもいち(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第1話</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>修羅幼女の英雄譚～半端者と言われた傭兵、幼女に転生して成り上がる～</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>作画：むらたん 原作：沙城流</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第8話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>推しにささげるダンジョングルメ ～最強探索者VTuberになる～</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>モノクロウサギ(原作) 藍川蓮(漫画)</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>CHAPTER　10-4</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>底辺冒険者だけど魔法を極めてみることにした ～無能スキルから神スキルに進化した【魔法創造】と【アイテム作成】で無双する～</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>蒼乃白兎 坂野杏梨 かわく</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第44話(後編) 深淵の魔印</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>ヤンデレかと思ったらもっとヤベー女だった</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>八木戸マト</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第69話　全てが終わるヤンデレ彼女</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>異世界はスマートフォンとともに。</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>そと(漫画) 冬原パトラ(原作) 兎塚エイジ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>EPISODE:103‐①</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>スキルがなければレベルを上げる～９９がカンストの世界でレベル800万からスタート～</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>倉橋ユウス(漫画) 岡沢六十四(原作)</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第52話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>ゴミ以下だと追放された使用人、実は前世賢者です　～史上最強の賢者、世界最高峰の学園に通う～</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>原作：夜分長文 漫画：矢部利恩 キャラクター原案：蔓木鋼音</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第14話 魔女対策（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>異世界転移したら愛犬が最強になりました～シルバーフェンリルと俺が異世界暮らしを始めたら～</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>漫画：一花ハナ 原作：龍央 キャラクター原案：りりんら</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第37話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>ダウナーお姉さんは遊びたい</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>山鷹景</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第16話</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>つぐもも</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>浜田よしかづ</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第173話</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>傭兵団の愛し子 ～死にかけ孤児は最強師匠たちに育てられる～</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>柿野レイ(漫画) 天野雪人(原作) 黒井ススム(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第7話前編：問題児シャルノア</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>え、社内システム全てワンオペしている私を解雇ですか？</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>漫画：伊於 原作：下城米雪 キャラクター原案：icchi</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>4巻発売告知漫画</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>漫画/すたひろ 原作/Y.A</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>chapter66【35話①】</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>限界超えの天賦は、転生者にしか扱えない ― オーバーリミット・スキルホルダー ―</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>長月みそか(漫画) 三上康明(原作) 大槍葦人(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第3章［14］前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティから追い出された不遇職【罠士】、ユニークスキル【矢印】で最強になる</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>作画：たつひこ 原作：白石 有希</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第8話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>二番目な僕と一番の彼女</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>ぬずタニ(漫画) 和尚(原作) ミュシャ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第1話</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>ブレイド＆バスタード</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>漫画/楓月 誠 原作/蝸牛くも キャラクター原案/so-bin</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第11話（1）</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>レベル1で挑む縛りプレイ!</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>北川ニキタ 大鐘いしや 刀 彼方</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>最終話 最高の気分②</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>やっぱ人間やめて正解だわ</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>偽BEなんとか</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第16話（前編）　ちんちんな二人</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>カバンの勇者の異世界のんびり旅 ～実は「カバン」は何でも吸収できるし、日本から何でも取り寄せができるチート武器でした～</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>きしだしき(漫画) 茨木野(原作) キャラクターデザイン(いずみけい)</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>チンチンデビルを追え！</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>くぼたふみお</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第３２話　新たなる目標</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>隠居暮らしのおっさん、女王陛下の剣となる</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>漫画/半二合 原作/天酒之瓢 キャラクター原案/みことあけみ</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第5話（3）</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>ギルドを追放された回復術士、実は魔力無限だったので規格外の回復魔法で伝説となる</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>漫画：坂下コウ 原作：霞杏檎</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第4話(3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>やめてくれ、強いのは俺じゃなくて剣なんだ……！</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>漫画/廃狼 原作/馬路まんじ キャラクター原案/かぼちゃ</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第8話（1）</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>影の英雄の日常譚 勇者の裏で暗躍していた最強のエージェント。組織が解体されたので、正体隠して人並みの日常を謳歌する。</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>kanco(漫画) 坂石遊作(原作) TYONE(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>Episode32-4</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>瞳ちゃんは人見知り</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>夏海ちょりすけ</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第137話</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>村上よしゆき 茨木野 あるてら</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第４１話　勇者、人魚王国を救い、歓迎される。あと、六邪神将が、全員来る（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>錬金術師の辺境再生スローライフ～S級パーティーで孤立した少女をかばったら追放されたので、一緒に幸せに暮らします～</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>作画：弥永扇 原作：三月菫</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第8話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>生徒会にも穴はある！</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>むちまろ</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第132話	ありす大ピンチ！（バッドエンド編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>本能寺から始める信長との天下統一</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>村橋リョウ(作画) 常陸之介寛浩(原作) 茨乃(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第五十四話（上）</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>ライブダンジョン！</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第88話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第2話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>追放されたおっさんタンク、実は防御力最強だったのでダメージゼロで無双する</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>漫画：化野九十九 原作：あけちともあき</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第4話(3)</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>女友達は頼めば意外とヤらせてくれる</t>
+          <t>いとこのこ</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ろくろ(漫画) 鏡遊(原作)</t>
+          <t>いぬちく(著者)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第23話②</t>
+          <t>第36話</t>
         </is>
       </c>
     </row>
@@ -36998,17 +38040,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Ｓ級ギルドを追放されたけど、実は俺だけドラゴンの言葉がわかるので、気付いたときには竜騎士の頂点を極めてました。</t>
+          <t>不純な彼女達は懺悔しない</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ひそな(漫画) 三木なずな(原作) 白狼(キャラクター原案)</t>
+          <t>ポロロッカ(著者)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第37話-2</t>
+          <t>第29話</t>
         </is>
       </c>
     </row>
@@ -37018,17 +38060,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>魔のものたちは企てる</t>
+          <t>リビルドワールド</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>加藤拓弐(原作) ガしガし(作画)</t>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第28話</t>
+          <t>第71話④</t>
         </is>
       </c>
     </row>
@@ -37038,17 +38080,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>小林さんちのメイドラゴン</t>
+          <t>まったく最近の探偵ときたら</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>クール教信者</t>
+          <t>五十嵐正邦(著者)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第147話</t>
+          <t>第114話</t>
         </is>
       </c>
     </row>
@@ -37058,17 +38100,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>遊遊じてき。</t>
+          <t>地味子な三葉さんが僕を誘惑する</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>カンケー</t>
+          <t>はぶらえる(著者)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第1話</t>
+          <t>第10話後半</t>
         </is>
       </c>
     </row